<commit_message>
DP-Tabel fertig designt + DP in Records kriterien
</commit_message>
<xml_diff>
--- a/web/utilities/records_kriterien.xlsx
+++ b/web/utilities/records_kriterien.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgna\Documents\GitHub\Lifesaving_Baden\web3\utilities\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgna\Documents\GitHub\Lifesaving_Baden\web\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86E0D624-F12C-4514-959F-992143F46C64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1243BF90-10B2-48AB-B5CF-809E1DCA4F6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
   </bookViews>
   <sheets>
     <sheet name="DR" sheetId="9" r:id="rId1"/>
     <sheet name="WR-Youth" sheetId="2" r:id="rId2"/>
     <sheet name="WR-Open" sheetId="4" r:id="rId3"/>
-    <sheet name="2024" sheetId="6" r:id="rId4"/>
-    <sheet name="2025" sheetId="5" r:id="rId5"/>
-    <sheet name="2026" sheetId="8" r:id="rId6"/>
+    <sheet name="DP" sheetId="10" r:id="rId4"/>
+    <sheet name="2024" sheetId="6" r:id="rId5"/>
+    <sheet name="2025" sheetId="5" r:id="rId6"/>
+    <sheet name="2026" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -215,7 +216,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="193">
   <si>
     <t>50m Retten</t>
   </si>
@@ -698,6 +699,102 @@
   </si>
   <si>
     <t>50m Retten - 17/18 - M</t>
+  </si>
+  <si>
+    <t>Tabellen Name</t>
+  </si>
+  <si>
+    <t>Weiblich</t>
+  </si>
+  <si>
+    <t>Mindest alter</t>
+  </si>
+  <si>
+    <t>Geschlecht</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>Qualizeitraum anfang</t>
+  </si>
+  <si>
+    <t>Qualizeitraum Ende</t>
+  </si>
+  <si>
+    <t>Letzter Wettkampf am</t>
+  </si>
+  <si>
+    <t>Landesverband</t>
+  </si>
+  <si>
+    <t>Pool-Länge</t>
+  </si>
+  <si>
+    <t>OMS</t>
+  </si>
+  <si>
+    <t>Regelwerk</t>
+  </si>
+  <si>
+    <t>Referenz</t>
+  </si>
+  <si>
+    <t>3-Kampf Regel</t>
+  </si>
+  <si>
+    <t>Anzahl Nominierte</t>
+  </si>
+  <si>
+    <t>Anzahl Nachrücker</t>
+  </si>
+  <si>
+    <t>Seiten Anzahl</t>
+  </si>
+  <si>
+    <t>4-Kampf</t>
+  </si>
+  <si>
+    <t>BA</t>
+  </si>
+  <si>
+    <t>Nein</t>
+  </si>
+  <si>
+    <t>Ja</t>
+  </si>
+  <si>
+    <t>1.11.Jahr - 1</t>
+  </si>
+  <si>
+    <t>30.10.Jahr</t>
+  </si>
+  <si>
+    <t>1.1.Jahr</t>
+  </si>
+  <si>
+    <t>Absagen</t>
+  </si>
+  <si>
+    <t>Männlich</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>Daniel Bittighofer, Roland Konietzny</t>
+  </si>
+  <si>
+    <t>Regina Blonski</t>
+  </si>
+  <si>
+    <t>Referenz Jahr</t>
+  </si>
+  <si>
+    <t>Jahr + 1</t>
+  </si>
+  <si>
+    <t>Mindest Punktzahl</t>
   </si>
 </sst>
 </file>
@@ -964,7 +1061,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1139,14 +1236,78 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="96">
+  <dxfs count="123">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4"/>
       </font>
     </dxf>
     <dxf>
@@ -1205,34 +1366,67 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <color theme="6"/>
-      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color theme="6"/>
-      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color theme="6"/>
-      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3226,108 +3420,158 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2C5E83EE-6B6F-478A-9C90-A846A1A76536}" name="WR_Open4" displayName="WR_Open4" ref="A4:AW31" totalsRowShown="0" headerRowDxfId="95" headerRowBorderDxfId="94" tableBorderDxfId="93">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2C5E83EE-6B6F-478A-9C90-A846A1A76536}" name="WR_Open4" displayName="WR_Open4" ref="A4:AW31" totalsRowShown="0" headerRowDxfId="122" headerRowBorderDxfId="121" tableBorderDxfId="120">
   <autoFilter ref="A4:AW31" xr:uid="{2C5E83EE-6B6F-478A-9C90-A846A1A76536}"/>
   <tableColumns count="49">
-    <tableColumn id="1" xr3:uid="{7C0C4105-A61A-4B8D-9129-EDC4F18765AF}" name="WR-Open" dataDxfId="92">
+    <tableColumn id="1" xr3:uid="{7C0C4105-A61A-4B8D-9129-EDC4F18765AF}" name="WR-Open" dataDxfId="119">
       <calculatedColumnFormula>A4+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{516F5612-F85F-413F-9012-E235F415E34B}" name="50m Retten - offen - W" dataDxfId="91"/>
-    <tableColumn id="3" xr3:uid="{BC9ACAC9-0D45-42FD-B596-D19FBE3A4D83}" name="100m Retten - offen - W" dataDxfId="90"/>
-    <tableColumn id="4" xr3:uid="{CB6DBE59-EB65-43F0-93E7-0BDC3F82832B}" name="100m Kombi - offen - W" dataDxfId="89"/>
-    <tableColumn id="5" xr3:uid="{AA603C60-6831-4C14-A8CD-0AA050DA7551}" name="100m Lifesaver - offen - W" dataDxfId="88"/>
-    <tableColumn id="6" xr3:uid="{7920F147-7717-4582-940A-2610F7D310CA}" name="200m Superlifesaver - offen - W" dataDxfId="87"/>
-    <tableColumn id="7" xr3:uid="{04E21F1D-AC8D-4A1B-9B43-59B8F7901673}" name="200m Hindernis - offen - W" dataDxfId="86"/>
-    <tableColumn id="8" xr3:uid="{40E8A083-653A-48A8-9B37-0A2D850B7829}" name="50m Retten - offen - M" dataDxfId="85"/>
-    <tableColumn id="9" xr3:uid="{863824A9-134F-4189-BB14-225AE224FC44}" name="100m Retten - offen - M" dataDxfId="84"/>
+    <tableColumn id="2" xr3:uid="{516F5612-F85F-413F-9012-E235F415E34B}" name="50m Retten - offen - W" dataDxfId="118"/>
+    <tableColumn id="3" xr3:uid="{BC9ACAC9-0D45-42FD-B596-D19FBE3A4D83}" name="100m Retten - offen - W" dataDxfId="117"/>
+    <tableColumn id="4" xr3:uid="{CB6DBE59-EB65-43F0-93E7-0BDC3F82832B}" name="100m Kombi - offen - W" dataDxfId="116"/>
+    <tableColumn id="5" xr3:uid="{AA603C60-6831-4C14-A8CD-0AA050DA7551}" name="100m Lifesaver - offen - W" dataDxfId="115"/>
+    <tableColumn id="6" xr3:uid="{7920F147-7717-4582-940A-2610F7D310CA}" name="200m Superlifesaver - offen - W" dataDxfId="114"/>
+    <tableColumn id="7" xr3:uid="{04E21F1D-AC8D-4A1B-9B43-59B8F7901673}" name="200m Hindernis - offen - W" dataDxfId="113"/>
+    <tableColumn id="8" xr3:uid="{40E8A083-653A-48A8-9B37-0A2D850B7829}" name="50m Retten - offen - M" dataDxfId="112"/>
+    <tableColumn id="9" xr3:uid="{863824A9-134F-4189-BB14-225AE224FC44}" name="100m Retten - offen - M" dataDxfId="111"/>
     <tableColumn id="10" xr3:uid="{598FC6AE-DEA2-4475-9A35-CDCB8C81496A}" name="100m Kombi - offen - M"/>
     <tableColumn id="11" xr3:uid="{9FC50B37-0D51-422E-A268-A6506D4F3854}" name="100m Lifesaver - offen - M"/>
     <tableColumn id="12" xr3:uid="{B8D2552B-5D82-442A-98F0-E47D5C5F6728}" name="200m Superlifesaver - offen - M"/>
-    <tableColumn id="13" xr3:uid="{5A5E9873-0C5F-4508-AF6B-4974E0526D84}" name="200m Hindernis - offen - M" dataDxfId="83"/>
-    <tableColumn id="14" xr3:uid="{FA907992-7FCE-4CAD-8CF2-F5BEBC9B3756}" name="50m Retten - 17/18 - W" dataDxfId="82"/>
-    <tableColumn id="15" xr3:uid="{76B63DC0-CB67-48F4-9B5A-D22902F59334}" name="100m Retten - 17/18 - W" dataDxfId="81"/>
-    <tableColumn id="16" xr3:uid="{614A2419-51B1-44C0-8469-ADBFB078B81A}" name="100m Kombi -17/18 - W" dataDxfId="80"/>
-    <tableColumn id="17" xr3:uid="{2EC953EE-367D-4524-A25E-8DE3B8168E34}" name="100m Lifesaver - 17/18 - W" dataDxfId="79"/>
-    <tableColumn id="18" xr3:uid="{25711867-9BD7-4197-9094-A21392411249}" name="200m Superlifesaver - 17/18 - W" dataDxfId="78"/>
-    <tableColumn id="19" xr3:uid="{262DB142-CFB1-45C3-9332-7273CACD1B62}" name="200m Hindernis - 17/18 - W" dataDxfId="77"/>
-    <tableColumn id="20" xr3:uid="{938BA45A-8244-4637-8A14-DF49CD91A945}" name="50m Retten - 17/18 - M" dataDxfId="76"/>
-    <tableColumn id="21" xr3:uid="{737E28D8-900F-4A98-95FE-EE7B0AFDEE90}" name="100m Retten - 17/18 - M" dataDxfId="75"/>
-    <tableColumn id="22" xr3:uid="{330BD3A8-061C-45E2-ADDB-40C2F346772F}" name="100m Kombi - 17/18 - M" dataDxfId="74"/>
-    <tableColumn id="23" xr3:uid="{0CADDE90-A167-4E1D-8D33-8624E5E1A4E2}" name="100m Lifesaver - 17/18 - M" dataDxfId="73"/>
-    <tableColumn id="24" xr3:uid="{FCF9F42C-1291-4985-9D37-B9DE2DAA5DCB}" name="200m Superlifesaver - 17/18 - M" dataDxfId="72"/>
-    <tableColumn id="25" xr3:uid="{4E5397B2-F924-4F48-AE69-AF6D650AF88D}" name="200m Hindernis - 17/18 - M" dataDxfId="71"/>
-    <tableColumn id="26" xr3:uid="{0A78315A-BFDC-43EE-A66F-48B301F66508}" name="50m Retten - 15/16 - W" dataDxfId="70"/>
-    <tableColumn id="27" xr3:uid="{D3FCF8BD-6C76-450D-80C0-CC0519A79731}" name="100m Retten - 15/16 - W" dataDxfId="69"/>
-    <tableColumn id="28" xr3:uid="{6BE7937E-D62D-47CD-95DE-1730304B0DF3}" name="100m Kombi - 15/16 - W" dataDxfId="68"/>
-    <tableColumn id="29" xr3:uid="{098BA5BE-5AF6-4187-89B6-534498F24C51}" name="100m Lifesaver -  15/16 - W" dataDxfId="67"/>
-    <tableColumn id="30" xr3:uid="{2A6822CF-143C-4BF7-A440-5777527BE512}" name="200m Superlifesaver -  15/16 - W" dataDxfId="66"/>
-    <tableColumn id="31" xr3:uid="{541C7145-CDEA-4E4E-9E7A-A4F05BA6C3E5}" name="200m Hindernis -  15/16 - W" dataDxfId="65"/>
-    <tableColumn id="32" xr3:uid="{342C4488-8C61-42E6-87A9-C75BD8EB7452}" name="50m Retten - 15/16 - M" dataDxfId="64"/>
-    <tableColumn id="33" xr3:uid="{857B1D46-7D20-47F7-AB9B-732D50346E32}" name="100m Retten - 15/16 - M" dataDxfId="63"/>
-    <tableColumn id="34" xr3:uid="{4C8A2EB4-804B-45F1-A768-9A6958957F8B}" name="100m Kombi -15/16 - M" dataDxfId="62"/>
-    <tableColumn id="35" xr3:uid="{26C75B4F-21EC-4EB0-A9A9-54BC80140672}" name="100m Lifesaver - 15/16 - M" dataDxfId="61"/>
-    <tableColumn id="36" xr3:uid="{DBBB2A23-1A06-429A-A5D1-A547EF5EC16F}" name="200m Superlifesaver - 15/16 - M" dataDxfId="60"/>
-    <tableColumn id="37" xr3:uid="{84061231-CAE5-427A-87F5-6DDBA99F77D2}" name="200m Hindernis - 15/16 - M" dataDxfId="59"/>
-    <tableColumn id="38" xr3:uid="{878CCA80-A742-4B3C-90C9-E93BB814201B}" name="50m Retten - 13/14 - W" dataDxfId="58"/>
-    <tableColumn id="39" xr3:uid="{A1F57102-61CF-4784-8DE2-0B8F32D5D699}" name="50m Retten mit Flossen - 13/14 - W" dataDxfId="57"/>
-    <tableColumn id="40" xr3:uid="{0F6BAF78-3D79-42A9-9FED-E6D0E335A920}" name="100m Hindernis - 13/14 - W" dataDxfId="56"/>
-    <tableColumn id="41" xr3:uid="{EB748A68-E10D-4D76-B315-8FDB3AC33C8D}" name="50m Retten - 13/14 - M" dataDxfId="55"/>
-    <tableColumn id="42" xr3:uid="{C7B04167-6430-40F0-9A0F-D0D0BE2F9C77}" name="50m Retten mit Flossen - 13/14 - M" dataDxfId="54"/>
-    <tableColumn id="43" xr3:uid="{48704BB7-A853-445A-8CDC-8D8F86C2B66A}" name="100m Hindernis - 13/14 - M" dataDxfId="53"/>
-    <tableColumn id="44" xr3:uid="{9605FE9A-F41C-4A5F-A59C-B7A9D45C460F}" name="50m Flossen - 12 - W" dataDxfId="52"/>
-    <tableColumn id="45" xr3:uid="{4C9DBF61-35B1-4BC2-8272-526E0AFAAFFB}" name="50m komb. Schwimmen - 12 - W" dataDxfId="51"/>
-    <tableColumn id="46" xr3:uid="{CF433C95-C272-48F9-98CD-7E3C8DBB6F2C}" name="50m Hindernis - 12 - W" dataDxfId="50"/>
-    <tableColumn id="47" xr3:uid="{FADB7411-DB43-4B14-B9E8-D74CA1BA18B8}" name="50m Flossen - 12 - M" dataDxfId="49"/>
-    <tableColumn id="48" xr3:uid="{02936F84-1D82-48AC-8D7C-6D2954D68A06}" name="50m komb. Schwimmen - 12 - M" dataDxfId="48"/>
-    <tableColumn id="49" xr3:uid="{7FD9BD11-0597-4E07-8DA5-DB53384197F5}" name="50m Hindernis - 12 - M" dataDxfId="47"/>
+    <tableColumn id="13" xr3:uid="{5A5E9873-0C5F-4508-AF6B-4974E0526D84}" name="200m Hindernis - offen - M" dataDxfId="110"/>
+    <tableColumn id="14" xr3:uid="{FA907992-7FCE-4CAD-8CF2-F5BEBC9B3756}" name="50m Retten - 17/18 - W" dataDxfId="109"/>
+    <tableColumn id="15" xr3:uid="{76B63DC0-CB67-48F4-9B5A-D22902F59334}" name="100m Retten - 17/18 - W" dataDxfId="108"/>
+    <tableColumn id="16" xr3:uid="{614A2419-51B1-44C0-8469-ADBFB078B81A}" name="100m Kombi -17/18 - W" dataDxfId="107"/>
+    <tableColumn id="17" xr3:uid="{2EC953EE-367D-4524-A25E-8DE3B8168E34}" name="100m Lifesaver - 17/18 - W" dataDxfId="106"/>
+    <tableColumn id="18" xr3:uid="{25711867-9BD7-4197-9094-A21392411249}" name="200m Superlifesaver - 17/18 - W" dataDxfId="105"/>
+    <tableColumn id="19" xr3:uid="{262DB142-CFB1-45C3-9332-7273CACD1B62}" name="200m Hindernis - 17/18 - W" dataDxfId="104"/>
+    <tableColumn id="20" xr3:uid="{938BA45A-8244-4637-8A14-DF49CD91A945}" name="50m Retten - 17/18 - M" dataDxfId="103"/>
+    <tableColumn id="21" xr3:uid="{737E28D8-900F-4A98-95FE-EE7B0AFDEE90}" name="100m Retten - 17/18 - M" dataDxfId="102"/>
+    <tableColumn id="22" xr3:uid="{330BD3A8-061C-45E2-ADDB-40C2F346772F}" name="100m Kombi - 17/18 - M" dataDxfId="101"/>
+    <tableColumn id="23" xr3:uid="{0CADDE90-A167-4E1D-8D33-8624E5E1A4E2}" name="100m Lifesaver - 17/18 - M" dataDxfId="100"/>
+    <tableColumn id="24" xr3:uid="{FCF9F42C-1291-4985-9D37-B9DE2DAA5DCB}" name="200m Superlifesaver - 17/18 - M" dataDxfId="99"/>
+    <tableColumn id="25" xr3:uid="{4E5397B2-F924-4F48-AE69-AF6D650AF88D}" name="200m Hindernis - 17/18 - M" dataDxfId="98"/>
+    <tableColumn id="26" xr3:uid="{0A78315A-BFDC-43EE-A66F-48B301F66508}" name="50m Retten - 15/16 - W" dataDxfId="97"/>
+    <tableColumn id="27" xr3:uid="{D3FCF8BD-6C76-450D-80C0-CC0519A79731}" name="100m Retten - 15/16 - W" dataDxfId="96"/>
+    <tableColumn id="28" xr3:uid="{6BE7937E-D62D-47CD-95DE-1730304B0DF3}" name="100m Kombi - 15/16 - W" dataDxfId="95"/>
+    <tableColumn id="29" xr3:uid="{098BA5BE-5AF6-4187-89B6-534498F24C51}" name="100m Lifesaver -  15/16 - W" dataDxfId="94"/>
+    <tableColumn id="30" xr3:uid="{2A6822CF-143C-4BF7-A440-5777527BE512}" name="200m Superlifesaver -  15/16 - W" dataDxfId="93"/>
+    <tableColumn id="31" xr3:uid="{541C7145-CDEA-4E4E-9E7A-A4F05BA6C3E5}" name="200m Hindernis -  15/16 - W" dataDxfId="92"/>
+    <tableColumn id="32" xr3:uid="{342C4488-8C61-42E6-87A9-C75BD8EB7452}" name="50m Retten - 15/16 - M" dataDxfId="91"/>
+    <tableColumn id="33" xr3:uid="{857B1D46-7D20-47F7-AB9B-732D50346E32}" name="100m Retten - 15/16 - M" dataDxfId="90"/>
+    <tableColumn id="34" xr3:uid="{4C8A2EB4-804B-45F1-A768-9A6958957F8B}" name="100m Kombi -15/16 - M" dataDxfId="89"/>
+    <tableColumn id="35" xr3:uid="{26C75B4F-21EC-4EB0-A9A9-54BC80140672}" name="100m Lifesaver - 15/16 - M" dataDxfId="88"/>
+    <tableColumn id="36" xr3:uid="{DBBB2A23-1A06-429A-A5D1-A547EF5EC16F}" name="200m Superlifesaver - 15/16 - M" dataDxfId="87"/>
+    <tableColumn id="37" xr3:uid="{84061231-CAE5-427A-87F5-6DDBA99F77D2}" name="200m Hindernis - 15/16 - M" dataDxfId="86"/>
+    <tableColumn id="38" xr3:uid="{878CCA80-A742-4B3C-90C9-E93BB814201B}" name="50m Retten - 13/14 - W" dataDxfId="85"/>
+    <tableColumn id="39" xr3:uid="{A1F57102-61CF-4784-8DE2-0B8F32D5D699}" name="50m Retten mit Flossen - 13/14 - W" dataDxfId="84"/>
+    <tableColumn id="40" xr3:uid="{0F6BAF78-3D79-42A9-9FED-E6D0E335A920}" name="100m Hindernis - 13/14 - W" dataDxfId="83"/>
+    <tableColumn id="41" xr3:uid="{EB748A68-E10D-4D76-B315-8FDB3AC33C8D}" name="50m Retten - 13/14 - M" dataDxfId="82"/>
+    <tableColumn id="42" xr3:uid="{C7B04167-6430-40F0-9A0F-D0D0BE2F9C77}" name="50m Retten mit Flossen - 13/14 - M" dataDxfId="81"/>
+    <tableColumn id="43" xr3:uid="{48704BB7-A853-445A-8CDC-8D8F86C2B66A}" name="100m Hindernis - 13/14 - M" dataDxfId="80"/>
+    <tableColumn id="44" xr3:uid="{9605FE9A-F41C-4A5F-A59C-B7A9D45C460F}" name="50m Flossen - 12 - W" dataDxfId="79"/>
+    <tableColumn id="45" xr3:uid="{4C9DBF61-35B1-4BC2-8272-526E0AFAAFFB}" name="50m komb. Schwimmen - 12 - W" dataDxfId="78"/>
+    <tableColumn id="46" xr3:uid="{CF433C95-C272-48F9-98CD-7E3C8DBB6F2C}" name="50m Hindernis - 12 - W" dataDxfId="77"/>
+    <tableColumn id="47" xr3:uid="{FADB7411-DB43-4B14-B9E8-D74CA1BA18B8}" name="50m Flossen - 12 - M" dataDxfId="76"/>
+    <tableColumn id="48" xr3:uid="{02936F84-1D82-48AC-8D7C-6D2954D68A06}" name="50m komb. Schwimmen - 12 - M" dataDxfId="75"/>
+    <tableColumn id="49" xr3:uid="{7FD9BD11-0597-4E07-8DA5-DB53384197F5}" name="50m Hindernis - 12 - M" dataDxfId="74"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4234D44E-A2BE-4790-B589-1A8CC19B714E}" name="WR_Youth" displayName="WR_Youth" ref="A4:M31" totalsRowShown="0" headerRowDxfId="46" dataDxfId="44" headerRowBorderDxfId="45" tableBorderDxfId="43">
-  <autoFilter ref="A4:M31" xr:uid="{4234D44E-A2BE-4790-B589-1A8CC19B714E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4234D44E-A2BE-4790-B589-1A8CC19B714E}" name="WR_Youth" displayName="WR_Youth" ref="A4:M32" totalsRowShown="0" headerRowDxfId="73" dataDxfId="71" headerRowBorderDxfId="72" tableBorderDxfId="70">
+  <autoFilter ref="A4:M32" xr:uid="{4234D44E-A2BE-4790-B589-1A8CC19B714E}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{848E691A-41B0-42DD-B122-FB6DF43CB3EF}" name="WR-Youth" dataDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{2FE43F18-485B-46A9-8946-FBC5FDAE5A8E}" name="50m Retten" dataDxfId="41"/>
-    <tableColumn id="3" xr3:uid="{CA5C3ABF-02E6-442B-868B-95B293B231D3}" name="100m Retten" dataDxfId="40"/>
-    <tableColumn id="4" xr3:uid="{7A6BBA52-2145-464D-8C04-B2CCFC1A90DC}" name="100m Kombi" dataDxfId="39"/>
-    <tableColumn id="5" xr3:uid="{21F420C9-E788-49EE-88F6-E37963ED31CF}" name="100m Lifesaver" dataDxfId="38"/>
-    <tableColumn id="6" xr3:uid="{CB87B7CD-8A9C-4775-A4D7-4D267F43FD1A}" name="200m Superlifesaver" dataDxfId="37"/>
-    <tableColumn id="7" xr3:uid="{2DC7F290-B564-4851-85AE-D211DA701B32}" name="200m Hindernis" dataDxfId="36"/>
-    <tableColumn id="8" xr3:uid="{8112783D-8796-4D6A-8414-AC675D745697}" name="50m Retten2" dataDxfId="35"/>
-    <tableColumn id="9" xr3:uid="{4E818CD4-8725-495D-9D1D-1AFCED9181F5}" name="100m Retten2" dataDxfId="34"/>
-    <tableColumn id="10" xr3:uid="{28C05A91-E302-40A9-B50A-ECF997F129FC}" name="100m Kombi2" dataDxfId="33"/>
-    <tableColumn id="11" xr3:uid="{D56FB9F2-45BF-4EC9-A84C-8A5FB59F2F05}" name="100m Lifesaver2" dataDxfId="32"/>
-    <tableColumn id="12" xr3:uid="{540169C0-2A40-4794-A872-F7DF8A887BF2}" name="200m Superlifesaver2" dataDxfId="31"/>
-    <tableColumn id="13" xr3:uid="{D104CB67-B55A-4C81-87E5-0AC758DD22A4}" name="200m Hindernis2" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{848E691A-41B0-42DD-B122-FB6DF43CB3EF}" name="WR-Youth" dataDxfId="69"/>
+    <tableColumn id="2" xr3:uid="{2FE43F18-485B-46A9-8946-FBC5FDAE5A8E}" name="50m Retten" dataDxfId="68"/>
+    <tableColumn id="3" xr3:uid="{CA5C3ABF-02E6-442B-868B-95B293B231D3}" name="100m Retten" dataDxfId="67"/>
+    <tableColumn id="4" xr3:uid="{7A6BBA52-2145-464D-8C04-B2CCFC1A90DC}" name="100m Kombi" dataDxfId="66"/>
+    <tableColumn id="5" xr3:uid="{21F420C9-E788-49EE-88F6-E37963ED31CF}" name="100m Lifesaver" dataDxfId="65"/>
+    <tableColumn id="6" xr3:uid="{CB87B7CD-8A9C-4775-A4D7-4D267F43FD1A}" name="200m Superlifesaver" dataDxfId="64"/>
+    <tableColumn id="7" xr3:uid="{2DC7F290-B564-4851-85AE-D211DA701B32}" name="200m Hindernis" dataDxfId="63"/>
+    <tableColumn id="8" xr3:uid="{8112783D-8796-4D6A-8414-AC675D745697}" name="50m Retten2" dataDxfId="62"/>
+    <tableColumn id="9" xr3:uid="{4E818CD4-8725-495D-9D1D-1AFCED9181F5}" name="100m Retten2" dataDxfId="61"/>
+    <tableColumn id="10" xr3:uid="{28C05A91-E302-40A9-B50A-ECF997F129FC}" name="100m Kombi2" dataDxfId="60"/>
+    <tableColumn id="11" xr3:uid="{D56FB9F2-45BF-4EC9-A84C-8A5FB59F2F05}" name="100m Lifesaver2" dataDxfId="59"/>
+    <tableColumn id="12" xr3:uid="{540169C0-2A40-4794-A872-F7DF8A887BF2}" name="200m Superlifesaver2" dataDxfId="58"/>
+    <tableColumn id="13" xr3:uid="{D104CB67-B55A-4C81-87E5-0AC758DD22A4}" name="200m Hindernis2" dataDxfId="57"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E2D2F97B-7645-4066-8AB3-F35CF6E035EB}" name="WR_Open" displayName="WR_Open" ref="A4:M31" totalsRowShown="0" headerRowDxfId="29" headerRowBorderDxfId="28" tableBorderDxfId="27">
-  <autoFilter ref="A4:M31" xr:uid="{E2D2F97B-7645-4066-8AB3-F35CF6E035EB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E2D2F97B-7645-4066-8AB3-F35CF6E035EB}" name="WR_Open" displayName="WR_Open" ref="A4:M32" totalsRowShown="0" headerRowDxfId="56" headerRowBorderDxfId="55" tableBorderDxfId="54">
+  <autoFilter ref="A4:M32" xr:uid="{E2D2F97B-7645-4066-8AB3-F35CF6E035EB}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{AE73402B-B27E-4B29-8DCF-30B7FC1855EF}" name="WR-Open" dataDxfId="26">
+    <tableColumn id="1" xr3:uid="{AE73402B-B27E-4B29-8DCF-30B7FC1855EF}" name="WR-Open" dataDxfId="53">
       <calculatedColumnFormula>A4+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{EA3EAC1F-184E-4A28-B3E3-08DE12F138EF}" name="50m Retten" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{E0305A3F-6087-4F8C-8B64-153E1ACAA32E}" name="100m Retten" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{F0B7AC37-315E-49AA-855C-7955D2B43A76}" name="100m Kombi" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{B5E690AB-DB7D-4864-8916-89D2A68C4128}" name="100m Lifesaver" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{D89BAF4D-36AE-4C73-9320-9C5736F02F8A}" name="200m Superlifesaver" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{58AE7517-1A90-459F-A7D2-B95265D217E7}" name="200m Hindernis" dataDxfId="20"/>
-    <tableColumn id="8" xr3:uid="{13A189FB-E897-4A1F-A001-525F61E9CFFF}" name="50m Retten2" dataDxfId="19"/>
-    <tableColumn id="9" xr3:uid="{36418AC5-46B8-400F-BD2E-D329CF4F92CD}" name="100m Retten2" dataDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{EA3EAC1F-184E-4A28-B3E3-08DE12F138EF}" name="50m Retten" dataDxfId="52"/>
+    <tableColumn id="3" xr3:uid="{E0305A3F-6087-4F8C-8B64-153E1ACAA32E}" name="100m Retten" dataDxfId="51"/>
+    <tableColumn id="4" xr3:uid="{F0B7AC37-315E-49AA-855C-7955D2B43A76}" name="100m Kombi" dataDxfId="50"/>
+    <tableColumn id="5" xr3:uid="{B5E690AB-DB7D-4864-8916-89D2A68C4128}" name="100m Lifesaver" dataDxfId="49"/>
+    <tableColumn id="6" xr3:uid="{D89BAF4D-36AE-4C73-9320-9C5736F02F8A}" name="200m Superlifesaver" dataDxfId="48"/>
+    <tableColumn id="7" xr3:uid="{58AE7517-1A90-459F-A7D2-B95265D217E7}" name="200m Hindernis" dataDxfId="47"/>
+    <tableColumn id="8" xr3:uid="{13A189FB-E897-4A1F-A001-525F61E9CFFF}" name="50m Retten2" dataDxfId="46"/>
+    <tableColumn id="9" xr3:uid="{36418AC5-46B8-400F-BD2E-D329CF4F92CD}" name="100m Retten2" dataDxfId="45"/>
     <tableColumn id="10" xr3:uid="{06A35C2D-7313-472B-BC1F-4F2FB1D14782}" name="100m Kombi2"/>
     <tableColumn id="11" xr3:uid="{89966D0D-9131-4245-A7BE-1A7384D5ADA0}" name="100m Lifesaver2"/>
     <tableColumn id="12" xr3:uid="{D9D6CF56-869C-4DDE-9886-572D4E523A8F}" name="200m Superlifesaver2"/>
     <tableColumn id="13" xr3:uid="{18A5C8DC-8C8E-4F2D-BDD1-01D37942869A}" name="200m Hindernis2"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CF3D303A-A04B-42DD-A44E-CEB6CECB77A4}" name="DP_konfig" displayName="DP_konfig" ref="A1:T3" totalsRowShown="0" headerRowDxfId="26" dataDxfId="27">
+  <autoFilter ref="A1:T3" xr:uid="{CF3D303A-A04B-42DD-A44E-CEB6CECB77A4}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+    <filterColumn colId="8" hiddenButton="1"/>
+    <filterColumn colId="9" hiddenButton="1"/>
+    <filterColumn colId="10" hiddenButton="1"/>
+    <filterColumn colId="11" hiddenButton="1"/>
+    <filterColumn colId="12" hiddenButton="1"/>
+    <filterColumn colId="13" hiddenButton="1"/>
+    <filterColumn colId="14" hiddenButton="1"/>
+    <filterColumn colId="15" hiddenButton="1"/>
+    <filterColumn colId="16" hiddenButton="1"/>
+    <filterColumn colId="17" hiddenButton="1"/>
+    <filterColumn colId="18" hiddenButton="1"/>
+    <filterColumn colId="19" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="20">
+    <tableColumn id="1" xr3:uid="{58D628F0-061E-4A82-8362-CDB37A2E7C60}" name="Tabellen Name" dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{2F302F6C-F8AF-4FDE-AB08-6F30F9671015}" name="Geschlecht" dataDxfId="43"/>
+    <tableColumn id="3" xr3:uid="{4D91FBF9-386D-43DD-90D0-B49823FDB629}" name="Mindest alter" dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{4126AAC6-AF2F-446C-B4EA-D86ACFD9FAC2}" name="Maximales Alter" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{8A10890A-A299-4B09-AC72-0E9AE9238AF3}" name="Qualizeitraum anfang" dataDxfId="40"/>
+    <tableColumn id="6" xr3:uid="{FBCD1C13-FC82-429B-8DE1-0C5A455FDAB8}" name="Qualizeitraum Ende" dataDxfId="39"/>
+    <tableColumn id="7" xr3:uid="{1DCCAC9B-BC46-468E-A3CE-57576C2FF11D}" name="Letzter Wettkampf am" dataDxfId="38"/>
+    <tableColumn id="8" xr3:uid="{9A6E47EE-ABD8-4A1E-87D3-9D286E4C124F}" name="Wertung" dataDxfId="37"/>
+    <tableColumn id="9" xr3:uid="{09E848D2-ED17-49C7-9775-CBF17D20DFC0}" name="Landesverband" dataDxfId="36"/>
+    <tableColumn id="10" xr3:uid="{70ABB713-23F6-4FCF-920E-3CB0CD451446}" name="OMS" dataDxfId="35"/>
+    <tableColumn id="11" xr3:uid="{9C108A1C-E6AB-4C13-9C1D-0FA8944A39A3}" name="Pool-Länge" dataDxfId="34"/>
+    <tableColumn id="12" xr3:uid="{087948DD-430D-48F1-906D-4F4EF4B46053}" name="Regelwerk" dataDxfId="33"/>
+    <tableColumn id="13" xr3:uid="{BF42D9C0-F77D-4971-A67E-32B0246C72C3}" name="Referenz" dataDxfId="32"/>
+    <tableColumn id="19" xr3:uid="{AFFB84E8-B398-4E99-805B-9A247071A040}" name="Referenz Jahr" dataDxfId="24"/>
+    <tableColumn id="20" xr3:uid="{0A59A474-DFBB-4437-8EFF-70284AFD9934}" name="Mindest Punktzahl" dataDxfId="0"/>
+    <tableColumn id="14" xr3:uid="{443CD4F6-A2B2-480B-BB35-DCEEBC531727}" name="3-Kampf Regel" dataDxfId="31"/>
+    <tableColumn id="15" xr3:uid="{70116160-7666-42B1-92AC-FAC2620E6A60}" name="Anzahl Nominierte" dataDxfId="30"/>
+    <tableColumn id="16" xr3:uid="{0EFD0A46-D12B-4AB0-907C-08E5D9F282E0}" name="Anzahl Nachrücker" dataDxfId="29"/>
+    <tableColumn id="17" xr3:uid="{AA5430A0-8ED8-40E8-B7F8-DA25E4E8790F}" name="Seiten Anzahl" dataDxfId="28"/>
+    <tableColumn id="18" xr3:uid="{16F699D9-2741-43F3-AD5F-826A568EFEAC}" name="Absagen" dataDxfId="25"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -3650,7 +3894,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0519F5DB-31A0-4819-8E86-33B1F16466A6}">
   <dimension ref="A1:AW31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+    <sheetView topLeftCell="M1" workbookViewId="0">
       <selection activeCell="Y25" sqref="Y25"/>
     </sheetView>
   </sheetViews>
@@ -7269,52 +7513,52 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B5:G31">
-    <cfRule type="expression" dxfId="17" priority="15">
+    <cfRule type="expression" dxfId="23" priority="15">
       <formula>B5&lt;&gt;B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:M31">
-    <cfRule type="expression" dxfId="16" priority="14">
+    <cfRule type="expression" dxfId="22" priority="14">
       <formula>H5&lt;&gt;H4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N5:S31">
-    <cfRule type="expression" dxfId="15" priority="13">
+    <cfRule type="expression" dxfId="21" priority="13">
       <formula>N5&lt;&gt;N4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T5:Y31">
-    <cfRule type="expression" dxfId="14" priority="12">
+    <cfRule type="expression" dxfId="20" priority="12">
       <formula>T5&lt;&gt;T4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z5:AE31">
-    <cfRule type="expression" dxfId="13" priority="9">
+    <cfRule type="expression" dxfId="19" priority="9">
       <formula>Z5&lt;&gt;Z4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF5:AK31">
-    <cfRule type="expression" dxfId="12" priority="8">
+    <cfRule type="expression" dxfId="18" priority="8">
       <formula>AF5&lt;&gt;AF4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL5:AN31">
-    <cfRule type="expression" dxfId="11" priority="6">
+    <cfRule type="expression" dxfId="17" priority="6">
       <formula>AL5&lt;&gt;AL4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO5:AQ31">
-    <cfRule type="expression" dxfId="10" priority="5">
+    <cfRule type="expression" dxfId="16" priority="5">
       <formula>AO5&lt;&gt;AO4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR5:AT31">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="15" priority="2">
       <formula>AR5&lt;&gt;AR4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU5:AW31">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="14" priority="1">
       <formula>AU5&lt;&gt;AU4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7330,10 +7574,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EB2B168-68B3-410F-B4A6-8D511F9C32E0}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7529,7 +7773,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <f t="shared" ref="A6:A31" si="0">A5+1</f>
+        <f t="shared" ref="A6:A32" si="0">A5+1</f>
         <v>2001</v>
       </c>
       <c r="B6" s="10"/>
@@ -8283,25 +8527,77 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <f t="shared" si="0"/>
+        <v>2027</v>
+      </c>
+      <c r="B32" s="10">
+        <v>3.8287037037037033E-4</v>
+      </c>
+      <c r="C32" s="10">
+        <v>5.7094907407407409E-4</v>
+      </c>
+      <c r="D32" s="10">
+        <v>7.9976851851851845E-4</v>
+      </c>
+      <c r="E32" s="10">
+        <v>6.607638888888889E-4</v>
+      </c>
+      <c r="F32" s="10">
+        <v>1.6468749999999999E-3</v>
+      </c>
+      <c r="G32" s="12">
+        <v>1.4339120370370371E-3</v>
+      </c>
+      <c r="H32" s="10">
+        <v>3.3425925925925924E-4</v>
+      </c>
+      <c r="I32" s="10">
+        <v>5.2685185185185192E-4</v>
+      </c>
+      <c r="J32" s="10">
+        <v>6.9027777777777783E-4</v>
+      </c>
+      <c r="K32" s="10">
+        <v>5.7881944444444441E-4</v>
+      </c>
+      <c r="L32" s="10">
+        <v>1.4707175925925927E-3</v>
+      </c>
+      <c r="M32" s="10">
+        <v>1.3511574074074075E-3</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="B6:G6">
+    <cfRule type="expression" dxfId="13" priority="20">
+      <formula>B6&lt;&gt;B4</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B7:G31">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="12" priority="3">
       <formula>B7&lt;&gt;B6</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H6:M6">
+    <cfRule type="expression" dxfId="11" priority="22">
+      <formula>H6&lt;&gt;H4</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="H7:M31">
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="10" priority="4">
       <formula>H7&lt;&gt;H6</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6:G6">
-    <cfRule type="expression" dxfId="1" priority="18">
-      <formula>B6&lt;&gt;B4</formula>
+  <conditionalFormatting sqref="B32:G32">
+    <cfRule type="expression" dxfId="9" priority="1">
+      <formula>B32&lt;&gt;B31</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H6:M6">
-    <cfRule type="expression" dxfId="0" priority="20">
-      <formula>H6&lt;&gt;H4</formula>
+  <conditionalFormatting sqref="H32:M32">
+    <cfRule type="expression" dxfId="8" priority="2">
+      <formula>H32&lt;&gt;H31</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -8315,10 +8611,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5FFB6C-7DEA-4C95-82B5-1769BD3934D8}">
   <sheetPr codeName="Tabelle2"/>
-  <dimension ref="A1:M31"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9592,25 +9888,77 @@
         <v>1.2931712962962962E-3</v>
       </c>
     </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <f>A31+1</f>
+        <v>2027</v>
+      </c>
+      <c r="B32" s="10">
+        <v>3.6435185185185187E-4</v>
+      </c>
+      <c r="C32" s="10">
+        <v>5.7060185185185187E-4</v>
+      </c>
+      <c r="D32" s="10">
+        <v>7.3715277777777776E-4</v>
+      </c>
+      <c r="E32" s="10">
+        <v>6.2731481481481481E-4</v>
+      </c>
+      <c r="F32" s="10">
+        <v>1.5748842592592594E-3</v>
+      </c>
+      <c r="G32" s="12">
+        <v>1.4106481481481481E-3</v>
+      </c>
+      <c r="H32" s="10">
+        <v>3.1481481481481481E-4</v>
+      </c>
+      <c r="I32" s="10">
+        <v>5.0104166666666667E-4</v>
+      </c>
+      <c r="J32" s="10">
+        <v>6.648148148148148E-4</v>
+      </c>
+      <c r="K32" s="10">
+        <v>5.5185185185185187E-4</v>
+      </c>
+      <c r="L32" s="10">
+        <v>1.4233796296296295E-3</v>
+      </c>
+      <c r="M32" s="10">
+        <v>1.2931712962962962E-3</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="B6:G6">
+    <cfRule type="expression" dxfId="7" priority="19">
+      <formula>B6&lt;&gt;B4</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="B7:G31">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="6" priority="5">
       <formula>B7&lt;&gt;B6</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H6:M6">
+    <cfRule type="expression" dxfId="5" priority="20">
+      <formula>H6&lt;&gt;H4</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="H7:M31">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="4" priority="4">
       <formula>H7&lt;&gt;H6</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6:G6">
-    <cfRule type="expression" dxfId="3" priority="16">
-      <formula>B6&lt;&gt;B4</formula>
+  <conditionalFormatting sqref="B32:G32">
+    <cfRule type="expression" dxfId="2" priority="2">
+      <formula>B32&lt;&gt;B31</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H6:M6">
-    <cfRule type="expression" dxfId="2" priority="17">
-      <formula>H6&lt;&gt;H4</formula>
+  <conditionalFormatting sqref="H32:M32">
+    <cfRule type="expression" dxfId="1" priority="1">
+      <formula>H32&lt;&gt;H31</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -9622,9 +9970,229 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{620E427F-1458-41E5-8334-8536EBB7542D}">
+  <sheetPr>
+    <tabColor theme="5"/>
+  </sheetPr>
+  <dimension ref="A1:T3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="15" max="15" width="19" customWidth="1"/>
+    <col min="16" max="16" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="47.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:20" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="63" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="63" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" s="63" t="s">
+        <v>163</v>
+      </c>
+      <c r="D1" s="63" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="63" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1" s="63" t="s">
+        <v>167</v>
+      </c>
+      <c r="G1" s="63" t="s">
+        <v>168</v>
+      </c>
+      <c r="H1" s="63" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="63" t="s">
+        <v>169</v>
+      </c>
+      <c r="J1" s="63" t="s">
+        <v>171</v>
+      </c>
+      <c r="K1" s="63" t="s">
+        <v>170</v>
+      </c>
+      <c r="L1" s="63" t="s">
+        <v>172</v>
+      </c>
+      <c r="M1" s="63" t="s">
+        <v>173</v>
+      </c>
+      <c r="N1" s="63" t="s">
+        <v>190</v>
+      </c>
+      <c r="O1" s="63" t="s">
+        <v>192</v>
+      </c>
+      <c r="P1" s="63" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q1" s="63" t="s">
+        <v>175</v>
+      </c>
+      <c r="R1" s="63" t="s">
+        <v>176</v>
+      </c>
+      <c r="S1" s="63" t="s">
+        <v>177</v>
+      </c>
+      <c r="T1" s="63" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="62" t="s">
+        <v>162</v>
+      </c>
+      <c r="B2" s="62" t="s">
+        <v>165</v>
+      </c>
+      <c r="C2" s="62">
+        <v>15</v>
+      </c>
+      <c r="D2" s="62">
+        <v>50</v>
+      </c>
+      <c r="E2" s="62" t="s">
+        <v>182</v>
+      </c>
+      <c r="F2" s="62" t="s">
+        <v>183</v>
+      </c>
+      <c r="G2" s="62" t="s">
+        <v>184</v>
+      </c>
+      <c r="H2" s="62" t="s">
+        <v>178</v>
+      </c>
+      <c r="I2" s="62" t="s">
+        <v>179</v>
+      </c>
+      <c r="J2" s="62" t="s">
+        <v>180</v>
+      </c>
+      <c r="K2" s="62"/>
+      <c r="L2" s="62"/>
+      <c r="M2" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="62" t="s">
+        <v>191</v>
+      </c>
+      <c r="O2" s="62">
+        <v>0</v>
+      </c>
+      <c r="P2" s="62" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q2" s="62">
+        <v>6</v>
+      </c>
+      <c r="R2" s="62">
+        <v>2</v>
+      </c>
+      <c r="S2" s="62">
+        <v>10</v>
+      </c>
+      <c r="T2" s="62" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="62" t="s">
+        <v>186</v>
+      </c>
+      <c r="B3" s="62" t="s">
+        <v>187</v>
+      </c>
+      <c r="C3" s="62">
+        <v>15</v>
+      </c>
+      <c r="D3" s="62">
+        <v>50</v>
+      </c>
+      <c r="E3" s="62" t="s">
+        <v>182</v>
+      </c>
+      <c r="F3" s="62" t="s">
+        <v>183</v>
+      </c>
+      <c r="G3" s="62" t="s">
+        <v>184</v>
+      </c>
+      <c r="H3" s="62" t="s">
+        <v>178</v>
+      </c>
+      <c r="I3" s="62" t="s">
+        <v>179</v>
+      </c>
+      <c r="J3" s="62" t="s">
+        <v>180</v>
+      </c>
+      <c r="K3" s="62"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="62" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="62" t="s">
+        <v>191</v>
+      </c>
+      <c r="O3" s="62">
+        <v>0</v>
+      </c>
+      <c r="P3" s="62" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q3" s="62">
+        <v>6</v>
+      </c>
+      <c r="R3" s="62">
+        <v>2</v>
+      </c>
+      <c r="S3" s="62">
+        <v>10</v>
+      </c>
+      <c r="T3" s="62" t="s">
+        <v>188</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3E1FA05-76A3-4AE3-B1B5-E78B06AE489F}">
   <sheetPr codeName="Tabelle3">
-    <tabColor theme="4"/>
+    <tabColor theme="1"/>
   </sheetPr>
   <dimension ref="A1:N37"/>
   <sheetViews>
@@ -10382,7 +10950,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7831D901-68D8-4F92-82B6-BCB1A3899285}">
   <sheetPr codeName="Tabelle4">
     <tabColor theme="4"/>
@@ -11178,13 +11746,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{453761C1-FFCA-45E5-8C71-AB7C914C935B}">
-  <sheetPr codeName="Tabelle5"/>
+  <sheetPr codeName="Tabelle5">
+    <tabColor theme="4"/>
+  </sheetPr>
   <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Test dynamischer Tabellen Code (KOMPLETTE DP.js) Ändernuf
</commit_message>
<xml_diff>
--- a/web/utilities/records_kriterien.xlsx
+++ b/web/utilities/records_kriterien.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgna\Documents\GitHub\Lifesaving_Baden\web\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1243BF90-10B2-48AB-B5CF-809E1DCA4F6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{282C1C67-14DC-4A9F-898B-2B09FDAA21C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
   </bookViews>
@@ -216,7 +216,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="196">
   <si>
     <t>50m Retten</t>
   </si>
@@ -795,6 +795,15 @@
   </si>
   <si>
     <t>Mindest Punktzahl</t>
+  </si>
+  <si>
+    <t>1.11.Jahr - 2</t>
+  </si>
+  <si>
+    <t>30.10.Jahr - 1</t>
+  </si>
+  <si>
+    <t>1.1.Jahr - 1</t>
   </si>
 </sst>
 </file>
@@ -1227,6 +1236,12 @@
     <xf numFmtId="0" fontId="14" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1236,35 +1251,11 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="123">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
-    </dxf>
+  <dxfs count="118">
     <dxf>
       <font>
         <color theme="6"/>
@@ -1278,16 +1269,6 @@
     <dxf>
       <font>
         <color theme="4"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6"/>
       </font>
     </dxf>
     <dxf>
@@ -1372,7 +1353,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1427,6 +1408,9 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3420,102 +3404,102 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2C5E83EE-6B6F-478A-9C90-A846A1A76536}" name="WR_Open4" displayName="WR_Open4" ref="A4:AW31" totalsRowShown="0" headerRowDxfId="122" headerRowBorderDxfId="121" tableBorderDxfId="120">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2C5E83EE-6B6F-478A-9C90-A846A1A76536}" name="WR_Open4" displayName="WR_Open4" ref="A4:AW31" totalsRowShown="0" headerRowDxfId="117" headerRowBorderDxfId="116" tableBorderDxfId="115">
   <autoFilter ref="A4:AW31" xr:uid="{2C5E83EE-6B6F-478A-9C90-A846A1A76536}"/>
   <tableColumns count="49">
-    <tableColumn id="1" xr3:uid="{7C0C4105-A61A-4B8D-9129-EDC4F18765AF}" name="WR-Open" dataDxfId="119">
+    <tableColumn id="1" xr3:uid="{7C0C4105-A61A-4B8D-9129-EDC4F18765AF}" name="WR-Open" dataDxfId="114">
       <calculatedColumnFormula>A4+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{516F5612-F85F-413F-9012-E235F415E34B}" name="50m Retten - offen - W" dataDxfId="118"/>
-    <tableColumn id="3" xr3:uid="{BC9ACAC9-0D45-42FD-B596-D19FBE3A4D83}" name="100m Retten - offen - W" dataDxfId="117"/>
-    <tableColumn id="4" xr3:uid="{CB6DBE59-EB65-43F0-93E7-0BDC3F82832B}" name="100m Kombi - offen - W" dataDxfId="116"/>
-    <tableColumn id="5" xr3:uid="{AA603C60-6831-4C14-A8CD-0AA050DA7551}" name="100m Lifesaver - offen - W" dataDxfId="115"/>
-    <tableColumn id="6" xr3:uid="{7920F147-7717-4582-940A-2610F7D310CA}" name="200m Superlifesaver - offen - W" dataDxfId="114"/>
-    <tableColumn id="7" xr3:uid="{04E21F1D-AC8D-4A1B-9B43-59B8F7901673}" name="200m Hindernis - offen - W" dataDxfId="113"/>
-    <tableColumn id="8" xr3:uid="{40E8A083-653A-48A8-9B37-0A2D850B7829}" name="50m Retten - offen - M" dataDxfId="112"/>
-    <tableColumn id="9" xr3:uid="{863824A9-134F-4189-BB14-225AE224FC44}" name="100m Retten - offen - M" dataDxfId="111"/>
+    <tableColumn id="2" xr3:uid="{516F5612-F85F-413F-9012-E235F415E34B}" name="50m Retten - offen - W" dataDxfId="113"/>
+    <tableColumn id="3" xr3:uid="{BC9ACAC9-0D45-42FD-B596-D19FBE3A4D83}" name="100m Retten - offen - W" dataDxfId="112"/>
+    <tableColumn id="4" xr3:uid="{CB6DBE59-EB65-43F0-93E7-0BDC3F82832B}" name="100m Kombi - offen - W" dataDxfId="111"/>
+    <tableColumn id="5" xr3:uid="{AA603C60-6831-4C14-A8CD-0AA050DA7551}" name="100m Lifesaver - offen - W" dataDxfId="110"/>
+    <tableColumn id="6" xr3:uid="{7920F147-7717-4582-940A-2610F7D310CA}" name="200m Superlifesaver - offen - W" dataDxfId="109"/>
+    <tableColumn id="7" xr3:uid="{04E21F1D-AC8D-4A1B-9B43-59B8F7901673}" name="200m Hindernis - offen - W" dataDxfId="108"/>
+    <tableColumn id="8" xr3:uid="{40E8A083-653A-48A8-9B37-0A2D850B7829}" name="50m Retten - offen - M" dataDxfId="107"/>
+    <tableColumn id="9" xr3:uid="{863824A9-134F-4189-BB14-225AE224FC44}" name="100m Retten - offen - M" dataDxfId="106"/>
     <tableColumn id="10" xr3:uid="{598FC6AE-DEA2-4475-9A35-CDCB8C81496A}" name="100m Kombi - offen - M"/>
     <tableColumn id="11" xr3:uid="{9FC50B37-0D51-422E-A268-A6506D4F3854}" name="100m Lifesaver - offen - M"/>
     <tableColumn id="12" xr3:uid="{B8D2552B-5D82-442A-98F0-E47D5C5F6728}" name="200m Superlifesaver - offen - M"/>
-    <tableColumn id="13" xr3:uid="{5A5E9873-0C5F-4508-AF6B-4974E0526D84}" name="200m Hindernis - offen - M" dataDxfId="110"/>
-    <tableColumn id="14" xr3:uid="{FA907992-7FCE-4CAD-8CF2-F5BEBC9B3756}" name="50m Retten - 17/18 - W" dataDxfId="109"/>
-    <tableColumn id="15" xr3:uid="{76B63DC0-CB67-48F4-9B5A-D22902F59334}" name="100m Retten - 17/18 - W" dataDxfId="108"/>
-    <tableColumn id="16" xr3:uid="{614A2419-51B1-44C0-8469-ADBFB078B81A}" name="100m Kombi -17/18 - W" dataDxfId="107"/>
-    <tableColumn id="17" xr3:uid="{2EC953EE-367D-4524-A25E-8DE3B8168E34}" name="100m Lifesaver - 17/18 - W" dataDxfId="106"/>
-    <tableColumn id="18" xr3:uid="{25711867-9BD7-4197-9094-A21392411249}" name="200m Superlifesaver - 17/18 - W" dataDxfId="105"/>
-    <tableColumn id="19" xr3:uid="{262DB142-CFB1-45C3-9332-7273CACD1B62}" name="200m Hindernis - 17/18 - W" dataDxfId="104"/>
-    <tableColumn id="20" xr3:uid="{938BA45A-8244-4637-8A14-DF49CD91A945}" name="50m Retten - 17/18 - M" dataDxfId="103"/>
-    <tableColumn id="21" xr3:uid="{737E28D8-900F-4A98-95FE-EE7B0AFDEE90}" name="100m Retten - 17/18 - M" dataDxfId="102"/>
-    <tableColumn id="22" xr3:uid="{330BD3A8-061C-45E2-ADDB-40C2F346772F}" name="100m Kombi - 17/18 - M" dataDxfId="101"/>
-    <tableColumn id="23" xr3:uid="{0CADDE90-A167-4E1D-8D33-8624E5E1A4E2}" name="100m Lifesaver - 17/18 - M" dataDxfId="100"/>
-    <tableColumn id="24" xr3:uid="{FCF9F42C-1291-4985-9D37-B9DE2DAA5DCB}" name="200m Superlifesaver - 17/18 - M" dataDxfId="99"/>
-    <tableColumn id="25" xr3:uid="{4E5397B2-F924-4F48-AE69-AF6D650AF88D}" name="200m Hindernis - 17/18 - M" dataDxfId="98"/>
-    <tableColumn id="26" xr3:uid="{0A78315A-BFDC-43EE-A66F-48B301F66508}" name="50m Retten - 15/16 - W" dataDxfId="97"/>
-    <tableColumn id="27" xr3:uid="{D3FCF8BD-6C76-450D-80C0-CC0519A79731}" name="100m Retten - 15/16 - W" dataDxfId="96"/>
-    <tableColumn id="28" xr3:uid="{6BE7937E-D62D-47CD-95DE-1730304B0DF3}" name="100m Kombi - 15/16 - W" dataDxfId="95"/>
-    <tableColumn id="29" xr3:uid="{098BA5BE-5AF6-4187-89B6-534498F24C51}" name="100m Lifesaver -  15/16 - W" dataDxfId="94"/>
-    <tableColumn id="30" xr3:uid="{2A6822CF-143C-4BF7-A440-5777527BE512}" name="200m Superlifesaver -  15/16 - W" dataDxfId="93"/>
-    <tableColumn id="31" xr3:uid="{541C7145-CDEA-4E4E-9E7A-A4F05BA6C3E5}" name="200m Hindernis -  15/16 - W" dataDxfId="92"/>
-    <tableColumn id="32" xr3:uid="{342C4488-8C61-42E6-87A9-C75BD8EB7452}" name="50m Retten - 15/16 - M" dataDxfId="91"/>
-    <tableColumn id="33" xr3:uid="{857B1D46-7D20-47F7-AB9B-732D50346E32}" name="100m Retten - 15/16 - M" dataDxfId="90"/>
-    <tableColumn id="34" xr3:uid="{4C8A2EB4-804B-45F1-A768-9A6958957F8B}" name="100m Kombi -15/16 - M" dataDxfId="89"/>
-    <tableColumn id="35" xr3:uid="{26C75B4F-21EC-4EB0-A9A9-54BC80140672}" name="100m Lifesaver - 15/16 - M" dataDxfId="88"/>
-    <tableColumn id="36" xr3:uid="{DBBB2A23-1A06-429A-A5D1-A547EF5EC16F}" name="200m Superlifesaver - 15/16 - M" dataDxfId="87"/>
-    <tableColumn id="37" xr3:uid="{84061231-CAE5-427A-87F5-6DDBA99F77D2}" name="200m Hindernis - 15/16 - M" dataDxfId="86"/>
-    <tableColumn id="38" xr3:uid="{878CCA80-A742-4B3C-90C9-E93BB814201B}" name="50m Retten - 13/14 - W" dataDxfId="85"/>
-    <tableColumn id="39" xr3:uid="{A1F57102-61CF-4784-8DE2-0B8F32D5D699}" name="50m Retten mit Flossen - 13/14 - W" dataDxfId="84"/>
-    <tableColumn id="40" xr3:uid="{0F6BAF78-3D79-42A9-9FED-E6D0E335A920}" name="100m Hindernis - 13/14 - W" dataDxfId="83"/>
-    <tableColumn id="41" xr3:uid="{EB748A68-E10D-4D76-B315-8FDB3AC33C8D}" name="50m Retten - 13/14 - M" dataDxfId="82"/>
-    <tableColumn id="42" xr3:uid="{C7B04167-6430-40F0-9A0F-D0D0BE2F9C77}" name="50m Retten mit Flossen - 13/14 - M" dataDxfId="81"/>
-    <tableColumn id="43" xr3:uid="{48704BB7-A853-445A-8CDC-8D8F86C2B66A}" name="100m Hindernis - 13/14 - M" dataDxfId="80"/>
-    <tableColumn id="44" xr3:uid="{9605FE9A-F41C-4A5F-A59C-B7A9D45C460F}" name="50m Flossen - 12 - W" dataDxfId="79"/>
-    <tableColumn id="45" xr3:uid="{4C9DBF61-35B1-4BC2-8272-526E0AFAAFFB}" name="50m komb. Schwimmen - 12 - W" dataDxfId="78"/>
-    <tableColumn id="46" xr3:uid="{CF433C95-C272-48F9-98CD-7E3C8DBB6F2C}" name="50m Hindernis - 12 - W" dataDxfId="77"/>
-    <tableColumn id="47" xr3:uid="{FADB7411-DB43-4B14-B9E8-D74CA1BA18B8}" name="50m Flossen - 12 - M" dataDxfId="76"/>
-    <tableColumn id="48" xr3:uid="{02936F84-1D82-48AC-8D7C-6D2954D68A06}" name="50m komb. Schwimmen - 12 - M" dataDxfId="75"/>
-    <tableColumn id="49" xr3:uid="{7FD9BD11-0597-4E07-8DA5-DB53384197F5}" name="50m Hindernis - 12 - M" dataDxfId="74"/>
+    <tableColumn id="13" xr3:uid="{5A5E9873-0C5F-4508-AF6B-4974E0526D84}" name="200m Hindernis - offen - M" dataDxfId="105"/>
+    <tableColumn id="14" xr3:uid="{FA907992-7FCE-4CAD-8CF2-F5BEBC9B3756}" name="50m Retten - 17/18 - W" dataDxfId="104"/>
+    <tableColumn id="15" xr3:uid="{76B63DC0-CB67-48F4-9B5A-D22902F59334}" name="100m Retten - 17/18 - W" dataDxfId="103"/>
+    <tableColumn id="16" xr3:uid="{614A2419-51B1-44C0-8469-ADBFB078B81A}" name="100m Kombi -17/18 - W" dataDxfId="102"/>
+    <tableColumn id="17" xr3:uid="{2EC953EE-367D-4524-A25E-8DE3B8168E34}" name="100m Lifesaver - 17/18 - W" dataDxfId="101"/>
+    <tableColumn id="18" xr3:uid="{25711867-9BD7-4197-9094-A21392411249}" name="200m Superlifesaver - 17/18 - W" dataDxfId="100"/>
+    <tableColumn id="19" xr3:uid="{262DB142-CFB1-45C3-9332-7273CACD1B62}" name="200m Hindernis - 17/18 - W" dataDxfId="99"/>
+    <tableColumn id="20" xr3:uid="{938BA45A-8244-4637-8A14-DF49CD91A945}" name="50m Retten - 17/18 - M" dataDxfId="98"/>
+    <tableColumn id="21" xr3:uid="{737E28D8-900F-4A98-95FE-EE7B0AFDEE90}" name="100m Retten - 17/18 - M" dataDxfId="97"/>
+    <tableColumn id="22" xr3:uid="{330BD3A8-061C-45E2-ADDB-40C2F346772F}" name="100m Kombi - 17/18 - M" dataDxfId="96"/>
+    <tableColumn id="23" xr3:uid="{0CADDE90-A167-4E1D-8D33-8624E5E1A4E2}" name="100m Lifesaver - 17/18 - M" dataDxfId="95"/>
+    <tableColumn id="24" xr3:uid="{FCF9F42C-1291-4985-9D37-B9DE2DAA5DCB}" name="200m Superlifesaver - 17/18 - M" dataDxfId="94"/>
+    <tableColumn id="25" xr3:uid="{4E5397B2-F924-4F48-AE69-AF6D650AF88D}" name="200m Hindernis - 17/18 - M" dataDxfId="93"/>
+    <tableColumn id="26" xr3:uid="{0A78315A-BFDC-43EE-A66F-48B301F66508}" name="50m Retten - 15/16 - W" dataDxfId="92"/>
+    <tableColumn id="27" xr3:uid="{D3FCF8BD-6C76-450D-80C0-CC0519A79731}" name="100m Retten - 15/16 - W" dataDxfId="91"/>
+    <tableColumn id="28" xr3:uid="{6BE7937E-D62D-47CD-95DE-1730304B0DF3}" name="100m Kombi - 15/16 - W" dataDxfId="90"/>
+    <tableColumn id="29" xr3:uid="{098BA5BE-5AF6-4187-89B6-534498F24C51}" name="100m Lifesaver -  15/16 - W" dataDxfId="89"/>
+    <tableColumn id="30" xr3:uid="{2A6822CF-143C-4BF7-A440-5777527BE512}" name="200m Superlifesaver -  15/16 - W" dataDxfId="88"/>
+    <tableColumn id="31" xr3:uid="{541C7145-CDEA-4E4E-9E7A-A4F05BA6C3E5}" name="200m Hindernis -  15/16 - W" dataDxfId="87"/>
+    <tableColumn id="32" xr3:uid="{342C4488-8C61-42E6-87A9-C75BD8EB7452}" name="50m Retten - 15/16 - M" dataDxfId="86"/>
+    <tableColumn id="33" xr3:uid="{857B1D46-7D20-47F7-AB9B-732D50346E32}" name="100m Retten - 15/16 - M" dataDxfId="85"/>
+    <tableColumn id="34" xr3:uid="{4C8A2EB4-804B-45F1-A768-9A6958957F8B}" name="100m Kombi -15/16 - M" dataDxfId="84"/>
+    <tableColumn id="35" xr3:uid="{26C75B4F-21EC-4EB0-A9A9-54BC80140672}" name="100m Lifesaver - 15/16 - M" dataDxfId="83"/>
+    <tableColumn id="36" xr3:uid="{DBBB2A23-1A06-429A-A5D1-A547EF5EC16F}" name="200m Superlifesaver - 15/16 - M" dataDxfId="82"/>
+    <tableColumn id="37" xr3:uid="{84061231-CAE5-427A-87F5-6DDBA99F77D2}" name="200m Hindernis - 15/16 - M" dataDxfId="81"/>
+    <tableColumn id="38" xr3:uid="{878CCA80-A742-4B3C-90C9-E93BB814201B}" name="50m Retten - 13/14 - W" dataDxfId="80"/>
+    <tableColumn id="39" xr3:uid="{A1F57102-61CF-4784-8DE2-0B8F32D5D699}" name="50m Retten mit Flossen - 13/14 - W" dataDxfId="79"/>
+    <tableColumn id="40" xr3:uid="{0F6BAF78-3D79-42A9-9FED-E6D0E335A920}" name="100m Hindernis - 13/14 - W" dataDxfId="78"/>
+    <tableColumn id="41" xr3:uid="{EB748A68-E10D-4D76-B315-8FDB3AC33C8D}" name="50m Retten - 13/14 - M" dataDxfId="77"/>
+    <tableColumn id="42" xr3:uid="{C7B04167-6430-40F0-9A0F-D0D0BE2F9C77}" name="50m Retten mit Flossen - 13/14 - M" dataDxfId="76"/>
+    <tableColumn id="43" xr3:uid="{48704BB7-A853-445A-8CDC-8D8F86C2B66A}" name="100m Hindernis - 13/14 - M" dataDxfId="75"/>
+    <tableColumn id="44" xr3:uid="{9605FE9A-F41C-4A5F-A59C-B7A9D45C460F}" name="50m Flossen - 12 - W" dataDxfId="74"/>
+    <tableColumn id="45" xr3:uid="{4C9DBF61-35B1-4BC2-8272-526E0AFAAFFB}" name="50m komb. Schwimmen - 12 - W" dataDxfId="73"/>
+    <tableColumn id="46" xr3:uid="{CF433C95-C272-48F9-98CD-7E3C8DBB6F2C}" name="50m Hindernis - 12 - W" dataDxfId="72"/>
+    <tableColumn id="47" xr3:uid="{FADB7411-DB43-4B14-B9E8-D74CA1BA18B8}" name="50m Flossen - 12 - M" dataDxfId="71"/>
+    <tableColumn id="48" xr3:uid="{02936F84-1D82-48AC-8D7C-6D2954D68A06}" name="50m komb. Schwimmen - 12 - M" dataDxfId="70"/>
+    <tableColumn id="49" xr3:uid="{7FD9BD11-0597-4E07-8DA5-DB53384197F5}" name="50m Hindernis - 12 - M" dataDxfId="69"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4234D44E-A2BE-4790-B589-1A8CC19B714E}" name="WR_Youth" displayName="WR_Youth" ref="A4:M32" totalsRowShown="0" headerRowDxfId="73" dataDxfId="71" headerRowBorderDxfId="72" tableBorderDxfId="70">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4234D44E-A2BE-4790-B589-1A8CC19B714E}" name="WR_Youth" displayName="WR_Youth" ref="A4:M32" totalsRowShown="0" headerRowDxfId="68" dataDxfId="66" headerRowBorderDxfId="67" tableBorderDxfId="65">
   <autoFilter ref="A4:M32" xr:uid="{4234D44E-A2BE-4790-B589-1A8CC19B714E}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{848E691A-41B0-42DD-B122-FB6DF43CB3EF}" name="WR-Youth" dataDxfId="69"/>
-    <tableColumn id="2" xr3:uid="{2FE43F18-485B-46A9-8946-FBC5FDAE5A8E}" name="50m Retten" dataDxfId="68"/>
-    <tableColumn id="3" xr3:uid="{CA5C3ABF-02E6-442B-868B-95B293B231D3}" name="100m Retten" dataDxfId="67"/>
-    <tableColumn id="4" xr3:uid="{7A6BBA52-2145-464D-8C04-B2CCFC1A90DC}" name="100m Kombi" dataDxfId="66"/>
-    <tableColumn id="5" xr3:uid="{21F420C9-E788-49EE-88F6-E37963ED31CF}" name="100m Lifesaver" dataDxfId="65"/>
-    <tableColumn id="6" xr3:uid="{CB87B7CD-8A9C-4775-A4D7-4D267F43FD1A}" name="200m Superlifesaver" dataDxfId="64"/>
-    <tableColumn id="7" xr3:uid="{2DC7F290-B564-4851-85AE-D211DA701B32}" name="200m Hindernis" dataDxfId="63"/>
-    <tableColumn id="8" xr3:uid="{8112783D-8796-4D6A-8414-AC675D745697}" name="50m Retten2" dataDxfId="62"/>
-    <tableColumn id="9" xr3:uid="{4E818CD4-8725-495D-9D1D-1AFCED9181F5}" name="100m Retten2" dataDxfId="61"/>
-    <tableColumn id="10" xr3:uid="{28C05A91-E302-40A9-B50A-ECF997F129FC}" name="100m Kombi2" dataDxfId="60"/>
-    <tableColumn id="11" xr3:uid="{D56FB9F2-45BF-4EC9-A84C-8A5FB59F2F05}" name="100m Lifesaver2" dataDxfId="59"/>
-    <tableColumn id="12" xr3:uid="{540169C0-2A40-4794-A872-F7DF8A887BF2}" name="200m Superlifesaver2" dataDxfId="58"/>
-    <tableColumn id="13" xr3:uid="{D104CB67-B55A-4C81-87E5-0AC758DD22A4}" name="200m Hindernis2" dataDxfId="57"/>
+    <tableColumn id="1" xr3:uid="{848E691A-41B0-42DD-B122-FB6DF43CB3EF}" name="WR-Youth" dataDxfId="64"/>
+    <tableColumn id="2" xr3:uid="{2FE43F18-485B-46A9-8946-FBC5FDAE5A8E}" name="50m Retten" dataDxfId="63"/>
+    <tableColumn id="3" xr3:uid="{CA5C3ABF-02E6-442B-868B-95B293B231D3}" name="100m Retten" dataDxfId="62"/>
+    <tableColumn id="4" xr3:uid="{7A6BBA52-2145-464D-8C04-B2CCFC1A90DC}" name="100m Kombi" dataDxfId="61"/>
+    <tableColumn id="5" xr3:uid="{21F420C9-E788-49EE-88F6-E37963ED31CF}" name="100m Lifesaver" dataDxfId="60"/>
+    <tableColumn id="6" xr3:uid="{CB87B7CD-8A9C-4775-A4D7-4D267F43FD1A}" name="200m Superlifesaver" dataDxfId="59"/>
+    <tableColumn id="7" xr3:uid="{2DC7F290-B564-4851-85AE-D211DA701B32}" name="200m Hindernis" dataDxfId="58"/>
+    <tableColumn id="8" xr3:uid="{8112783D-8796-4D6A-8414-AC675D745697}" name="50m Retten2" dataDxfId="57"/>
+    <tableColumn id="9" xr3:uid="{4E818CD4-8725-495D-9D1D-1AFCED9181F5}" name="100m Retten2" dataDxfId="56"/>
+    <tableColumn id="10" xr3:uid="{28C05A91-E302-40A9-B50A-ECF997F129FC}" name="100m Kombi2" dataDxfId="55"/>
+    <tableColumn id="11" xr3:uid="{D56FB9F2-45BF-4EC9-A84C-8A5FB59F2F05}" name="100m Lifesaver2" dataDxfId="54"/>
+    <tableColumn id="12" xr3:uid="{540169C0-2A40-4794-A872-F7DF8A887BF2}" name="200m Superlifesaver2" dataDxfId="53"/>
+    <tableColumn id="13" xr3:uid="{D104CB67-B55A-4C81-87E5-0AC758DD22A4}" name="200m Hindernis2" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E2D2F97B-7645-4066-8AB3-F35CF6E035EB}" name="WR_Open" displayName="WR_Open" ref="A4:M32" totalsRowShown="0" headerRowDxfId="56" headerRowBorderDxfId="55" tableBorderDxfId="54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E2D2F97B-7645-4066-8AB3-F35CF6E035EB}" name="WR_Open" displayName="WR_Open" ref="A4:M32" totalsRowShown="0" headerRowDxfId="51" headerRowBorderDxfId="50" tableBorderDxfId="49">
   <autoFilter ref="A4:M32" xr:uid="{E2D2F97B-7645-4066-8AB3-F35CF6E035EB}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{AE73402B-B27E-4B29-8DCF-30B7FC1855EF}" name="WR-Open" dataDxfId="53">
+    <tableColumn id="1" xr3:uid="{AE73402B-B27E-4B29-8DCF-30B7FC1855EF}" name="WR-Open" dataDxfId="48">
       <calculatedColumnFormula>A4+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{EA3EAC1F-184E-4A28-B3E3-08DE12F138EF}" name="50m Retten" dataDxfId="52"/>
-    <tableColumn id="3" xr3:uid="{E0305A3F-6087-4F8C-8B64-153E1ACAA32E}" name="100m Retten" dataDxfId="51"/>
-    <tableColumn id="4" xr3:uid="{F0B7AC37-315E-49AA-855C-7955D2B43A76}" name="100m Kombi" dataDxfId="50"/>
-    <tableColumn id="5" xr3:uid="{B5E690AB-DB7D-4864-8916-89D2A68C4128}" name="100m Lifesaver" dataDxfId="49"/>
-    <tableColumn id="6" xr3:uid="{D89BAF4D-36AE-4C73-9320-9C5736F02F8A}" name="200m Superlifesaver" dataDxfId="48"/>
-    <tableColumn id="7" xr3:uid="{58AE7517-1A90-459F-A7D2-B95265D217E7}" name="200m Hindernis" dataDxfId="47"/>
-    <tableColumn id="8" xr3:uid="{13A189FB-E897-4A1F-A001-525F61E9CFFF}" name="50m Retten2" dataDxfId="46"/>
-    <tableColumn id="9" xr3:uid="{36418AC5-46B8-400F-BD2E-D329CF4F92CD}" name="100m Retten2" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{EA3EAC1F-184E-4A28-B3E3-08DE12F138EF}" name="50m Retten" dataDxfId="47"/>
+    <tableColumn id="3" xr3:uid="{E0305A3F-6087-4F8C-8B64-153E1ACAA32E}" name="100m Retten" dataDxfId="46"/>
+    <tableColumn id="4" xr3:uid="{F0B7AC37-315E-49AA-855C-7955D2B43A76}" name="100m Kombi" dataDxfId="45"/>
+    <tableColumn id="5" xr3:uid="{B5E690AB-DB7D-4864-8916-89D2A68C4128}" name="100m Lifesaver" dataDxfId="44"/>
+    <tableColumn id="6" xr3:uid="{D89BAF4D-36AE-4C73-9320-9C5736F02F8A}" name="200m Superlifesaver" dataDxfId="43"/>
+    <tableColumn id="7" xr3:uid="{58AE7517-1A90-459F-A7D2-B95265D217E7}" name="200m Hindernis" dataDxfId="42"/>
+    <tableColumn id="8" xr3:uid="{13A189FB-E897-4A1F-A001-525F61E9CFFF}" name="50m Retten2" dataDxfId="41"/>
+    <tableColumn id="9" xr3:uid="{36418AC5-46B8-400F-BD2E-D329CF4F92CD}" name="100m Retten2" dataDxfId="40"/>
     <tableColumn id="10" xr3:uid="{06A35C2D-7313-472B-BC1F-4F2FB1D14782}" name="100m Kombi2"/>
     <tableColumn id="11" xr3:uid="{89966D0D-9131-4245-A7BE-1A7384D5ADA0}" name="100m Lifesaver2"/>
     <tableColumn id="12" xr3:uid="{D9D6CF56-869C-4DDE-9886-572D4E523A8F}" name="200m Superlifesaver2"/>
@@ -3526,7 +3510,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CF3D303A-A04B-42DD-A44E-CEB6CECB77A4}" name="DP_konfig" displayName="DP_konfig" ref="A1:T3" totalsRowShown="0" headerRowDxfId="26" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CF3D303A-A04B-42DD-A44E-CEB6CECB77A4}" name="DP_konfig" displayName="DP_konfig" ref="A1:T3" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
   <autoFilter ref="A1:T3" xr:uid="{CF3D303A-A04B-42DD-A44E-CEB6CECB77A4}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3550,26 +3534,26 @@
     <filterColumn colId="19" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{58D628F0-061E-4A82-8362-CDB37A2E7C60}" name="Tabellen Name" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{2F302F6C-F8AF-4FDE-AB08-6F30F9671015}" name="Geschlecht" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{4D91FBF9-386D-43DD-90D0-B49823FDB629}" name="Mindest alter" dataDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{4126AAC6-AF2F-446C-B4EA-D86ACFD9FAC2}" name="Maximales Alter" dataDxfId="41"/>
-    <tableColumn id="5" xr3:uid="{8A10890A-A299-4B09-AC72-0E9AE9238AF3}" name="Qualizeitraum anfang" dataDxfId="40"/>
-    <tableColumn id="6" xr3:uid="{FBCD1C13-FC82-429B-8DE1-0C5A455FDAB8}" name="Qualizeitraum Ende" dataDxfId="39"/>
-    <tableColumn id="7" xr3:uid="{1DCCAC9B-BC46-468E-A3CE-57576C2FF11D}" name="Letzter Wettkampf am" dataDxfId="38"/>
-    <tableColumn id="8" xr3:uid="{9A6E47EE-ABD8-4A1E-87D3-9D286E4C124F}" name="Wertung" dataDxfId="37"/>
-    <tableColumn id="9" xr3:uid="{09E848D2-ED17-49C7-9775-CBF17D20DFC0}" name="Landesverband" dataDxfId="36"/>
-    <tableColumn id="10" xr3:uid="{70ABB713-23F6-4FCF-920E-3CB0CD451446}" name="OMS" dataDxfId="35"/>
-    <tableColumn id="11" xr3:uid="{9C108A1C-E6AB-4C13-9C1D-0FA8944A39A3}" name="Pool-Länge" dataDxfId="34"/>
-    <tableColumn id="12" xr3:uid="{087948DD-430D-48F1-906D-4F4EF4B46053}" name="Regelwerk" dataDxfId="33"/>
-    <tableColumn id="13" xr3:uid="{BF42D9C0-F77D-4971-A67E-32B0246C72C3}" name="Referenz" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{58D628F0-061E-4A82-8362-CDB37A2E7C60}" name="Tabellen Name" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{2F302F6C-F8AF-4FDE-AB08-6F30F9671015}" name="Geschlecht" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{4D91FBF9-386D-43DD-90D0-B49823FDB629}" name="Mindest alter" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{4126AAC6-AF2F-446C-B4EA-D86ACFD9FAC2}" name="Maximales Alter" dataDxfId="34"/>
+    <tableColumn id="5" xr3:uid="{8A10890A-A299-4B09-AC72-0E9AE9238AF3}" name="Qualizeitraum anfang" dataDxfId="33"/>
+    <tableColumn id="6" xr3:uid="{FBCD1C13-FC82-429B-8DE1-0C5A455FDAB8}" name="Qualizeitraum Ende" dataDxfId="32"/>
+    <tableColumn id="7" xr3:uid="{1DCCAC9B-BC46-468E-A3CE-57576C2FF11D}" name="Letzter Wettkampf am" dataDxfId="31"/>
+    <tableColumn id="8" xr3:uid="{9A6E47EE-ABD8-4A1E-87D3-9D286E4C124F}" name="Wertung" dataDxfId="30"/>
+    <tableColumn id="9" xr3:uid="{09E848D2-ED17-49C7-9775-CBF17D20DFC0}" name="Landesverband" dataDxfId="29"/>
+    <tableColumn id="10" xr3:uid="{70ABB713-23F6-4FCF-920E-3CB0CD451446}" name="OMS" dataDxfId="28"/>
+    <tableColumn id="11" xr3:uid="{9C108A1C-E6AB-4C13-9C1D-0FA8944A39A3}" name="Pool-Länge" dataDxfId="27"/>
+    <tableColumn id="12" xr3:uid="{087948DD-430D-48F1-906D-4F4EF4B46053}" name="Regelwerk" dataDxfId="26"/>
+    <tableColumn id="13" xr3:uid="{BF42D9C0-F77D-4971-A67E-32B0246C72C3}" name="Referenz" dataDxfId="25"/>
     <tableColumn id="19" xr3:uid="{AFFB84E8-B398-4E99-805B-9A247071A040}" name="Referenz Jahr" dataDxfId="24"/>
-    <tableColumn id="20" xr3:uid="{0A59A474-DFBB-4437-8EFF-70284AFD9934}" name="Mindest Punktzahl" dataDxfId="0"/>
-    <tableColumn id="14" xr3:uid="{443CD4F6-A2B2-480B-BB35-DCEEBC531727}" name="3-Kampf Regel" dataDxfId="31"/>
-    <tableColumn id="15" xr3:uid="{70116160-7666-42B1-92AC-FAC2620E6A60}" name="Anzahl Nominierte" dataDxfId="30"/>
-    <tableColumn id="16" xr3:uid="{0EFD0A46-D12B-4AB0-907C-08E5D9F282E0}" name="Anzahl Nachrücker" dataDxfId="29"/>
-    <tableColumn id="17" xr3:uid="{AA5430A0-8ED8-40E8-B7F8-DA25E4E8790F}" name="Seiten Anzahl" dataDxfId="28"/>
-    <tableColumn id="18" xr3:uid="{16F699D9-2741-43F3-AD5F-826A568EFEAC}" name="Absagen" dataDxfId="25"/>
+    <tableColumn id="20" xr3:uid="{0A59A474-DFBB-4437-8EFF-70284AFD9934}" name="Mindest Punktzahl" dataDxfId="23"/>
+    <tableColumn id="14" xr3:uid="{443CD4F6-A2B2-480B-BB35-DCEEBC531727}" name="3-Kampf Regel" dataDxfId="22"/>
+    <tableColumn id="15" xr3:uid="{70116160-7666-42B1-92AC-FAC2620E6A60}" name="Anzahl Nominierte" dataDxfId="21"/>
+    <tableColumn id="16" xr3:uid="{0EFD0A46-D12B-4AB0-907C-08E5D9F282E0}" name="Anzahl Nachrücker" dataDxfId="20"/>
+    <tableColumn id="17" xr3:uid="{AA5430A0-8ED8-40E8-B7F8-DA25E4E8790F}" name="Seiten Anzahl" dataDxfId="19"/>
+    <tableColumn id="18" xr3:uid="{16F699D9-2741-43F3-AD5F-826A568EFEAC}" name="Absagen" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7513,52 +7497,52 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B5:G31">
-    <cfRule type="expression" dxfId="23" priority="15">
+    <cfRule type="expression" dxfId="17" priority="15">
       <formula>B5&lt;&gt;B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:M31">
-    <cfRule type="expression" dxfId="22" priority="14">
+    <cfRule type="expression" dxfId="16" priority="14">
       <formula>H5&lt;&gt;H4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N5:S31">
-    <cfRule type="expression" dxfId="21" priority="13">
+    <cfRule type="expression" dxfId="15" priority="13">
       <formula>N5&lt;&gt;N4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T5:Y31">
-    <cfRule type="expression" dxfId="20" priority="12">
+    <cfRule type="expression" dxfId="14" priority="12">
       <formula>T5&lt;&gt;T4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z5:AE31">
-    <cfRule type="expression" dxfId="19" priority="9">
+    <cfRule type="expression" dxfId="13" priority="9">
       <formula>Z5&lt;&gt;Z4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF5:AK31">
-    <cfRule type="expression" dxfId="18" priority="8">
+    <cfRule type="expression" dxfId="12" priority="8">
       <formula>AF5&lt;&gt;AF4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL5:AN31">
-    <cfRule type="expression" dxfId="17" priority="6">
+    <cfRule type="expression" dxfId="11" priority="6">
       <formula>AL5&lt;&gt;AL4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO5:AQ31">
-    <cfRule type="expression" dxfId="16" priority="5">
+    <cfRule type="expression" dxfId="10" priority="5">
       <formula>AO5&lt;&gt;AO4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR5:AT31">
-    <cfRule type="expression" dxfId="15" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>AR5&lt;&gt;AR4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU5:AW31">
-    <cfRule type="expression" dxfId="14" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>AU5&lt;&gt;AU4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8571,33 +8555,23 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B6:G6">
-    <cfRule type="expression" dxfId="13" priority="20">
+    <cfRule type="expression" dxfId="7" priority="20">
       <formula>B6&lt;&gt;B4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7:G31">
-    <cfRule type="expression" dxfId="12" priority="3">
+  <conditionalFormatting sqref="B7:G32">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>B7&lt;&gt;B6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:M6">
-    <cfRule type="expression" dxfId="11" priority="22">
+    <cfRule type="expression" dxfId="5" priority="22">
       <formula>H6&lt;&gt;H4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7:M31">
-    <cfRule type="expression" dxfId="10" priority="4">
+  <conditionalFormatting sqref="H7:M32">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>H7&lt;&gt;H6</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B32:G32">
-    <cfRule type="expression" dxfId="9" priority="1">
-      <formula>B32&lt;&gt;B31</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H32:M32">
-    <cfRule type="expression" dxfId="8" priority="2">
-      <formula>H32&lt;&gt;H31</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -9932,33 +9906,23 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B6:G6">
-    <cfRule type="expression" dxfId="7" priority="19">
+    <cfRule type="expression" dxfId="3" priority="19">
       <formula>B6&lt;&gt;B4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7:G31">
-    <cfRule type="expression" dxfId="6" priority="5">
+  <conditionalFormatting sqref="B7:G32">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>B7&lt;&gt;B6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:M6">
-    <cfRule type="expression" dxfId="5" priority="20">
+    <cfRule type="expression" dxfId="1" priority="20">
       <formula>H6&lt;&gt;H4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H7:M31">
-    <cfRule type="expression" dxfId="4" priority="4">
+  <conditionalFormatting sqref="H7:M32">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>H7&lt;&gt;H6</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B32:G32">
-    <cfRule type="expression" dxfId="2" priority="2">
-      <formula>B32&lt;&gt;B31</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H32:M32">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>H32&lt;&gt;H31</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -9976,8 +9940,8 @@
   </sheetPr>
   <dimension ref="A1:T3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10004,180 +9968,180 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="60" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="60" t="s">
         <v>164</v>
       </c>
-      <c r="C1" s="63" t="s">
+      <c r="C1" s="60" t="s">
         <v>163</v>
       </c>
-      <c r="D1" s="63" t="s">
+      <c r="D1" s="60" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="63" t="s">
+      <c r="E1" s="60" t="s">
         <v>166</v>
       </c>
-      <c r="F1" s="63" t="s">
+      <c r="F1" s="60" t="s">
         <v>167</v>
       </c>
-      <c r="G1" s="63" t="s">
+      <c r="G1" s="60" t="s">
         <v>168</v>
       </c>
-      <c r="H1" s="63" t="s">
+      <c r="H1" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="63" t="s">
+      <c r="I1" s="60" t="s">
         <v>169</v>
       </c>
-      <c r="J1" s="63" t="s">
+      <c r="J1" s="60" t="s">
         <v>171</v>
       </c>
-      <c r="K1" s="63" t="s">
+      <c r="K1" s="60" t="s">
         <v>170</v>
       </c>
-      <c r="L1" s="63" t="s">
+      <c r="L1" s="60" t="s">
         <v>172</v>
       </c>
-      <c r="M1" s="63" t="s">
+      <c r="M1" s="60" t="s">
         <v>173</v>
       </c>
-      <c r="N1" s="63" t="s">
+      <c r="N1" s="60" t="s">
         <v>190</v>
       </c>
-      <c r="O1" s="63" t="s">
+      <c r="O1" s="60" t="s">
         <v>192</v>
       </c>
-      <c r="P1" s="63" t="s">
+      <c r="P1" s="60" t="s">
         <v>174</v>
       </c>
-      <c r="Q1" s="63" t="s">
+      <c r="Q1" s="60" t="s">
         <v>175</v>
       </c>
-      <c r="R1" s="63" t="s">
+      <c r="R1" s="60" t="s">
         <v>176</v>
       </c>
-      <c r="S1" s="63" t="s">
+      <c r="S1" s="60" t="s">
         <v>177</v>
       </c>
-      <c r="T1" s="63" t="s">
+      <c r="T1" s="60" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="59" t="s">
         <v>162</v>
       </c>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="59" t="s">
         <v>165</v>
       </c>
-      <c r="C2" s="62">
+      <c r="C2" s="59">
         <v>15</v>
       </c>
-      <c r="D2" s="62">
+      <c r="D2" s="59">
         <v>50</v>
       </c>
-      <c r="E2" s="62" t="s">
+      <c r="E2" s="59" t="s">
+        <v>193</v>
+      </c>
+      <c r="F2" s="59" t="s">
+        <v>194</v>
+      </c>
+      <c r="G2" s="59" t="s">
+        <v>195</v>
+      </c>
+      <c r="H2" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="I2" s="59" t="s">
+        <v>179</v>
+      </c>
+      <c r="J2" s="59" t="s">
+        <v>180</v>
+      </c>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59"/>
+      <c r="M2" s="59" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="59" t="s">
+        <v>191</v>
+      </c>
+      <c r="O2" s="59">
+        <v>0</v>
+      </c>
+      <c r="P2" s="59" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q2" s="59">
+        <v>6</v>
+      </c>
+      <c r="R2" s="59">
+        <v>2</v>
+      </c>
+      <c r="S2" s="59">
+        <v>10</v>
+      </c>
+      <c r="T2" s="59" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="59" t="s">
+        <v>186</v>
+      </c>
+      <c r="B3" s="59" t="s">
+        <v>187</v>
+      </c>
+      <c r="C3" s="59">
+        <v>15</v>
+      </c>
+      <c r="D3" s="59">
+        <v>50</v>
+      </c>
+      <c r="E3" s="59" t="s">
         <v>182</v>
       </c>
-      <c r="F2" s="62" t="s">
+      <c r="F3" s="59" t="s">
         <v>183</v>
       </c>
-      <c r="G2" s="62" t="s">
+      <c r="G3" s="59" t="s">
         <v>184</v>
       </c>
-      <c r="H2" s="62" t="s">
+      <c r="H3" s="59" t="s">
         <v>178</v>
       </c>
-      <c r="I2" s="62" t="s">
+      <c r="I3" s="59" t="s">
         <v>179</v>
       </c>
-      <c r="J2" s="62" t="s">
+      <c r="J3" s="59" t="s">
         <v>180</v>
       </c>
-      <c r="K2" s="62"/>
-      <c r="L2" s="62"/>
-      <c r="M2" s="62" t="s">
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="62" t="s">
+      <c r="N3" s="59" t="s">
         <v>191</v>
       </c>
-      <c r="O2" s="62">
+      <c r="O3" s="59">
         <v>0</v>
       </c>
-      <c r="P2" s="62" t="s">
+      <c r="P3" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="Q2" s="62">
+      <c r="Q3" s="59">
         <v>6</v>
       </c>
-      <c r="R2" s="62">
+      <c r="R3" s="59">
         <v>2</v>
       </c>
-      <c r="S2" s="62">
+      <c r="S3" s="59">
         <v>10</v>
       </c>
-      <c r="T2" s="62" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="62" t="s">
-        <v>186</v>
-      </c>
-      <c r="B3" s="62" t="s">
-        <v>187</v>
-      </c>
-      <c r="C3" s="62">
-        <v>15</v>
-      </c>
-      <c r="D3" s="62">
-        <v>50</v>
-      </c>
-      <c r="E3" s="62" t="s">
-        <v>182</v>
-      </c>
-      <c r="F3" s="62" t="s">
-        <v>183</v>
-      </c>
-      <c r="G3" s="62" t="s">
-        <v>184</v>
-      </c>
-      <c r="H3" s="62" t="s">
-        <v>178</v>
-      </c>
-      <c r="I3" s="62" t="s">
-        <v>179</v>
-      </c>
-      <c r="J3" s="62" t="s">
-        <v>180</v>
-      </c>
-      <c r="K3" s="62"/>
-      <c r="L3" s="62"/>
-      <c r="M3" s="62" t="s">
-        <v>10</v>
-      </c>
-      <c r="N3" s="62" t="s">
-        <v>191</v>
-      </c>
-      <c r="O3" s="62">
-        <v>0</v>
-      </c>
-      <c r="P3" s="62" t="s">
-        <v>181</v>
-      </c>
-      <c r="Q3" s="62">
-        <v>6</v>
-      </c>
-      <c r="R3" s="62">
-        <v>2</v>
-      </c>
-      <c r="S3" s="62">
-        <v>10</v>
-      </c>
-      <c r="T3" s="62" t="s">
+      <c r="T3" s="59" t="s">
         <v>188</v>
       </c>
     </row>
@@ -10421,38 +10385,38 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="60" t="s">
+      <c r="A7" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="60"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="60"/>
-      <c r="L7" s="60"/>
-      <c r="M7" s="60"/>
-      <c r="N7" s="60"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="62"/>
+      <c r="K7" s="62"/>
+      <c r="L7" s="62"/>
+      <c r="M7" s="62"/>
+      <c r="N7" s="62"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="60"/>
-      <c r="B8" s="60"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="60"/>
-      <c r="L8" s="60"/>
-      <c r="M8" s="60"/>
-      <c r="N8" s="60"/>
+      <c r="A8" s="62"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="62"/>
+      <c r="L8" s="62"/>
+      <c r="M8" s="62"/>
+      <c r="N8" s="62"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
@@ -10617,38 +10581,38 @@
       <c r="N11" s="23"/>
     </row>
     <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="59" t="s">
+      <c r="A14" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="59"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="59"/>
-      <c r="F14" s="59"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
       <c r="G14"/>
-      <c r="H14" s="61" t="s">
+      <c r="H14" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="I14" s="61"/>
-      <c r="J14" s="61"/>
-      <c r="L14" s="61" t="s">
+      <c r="I14" s="63"/>
+      <c r="J14" s="63"/>
+      <c r="L14" s="63" t="s">
         <v>36</v>
       </c>
       <c r="M14"/>
       <c r="N14"/>
     </row>
     <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="59"/>
-      <c r="B15" s="59"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
+      <c r="A15" s="61"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="61"/>
       <c r="G15"/>
-      <c r="H15" s="61"/>
-      <c r="I15" s="61"/>
-      <c r="J15" s="61"/>
-      <c r="L15" s="61"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
+      <c r="L15" s="63"/>
       <c r="M15"/>
       <c r="N15"/>
     </row>
@@ -11182,38 +11146,38 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="60" t="s">
+      <c r="A7" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="60"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="60"/>
-      <c r="L7" s="60"/>
-      <c r="M7" s="60"/>
-      <c r="N7" s="60"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="62"/>
+      <c r="K7" s="62"/>
+      <c r="L7" s="62"/>
+      <c r="M7" s="62"/>
+      <c r="N7" s="62"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="60"/>
-      <c r="B8" s="60"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="60"/>
-      <c r="L8" s="60"/>
-      <c r="M8" s="60"/>
-      <c r="N8" s="60"/>
+      <c r="A8" s="62"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="62"/>
+      <c r="L8" s="62"/>
+      <c r="M8" s="62"/>
+      <c r="N8" s="62"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
@@ -11378,35 +11342,35 @@
       <c r="N11" s="23"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="59" t="s">
+      <c r="A14" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="59"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="59"/>
-      <c r="F14" s="59"/>
-      <c r="H14" s="61" t="s">
+      <c r="B14" s="61"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
+      <c r="H14" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="I14" s="61"/>
-      <c r="J14" s="61"/>
-      <c r="L14" s="61" t="s">
+      <c r="I14" s="63"/>
+      <c r="J14" s="63"/>
+      <c r="L14" s="63" t="s">
         <v>36</v>
       </c>
       <c r="M14"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="59"/>
-      <c r="B15" s="59"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="H15" s="61"/>
-      <c r="I15" s="61"/>
-      <c r="J15" s="61"/>
-      <c r="L15" s="61"/>
+      <c r="A15" s="61"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="61"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
+      <c r="L15" s="63"/>
       <c r="M15"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -11978,38 +11942,38 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="60" t="s">
+      <c r="A7" s="62" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="60"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="60"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="60"/>
-      <c r="L7" s="60"/>
-      <c r="M7" s="60"/>
-      <c r="N7" s="60"/>
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="62"/>
+      <c r="K7" s="62"/>
+      <c r="L7" s="62"/>
+      <c r="M7" s="62"/>
+      <c r="N7" s="62"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="60"/>
-      <c r="B8" s="60"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="60"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="60"/>
-      <c r="L8" s="60"/>
-      <c r="M8" s="60"/>
-      <c r="N8" s="60"/>
+      <c r="A8" s="62"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="62"/>
+      <c r="L8" s="62"/>
+      <c r="M8" s="62"/>
+      <c r="N8" s="62"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
@@ -12174,35 +12138,35 @@
       <c r="N11" s="23"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="59" t="s">
+      <c r="A14" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="59"/>
-      <c r="C14" s="59"/>
-      <c r="D14" s="59"/>
-      <c r="E14" s="59"/>
-      <c r="F14" s="59"/>
-      <c r="H14" s="61" t="s">
+      <c r="B14" s="61"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
+      <c r="H14" s="63" t="s">
         <v>35</v>
       </c>
-      <c r="I14" s="61"/>
-      <c r="J14" s="61"/>
-      <c r="L14" s="61" t="s">
+      <c r="I14" s="63"/>
+      <c r="J14" s="63"/>
+      <c r="L14" s="63" t="s">
         <v>36</v>
       </c>
       <c r="M14"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="59"/>
-      <c r="B15" s="59"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="H15" s="61"/>
-      <c r="I15" s="61"/>
-      <c r="J15" s="61"/>
-      <c r="L15" s="61"/>
+      <c r="A15" s="61"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="61"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
+      <c r="L15" s="63"/>
       <c r="M15"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Repaired + Record Kriterien 2025 right
</commit_message>
<xml_diff>
--- a/web/utilities/records_kriterien.xlsx
+++ b/web/utilities/records_kriterien.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgna\Documents\GitHub\Lifesaving_Baden\web\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07F7FFA-11B2-473A-B89F-401C2BD4DD5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4932DC8A-2985-496E-9091-6397CA6397CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
   </bookViews>
@@ -216,7 +216,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="194">
   <si>
     <t>50m Retten</t>
   </si>
@@ -761,15 +761,6 @@
     <t>Ja</t>
   </si>
   <si>
-    <t>1.11.Jahr - 1</t>
-  </si>
-  <si>
-    <t>30.10.Jahr</t>
-  </si>
-  <si>
-    <t>1.1.Jahr</t>
-  </si>
-  <si>
     <t>Absagen</t>
   </si>
   <si>
@@ -807,9 +798,6 @@
   </si>
   <si>
     <t>Mindest Disziplinen</t>
-  </si>
-  <si>
-    <t>3-Kampf</t>
   </si>
 </sst>
 </file>
@@ -9951,8 +9939,8 @@
   </sheetPr>
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10019,13 +10007,13 @@
         <v>172</v>
       </c>
       <c r="N1" s="60" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="O1" s="60" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="P1" s="60" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="Q1" s="60" t="s">
         <v>173</v>
@@ -10040,12 +10028,12 @@
         <v>176</v>
       </c>
       <c r="U1" s="60" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="59" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B2" s="59" t="s">
         <v>164</v>
@@ -10057,16 +10045,16 @@
         <v>50</v>
       </c>
       <c r="E2" s="59" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F2" s="59" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="G2" s="59" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="H2" s="59" t="s">
-        <v>197</v>
+        <v>177</v>
       </c>
       <c r="I2" s="59" t="s">
         <v>178</v>
@@ -10080,7 +10068,7 @@
         <v>10</v>
       </c>
       <c r="N2" s="59" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="O2" s="59">
         <v>0</v>
@@ -10101,15 +10089,15 @@
         <v>10</v>
       </c>
       <c r="U2" s="59" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="59" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B3" s="59" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C3" s="59">
         <v>15</v>
@@ -10118,13 +10106,13 @@
         <v>50</v>
       </c>
       <c r="E3" s="59" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="F3" s="59" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="G3" s="59" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="H3" s="59" t="s">
         <v>177</v>
@@ -10141,7 +10129,7 @@
         <v>10</v>
       </c>
       <c r="N3" s="59" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="O3" s="59">
         <v>0</v>
@@ -10162,7 +10150,7 @@
         <v>10</v>
       </c>
       <c r="U3" s="59" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Kriterien Bodenseepokal ohne Nominierung
</commit_message>
<xml_diff>
--- a/web/utilities/records_kriterien.xlsx
+++ b/web/utilities/records_kriterien.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgna\Documents\GitHub\Lifesaving_Baden\web\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B059E8-E714-4033-97CF-98FB8809172C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98109EB9-3F53-4BB6-92FB-DE50D767F99B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
   </bookViews>
@@ -10293,7 +10293,7 @@
   <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10433,10 +10433,10 @@
         <v>179</v>
       </c>
       <c r="R2" s="59">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="S2" s="59">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T2" s="59">
         <v>10</v>
@@ -10494,10 +10494,10 @@
         <v>179</v>
       </c>
       <c r="R3" s="59">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="S3" s="59">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T3" s="59">
         <v>10</v>
@@ -10555,13 +10555,13 @@
         <v>179</v>
       </c>
       <c r="R4" s="59">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S4" s="59">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T4" s="59">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="U4" s="59"/>
     </row>
@@ -10614,13 +10614,13 @@
         <v>179</v>
       </c>
       <c r="R5" s="59">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S5" s="59">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T5" s="59">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="U5" s="59"/>
     </row>
@@ -10673,13 +10673,13 @@
         <v>179</v>
       </c>
       <c r="R6" s="59">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S6" s="59">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T6" s="59">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="U6" s="59"/>
     </row>
@@ -10732,13 +10732,13 @@
         <v>179</v>
       </c>
       <c r="R7" s="59">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S7" s="59">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="T7" s="59">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="U7" s="59"/>
     </row>

</xml_diff>

<commit_message>
Tabelle Code for smooth infos
</commit_message>
<xml_diff>
--- a/web/utilities/records_kriterien.xlsx
+++ b/web/utilities/records_kriterien.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgna\Documents\GitHub\Lifesaving_Baden\web\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81DB4840-3AF7-4347-98F3-42A56E2F95FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB38C40-687F-4D08-A851-3DEA19BAA54A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="4" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
   </bookViews>
   <sheets>
     <sheet name="DR" sheetId="9" r:id="rId1"/>
@@ -217,7 +217,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="204">
   <si>
     <t>50m Retten</t>
   </si>
@@ -826,6 +826,9 @@
   </si>
   <si>
     <t>Männlich (2026 findet kein DP statt)</t>
+  </si>
+  <si>
+    <t>Lara Ramackers</t>
   </si>
 </sst>
 </file>
@@ -4008,9 +4011,9 @@
       <selection activeCell="Y25" sqref="Y25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.265625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="42" t="s">
         <v>39</v>
       </c>
@@ -4079,7 +4082,7 @@
       <c r="AV1" s="44"/>
       <c r="AW1" s="44"/>
     </row>
-    <row r="2" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="42" t="s">
         <v>40</v>
       </c>
@@ -4146,7 +4149,7 @@
       <c r="AV2" s="45"/>
       <c r="AW2" s="45"/>
     </row>
-    <row r="3" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="42" t="s">
         <v>101</v>
       </c>
@@ -4207,7 +4210,7 @@
       <c r="AV3" s="45"/>
       <c r="AW3" s="45"/>
     </row>
-    <row r="4" spans="1:49" s="53" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:49" s="53" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="49" t="s">
         <v>10</v>
       </c>
@@ -4356,7 +4359,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>2000</v>
       </c>
@@ -4409,7 +4412,7 @@
       <c r="AV5" s="10"/>
       <c r="AW5" s="10"/>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <f t="shared" ref="A6:A31" si="0">A5+1</f>
         <v>2001</v>
@@ -4487,7 +4490,7 @@
       <c r="AV6" s="11"/>
       <c r="AW6" s="11"/>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>2002</v>
@@ -4565,7 +4568,7 @@
       <c r="AV7" s="10"/>
       <c r="AW7" s="10"/>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>2003</v>
@@ -4643,7 +4646,7 @@
       <c r="AV8" s="11"/>
       <c r="AW8" s="11"/>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>2004</v>
@@ -4721,7 +4724,7 @@
       <c r="AV9" s="10"/>
       <c r="AW9" s="10"/>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>2005</v>
@@ -4799,7 +4802,7 @@
       <c r="AV10" s="11"/>
       <c r="AW10" s="11"/>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>2006</v>
@@ -4877,7 +4880,7 @@
       <c r="AV11" s="10"/>
       <c r="AW11" s="10"/>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>2007</v>
@@ -4999,7 +5002,7 @@
         <v>3.5995370370370369E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>2008</v>
@@ -5121,7 +5124,7 @@
         <v>3.5995370370370369E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>2009</v>
@@ -5243,7 +5246,7 @@
         <v>3.5995370370370369E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>2010</v>
@@ -5365,7 +5368,7 @@
         <v>3.5995370370370369E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>2011</v>
@@ -5499,7 +5502,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>2012</v>
@@ -5633,7 +5636,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>2013</v>
@@ -5767,7 +5770,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>2014</v>
@@ -5901,7 +5904,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>2015</v>
@@ -6035,7 +6038,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>2016</v>
@@ -6169,7 +6172,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>2017</v>
@@ -6303,7 +6306,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>2018</v>
@@ -6437,7 +6440,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>2019</v>
@@ -6571,7 +6574,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>2020</v>
@@ -6721,7 +6724,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>2021</v>
@@ -6871,7 +6874,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>2022</v>
@@ -7021,7 +7024,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>2023</v>
@@ -7171,7 +7174,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>2024</v>
@@ -7321,7 +7324,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>2025</v>
@@ -7471,7 +7474,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>2026</v>
@@ -7690,17 +7693,17 @@
       <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" customWidth="1"/>
-    <col min="7" max="11" width="18.7109375" customWidth="1"/>
-    <col min="12" max="12" width="22.140625" customWidth="1"/>
-    <col min="13" max="13" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.265625" customWidth="1"/>
+    <col min="2" max="5" width="18.73046875" customWidth="1"/>
+    <col min="6" max="6" width="21.1328125" customWidth="1"/>
+    <col min="7" max="11" width="18.73046875" customWidth="1"/>
+    <col min="12" max="12" width="22.1328125" customWidth="1"/>
+    <col min="13" max="13" width="18.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="42" t="s">
         <v>39</v>
       </c>
@@ -7741,7 +7744,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="42" t="s">
         <v>40</v>
       </c>
@@ -7782,7 +7785,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="42" t="s">
         <v>41</v>
       </c>
@@ -7823,7 +7826,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -7864,7 +7867,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>2000</v>
       </c>
@@ -7881,7 +7884,7 @@
       <c r="L5" s="11"/>
       <c r="M5" s="11"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <f t="shared" ref="A6:A32" si="0">A5+1</f>
         <v>2001</v>
@@ -7899,7 +7902,7 @@
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>2002</v>
@@ -7917,7 +7920,7 @@
       <c r="L7" s="11"/>
       <c r="M7" s="11"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>2003</v>
@@ -7935,7 +7938,7 @@
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>2004</v>
@@ -7953,7 +7956,7 @@
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>2005</v>
@@ -7971,7 +7974,7 @@
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>2006</v>
@@ -7989,7 +7992,7 @@
       <c r="L11" s="11"/>
       <c r="M11" s="11"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>2007</v>
@@ -8007,7 +8010,7 @@
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>2008</v>
@@ -8025,7 +8028,7 @@
       <c r="L13" s="11"/>
       <c r="M13" s="11"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>2009</v>
@@ -8043,7 +8046,7 @@
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>2010</v>
@@ -8061,7 +8064,7 @@
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>2011</v>
@@ -8079,7 +8082,7 @@
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>2012</v>
@@ -8097,7 +8100,7 @@
       <c r="L17" s="11"/>
       <c r="M17" s="11"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>2013</v>
@@ -8115,7 +8118,7 @@
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>2014</v>
@@ -8133,7 +8136,7 @@
       <c r="L19" s="11"/>
       <c r="M19" s="11"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>2015</v>
@@ -8175,7 +8178,7 @@
         <v>1.3592592592592591E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>2016</v>
@@ -8217,7 +8220,7 @@
         <v>1.3592592592592591E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>2017</v>
@@ -8259,7 +8262,7 @@
         <v>1.3577546296296298E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>2018</v>
@@ -8301,7 +8304,7 @@
         <v>1.3577546296296298E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>2019</v>
@@ -8343,7 +8346,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>2020</v>
@@ -8385,7 +8388,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>2021</v>
@@ -8427,7 +8430,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>2022</v>
@@ -8469,7 +8472,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>2023</v>
@@ -8511,7 +8514,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>2024</v>
@@ -8553,7 +8556,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>2025</v>
@@ -8595,7 +8598,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>2026</v>
@@ -8637,7 +8640,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A32" s="2">
         <f t="shared" si="0"/>
         <v>2027</v>
@@ -8717,17 +8720,17 @@
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" customWidth="1"/>
-    <col min="7" max="11" width="18.7109375" customWidth="1"/>
-    <col min="12" max="12" width="22.140625" customWidth="1"/>
-    <col min="13" max="13" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.86328125" customWidth="1"/>
+    <col min="2" max="5" width="18.73046875" customWidth="1"/>
+    <col min="6" max="6" width="21.1328125" customWidth="1"/>
+    <col min="7" max="11" width="18.73046875" customWidth="1"/>
+    <col min="12" max="12" width="22.1328125" customWidth="1"/>
+    <col min="13" max="13" width="18.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="42" t="s">
         <v>39</v>
       </c>
@@ -8768,7 +8771,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="42" t="s">
         <v>40</v>
       </c>
@@ -8809,7 +8812,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="42" t="s">
         <v>41</v>
       </c>
@@ -8850,7 +8853,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -8891,7 +8894,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>2000</v>
       </c>
@@ -8908,7 +8911,7 @@
       <c r="L5" s="38"/>
       <c r="M5" s="38"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <f t="shared" ref="A6:A31" si="0">A5+1</f>
         <v>2001</v>
@@ -8938,7 +8941,7 @@
         <v>1.3629629629629632E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>2002</v>
@@ -8980,7 +8983,7 @@
         <v>1.3629629629629632E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>2003</v>
@@ -9022,7 +9025,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>2004</v>
@@ -9064,7 +9067,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>2005</v>
@@ -9106,7 +9109,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>2006</v>
@@ -9148,7 +9151,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>2007</v>
@@ -9190,7 +9193,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>2008</v>
@@ -9232,7 +9235,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>2009</v>
@@ -9274,7 +9277,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>2010</v>
@@ -9316,7 +9319,7 @@
         <v>1.3306712962962966E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>2011</v>
@@ -9358,7 +9361,7 @@
         <v>1.3306712962962966E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>2012</v>
@@ -9400,7 +9403,7 @@
         <v>1.3306712962962966E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>2013</v>
@@ -9442,7 +9445,7 @@
         <v>1.312962962962963E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>2014</v>
@@ -9484,7 +9487,7 @@
         <v>1.312962962962963E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>2015</v>
@@ -9526,7 +9529,7 @@
         <v>1.3116898148148148E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>2016</v>
@@ -9568,7 +9571,7 @@
         <v>1.3116898148148148E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>2017</v>
@@ -9610,7 +9613,7 @@
         <v>1.3116898148148148E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>2018</v>
@@ -9652,7 +9655,7 @@
         <v>1.3116898148148148E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>2019</v>
@@ -9694,7 +9697,7 @@
         <v>1.3116898148148148E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>2020</v>
@@ -9736,7 +9739,7 @@
         <v>1.3097222222222223E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>2021</v>
@@ -9778,7 +9781,7 @@
         <v>1.3097222222222223E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>2022</v>
@@ -9820,7 +9823,7 @@
         <v>1.3097222222222223E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>2023</v>
@@ -9862,7 +9865,7 @@
         <v>1.3097222222222223E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>2024</v>
@@ -9904,7 +9907,7 @@
         <v>1.3097222222222223E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>2025</v>
@@ -9946,7 +9949,7 @@
         <v>1.2931712962962962E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>2026</v>
@@ -9988,7 +9991,7 @@
         <v>1.2931712962962962E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A32" s="2">
         <f>A31+1</f>
         <v>2027</v>
@@ -10066,34 +10069,34 @@
   </sheetPr>
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.59765625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.73046875" customWidth="1"/>
     <col min="15" max="16" width="19" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="22.265625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.73046875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="47.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="60" t="s">
         <v>161</v>
       </c>
@@ -10158,7 +10161,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A2" s="59" t="s">
         <v>201</v>
       </c>
@@ -10219,7 +10222,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A3" s="59" t="s">
         <v>202</v>
       </c>
@@ -10295,34 +10298,34 @@
   </sheetPr>
   <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.59765625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.73046875" customWidth="1"/>
     <col min="15" max="16" width="19" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="22.265625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.73046875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="47.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="60" t="s">
         <v>161</v>
       </c>
@@ -10387,7 +10390,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A2" s="59" t="s">
         <v>190</v>
       </c>
@@ -10448,7 +10451,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A3" s="59" t="s">
         <v>191</v>
       </c>
@@ -10509,7 +10512,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A4" s="59" t="s">
         <v>192</v>
       </c>
@@ -10566,9 +10569,11 @@
       <c r="T4" s="59">
         <v>10</v>
       </c>
-      <c r="U4" s="59"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="U4" s="59" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A5" s="59" t="s">
         <v>193</v>
       </c>
@@ -10627,7 +10632,7 @@
       </c>
       <c r="U5" s="59"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A6" s="59" t="s">
         <v>194</v>
       </c>
@@ -10686,7 +10691,7 @@
       </c>
       <c r="U6" s="59"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A7" s="59" t="s">
         <v>195</v>
       </c>
@@ -10764,15 +10769,15 @@
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
-    <col min="2" max="13" width="18.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.86328125" style="1" customWidth="1"/>
+    <col min="2" max="13" width="18.73046875" style="1" customWidth="1"/>
     <col min="14" max="14" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="11.42578125" style="1"/>
+    <col min="15" max="16384" width="11.3984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="18">
         <v>2024</v>
       </c>
@@ -10816,7 +10821,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
@@ -10872,7 +10877,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -10928,7 +10933,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="19" t="s">
         <v>8</v>
       </c>
@@ -10984,7 +10989,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" s="62" t="s">
         <v>13</v>
       </c>
@@ -11002,7 +11007,7 @@
       <c r="M7" s="62"/>
       <c r="N7" s="62"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" s="62"/>
       <c r="B8" s="62"/>
       <c r="C8" s="62"/>
@@ -11018,7 +11023,7 @@
       <c r="M8" s="62"/>
       <c r="N8" s="62"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" s="20" t="s">
         <v>6</v>
       </c>
@@ -11072,7 +11077,7 @@
       </c>
       <c r="N9" s="21"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" s="20" t="s">
         <v>7</v>
       </c>
@@ -11126,7 +11131,7 @@
       </c>
       <c r="N10" s="21"/>
     </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="22" t="s">
         <v>8</v>
       </c>
@@ -11180,7 +11185,7 @@
       </c>
       <c r="N11" s="23"/>
     </row>
-    <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="61" t="s">
         <v>14</v>
       </c>
@@ -11201,7 +11206,7 @@
       <c r="M14"/>
       <c r="N14"/>
     </row>
-    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="61"/>
       <c r="B15" s="61"/>
       <c r="C15" s="61"/>
@@ -11216,7 +11221,7 @@
       <c r="M15"/>
       <c r="N15"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -11251,7 +11256,7 @@
       <c r="M16"/>
       <c r="N16"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A17" s="8" t="s">
         <v>19</v>
       </c>
@@ -11286,7 +11291,7 @@
       <c r="M17"/>
       <c r="N17"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>19</v>
       </c>
@@ -11319,7 +11324,7 @@
       <c r="M18"/>
       <c r="N18"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A19" s="8" t="s">
         <v>22</v>
       </c>
@@ -11352,7 +11357,7 @@
       <c r="M19"/>
       <c r="N19"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A20" s="9" t="s">
         <v>24</v>
       </c>
@@ -11383,7 +11388,7 @@
       <c r="M20"/>
       <c r="N20"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A21" s="8" t="s">
         <v>22</v>
       </c>
@@ -11410,7 +11415,7 @@
       <c r="M21"/>
       <c r="N21"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
         <v>19</v>
       </c>
@@ -11433,7 +11438,7 @@
       <c r="I22" s="33"/>
       <c r="L22" s="41"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A23" s="8" t="s">
         <v>19</v>
       </c>
@@ -11456,50 +11461,50 @@
       <c r="I23" s="33"/>
       <c r="L23" s="40"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
       <c r="H24" s="33"/>
       <c r="I24" s="33"/>
       <c r="L24" s="41"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
       <c r="H25" s="33"/>
       <c r="I25" s="33"/>
       <c r="L25" s="40"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L26" s="41"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L27" s="40"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L28" s="41"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L29" s="40"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L30" s="41"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L31" s="40"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L32" s="41"/>
     </row>
-    <row r="33" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L33" s="40"/>
     </row>
-    <row r="34" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L34" s="41"/>
     </row>
-    <row r="35" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L35" s="33"/>
     </row>
-    <row r="36" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L36" s="41"/>
     </row>
-    <row r="37" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L37" s="33"/>
     </row>
   </sheetData>
@@ -11525,15 +11530,15 @@
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
-    <col min="2" max="13" width="18.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.86328125" style="1" customWidth="1"/>
+    <col min="2" max="13" width="18.73046875" style="1" customWidth="1"/>
     <col min="14" max="14" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="11.42578125" style="1"/>
+    <col min="15" max="16384" width="11.3984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="18">
         <v>2025</v>
       </c>
@@ -11577,7 +11582,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
@@ -11633,7 +11638,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -11689,7 +11694,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="19" t="s">
         <v>8</v>
       </c>
@@ -11745,7 +11750,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" s="62" t="s">
         <v>13</v>
       </c>
@@ -11763,7 +11768,7 @@
       <c r="M7" s="62"/>
       <c r="N7" s="62"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" s="62"/>
       <c r="B8" s="62"/>
       <c r="C8" s="62"/>
@@ -11779,7 +11784,7 @@
       <c r="M8" s="62"/>
       <c r="N8" s="62"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" s="20" t="s">
         <v>6</v>
       </c>
@@ -11833,7 +11838,7 @@
       </c>
       <c r="N9" s="21"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" s="20" t="s">
         <v>7</v>
       </c>
@@ -11887,7 +11892,7 @@
       </c>
       <c r="N10" s="21"/>
     </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="22" t="s">
         <v>8</v>
       </c>
@@ -11941,7 +11946,7 @@
       </c>
       <c r="N11" s="23"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A14" s="61" t="s">
         <v>14</v>
       </c>
@@ -11960,7 +11965,7 @@
       </c>
       <c r="M14"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A15" s="61"/>
       <c r="B15" s="61"/>
       <c r="C15" s="61"/>
@@ -11973,7 +11978,7 @@
       <c r="L15" s="63"/>
       <c r="M15"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -12006,7 +12011,7 @@
       </c>
       <c r="M16"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="8" t="s">
         <v>28</v>
       </c>
@@ -12039,7 +12044,7 @@
       </c>
       <c r="M17"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>28</v>
       </c>
@@ -12070,7 +12075,7 @@
       <c r="L18" s="38"/>
       <c r="M18"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="8" t="s">
         <v>29</v>
       </c>
@@ -12101,7 +12106,7 @@
       <c r="L19" s="36"/>
       <c r="M19"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="9" t="s">
         <v>30</v>
       </c>
@@ -12130,7 +12135,7 @@
       <c r="L20" s="38"/>
       <c r="M20"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="8" t="s">
         <v>29</v>
       </c>
@@ -12161,7 +12166,7 @@
       <c r="L21" s="36"/>
       <c r="M21"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
         <v>28</v>
       </c>
@@ -12192,7 +12197,7 @@
       <c r="L22" s="39"/>
       <c r="M22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" s="8" t="s">
         <v>28</v>
       </c>
@@ -12223,66 +12228,66 @@
       <c r="L23" s="37"/>
       <c r="M23"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="H24" s="40"/>
       <c r="I24" s="40"/>
       <c r="J24" s="40"/>
       <c r="L24" s="39"/>
       <c r="M24"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="H25" s="33"/>
       <c r="I25" s="33"/>
       <c r="L25" s="37"/>
       <c r="M25"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L26" s="39"/>
       <c r="M26"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L27" s="37"/>
       <c r="M27"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L28" s="39"/>
       <c r="M28"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L29" s="37"/>
       <c r="M29"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L30" s="39"/>
       <c r="M30"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L31" s="37"/>
       <c r="M31"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L32" s="39"/>
       <c r="M32"/>
     </row>
-    <row r="33" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="8:13" x14ac:dyDescent="0.45">
       <c r="L33" s="37"/>
       <c r="M33"/>
     </row>
-    <row r="34" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="8:13" x14ac:dyDescent="0.45">
       <c r="L34" s="39"/>
       <c r="M34"/>
     </row>
-    <row r="35" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:13" x14ac:dyDescent="0.45">
       <c r="M35"/>
     </row>
-    <row r="36" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="8:13" x14ac:dyDescent="0.45">
       <c r="L36" s="39"/>
       <c r="M36"/>
     </row>
-    <row r="37" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="8:13" x14ac:dyDescent="0.45">
       <c r="M37"/>
     </row>
-    <row r="38" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="8:13" x14ac:dyDescent="0.45">
       <c r="H38"/>
       <c r="I38"/>
       <c r="J38"/>
@@ -12290,7 +12295,7 @@
       <c r="L38"/>
       <c r="M38"/>
     </row>
-    <row r="39" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="8:13" x14ac:dyDescent="0.45">
       <c r="H39"/>
       <c r="I39"/>
       <c r="J39"/>
@@ -12321,15 +12326,15 @@
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
-    <col min="2" max="13" width="18.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.86328125" style="1" customWidth="1"/>
+    <col min="2" max="13" width="18.73046875" style="1" customWidth="1"/>
     <col min="14" max="14" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="11.42578125" style="1"/>
+    <col min="15" max="16384" width="11.3984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="18">
         <v>2026</v>
       </c>
@@ -12373,7 +12378,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
@@ -12429,7 +12434,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -12485,7 +12490,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="19" t="s">
         <v>8</v>
       </c>
@@ -12541,7 +12546,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" s="62" t="s">
         <v>13</v>
       </c>
@@ -12559,7 +12564,7 @@
       <c r="M7" s="62"/>
       <c r="N7" s="62"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" s="62"/>
       <c r="B8" s="62"/>
       <c r="C8" s="62"/>
@@ -12575,7 +12580,7 @@
       <c r="M8" s="62"/>
       <c r="N8" s="62"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" s="20" t="s">
         <v>6</v>
       </c>
@@ -12629,7 +12634,7 @@
       </c>
       <c r="N9" s="21"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" s="20" t="s">
         <v>7</v>
       </c>
@@ -12683,7 +12688,7 @@
       </c>
       <c r="N10" s="21"/>
     </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="22" t="s">
         <v>8</v>
       </c>
@@ -12737,7 +12742,7 @@
       </c>
       <c r="N11" s="23"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A14" s="61" t="s">
         <v>14</v>
       </c>
@@ -12756,7 +12761,7 @@
       </c>
       <c r="M14"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A15" s="61"/>
       <c r="B15" s="61"/>
       <c r="C15" s="61"/>
@@ -12769,7 +12774,7 @@
       <c r="L15" s="63"/>
       <c r="M15"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -12802,7 +12807,7 @@
       </c>
       <c r="M16"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="8" t="s">
         <v>28</v>
       </c>
@@ -12835,7 +12840,7 @@
       </c>
       <c r="M17"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>28</v>
       </c>
@@ -12866,7 +12871,7 @@
       <c r="L18" s="38"/>
       <c r="M18"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="8" t="s">
         <v>29</v>
       </c>
@@ -12897,7 +12902,7 @@
       <c r="L19" s="36"/>
       <c r="M19"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="9" t="s">
         <v>30</v>
       </c>
@@ -12926,7 +12931,7 @@
       <c r="L20" s="38"/>
       <c r="M20"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="8" t="s">
         <v>29</v>
       </c>
@@ -12957,7 +12962,7 @@
       <c r="L21" s="36"/>
       <c r="M21"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
         <v>28</v>
       </c>
@@ -12988,7 +12993,7 @@
       <c r="L22" s="39"/>
       <c r="M22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" s="8" t="s">
         <v>28</v>
       </c>
@@ -13019,66 +13024,66 @@
       <c r="L23" s="37"/>
       <c r="M23"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="H24" s="40"/>
       <c r="I24" s="40"/>
       <c r="J24" s="40"/>
       <c r="L24" s="39"/>
       <c r="M24"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="H25" s="33"/>
       <c r="I25" s="33"/>
       <c r="L25" s="37"/>
       <c r="M25"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L26" s="39"/>
       <c r="M26"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L27" s="37"/>
       <c r="M27"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L28" s="39"/>
       <c r="M28"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L29" s="37"/>
       <c r="M29"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L30" s="39"/>
       <c r="M30"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L31" s="37"/>
       <c r="M31"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L32" s="39"/>
       <c r="M32"/>
     </row>
-    <row r="33" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="8:13" x14ac:dyDescent="0.45">
       <c r="L33" s="37"/>
       <c r="M33"/>
     </row>
-    <row r="34" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="8:13" x14ac:dyDescent="0.45">
       <c r="L34" s="39"/>
       <c r="M34"/>
     </row>
-    <row r="35" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:13" x14ac:dyDescent="0.45">
       <c r="M35"/>
     </row>
-    <row r="36" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="8:13" x14ac:dyDescent="0.45">
       <c r="L36" s="39"/>
       <c r="M36"/>
     </row>
-    <row r="37" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="8:13" x14ac:dyDescent="0.45">
       <c r="M37"/>
     </row>
-    <row r="38" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="8:13" x14ac:dyDescent="0.45">
       <c r="H38"/>
       <c r="I38"/>
       <c r="J38"/>
@@ -13086,7 +13091,7 @@
       <c r="L38"/>
       <c r="M38"/>
     </row>
-    <row r="39" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="8:13" x14ac:dyDescent="0.45">
       <c r="H39"/>
       <c r="I39"/>
       <c r="J39"/>

</xml_diff>

<commit_message>
dem und dynamische Referenz Rekorde
</commit_message>
<xml_diff>
--- a/web/utilities/records_kriterien.xlsx
+++ b/web/utilities/records_kriterien.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgna\Documents\GitHub\Lifesaving_Baden\web\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AB38C40-687F-4D08-A851-3DEA19BAA54A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646EEA68-94AE-4513-BF57-D39B88D485D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="4" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
   </bookViews>
@@ -18,9 +18,11 @@
     <sheet name="WR-Open" sheetId="4" r:id="rId3"/>
     <sheet name="DP" sheetId="10" r:id="rId4"/>
     <sheet name="BP" sheetId="11" r:id="rId5"/>
-    <sheet name="2024" sheetId="6" r:id="rId6"/>
-    <sheet name="2025" sheetId="5" r:id="rId7"/>
-    <sheet name="2026" sheetId="8" r:id="rId8"/>
+    <sheet name="DEM" sheetId="12" r:id="rId6"/>
+    <sheet name="JRP" sheetId="13" r:id="rId7"/>
+    <sheet name="2024" sheetId="6" r:id="rId8"/>
+    <sheet name="2025" sheetId="5" r:id="rId9"/>
+    <sheet name="2026" sheetId="8" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -217,7 +219,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="526" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="225">
   <si>
     <t>50m Retten</t>
   </si>
@@ -829,6 +831,69 @@
   </si>
   <si>
     <t>Lara Ramackers</t>
+  </si>
+  <si>
+    <t>Mindest Alter</t>
+  </si>
+  <si>
+    <t>PZ1 - 50m Retten</t>
+  </si>
+  <si>
+    <t>PZ1 - 100m Retten</t>
+  </si>
+  <si>
+    <t>PZ1 - 100m Kombi</t>
+  </si>
+  <si>
+    <t>PZ1 - 200m Hindernis</t>
+  </si>
+  <si>
+    <t>PZ1 - 200m Super-Lifesaver</t>
+  </si>
+  <si>
+    <t>PZ1 - 100m Lifesaver</t>
+  </si>
+  <si>
+    <t>PZ2 - 50m Retten</t>
+  </si>
+  <si>
+    <t>PZ2 - 100m Retten</t>
+  </si>
+  <si>
+    <t>PZ2 - 100m Kombi</t>
+  </si>
+  <si>
+    <t>PZ2 - 100m Lifesaver</t>
+  </si>
+  <si>
+    <t>PZ2 - 200m Super-Lifesaver</t>
+  </si>
+  <si>
+    <t>PZ2 - 200m Hindernis</t>
+  </si>
+  <si>
+    <t>Weiblich</t>
+  </si>
+  <si>
+    <t>Männlich</t>
+  </si>
+  <si>
+    <t>Weiblich U17</t>
+  </si>
+  <si>
+    <t>Männlich U17</t>
+  </si>
+  <si>
+    <t>Weiblich U19</t>
+  </si>
+  <si>
+    <t>Männlich U19</t>
+  </si>
+  <si>
+    <t>1.3.Jahr</t>
+  </si>
+  <si>
+    <t>1.6.Jahr</t>
   </si>
 </sst>
 </file>
@@ -1280,7 +1345,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="142">
+  <dxfs count="194">
     <dxf>
       <font>
         <color theme="6"/>
@@ -1370,6 +1435,162 @@
       <font>
         <color theme="4"/>
       </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3501,102 +3722,102 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2C5E83EE-6B6F-478A-9C90-A846A1A76536}" name="WR_Open4" displayName="WR_Open4" ref="A4:AW31" totalsRowShown="0" headerRowDxfId="141" headerRowBorderDxfId="140" tableBorderDxfId="139">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2C5E83EE-6B6F-478A-9C90-A846A1A76536}" name="WR_Open4" displayName="WR_Open4" ref="A4:AW31" totalsRowShown="0" headerRowDxfId="193" headerRowBorderDxfId="192" tableBorderDxfId="191">
   <autoFilter ref="A4:AW31" xr:uid="{2C5E83EE-6B6F-478A-9C90-A846A1A76536}"/>
   <tableColumns count="49">
-    <tableColumn id="1" xr3:uid="{7C0C4105-A61A-4B8D-9129-EDC4F18765AF}" name="WR-Open" dataDxfId="138">
+    <tableColumn id="1" xr3:uid="{7C0C4105-A61A-4B8D-9129-EDC4F18765AF}" name="WR-Open" dataDxfId="190">
       <calculatedColumnFormula>A4+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{516F5612-F85F-413F-9012-E235F415E34B}" name="50m Retten - offen - W" dataDxfId="137"/>
-    <tableColumn id="3" xr3:uid="{BC9ACAC9-0D45-42FD-B596-D19FBE3A4D83}" name="100m Retten - offen - W" dataDxfId="136"/>
-    <tableColumn id="4" xr3:uid="{CB6DBE59-EB65-43F0-93E7-0BDC3F82832B}" name="100m Kombi - offen - W" dataDxfId="135"/>
-    <tableColumn id="5" xr3:uid="{AA603C60-6831-4C14-A8CD-0AA050DA7551}" name="100m Lifesaver - offen - W" dataDxfId="134"/>
-    <tableColumn id="6" xr3:uid="{7920F147-7717-4582-940A-2610F7D310CA}" name="200m Superlifesaver - offen - W" dataDxfId="133"/>
-    <tableColumn id="7" xr3:uid="{04E21F1D-AC8D-4A1B-9B43-59B8F7901673}" name="200m Hindernis - offen - W" dataDxfId="132"/>
-    <tableColumn id="8" xr3:uid="{40E8A083-653A-48A8-9B37-0A2D850B7829}" name="50m Retten - offen - M" dataDxfId="131"/>
-    <tableColumn id="9" xr3:uid="{863824A9-134F-4189-BB14-225AE224FC44}" name="100m Retten - offen - M" dataDxfId="130"/>
+    <tableColumn id="2" xr3:uid="{516F5612-F85F-413F-9012-E235F415E34B}" name="50m Retten - offen - W" dataDxfId="189"/>
+    <tableColumn id="3" xr3:uid="{BC9ACAC9-0D45-42FD-B596-D19FBE3A4D83}" name="100m Retten - offen - W" dataDxfId="188"/>
+    <tableColumn id="4" xr3:uid="{CB6DBE59-EB65-43F0-93E7-0BDC3F82832B}" name="100m Kombi - offen - W" dataDxfId="187"/>
+    <tableColumn id="5" xr3:uid="{AA603C60-6831-4C14-A8CD-0AA050DA7551}" name="100m Lifesaver - offen - W" dataDxfId="186"/>
+    <tableColumn id="6" xr3:uid="{7920F147-7717-4582-940A-2610F7D310CA}" name="200m Superlifesaver - offen - W" dataDxfId="185"/>
+    <tableColumn id="7" xr3:uid="{04E21F1D-AC8D-4A1B-9B43-59B8F7901673}" name="200m Hindernis - offen - W" dataDxfId="184"/>
+    <tableColumn id="8" xr3:uid="{40E8A083-653A-48A8-9B37-0A2D850B7829}" name="50m Retten - offen - M" dataDxfId="183"/>
+    <tableColumn id="9" xr3:uid="{863824A9-134F-4189-BB14-225AE224FC44}" name="100m Retten - offen - M" dataDxfId="182"/>
     <tableColumn id="10" xr3:uid="{598FC6AE-DEA2-4475-9A35-CDCB8C81496A}" name="100m Kombi - offen - M"/>
     <tableColumn id="11" xr3:uid="{9FC50B37-0D51-422E-A268-A6506D4F3854}" name="100m Lifesaver - offen - M"/>
     <tableColumn id="12" xr3:uid="{B8D2552B-5D82-442A-98F0-E47D5C5F6728}" name="200m Superlifesaver - offen - M"/>
-    <tableColumn id="13" xr3:uid="{5A5E9873-0C5F-4508-AF6B-4974E0526D84}" name="200m Hindernis - offen - M" dataDxfId="129"/>
-    <tableColumn id="14" xr3:uid="{FA907992-7FCE-4CAD-8CF2-F5BEBC9B3756}" name="50m Retten - 17/18 - W" dataDxfId="128"/>
-    <tableColumn id="15" xr3:uid="{76B63DC0-CB67-48F4-9B5A-D22902F59334}" name="100m Retten - 17/18 - W" dataDxfId="127"/>
-    <tableColumn id="16" xr3:uid="{614A2419-51B1-44C0-8469-ADBFB078B81A}" name="100m Kombi -17/18 - W" dataDxfId="126"/>
-    <tableColumn id="17" xr3:uid="{2EC953EE-367D-4524-A25E-8DE3B8168E34}" name="100m Lifesaver - 17/18 - W" dataDxfId="125"/>
-    <tableColumn id="18" xr3:uid="{25711867-9BD7-4197-9094-A21392411249}" name="200m Superlifesaver - 17/18 - W" dataDxfId="124"/>
-    <tableColumn id="19" xr3:uid="{262DB142-CFB1-45C3-9332-7273CACD1B62}" name="200m Hindernis - 17/18 - W" dataDxfId="123"/>
-    <tableColumn id="20" xr3:uid="{938BA45A-8244-4637-8A14-DF49CD91A945}" name="50m Retten - 17/18 - M" dataDxfId="122"/>
-    <tableColumn id="21" xr3:uid="{737E28D8-900F-4A98-95FE-EE7B0AFDEE90}" name="100m Retten - 17/18 - M" dataDxfId="121"/>
-    <tableColumn id="22" xr3:uid="{330BD3A8-061C-45E2-ADDB-40C2F346772F}" name="100m Kombi - 17/18 - M" dataDxfId="120"/>
-    <tableColumn id="23" xr3:uid="{0CADDE90-A167-4E1D-8D33-8624E5E1A4E2}" name="100m Lifesaver - 17/18 - M" dataDxfId="119"/>
-    <tableColumn id="24" xr3:uid="{FCF9F42C-1291-4985-9D37-B9DE2DAA5DCB}" name="200m Superlifesaver - 17/18 - M" dataDxfId="118"/>
-    <tableColumn id="25" xr3:uid="{4E5397B2-F924-4F48-AE69-AF6D650AF88D}" name="200m Hindernis - 17/18 - M" dataDxfId="117"/>
-    <tableColumn id="26" xr3:uid="{0A78315A-BFDC-43EE-A66F-48B301F66508}" name="50m Retten - 15/16 - W" dataDxfId="116"/>
-    <tableColumn id="27" xr3:uid="{D3FCF8BD-6C76-450D-80C0-CC0519A79731}" name="100m Retten - 15/16 - W" dataDxfId="115"/>
-    <tableColumn id="28" xr3:uid="{6BE7937E-D62D-47CD-95DE-1730304B0DF3}" name="100m Kombi - 15/16 - W" dataDxfId="114"/>
-    <tableColumn id="29" xr3:uid="{098BA5BE-5AF6-4187-89B6-534498F24C51}" name="100m Lifesaver -  15/16 - W" dataDxfId="113"/>
-    <tableColumn id="30" xr3:uid="{2A6822CF-143C-4BF7-A440-5777527BE512}" name="200m Superlifesaver -  15/16 - W" dataDxfId="112"/>
-    <tableColumn id="31" xr3:uid="{541C7145-CDEA-4E4E-9E7A-A4F05BA6C3E5}" name="200m Hindernis -  15/16 - W" dataDxfId="111"/>
-    <tableColumn id="32" xr3:uid="{342C4488-8C61-42E6-87A9-C75BD8EB7452}" name="50m Retten - 15/16 - M" dataDxfId="110"/>
-    <tableColumn id="33" xr3:uid="{857B1D46-7D20-47F7-AB9B-732D50346E32}" name="100m Retten - 15/16 - M" dataDxfId="109"/>
-    <tableColumn id="34" xr3:uid="{4C8A2EB4-804B-45F1-A768-9A6958957F8B}" name="100m Kombi -15/16 - M" dataDxfId="108"/>
-    <tableColumn id="35" xr3:uid="{26C75B4F-21EC-4EB0-A9A9-54BC80140672}" name="100m Lifesaver - 15/16 - M" dataDxfId="107"/>
-    <tableColumn id="36" xr3:uid="{DBBB2A23-1A06-429A-A5D1-A547EF5EC16F}" name="200m Superlifesaver - 15/16 - M" dataDxfId="106"/>
-    <tableColumn id="37" xr3:uid="{84061231-CAE5-427A-87F5-6DDBA99F77D2}" name="200m Hindernis - 15/16 - M" dataDxfId="105"/>
-    <tableColumn id="38" xr3:uid="{878CCA80-A742-4B3C-90C9-E93BB814201B}" name="50m Retten - 13/14 - W" dataDxfId="104"/>
-    <tableColumn id="39" xr3:uid="{A1F57102-61CF-4784-8DE2-0B8F32D5D699}" name="50m Retten mit Flossen - 13/14 - W" dataDxfId="103"/>
-    <tableColumn id="40" xr3:uid="{0F6BAF78-3D79-42A9-9FED-E6D0E335A920}" name="100m Hindernis - 13/14 - W" dataDxfId="102"/>
-    <tableColumn id="41" xr3:uid="{EB748A68-E10D-4D76-B315-8FDB3AC33C8D}" name="50m Retten - 13/14 - M" dataDxfId="101"/>
-    <tableColumn id="42" xr3:uid="{C7B04167-6430-40F0-9A0F-D0D0BE2F9C77}" name="50m Retten mit Flossen - 13/14 - M" dataDxfId="100"/>
-    <tableColumn id="43" xr3:uid="{48704BB7-A853-445A-8CDC-8D8F86C2B66A}" name="100m Hindernis - 13/14 - M" dataDxfId="99"/>
-    <tableColumn id="44" xr3:uid="{9605FE9A-F41C-4A5F-A59C-B7A9D45C460F}" name="50m Flossen - 12 - W" dataDxfId="98"/>
-    <tableColumn id="45" xr3:uid="{4C9DBF61-35B1-4BC2-8272-526E0AFAAFFB}" name="50m komb. Schwimmen - 12 - W" dataDxfId="97"/>
-    <tableColumn id="46" xr3:uid="{CF433C95-C272-48F9-98CD-7E3C8DBB6F2C}" name="50m Hindernis - 12 - W" dataDxfId="96"/>
-    <tableColumn id="47" xr3:uid="{FADB7411-DB43-4B14-B9E8-D74CA1BA18B8}" name="50m Flossen - 12 - M" dataDxfId="95"/>
-    <tableColumn id="48" xr3:uid="{02936F84-1D82-48AC-8D7C-6D2954D68A06}" name="50m komb. Schwimmen - 12 - M" dataDxfId="94"/>
-    <tableColumn id="49" xr3:uid="{7FD9BD11-0597-4E07-8DA5-DB53384197F5}" name="50m Hindernis - 12 - M" dataDxfId="93"/>
+    <tableColumn id="13" xr3:uid="{5A5E9873-0C5F-4508-AF6B-4974E0526D84}" name="200m Hindernis - offen - M" dataDxfId="181"/>
+    <tableColumn id="14" xr3:uid="{FA907992-7FCE-4CAD-8CF2-F5BEBC9B3756}" name="50m Retten - 17/18 - W" dataDxfId="180"/>
+    <tableColumn id="15" xr3:uid="{76B63DC0-CB67-48F4-9B5A-D22902F59334}" name="100m Retten - 17/18 - W" dataDxfId="179"/>
+    <tableColumn id="16" xr3:uid="{614A2419-51B1-44C0-8469-ADBFB078B81A}" name="100m Kombi -17/18 - W" dataDxfId="178"/>
+    <tableColumn id="17" xr3:uid="{2EC953EE-367D-4524-A25E-8DE3B8168E34}" name="100m Lifesaver - 17/18 - W" dataDxfId="177"/>
+    <tableColumn id="18" xr3:uid="{25711867-9BD7-4197-9094-A21392411249}" name="200m Superlifesaver - 17/18 - W" dataDxfId="176"/>
+    <tableColumn id="19" xr3:uid="{262DB142-CFB1-45C3-9332-7273CACD1B62}" name="200m Hindernis - 17/18 - W" dataDxfId="175"/>
+    <tableColumn id="20" xr3:uid="{938BA45A-8244-4637-8A14-DF49CD91A945}" name="50m Retten - 17/18 - M" dataDxfId="174"/>
+    <tableColumn id="21" xr3:uid="{737E28D8-900F-4A98-95FE-EE7B0AFDEE90}" name="100m Retten - 17/18 - M" dataDxfId="173"/>
+    <tableColumn id="22" xr3:uid="{330BD3A8-061C-45E2-ADDB-40C2F346772F}" name="100m Kombi - 17/18 - M" dataDxfId="172"/>
+    <tableColumn id="23" xr3:uid="{0CADDE90-A167-4E1D-8D33-8624E5E1A4E2}" name="100m Lifesaver - 17/18 - M" dataDxfId="171"/>
+    <tableColumn id="24" xr3:uid="{FCF9F42C-1291-4985-9D37-B9DE2DAA5DCB}" name="200m Superlifesaver - 17/18 - M" dataDxfId="170"/>
+    <tableColumn id="25" xr3:uid="{4E5397B2-F924-4F48-AE69-AF6D650AF88D}" name="200m Hindernis - 17/18 - M" dataDxfId="169"/>
+    <tableColumn id="26" xr3:uid="{0A78315A-BFDC-43EE-A66F-48B301F66508}" name="50m Retten - 15/16 - W" dataDxfId="168"/>
+    <tableColumn id="27" xr3:uid="{D3FCF8BD-6C76-450D-80C0-CC0519A79731}" name="100m Retten - 15/16 - W" dataDxfId="167"/>
+    <tableColumn id="28" xr3:uid="{6BE7937E-D62D-47CD-95DE-1730304B0DF3}" name="100m Kombi - 15/16 - W" dataDxfId="166"/>
+    <tableColumn id="29" xr3:uid="{098BA5BE-5AF6-4187-89B6-534498F24C51}" name="100m Lifesaver -  15/16 - W" dataDxfId="165"/>
+    <tableColumn id="30" xr3:uid="{2A6822CF-143C-4BF7-A440-5777527BE512}" name="200m Superlifesaver -  15/16 - W" dataDxfId="164"/>
+    <tableColumn id="31" xr3:uid="{541C7145-CDEA-4E4E-9E7A-A4F05BA6C3E5}" name="200m Hindernis -  15/16 - W" dataDxfId="163"/>
+    <tableColumn id="32" xr3:uid="{342C4488-8C61-42E6-87A9-C75BD8EB7452}" name="50m Retten - 15/16 - M" dataDxfId="162"/>
+    <tableColumn id="33" xr3:uid="{857B1D46-7D20-47F7-AB9B-732D50346E32}" name="100m Retten - 15/16 - M" dataDxfId="161"/>
+    <tableColumn id="34" xr3:uid="{4C8A2EB4-804B-45F1-A768-9A6958957F8B}" name="100m Kombi -15/16 - M" dataDxfId="160"/>
+    <tableColumn id="35" xr3:uid="{26C75B4F-21EC-4EB0-A9A9-54BC80140672}" name="100m Lifesaver - 15/16 - M" dataDxfId="159"/>
+    <tableColumn id="36" xr3:uid="{DBBB2A23-1A06-429A-A5D1-A547EF5EC16F}" name="200m Superlifesaver - 15/16 - M" dataDxfId="158"/>
+    <tableColumn id="37" xr3:uid="{84061231-CAE5-427A-87F5-6DDBA99F77D2}" name="200m Hindernis - 15/16 - M" dataDxfId="157"/>
+    <tableColumn id="38" xr3:uid="{878CCA80-A742-4B3C-90C9-E93BB814201B}" name="50m Retten - 13/14 - W" dataDxfId="156"/>
+    <tableColumn id="39" xr3:uid="{A1F57102-61CF-4784-8DE2-0B8F32D5D699}" name="50m Retten mit Flossen - 13/14 - W" dataDxfId="155"/>
+    <tableColumn id="40" xr3:uid="{0F6BAF78-3D79-42A9-9FED-E6D0E335A920}" name="100m Hindernis - 13/14 - W" dataDxfId="154"/>
+    <tableColumn id="41" xr3:uid="{EB748A68-E10D-4D76-B315-8FDB3AC33C8D}" name="50m Retten - 13/14 - M" dataDxfId="153"/>
+    <tableColumn id="42" xr3:uid="{C7B04167-6430-40F0-9A0F-D0D0BE2F9C77}" name="50m Retten mit Flossen - 13/14 - M" dataDxfId="152"/>
+    <tableColumn id="43" xr3:uid="{48704BB7-A853-445A-8CDC-8D8F86C2B66A}" name="100m Hindernis - 13/14 - M" dataDxfId="151"/>
+    <tableColumn id="44" xr3:uid="{9605FE9A-F41C-4A5F-A59C-B7A9D45C460F}" name="50m Flossen - 12 - W" dataDxfId="150"/>
+    <tableColumn id="45" xr3:uid="{4C9DBF61-35B1-4BC2-8272-526E0AFAAFFB}" name="50m komb. Schwimmen - 12 - W" dataDxfId="149"/>
+    <tableColumn id="46" xr3:uid="{CF433C95-C272-48F9-98CD-7E3C8DBB6F2C}" name="50m Hindernis - 12 - W" dataDxfId="148"/>
+    <tableColumn id="47" xr3:uid="{FADB7411-DB43-4B14-B9E8-D74CA1BA18B8}" name="50m Flossen - 12 - M" dataDxfId="147"/>
+    <tableColumn id="48" xr3:uid="{02936F84-1D82-48AC-8D7C-6D2954D68A06}" name="50m komb. Schwimmen - 12 - M" dataDxfId="146"/>
+    <tableColumn id="49" xr3:uid="{7FD9BD11-0597-4E07-8DA5-DB53384197F5}" name="50m Hindernis - 12 - M" dataDxfId="145"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4234D44E-A2BE-4790-B589-1A8CC19B714E}" name="WR_Youth" displayName="WR_Youth" ref="A4:M32" totalsRowShown="0" headerRowDxfId="92" dataDxfId="90" headerRowBorderDxfId="91" tableBorderDxfId="89">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4234D44E-A2BE-4790-B589-1A8CC19B714E}" name="WR_Youth" displayName="WR_Youth" ref="A4:M32" totalsRowShown="0" headerRowDxfId="144" dataDxfId="142" headerRowBorderDxfId="143" tableBorderDxfId="141">
   <autoFilter ref="A4:M32" xr:uid="{4234D44E-A2BE-4790-B589-1A8CC19B714E}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{848E691A-41B0-42DD-B122-FB6DF43CB3EF}" name="WR-Youth" dataDxfId="88"/>
-    <tableColumn id="2" xr3:uid="{2FE43F18-485B-46A9-8946-FBC5FDAE5A8E}" name="50m Retten" dataDxfId="87"/>
-    <tableColumn id="3" xr3:uid="{CA5C3ABF-02E6-442B-868B-95B293B231D3}" name="100m Retten" dataDxfId="86"/>
-    <tableColumn id="4" xr3:uid="{7A6BBA52-2145-464D-8C04-B2CCFC1A90DC}" name="100m Kombi" dataDxfId="85"/>
-    <tableColumn id="5" xr3:uid="{21F420C9-E788-49EE-88F6-E37963ED31CF}" name="100m Lifesaver" dataDxfId="84"/>
-    <tableColumn id="6" xr3:uid="{CB87B7CD-8A9C-4775-A4D7-4D267F43FD1A}" name="200m Superlifesaver" dataDxfId="83"/>
-    <tableColumn id="7" xr3:uid="{2DC7F290-B564-4851-85AE-D211DA701B32}" name="200m Hindernis" dataDxfId="82"/>
-    <tableColumn id="8" xr3:uid="{8112783D-8796-4D6A-8414-AC675D745697}" name="50m Retten2" dataDxfId="81"/>
-    <tableColumn id="9" xr3:uid="{4E818CD4-8725-495D-9D1D-1AFCED9181F5}" name="100m Retten2" dataDxfId="80"/>
-    <tableColumn id="10" xr3:uid="{28C05A91-E302-40A9-B50A-ECF997F129FC}" name="100m Kombi2" dataDxfId="79"/>
-    <tableColumn id="11" xr3:uid="{D56FB9F2-45BF-4EC9-A84C-8A5FB59F2F05}" name="100m Lifesaver2" dataDxfId="78"/>
-    <tableColumn id="12" xr3:uid="{540169C0-2A40-4794-A872-F7DF8A887BF2}" name="200m Superlifesaver2" dataDxfId="77"/>
-    <tableColumn id="13" xr3:uid="{D104CB67-B55A-4C81-87E5-0AC758DD22A4}" name="200m Hindernis2" dataDxfId="76"/>
+    <tableColumn id="1" xr3:uid="{848E691A-41B0-42DD-B122-FB6DF43CB3EF}" name="WR-Youth" dataDxfId="140"/>
+    <tableColumn id="2" xr3:uid="{2FE43F18-485B-46A9-8946-FBC5FDAE5A8E}" name="50m Retten" dataDxfId="139"/>
+    <tableColumn id="3" xr3:uid="{CA5C3ABF-02E6-442B-868B-95B293B231D3}" name="100m Retten" dataDxfId="138"/>
+    <tableColumn id="4" xr3:uid="{7A6BBA52-2145-464D-8C04-B2CCFC1A90DC}" name="100m Kombi" dataDxfId="137"/>
+    <tableColumn id="5" xr3:uid="{21F420C9-E788-49EE-88F6-E37963ED31CF}" name="100m Lifesaver" dataDxfId="136"/>
+    <tableColumn id="6" xr3:uid="{CB87B7CD-8A9C-4775-A4D7-4D267F43FD1A}" name="200m Superlifesaver" dataDxfId="135"/>
+    <tableColumn id="7" xr3:uid="{2DC7F290-B564-4851-85AE-D211DA701B32}" name="200m Hindernis" dataDxfId="134"/>
+    <tableColumn id="8" xr3:uid="{8112783D-8796-4D6A-8414-AC675D745697}" name="50m Retten2" dataDxfId="133"/>
+    <tableColumn id="9" xr3:uid="{4E818CD4-8725-495D-9D1D-1AFCED9181F5}" name="100m Retten2" dataDxfId="132"/>
+    <tableColumn id="10" xr3:uid="{28C05A91-E302-40A9-B50A-ECF997F129FC}" name="100m Kombi2" dataDxfId="131"/>
+    <tableColumn id="11" xr3:uid="{D56FB9F2-45BF-4EC9-A84C-8A5FB59F2F05}" name="100m Lifesaver2" dataDxfId="130"/>
+    <tableColumn id="12" xr3:uid="{540169C0-2A40-4794-A872-F7DF8A887BF2}" name="200m Superlifesaver2" dataDxfId="129"/>
+    <tableColumn id="13" xr3:uid="{D104CB67-B55A-4C81-87E5-0AC758DD22A4}" name="200m Hindernis2" dataDxfId="128"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E2D2F97B-7645-4066-8AB3-F35CF6E035EB}" name="WR_Open" displayName="WR_Open" ref="A4:M32" totalsRowShown="0" headerRowDxfId="75" headerRowBorderDxfId="74" tableBorderDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E2D2F97B-7645-4066-8AB3-F35CF6E035EB}" name="WR_Open" displayName="WR_Open" ref="A4:M32" totalsRowShown="0" headerRowDxfId="127" headerRowBorderDxfId="126" tableBorderDxfId="125">
   <autoFilter ref="A4:M32" xr:uid="{E2D2F97B-7645-4066-8AB3-F35CF6E035EB}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{AE73402B-B27E-4B29-8DCF-30B7FC1855EF}" name="WR-Open" dataDxfId="72">
+    <tableColumn id="1" xr3:uid="{AE73402B-B27E-4B29-8DCF-30B7FC1855EF}" name="WR-Open" dataDxfId="124">
       <calculatedColumnFormula>A4+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{EA3EAC1F-184E-4A28-B3E3-08DE12F138EF}" name="50m Retten" dataDxfId="71"/>
-    <tableColumn id="3" xr3:uid="{E0305A3F-6087-4F8C-8B64-153E1ACAA32E}" name="100m Retten" dataDxfId="70"/>
-    <tableColumn id="4" xr3:uid="{F0B7AC37-315E-49AA-855C-7955D2B43A76}" name="100m Kombi" dataDxfId="69"/>
-    <tableColumn id="5" xr3:uid="{B5E690AB-DB7D-4864-8916-89D2A68C4128}" name="100m Lifesaver" dataDxfId="68"/>
-    <tableColumn id="6" xr3:uid="{D89BAF4D-36AE-4C73-9320-9C5736F02F8A}" name="200m Superlifesaver" dataDxfId="67"/>
-    <tableColumn id="7" xr3:uid="{58AE7517-1A90-459F-A7D2-B95265D217E7}" name="200m Hindernis" dataDxfId="66"/>
-    <tableColumn id="8" xr3:uid="{13A189FB-E897-4A1F-A001-525F61E9CFFF}" name="50m Retten2" dataDxfId="65"/>
-    <tableColumn id="9" xr3:uid="{36418AC5-46B8-400F-BD2E-D329CF4F92CD}" name="100m Retten2" dataDxfId="64"/>
+    <tableColumn id="2" xr3:uid="{EA3EAC1F-184E-4A28-B3E3-08DE12F138EF}" name="50m Retten" dataDxfId="123"/>
+    <tableColumn id="3" xr3:uid="{E0305A3F-6087-4F8C-8B64-153E1ACAA32E}" name="100m Retten" dataDxfId="122"/>
+    <tableColumn id="4" xr3:uid="{F0B7AC37-315E-49AA-855C-7955D2B43A76}" name="100m Kombi" dataDxfId="121"/>
+    <tableColumn id="5" xr3:uid="{B5E690AB-DB7D-4864-8916-89D2A68C4128}" name="100m Lifesaver" dataDxfId="120"/>
+    <tableColumn id="6" xr3:uid="{D89BAF4D-36AE-4C73-9320-9C5736F02F8A}" name="200m Superlifesaver" dataDxfId="119"/>
+    <tableColumn id="7" xr3:uid="{58AE7517-1A90-459F-A7D2-B95265D217E7}" name="200m Hindernis" dataDxfId="118"/>
+    <tableColumn id="8" xr3:uid="{13A189FB-E897-4A1F-A001-525F61E9CFFF}" name="50m Retten2" dataDxfId="117"/>
+    <tableColumn id="9" xr3:uid="{36418AC5-46B8-400F-BD2E-D329CF4F92CD}" name="100m Retten2" dataDxfId="116"/>
     <tableColumn id="10" xr3:uid="{06A35C2D-7313-472B-BC1F-4F2FB1D14782}" name="100m Kombi2"/>
     <tableColumn id="11" xr3:uid="{89966D0D-9131-4245-A7BE-1A7384D5ADA0}" name="100m Lifesaver2"/>
     <tableColumn id="12" xr3:uid="{D9D6CF56-869C-4DDE-9886-572D4E523A8F}" name="200m Superlifesaver2"/>
@@ -3607,7 +3828,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CF3D303A-A04B-42DD-A44E-CEB6CECB77A4}" name="DP_konfig" displayName="DP_konfig" ref="A1:U3" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CF3D303A-A04B-42DD-A44E-CEB6CECB77A4}" name="DP_konfig" displayName="DP_konfig" ref="A1:U3" totalsRowShown="0" headerRowDxfId="115" dataDxfId="114">
   <autoFilter ref="A1:U3" xr:uid="{CF3D303A-A04B-42DD-A44E-CEB6CECB77A4}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3632,57 +3853,173 @@
     <filterColumn colId="20" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="21">
-    <tableColumn id="1" xr3:uid="{58D628F0-061E-4A82-8362-CDB37A2E7C60}" name="Tabellen Name" dataDxfId="61"/>
-    <tableColumn id="2" xr3:uid="{2F302F6C-F8AF-4FDE-AB08-6F30F9671015}" name="Geschlecht" dataDxfId="60"/>
-    <tableColumn id="3" xr3:uid="{4D91FBF9-386D-43DD-90D0-B49823FDB629}" name="Mindest alter" dataDxfId="59"/>
-    <tableColumn id="4" xr3:uid="{4126AAC6-AF2F-446C-B4EA-D86ACFD9FAC2}" name="Maximales Alter" dataDxfId="58"/>
-    <tableColumn id="5" xr3:uid="{8A10890A-A299-4B09-AC72-0E9AE9238AF3}" name="Qualizeitraum anfang" dataDxfId="57"/>
-    <tableColumn id="6" xr3:uid="{FBCD1C13-FC82-429B-8DE1-0C5A455FDAB8}" name="Qualizeitraum Ende" dataDxfId="56"/>
-    <tableColumn id="7" xr3:uid="{1DCCAC9B-BC46-468E-A3CE-57576C2FF11D}" name="Letzter Wettkampf am" dataDxfId="55"/>
-    <tableColumn id="8" xr3:uid="{9A6E47EE-ABD8-4A1E-87D3-9D286E4C124F}" name="Wertung" dataDxfId="54"/>
-    <tableColumn id="9" xr3:uid="{09E848D2-ED17-49C7-9775-CBF17D20DFC0}" name="Landesverband" dataDxfId="53"/>
-    <tableColumn id="10" xr3:uid="{70ABB713-23F6-4FCF-920E-3CB0CD451446}" name="OMS" dataDxfId="52"/>
-    <tableColumn id="11" xr3:uid="{9C108A1C-E6AB-4C13-9C1D-0FA8944A39A3}" name="Pool-Länge" dataDxfId="51"/>
-    <tableColumn id="12" xr3:uid="{087948DD-430D-48F1-906D-4F4EF4B46053}" name="Regelwerk" dataDxfId="50"/>
-    <tableColumn id="13" xr3:uid="{BF42D9C0-F77D-4971-A67E-32B0246C72C3}" name="Referenz" dataDxfId="49"/>
-    <tableColumn id="19" xr3:uid="{AFFB84E8-B398-4E99-805B-9A247071A040}" name="Referenz Jahr" dataDxfId="48"/>
-    <tableColumn id="20" xr3:uid="{0A59A474-DFBB-4437-8EFF-70284AFD9934}" name="Mindest Punktzahl" dataDxfId="47"/>
-    <tableColumn id="21" xr3:uid="{198BD231-EEF3-43C9-AD9B-39B4B7E9B337}" name="Mindest Disziplinen" dataDxfId="46"/>
-    <tableColumn id="14" xr3:uid="{443CD4F6-A2B2-480B-BB35-DCEEBC531727}" name="3-Kampf Regel" dataDxfId="45"/>
-    <tableColumn id="15" xr3:uid="{70116160-7666-42B1-92AC-FAC2620E6A60}" name="Anzahl Nominierte" dataDxfId="44"/>
-    <tableColumn id="16" xr3:uid="{0EFD0A46-D12B-4AB0-907C-08E5D9F282E0}" name="Anzahl Nachrücker" dataDxfId="43"/>
-    <tableColumn id="17" xr3:uid="{AA5430A0-8ED8-40E8-B7F8-DA25E4E8790F}" name="Seiten Anzahl" dataDxfId="42"/>
-    <tableColumn id="18" xr3:uid="{16F699D9-2741-43F3-AD5F-826A568EFEAC}" name="Absagen" dataDxfId="41"/>
+    <tableColumn id="1" xr3:uid="{58D628F0-061E-4A82-8362-CDB37A2E7C60}" name="Tabellen Name" dataDxfId="113"/>
+    <tableColumn id="2" xr3:uid="{2F302F6C-F8AF-4FDE-AB08-6F30F9671015}" name="Geschlecht" dataDxfId="112"/>
+    <tableColumn id="3" xr3:uid="{4D91FBF9-386D-43DD-90D0-B49823FDB629}" name="Mindest alter" dataDxfId="111"/>
+    <tableColumn id="4" xr3:uid="{4126AAC6-AF2F-446C-B4EA-D86ACFD9FAC2}" name="Maximales Alter" dataDxfId="110"/>
+    <tableColumn id="5" xr3:uid="{8A10890A-A299-4B09-AC72-0E9AE9238AF3}" name="Qualizeitraum anfang" dataDxfId="109"/>
+    <tableColumn id="6" xr3:uid="{FBCD1C13-FC82-429B-8DE1-0C5A455FDAB8}" name="Qualizeitraum Ende" dataDxfId="108"/>
+    <tableColumn id="7" xr3:uid="{1DCCAC9B-BC46-468E-A3CE-57576C2FF11D}" name="Letzter Wettkampf am" dataDxfId="107"/>
+    <tableColumn id="8" xr3:uid="{9A6E47EE-ABD8-4A1E-87D3-9D286E4C124F}" name="Wertung" dataDxfId="106"/>
+    <tableColumn id="9" xr3:uid="{09E848D2-ED17-49C7-9775-CBF17D20DFC0}" name="Landesverband" dataDxfId="105"/>
+    <tableColumn id="10" xr3:uid="{70ABB713-23F6-4FCF-920E-3CB0CD451446}" name="OMS" dataDxfId="104"/>
+    <tableColumn id="11" xr3:uid="{9C108A1C-E6AB-4C13-9C1D-0FA8944A39A3}" name="Pool-Länge" dataDxfId="103"/>
+    <tableColumn id="12" xr3:uid="{087948DD-430D-48F1-906D-4F4EF4B46053}" name="Regelwerk" dataDxfId="102"/>
+    <tableColumn id="13" xr3:uid="{BF42D9C0-F77D-4971-A67E-32B0246C72C3}" name="Referenz" dataDxfId="101"/>
+    <tableColumn id="19" xr3:uid="{AFFB84E8-B398-4E99-805B-9A247071A040}" name="Referenz Jahr" dataDxfId="100"/>
+    <tableColumn id="20" xr3:uid="{0A59A474-DFBB-4437-8EFF-70284AFD9934}" name="Mindest Punktzahl" dataDxfId="99"/>
+    <tableColumn id="21" xr3:uid="{198BD231-EEF3-43C9-AD9B-39B4B7E9B337}" name="Mindest Disziplinen" dataDxfId="98"/>
+    <tableColumn id="14" xr3:uid="{443CD4F6-A2B2-480B-BB35-DCEEBC531727}" name="3-Kampf Regel" dataDxfId="97"/>
+    <tableColumn id="15" xr3:uid="{70116160-7666-42B1-92AC-FAC2620E6A60}" name="Anzahl Nominierte" dataDxfId="96"/>
+    <tableColumn id="16" xr3:uid="{0EFD0A46-D12B-4AB0-907C-08E5D9F282E0}" name="Anzahl Nachrücker" dataDxfId="95"/>
+    <tableColumn id="17" xr3:uid="{AA5430A0-8ED8-40E8-B7F8-DA25E4E8790F}" name="Seiten Anzahl" dataDxfId="94"/>
+    <tableColumn id="18" xr3:uid="{16F699D9-2741-43F3-AD5F-826A568EFEAC}" name="Absagen" dataDxfId="93"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CDBF6724-48A1-41AB-94B5-CC35C54BB15C}" name="DP_konfig6" displayName="DP_konfig6" ref="A1:U7" totalsRowShown="0" headerRowDxfId="40" dataDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CDBF6724-48A1-41AB-94B5-CC35C54BB15C}" name="BP_konfig" displayName="BP_konfig" ref="A1:U7" totalsRowShown="0" headerRowDxfId="92" dataDxfId="91">
   <autoFilter ref="A1:U7" xr:uid="{CDBF6724-48A1-41AB-94B5-CC35C54BB15C}"/>
   <tableColumns count="21">
-    <tableColumn id="1" xr3:uid="{E1FB3D0C-B874-4874-BACC-6872CF171957}" name="Tabellen Name" dataDxfId="38"/>
-    <tableColumn id="2" xr3:uid="{FFDD2777-2097-450C-B020-F133CF643855}" name="Geschlecht" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{8CF52BE2-8020-48BD-A36D-63F13A1878DE}" name="Mindest alter" dataDxfId="36"/>
-    <tableColumn id="4" xr3:uid="{FD3A030F-CD97-4B6F-8E8C-BC2E67D79F1D}" name="Maximales Alter" dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{3E22B645-D77C-4509-B031-9914FCB91599}" name="Qualizeitraum anfang" dataDxfId="34"/>
-    <tableColumn id="6" xr3:uid="{AE299324-3C1C-4063-ADF9-54555A161734}" name="Qualizeitraum Ende" dataDxfId="33"/>
-    <tableColumn id="7" xr3:uid="{DCC178B3-11FC-4C53-BBC6-C2FDA2C89857}" name="Letzter Wettkampf am" dataDxfId="32"/>
-    <tableColumn id="8" xr3:uid="{2811DB01-60A5-4BE4-B6F9-A806398A602A}" name="Wertung" dataDxfId="31"/>
-    <tableColumn id="9" xr3:uid="{0C16DAFE-847D-4E9E-9604-3A7D9FE924D0}" name="Landesverband" dataDxfId="30"/>
-    <tableColumn id="10" xr3:uid="{7A8A4101-A553-4BD5-9116-9AA5876B9401}" name="OMS" dataDxfId="29"/>
-    <tableColumn id="11" xr3:uid="{9807C9BD-6499-45F6-ACE0-4D13D64EF675}" name="Pool-Länge" dataDxfId="28"/>
-    <tableColumn id="12" xr3:uid="{13D336DD-650F-4F2C-836F-361CA1528F6D}" name="Regelwerk" dataDxfId="27"/>
-    <tableColumn id="13" xr3:uid="{66660E2D-ADF2-4FB5-8A13-004F826EE908}" name="Referenz" dataDxfId="26"/>
-    <tableColumn id="19" xr3:uid="{D72EDF8B-ECC3-4FF7-ABE6-B60BCE4A5E26}" name="Referenz Jahr" dataDxfId="25"/>
-    <tableColumn id="20" xr3:uid="{7B18E667-70F7-4BC1-AB1B-21C019F2AA89}" name="Mindest Punktzahl" dataDxfId="24"/>
-    <tableColumn id="21" xr3:uid="{FC185946-681B-42A6-AB1A-FC1EABB668C5}" name="Mindest Disziplinen" dataDxfId="23"/>
-    <tableColumn id="14" xr3:uid="{6A2676FD-2EC7-4C41-A35E-A1597A38F932}" name="3-Kampf Regel" dataDxfId="22"/>
-    <tableColumn id="15" xr3:uid="{718E0917-4F83-4A2B-832F-EBB16D5E21BF}" name="Anzahl Nominierte" dataDxfId="21"/>
-    <tableColumn id="16" xr3:uid="{5C66A461-D647-4E00-A81C-FD7AD44D7CC2}" name="Anzahl Nachrücker" dataDxfId="20"/>
-    <tableColumn id="17" xr3:uid="{D434BDEC-293B-4B4E-A5E9-479438960A03}" name="Seiten Anzahl" dataDxfId="19"/>
-    <tableColumn id="18" xr3:uid="{80908229-9247-473F-81C0-9C9D4C12FF06}" name="Absagen" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{E1FB3D0C-B874-4874-BACC-6872CF171957}" name="Tabellen Name" dataDxfId="90"/>
+    <tableColumn id="2" xr3:uid="{FFDD2777-2097-450C-B020-F133CF643855}" name="Geschlecht" dataDxfId="89"/>
+    <tableColumn id="3" xr3:uid="{8CF52BE2-8020-48BD-A36D-63F13A1878DE}" name="Mindest alter" dataDxfId="88"/>
+    <tableColumn id="4" xr3:uid="{FD3A030F-CD97-4B6F-8E8C-BC2E67D79F1D}" name="Maximales Alter" dataDxfId="87"/>
+    <tableColumn id="5" xr3:uid="{3E22B645-D77C-4509-B031-9914FCB91599}" name="Qualizeitraum anfang" dataDxfId="86"/>
+    <tableColumn id="6" xr3:uid="{AE299324-3C1C-4063-ADF9-54555A161734}" name="Qualizeitraum Ende" dataDxfId="85"/>
+    <tableColumn id="7" xr3:uid="{DCC178B3-11FC-4C53-BBC6-C2FDA2C89857}" name="Letzter Wettkampf am" dataDxfId="84"/>
+    <tableColumn id="8" xr3:uid="{2811DB01-60A5-4BE4-B6F9-A806398A602A}" name="Wertung" dataDxfId="83"/>
+    <tableColumn id="9" xr3:uid="{0C16DAFE-847D-4E9E-9604-3A7D9FE924D0}" name="Landesverband" dataDxfId="82"/>
+    <tableColumn id="10" xr3:uid="{7A8A4101-A553-4BD5-9116-9AA5876B9401}" name="OMS" dataDxfId="81"/>
+    <tableColumn id="11" xr3:uid="{9807C9BD-6499-45F6-ACE0-4D13D64EF675}" name="Pool-Länge" dataDxfId="80"/>
+    <tableColumn id="12" xr3:uid="{13D336DD-650F-4F2C-836F-361CA1528F6D}" name="Regelwerk" dataDxfId="79"/>
+    <tableColumn id="13" xr3:uid="{66660E2D-ADF2-4FB5-8A13-004F826EE908}" name="Referenz" dataDxfId="78"/>
+    <tableColumn id="19" xr3:uid="{D72EDF8B-ECC3-4FF7-ABE6-B60BCE4A5E26}" name="Referenz Jahr" dataDxfId="77"/>
+    <tableColumn id="20" xr3:uid="{7B18E667-70F7-4BC1-AB1B-21C019F2AA89}" name="Mindest Punktzahl" dataDxfId="76"/>
+    <tableColumn id="21" xr3:uid="{FC185946-681B-42A6-AB1A-FC1EABB668C5}" name="Mindest Disziplinen" dataDxfId="75"/>
+    <tableColumn id="14" xr3:uid="{6A2676FD-2EC7-4C41-A35E-A1597A38F932}" name="3-Kampf Regel" dataDxfId="74"/>
+    <tableColumn id="15" xr3:uid="{718E0917-4F83-4A2B-832F-EBB16D5E21BF}" name="Anzahl Nominierte" dataDxfId="73"/>
+    <tableColumn id="16" xr3:uid="{5C66A461-D647-4E00-A81C-FD7AD44D7CC2}" name="Anzahl Nachrücker" dataDxfId="72"/>
+    <tableColumn id="17" xr3:uid="{D434BDEC-293B-4B4E-A5E9-479438960A03}" name="Seiten Anzahl" dataDxfId="71"/>
+    <tableColumn id="18" xr3:uid="{80908229-9247-473F-81C0-9C9D4C12FF06}" name="Absagen" dataDxfId="70"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{16F87202-5A6A-4E2F-B973-3CE7EC2566C1}" name="Tabelle6" displayName="Tabelle6" ref="A1:X7" totalsRowShown="0" headerRowDxfId="52" dataDxfId="53">
+  <autoFilter ref="A1:X7" xr:uid="{16F87202-5A6A-4E2F-B973-3CE7EC2566C1}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+    <filterColumn colId="8" hiddenButton="1"/>
+    <filterColumn colId="9" hiddenButton="1"/>
+    <filterColumn colId="10" hiddenButton="1"/>
+    <filterColumn colId="11" hiddenButton="1"/>
+    <filterColumn colId="12" hiddenButton="1"/>
+    <filterColumn colId="13" hiddenButton="1"/>
+    <filterColumn colId="14" hiddenButton="1"/>
+    <filterColumn colId="15" hiddenButton="1"/>
+    <filterColumn colId="16" hiddenButton="1"/>
+    <filterColumn colId="17" hiddenButton="1"/>
+    <filterColumn colId="18" hiddenButton="1"/>
+    <filterColumn colId="19" hiddenButton="1"/>
+    <filterColumn colId="20" hiddenButton="1"/>
+    <filterColumn colId="21" hiddenButton="1"/>
+    <filterColumn colId="22" hiddenButton="1"/>
+    <filterColumn colId="23" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="24">
+    <tableColumn id="1" xr3:uid="{4847B567-64E1-4AC3-8C4B-EFCF3F00CC6C}" name="Tabellen Name" dataDxfId="69"/>
+    <tableColumn id="2" xr3:uid="{6346FF3B-B334-4CD8-8B23-F2347E29C536}" name="Geschlecht" dataDxfId="68"/>
+    <tableColumn id="3" xr3:uid="{E793B48A-BC8A-439F-8AAF-6FD08104A619}" name="Mindest Alter" dataDxfId="67"/>
+    <tableColumn id="4" xr3:uid="{01A62C29-2F75-4107-A431-F69230BCCD0C}" name="Maximales Alter" dataDxfId="66"/>
+    <tableColumn id="5" xr3:uid="{B7E4DE90-7856-4A0C-9063-61414D7F227C}" name="Qualizeitraum anfang" dataDxfId="51"/>
+    <tableColumn id="6" xr3:uid="{B00F7CD1-82CB-42B9-A396-89F79EF419CA}" name="Qualizeitraum Ende" dataDxfId="50"/>
+    <tableColumn id="7" xr3:uid="{9E50DDE5-12E3-4BCB-801C-FBABCE309F0E}" name="Letzter Wettkampf am" dataDxfId="49"/>
+    <tableColumn id="8" xr3:uid="{57E68247-0FF2-48D8-8ACD-AB057E576A21}" name="Landesverband" dataDxfId="48"/>
+    <tableColumn id="9" xr3:uid="{EBAA439D-F69A-4C2A-8193-9AE08F1E57B8}" name="OMS" dataDxfId="47"/>
+    <tableColumn id="10" xr3:uid="{BBD11E7F-3DDF-428A-B005-4A40E6FA78DC}" name="Pool-Länge" dataDxfId="46"/>
+    <tableColumn id="11" xr3:uid="{6AE38DCA-A084-4F3D-A6A4-4E76E3E2CBC6}" name="Regelwerk" dataDxfId="45"/>
+    <tableColumn id="12" xr3:uid="{7F7470AD-5502-4CEE-BB4C-44BA308E61D7}" name="Seiten Anzahl" dataDxfId="44"/>
+    <tableColumn id="13" xr3:uid="{F416CBFA-4C9D-45CD-9BA7-E4BC57A08BC2}" name="PZ1 - 50m Retten" dataDxfId="65"/>
+    <tableColumn id="14" xr3:uid="{7117DBCA-0DA7-462C-84FE-0DC7E33B124C}" name="PZ1 - 100m Retten" dataDxfId="64"/>
+    <tableColumn id="15" xr3:uid="{E8630E91-DC30-4822-9E53-6D65487C3670}" name="PZ1 - 100m Kombi" dataDxfId="63"/>
+    <tableColumn id="16" xr3:uid="{4B3AA225-E042-430F-8259-D176887B4528}" name="PZ1 - 100m Lifesaver" dataDxfId="62"/>
+    <tableColumn id="17" xr3:uid="{798674BD-98CE-4531-BDFF-6AB06253AD7C}" name="PZ1 - 200m Super-Lifesaver" dataDxfId="61"/>
+    <tableColumn id="18" xr3:uid="{8809BB71-D58B-4E8B-A442-D0EB9A65A25D}" name="PZ1 - 200m Hindernis" dataDxfId="60"/>
+    <tableColumn id="19" xr3:uid="{93DCF463-806B-4117-B4E3-1FFAE976B37C}" name="PZ2 - 50m Retten" dataDxfId="59"/>
+    <tableColumn id="20" xr3:uid="{A514C961-559E-462F-B143-BA30974C0129}" name="PZ2 - 100m Retten" dataDxfId="58"/>
+    <tableColumn id="21" xr3:uid="{F1CF6143-45FE-498D-93D6-36F26D2F3C0B}" name="PZ2 - 100m Kombi" dataDxfId="57"/>
+    <tableColumn id="22" xr3:uid="{E90962FC-C214-467F-841F-40DF60E41456}" name="PZ2 - 100m Lifesaver" dataDxfId="56"/>
+    <tableColumn id="23" xr3:uid="{7FBC6334-C4C8-4B38-9F59-30ED95A44379}" name="PZ2 - 200m Super-Lifesaver" dataDxfId="55"/>
+    <tableColumn id="24" xr3:uid="{231BFF86-8F3A-4BA1-B25E-28175D9EDFA9}" name="PZ2 - 200m Hindernis" dataDxfId="54"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{38173103-C137-4989-84EA-9BDFE7009E50}" name="Tabelle68" displayName="Tabelle68" ref="A1:X3" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+  <autoFilter ref="A1:X3" xr:uid="{38173103-C137-4989-84EA-9BDFE7009E50}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+    <filterColumn colId="8" hiddenButton="1"/>
+    <filterColumn colId="9" hiddenButton="1"/>
+    <filterColumn colId="10" hiddenButton="1"/>
+    <filterColumn colId="11" hiddenButton="1"/>
+    <filterColumn colId="12" hiddenButton="1"/>
+    <filterColumn colId="13" hiddenButton="1"/>
+    <filterColumn colId="14" hiddenButton="1"/>
+    <filterColumn colId="15" hiddenButton="1"/>
+    <filterColumn colId="16" hiddenButton="1"/>
+    <filterColumn colId="17" hiddenButton="1"/>
+    <filterColumn colId="18" hiddenButton="1"/>
+    <filterColumn colId="19" hiddenButton="1"/>
+    <filterColumn colId="20" hiddenButton="1"/>
+    <filterColumn colId="21" hiddenButton="1"/>
+    <filterColumn colId="22" hiddenButton="1"/>
+    <filterColumn colId="23" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="24">
+    <tableColumn id="1" xr3:uid="{EC191D47-103E-4808-B80B-20281F480A7B}" name="Tabellen Name" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{B4135B5F-F957-45A0-BE67-B4F753711A01}" name="Geschlecht" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{3E8C5D70-845D-4A0C-8911-63692B806EE3}" name="Mindest Alter" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{951555AA-1D48-4F58-84DA-5A388BC7ACA6}" name="Maximales Alter" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{532345E9-A3F4-4BC3-83A4-BBE007D5BF2F}" name="Qualizeitraum anfang" dataDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{71A6260E-6437-4311-B1E5-334D777DE23B}" name="Qualizeitraum Ende" dataDxfId="36"/>
+    <tableColumn id="7" xr3:uid="{C4D53DE9-9819-4221-8397-DAA183E26E63}" name="Letzter Wettkampf am" dataDxfId="35"/>
+    <tableColumn id="8" xr3:uid="{8A29AFA5-6619-4699-AB42-78F4AD5566E1}" name="Landesverband" dataDxfId="34"/>
+    <tableColumn id="9" xr3:uid="{9AB45004-0EB4-4304-AFD0-4496973A950F}" name="OMS" dataDxfId="33"/>
+    <tableColumn id="10" xr3:uid="{71319762-F54F-4493-84F3-802DFD3DE0D2}" name="Pool-Länge" dataDxfId="32"/>
+    <tableColumn id="11" xr3:uid="{E91F6E89-282A-4B79-A6DF-C43103E9413B}" name="Regelwerk" dataDxfId="31"/>
+    <tableColumn id="12" xr3:uid="{D4638146-A857-41ED-83D1-8E2711E1ED0F}" name="Seiten Anzahl" dataDxfId="30"/>
+    <tableColumn id="13" xr3:uid="{08DB5C03-8197-4058-AF4C-5A2A8CB975EF}" name="PZ1 - 50m Retten" dataDxfId="29"/>
+    <tableColumn id="14" xr3:uid="{94966042-A021-4D1B-83E0-516EF43C47BF}" name="PZ1 - 100m Retten" dataDxfId="28"/>
+    <tableColumn id="15" xr3:uid="{3D118CE3-B383-4B67-8BD7-A4E7270B694D}" name="PZ1 - 100m Kombi" dataDxfId="27"/>
+    <tableColumn id="16" xr3:uid="{2EF5524D-F52F-403A-B1F2-26B06E1561D7}" name="PZ1 - 100m Lifesaver" dataDxfId="26"/>
+    <tableColumn id="17" xr3:uid="{90AFAED0-E3F7-430F-B477-A7B8C0F28C92}" name="PZ1 - 200m Super-Lifesaver" dataDxfId="25"/>
+    <tableColumn id="18" xr3:uid="{234BF89C-A472-4472-A7B5-6E8956546AEB}" name="PZ1 - 200m Hindernis" dataDxfId="24"/>
+    <tableColumn id="19" xr3:uid="{0630350F-8319-4C46-926A-11BAE7DA4892}" name="PZ2 - 50m Retten" dataDxfId="23"/>
+    <tableColumn id="20" xr3:uid="{923F9722-E09F-460A-8B02-64E9F03F0806}" name="PZ2 - 100m Retten" dataDxfId="22"/>
+    <tableColumn id="21" xr3:uid="{AA307655-1197-43FB-A00A-75C1438B2412}" name="PZ2 - 100m Kombi" dataDxfId="21"/>
+    <tableColumn id="22" xr3:uid="{92C209F1-CAD1-4D8C-888D-8F65EE77FFDE}" name="PZ2 - 100m Lifesaver" dataDxfId="20"/>
+    <tableColumn id="23" xr3:uid="{AE53DAA0-7669-4EC4-A7F2-6BFCE8E6960F}" name="PZ2 - 200m Super-Lifesaver" dataDxfId="19"/>
+    <tableColumn id="24" xr3:uid="{AB5DE385-0AE1-401A-8EF5-9ED15B7100C9}" name="PZ2 - 200m Hindernis" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7684,13 +8021,809 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{453761C1-FFCA-45E5-8C71-AB7C914C935B}">
+  <sheetPr codeName="Tabelle5">
+    <tabColor theme="4"/>
+  </sheetPr>
+  <dimension ref="A1:N39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="16.86328125" style="1" customWidth="1"/>
+    <col min="2" max="13" width="18.73046875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="25" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="11.3984375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="18">
+        <v>2026</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(B$1))*86400,2)</f>
+        <v>44.41</v>
+      </c>
+      <c r="C2" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(C$1))*86400,2)</f>
+        <v>65.53</v>
+      </c>
+      <c r="D2" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(D$1))*86400,2)</f>
+        <v>91.79</v>
+      </c>
+      <c r="E2" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(E$1))*86400,2)</f>
+        <v>75.84</v>
+      </c>
+      <c r="F2" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(F$1))*86400,2)</f>
+        <v>189.05</v>
+      </c>
+      <c r="G2" s="27">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(G$1))*86400,2)</f>
+        <v>164.57</v>
+      </c>
+      <c r="H2" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(H$1))*86400,2)</f>
+        <v>38.36</v>
+      </c>
+      <c r="I2" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(I$1))*86400,2)</f>
+        <v>60.47</v>
+      </c>
+      <c r="J2" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(J$1))*86400,2)</f>
+        <v>79.22</v>
+      </c>
+      <c r="K2" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(K$1))*86400,2)</f>
+        <v>66.430000000000007</v>
+      </c>
+      <c r="L2" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(L$1))*86400,2)</f>
+        <v>168.79</v>
+      </c>
+      <c r="M2" s="15">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(M$1))*86400,2)</f>
+        <v>155.07</v>
+      </c>
+      <c r="N2" s="2">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="16">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(B$1))*86400,2)</f>
+        <v>43.12</v>
+      </c>
+      <c r="C3" s="16">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(C$1))*86400,2)</f>
+        <v>63.63</v>
+      </c>
+      <c r="D3" s="16">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(D$1))*86400,2)</f>
+        <v>89.13</v>
+      </c>
+      <c r="E3" s="16">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(E$1))*86400,2)</f>
+        <v>73.63</v>
+      </c>
+      <c r="F3" s="16">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(F$1))*86400,2)</f>
+        <v>183.57</v>
+      </c>
+      <c r="G3" s="28">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(G$1))*86400,2)</f>
+        <v>159.79</v>
+      </c>
+      <c r="H3" s="16">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(H$1))*86400,2)</f>
+        <v>37.25</v>
+      </c>
+      <c r="I3" s="16">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(I$1))*86400,2)</f>
+        <v>58.71</v>
+      </c>
+      <c r="J3" s="16">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(J$1))*86400,2)</f>
+        <v>76.92</v>
+      </c>
+      <c r="K3" s="16">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(K$1))*86400,2)</f>
+        <v>64.5</v>
+      </c>
+      <c r="L3" s="16">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(L$1))*86400,2)</f>
+        <v>163.9</v>
+      </c>
+      <c r="M3" s="17">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(M$1))*86400,2)</f>
+        <v>150.57</v>
+      </c>
+      <c r="N3" s="2">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(B$1))*86400,2)</f>
+        <v>41.13</v>
+      </c>
+      <c r="C4" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(C$1))*86400,2)</f>
+        <v>62.97</v>
+      </c>
+      <c r="D4" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(D$1))*86400,2)</f>
+        <v>83.98</v>
+      </c>
+      <c r="E4" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(E$1))*86400,2)</f>
+        <v>70.290000000000006</v>
+      </c>
+      <c r="F4" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(F$1))*86400,2)</f>
+        <v>173.81</v>
+      </c>
+      <c r="G4" s="27">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(G$1))*86400,2)</f>
+        <v>155.68</v>
+      </c>
+      <c r="H4" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(H$1))*86400,2)</f>
+        <v>34.74</v>
+      </c>
+      <c r="I4" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(I$1))*86400,2)</f>
+        <v>56.16</v>
+      </c>
+      <c r="J4" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(J$1))*86400,2)</f>
+        <v>73.650000000000006</v>
+      </c>
+      <c r="K4" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(K$1))*86400,2)</f>
+        <v>60.9</v>
+      </c>
+      <c r="L4" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(L$1))*86400,2)</f>
+        <v>157.09</v>
+      </c>
+      <c r="M4" s="15">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(M$1))*86400,2)</f>
+        <v>142.72</v>
+      </c>
+      <c r="N4" s="2">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A7" s="62" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="62"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="62"/>
+      <c r="K7" s="62"/>
+      <c r="L7" s="62"/>
+      <c r="M7" s="62"/>
+      <c r="N7" s="62"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A8" s="62"/>
+      <c r="B8" s="62"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="62"/>
+      <c r="F8" s="62"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="62"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="62"/>
+      <c r="L8" s="62"/>
+      <c r="M8" s="62"/>
+      <c r="N8" s="62"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A9" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="31" t="str">
+        <f t="shared" ref="B9:M11" si="0">CONCATENATE(ROUNDDOWN(B2/60,0),":",TEXT(B2-(60*ROUNDDOWN(B2/60,0)),"00,00"))</f>
+        <v>0:44,41</v>
+      </c>
+      <c r="C9" s="31" t="str">
+        <f>CONCATENATE(ROUNDDOWN(C2/60,0),":",TEXT(C2-(60*ROUNDDOWN(C2/60,0)),"00,00"))</f>
+        <v>1:05,53</v>
+      </c>
+      <c r="D9" s="31" t="str">
+        <f t="shared" ref="D9:M9" si="1">CONCATENATE(ROUNDDOWN(D2/60,0),":",TEXT(D2-(60*ROUNDDOWN(D2/60,0)),"00,00"))</f>
+        <v>1:31,79</v>
+      </c>
+      <c r="E9" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v>1:15,84</v>
+      </c>
+      <c r="F9" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v>3:09,05</v>
+      </c>
+      <c r="G9" s="32" t="str">
+        <f t="shared" si="1"/>
+        <v>2:44,57</v>
+      </c>
+      <c r="H9" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v>0:38,36</v>
+      </c>
+      <c r="I9" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v>1:00,47</v>
+      </c>
+      <c r="J9" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v>1:19,22</v>
+      </c>
+      <c r="K9" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v>1:06,43</v>
+      </c>
+      <c r="L9" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v>2:48,79</v>
+      </c>
+      <c r="M9" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v>2:35,07</v>
+      </c>
+      <c r="N9" s="21"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A10" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>0:43,12</v>
+      </c>
+      <c r="C10" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>1:03,63</v>
+      </c>
+      <c r="D10" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>1:29,13</v>
+      </c>
+      <c r="E10" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>1:13,63</v>
+      </c>
+      <c r="F10" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>3:03,57</v>
+      </c>
+      <c r="G10" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>2:39,79</v>
+      </c>
+      <c r="H10" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>0:37,25</v>
+      </c>
+      <c r="I10" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>0:58,71</v>
+      </c>
+      <c r="J10" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>1:16,92</v>
+      </c>
+      <c r="K10" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>1:04,50</v>
+      </c>
+      <c r="L10" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>2:43,90</v>
+      </c>
+      <c r="M10" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>2:30,57</v>
+      </c>
+      <c r="N10" s="21"/>
+    </row>
+    <row r="11" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>0:41,13</v>
+      </c>
+      <c r="C11" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>1:02,97</v>
+      </c>
+      <c r="D11" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>1:23,98</v>
+      </c>
+      <c r="E11" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>1:10,29</v>
+      </c>
+      <c r="F11" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>2:53,81</v>
+      </c>
+      <c r="G11" s="30" t="str">
+        <f t="shared" si="0"/>
+        <v>2:35,68</v>
+      </c>
+      <c r="H11" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>0:34,74</v>
+      </c>
+      <c r="I11" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>0:56,16</v>
+      </c>
+      <c r="J11" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>1:13,65</v>
+      </c>
+      <c r="K11" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>1:00,90</v>
+      </c>
+      <c r="L11" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>2:37,09</v>
+      </c>
+      <c r="M11" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>2:22,72</v>
+      </c>
+      <c r="N11" s="23"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A14" s="61" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="61"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
+      <c r="H14" s="63" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" s="63"/>
+      <c r="J14" s="63"/>
+      <c r="L14" s="63" t="s">
+        <v>36</v>
+      </c>
+      <c r="M14"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A15" s="61"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="61"/>
+      <c r="H15" s="63"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="63"/>
+      <c r="L15" s="63"/>
+      <c r="M15"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M16"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A17" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="8">
+        <v>15</v>
+      </c>
+      <c r="C17" s="8">
+        <v>18</v>
+      </c>
+      <c r="D17" s="8">
+        <v>3</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L17" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="M17"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A18" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="9">
+        <v>13</v>
+      </c>
+      <c r="C18" s="9">
+        <v>14</v>
+      </c>
+      <c r="D18" s="9">
+        <v>1</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="I18" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="J18" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="L18" s="38"/>
+      <c r="M18"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A19" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="8">
+        <v>12</v>
+      </c>
+      <c r="C19" s="8">
+        <v>18</v>
+      </c>
+      <c r="D19" s="8">
+        <v>16</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="I19" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="J19" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="L19" s="36"/>
+      <c r="M19"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A20" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="9">
+        <v>12</v>
+      </c>
+      <c r="C20" s="9">
+        <v>18</v>
+      </c>
+      <c r="D20" s="9">
+        <v>10</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H20" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="I20" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="J20" s="35"/>
+      <c r="L20" s="38"/>
+      <c r="M20"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A21" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="8">
+        <v>12</v>
+      </c>
+      <c r="C21" s="8">
+        <v>100</v>
+      </c>
+      <c r="D21" s="8">
+        <v>8</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H21" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="I21" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="J21" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="L21" s="36"/>
+      <c r="M21"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A22" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="9">
+        <v>17</v>
+      </c>
+      <c r="C22" s="9">
+        <v>18</v>
+      </c>
+      <c r="D22" s="9">
+        <v>1</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H22" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="I22" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="J22" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L22" s="39"/>
+      <c r="M22"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A23" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="8">
+        <v>19</v>
+      </c>
+      <c r="C23" s="8">
+        <v>100</v>
+      </c>
+      <c r="D23" s="8">
+        <v>4</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H23" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="I23" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="J23" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="L23" s="37"/>
+      <c r="M23"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
+      <c r="L24" s="39"/>
+      <c r="M24"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="L25" s="37"/>
+      <c r="M25"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="L26" s="39"/>
+      <c r="M26"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="L27" s="37"/>
+      <c r="M27"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="L28" s="39"/>
+      <c r="M28"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="L29" s="37"/>
+      <c r="M29"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="L30" s="39"/>
+      <c r="M30"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="L31" s="37"/>
+      <c r="M31"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="L32" s="39"/>
+      <c r="M32"/>
+    </row>
+    <row r="33" spans="8:13" x14ac:dyDescent="0.45">
+      <c r="L33" s="37"/>
+      <c r="M33"/>
+    </row>
+    <row r="34" spans="8:13" x14ac:dyDescent="0.45">
+      <c r="L34" s="39"/>
+      <c r="M34"/>
+    </row>
+    <row r="35" spans="8:13" x14ac:dyDescent="0.45">
+      <c r="M35"/>
+    </row>
+    <row r="36" spans="8:13" x14ac:dyDescent="0.45">
+      <c r="L36" s="39"/>
+      <c r="M36"/>
+    </row>
+    <row r="37" spans="8:13" x14ac:dyDescent="0.45">
+      <c r="M37"/>
+    </row>
+    <row r="38" spans="8:13" x14ac:dyDescent="0.45">
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="J38"/>
+      <c r="K38"/>
+      <c r="L38"/>
+      <c r="M38"/>
+    </row>
+    <row r="39" spans="8:13" x14ac:dyDescent="0.45">
+      <c r="H39"/>
+      <c r="I39"/>
+      <c r="J39"/>
+      <c r="K39"/>
+      <c r="L39"/>
+      <c r="M39"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A7:N8"/>
+    <mergeCell ref="A14:F15"/>
+    <mergeCell ref="H14:J15"/>
+    <mergeCell ref="L14:L15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EB2B168-68B3-410F-B4A6-8D511F9C32E0}">
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8716,8 +9849,8 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10070,7 +11203,7 @@
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10298,8 +11431,8 @@
   </sheetPr>
   <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="U4" sqref="U4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10759,6 +11892,616 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26A97B8-4E61-4811-AFAC-69F978DDEBB3}">
+  <sheetPr>
+    <tabColor theme="5"/>
+  </sheetPr>
+  <dimension ref="A1:X7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.06640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.46484375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.53125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.46484375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.06640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.1328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.796875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.86328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.1328125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="24.796875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.86328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A1" s="59" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="59" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" s="59" t="s">
+        <v>204</v>
+      </c>
+      <c r="D1" s="59" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="59" t="s">
+        <v>165</v>
+      </c>
+      <c r="F1" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="G1" s="59" t="s">
+        <v>167</v>
+      </c>
+      <c r="H1" s="59" t="s">
+        <v>168</v>
+      </c>
+      <c r="I1" s="59" t="s">
+        <v>170</v>
+      </c>
+      <c r="J1" s="59" t="s">
+        <v>169</v>
+      </c>
+      <c r="K1" s="59" t="s">
+        <v>171</v>
+      </c>
+      <c r="L1" s="59" t="s">
+        <v>176</v>
+      </c>
+      <c r="M1" s="59" t="s">
+        <v>205</v>
+      </c>
+      <c r="N1" s="59" t="s">
+        <v>206</v>
+      </c>
+      <c r="O1" s="59" t="s">
+        <v>207</v>
+      </c>
+      <c r="P1" s="59" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q1" s="59" t="s">
+        <v>209</v>
+      </c>
+      <c r="R1" s="59" t="s">
+        <v>208</v>
+      </c>
+      <c r="S1" s="59" t="s">
+        <v>211</v>
+      </c>
+      <c r="T1" s="59" t="s">
+        <v>212</v>
+      </c>
+      <c r="U1" s="59" t="s">
+        <v>213</v>
+      </c>
+      <c r="V1" s="59" t="s">
+        <v>214</v>
+      </c>
+      <c r="W1" s="59" t="s">
+        <v>215</v>
+      </c>
+      <c r="X1" s="59" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A2" s="59" t="s">
+        <v>219</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>164</v>
+      </c>
+      <c r="C2" s="59">
+        <v>15</v>
+      </c>
+      <c r="D2" s="59">
+        <v>16</v>
+      </c>
+      <c r="E2" s="59" t="s">
+        <v>188</v>
+      </c>
+      <c r="F2" s="59" t="s">
+        <v>223</v>
+      </c>
+      <c r="G2" s="59" t="s">
+        <v>188</v>
+      </c>
+      <c r="H2" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="I2" s="59" t="s">
+        <v>179</v>
+      </c>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59">
+        <v>200</v>
+      </c>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="59"/>
+      <c r="R2" s="59"/>
+      <c r="S2" s="59"/>
+      <c r="T2" s="59"/>
+      <c r="U2" s="59"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="59"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A3" s="59" t="s">
+        <v>220</v>
+      </c>
+      <c r="B3" s="59" t="s">
+        <v>182</v>
+      </c>
+      <c r="C3" s="59">
+        <v>15</v>
+      </c>
+      <c r="D3" s="59">
+        <v>16</v>
+      </c>
+      <c r="E3" s="59" t="s">
+        <v>188</v>
+      </c>
+      <c r="F3" s="59" t="s">
+        <v>223</v>
+      </c>
+      <c r="G3" s="59" t="s">
+        <v>188</v>
+      </c>
+      <c r="H3" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="I3" s="59" t="s">
+        <v>179</v>
+      </c>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59">
+        <v>200</v>
+      </c>
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="59"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59"/>
+      <c r="R3" s="59"/>
+      <c r="S3" s="59"/>
+      <c r="T3" s="59"/>
+      <c r="U3" s="59"/>
+      <c r="V3" s="59"/>
+      <c r="W3" s="59"/>
+      <c r="X3" s="59"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A4" s="59" t="s">
+        <v>221</v>
+      </c>
+      <c r="B4" s="59" t="s">
+        <v>164</v>
+      </c>
+      <c r="C4" s="59">
+        <v>17</v>
+      </c>
+      <c r="D4" s="59">
+        <v>18</v>
+      </c>
+      <c r="E4" s="59" t="s">
+        <v>188</v>
+      </c>
+      <c r="F4" s="59" t="s">
+        <v>223</v>
+      </c>
+      <c r="G4" s="59" t="s">
+        <v>188</v>
+      </c>
+      <c r="H4" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="I4" s="59" t="s">
+        <v>179</v>
+      </c>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59">
+        <v>200</v>
+      </c>
+      <c r="M4" s="59"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="59"/>
+      <c r="Q4" s="59"/>
+      <c r="R4" s="59"/>
+      <c r="S4" s="59"/>
+      <c r="T4" s="59"/>
+      <c r="U4" s="59"/>
+      <c r="V4" s="59"/>
+      <c r="W4" s="59"/>
+      <c r="X4" s="59"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A5" s="59" t="s">
+        <v>222</v>
+      </c>
+      <c r="B5" s="59" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" s="59">
+        <v>17</v>
+      </c>
+      <c r="D5" s="59">
+        <v>18</v>
+      </c>
+      <c r="E5" s="59" t="s">
+        <v>188</v>
+      </c>
+      <c r="F5" s="59" t="s">
+        <v>223</v>
+      </c>
+      <c r="G5" s="59" t="s">
+        <v>188</v>
+      </c>
+      <c r="H5" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="I5" s="59" t="s">
+        <v>179</v>
+      </c>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59">
+        <v>200</v>
+      </c>
+      <c r="M5" s="59"/>
+      <c r="N5" s="59"/>
+      <c r="O5" s="59"/>
+      <c r="P5" s="59"/>
+      <c r="Q5" s="59"/>
+      <c r="R5" s="59"/>
+      <c r="S5" s="59"/>
+      <c r="T5" s="59"/>
+      <c r="U5" s="59"/>
+      <c r="V5" s="59"/>
+      <c r="W5" s="59"/>
+      <c r="X5" s="59"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A6" s="59" t="s">
+        <v>190</v>
+      </c>
+      <c r="B6" s="59" t="s">
+        <v>164</v>
+      </c>
+      <c r="C6" s="59">
+        <v>19</v>
+      </c>
+      <c r="D6" s="59">
+        <v>100</v>
+      </c>
+      <c r="E6" s="59" t="s">
+        <v>188</v>
+      </c>
+      <c r="F6" s="59" t="s">
+        <v>223</v>
+      </c>
+      <c r="G6" s="59" t="s">
+        <v>188</v>
+      </c>
+      <c r="H6" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="I6" s="59" t="s">
+        <v>179</v>
+      </c>
+      <c r="J6" s="59"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="59">
+        <v>200</v>
+      </c>
+      <c r="M6" s="59"/>
+      <c r="N6" s="59"/>
+      <c r="O6" s="59"/>
+      <c r="P6" s="59"/>
+      <c r="Q6" s="59"/>
+      <c r="R6" s="59"/>
+      <c r="S6" s="59"/>
+      <c r="T6" s="59"/>
+      <c r="U6" s="59"/>
+      <c r="V6" s="59"/>
+      <c r="W6" s="59"/>
+      <c r="X6" s="59"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A7" s="59" t="s">
+        <v>191</v>
+      </c>
+      <c r="B7" s="59" t="s">
+        <v>182</v>
+      </c>
+      <c r="C7" s="59">
+        <v>19</v>
+      </c>
+      <c r="D7" s="59">
+        <v>100</v>
+      </c>
+      <c r="E7" s="59" t="s">
+        <v>188</v>
+      </c>
+      <c r="F7" s="59" t="s">
+        <v>223</v>
+      </c>
+      <c r="G7" s="59" t="s">
+        <v>188</v>
+      </c>
+      <c r="H7" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="I7" s="59" t="s">
+        <v>179</v>
+      </c>
+      <c r="J7" s="59"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="59">
+        <v>200</v>
+      </c>
+      <c r="M7" s="59"/>
+      <c r="N7" s="59"/>
+      <c r="O7" s="59"/>
+      <c r="P7" s="59"/>
+      <c r="Q7" s="59"/>
+      <c r="R7" s="59"/>
+      <c r="S7" s="59"/>
+      <c r="T7" s="59"/>
+      <c r="U7" s="59"/>
+      <c r="V7" s="59"/>
+      <c r="W7" s="59"/>
+      <c r="X7" s="59"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B608451-5D1D-4665-BFE6-00A11E29A180}">
+  <sheetPr>
+    <tabColor theme="5"/>
+  </sheetPr>
+  <dimension ref="A1:X3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="17.06640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.06640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.9296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.59765625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.59765625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="27" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.06640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.59765625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.59765625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="27" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="22.06640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A1" s="59" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="59" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" s="59" t="s">
+        <v>204</v>
+      </c>
+      <c r="D1" s="59" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="59" t="s">
+        <v>165</v>
+      </c>
+      <c r="F1" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="G1" s="59" t="s">
+        <v>167</v>
+      </c>
+      <c r="H1" s="59" t="s">
+        <v>168</v>
+      </c>
+      <c r="I1" s="59" t="s">
+        <v>170</v>
+      </c>
+      <c r="J1" s="59" t="s">
+        <v>169</v>
+      </c>
+      <c r="K1" s="59" t="s">
+        <v>171</v>
+      </c>
+      <c r="L1" s="59" t="s">
+        <v>176</v>
+      </c>
+      <c r="M1" s="59" t="s">
+        <v>205</v>
+      </c>
+      <c r="N1" s="59" t="s">
+        <v>206</v>
+      </c>
+      <c r="O1" s="59" t="s">
+        <v>207</v>
+      </c>
+      <c r="P1" s="59" t="s">
+        <v>210</v>
+      </c>
+      <c r="Q1" s="59" t="s">
+        <v>209</v>
+      </c>
+      <c r="R1" s="59" t="s">
+        <v>208</v>
+      </c>
+      <c r="S1" s="59" t="s">
+        <v>211</v>
+      </c>
+      <c r="T1" s="59" t="s">
+        <v>212</v>
+      </c>
+      <c r="U1" s="59" t="s">
+        <v>213</v>
+      </c>
+      <c r="V1" s="59" t="s">
+        <v>214</v>
+      </c>
+      <c r="W1" s="59" t="s">
+        <v>215</v>
+      </c>
+      <c r="X1" s="59" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A2" s="59" t="s">
+        <v>217</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>164</v>
+      </c>
+      <c r="C2" s="59">
+        <v>15</v>
+      </c>
+      <c r="D2" s="59">
+        <v>18</v>
+      </c>
+      <c r="E2" s="59" t="s">
+        <v>188</v>
+      </c>
+      <c r="F2" s="59" t="s">
+        <v>224</v>
+      </c>
+      <c r="G2" s="59" t="s">
+        <v>200</v>
+      </c>
+      <c r="H2" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="I2" s="59" t="s">
+        <v>180</v>
+      </c>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59">
+        <v>200</v>
+      </c>
+      <c r="M2" s="59"/>
+      <c r="N2" s="59"/>
+      <c r="O2" s="59"/>
+      <c r="P2" s="59"/>
+      <c r="Q2" s="59"/>
+      <c r="R2" s="59"/>
+      <c r="S2" s="59"/>
+      <c r="T2" s="59"/>
+      <c r="U2" s="59"/>
+      <c r="V2" s="59"/>
+      <c r="W2" s="59"/>
+      <c r="X2" s="59"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A3" s="59" t="s">
+        <v>218</v>
+      </c>
+      <c r="B3" s="59" t="s">
+        <v>182</v>
+      </c>
+      <c r="C3" s="59">
+        <v>15</v>
+      </c>
+      <c r="D3" s="59">
+        <v>18</v>
+      </c>
+      <c r="E3" s="59" t="s">
+        <v>188</v>
+      </c>
+      <c r="F3" s="59" t="s">
+        <v>224</v>
+      </c>
+      <c r="G3" s="59" t="s">
+        <v>200</v>
+      </c>
+      <c r="H3" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="I3" s="59" t="s">
+        <v>180</v>
+      </c>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59">
+        <v>200</v>
+      </c>
+      <c r="M3" s="59"/>
+      <c r="N3" s="59"/>
+      <c r="O3" s="59"/>
+      <c r="P3" s="59"/>
+      <c r="Q3" s="59"/>
+      <c r="R3" s="59"/>
+      <c r="S3" s="59"/>
+      <c r="T3" s="59"/>
+      <c r="U3" s="59"/>
+      <c r="V3" s="59"/>
+      <c r="W3" s="59"/>
+      <c r="X3" s="59"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3E1FA05-76A3-4AE3-B1B5-E78B06AE489F}">
   <sheetPr codeName="Tabelle3">
     <tabColor theme="1"/>
@@ -11519,7 +13262,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7831D901-68D8-4F92-82B6-BCB1A3899285}">
   <sheetPr codeName="Tabelle4">
     <tabColor theme="4"/>
@@ -12313,800 +14056,4 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{453761C1-FFCA-45E5-8C71-AB7C914C935B}">
-  <sheetPr codeName="Tabelle5">
-    <tabColor theme="4"/>
-  </sheetPr>
-  <dimension ref="A1:N39"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="16.86328125" style="1" customWidth="1"/>
-    <col min="2" max="13" width="18.73046875" style="1" customWidth="1"/>
-    <col min="14" max="14" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="11.3984375" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="18">
-        <v>2026</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(B$1))*86400,2)</f>
-        <v>44.41</v>
-      </c>
-      <c r="C2" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(C$1))*86400,2)</f>
-        <v>65.53</v>
-      </c>
-      <c r="D2" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(D$1))*86400,2)</f>
-        <v>91.79</v>
-      </c>
-      <c r="E2" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(E$1))*86400,2)</f>
-        <v>75.84</v>
-      </c>
-      <c r="F2" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(F$1))*86400,2)</f>
-        <v>189.05</v>
-      </c>
-      <c r="G2" s="27">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(G$1))*86400,2)</f>
-        <v>164.57</v>
-      </c>
-      <c r="H2" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(H$1))*86400,2)</f>
-        <v>38.36</v>
-      </c>
-      <c r="I2" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(I$1))*86400,2)</f>
-        <v>60.47</v>
-      </c>
-      <c r="J2" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(J$1))*86400,2)</f>
-        <v>79.22</v>
-      </c>
-      <c r="K2" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(K$1))*86400,2)</f>
-        <v>66.430000000000007</v>
-      </c>
-      <c r="L2" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(L$1))*86400,2)</f>
-        <v>168.79</v>
-      </c>
-      <c r="M2" s="15">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(M$1))*86400,2)</f>
-        <v>155.07</v>
-      </c>
-      <c r="N2" s="2">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="16">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(B$1))*86400,2)</f>
-        <v>43.12</v>
-      </c>
-      <c r="C3" s="16">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(C$1))*86400,2)</f>
-        <v>63.63</v>
-      </c>
-      <c r="D3" s="16">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(D$1))*86400,2)</f>
-        <v>89.13</v>
-      </c>
-      <c r="E3" s="16">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(E$1))*86400,2)</f>
-        <v>73.63</v>
-      </c>
-      <c r="F3" s="16">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(F$1))*86400,2)</f>
-        <v>183.57</v>
-      </c>
-      <c r="G3" s="28">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(G$1))*86400,2)</f>
-        <v>159.79</v>
-      </c>
-      <c r="H3" s="16">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(H$1))*86400,2)</f>
-        <v>37.25</v>
-      </c>
-      <c r="I3" s="16">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(I$1))*86400,2)</f>
-        <v>58.71</v>
-      </c>
-      <c r="J3" s="16">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(J$1))*86400,2)</f>
-        <v>76.92</v>
-      </c>
-      <c r="K3" s="16">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(K$1))*86400,2)</f>
-        <v>64.5</v>
-      </c>
-      <c r="L3" s="16">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(L$1))*86400,2)</f>
-        <v>163.9</v>
-      </c>
-      <c r="M3" s="17">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(M$1))*86400,2)</f>
-        <v>150.57</v>
-      </c>
-      <c r="N3" s="2">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(B$1))*86400,2)</f>
-        <v>41.13</v>
-      </c>
-      <c r="C4" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(C$1))*86400,2)</f>
-        <v>62.97</v>
-      </c>
-      <c r="D4" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(D$1))*86400,2)</f>
-        <v>83.98</v>
-      </c>
-      <c r="E4" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(E$1))*86400,2)</f>
-        <v>70.290000000000006</v>
-      </c>
-      <c r="F4" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(F$1))*86400,2)</f>
-        <v>173.81</v>
-      </c>
-      <c r="G4" s="27">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(G$1))*86400,2)</f>
-        <v>155.68</v>
-      </c>
-      <c r="H4" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(H$1))*86400,2)</f>
-        <v>34.74</v>
-      </c>
-      <c r="I4" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(I$1))*86400,2)</f>
-        <v>56.16</v>
-      </c>
-      <c r="J4" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(J$1))*86400,2)</f>
-        <v>73.650000000000006</v>
-      </c>
-      <c r="K4" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(K$1))*86400,2)</f>
-        <v>60.9</v>
-      </c>
-      <c r="L4" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(L$1))*86400,2)</f>
-        <v>157.09</v>
-      </c>
-      <c r="M4" s="15">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(M$1))*86400,2)</f>
-        <v>142.72</v>
-      </c>
-      <c r="N4" s="2">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A7" s="62" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="62"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="62"/>
-      <c r="J7" s="62"/>
-      <c r="K7" s="62"/>
-      <c r="L7" s="62"/>
-      <c r="M7" s="62"/>
-      <c r="N7" s="62"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A8" s="62"/>
-      <c r="B8" s="62"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="62"/>
-      <c r="E8" s="62"/>
-      <c r="F8" s="62"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="62"/>
-      <c r="I8" s="62"/>
-      <c r="J8" s="62"/>
-      <c r="K8" s="62"/>
-      <c r="L8" s="62"/>
-      <c r="M8" s="62"/>
-      <c r="N8" s="62"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A9" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="31" t="str">
-        <f t="shared" ref="B9:M11" si="0">CONCATENATE(ROUNDDOWN(B2/60,0),":",TEXT(B2-(60*ROUNDDOWN(B2/60,0)),"00,00"))</f>
-        <v>0:44,41</v>
-      </c>
-      <c r="C9" s="31" t="str">
-        <f>CONCATENATE(ROUNDDOWN(C2/60,0),":",TEXT(C2-(60*ROUNDDOWN(C2/60,0)),"00,00"))</f>
-        <v>1:05,53</v>
-      </c>
-      <c r="D9" s="31" t="str">
-        <f t="shared" ref="D9:M9" si="1">CONCATENATE(ROUNDDOWN(D2/60,0),":",TEXT(D2-(60*ROUNDDOWN(D2/60,0)),"00,00"))</f>
-        <v>1:31,79</v>
-      </c>
-      <c r="E9" s="31" t="str">
-        <f t="shared" si="1"/>
-        <v>1:15,84</v>
-      </c>
-      <c r="F9" s="31" t="str">
-        <f t="shared" si="1"/>
-        <v>3:09,05</v>
-      </c>
-      <c r="G9" s="32" t="str">
-        <f t="shared" si="1"/>
-        <v>2:44,57</v>
-      </c>
-      <c r="H9" s="31" t="str">
-        <f t="shared" si="1"/>
-        <v>0:38,36</v>
-      </c>
-      <c r="I9" s="31" t="str">
-        <f t="shared" si="1"/>
-        <v>1:00,47</v>
-      </c>
-      <c r="J9" s="31" t="str">
-        <f t="shared" si="1"/>
-        <v>1:19,22</v>
-      </c>
-      <c r="K9" s="31" t="str">
-        <f t="shared" si="1"/>
-        <v>1:06,43</v>
-      </c>
-      <c r="L9" s="31" t="str">
-        <f t="shared" si="1"/>
-        <v>2:48,79</v>
-      </c>
-      <c r="M9" s="31" t="str">
-        <f t="shared" si="1"/>
-        <v>2:35,07</v>
-      </c>
-      <c r="N9" s="21"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A10" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>0:43,12</v>
-      </c>
-      <c r="C10" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1:03,63</v>
-      </c>
-      <c r="D10" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1:29,13</v>
-      </c>
-      <c r="E10" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1:13,63</v>
-      </c>
-      <c r="F10" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>3:03,57</v>
-      </c>
-      <c r="G10" s="29" t="str">
-        <f t="shared" si="0"/>
-        <v>2:39,79</v>
-      </c>
-      <c r="H10" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>0:37,25</v>
-      </c>
-      <c r="I10" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>0:58,71</v>
-      </c>
-      <c r="J10" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1:16,92</v>
-      </c>
-      <c r="K10" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1:04,50</v>
-      </c>
-      <c r="L10" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>2:43,90</v>
-      </c>
-      <c r="M10" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>2:30,57</v>
-      </c>
-      <c r="N10" s="21"/>
-    </row>
-    <row r="11" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>0:41,13</v>
-      </c>
-      <c r="C11" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>1:02,97</v>
-      </c>
-      <c r="D11" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>1:23,98</v>
-      </c>
-      <c r="E11" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>1:10,29</v>
-      </c>
-      <c r="F11" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>2:53,81</v>
-      </c>
-      <c r="G11" s="30" t="str">
-        <f t="shared" si="0"/>
-        <v>2:35,68</v>
-      </c>
-      <c r="H11" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>0:34,74</v>
-      </c>
-      <c r="I11" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>0:56,16</v>
-      </c>
-      <c r="J11" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>1:13,65</v>
-      </c>
-      <c r="K11" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>1:00,90</v>
-      </c>
-      <c r="L11" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>2:37,09</v>
-      </c>
-      <c r="M11" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>2:22,72</v>
-      </c>
-      <c r="N11" s="23"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A14" s="61" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="61"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="61"/>
-      <c r="H14" s="63" t="s">
-        <v>35</v>
-      </c>
-      <c r="I14" s="63"/>
-      <c r="J14" s="63"/>
-      <c r="L14" s="63" t="s">
-        <v>36</v>
-      </c>
-      <c r="M14"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A15" s="61"/>
-      <c r="B15" s="61"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="61"/>
-      <c r="H15" s="63"/>
-      <c r="I15" s="63"/>
-      <c r="J15" s="63"/>
-      <c r="L15" s="63"/>
-      <c r="M15"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M16"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A17" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="8">
-        <v>15</v>
-      </c>
-      <c r="C17" s="8">
-        <v>18</v>
-      </c>
-      <c r="D17" s="8">
-        <v>3</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H17" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="J17" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="L17" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="M17"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A18" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="9">
-        <v>13</v>
-      </c>
-      <c r="C18" s="9">
-        <v>14</v>
-      </c>
-      <c r="D18" s="9">
-        <v>1</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H18" s="35" t="s">
-        <v>89</v>
-      </c>
-      <c r="I18" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="J18" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="L18" s="38"/>
-      <c r="M18"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A19" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="8">
-        <v>12</v>
-      </c>
-      <c r="C19" s="8">
-        <v>18</v>
-      </c>
-      <c r="D19" s="8">
-        <v>16</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H19" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="I19" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="J19" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="L19" s="36"/>
-      <c r="M19"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A20" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="9">
-        <v>12</v>
-      </c>
-      <c r="C20" s="9">
-        <v>18</v>
-      </c>
-      <c r="D20" s="9">
-        <v>10</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H20" s="35" t="s">
-        <v>91</v>
-      </c>
-      <c r="I20" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="J20" s="35"/>
-      <c r="L20" s="38"/>
-      <c r="M20"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A21" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="8">
-        <v>12</v>
-      </c>
-      <c r="C21" s="8">
-        <v>100</v>
-      </c>
-      <c r="D21" s="8">
-        <v>8</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H21" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="I21" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="J21" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="L21" s="36"/>
-      <c r="M21"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A22" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="9">
-        <v>17</v>
-      </c>
-      <c r="C22" s="9">
-        <v>18</v>
-      </c>
-      <c r="D22" s="9">
-        <v>1</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H22" s="40" t="s">
-        <v>93</v>
-      </c>
-      <c r="I22" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="J22" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="L22" s="39"/>
-      <c r="M22"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="A23" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" s="8">
-        <v>19</v>
-      </c>
-      <c r="C23" s="8">
-        <v>100</v>
-      </c>
-      <c r="D23" s="8">
-        <v>4</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H23" s="41" t="s">
-        <v>95</v>
-      </c>
-      <c r="I23" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="J23" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="L23" s="37"/>
-      <c r="M23"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
-      <c r="L24" s="39"/>
-      <c r="M24"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="H25" s="33"/>
-      <c r="I25" s="33"/>
-      <c r="L25" s="37"/>
-      <c r="M25"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="L26" s="39"/>
-      <c r="M26"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="L27" s="37"/>
-      <c r="M27"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="L28" s="39"/>
-      <c r="M28"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="L29" s="37"/>
-      <c r="M29"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="L30" s="39"/>
-      <c r="M30"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="L31" s="37"/>
-      <c r="M31"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
-      <c r="L32" s="39"/>
-      <c r="M32"/>
-    </row>
-    <row r="33" spans="8:13" x14ac:dyDescent="0.45">
-      <c r="L33" s="37"/>
-      <c r="M33"/>
-    </row>
-    <row r="34" spans="8:13" x14ac:dyDescent="0.45">
-      <c r="L34" s="39"/>
-      <c r="M34"/>
-    </row>
-    <row r="35" spans="8:13" x14ac:dyDescent="0.45">
-      <c r="M35"/>
-    </row>
-    <row r="36" spans="8:13" x14ac:dyDescent="0.45">
-      <c r="L36" s="39"/>
-      <c r="M36"/>
-    </row>
-    <row r="37" spans="8:13" x14ac:dyDescent="0.45">
-      <c r="M37"/>
-    </row>
-    <row r="38" spans="8:13" x14ac:dyDescent="0.45">
-      <c r="H38"/>
-      <c r="I38"/>
-      <c r="J38"/>
-      <c r="K38"/>
-      <c r="L38"/>
-      <c r="M38"/>
-    </row>
-    <row r="39" spans="8:13" x14ac:dyDescent="0.45">
-      <c r="H39"/>
-      <c r="I39"/>
-      <c r="J39"/>
-      <c r="K39"/>
-      <c r="L39"/>
-      <c r="M39"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A7:N8"/>
-    <mergeCell ref="A14:F15"/>
-    <mergeCell ref="H14:J15"/>
-    <mergeCell ref="L14:L15"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
DP Code nun auch dynamisch!
</commit_message>
<xml_diff>
--- a/web/utilities/records_kriterien.xlsx
+++ b/web/utilities/records_kriterien.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgna\Documents\GitHub\Lifesaving_Baden\web\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E024A340-E74C-46CD-9DF6-AE9652B2883D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F30DC9-E692-442A-AD9F-176212713E01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="3" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
   </bookViews>
@@ -11205,8 +11205,8 @@
   </sheetPr>
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -11392,7 +11392,7 @@
       <c r="K3" s="59"/>
       <c r="L3" s="59"/>
       <c r="M3" s="59" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="N3" s="59" t="s">
         <v>225</v>

</xml_diff>

<commit_message>
DEM Tabels über Excel
</commit_message>
<xml_diff>
--- a/web/utilities/records_kriterien.xlsx
+++ b/web/utilities/records_kriterien.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgna\Documents\GitHub\Lifesaving_Baden\web\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7577A8A6-8575-462C-93E7-D6EFFCDC5329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D509DC-20C8-4725-96CA-B047B786CA17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="3" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
   </bookViews>
   <sheets>
     <sheet name="DR" sheetId="9" r:id="rId1"/>
@@ -219,7 +219,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="225">
   <si>
     <t>50m Retten</t>
   </si>
@@ -882,9 +882,6 @@
   </si>
   <si>
     <t>Männlich U19</t>
-  </si>
-  <si>
-    <t>1.3.Jahr</t>
   </si>
   <si>
     <t>1.6.Jahr</t>
@@ -1163,7 +1160,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1344,12 +1341,78 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="194">
     <dxf>
+      <numFmt numFmtId="164" formatCode="m:ss.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m:ss.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m:ss.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m:ss.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m:ss.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m:ss.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m:ss.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m:ss.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m:ss.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m:ss.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m:ss.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m:ss.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <color theme="6"/>
       </font>
@@ -1438,51 +1501,6 @@
       <font>
         <color theme="4"/>
       </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3913,7 +3931,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{16F87202-5A6A-4E2F-B973-3CE7EC2566C1}" name="Tabelle6" displayName="Tabelle6" ref="A1:X7" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{16F87202-5A6A-4E2F-B973-3CE7EC2566C1}" name="DEM_konfig" displayName="DEM_konfig" ref="A1:X7" totalsRowShown="0" headerRowDxfId="69" dataDxfId="68">
   <autoFilter ref="A1:X7" xr:uid="{16F87202-5A6A-4E2F-B973-3CE7EC2566C1}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3945,33 +3963,33 @@
     <tableColumn id="2" xr3:uid="{6346FF3B-B334-4CD8-8B23-F2347E29C536}" name="Geschlecht" dataDxfId="66"/>
     <tableColumn id="3" xr3:uid="{E793B48A-BC8A-439F-8AAF-6FD08104A619}" name="Mindest Alter" dataDxfId="65"/>
     <tableColumn id="4" xr3:uid="{01A62C29-2F75-4107-A431-F69230BCCD0C}" name="Maximales Alter" dataDxfId="64"/>
-    <tableColumn id="5" xr3:uid="{B7E4DE90-7856-4A0C-9063-61414D7F227C}" name="Qualizeitraum anfang" dataDxfId="63"/>
-    <tableColumn id="6" xr3:uid="{B00F7CD1-82CB-42B9-A396-89F79EF419CA}" name="Qualizeitraum Ende" dataDxfId="62"/>
-    <tableColumn id="7" xr3:uid="{9E50DDE5-12E3-4BCB-801C-FBABCE309F0E}" name="Letzter Wettkampf am" dataDxfId="61"/>
-    <tableColumn id="8" xr3:uid="{57E68247-0FF2-48D8-8ACD-AB057E576A21}" name="Landesverband" dataDxfId="60"/>
-    <tableColumn id="9" xr3:uid="{EBAA439D-F69A-4C2A-8193-9AE08F1E57B8}" name="OMS" dataDxfId="59"/>
-    <tableColumn id="10" xr3:uid="{BBD11E7F-3DDF-428A-B005-4A40E6FA78DC}" name="Pool-Länge" dataDxfId="58"/>
-    <tableColumn id="11" xr3:uid="{6AE38DCA-A084-4F3D-A6A4-4E76E3E2CBC6}" name="Regelwerk" dataDxfId="57"/>
-    <tableColumn id="12" xr3:uid="{7F7470AD-5502-4CEE-BB4C-44BA308E61D7}" name="Seiten Anzahl" dataDxfId="56"/>
-    <tableColumn id="13" xr3:uid="{F416CBFA-4C9D-45CD-9BA7-E4BC57A08BC2}" name="PZ1 - 50m Retten" dataDxfId="55"/>
-    <tableColumn id="14" xr3:uid="{7117DBCA-0DA7-462C-84FE-0DC7E33B124C}" name="PZ1 - 100m Retten" dataDxfId="54"/>
-    <tableColumn id="15" xr3:uid="{E8630E91-DC30-4822-9E53-6D65487C3670}" name="PZ1 - 100m Kombi" dataDxfId="53"/>
-    <tableColumn id="16" xr3:uid="{4B3AA225-E042-430F-8259-D176887B4528}" name="PZ1 - 100m Lifesaver" dataDxfId="52"/>
-    <tableColumn id="17" xr3:uid="{798674BD-98CE-4531-BDFF-6AB06253AD7C}" name="PZ1 - 200m Super-Lifesaver" dataDxfId="51"/>
-    <tableColumn id="18" xr3:uid="{8809BB71-D58B-4E8B-A442-D0EB9A65A25D}" name="PZ1 - 200m Hindernis" dataDxfId="50"/>
-    <tableColumn id="19" xr3:uid="{93DCF463-806B-4117-B4E3-1FFAE976B37C}" name="PZ2 - 50m Retten" dataDxfId="49"/>
-    <tableColumn id="20" xr3:uid="{A514C961-559E-462F-B143-BA30974C0129}" name="PZ2 - 100m Retten" dataDxfId="48"/>
-    <tableColumn id="21" xr3:uid="{F1CF6143-45FE-498D-93D6-36F26D2F3C0B}" name="PZ2 - 100m Kombi" dataDxfId="47"/>
-    <tableColumn id="22" xr3:uid="{E90962FC-C214-467F-841F-40DF60E41456}" name="PZ2 - 100m Lifesaver" dataDxfId="46"/>
-    <tableColumn id="23" xr3:uid="{7FBC6334-C4C8-4B38-9F59-30ED95A44379}" name="PZ2 - 200m Super-Lifesaver" dataDxfId="45"/>
-    <tableColumn id="24" xr3:uid="{231BFF86-8F3A-4BA1-B25E-28175D9EDFA9}" name="PZ2 - 200m Hindernis" dataDxfId="44"/>
+    <tableColumn id="5" xr3:uid="{B7E4DE90-7856-4A0C-9063-61414D7F227C}" name="Qualizeitraum anfang" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{B00F7CD1-82CB-42B9-A396-89F79EF419CA}" name="Qualizeitraum Ende" dataDxfId="13"/>
+    <tableColumn id="7" xr3:uid="{9E50DDE5-12E3-4BCB-801C-FBABCE309F0E}" name="Letzter Wettkampf am" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{57E68247-0FF2-48D8-8ACD-AB057E576A21}" name="Landesverband" dataDxfId="63"/>
+    <tableColumn id="9" xr3:uid="{EBAA439D-F69A-4C2A-8193-9AE08F1E57B8}" name="OMS" dataDxfId="62"/>
+    <tableColumn id="10" xr3:uid="{BBD11E7F-3DDF-428A-B005-4A40E6FA78DC}" name="Pool-Länge" dataDxfId="61"/>
+    <tableColumn id="11" xr3:uid="{6AE38DCA-A084-4F3D-A6A4-4E76E3E2CBC6}" name="Regelwerk" dataDxfId="60"/>
+    <tableColumn id="12" xr3:uid="{7F7470AD-5502-4CEE-BB4C-44BA308E61D7}" name="Seiten Anzahl" dataDxfId="59"/>
+    <tableColumn id="13" xr3:uid="{F416CBFA-4C9D-45CD-9BA7-E4BC57A08BC2}" name="PZ1 - 50m Retten" dataDxfId="11"/>
+    <tableColumn id="14" xr3:uid="{7117DBCA-0DA7-462C-84FE-0DC7E33B124C}" name="PZ1 - 100m Retten" dataDxfId="10"/>
+    <tableColumn id="15" xr3:uid="{E8630E91-DC30-4822-9E53-6D65487C3670}" name="PZ1 - 100m Kombi" dataDxfId="9"/>
+    <tableColumn id="16" xr3:uid="{4B3AA225-E042-430F-8259-D176887B4528}" name="PZ1 - 100m Lifesaver" dataDxfId="8"/>
+    <tableColumn id="17" xr3:uid="{798674BD-98CE-4531-BDFF-6AB06253AD7C}" name="PZ1 - 200m Super-Lifesaver" dataDxfId="7"/>
+    <tableColumn id="18" xr3:uid="{8809BB71-D58B-4E8B-A442-D0EB9A65A25D}" name="PZ1 - 200m Hindernis" dataDxfId="6"/>
+    <tableColumn id="19" xr3:uid="{93DCF463-806B-4117-B4E3-1FFAE976B37C}" name="PZ2 - 50m Retten" dataDxfId="5"/>
+    <tableColumn id="20" xr3:uid="{A514C961-559E-462F-B143-BA30974C0129}" name="PZ2 - 100m Retten" dataDxfId="4"/>
+    <tableColumn id="21" xr3:uid="{F1CF6143-45FE-498D-93D6-36F26D2F3C0B}" name="PZ2 - 100m Kombi" dataDxfId="3"/>
+    <tableColumn id="22" xr3:uid="{E90962FC-C214-467F-841F-40DF60E41456}" name="PZ2 - 100m Lifesaver" dataDxfId="2"/>
+    <tableColumn id="23" xr3:uid="{7FBC6334-C4C8-4B38-9F59-30ED95A44379}" name="PZ2 - 200m Super-Lifesaver" dataDxfId="1"/>
+    <tableColumn id="24" xr3:uid="{231BFF86-8F3A-4BA1-B25E-28175D9EDFA9}" name="PZ2 - 200m Hindernis" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{38173103-C137-4989-84EA-9BDFE7009E50}" name="Tabelle68" displayName="Tabelle68" ref="A1:X3" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{38173103-C137-4989-84EA-9BDFE7009E50}" name="Tabelle68" displayName="Tabelle68" ref="A1:X3" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
   <autoFilter ref="A1:X3" xr:uid="{38173103-C137-4989-84EA-9BDFE7009E50}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -3999,30 +4017,30 @@
     <filterColumn colId="23" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{EC191D47-103E-4808-B80B-20281F480A7B}" name="Tabellen Name" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{B4135B5F-F957-45A0-BE67-B4F753711A01}" name="Geschlecht" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{3E8C5D70-845D-4A0C-8911-63692B806EE3}" name="Mindest Alter" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{951555AA-1D48-4F58-84DA-5A388BC7ACA6}" name="Maximales Alter" dataDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{532345E9-A3F4-4BC3-83A4-BBE007D5BF2F}" name="Qualizeitraum anfang" dataDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{71A6260E-6437-4311-B1E5-334D777DE23B}" name="Qualizeitraum Ende" dataDxfId="36"/>
-    <tableColumn id="7" xr3:uid="{C4D53DE9-9819-4221-8397-DAA183E26E63}" name="Letzter Wettkampf am" dataDxfId="35"/>
-    <tableColumn id="8" xr3:uid="{8A29AFA5-6619-4699-AB42-78F4AD5566E1}" name="Landesverband" dataDxfId="34"/>
-    <tableColumn id="9" xr3:uid="{9AB45004-0EB4-4304-AFD0-4496973A950F}" name="OMS" dataDxfId="33"/>
-    <tableColumn id="10" xr3:uid="{71319762-F54F-4493-84F3-802DFD3DE0D2}" name="Pool-Länge" dataDxfId="32"/>
-    <tableColumn id="11" xr3:uid="{E91F6E89-282A-4B79-A6DF-C43103E9413B}" name="Regelwerk" dataDxfId="31"/>
-    <tableColumn id="12" xr3:uid="{D4638146-A857-41ED-83D1-8E2711E1ED0F}" name="Seiten Anzahl" dataDxfId="30"/>
-    <tableColumn id="13" xr3:uid="{08DB5C03-8197-4058-AF4C-5A2A8CB975EF}" name="PZ1 - 50m Retten" dataDxfId="29"/>
-    <tableColumn id="14" xr3:uid="{94966042-A021-4D1B-83E0-516EF43C47BF}" name="PZ1 - 100m Retten" dataDxfId="28"/>
-    <tableColumn id="15" xr3:uid="{3D118CE3-B383-4B67-8BD7-A4E7270B694D}" name="PZ1 - 100m Kombi" dataDxfId="27"/>
-    <tableColumn id="16" xr3:uid="{2EF5524D-F52F-403A-B1F2-26B06E1561D7}" name="PZ1 - 100m Lifesaver" dataDxfId="26"/>
-    <tableColumn id="17" xr3:uid="{90AFAED0-E3F7-430F-B477-A7B8C0F28C92}" name="PZ1 - 200m Super-Lifesaver" dataDxfId="25"/>
-    <tableColumn id="18" xr3:uid="{234BF89C-A472-4472-A7B5-6E8956546AEB}" name="PZ1 - 200m Hindernis" dataDxfId="24"/>
-    <tableColumn id="19" xr3:uid="{0630350F-8319-4C46-926A-11BAE7DA4892}" name="PZ2 - 50m Retten" dataDxfId="23"/>
-    <tableColumn id="20" xr3:uid="{923F9722-E09F-460A-8B02-64E9F03F0806}" name="PZ2 - 100m Retten" dataDxfId="22"/>
-    <tableColumn id="21" xr3:uid="{AA307655-1197-43FB-A00A-75C1438B2412}" name="PZ2 - 100m Kombi" dataDxfId="21"/>
-    <tableColumn id="22" xr3:uid="{92C209F1-CAD1-4D8C-888D-8F65EE77FFDE}" name="PZ2 - 100m Lifesaver" dataDxfId="20"/>
-    <tableColumn id="23" xr3:uid="{AE53DAA0-7669-4EC4-A7F2-6BFCE8E6960F}" name="PZ2 - 200m Super-Lifesaver" dataDxfId="19"/>
-    <tableColumn id="24" xr3:uid="{AB5DE385-0AE1-401A-8EF5-9ED15B7100C9}" name="PZ2 - 200m Hindernis" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{EC191D47-103E-4808-B80B-20281F480A7B}" name="Tabellen Name" dataDxfId="56"/>
+    <tableColumn id="2" xr3:uid="{B4135B5F-F957-45A0-BE67-B4F753711A01}" name="Geschlecht" dataDxfId="55"/>
+    <tableColumn id="3" xr3:uid="{3E8C5D70-845D-4A0C-8911-63692B806EE3}" name="Mindest Alter" dataDxfId="54"/>
+    <tableColumn id="4" xr3:uid="{951555AA-1D48-4F58-84DA-5A388BC7ACA6}" name="Maximales Alter" dataDxfId="53"/>
+    <tableColumn id="5" xr3:uid="{532345E9-A3F4-4BC3-83A4-BBE007D5BF2F}" name="Qualizeitraum anfang" dataDxfId="52"/>
+    <tableColumn id="6" xr3:uid="{71A6260E-6437-4311-B1E5-334D777DE23B}" name="Qualizeitraum Ende" dataDxfId="51"/>
+    <tableColumn id="7" xr3:uid="{C4D53DE9-9819-4221-8397-DAA183E26E63}" name="Letzter Wettkampf am" dataDxfId="50"/>
+    <tableColumn id="8" xr3:uid="{8A29AFA5-6619-4699-AB42-78F4AD5566E1}" name="Landesverband" dataDxfId="49"/>
+    <tableColumn id="9" xr3:uid="{9AB45004-0EB4-4304-AFD0-4496973A950F}" name="OMS" dataDxfId="48"/>
+    <tableColumn id="10" xr3:uid="{71319762-F54F-4493-84F3-802DFD3DE0D2}" name="Pool-Länge" dataDxfId="47"/>
+    <tableColumn id="11" xr3:uid="{E91F6E89-282A-4B79-A6DF-C43103E9413B}" name="Regelwerk" dataDxfId="46"/>
+    <tableColumn id="12" xr3:uid="{D4638146-A857-41ED-83D1-8E2711E1ED0F}" name="Seiten Anzahl" dataDxfId="45"/>
+    <tableColumn id="13" xr3:uid="{08DB5C03-8197-4058-AF4C-5A2A8CB975EF}" name="PZ1 - 50m Retten" dataDxfId="44"/>
+    <tableColumn id="14" xr3:uid="{94966042-A021-4D1B-83E0-516EF43C47BF}" name="PZ1 - 100m Retten" dataDxfId="43"/>
+    <tableColumn id="15" xr3:uid="{3D118CE3-B383-4B67-8BD7-A4E7270B694D}" name="PZ1 - 100m Kombi" dataDxfId="42"/>
+    <tableColumn id="16" xr3:uid="{2EF5524D-F52F-403A-B1F2-26B06E1561D7}" name="PZ1 - 100m Lifesaver" dataDxfId="41"/>
+    <tableColumn id="17" xr3:uid="{90AFAED0-E3F7-430F-B477-A7B8C0F28C92}" name="PZ1 - 200m Super-Lifesaver" dataDxfId="40"/>
+    <tableColumn id="18" xr3:uid="{234BF89C-A472-4472-A7B5-6E8956546AEB}" name="PZ1 - 200m Hindernis" dataDxfId="39"/>
+    <tableColumn id="19" xr3:uid="{0630350F-8319-4C46-926A-11BAE7DA4892}" name="PZ2 - 50m Retten" dataDxfId="38"/>
+    <tableColumn id="20" xr3:uid="{923F9722-E09F-460A-8B02-64E9F03F0806}" name="PZ2 - 100m Retten" dataDxfId="37"/>
+    <tableColumn id="21" xr3:uid="{AA307655-1197-43FB-A00A-75C1438B2412}" name="PZ2 - 100m Kombi" dataDxfId="36"/>
+    <tableColumn id="22" xr3:uid="{92C209F1-CAD1-4D8C-888D-8F65EE77FFDE}" name="PZ2 - 100m Lifesaver" dataDxfId="35"/>
+    <tableColumn id="23" xr3:uid="{AE53DAA0-7669-4EC4-A7F2-6BFCE8E6960F}" name="PZ2 - 200m Super-Lifesaver" dataDxfId="34"/>
+    <tableColumn id="24" xr3:uid="{AB5DE385-0AE1-401A-8EF5-9ED15B7100C9}" name="PZ2 - 200m Hindernis" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4345,15 +4363,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0519F5DB-31A0-4819-8E86-33B1F16466A6}">
+  <sheetPr codeName="Tabelle6"/>
   <dimension ref="A1:AW31"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0">
       <selection activeCell="Y25" sqref="Y25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.265625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>39</v>
       </c>
@@ -4422,7 +4441,7 @@
       <c r="AV1" s="44"/>
       <c r="AW1" s="44"/>
     </row>
-    <row r="2" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
         <v>40</v>
       </c>
@@ -4489,7 +4508,7 @@
       <c r="AV2" s="45"/>
       <c r="AW2" s="45"/>
     </row>
-    <row r="3" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">
         <v>101</v>
       </c>
@@ -4550,7 +4569,7 @@
       <c r="AV3" s="45"/>
       <c r="AW3" s="45"/>
     </row>
-    <row r="4" spans="1:49" s="53" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:49" s="53" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="49" t="s">
         <v>10</v>
       </c>
@@ -4699,7 +4718,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2000</v>
       </c>
@@ -4752,7 +4771,7 @@
       <c r="AV5" s="10"/>
       <c r="AW5" s="10"/>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f t="shared" ref="A6:A31" si="0">A5+1</f>
         <v>2001</v>
@@ -4830,7 +4849,7 @@
       <c r="AV6" s="11"/>
       <c r="AW6" s="11"/>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>2002</v>
@@ -4908,7 +4927,7 @@
       <c r="AV7" s="10"/>
       <c r="AW7" s="10"/>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>2003</v>
@@ -4986,7 +5005,7 @@
       <c r="AV8" s="11"/>
       <c r="AW8" s="11"/>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>2004</v>
@@ -5064,7 +5083,7 @@
       <c r="AV9" s="10"/>
       <c r="AW9" s="10"/>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>2005</v>
@@ -5142,7 +5161,7 @@
       <c r="AV10" s="11"/>
       <c r="AW10" s="11"/>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>2006</v>
@@ -5220,7 +5239,7 @@
       <c r="AV11" s="10"/>
       <c r="AW11" s="10"/>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>2007</v>
@@ -5342,7 +5361,7 @@
         <v>3.5995370370370369E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>2008</v>
@@ -5464,7 +5483,7 @@
         <v>3.5995370370370369E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>2009</v>
@@ -5586,7 +5605,7 @@
         <v>3.5995370370370369E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>2010</v>
@@ -5708,7 +5727,7 @@
         <v>3.5995370370370369E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>2011</v>
@@ -5842,7 +5861,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>2012</v>
@@ -5976,7 +5995,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>2013</v>
@@ -6110,7 +6129,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>2014</v>
@@ -6244,7 +6263,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>2015</v>
@@ -6378,7 +6397,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>2016</v>
@@ -6512,7 +6531,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>2017</v>
@@ -6646,7 +6665,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>2018</v>
@@ -6780,7 +6799,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>2019</v>
@@ -6914,7 +6933,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>2020</v>
@@ -7064,7 +7083,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>2021</v>
@@ -7214,7 +7233,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>2022</v>
@@ -7364,7 +7383,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>2023</v>
@@ -7514,7 +7533,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>2024</v>
@@ -7664,7 +7683,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>2025</v>
@@ -7814,7 +7833,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>2026</v>
@@ -7966,52 +7985,52 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B5:G31">
-    <cfRule type="expression" dxfId="17" priority="15">
+    <cfRule type="expression" dxfId="32" priority="15">
       <formula>B5&lt;&gt;B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:M31">
-    <cfRule type="expression" dxfId="16" priority="14">
+    <cfRule type="expression" dxfId="31" priority="14">
       <formula>H5&lt;&gt;H4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N5:S31">
-    <cfRule type="expression" dxfId="15" priority="13">
+    <cfRule type="expression" dxfId="30" priority="13">
       <formula>N5&lt;&gt;N4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T5:Y31">
-    <cfRule type="expression" dxfId="14" priority="12">
+    <cfRule type="expression" dxfId="29" priority="12">
       <formula>T5&lt;&gt;T4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z5:AE31">
-    <cfRule type="expression" dxfId="13" priority="9">
+    <cfRule type="expression" dxfId="28" priority="9">
       <formula>Z5&lt;&gt;Z4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF5:AK31">
-    <cfRule type="expression" dxfId="12" priority="8">
+    <cfRule type="expression" dxfId="27" priority="8">
       <formula>AF5&lt;&gt;AF4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL5:AN31">
-    <cfRule type="expression" dxfId="11" priority="6">
+    <cfRule type="expression" dxfId="26" priority="6">
       <formula>AL5&lt;&gt;AL4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO5:AQ31">
-    <cfRule type="expression" dxfId="10" priority="5">
+    <cfRule type="expression" dxfId="25" priority="5">
       <formula>AO5&lt;&gt;AO4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR5:AT31">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="24" priority="2">
       <formula>AR5&lt;&gt;AR4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU5:AW31">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="23" priority="1">
       <formula>AU5&lt;&gt;AU4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8035,15 +8054,15 @@
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.86328125" style="1" customWidth="1"/>
-    <col min="2" max="13" width="18.73046875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
+    <col min="2" max="13" width="18.7109375" style="1" customWidth="1"/>
     <col min="14" max="14" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="11.3984375" style="1"/>
+    <col min="15" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18">
         <v>2026</v>
       </c>
@@ -8087,7 +8106,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
@@ -8143,7 +8162,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -8199,7 +8218,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>8</v>
       </c>
@@ -8255,7 +8274,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="62" t="s">
         <v>13</v>
       </c>
@@ -8273,7 +8292,7 @@
       <c r="M7" s="62"/>
       <c r="N7" s="62"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="62"/>
       <c r="B8" s="62"/>
       <c r="C8" s="62"/>
@@ -8289,7 +8308,7 @@
       <c r="M8" s="62"/>
       <c r="N8" s="62"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>6</v>
       </c>
@@ -8343,7 +8362,7 @@
       </c>
       <c r="N9" s="21"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>7</v>
       </c>
@@ -8397,7 +8416,7 @@
       </c>
       <c r="N10" s="21"/>
     </row>
-    <row r="11" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>8</v>
       </c>
@@ -8451,7 +8470,7 @@
       </c>
       <c r="N11" s="23"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="61" t="s">
         <v>14</v>
       </c>
@@ -8470,7 +8489,7 @@
       </c>
       <c r="M14"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="61"/>
       <c r="B15" s="61"/>
       <c r="C15" s="61"/>
@@ -8483,7 +8502,7 @@
       <c r="L15" s="63"/>
       <c r="M15"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -8516,7 +8535,7 @@
       </c>
       <c r="M16"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>28</v>
       </c>
@@ -8549,7 +8568,7 @@
       </c>
       <c r="M17"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>28</v>
       </c>
@@ -8580,7 +8599,7 @@
       <c r="L18" s="38"/>
       <c r="M18"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>29</v>
       </c>
@@ -8611,7 +8630,7 @@
       <c r="L19" s="36"/>
       <c r="M19"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>30</v>
       </c>
@@ -8640,7 +8659,7 @@
       <c r="L20" s="38"/>
       <c r="M20"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>29</v>
       </c>
@@ -8671,7 +8690,7 @@
       <c r="L21" s="36"/>
       <c r="M21"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>28</v>
       </c>
@@ -8702,7 +8721,7 @@
       <c r="L22" s="39"/>
       <c r="M22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>28</v>
       </c>
@@ -8733,66 +8752,66 @@
       <c r="L23" s="37"/>
       <c r="M23"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H24" s="40"/>
       <c r="I24" s="40"/>
       <c r="J24" s="40"/>
       <c r="L24" s="39"/>
       <c r="M24"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H25" s="33"/>
       <c r="I25" s="33"/>
       <c r="L25" s="37"/>
       <c r="M25"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L26" s="39"/>
       <c r="M26"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L27" s="37"/>
       <c r="M27"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L28" s="39"/>
       <c r="M28"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L29" s="37"/>
       <c r="M29"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L30" s="39"/>
       <c r="M30"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L31" s="37"/>
       <c r="M31"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L32" s="39"/>
       <c r="M32"/>
     </row>
-    <row r="33" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="33" spans="8:13" x14ac:dyDescent="0.25">
       <c r="L33" s="37"/>
       <c r="M33"/>
     </row>
-    <row r="34" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="34" spans="8:13" x14ac:dyDescent="0.25">
       <c r="L34" s="39"/>
       <c r="M34"/>
     </row>
-    <row r="35" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="35" spans="8:13" x14ac:dyDescent="0.25">
       <c r="M35"/>
     </row>
-    <row r="36" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="36" spans="8:13" x14ac:dyDescent="0.25">
       <c r="L36" s="39"/>
       <c r="M36"/>
     </row>
-    <row r="37" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="37" spans="8:13" x14ac:dyDescent="0.25">
       <c r="M37"/>
     </row>
-    <row r="38" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="38" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H38"/>
       <c r="I38"/>
       <c r="J38"/>
@@ -8800,7 +8819,7 @@
       <c r="L38"/>
       <c r="M38"/>
     </row>
-    <row r="39" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="39" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H39"/>
       <c r="I39"/>
       <c r="J39"/>
@@ -8829,17 +8848,17 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.265625" customWidth="1"/>
-    <col min="2" max="5" width="18.73046875" customWidth="1"/>
-    <col min="6" max="6" width="21.1328125" customWidth="1"/>
-    <col min="7" max="11" width="18.73046875" customWidth="1"/>
-    <col min="12" max="12" width="22.1328125" customWidth="1"/>
-    <col min="13" max="13" width="18.73046875" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="7" max="11" width="18.7109375" customWidth="1"/>
+    <col min="12" max="12" width="22.140625" customWidth="1"/>
+    <col min="13" max="13" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>39</v>
       </c>
@@ -8880,7 +8899,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
         <v>40</v>
       </c>
@@ -8921,7 +8940,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">
         <v>41</v>
       </c>
@@ -8962,7 +8981,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -9003,7 +9022,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2000</v>
       </c>
@@ -9020,7 +9039,7 @@
       <c r="L5" s="11"/>
       <c r="M5" s="11"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f t="shared" ref="A6:A32" si="0">A5+1</f>
         <v>2001</v>
@@ -9038,7 +9057,7 @@
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>2002</v>
@@ -9056,7 +9075,7 @@
       <c r="L7" s="11"/>
       <c r="M7" s="11"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>2003</v>
@@ -9074,7 +9093,7 @@
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>2004</v>
@@ -9092,7 +9111,7 @@
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>2005</v>
@@ -9110,7 +9129,7 @@
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>2006</v>
@@ -9128,7 +9147,7 @@
       <c r="L11" s="11"/>
       <c r="M11" s="11"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>2007</v>
@@ -9146,7 +9165,7 @@
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>2008</v>
@@ -9164,7 +9183,7 @@
       <c r="L13" s="11"/>
       <c r="M13" s="11"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>2009</v>
@@ -9182,7 +9201,7 @@
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>2010</v>
@@ -9200,7 +9219,7 @@
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>2011</v>
@@ -9218,7 +9237,7 @@
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>2012</v>
@@ -9236,7 +9255,7 @@
       <c r="L17" s="11"/>
       <c r="M17" s="11"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>2013</v>
@@ -9254,7 +9273,7 @@
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>2014</v>
@@ -9272,7 +9291,7 @@
       <c r="L19" s="11"/>
       <c r="M19" s="11"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>2015</v>
@@ -9314,7 +9333,7 @@
         <v>1.3592592592592591E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>2016</v>
@@ -9356,7 +9375,7 @@
         <v>1.3592592592592591E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>2017</v>
@@ -9398,7 +9417,7 @@
         <v>1.3577546296296298E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>2018</v>
@@ -9440,7 +9459,7 @@
         <v>1.3577546296296298E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>2019</v>
@@ -9482,7 +9501,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>2020</v>
@@ -9524,7 +9543,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>2021</v>
@@ -9566,7 +9585,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>2022</v>
@@ -9608,7 +9627,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>2023</v>
@@ -9650,7 +9669,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>2024</v>
@@ -9692,7 +9711,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>2025</v>
@@ -9734,7 +9753,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>2026</v>
@@ -9776,7 +9795,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <f t="shared" si="0"/>
         <v>2027</v>
@@ -9820,22 +9839,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B6:G6">
-    <cfRule type="expression" dxfId="7" priority="20">
+    <cfRule type="expression" dxfId="22" priority="20">
       <formula>B6&lt;&gt;B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:G32">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="21" priority="1">
       <formula>B7&lt;&gt;B6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:M6">
-    <cfRule type="expression" dxfId="5" priority="22">
+    <cfRule type="expression" dxfId="20" priority="22">
       <formula>H6&lt;&gt;H4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:M32">
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="19" priority="2">
       <formula>H7&lt;&gt;H6</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9856,17 +9875,17 @@
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.86328125" customWidth="1"/>
-    <col min="2" max="5" width="18.73046875" customWidth="1"/>
-    <col min="6" max="6" width="21.1328125" customWidth="1"/>
-    <col min="7" max="11" width="18.73046875" customWidth="1"/>
-    <col min="12" max="12" width="22.1328125" customWidth="1"/>
-    <col min="13" max="13" width="18.73046875" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="7" max="11" width="18.7109375" customWidth="1"/>
+    <col min="12" max="12" width="22.140625" customWidth="1"/>
+    <col min="13" max="13" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>39</v>
       </c>
@@ -9907,7 +9926,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
         <v>40</v>
       </c>
@@ -9948,7 +9967,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">
         <v>41</v>
       </c>
@@ -9989,7 +10008,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -10030,7 +10049,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2000</v>
       </c>
@@ -10047,7 +10066,7 @@
       <c r="L5" s="38"/>
       <c r="M5" s="38"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f t="shared" ref="A6:A31" si="0">A5+1</f>
         <v>2001</v>
@@ -10077,7 +10096,7 @@
         <v>1.3629629629629632E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>2002</v>
@@ -10119,7 +10138,7 @@
         <v>1.3629629629629632E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>2003</v>
@@ -10161,7 +10180,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>2004</v>
@@ -10203,7 +10222,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>2005</v>
@@ -10245,7 +10264,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>2006</v>
@@ -10287,7 +10306,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>2007</v>
@@ -10329,7 +10348,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>2008</v>
@@ -10371,7 +10390,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>2009</v>
@@ -10413,7 +10432,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>2010</v>
@@ -10455,7 +10474,7 @@
         <v>1.3306712962962966E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>2011</v>
@@ -10497,7 +10516,7 @@
         <v>1.3306712962962966E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>2012</v>
@@ -10539,7 +10558,7 @@
         <v>1.3306712962962966E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>2013</v>
@@ -10581,7 +10600,7 @@
         <v>1.312962962962963E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>2014</v>
@@ -10623,7 +10642,7 @@
         <v>1.312962962962963E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>2015</v>
@@ -10665,7 +10684,7 @@
         <v>1.3116898148148148E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>2016</v>
@@ -10707,7 +10726,7 @@
         <v>1.3116898148148148E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>2017</v>
@@ -10749,7 +10768,7 @@
         <v>1.3116898148148148E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>2018</v>
@@ -10791,7 +10810,7 @@
         <v>1.3116898148148148E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>2019</v>
@@ -10833,7 +10852,7 @@
         <v>1.3116898148148148E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>2020</v>
@@ -10875,7 +10894,7 @@
         <v>1.3097222222222223E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>2021</v>
@@ -10917,7 +10936,7 @@
         <v>1.3097222222222223E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>2022</v>
@@ -10959,7 +10978,7 @@
         <v>1.3097222222222223E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>2023</v>
@@ -11001,7 +11020,7 @@
         <v>1.3097222222222223E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>2024</v>
@@ -11043,7 +11062,7 @@
         <v>1.3097222222222223E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>2025</v>
@@ -11085,7 +11104,7 @@
         <v>1.2931712962962962E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>2026</v>
@@ -11127,7 +11146,7 @@
         <v>1.2931712962962962E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <f>A31+1</f>
         <v>2027</v>
@@ -11171,22 +11190,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B6:G6">
-    <cfRule type="expression" dxfId="3" priority="19">
+    <cfRule type="expression" dxfId="18" priority="19">
       <formula>B6&lt;&gt;B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:G32">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="17" priority="2">
       <formula>B7&lt;&gt;B6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:M6">
-    <cfRule type="expression" dxfId="1" priority="20">
+    <cfRule type="expression" dxfId="16" priority="20">
       <formula>H6&lt;&gt;H4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:M32">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="15" priority="1">
       <formula>H7&lt;&gt;H6</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11200,39 +11219,39 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{620E427F-1458-41E5-8334-8536EBB7542D}">
-  <sheetPr>
+  <sheetPr codeName="Tabelle7">
     <tabColor theme="5"/>
   </sheetPr>
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.73046875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.73046875" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
     <col min="15" max="16" width="19" customWidth="1"/>
-    <col min="17" max="17" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="22.265625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.73046875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="47.265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="47.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="60" t="s">
         <v>161</v>
       </c>
@@ -11297,7 +11316,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="59" t="s">
         <v>199</v>
       </c>
@@ -11311,10 +11330,10 @@
         <v>50</v>
       </c>
       <c r="E2" s="59" t="s">
+        <v>223</v>
+      </c>
+      <c r="F2" s="59" t="s">
         <v>224</v>
-      </c>
-      <c r="F2" s="59" t="s">
-        <v>225</v>
       </c>
       <c r="G2" s="59" t="s">
         <v>198</v>
@@ -11334,7 +11353,7 @@
         <v>10</v>
       </c>
       <c r="N2" s="59" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="O2" s="59">
         <v>0</v>
@@ -11358,7 +11377,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="59" t="s">
         <v>200</v>
       </c>
@@ -11372,10 +11391,10 @@
         <v>50</v>
       </c>
       <c r="E3" s="59" t="s">
+        <v>223</v>
+      </c>
+      <c r="F3" s="59" t="s">
         <v>224</v>
-      </c>
-      <c r="F3" s="59" t="s">
-        <v>225</v>
       </c>
       <c r="G3" s="59" t="s">
         <v>198</v>
@@ -11395,7 +11414,7 @@
         <v>10</v>
       </c>
       <c r="N3" s="59" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="O3" s="59">
         <v>0</v>
@@ -11429,39 +11448,39 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3997671C-060D-4DE3-898D-CFDBFAA908F9}">
-  <sheetPr>
+  <sheetPr codeName="Tabelle8">
     <tabColor theme="5"/>
   </sheetPr>
   <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.73046875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.73046875" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
     <col min="15" max="16" width="19" customWidth="1"/>
-    <col min="17" max="17" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="22.265625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.73046875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="47.265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="47.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="60" t="s">
         <v>161</v>
       </c>
@@ -11526,7 +11545,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="59" t="s">
         <v>190</v>
       </c>
@@ -11587,7 +11606,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="59" t="s">
         <v>191</v>
       </c>
@@ -11648,7 +11667,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
         <v>192</v>
       </c>
@@ -11709,7 +11728,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
         <v>193</v>
       </c>
@@ -11768,7 +11787,7 @@
       </c>
       <c r="U5" s="59"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="59" t="s">
         <v>194</v>
       </c>
@@ -11827,7 +11846,7 @@
       </c>
       <c r="U6" s="59"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="59" t="s">
         <v>195</v>
       </c>
@@ -11896,44 +11915,44 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B26A97B8-4E61-4811-AFAC-69F978DDEBB3}">
-  <sheetPr>
+  <sheetPr codeName="Tabelle9">
     <tabColor theme="5"/>
   </sheetPr>
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.06640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.46484375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.86328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.53125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.46484375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.06640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.73046875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.3984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.1328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.796875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.86328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.3984375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.1328125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="24.796875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="59" t="s">
         <v>161</v>
       </c>
@@ -12007,7 +12026,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="59" t="s">
         <v>217</v>
       </c>
@@ -12020,6 +12039,427 @@
       <c r="D2" s="59">
         <v>16</v>
       </c>
+      <c r="E2" s="64">
+        <v>45658</v>
+      </c>
+      <c r="F2" s="64">
+        <v>46113</v>
+      </c>
+      <c r="G2" s="64">
+        <v>45658</v>
+      </c>
+      <c r="H2" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="I2" s="59" t="s">
+        <v>179</v>
+      </c>
+      <c r="J2" s="59"/>
+      <c r="K2" s="59"/>
+      <c r="L2" s="59">
+        <v>200</v>
+      </c>
+      <c r="M2" s="65"/>
+      <c r="N2" s="65"/>
+      <c r="O2" s="65"/>
+      <c r="P2" s="65"/>
+      <c r="Q2" s="65"/>
+      <c r="R2" s="65"/>
+      <c r="S2" s="65"/>
+      <c r="T2" s="65"/>
+      <c r="U2" s="65"/>
+      <c r="V2" s="65"/>
+      <c r="W2" s="65"/>
+      <c r="X2" s="65"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A3" s="59" t="s">
+        <v>218</v>
+      </c>
+      <c r="B3" s="59" t="s">
+        <v>182</v>
+      </c>
+      <c r="C3" s="59">
+        <v>15</v>
+      </c>
+      <c r="D3" s="59">
+        <v>16</v>
+      </c>
+      <c r="E3" s="64">
+        <v>45658</v>
+      </c>
+      <c r="F3" s="64">
+        <v>46113</v>
+      </c>
+      <c r="G3" s="64">
+        <v>45658</v>
+      </c>
+      <c r="H3" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="I3" s="59" t="s">
+        <v>179</v>
+      </c>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59">
+        <v>200</v>
+      </c>
+      <c r="M3" s="65"/>
+      <c r="N3" s="65"/>
+      <c r="O3" s="65"/>
+      <c r="P3" s="65"/>
+      <c r="Q3" s="65"/>
+      <c r="R3" s="65"/>
+      <c r="S3" s="65"/>
+      <c r="T3" s="65"/>
+      <c r="U3" s="65"/>
+      <c r="V3" s="65"/>
+      <c r="W3" s="65"/>
+      <c r="X3" s="65"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A4" s="59" t="s">
+        <v>219</v>
+      </c>
+      <c r="B4" s="59" t="s">
+        <v>164</v>
+      </c>
+      <c r="C4" s="59">
+        <v>17</v>
+      </c>
+      <c r="D4" s="59">
+        <v>18</v>
+      </c>
+      <c r="E4" s="64">
+        <v>45658</v>
+      </c>
+      <c r="F4" s="64">
+        <v>46113</v>
+      </c>
+      <c r="G4" s="64">
+        <v>45658</v>
+      </c>
+      <c r="H4" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="I4" s="59" t="s">
+        <v>179</v>
+      </c>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59">
+        <v>200</v>
+      </c>
+      <c r="M4" s="65"/>
+      <c r="N4" s="65"/>
+      <c r="O4" s="65"/>
+      <c r="P4" s="65"/>
+      <c r="Q4" s="65"/>
+      <c r="R4" s="65"/>
+      <c r="S4" s="65"/>
+      <c r="T4" s="65"/>
+      <c r="U4" s="65"/>
+      <c r="V4" s="65"/>
+      <c r="W4" s="65"/>
+      <c r="X4" s="65"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A5" s="59" t="s">
+        <v>220</v>
+      </c>
+      <c r="B5" s="59" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" s="59">
+        <v>17</v>
+      </c>
+      <c r="D5" s="59">
+        <v>18</v>
+      </c>
+      <c r="E5" s="64">
+        <v>45658</v>
+      </c>
+      <c r="F5" s="64">
+        <v>46113</v>
+      </c>
+      <c r="G5" s="64">
+        <v>45658</v>
+      </c>
+      <c r="H5" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="I5" s="59" t="s">
+        <v>179</v>
+      </c>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59">
+        <v>200</v>
+      </c>
+      <c r="M5" s="65"/>
+      <c r="N5" s="65"/>
+      <c r="O5" s="65"/>
+      <c r="P5" s="65"/>
+      <c r="Q5" s="65"/>
+      <c r="R5" s="65"/>
+      <c r="S5" s="65"/>
+      <c r="T5" s="65"/>
+      <c r="U5" s="65"/>
+      <c r="V5" s="65"/>
+      <c r="W5" s="65"/>
+      <c r="X5" s="65"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A6" s="59" t="s">
+        <v>190</v>
+      </c>
+      <c r="B6" s="59" t="s">
+        <v>164</v>
+      </c>
+      <c r="C6" s="59">
+        <v>19</v>
+      </c>
+      <c r="D6" s="59">
+        <v>100</v>
+      </c>
+      <c r="E6" s="64">
+        <v>45658</v>
+      </c>
+      <c r="F6" s="64">
+        <v>46113</v>
+      </c>
+      <c r="G6" s="64">
+        <v>45658</v>
+      </c>
+      <c r="H6" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="I6" s="59" t="s">
+        <v>179</v>
+      </c>
+      <c r="J6" s="59"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="59">
+        <v>200</v>
+      </c>
+      <c r="M6" s="65"/>
+      <c r="N6" s="65"/>
+      <c r="O6" s="65"/>
+      <c r="P6" s="65"/>
+      <c r="Q6" s="65"/>
+      <c r="R6" s="65"/>
+      <c r="S6" s="65"/>
+      <c r="T6" s="65"/>
+      <c r="U6" s="65"/>
+      <c r="V6" s="65"/>
+      <c r="W6" s="65"/>
+      <c r="X6" s="65"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A7" s="59" t="s">
+        <v>191</v>
+      </c>
+      <c r="B7" s="59" t="s">
+        <v>182</v>
+      </c>
+      <c r="C7" s="59">
+        <v>19</v>
+      </c>
+      <c r="D7" s="59">
+        <v>100</v>
+      </c>
+      <c r="E7" s="64">
+        <v>45658</v>
+      </c>
+      <c r="F7" s="64">
+        <v>46113</v>
+      </c>
+      <c r="G7" s="64">
+        <v>45658</v>
+      </c>
+      <c r="H7" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="I7" s="59" t="s">
+        <v>179</v>
+      </c>
+      <c r="J7" s="59"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="59">
+        <v>200</v>
+      </c>
+      <c r="M7" s="65">
+        <v>3.6493055555555557E-4</v>
+      </c>
+      <c r="N7" s="65">
+        <v>5.7962962962962959E-4</v>
+      </c>
+      <c r="O7" s="65">
+        <v>7.8923611111111111E-4</v>
+      </c>
+      <c r="P7" s="65">
+        <v>6.3819444444444449E-4</v>
+      </c>
+      <c r="Q7" s="65">
+        <v>1.6078703703703706E-3</v>
+      </c>
+      <c r="R7" s="65">
+        <v>1.5675925925925926E-3</v>
+      </c>
+      <c r="S7" s="65">
+        <v>3.8645833333333333E-4</v>
+      </c>
+      <c r="T7" s="65">
+        <v>6.1435185185185182E-4</v>
+      </c>
+      <c r="U7" s="65">
+        <v>8.3657407407407411E-4</v>
+      </c>
+      <c r="V7" s="65">
+        <v>6.7650462962962966E-4</v>
+      </c>
+      <c r="W7" s="65">
+        <v>1.704398148148148E-3</v>
+      </c>
+      <c r="X7" s="65">
+        <v>1.6616898148148148E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B608451-5D1D-4665-BFE6-00A11E29A180}">
+  <sheetPr codeName="Tabelle10">
+    <tabColor theme="5"/>
+  </sheetPr>
+  <dimension ref="A1:X3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="27" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="27" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="22" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A1" s="59" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="59" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" s="59" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1" s="59" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="59" t="s">
+        <v>165</v>
+      </c>
+      <c r="F1" s="59" t="s">
+        <v>166</v>
+      </c>
+      <c r="G1" s="59" t="s">
+        <v>167</v>
+      </c>
+      <c r="H1" s="59" t="s">
+        <v>168</v>
+      </c>
+      <c r="I1" s="59" t="s">
+        <v>170</v>
+      </c>
+      <c r="J1" s="59" t="s">
+        <v>169</v>
+      </c>
+      <c r="K1" s="59" t="s">
+        <v>171</v>
+      </c>
+      <c r="L1" s="59" t="s">
+        <v>176</v>
+      </c>
+      <c r="M1" s="59" t="s">
+        <v>203</v>
+      </c>
+      <c r="N1" s="59" t="s">
+        <v>204</v>
+      </c>
+      <c r="O1" s="59" t="s">
+        <v>205</v>
+      </c>
+      <c r="P1" s="59" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q1" s="59" t="s">
+        <v>207</v>
+      </c>
+      <c r="R1" s="59" t="s">
+        <v>206</v>
+      </c>
+      <c r="S1" s="59" t="s">
+        <v>209</v>
+      </c>
+      <c r="T1" s="59" t="s">
+        <v>210</v>
+      </c>
+      <c r="U1" s="59" t="s">
+        <v>211</v>
+      </c>
+      <c r="V1" s="59" t="s">
+        <v>212</v>
+      </c>
+      <c r="W1" s="59" t="s">
+        <v>213</v>
+      </c>
+      <c r="X1" s="59" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2" s="59" t="s">
+        <v>215</v>
+      </c>
+      <c r="B2" s="59" t="s">
+        <v>164</v>
+      </c>
+      <c r="C2" s="59">
+        <v>15</v>
+      </c>
+      <c r="D2" s="59">
+        <v>18</v>
+      </c>
       <c r="E2" s="59" t="s">
         <v>188</v>
       </c>
@@ -12027,13 +12467,13 @@
         <v>221</v>
       </c>
       <c r="G2" s="59" t="s">
-        <v>188</v>
+        <v>198</v>
       </c>
       <c r="H2" s="59" t="s">
         <v>178</v>
       </c>
       <c r="I2" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J2" s="59"/>
       <c r="K2" s="59"/>
@@ -12053,9 +12493,9 @@
       <c r="W2" s="59"/>
       <c r="X2" s="59"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="59" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B3" s="59" t="s">
         <v>182</v>
@@ -12064,410 +12504,13 @@
         <v>15</v>
       </c>
       <c r="D3" s="59">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E3" s="59" t="s">
         <v>188</v>
       </c>
       <c r="F3" s="59" t="s">
         <v>221</v>
-      </c>
-      <c r="G3" s="59" t="s">
-        <v>188</v>
-      </c>
-      <c r="H3" s="59" t="s">
-        <v>178</v>
-      </c>
-      <c r="I3" s="59" t="s">
-        <v>179</v>
-      </c>
-      <c r="J3" s="59"/>
-      <c r="K3" s="59"/>
-      <c r="L3" s="59">
-        <v>200</v>
-      </c>
-      <c r="M3" s="59"/>
-      <c r="N3" s="59"/>
-      <c r="O3" s="59"/>
-      <c r="P3" s="59"/>
-      <c r="Q3" s="59"/>
-      <c r="R3" s="59"/>
-      <c r="S3" s="59"/>
-      <c r="T3" s="59"/>
-      <c r="U3" s="59"/>
-      <c r="V3" s="59"/>
-      <c r="W3" s="59"/>
-      <c r="X3" s="59"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A4" s="59" t="s">
-        <v>219</v>
-      </c>
-      <c r="B4" s="59" t="s">
-        <v>164</v>
-      </c>
-      <c r="C4" s="59">
-        <v>17</v>
-      </c>
-      <c r="D4" s="59">
-        <v>18</v>
-      </c>
-      <c r="E4" s="59" t="s">
-        <v>188</v>
-      </c>
-      <c r="F4" s="59" t="s">
-        <v>221</v>
-      </c>
-      <c r="G4" s="59" t="s">
-        <v>188</v>
-      </c>
-      <c r="H4" s="59" t="s">
-        <v>178</v>
-      </c>
-      <c r="I4" s="59" t="s">
-        <v>179</v>
-      </c>
-      <c r="J4" s="59"/>
-      <c r="K4" s="59"/>
-      <c r="L4" s="59">
-        <v>200</v>
-      </c>
-      <c r="M4" s="59"/>
-      <c r="N4" s="59"/>
-      <c r="O4" s="59"/>
-      <c r="P4" s="59"/>
-      <c r="Q4" s="59"/>
-      <c r="R4" s="59"/>
-      <c r="S4" s="59"/>
-      <c r="T4" s="59"/>
-      <c r="U4" s="59"/>
-      <c r="V4" s="59"/>
-      <c r="W4" s="59"/>
-      <c r="X4" s="59"/>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A5" s="59" t="s">
-        <v>220</v>
-      </c>
-      <c r="B5" s="59" t="s">
-        <v>182</v>
-      </c>
-      <c r="C5" s="59">
-        <v>17</v>
-      </c>
-      <c r="D5" s="59">
-        <v>18</v>
-      </c>
-      <c r="E5" s="59" t="s">
-        <v>188</v>
-      </c>
-      <c r="F5" s="59" t="s">
-        <v>221</v>
-      </c>
-      <c r="G5" s="59" t="s">
-        <v>188</v>
-      </c>
-      <c r="H5" s="59" t="s">
-        <v>178</v>
-      </c>
-      <c r="I5" s="59" t="s">
-        <v>179</v>
-      </c>
-      <c r="J5" s="59"/>
-      <c r="K5" s="59"/>
-      <c r="L5" s="59">
-        <v>200</v>
-      </c>
-      <c r="M5" s="59"/>
-      <c r="N5" s="59"/>
-      <c r="O5" s="59"/>
-      <c r="P5" s="59"/>
-      <c r="Q5" s="59"/>
-      <c r="R5" s="59"/>
-      <c r="S5" s="59"/>
-      <c r="T5" s="59"/>
-      <c r="U5" s="59"/>
-      <c r="V5" s="59"/>
-      <c r="W5" s="59"/>
-      <c r="X5" s="59"/>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A6" s="59" t="s">
-        <v>190</v>
-      </c>
-      <c r="B6" s="59" t="s">
-        <v>164</v>
-      </c>
-      <c r="C6" s="59">
-        <v>19</v>
-      </c>
-      <c r="D6" s="59">
-        <v>100</v>
-      </c>
-      <c r="E6" s="59" t="s">
-        <v>188</v>
-      </c>
-      <c r="F6" s="59" t="s">
-        <v>221</v>
-      </c>
-      <c r="G6" s="59" t="s">
-        <v>188</v>
-      </c>
-      <c r="H6" s="59" t="s">
-        <v>178</v>
-      </c>
-      <c r="I6" s="59" t="s">
-        <v>179</v>
-      </c>
-      <c r="J6" s="59"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="59">
-        <v>200</v>
-      </c>
-      <c r="M6" s="59"/>
-      <c r="N6" s="59"/>
-      <c r="O6" s="59"/>
-      <c r="P6" s="59"/>
-      <c r="Q6" s="59"/>
-      <c r="R6" s="59"/>
-      <c r="S6" s="59"/>
-      <c r="T6" s="59"/>
-      <c r="U6" s="59"/>
-      <c r="V6" s="59"/>
-      <c r="W6" s="59"/>
-      <c r="X6" s="59"/>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A7" s="59" t="s">
-        <v>191</v>
-      </c>
-      <c r="B7" s="59" t="s">
-        <v>182</v>
-      </c>
-      <c r="C7" s="59">
-        <v>19</v>
-      </c>
-      <c r="D7" s="59">
-        <v>100</v>
-      </c>
-      <c r="E7" s="59" t="s">
-        <v>188</v>
-      </c>
-      <c r="F7" s="59" t="s">
-        <v>221</v>
-      </c>
-      <c r="G7" s="59" t="s">
-        <v>188</v>
-      </c>
-      <c r="H7" s="59" t="s">
-        <v>178</v>
-      </c>
-      <c r="I7" s="59" t="s">
-        <v>179</v>
-      </c>
-      <c r="J7" s="59"/>
-      <c r="K7" s="59"/>
-      <c r="L7" s="59">
-        <v>200</v>
-      </c>
-      <c r="M7" s="59"/>
-      <c r="N7" s="59"/>
-      <c r="O7" s="59"/>
-      <c r="P7" s="59"/>
-      <c r="Q7" s="59"/>
-      <c r="R7" s="59"/>
-      <c r="S7" s="59"/>
-      <c r="T7" s="59"/>
-      <c r="U7" s="59"/>
-      <c r="V7" s="59"/>
-      <c r="W7" s="59"/>
-      <c r="X7" s="59"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B608451-5D1D-4665-BFE6-00A11E29A180}">
-  <sheetPr>
-    <tabColor theme="5"/>
-  </sheetPr>
-  <dimension ref="A1:X3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="17.06640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.06640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.86328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.59765625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.9296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.59765625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.59765625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="27" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.06640625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.59765625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21.59765625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="27" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="22.06640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A1" s="59" t="s">
-        <v>161</v>
-      </c>
-      <c r="B1" s="59" t="s">
-        <v>163</v>
-      </c>
-      <c r="C1" s="59" t="s">
-        <v>202</v>
-      </c>
-      <c r="D1" s="59" t="s">
-        <v>16</v>
-      </c>
-      <c r="E1" s="59" t="s">
-        <v>165</v>
-      </c>
-      <c r="F1" s="59" t="s">
-        <v>166</v>
-      </c>
-      <c r="G1" s="59" t="s">
-        <v>167</v>
-      </c>
-      <c r="H1" s="59" t="s">
-        <v>168</v>
-      </c>
-      <c r="I1" s="59" t="s">
-        <v>170</v>
-      </c>
-      <c r="J1" s="59" t="s">
-        <v>169</v>
-      </c>
-      <c r="K1" s="59" t="s">
-        <v>171</v>
-      </c>
-      <c r="L1" s="59" t="s">
-        <v>176</v>
-      </c>
-      <c r="M1" s="59" t="s">
-        <v>203</v>
-      </c>
-      <c r="N1" s="59" t="s">
-        <v>204</v>
-      </c>
-      <c r="O1" s="59" t="s">
-        <v>205</v>
-      </c>
-      <c r="P1" s="59" t="s">
-        <v>208</v>
-      </c>
-      <c r="Q1" s="59" t="s">
-        <v>207</v>
-      </c>
-      <c r="R1" s="59" t="s">
-        <v>206</v>
-      </c>
-      <c r="S1" s="59" t="s">
-        <v>209</v>
-      </c>
-      <c r="T1" s="59" t="s">
-        <v>210</v>
-      </c>
-      <c r="U1" s="59" t="s">
-        <v>211</v>
-      </c>
-      <c r="V1" s="59" t="s">
-        <v>212</v>
-      </c>
-      <c r="W1" s="59" t="s">
-        <v>213</v>
-      </c>
-      <c r="X1" s="59" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A2" s="59" t="s">
-        <v>215</v>
-      </c>
-      <c r="B2" s="59" t="s">
-        <v>164</v>
-      </c>
-      <c r="C2" s="59">
-        <v>15</v>
-      </c>
-      <c r="D2" s="59">
-        <v>18</v>
-      </c>
-      <c r="E2" s="59" t="s">
-        <v>188</v>
-      </c>
-      <c r="F2" s="59" t="s">
-        <v>222</v>
-      </c>
-      <c r="G2" s="59" t="s">
-        <v>198</v>
-      </c>
-      <c r="H2" s="59" t="s">
-        <v>178</v>
-      </c>
-      <c r="I2" s="59" t="s">
-        <v>180</v>
-      </c>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59">
-        <v>200</v>
-      </c>
-      <c r="M2" s="59"/>
-      <c r="N2" s="59"/>
-      <c r="O2" s="59"/>
-      <c r="P2" s="59"/>
-      <c r="Q2" s="59"/>
-      <c r="R2" s="59"/>
-      <c r="S2" s="59"/>
-      <c r="T2" s="59"/>
-      <c r="U2" s="59"/>
-      <c r="V2" s="59"/>
-      <c r="W2" s="59"/>
-      <c r="X2" s="59"/>
-    </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A3" s="59" t="s">
-        <v>216</v>
-      </c>
-      <c r="B3" s="59" t="s">
-        <v>182</v>
-      </c>
-      <c r="C3" s="59">
-        <v>15</v>
-      </c>
-      <c r="D3" s="59">
-        <v>18</v>
-      </c>
-      <c r="E3" s="59" t="s">
-        <v>188</v>
-      </c>
-      <c r="F3" s="59" t="s">
-        <v>222</v>
       </c>
       <c r="G3" s="59" t="s">
         <v>198</v>
@@ -12515,15 +12558,15 @@
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.86328125" style="1" customWidth="1"/>
-    <col min="2" max="13" width="18.73046875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
+    <col min="2" max="13" width="18.7109375" style="1" customWidth="1"/>
     <col min="14" max="14" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="11.3984375" style="1"/>
+    <col min="15" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18">
         <v>2024</v>
       </c>
@@ -12567,7 +12610,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
@@ -12623,7 +12666,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -12679,7 +12722,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>8</v>
       </c>
@@ -12735,7 +12778,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="62" t="s">
         <v>13</v>
       </c>
@@ -12753,7 +12796,7 @@
       <c r="M7" s="62"/>
       <c r="N7" s="62"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="62"/>
       <c r="B8" s="62"/>
       <c r="C8" s="62"/>
@@ -12769,7 +12812,7 @@
       <c r="M8" s="62"/>
       <c r="N8" s="62"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>6</v>
       </c>
@@ -12823,7 +12866,7 @@
       </c>
       <c r="N9" s="21"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>7</v>
       </c>
@@ -12877,7 +12920,7 @@
       </c>
       <c r="N10" s="21"/>
     </row>
-    <row r="11" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>8</v>
       </c>
@@ -12931,7 +12974,7 @@
       </c>
       <c r="N11" s="23"/>
     </row>
-    <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="61" t="s">
         <v>14</v>
       </c>
@@ -12952,7 +12995,7 @@
       <c r="M14"/>
       <c r="N14"/>
     </row>
-    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="61"/>
       <c r="B15" s="61"/>
       <c r="C15" s="61"/>
@@ -12967,7 +13010,7 @@
       <c r="M15"/>
       <c r="N15"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -13002,7 +13045,7 @@
       <c r="M16"/>
       <c r="N16"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>19</v>
       </c>
@@ -13037,7 +13080,7 @@
       <c r="M17"/>
       <c r="N17"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>19</v>
       </c>
@@ -13070,7 +13113,7 @@
       <c r="M18"/>
       <c r="N18"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>22</v>
       </c>
@@ -13103,7 +13146,7 @@
       <c r="M19"/>
       <c r="N19"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>24</v>
       </c>
@@ -13134,7 +13177,7 @@
       <c r="M20"/>
       <c r="N20"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>22</v>
       </c>
@@ -13161,7 +13204,7 @@
       <c r="M21"/>
       <c r="N21"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>19</v>
       </c>
@@ -13184,7 +13227,7 @@
       <c r="I22" s="33"/>
       <c r="L22" s="41"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>19</v>
       </c>
@@ -13207,50 +13250,50 @@
       <c r="I23" s="33"/>
       <c r="L23" s="40"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H24" s="33"/>
       <c r="I24" s="33"/>
       <c r="L24" s="41"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H25" s="33"/>
       <c r="I25" s="33"/>
       <c r="L25" s="40"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L26" s="41"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L27" s="40"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L28" s="41"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L29" s="40"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L30" s="41"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L31" s="40"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L32" s="41"/>
     </row>
-    <row r="33" spans="12:12" x14ac:dyDescent="0.45">
+    <row r="33" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L33" s="40"/>
     </row>
-    <row r="34" spans="12:12" x14ac:dyDescent="0.45">
+    <row r="34" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L34" s="41"/>
     </row>
-    <row r="35" spans="12:12" x14ac:dyDescent="0.45">
+    <row r="35" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L35" s="33"/>
     </row>
-    <row r="36" spans="12:12" x14ac:dyDescent="0.45">
+    <row r="36" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L36" s="41"/>
     </row>
-    <row r="37" spans="12:12" x14ac:dyDescent="0.45">
+    <row r="37" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L37" s="33"/>
     </row>
   </sheetData>
@@ -13276,15 +13319,15 @@
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.86328125" style="1" customWidth="1"/>
-    <col min="2" max="13" width="18.73046875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
+    <col min="2" max="13" width="18.7109375" style="1" customWidth="1"/>
     <col min="14" max="14" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="11.3984375" style="1"/>
+    <col min="15" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18">
         <v>2025</v>
       </c>
@@ -13328,7 +13371,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
@@ -13384,7 +13427,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -13440,7 +13483,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>8</v>
       </c>
@@ -13496,7 +13539,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="62" t="s">
         <v>13</v>
       </c>
@@ -13514,7 +13557,7 @@
       <c r="M7" s="62"/>
       <c r="N7" s="62"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="62"/>
       <c r="B8" s="62"/>
       <c r="C8" s="62"/>
@@ -13530,7 +13573,7 @@
       <c r="M8" s="62"/>
       <c r="N8" s="62"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>6</v>
       </c>
@@ -13584,7 +13627,7 @@
       </c>
       <c r="N9" s="21"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>7</v>
       </c>
@@ -13638,7 +13681,7 @@
       </c>
       <c r="N10" s="21"/>
     </row>
-    <row r="11" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>8</v>
       </c>
@@ -13692,7 +13735,7 @@
       </c>
       <c r="N11" s="23"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="61" t="s">
         <v>14</v>
       </c>
@@ -13711,7 +13754,7 @@
       </c>
       <c r="M14"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="61"/>
       <c r="B15" s="61"/>
       <c r="C15" s="61"/>
@@ -13724,7 +13767,7 @@
       <c r="L15" s="63"/>
       <c r="M15"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -13757,7 +13800,7 @@
       </c>
       <c r="M16"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>28</v>
       </c>
@@ -13790,7 +13833,7 @@
       </c>
       <c r="M17"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>28</v>
       </c>
@@ -13821,7 +13864,7 @@
       <c r="L18" s="38"/>
       <c r="M18"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>29</v>
       </c>
@@ -13852,7 +13895,7 @@
       <c r="L19" s="36"/>
       <c r="M19"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>30</v>
       </c>
@@ -13881,7 +13924,7 @@
       <c r="L20" s="38"/>
       <c r="M20"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>29</v>
       </c>
@@ -13912,7 +13955,7 @@
       <c r="L21" s="36"/>
       <c r="M21"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>28</v>
       </c>
@@ -13943,7 +13986,7 @@
       <c r="L22" s="39"/>
       <c r="M22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>28</v>
       </c>
@@ -13974,66 +14017,66 @@
       <c r="L23" s="37"/>
       <c r="M23"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H24" s="40"/>
       <c r="I24" s="40"/>
       <c r="J24" s="40"/>
       <c r="L24" s="39"/>
       <c r="M24"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H25" s="33"/>
       <c r="I25" s="33"/>
       <c r="L25" s="37"/>
       <c r="M25"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L26" s="39"/>
       <c r="M26"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L27" s="37"/>
       <c r="M27"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L28" s="39"/>
       <c r="M28"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L29" s="37"/>
       <c r="M29"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L30" s="39"/>
       <c r="M30"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L31" s="37"/>
       <c r="M31"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L32" s="39"/>
       <c r="M32"/>
     </row>
-    <row r="33" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="33" spans="8:13" x14ac:dyDescent="0.25">
       <c r="L33" s="37"/>
       <c r="M33"/>
     </row>
-    <row r="34" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="34" spans="8:13" x14ac:dyDescent="0.25">
       <c r="L34" s="39"/>
       <c r="M34"/>
     </row>
-    <row r="35" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="35" spans="8:13" x14ac:dyDescent="0.25">
       <c r="M35"/>
     </row>
-    <row r="36" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="36" spans="8:13" x14ac:dyDescent="0.25">
       <c r="L36" s="39"/>
       <c r="M36"/>
     </row>
-    <row r="37" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="37" spans="8:13" x14ac:dyDescent="0.25">
       <c r="M37"/>
     </row>
-    <row r="38" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="38" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H38"/>
       <c r="I38"/>
       <c r="J38"/>
@@ -14041,7 +14084,7 @@
       <c r="L38"/>
       <c r="M38"/>
     </row>
-    <row r="39" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="39" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H39"/>
       <c r="I39"/>
       <c r="J39"/>

</xml_diff>

<commit_message>
Record Krits full with dem PZ times
</commit_message>
<xml_diff>
--- a/web/utilities/records_kriterien.xlsx
+++ b/web/utilities/records_kriterien.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgna\Documents\GitHub\Lifesaving_Baden\web\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D509DC-20C8-4725-96CA-B047B786CA17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E630187B-B96C-4675-A2D4-D95AD23C151E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
   </bookViews>
@@ -1332,6 +1332,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1341,78 +1347,12 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="194">
     <dxf>
-      <numFmt numFmtId="164" formatCode="m:ss.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m:ss.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m:ss.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m:ss.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m:ss.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m:ss.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m:ss.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m:ss.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m:ss.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m:ss.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m:ss.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m:ss.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <color theme="6"/>
       </font>
@@ -1581,18 +1521,78 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="m:ss.00"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="m:ss.00"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="m:ss.00"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="m:ss.00"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="m:ss.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m:ss.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m:ss.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m:ss.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m:ss.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m:ss.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m:ss.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m:ss.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -3963,33 +3963,33 @@
     <tableColumn id="2" xr3:uid="{6346FF3B-B334-4CD8-8B23-F2347E29C536}" name="Geschlecht" dataDxfId="66"/>
     <tableColumn id="3" xr3:uid="{E793B48A-BC8A-439F-8AAF-6FD08104A619}" name="Mindest Alter" dataDxfId="65"/>
     <tableColumn id="4" xr3:uid="{01A62C29-2F75-4107-A431-F69230BCCD0C}" name="Maximales Alter" dataDxfId="64"/>
-    <tableColumn id="5" xr3:uid="{B7E4DE90-7856-4A0C-9063-61414D7F227C}" name="Qualizeitraum anfang" dataDxfId="14"/>
-    <tableColumn id="6" xr3:uid="{B00F7CD1-82CB-42B9-A396-89F79EF419CA}" name="Qualizeitraum Ende" dataDxfId="13"/>
-    <tableColumn id="7" xr3:uid="{9E50DDE5-12E3-4BCB-801C-FBABCE309F0E}" name="Letzter Wettkampf am" dataDxfId="12"/>
-    <tableColumn id="8" xr3:uid="{57E68247-0FF2-48D8-8ACD-AB057E576A21}" name="Landesverband" dataDxfId="63"/>
-    <tableColumn id="9" xr3:uid="{EBAA439D-F69A-4C2A-8193-9AE08F1E57B8}" name="OMS" dataDxfId="62"/>
-    <tableColumn id="10" xr3:uid="{BBD11E7F-3DDF-428A-B005-4A40E6FA78DC}" name="Pool-Länge" dataDxfId="61"/>
-    <tableColumn id="11" xr3:uid="{6AE38DCA-A084-4F3D-A6A4-4E76E3E2CBC6}" name="Regelwerk" dataDxfId="60"/>
-    <tableColumn id="12" xr3:uid="{7F7470AD-5502-4CEE-BB4C-44BA308E61D7}" name="Seiten Anzahl" dataDxfId="59"/>
-    <tableColumn id="13" xr3:uid="{F416CBFA-4C9D-45CD-9BA7-E4BC57A08BC2}" name="PZ1 - 50m Retten" dataDxfId="11"/>
-    <tableColumn id="14" xr3:uid="{7117DBCA-0DA7-462C-84FE-0DC7E33B124C}" name="PZ1 - 100m Retten" dataDxfId="10"/>
-    <tableColumn id="15" xr3:uid="{E8630E91-DC30-4822-9E53-6D65487C3670}" name="PZ1 - 100m Kombi" dataDxfId="9"/>
-    <tableColumn id="16" xr3:uid="{4B3AA225-E042-430F-8259-D176887B4528}" name="PZ1 - 100m Lifesaver" dataDxfId="8"/>
-    <tableColumn id="17" xr3:uid="{798674BD-98CE-4531-BDFF-6AB06253AD7C}" name="PZ1 - 200m Super-Lifesaver" dataDxfId="7"/>
-    <tableColumn id="18" xr3:uid="{8809BB71-D58B-4E8B-A442-D0EB9A65A25D}" name="PZ1 - 200m Hindernis" dataDxfId="6"/>
-    <tableColumn id="19" xr3:uid="{93DCF463-806B-4117-B4E3-1FFAE976B37C}" name="PZ2 - 50m Retten" dataDxfId="5"/>
-    <tableColumn id="20" xr3:uid="{A514C961-559E-462F-B143-BA30974C0129}" name="PZ2 - 100m Retten" dataDxfId="4"/>
-    <tableColumn id="21" xr3:uid="{F1CF6143-45FE-498D-93D6-36F26D2F3C0B}" name="PZ2 - 100m Kombi" dataDxfId="3"/>
-    <tableColumn id="22" xr3:uid="{E90962FC-C214-467F-841F-40DF60E41456}" name="PZ2 - 100m Lifesaver" dataDxfId="2"/>
-    <tableColumn id="23" xr3:uid="{7FBC6334-C4C8-4B38-9F59-30ED95A44379}" name="PZ2 - 200m Super-Lifesaver" dataDxfId="1"/>
-    <tableColumn id="24" xr3:uid="{231BFF86-8F3A-4BA1-B25E-28175D9EDFA9}" name="PZ2 - 200m Hindernis" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{B7E4DE90-7856-4A0C-9063-61414D7F227C}" name="Qualizeitraum anfang" dataDxfId="63"/>
+    <tableColumn id="6" xr3:uid="{B00F7CD1-82CB-42B9-A396-89F79EF419CA}" name="Qualizeitraum Ende" dataDxfId="62"/>
+    <tableColumn id="7" xr3:uid="{9E50DDE5-12E3-4BCB-801C-FBABCE309F0E}" name="Letzter Wettkampf am" dataDxfId="61"/>
+    <tableColumn id="8" xr3:uid="{57E68247-0FF2-48D8-8ACD-AB057E576A21}" name="Landesverband" dataDxfId="60"/>
+    <tableColumn id="9" xr3:uid="{EBAA439D-F69A-4C2A-8193-9AE08F1E57B8}" name="OMS" dataDxfId="59"/>
+    <tableColumn id="10" xr3:uid="{BBD11E7F-3DDF-428A-B005-4A40E6FA78DC}" name="Pool-Länge" dataDxfId="58"/>
+    <tableColumn id="11" xr3:uid="{6AE38DCA-A084-4F3D-A6A4-4E76E3E2CBC6}" name="Regelwerk" dataDxfId="57"/>
+    <tableColumn id="12" xr3:uid="{7F7470AD-5502-4CEE-BB4C-44BA308E61D7}" name="Seiten Anzahl" dataDxfId="56"/>
+    <tableColumn id="13" xr3:uid="{F416CBFA-4C9D-45CD-9BA7-E4BC57A08BC2}" name="PZ1 - 50m Retten" dataDxfId="55"/>
+    <tableColumn id="14" xr3:uid="{7117DBCA-0DA7-462C-84FE-0DC7E33B124C}" name="PZ1 - 100m Retten" dataDxfId="54"/>
+    <tableColumn id="15" xr3:uid="{E8630E91-DC30-4822-9E53-6D65487C3670}" name="PZ1 - 100m Kombi" dataDxfId="53"/>
+    <tableColumn id="16" xr3:uid="{4B3AA225-E042-430F-8259-D176887B4528}" name="PZ1 - 100m Lifesaver" dataDxfId="52"/>
+    <tableColumn id="17" xr3:uid="{798674BD-98CE-4531-BDFF-6AB06253AD7C}" name="PZ1 - 200m Super-Lifesaver" dataDxfId="51"/>
+    <tableColumn id="18" xr3:uid="{8809BB71-D58B-4E8B-A442-D0EB9A65A25D}" name="PZ1 - 200m Hindernis" dataDxfId="50"/>
+    <tableColumn id="19" xr3:uid="{93DCF463-806B-4117-B4E3-1FFAE976B37C}" name="PZ2 - 50m Retten" dataDxfId="49"/>
+    <tableColumn id="20" xr3:uid="{A514C961-559E-462F-B143-BA30974C0129}" name="PZ2 - 100m Retten" dataDxfId="48"/>
+    <tableColumn id="21" xr3:uid="{F1CF6143-45FE-498D-93D6-36F26D2F3C0B}" name="PZ2 - 100m Kombi" dataDxfId="47"/>
+    <tableColumn id="22" xr3:uid="{E90962FC-C214-467F-841F-40DF60E41456}" name="PZ2 - 100m Lifesaver" dataDxfId="46"/>
+    <tableColumn id="23" xr3:uid="{7FBC6334-C4C8-4B38-9F59-30ED95A44379}" name="PZ2 - 200m Super-Lifesaver" dataDxfId="45"/>
+    <tableColumn id="24" xr3:uid="{231BFF86-8F3A-4BA1-B25E-28175D9EDFA9}" name="PZ2 - 200m Hindernis" dataDxfId="44"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{38173103-C137-4989-84EA-9BDFE7009E50}" name="Tabelle68" displayName="Tabelle68" ref="A1:X3" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{38173103-C137-4989-84EA-9BDFE7009E50}" name="Tabelle68" displayName="Tabelle68" ref="A1:X3" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
   <autoFilter ref="A1:X3" xr:uid="{38173103-C137-4989-84EA-9BDFE7009E50}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4017,30 +4017,30 @@
     <filterColumn colId="23" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{EC191D47-103E-4808-B80B-20281F480A7B}" name="Tabellen Name" dataDxfId="56"/>
-    <tableColumn id="2" xr3:uid="{B4135B5F-F957-45A0-BE67-B4F753711A01}" name="Geschlecht" dataDxfId="55"/>
-    <tableColumn id="3" xr3:uid="{3E8C5D70-845D-4A0C-8911-63692B806EE3}" name="Mindest Alter" dataDxfId="54"/>
-    <tableColumn id="4" xr3:uid="{951555AA-1D48-4F58-84DA-5A388BC7ACA6}" name="Maximales Alter" dataDxfId="53"/>
-    <tableColumn id="5" xr3:uid="{532345E9-A3F4-4BC3-83A4-BBE007D5BF2F}" name="Qualizeitraum anfang" dataDxfId="52"/>
-    <tableColumn id="6" xr3:uid="{71A6260E-6437-4311-B1E5-334D777DE23B}" name="Qualizeitraum Ende" dataDxfId="51"/>
-    <tableColumn id="7" xr3:uid="{C4D53DE9-9819-4221-8397-DAA183E26E63}" name="Letzter Wettkampf am" dataDxfId="50"/>
-    <tableColumn id="8" xr3:uid="{8A29AFA5-6619-4699-AB42-78F4AD5566E1}" name="Landesverband" dataDxfId="49"/>
-    <tableColumn id="9" xr3:uid="{9AB45004-0EB4-4304-AFD0-4496973A950F}" name="OMS" dataDxfId="48"/>
-    <tableColumn id="10" xr3:uid="{71319762-F54F-4493-84F3-802DFD3DE0D2}" name="Pool-Länge" dataDxfId="47"/>
-    <tableColumn id="11" xr3:uid="{E91F6E89-282A-4B79-A6DF-C43103E9413B}" name="Regelwerk" dataDxfId="46"/>
-    <tableColumn id="12" xr3:uid="{D4638146-A857-41ED-83D1-8E2711E1ED0F}" name="Seiten Anzahl" dataDxfId="45"/>
-    <tableColumn id="13" xr3:uid="{08DB5C03-8197-4058-AF4C-5A2A8CB975EF}" name="PZ1 - 50m Retten" dataDxfId="44"/>
-    <tableColumn id="14" xr3:uid="{94966042-A021-4D1B-83E0-516EF43C47BF}" name="PZ1 - 100m Retten" dataDxfId="43"/>
-    <tableColumn id="15" xr3:uid="{3D118CE3-B383-4B67-8BD7-A4E7270B694D}" name="PZ1 - 100m Kombi" dataDxfId="42"/>
-    <tableColumn id="16" xr3:uid="{2EF5524D-F52F-403A-B1F2-26B06E1561D7}" name="PZ1 - 100m Lifesaver" dataDxfId="41"/>
-    <tableColumn id="17" xr3:uid="{90AFAED0-E3F7-430F-B477-A7B8C0F28C92}" name="PZ1 - 200m Super-Lifesaver" dataDxfId="40"/>
-    <tableColumn id="18" xr3:uid="{234BF89C-A472-4472-A7B5-6E8956546AEB}" name="PZ1 - 200m Hindernis" dataDxfId="39"/>
-    <tableColumn id="19" xr3:uid="{0630350F-8319-4C46-926A-11BAE7DA4892}" name="PZ2 - 50m Retten" dataDxfId="38"/>
-    <tableColumn id="20" xr3:uid="{923F9722-E09F-460A-8B02-64E9F03F0806}" name="PZ2 - 100m Retten" dataDxfId="37"/>
-    <tableColumn id="21" xr3:uid="{AA307655-1197-43FB-A00A-75C1438B2412}" name="PZ2 - 100m Kombi" dataDxfId="36"/>
-    <tableColumn id="22" xr3:uid="{92C209F1-CAD1-4D8C-888D-8F65EE77FFDE}" name="PZ2 - 100m Lifesaver" dataDxfId="35"/>
-    <tableColumn id="23" xr3:uid="{AE53DAA0-7669-4EC4-A7F2-6BFCE8E6960F}" name="PZ2 - 200m Super-Lifesaver" dataDxfId="34"/>
-    <tableColumn id="24" xr3:uid="{AB5DE385-0AE1-401A-8EF5-9ED15B7100C9}" name="PZ2 - 200m Hindernis" dataDxfId="33"/>
+    <tableColumn id="1" xr3:uid="{EC191D47-103E-4808-B80B-20281F480A7B}" name="Tabellen Name" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{B4135B5F-F957-45A0-BE67-B4F753711A01}" name="Geschlecht" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{3E8C5D70-845D-4A0C-8911-63692B806EE3}" name="Mindest Alter" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{951555AA-1D48-4F58-84DA-5A388BC7ACA6}" name="Maximales Alter" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{532345E9-A3F4-4BC3-83A4-BBE007D5BF2F}" name="Qualizeitraum anfang" dataDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{71A6260E-6437-4311-B1E5-334D777DE23B}" name="Qualizeitraum Ende" dataDxfId="36"/>
+    <tableColumn id="7" xr3:uid="{C4D53DE9-9819-4221-8397-DAA183E26E63}" name="Letzter Wettkampf am" dataDxfId="35"/>
+    <tableColumn id="8" xr3:uid="{8A29AFA5-6619-4699-AB42-78F4AD5566E1}" name="Landesverband" dataDxfId="34"/>
+    <tableColumn id="9" xr3:uid="{9AB45004-0EB4-4304-AFD0-4496973A950F}" name="OMS" dataDxfId="33"/>
+    <tableColumn id="10" xr3:uid="{71319762-F54F-4493-84F3-802DFD3DE0D2}" name="Pool-Länge" dataDxfId="32"/>
+    <tableColumn id="11" xr3:uid="{E91F6E89-282A-4B79-A6DF-C43103E9413B}" name="Regelwerk" dataDxfId="31"/>
+    <tableColumn id="12" xr3:uid="{D4638146-A857-41ED-83D1-8E2711E1ED0F}" name="Seiten Anzahl" dataDxfId="30"/>
+    <tableColumn id="13" xr3:uid="{08DB5C03-8197-4058-AF4C-5A2A8CB975EF}" name="PZ1 - 50m Retten" dataDxfId="29"/>
+    <tableColumn id="14" xr3:uid="{94966042-A021-4D1B-83E0-516EF43C47BF}" name="PZ1 - 100m Retten" dataDxfId="28"/>
+    <tableColumn id="15" xr3:uid="{3D118CE3-B383-4B67-8BD7-A4E7270B694D}" name="PZ1 - 100m Kombi" dataDxfId="27"/>
+    <tableColumn id="16" xr3:uid="{2EF5524D-F52F-403A-B1F2-26B06E1561D7}" name="PZ1 - 100m Lifesaver" dataDxfId="26"/>
+    <tableColumn id="17" xr3:uid="{90AFAED0-E3F7-430F-B477-A7B8C0F28C92}" name="PZ1 - 200m Super-Lifesaver" dataDxfId="25"/>
+    <tableColumn id="18" xr3:uid="{234BF89C-A472-4472-A7B5-6E8956546AEB}" name="PZ1 - 200m Hindernis" dataDxfId="24"/>
+    <tableColumn id="19" xr3:uid="{0630350F-8319-4C46-926A-11BAE7DA4892}" name="PZ2 - 50m Retten" dataDxfId="23"/>
+    <tableColumn id="20" xr3:uid="{923F9722-E09F-460A-8B02-64E9F03F0806}" name="PZ2 - 100m Retten" dataDxfId="22"/>
+    <tableColumn id="21" xr3:uid="{AA307655-1197-43FB-A00A-75C1438B2412}" name="PZ2 - 100m Kombi" dataDxfId="21"/>
+    <tableColumn id="22" xr3:uid="{92C209F1-CAD1-4D8C-888D-8F65EE77FFDE}" name="PZ2 - 100m Lifesaver" dataDxfId="20"/>
+    <tableColumn id="23" xr3:uid="{AE53DAA0-7669-4EC4-A7F2-6BFCE8E6960F}" name="PZ2 - 200m Super-Lifesaver" dataDxfId="19"/>
+    <tableColumn id="24" xr3:uid="{AB5DE385-0AE1-401A-8EF5-9ED15B7100C9}" name="PZ2 - 200m Hindernis" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -7985,52 +7985,52 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B5:G31">
-    <cfRule type="expression" dxfId="32" priority="15">
+    <cfRule type="expression" dxfId="17" priority="15">
       <formula>B5&lt;&gt;B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:M31">
-    <cfRule type="expression" dxfId="31" priority="14">
+    <cfRule type="expression" dxfId="16" priority="14">
       <formula>H5&lt;&gt;H4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N5:S31">
-    <cfRule type="expression" dxfId="30" priority="13">
+    <cfRule type="expression" dxfId="15" priority="13">
       <formula>N5&lt;&gt;N4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T5:Y31">
-    <cfRule type="expression" dxfId="29" priority="12">
+    <cfRule type="expression" dxfId="14" priority="12">
       <formula>T5&lt;&gt;T4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z5:AE31">
-    <cfRule type="expression" dxfId="28" priority="9">
+    <cfRule type="expression" dxfId="13" priority="9">
       <formula>Z5&lt;&gt;Z4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF5:AK31">
-    <cfRule type="expression" dxfId="27" priority="8">
+    <cfRule type="expression" dxfId="12" priority="8">
       <formula>AF5&lt;&gt;AF4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL5:AN31">
-    <cfRule type="expression" dxfId="26" priority="6">
+    <cfRule type="expression" dxfId="11" priority="6">
       <formula>AL5&lt;&gt;AL4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO5:AQ31">
-    <cfRule type="expression" dxfId="25" priority="5">
+    <cfRule type="expression" dxfId="10" priority="5">
       <formula>AO5&lt;&gt;AO4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR5:AT31">
-    <cfRule type="expression" dxfId="24" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>AR5&lt;&gt;AR4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU5:AW31">
-    <cfRule type="expression" dxfId="23" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>AU5&lt;&gt;AU4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8275,38 +8275,38 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="62"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="62"/>
-      <c r="J7" s="62"/>
-      <c r="K7" s="62"/>
-      <c r="L7" s="62"/>
-      <c r="M7" s="62"/>
-      <c r="N7" s="62"/>
+      <c r="B7" s="64"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="64"/>
+      <c r="K7" s="64"/>
+      <c r="L7" s="64"/>
+      <c r="M7" s="64"/>
+      <c r="N7" s="64"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="62"/>
-      <c r="B8" s="62"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="62"/>
-      <c r="E8" s="62"/>
-      <c r="F8" s="62"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="62"/>
-      <c r="I8" s="62"/>
-      <c r="J8" s="62"/>
-      <c r="K8" s="62"/>
-      <c r="L8" s="62"/>
-      <c r="M8" s="62"/>
-      <c r="N8" s="62"/>
+      <c r="A8" s="64"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="64"/>
+      <c r="J8" s="64"/>
+      <c r="K8" s="64"/>
+      <c r="L8" s="64"/>
+      <c r="M8" s="64"/>
+      <c r="N8" s="64"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
@@ -8471,35 +8471,35 @@
       <c r="N11" s="23"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="61" t="s">
+      <c r="A14" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="61"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="61"/>
-      <c r="H14" s="63" t="s">
+      <c r="B14" s="63"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
+      <c r="H14" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="I14" s="63"/>
-      <c r="J14" s="63"/>
-      <c r="L14" s="63" t="s">
+      <c r="I14" s="65"/>
+      <c r="J14" s="65"/>
+      <c r="L14" s="65" t="s">
         <v>36</v>
       </c>
       <c r="M14"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="61"/>
-      <c r="B15" s="61"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="61"/>
-      <c r="H15" s="63"/>
-      <c r="I15" s="63"/>
-      <c r="J15" s="63"/>
-      <c r="L15" s="63"/>
+      <c r="A15" s="63"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="65"/>
+      <c r="J15" s="65"/>
+      <c r="L15" s="65"/>
       <c r="M15"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
@@ -9839,22 +9839,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B6:G6">
-    <cfRule type="expression" dxfId="22" priority="20">
+    <cfRule type="expression" dxfId="7" priority="20">
       <formula>B6&lt;&gt;B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:G32">
-    <cfRule type="expression" dxfId="21" priority="1">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>B7&lt;&gt;B6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:M6">
-    <cfRule type="expression" dxfId="20" priority="22">
+    <cfRule type="expression" dxfId="5" priority="22">
       <formula>H6&lt;&gt;H4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:M32">
-    <cfRule type="expression" dxfId="19" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>H7&lt;&gt;H6</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11190,22 +11190,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B6:G6">
-    <cfRule type="expression" dxfId="18" priority="19">
+    <cfRule type="expression" dxfId="3" priority="19">
       <formula>B6&lt;&gt;B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:G32">
-    <cfRule type="expression" dxfId="17" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>B7&lt;&gt;B6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:M6">
-    <cfRule type="expression" dxfId="16" priority="20">
+    <cfRule type="expression" dxfId="1" priority="20">
       <formula>H6&lt;&gt;H4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:M32">
-    <cfRule type="expression" dxfId="15" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>H7&lt;&gt;H6</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11920,8 +11920,8 @@
   </sheetPr>
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="W7" sqref="W7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12039,13 +12039,13 @@
       <c r="D2" s="59">
         <v>16</v>
       </c>
-      <c r="E2" s="64">
+      <c r="E2" s="61">
         <v>45658</v>
       </c>
-      <c r="F2" s="64">
+      <c r="F2" s="61">
         <v>46113</v>
       </c>
-      <c r="G2" s="64">
+      <c r="G2" s="61">
         <v>45658</v>
       </c>
       <c r="H2" s="59" t="s">
@@ -12057,20 +12057,44 @@
       <c r="J2" s="59"/>
       <c r="K2" s="59"/>
       <c r="L2" s="59">
-        <v>200</v>
-      </c>
-      <c r="M2" s="65"/>
-      <c r="N2" s="65"/>
-      <c r="O2" s="65"/>
-      <c r="P2" s="65"/>
-      <c r="Q2" s="65"/>
-      <c r="R2" s="65"/>
-      <c r="S2" s="65"/>
-      <c r="T2" s="65"/>
-      <c r="U2" s="65"/>
-      <c r="V2" s="65"/>
-      <c r="W2" s="65"/>
-      <c r="X2" s="65"/>
+        <v>10</v>
+      </c>
+      <c r="M2" s="62">
+        <v>4.8136574074074076E-4</v>
+      </c>
+      <c r="N2" s="62">
+        <v>8.0497685185185186E-4</v>
+      </c>
+      <c r="O2" s="62">
+        <v>1.0570601851851852E-3</v>
+      </c>
+      <c r="P2" s="62">
+        <v>8.5497685185185188E-4</v>
+      </c>
+      <c r="Q2" s="62">
+        <v>2.0892361111111112E-3</v>
+      </c>
+      <c r="R2" s="62">
+        <v>1.8401620370370371E-3</v>
+      </c>
+      <c r="S2" s="62">
+        <v>5.0462962962962961E-4</v>
+      </c>
+      <c r="T2" s="62">
+        <v>8.5474537037037029E-4</v>
+      </c>
+      <c r="U2" s="62">
+        <v>1.1590277777777777E-3</v>
+      </c>
+      <c r="V2" s="62">
+        <v>8.9409722222222223E-4</v>
+      </c>
+      <c r="W2" s="62">
+        <v>2.2304398148148149E-3</v>
+      </c>
+      <c r="X2" s="62">
+        <v>1.9623842592592592E-3</v>
+      </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="59" t="s">
@@ -12085,13 +12109,13 @@
       <c r="D3" s="59">
         <v>16</v>
       </c>
-      <c r="E3" s="64">
+      <c r="E3" s="61">
         <v>45658</v>
       </c>
-      <c r="F3" s="64">
+      <c r="F3" s="61">
         <v>46113</v>
       </c>
-      <c r="G3" s="64">
+      <c r="G3" s="61">
         <v>45658</v>
       </c>
       <c r="H3" s="59" t="s">
@@ -12103,20 +12127,44 @@
       <c r="J3" s="59"/>
       <c r="K3" s="59"/>
       <c r="L3" s="59">
-        <v>200</v>
-      </c>
-      <c r="M3" s="65"/>
-      <c r="N3" s="65"/>
-      <c r="O3" s="65"/>
-      <c r="P3" s="65"/>
-      <c r="Q3" s="65"/>
-      <c r="R3" s="65"/>
-      <c r="S3" s="65"/>
-      <c r="T3" s="65"/>
-      <c r="U3" s="65"/>
-      <c r="V3" s="65"/>
-      <c r="W3" s="65"/>
-      <c r="X3" s="65"/>
+        <v>10</v>
+      </c>
+      <c r="M3" s="62">
+        <v>4.2962962962962958E-4</v>
+      </c>
+      <c r="N3" s="62">
+        <v>7.1435185185185187E-4</v>
+      </c>
+      <c r="O3" s="62">
+        <v>9.710648148148149E-4</v>
+      </c>
+      <c r="P3" s="62">
+        <v>7.6932870370370371E-4</v>
+      </c>
+      <c r="Q3" s="62">
+        <v>1.8946759259259257E-3</v>
+      </c>
+      <c r="R3" s="62">
+        <v>1.6849537037037035E-3</v>
+      </c>
+      <c r="S3" s="62">
+        <v>4.5416666666666668E-4</v>
+      </c>
+      <c r="T3" s="62">
+        <v>7.6006944444444451E-4</v>
+      </c>
+      <c r="U3" s="62">
+        <v>1.0402777777777778E-3</v>
+      </c>
+      <c r="V3" s="62">
+        <v>8.1701388888888893E-4</v>
+      </c>
+      <c r="W3" s="62">
+        <v>2.0715277777777776E-3</v>
+      </c>
+      <c r="X3" s="62">
+        <v>1.8121527777777778E-3</v>
+      </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
@@ -12131,13 +12179,13 @@
       <c r="D4" s="59">
         <v>18</v>
       </c>
-      <c r="E4" s="64">
+      <c r="E4" s="61">
         <v>45658</v>
       </c>
-      <c r="F4" s="64">
+      <c r="F4" s="61">
         <v>46113</v>
       </c>
-      <c r="G4" s="64">
+      <c r="G4" s="61">
         <v>45658</v>
       </c>
       <c r="H4" s="59" t="s">
@@ -12149,20 +12197,44 @@
       <c r="J4" s="59"/>
       <c r="K4" s="59"/>
       <c r="L4" s="59">
-        <v>200</v>
-      </c>
-      <c r="M4" s="65"/>
-      <c r="N4" s="65"/>
-      <c r="O4" s="65"/>
-      <c r="P4" s="65"/>
-      <c r="Q4" s="65"/>
-      <c r="R4" s="65"/>
-      <c r="S4" s="65"/>
-      <c r="T4" s="65"/>
-      <c r="U4" s="65"/>
-      <c r="V4" s="65"/>
-      <c r="W4" s="65"/>
-      <c r="X4" s="65"/>
+        <v>10</v>
+      </c>
+      <c r="M4" s="62">
+        <v>4.7048611111111108E-4</v>
+      </c>
+      <c r="N4" s="62">
+        <v>7.8125000000000004E-4</v>
+      </c>
+      <c r="O4" s="62">
+        <v>1.0002314814814815E-3</v>
+      </c>
+      <c r="P4" s="62">
+        <v>8.2349537037037048E-4</v>
+      </c>
+      <c r="Q4" s="62">
+        <v>1.9892361111111113E-3</v>
+      </c>
+      <c r="R4" s="62">
+        <v>1.8848379629629629E-3</v>
+      </c>
+      <c r="S4" s="62">
+        <v>5.0428240740740739E-4</v>
+      </c>
+      <c r="T4" s="62">
+        <v>8.2812499999999998E-4</v>
+      </c>
+      <c r="U4" s="62">
+        <v>1.0603009259259259E-3</v>
+      </c>
+      <c r="V4" s="62">
+        <v>8.729166666666667E-4</v>
+      </c>
+      <c r="W4" s="62">
+        <v>2.1085648148148149E-3</v>
+      </c>
+      <c r="X4" s="62">
+        <v>1.9979166666666665E-3</v>
+      </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
@@ -12177,13 +12249,13 @@
       <c r="D5" s="59">
         <v>18</v>
       </c>
-      <c r="E5" s="64">
+      <c r="E5" s="61">
         <v>45658</v>
       </c>
-      <c r="F5" s="64">
+      <c r="F5" s="61">
         <v>46113</v>
       </c>
-      <c r="G5" s="64">
+      <c r="G5" s="61">
         <v>45658</v>
       </c>
       <c r="H5" s="59" t="s">
@@ -12195,20 +12267,44 @@
       <c r="J5" s="59"/>
       <c r="K5" s="59"/>
       <c r="L5" s="59">
-        <v>200</v>
-      </c>
-      <c r="M5" s="65"/>
-      <c r="N5" s="65"/>
-      <c r="O5" s="65"/>
-      <c r="P5" s="65"/>
-      <c r="Q5" s="65"/>
-      <c r="R5" s="65"/>
-      <c r="S5" s="65"/>
-      <c r="T5" s="65"/>
-      <c r="U5" s="65"/>
-      <c r="V5" s="65"/>
-      <c r="W5" s="65"/>
-      <c r="X5" s="65"/>
+        <v>10</v>
+      </c>
+      <c r="M5" s="62">
+        <v>3.9583333333333338E-4</v>
+      </c>
+      <c r="N5" s="62">
+        <v>6.596064814814815E-4</v>
+      </c>
+      <c r="O5" s="62">
+        <v>8.7384259259259262E-4</v>
+      </c>
+      <c r="P5" s="62">
+        <v>7.2835648148148152E-4</v>
+      </c>
+      <c r="Q5" s="62">
+        <v>1.7810185185185184E-3</v>
+      </c>
+      <c r="R5" s="62">
+        <v>1.6655092592592594E-3</v>
+      </c>
+      <c r="S5" s="62">
+        <v>4.1574074074074077E-4</v>
+      </c>
+      <c r="T5" s="62">
+        <v>6.9918981481481481E-4</v>
+      </c>
+      <c r="U5" s="62">
+        <v>9.2627314814814818E-4</v>
+      </c>
+      <c r="V5" s="62">
+        <v>7.7210648148148136E-4</v>
+      </c>
+      <c r="W5" s="62">
+        <v>1.8949074074074074E-3</v>
+      </c>
+      <c r="X5" s="62">
+        <v>1.7653935185185186E-3</v>
+      </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="59" t="s">
@@ -12223,13 +12319,13 @@
       <c r="D6" s="59">
         <v>100</v>
       </c>
-      <c r="E6" s="64">
+      <c r="E6" s="61">
         <v>45658</v>
       </c>
-      <c r="F6" s="64">
+      <c r="F6" s="61">
         <v>46113</v>
       </c>
-      <c r="G6" s="64">
+      <c r="G6" s="61">
         <v>45658</v>
       </c>
       <c r="H6" s="59" t="s">
@@ -12241,20 +12337,44 @@
       <c r="J6" s="59"/>
       <c r="K6" s="59"/>
       <c r="L6" s="59">
-        <v>200</v>
-      </c>
-      <c r="M6" s="65"/>
-      <c r="N6" s="65"/>
-      <c r="O6" s="65"/>
-      <c r="P6" s="65"/>
-      <c r="Q6" s="65"/>
-      <c r="R6" s="65"/>
-      <c r="S6" s="65"/>
-      <c r="T6" s="65"/>
-      <c r="U6" s="65"/>
-      <c r="V6" s="65"/>
-      <c r="W6" s="65"/>
-      <c r="X6" s="65"/>
+        <v>10</v>
+      </c>
+      <c r="M6" s="62">
+        <v>4.5150462962962961E-4</v>
+      </c>
+      <c r="N6" s="62">
+        <v>7.2407407407407414E-4</v>
+      </c>
+      <c r="O6" s="62">
+        <v>1.0059027777777777E-3</v>
+      </c>
+      <c r="P6" s="62">
+        <v>7.6840277777777779E-4</v>
+      </c>
+      <c r="Q6" s="62">
+        <v>1.9185185185185184E-3</v>
+      </c>
+      <c r="R6" s="62">
+        <v>1.7923611111111113E-3</v>
+      </c>
+      <c r="S6" s="62">
+        <v>4.7858796296296299E-4</v>
+      </c>
+      <c r="T6" s="62">
+        <v>7.6747685185185187E-4</v>
+      </c>
+      <c r="U6" s="62">
+        <v>1.0662037037037038E-3</v>
+      </c>
+      <c r="V6" s="62">
+        <v>8.1446759259259265E-4</v>
+      </c>
+      <c r="W6" s="62">
+        <v>2.0336805555555555E-3</v>
+      </c>
+      <c r="X6" s="62">
+        <v>1.8998842592592594E-3</v>
+      </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="59" t="s">
@@ -12269,13 +12389,13 @@
       <c r="D7" s="59">
         <v>100</v>
       </c>
-      <c r="E7" s="64">
+      <c r="E7" s="61">
         <v>45658</v>
       </c>
-      <c r="F7" s="64">
+      <c r="F7" s="61">
         <v>46113</v>
       </c>
-      <c r="G7" s="64">
+      <c r="G7" s="61">
         <v>45658</v>
       </c>
       <c r="H7" s="59" t="s">
@@ -12287,42 +12407,42 @@
       <c r="J7" s="59"/>
       <c r="K7" s="59"/>
       <c r="L7" s="59">
-        <v>200</v>
-      </c>
-      <c r="M7" s="65">
+        <v>10</v>
+      </c>
+      <c r="M7" s="62">
         <v>3.6493055555555557E-4</v>
       </c>
-      <c r="N7" s="65">
+      <c r="N7" s="62">
         <v>5.7962962962962959E-4</v>
       </c>
-      <c r="O7" s="65">
+      <c r="O7" s="62">
         <v>7.8923611111111111E-4</v>
       </c>
-      <c r="P7" s="65">
+      <c r="P7" s="62">
         <v>6.3819444444444449E-4</v>
       </c>
-      <c r="Q7" s="65">
+      <c r="Q7" s="62">
         <v>1.6078703703703706E-3</v>
       </c>
-      <c r="R7" s="65">
+      <c r="R7" s="62">
         <v>1.5675925925925926E-3</v>
       </c>
-      <c r="S7" s="65">
+      <c r="S7" s="62">
         <v>3.8645833333333333E-4</v>
       </c>
-      <c r="T7" s="65">
+      <c r="T7" s="62">
         <v>6.1435185185185182E-4</v>
       </c>
-      <c r="U7" s="65">
+      <c r="U7" s="62">
         <v>8.3657407407407411E-4</v>
       </c>
-      <c r="V7" s="65">
+      <c r="V7" s="62">
         <v>6.7650462962962966E-4</v>
       </c>
-      <c r="W7" s="65">
+      <c r="W7" s="62">
         <v>1.704398148148148E-3</v>
       </c>
-      <c r="X7" s="65">
+      <c r="X7" s="62">
         <v>1.6616898148148148E-3</v>
       </c>
     </row>
@@ -12779,38 +12899,38 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="62"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="62"/>
-      <c r="J7" s="62"/>
-      <c r="K7" s="62"/>
-      <c r="L7" s="62"/>
-      <c r="M7" s="62"/>
-      <c r="N7" s="62"/>
+      <c r="B7" s="64"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="64"/>
+      <c r="K7" s="64"/>
+      <c r="L7" s="64"/>
+      <c r="M7" s="64"/>
+      <c r="N7" s="64"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="62"/>
-      <c r="B8" s="62"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="62"/>
-      <c r="E8" s="62"/>
-      <c r="F8" s="62"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="62"/>
-      <c r="I8" s="62"/>
-      <c r="J8" s="62"/>
-      <c r="K8" s="62"/>
-      <c r="L8" s="62"/>
-      <c r="M8" s="62"/>
-      <c r="N8" s="62"/>
+      <c r="A8" s="64"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="64"/>
+      <c r="J8" s="64"/>
+      <c r="K8" s="64"/>
+      <c r="L8" s="64"/>
+      <c r="M8" s="64"/>
+      <c r="N8" s="64"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
@@ -12975,38 +13095,38 @@
       <c r="N11" s="23"/>
     </row>
     <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="61" t="s">
+      <c r="A14" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="61"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="61"/>
+      <c r="B14" s="63"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
       <c r="G14"/>
-      <c r="H14" s="63" t="s">
+      <c r="H14" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="I14" s="63"/>
-      <c r="J14" s="63"/>
-      <c r="L14" s="63" t="s">
+      <c r="I14" s="65"/>
+      <c r="J14" s="65"/>
+      <c r="L14" s="65" t="s">
         <v>36</v>
       </c>
       <c r="M14"/>
       <c r="N14"/>
     </row>
     <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="61"/>
-      <c r="B15" s="61"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="61"/>
+      <c r="A15" s="63"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
       <c r="G15"/>
-      <c r="H15" s="63"/>
-      <c r="I15" s="63"/>
-      <c r="J15" s="63"/>
-      <c r="L15" s="63"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="65"/>
+      <c r="J15" s="65"/>
+      <c r="L15" s="65"/>
       <c r="M15"/>
       <c r="N15"/>
     </row>
@@ -13540,38 +13660,38 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="62"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="62"/>
-      <c r="H7" s="62"/>
-      <c r="I7" s="62"/>
-      <c r="J7" s="62"/>
-      <c r="K7" s="62"/>
-      <c r="L7" s="62"/>
-      <c r="M7" s="62"/>
-      <c r="N7" s="62"/>
+      <c r="B7" s="64"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="64"/>
+      <c r="K7" s="64"/>
+      <c r="L7" s="64"/>
+      <c r="M7" s="64"/>
+      <c r="N7" s="64"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="62"/>
-      <c r="B8" s="62"/>
-      <c r="C8" s="62"/>
-      <c r="D8" s="62"/>
-      <c r="E8" s="62"/>
-      <c r="F8" s="62"/>
-      <c r="G8" s="62"/>
-      <c r="H8" s="62"/>
-      <c r="I8" s="62"/>
-      <c r="J8" s="62"/>
-      <c r="K8" s="62"/>
-      <c r="L8" s="62"/>
-      <c r="M8" s="62"/>
-      <c r="N8" s="62"/>
+      <c r="A8" s="64"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="64"/>
+      <c r="J8" s="64"/>
+      <c r="K8" s="64"/>
+      <c r="L8" s="64"/>
+      <c r="M8" s="64"/>
+      <c r="N8" s="64"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
@@ -13736,35 +13856,35 @@
       <c r="N11" s="23"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="61" t="s">
+      <c r="A14" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="61"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="61"/>
-      <c r="H14" s="63" t="s">
+      <c r="B14" s="63"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
+      <c r="H14" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="I14" s="63"/>
-      <c r="J14" s="63"/>
-      <c r="L14" s="63" t="s">
+      <c r="I14" s="65"/>
+      <c r="J14" s="65"/>
+      <c r="L14" s="65" t="s">
         <v>36</v>
       </c>
       <c r="M14"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="61"/>
-      <c r="B15" s="61"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="61"/>
-      <c r="H15" s="63"/>
-      <c r="I15" s="63"/>
-      <c r="J15" s="63"/>
-      <c r="L15" s="63"/>
+      <c r="A15" s="63"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="65"/>
+      <c r="J15" s="65"/>
+      <c r="L15" s="65"/>
       <c r="M15"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
JRP mit JRP Zeiten in Rec.Krit von 2025 (8. und 16. Platz Vorlauf)
</commit_message>
<xml_diff>
--- a/web/utilities/records_kriterien.xlsx
+++ b/web/utilities/records_kriterien.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgna\Documents\GitHub\Lifesaving_Baden\web\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31834D02-0978-44B3-A430-BB215E261E3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF1B48FB-9823-4752-8890-DD64062267C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
   </bookViews>
   <sheets>
     <sheet name="DR" sheetId="9" r:id="rId1"/>
@@ -12473,8 +12473,8 @@
   </sheetPr>
   <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="X3" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12613,40 +12613,40 @@
         <v>10</v>
       </c>
       <c r="M2" s="62">
-        <v>4.8136574074074076E-4</v>
+        <v>4.5474537037037038E-4</v>
       </c>
       <c r="N2" s="62">
-        <v>8.0497685185185186E-4</v>
+        <v>7.3738425925925924E-4</v>
       </c>
       <c r="O2" s="62">
-        <v>1.0570601851851852E-3</v>
+        <v>9.592592592592592E-4</v>
       </c>
       <c r="P2" s="62">
-        <v>8.5497685185185188E-4</v>
+        <v>7.6875000000000001E-4</v>
       </c>
       <c r="Q2" s="62">
-        <v>2.0892361111111112E-3</v>
+        <v>1.9131944444444446E-3</v>
       </c>
       <c r="R2" s="62">
-        <v>1.8401620370370371E-3</v>
+        <v>1.763773148148148E-3</v>
       </c>
       <c r="S2" s="62">
-        <v>5.0462962962962961E-4</v>
+        <v>4.7893518518518521E-4</v>
       </c>
       <c r="T2" s="62">
-        <v>8.5474537037037029E-4</v>
+        <v>7.6481481481481485E-4</v>
       </c>
       <c r="U2" s="62">
-        <v>1.1590277777777777E-3</v>
+        <v>1.0063657407407408E-3</v>
       </c>
       <c r="V2" s="62">
-        <v>8.9409722222222223E-4</v>
+        <v>8.1157407407407415E-4</v>
       </c>
       <c r="W2" s="62">
-        <v>2.2304398148148149E-3</v>
+        <v>1.9793981481481481E-3</v>
       </c>
       <c r="X2" s="62">
-        <v>1.9623842592592592E-3</v>
+        <v>1.8128472222222222E-3</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
@@ -12683,40 +12683,40 @@
         <v>10</v>
       </c>
       <c r="M3" s="62">
-        <v>4.2962962962962958E-4</v>
+        <v>3.8576388888888889E-4</v>
       </c>
       <c r="N3" s="62">
-        <v>7.1435185185185187E-4</v>
+        <v>6.064814814814815E-4</v>
       </c>
       <c r="O3" s="62">
-        <v>9.710648148148149E-4</v>
+        <v>8.3912037037037039E-4</v>
       </c>
       <c r="P3" s="62">
-        <v>7.6932870370370371E-4</v>
+        <v>6.8599537037037045E-4</v>
       </c>
       <c r="Q3" s="62">
-        <v>1.8946759259259257E-3</v>
+        <v>1.6768518518518519E-3</v>
       </c>
       <c r="R3" s="62">
-        <v>1.6849537037037035E-3</v>
+        <v>1.5944444444444443E-3</v>
       </c>
       <c r="S3" s="62">
-        <v>4.5416666666666668E-4</v>
+        <v>4.0127314814814816E-4</v>
       </c>
       <c r="T3" s="62">
-        <v>7.6006944444444451E-4</v>
+        <v>6.4421296296296297E-4</v>
       </c>
       <c r="U3" s="62">
-        <v>1.0402777777777778E-3</v>
+        <v>8.879629629629629E-4</v>
       </c>
       <c r="V3" s="62">
-        <v>8.1701388888888893E-4</v>
+        <v>7.0787037037037032E-4</v>
       </c>
       <c r="W3" s="62">
-        <v>2.0715277777777776E-3</v>
+        <v>1.784722222222222E-3</v>
       </c>
       <c r="X3" s="62">
-        <v>1.8121527777777778E-3</v>
+        <v>1.6582175925925926E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New JRP Record Krit (12. 20. Platz Vorlauf 2025)
</commit_message>
<xml_diff>
--- a/web/utilities/records_kriterien.xlsx
+++ b/web/utilities/records_kriterien.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgna\Documents\GitHub\Lifesaving_Baden\web\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD25F714-0F14-4E5B-ADB4-00830A74F400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FA907B-837B-42C5-8F87-0B753394FB31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
   </bookViews>
   <sheets>
     <sheet name="DR" sheetId="9" r:id="rId1"/>
@@ -12473,8 +12473,8 @@
   </sheetPr>
   <dimension ref="A1:X3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12613,40 +12613,40 @@
         <v>10</v>
       </c>
       <c r="M2" s="62">
-        <v>4.5474537037037038E-4</v>
+        <v>4.6817129629629634E-4</v>
       </c>
       <c r="N2" s="62">
-        <v>7.3738425925925924E-4</v>
+        <v>7.4872685185185188E-4</v>
       </c>
       <c r="O2" s="62">
-        <v>9.592592592592592E-4</v>
+        <v>9.9224537037037033E-4</v>
       </c>
       <c r="P2" s="62">
-        <v>7.6875000000000001E-4</v>
+        <v>7.8888888888888889E-4</v>
       </c>
       <c r="Q2" s="62">
-        <v>1.9131944444444446E-3</v>
+        <v>1.9605324074074074E-3</v>
       </c>
       <c r="R2" s="62">
-        <v>1.763773148148148E-3</v>
+        <v>1.7837962962962963E-3</v>
       </c>
       <c r="S2" s="62">
-        <v>4.7893518518518521E-4</v>
+        <v>4.803240740740741E-4</v>
       </c>
       <c r="T2" s="62">
-        <v>7.6481481481481485E-4</v>
+        <v>7.8599537037037039E-4</v>
       </c>
       <c r="U2" s="62">
-        <v>1.0063657407407408E-3</v>
+        <v>1.0240740740740742E-3</v>
       </c>
       <c r="V2" s="62">
-        <v>8.1157407407407415E-4</v>
+        <v>8.2766203703703712E-4</v>
       </c>
       <c r="W2" s="62">
-        <v>1.9793981481481481E-3</v>
+        <v>2.0114583333333334E-3</v>
       </c>
       <c r="X2" s="62">
-        <v>1.8128472222222222E-3</v>
+        <v>1.8332175925925925E-3</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
@@ -12683,40 +12683,40 @@
         <v>10</v>
       </c>
       <c r="M3" s="62">
-        <v>3.8576388888888889E-4</v>
+        <v>3.9178240740740742E-4</v>
       </c>
       <c r="N3" s="62">
-        <v>6.064814814814815E-4</v>
+        <v>6.310185185185186E-4</v>
       </c>
       <c r="O3" s="62">
-        <v>8.3912037037037039E-4</v>
+        <v>8.5555555555555558E-4</v>
       </c>
       <c r="P3" s="62">
-        <v>6.8599537037037045E-4</v>
+        <v>7.0196759259259257E-4</v>
       </c>
       <c r="Q3" s="62">
-        <v>1.6768518518518519E-3</v>
+        <v>1.7359953703703704E-3</v>
       </c>
       <c r="R3" s="62">
-        <v>1.5944444444444443E-3</v>
+        <v>1.6295138888888889E-3</v>
       </c>
       <c r="S3" s="62">
-        <v>4.0127314814814816E-4</v>
+        <v>4.1747685185185187E-4</v>
       </c>
       <c r="T3" s="62">
-        <v>6.4421296296296297E-4</v>
+        <v>6.7627314814814818E-4</v>
       </c>
       <c r="U3" s="62">
-        <v>8.879629629629629E-4</v>
+        <v>8.9861111111111109E-4</v>
       </c>
       <c r="V3" s="62">
-        <v>7.0787037037037032E-4</v>
+        <v>7.2384259259259255E-4</v>
       </c>
       <c r="W3" s="62">
-        <v>1.784722222222222E-3</v>
+        <v>1.8050925925925927E-3</v>
       </c>
       <c r="X3" s="62">
-        <v>1.6582175925925926E-3</v>
+        <v>1.7003472222222222E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test Tabel NK% Times in JRP
</commit_message>
<xml_diff>
--- a/web/utilities/records_kriterien.xlsx
+++ b/web/utilities/records_kriterien.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgna\Documents\GitHub\Lifesaving_Baden\web\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74FA907B-837B-42C5-8F87-0B753394FB31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81B72674-C26E-4281-9CBF-AF67E38698EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="6" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
   </bookViews>
   <sheets>
     <sheet name="DR" sheetId="9" r:id="rId1"/>
@@ -20,9 +20,10 @@
     <sheet name="BP" sheetId="11" r:id="rId5"/>
     <sheet name="DEM" sheetId="12" r:id="rId6"/>
     <sheet name="JRP" sheetId="13" r:id="rId7"/>
-    <sheet name="2024" sheetId="6" r:id="rId8"/>
-    <sheet name="2025" sheetId="5" r:id="rId9"/>
-    <sheet name="2026" sheetId="8" r:id="rId10"/>
+    <sheet name="Tabelle1" sheetId="14" r:id="rId8"/>
+    <sheet name="2024" sheetId="6" r:id="rId9"/>
+    <sheet name="2025" sheetId="5" r:id="rId10"/>
+    <sheet name="2026" sheetId="8" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -219,7 +220,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="236">
   <si>
     <t>50m Retten</t>
   </si>
@@ -891,6 +892,42 @@
   </si>
   <si>
     <t>30.10.Jahr</t>
+  </si>
+  <si>
+    <t>Disziplin</t>
+  </si>
+  <si>
+    <t>100m Kombinierte Rettungsübung</t>
+  </si>
+  <si>
+    <t>100m Retten mit Flossen</t>
+  </si>
+  <si>
+    <t>100m Retten mit Flossen und Gurtretter</t>
+  </si>
+  <si>
+    <t>200m Hindernisschwimmen</t>
+  </si>
+  <si>
+    <t>NK2 Orginal M</t>
+  </si>
+  <si>
+    <t>NK2 +10% M</t>
+  </si>
+  <si>
+    <t>NK2-M (10%Test)</t>
+  </si>
+  <si>
+    <t>200m Super Lifesaver</t>
+  </si>
+  <si>
+    <t>NK2 Orginal W</t>
+  </si>
+  <si>
+    <t>NK2 +10% W</t>
+  </si>
+  <si>
+    <t>NK2-W (10%Test)</t>
   </si>
 </sst>
 </file>
@@ -900,7 +937,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m:ss.00"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1006,6 +1043,14 @@
       <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -1157,7 +1202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1344,6 +1389,16 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -4001,8 +4056,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}" name="JRP_konfig" displayName="JRP_konfig" ref="A1:X3" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
-  <autoFilter ref="A1:X3" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}" name="JRP_konfig" displayName="JRP_konfig" ref="A1:X9" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+  <autoFilter ref="A1:X9" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -4382,9 +4437,9 @@
       <selection activeCell="Y25" sqref="Y25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.265625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="42" t="s">
         <v>39</v>
       </c>
@@ -4453,7 +4508,7 @@
       <c r="AV1" s="44"/>
       <c r="AW1" s="44"/>
     </row>
-    <row r="2" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="42" t="s">
         <v>40</v>
       </c>
@@ -4520,7 +4575,7 @@
       <c r="AV2" s="45"/>
       <c r="AW2" s="45"/>
     </row>
-    <row r="3" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="42" t="s">
         <v>101</v>
       </c>
@@ -4581,7 +4636,7 @@
       <c r="AV3" s="45"/>
       <c r="AW3" s="45"/>
     </row>
-    <row r="4" spans="1:49" s="53" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:49" s="53" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="49" t="s">
         <v>10</v>
       </c>
@@ -4730,7 +4785,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>2000</v>
       </c>
@@ -4783,7 +4838,7 @@
       <c r="AV5" s="10"/>
       <c r="AW5" s="10"/>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <f t="shared" ref="A6:A31" si="0">A5+1</f>
         <v>2001</v>
@@ -4861,7 +4916,7 @@
       <c r="AV6" s="11"/>
       <c r="AW6" s="11"/>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>2002</v>
@@ -4939,7 +4994,7 @@
       <c r="AV7" s="10"/>
       <c r="AW7" s="10"/>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>2003</v>
@@ -5017,7 +5072,7 @@
       <c r="AV8" s="11"/>
       <c r="AW8" s="11"/>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>2004</v>
@@ -5095,7 +5150,7 @@
       <c r="AV9" s="10"/>
       <c r="AW9" s="10"/>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>2005</v>
@@ -5173,7 +5228,7 @@
       <c r="AV10" s="11"/>
       <c r="AW10" s="11"/>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>2006</v>
@@ -5251,7 +5306,7 @@
       <c r="AV11" s="10"/>
       <c r="AW11" s="10"/>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>2007</v>
@@ -5373,7 +5428,7 @@
         <v>3.5995370370370369E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>2008</v>
@@ -5495,7 +5550,7 @@
         <v>3.5995370370370369E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>2009</v>
@@ -5617,7 +5672,7 @@
         <v>3.5995370370370369E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>2010</v>
@@ -5739,7 +5794,7 @@
         <v>3.5995370370370369E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>2011</v>
@@ -5873,7 +5928,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>2012</v>
@@ -6007,7 +6062,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>2013</v>
@@ -6141,7 +6196,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>2014</v>
@@ -6275,7 +6330,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>2015</v>
@@ -6409,7 +6464,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>2016</v>
@@ -6543,7 +6598,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>2017</v>
@@ -6677,7 +6732,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>2018</v>
@@ -6811,7 +6866,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>2019</v>
@@ -6945,7 +7000,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>2020</v>
@@ -7095,7 +7150,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>2021</v>
@@ -7245,7 +7300,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>2022</v>
@@ -7395,7 +7450,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>2023</v>
@@ -7545,7 +7600,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>2024</v>
@@ -7695,7 +7750,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>2025</v>
@@ -7845,7 +7900,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>2026</v>
@@ -8056,27 +8111,27 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{453761C1-FFCA-45E5-8C71-AB7C914C935B}">
-  <sheetPr codeName="Tabelle5">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7831D901-68D8-4F92-82B6-BCB1A3899285}">
+  <sheetPr codeName="Tabelle4">
     <tabColor theme="4"/>
   </sheetPr>
   <dimension ref="A1:N39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
-    <col min="2" max="13" width="18.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.86328125" style="1" customWidth="1"/>
+    <col min="2" max="13" width="18.73046875" style="1" customWidth="1"/>
     <col min="14" max="14" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="11.42578125" style="1"/>
+    <col min="15" max="16384" width="11.3984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="18">
-        <v>2026</v>
+        <v>2025</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -8118,7 +8173,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
@@ -8132,11 +8187,11 @@
       </c>
       <c r="D2" s="14">
         <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(D$1))*86400,2)</f>
-        <v>91.79</v>
+        <v>93.26</v>
       </c>
       <c r="E2" s="14">
         <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(E$1))*86400,2)</f>
-        <v>75.84</v>
+        <v>75.900000000000006</v>
       </c>
       <c r="F2" s="14">
         <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(F$1))*86400,2)</f>
@@ -8148,11 +8203,11 @@
       </c>
       <c r="H2" s="14">
         <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(H$1))*86400,2)</f>
-        <v>38.36</v>
+        <v>38.799999999999997</v>
       </c>
       <c r="I2" s="14">
         <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(I$1))*86400,2)</f>
-        <v>60.47</v>
+        <v>61.05</v>
       </c>
       <c r="J2" s="14">
         <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(J$1))*86400,2)</f>
@@ -8174,7 +8229,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -8188,11 +8243,11 @@
       </c>
       <c r="D3" s="16">
         <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(D$1))*86400,2)</f>
-        <v>89.13</v>
+        <v>90.56</v>
       </c>
       <c r="E3" s="16">
         <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(E$1))*86400,2)</f>
-        <v>73.63</v>
+        <v>73.7</v>
       </c>
       <c r="F3" s="16">
         <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(F$1))*86400,2)</f>
@@ -8204,11 +8259,11 @@
       </c>
       <c r="H3" s="16">
         <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(H$1))*86400,2)</f>
-        <v>37.25</v>
+        <v>37.68</v>
       </c>
       <c r="I3" s="16">
         <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(I$1))*86400,2)</f>
-        <v>58.71</v>
+        <v>59.28</v>
       </c>
       <c r="J3" s="16">
         <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(J$1))*86400,2)</f>
@@ -8230,13 +8285,13 @@
         <v>730</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="19" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="14">
         <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(B$1))*86400,2)</f>
-        <v>41.13</v>
+        <v>41.76</v>
       </c>
       <c r="C4" s="14">
         <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(C$1))*86400,2)</f>
@@ -8244,11 +8299,11 @@
       </c>
       <c r="D4" s="14">
         <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(D$1))*86400,2)</f>
-        <v>83.98</v>
+        <v>84.9</v>
       </c>
       <c r="E4" s="14">
         <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(E$1))*86400,2)</f>
-        <v>70.290000000000006</v>
+        <v>70.760000000000005</v>
       </c>
       <c r="F4" s="14">
         <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(F$1))*86400,2)</f>
@@ -8260,11 +8315,11 @@
       </c>
       <c r="H4" s="14">
         <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(H$1))*86400,2)</f>
-        <v>34.74</v>
+        <v>34.83</v>
       </c>
       <c r="I4" s="14">
         <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(I$1))*86400,2)</f>
-        <v>56.16</v>
+        <v>56.25</v>
       </c>
       <c r="J4" s="14">
         <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(J$1))*86400,2)</f>
@@ -8272,7 +8327,7 @@
       </c>
       <c r="K4" s="14">
         <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(K$1))*86400,2)</f>
-        <v>60.9</v>
+        <v>62.47</v>
       </c>
       <c r="L4" s="14">
         <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(L$1))*86400,2)</f>
@@ -8280,13 +8335,13 @@
       </c>
       <c r="M4" s="15">
         <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(M$1))*86400,2)</f>
-        <v>142.72</v>
+        <v>144.54</v>
       </c>
       <c r="N4" s="2">
         <v>740</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" s="64" t="s">
         <v>13</v>
       </c>
@@ -8304,7 +8359,7 @@
       <c r="M7" s="64"/>
       <c r="N7" s="64"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" s="64"/>
       <c r="B8" s="64"/>
       <c r="C8" s="64"/>
@@ -8320,12 +8375,12 @@
       <c r="M8" s="64"/>
       <c r="N8" s="64"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" s="20" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="31" t="str">
-        <f t="shared" ref="B9:M11" si="0">CONCATENATE(ROUNDDOWN(B2/60,0),":",TEXT(B2-(60*ROUNDDOWN(B2/60,0)),"00,00"))</f>
+        <f t="shared" ref="B9" si="0">CONCATENATE(ROUNDDOWN(B2/60,0),":",TEXT(B2-(60*ROUNDDOWN(B2/60,0)),"00,00"))</f>
         <v>0:44,41</v>
       </c>
       <c r="C9" s="31" t="str">
@@ -8334,11 +8389,11 @@
       </c>
       <c r="D9" s="31" t="str">
         <f t="shared" ref="D9:M9" si="1">CONCATENATE(ROUNDDOWN(D2/60,0),":",TEXT(D2-(60*ROUNDDOWN(D2/60,0)),"00,00"))</f>
-        <v>1:31,79</v>
+        <v>1:33,26</v>
       </c>
       <c r="E9" s="31" t="str">
         <f t="shared" si="1"/>
-        <v>1:15,84</v>
+        <v>1:15,90</v>
       </c>
       <c r="F9" s="31" t="str">
         <f t="shared" si="1"/>
@@ -8350,11 +8405,11 @@
       </c>
       <c r="H9" s="31" t="str">
         <f t="shared" si="1"/>
-        <v>0:38,36</v>
+        <v>0:38,80</v>
       </c>
       <c r="I9" s="31" t="str">
         <f t="shared" si="1"/>
-        <v>1:00,47</v>
+        <v>1:01,05</v>
       </c>
       <c r="J9" s="31" t="str">
         <f t="shared" si="1"/>
@@ -8374,115 +8429,115 @@
       </c>
       <c r="N9" s="21"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" s="20" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B10:M10" si="2">CONCATENATE(ROUNDDOWN(B3/60,0),":",TEXT(B3-(60*ROUNDDOWN(B3/60,0)),"00,00"))</f>
         <v>0:43,12</v>
       </c>
       <c r="C10" s="24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1:03,63</v>
       </c>
       <c r="D10" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1:29,13</v>
+        <f t="shared" si="2"/>
+        <v>1:30,56</v>
       </c>
       <c r="E10" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>1:13,63</v>
+        <f t="shared" si="2"/>
+        <v>1:13,70</v>
       </c>
       <c r="F10" s="24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>3:03,57</v>
       </c>
       <c r="G10" s="29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2:39,79</v>
       </c>
       <c r="H10" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>0:37,25</v>
+        <f t="shared" si="2"/>
+        <v>0:37,68</v>
       </c>
       <c r="I10" s="24" t="str">
-        <f t="shared" si="0"/>
-        <v>0:58,71</v>
+        <f t="shared" si="2"/>
+        <v>0:59,28</v>
       </c>
       <c r="J10" s="24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1:16,92</v>
       </c>
       <c r="K10" s="24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>1:04,50</v>
       </c>
       <c r="L10" s="24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2:43,90</v>
       </c>
       <c r="M10" s="24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>2:30,57</v>
       </c>
       <c r="N10" s="21"/>
     </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="22" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>0:41,13</v>
+        <f t="shared" ref="B11:M11" si="3">CONCATENATE(ROUNDDOWN(B4/60,0),":",TEXT(B4-(60*ROUNDDOWN(B4/60,0)),"00,00"))</f>
+        <v>0:41,76</v>
       </c>
       <c r="C11" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1:02,97</v>
       </c>
       <c r="D11" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>1:23,98</v>
+        <f t="shared" si="3"/>
+        <v>1:24,90</v>
       </c>
       <c r="E11" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>1:10,29</v>
+        <f t="shared" si="3"/>
+        <v>1:10,76</v>
       </c>
       <c r="F11" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2:53,81</v>
       </c>
       <c r="G11" s="30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2:35,68</v>
       </c>
       <c r="H11" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>0:34,74</v>
+        <f t="shared" si="3"/>
+        <v>0:34,83</v>
       </c>
       <c r="I11" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>0:56,16</v>
+        <f t="shared" si="3"/>
+        <v>0:56,25</v>
       </c>
       <c r="J11" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1:13,65</v>
       </c>
       <c r="K11" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>1:00,90</v>
+        <f t="shared" si="3"/>
+        <v>1:02,47</v>
       </c>
       <c r="L11" s="25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2:37,09</v>
       </c>
       <c r="M11" s="25" t="str">
-        <f t="shared" si="0"/>
-        <v>2:22,72</v>
+        <f t="shared" si="3"/>
+        <v>2:24,54</v>
       </c>
       <c r="N11" s="23"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A14" s="63" t="s">
         <v>14</v>
       </c>
@@ -8501,7 +8556,7 @@
       </c>
       <c r="M14"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A15" s="63"/>
       <c r="B15" s="63"/>
       <c r="C15" s="63"/>
@@ -8514,7 +8569,7 @@
       <c r="L15" s="65"/>
       <c r="M15"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -8547,7 +8602,7 @@
       </c>
       <c r="M16"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="8" t="s">
         <v>28</v>
       </c>
@@ -8576,11 +8631,11 @@
         <v>27</v>
       </c>
       <c r="L17" s="35" t="s">
-        <v>33</v>
+        <v>88</v>
       </c>
       <c r="M17"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>28</v>
       </c>
@@ -8611,7 +8666,7 @@
       <c r="L18" s="38"/>
       <c r="M18"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="8" t="s">
         <v>29</v>
       </c>
@@ -8642,7 +8697,7 @@
       <c r="L19" s="36"/>
       <c r="M19"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="9" t="s">
         <v>30</v>
       </c>
@@ -8671,7 +8726,7 @@
       <c r="L20" s="38"/>
       <c r="M20"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="8" t="s">
         <v>29</v>
       </c>
@@ -8702,7 +8757,7 @@
       <c r="L21" s="36"/>
       <c r="M21"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
         <v>28</v>
       </c>
@@ -8733,7 +8788,7 @@
       <c r="L22" s="39"/>
       <c r="M22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" s="8" t="s">
         <v>28</v>
       </c>
@@ -8753,7 +8808,7 @@
         <v>27</v>
       </c>
       <c r="H23" s="41" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I23" s="41" t="s">
         <v>38</v>
@@ -8764,66 +8819,66 @@
       <c r="L23" s="37"/>
       <c r="M23"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="H24" s="40"/>
       <c r="I24" s="40"/>
       <c r="J24" s="40"/>
       <c r="L24" s="39"/>
       <c r="M24"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="H25" s="33"/>
       <c r="I25" s="33"/>
       <c r="L25" s="37"/>
       <c r="M25"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L26" s="39"/>
       <c r="M26"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L27" s="37"/>
       <c r="M27"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L28" s="39"/>
       <c r="M28"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L29" s="37"/>
       <c r="M29"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L30" s="39"/>
       <c r="M30"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L31" s="37"/>
       <c r="M31"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L32" s="39"/>
       <c r="M32"/>
     </row>
-    <row r="33" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="8:13" x14ac:dyDescent="0.45">
       <c r="L33" s="37"/>
       <c r="M33"/>
     </row>
-    <row r="34" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="8:13" x14ac:dyDescent="0.45">
       <c r="L34" s="39"/>
       <c r="M34"/>
     </row>
-    <row r="35" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:13" x14ac:dyDescent="0.45">
       <c r="M35"/>
     </row>
-    <row r="36" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="8:13" x14ac:dyDescent="0.45">
       <c r="L36" s="39"/>
       <c r="M36"/>
     </row>
-    <row r="37" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="8:13" x14ac:dyDescent="0.45">
       <c r="M37"/>
     </row>
-    <row r="38" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="8:13" x14ac:dyDescent="0.45">
       <c r="H38"/>
       <c r="I38"/>
       <c r="J38"/>
@@ -8831,7 +8886,803 @@
       <c r="L38"/>
       <c r="M38"/>
     </row>
-    <row r="39" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="8:13" x14ac:dyDescent="0.45">
+      <c r="H39"/>
+      <c r="I39"/>
+      <c r="J39"/>
+      <c r="K39"/>
+      <c r="L39"/>
+      <c r="M39"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A7:N8"/>
+    <mergeCell ref="A14:F15"/>
+    <mergeCell ref="H14:J15"/>
+    <mergeCell ref="L14:L15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{453761C1-FFCA-45E5-8C71-AB7C914C935B}">
+  <sheetPr codeName="Tabelle5">
+    <tabColor theme="4"/>
+  </sheetPr>
+  <dimension ref="A1:N39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="16.86328125" style="1" customWidth="1"/>
+    <col min="2" max="13" width="18.73046875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="25" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="11.3984375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="18">
+        <v>2026</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(B$1))*86400,2)</f>
+        <v>44.41</v>
+      </c>
+      <c r="C2" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(C$1))*86400,2)</f>
+        <v>65.53</v>
+      </c>
+      <c r="D2" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(D$1))*86400,2)</f>
+        <v>91.79</v>
+      </c>
+      <c r="E2" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(E$1))*86400,2)</f>
+        <v>75.84</v>
+      </c>
+      <c r="F2" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(F$1))*86400,2)</f>
+        <v>189.05</v>
+      </c>
+      <c r="G2" s="27">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(G$1))*86400,2)</f>
+        <v>164.57</v>
+      </c>
+      <c r="H2" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(H$1))*86400,2)</f>
+        <v>38.36</v>
+      </c>
+      <c r="I2" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(I$1))*86400,2)</f>
+        <v>60.47</v>
+      </c>
+      <c r="J2" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(J$1))*86400,2)</f>
+        <v>79.22</v>
+      </c>
+      <c r="K2" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(K$1))*86400,2)</f>
+        <v>66.430000000000007</v>
+      </c>
+      <c r="L2" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(L$1))*86400,2)</f>
+        <v>168.79</v>
+      </c>
+      <c r="M2" s="15">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(M$1))*86400,2)</f>
+        <v>155.07</v>
+      </c>
+      <c r="N2" s="2">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="16">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(B$1))*86400,2)</f>
+        <v>43.12</v>
+      </c>
+      <c r="C3" s="16">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(C$1))*86400,2)</f>
+        <v>63.63</v>
+      </c>
+      <c r="D3" s="16">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(D$1))*86400,2)</f>
+        <v>89.13</v>
+      </c>
+      <c r="E3" s="16">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(E$1))*86400,2)</f>
+        <v>73.63</v>
+      </c>
+      <c r="F3" s="16">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(F$1))*86400,2)</f>
+        <v>183.57</v>
+      </c>
+      <c r="G3" s="28">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(G$1))*86400,2)</f>
+        <v>159.79</v>
+      </c>
+      <c r="H3" s="16">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(H$1))*86400,2)</f>
+        <v>37.25</v>
+      </c>
+      <c r="I3" s="16">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(I$1))*86400,2)</f>
+        <v>58.71</v>
+      </c>
+      <c r="J3" s="16">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(J$1))*86400,2)</f>
+        <v>76.92</v>
+      </c>
+      <c r="K3" s="16">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(K$1))*86400,2)</f>
+        <v>64.5</v>
+      </c>
+      <c r="L3" s="16">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(L$1))*86400,2)</f>
+        <v>163.9</v>
+      </c>
+      <c r="M3" s="17">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(M$1))*86400,2)</f>
+        <v>150.57</v>
+      </c>
+      <c r="N3" s="2">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(B$1))*86400,2)</f>
+        <v>41.13</v>
+      </c>
+      <c r="C4" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(C$1))*86400,2)</f>
+        <v>62.97</v>
+      </c>
+      <c r="D4" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(D$1))*86400,2)</f>
+        <v>83.98</v>
+      </c>
+      <c r="E4" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(E$1))*86400,2)</f>
+        <v>70.290000000000006</v>
+      </c>
+      <c r="F4" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(F$1))*86400,2)</f>
+        <v>173.81</v>
+      </c>
+      <c r="G4" s="27">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(G$1))*86400,2)</f>
+        <v>155.68</v>
+      </c>
+      <c r="H4" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(H$1))*86400,2)</f>
+        <v>34.74</v>
+      </c>
+      <c r="I4" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(I$1))*86400,2)</f>
+        <v>56.16</v>
+      </c>
+      <c r="J4" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(J$1))*86400,2)</f>
+        <v>73.650000000000006</v>
+      </c>
+      <c r="K4" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(K$1))*86400,2)</f>
+        <v>60.9</v>
+      </c>
+      <c r="L4" s="14">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(L$1))*86400,2)</f>
+        <v>157.09</v>
+      </c>
+      <c r="M4" s="15">
+        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(M$1))*86400,2)</f>
+        <v>142.72</v>
+      </c>
+      <c r="N4" s="2">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A7" s="64" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="64"/>
+      <c r="C7" s="64"/>
+      <c r="D7" s="64"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="64"/>
+      <c r="G7" s="64"/>
+      <c r="H7" s="64"/>
+      <c r="I7" s="64"/>
+      <c r="J7" s="64"/>
+      <c r="K7" s="64"/>
+      <c r="L7" s="64"/>
+      <c r="M7" s="64"/>
+      <c r="N7" s="64"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A8" s="64"/>
+      <c r="B8" s="64"/>
+      <c r="C8" s="64"/>
+      <c r="D8" s="64"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="64"/>
+      <c r="J8" s="64"/>
+      <c r="K8" s="64"/>
+      <c r="L8" s="64"/>
+      <c r="M8" s="64"/>
+      <c r="N8" s="64"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A9" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="31" t="str">
+        <f t="shared" ref="B9:M11" si="0">CONCATENATE(ROUNDDOWN(B2/60,0),":",TEXT(B2-(60*ROUNDDOWN(B2/60,0)),"00,00"))</f>
+        <v>0:44,41</v>
+      </c>
+      <c r="C9" s="31" t="str">
+        <f>CONCATENATE(ROUNDDOWN(C2/60,0),":",TEXT(C2-(60*ROUNDDOWN(C2/60,0)),"00,00"))</f>
+        <v>1:05,53</v>
+      </c>
+      <c r="D9" s="31" t="str">
+        <f t="shared" ref="D9:M9" si="1">CONCATENATE(ROUNDDOWN(D2/60,0),":",TEXT(D2-(60*ROUNDDOWN(D2/60,0)),"00,00"))</f>
+        <v>1:31,79</v>
+      </c>
+      <c r="E9" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v>1:15,84</v>
+      </c>
+      <c r="F9" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v>3:09,05</v>
+      </c>
+      <c r="G9" s="32" t="str">
+        <f t="shared" si="1"/>
+        <v>2:44,57</v>
+      </c>
+      <c r="H9" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v>0:38,36</v>
+      </c>
+      <c r="I9" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v>1:00,47</v>
+      </c>
+      <c r="J9" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v>1:19,22</v>
+      </c>
+      <c r="K9" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v>1:06,43</v>
+      </c>
+      <c r="L9" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v>2:48,79</v>
+      </c>
+      <c r="M9" s="31" t="str">
+        <f t="shared" si="1"/>
+        <v>2:35,07</v>
+      </c>
+      <c r="N9" s="21"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A10" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>0:43,12</v>
+      </c>
+      <c r="C10" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>1:03,63</v>
+      </c>
+      <c r="D10" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>1:29,13</v>
+      </c>
+      <c r="E10" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>1:13,63</v>
+      </c>
+      <c r="F10" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>3:03,57</v>
+      </c>
+      <c r="G10" s="29" t="str">
+        <f t="shared" si="0"/>
+        <v>2:39,79</v>
+      </c>
+      <c r="H10" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>0:37,25</v>
+      </c>
+      <c r="I10" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>0:58,71</v>
+      </c>
+      <c r="J10" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>1:16,92</v>
+      </c>
+      <c r="K10" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>1:04,50</v>
+      </c>
+      <c r="L10" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>2:43,90</v>
+      </c>
+      <c r="M10" s="24" t="str">
+        <f t="shared" si="0"/>
+        <v>2:30,57</v>
+      </c>
+      <c r="N10" s="21"/>
+    </row>
+    <row r="11" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>0:41,13</v>
+      </c>
+      <c r="C11" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>1:02,97</v>
+      </c>
+      <c r="D11" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>1:23,98</v>
+      </c>
+      <c r="E11" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>1:10,29</v>
+      </c>
+      <c r="F11" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>2:53,81</v>
+      </c>
+      <c r="G11" s="30" t="str">
+        <f t="shared" si="0"/>
+        <v>2:35,68</v>
+      </c>
+      <c r="H11" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>0:34,74</v>
+      </c>
+      <c r="I11" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>0:56,16</v>
+      </c>
+      <c r="J11" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>1:13,65</v>
+      </c>
+      <c r="K11" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>1:00,90</v>
+      </c>
+      <c r="L11" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>2:37,09</v>
+      </c>
+      <c r="M11" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v>2:22,72</v>
+      </c>
+      <c r="N11" s="23"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A14" s="63" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="63"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
+      <c r="H14" s="65" t="s">
+        <v>35</v>
+      </c>
+      <c r="I14" s="65"/>
+      <c r="J14" s="65"/>
+      <c r="L14" s="65" t="s">
+        <v>36</v>
+      </c>
+      <c r="M14"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A15" s="63"/>
+      <c r="B15" s="63"/>
+      <c r="C15" s="63"/>
+      <c r="D15" s="63"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="63"/>
+      <c r="H15" s="65"/>
+      <c r="I15" s="65"/>
+      <c r="J15" s="65"/>
+      <c r="L15" s="65"/>
+      <c r="M15"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+      <c r="A16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M16"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A17" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="8">
+        <v>15</v>
+      </c>
+      <c r="C17" s="8">
+        <v>18</v>
+      </c>
+      <c r="D17" s="8">
+        <v>3</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H17" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L17" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="M17"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A18" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="9">
+        <v>13</v>
+      </c>
+      <c r="C18" s="9">
+        <v>14</v>
+      </c>
+      <c r="D18" s="9">
+        <v>1</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H18" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="I18" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="J18" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="L18" s="38"/>
+      <c r="M18"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A19" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" s="8">
+        <v>12</v>
+      </c>
+      <c r="C19" s="8">
+        <v>18</v>
+      </c>
+      <c r="D19" s="8">
+        <v>16</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="I19" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="J19" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="L19" s="36"/>
+      <c r="M19"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A20" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="9">
+        <v>12</v>
+      </c>
+      <c r="C20" s="9">
+        <v>18</v>
+      </c>
+      <c r="D20" s="9">
+        <v>10</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="H20" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="I20" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="J20" s="35"/>
+      <c r="L20" s="38"/>
+      <c r="M20"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A21" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" s="8">
+        <v>12</v>
+      </c>
+      <c r="C21" s="8">
+        <v>100</v>
+      </c>
+      <c r="D21" s="8">
+        <v>8</v>
+      </c>
+      <c r="E21" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H21" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="I21" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="J21" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="L21" s="36"/>
+      <c r="M21"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A22" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="9">
+        <v>17</v>
+      </c>
+      <c r="C22" s="9">
+        <v>18</v>
+      </c>
+      <c r="D22" s="9">
+        <v>1</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H22" s="40" t="s">
+        <v>93</v>
+      </c>
+      <c r="I22" s="40" t="s">
+        <v>31</v>
+      </c>
+      <c r="J22" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="L22" s="39"/>
+      <c r="M22"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="A23" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="8">
+        <v>19</v>
+      </c>
+      <c r="C23" s="8">
+        <v>100</v>
+      </c>
+      <c r="D23" s="8">
+        <v>4</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H23" s="41" t="s">
+        <v>95</v>
+      </c>
+      <c r="I23" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="J23" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="L23" s="37"/>
+      <c r="M23"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
+      <c r="L24" s="39"/>
+      <c r="M24"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="H25" s="33"/>
+      <c r="I25" s="33"/>
+      <c r="L25" s="37"/>
+      <c r="M25"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="L26" s="39"/>
+      <c r="M26"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="L27" s="37"/>
+      <c r="M27"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="L28" s="39"/>
+      <c r="M28"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="L29" s="37"/>
+      <c r="M29"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="L30" s="39"/>
+      <c r="M30"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="L31" s="37"/>
+      <c r="M31"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+      <c r="L32" s="39"/>
+      <c r="M32"/>
+    </row>
+    <row r="33" spans="8:13" x14ac:dyDescent="0.45">
+      <c r="L33" s="37"/>
+      <c r="M33"/>
+    </row>
+    <row r="34" spans="8:13" x14ac:dyDescent="0.45">
+      <c r="L34" s="39"/>
+      <c r="M34"/>
+    </row>
+    <row r="35" spans="8:13" x14ac:dyDescent="0.45">
+      <c r="M35"/>
+    </row>
+    <row r="36" spans="8:13" x14ac:dyDescent="0.45">
+      <c r="L36" s="39"/>
+      <c r="M36"/>
+    </row>
+    <row r="37" spans="8:13" x14ac:dyDescent="0.45">
+      <c r="M37"/>
+    </row>
+    <row r="38" spans="8:13" x14ac:dyDescent="0.45">
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="J38"/>
+      <c r="K38"/>
+      <c r="L38"/>
+      <c r="M38"/>
+    </row>
+    <row r="39" spans="8:13" x14ac:dyDescent="0.45">
       <c r="H39"/>
       <c r="I39"/>
       <c r="J39"/>
@@ -8860,17 +9711,17 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" customWidth="1"/>
-    <col min="7" max="11" width="18.7109375" customWidth="1"/>
-    <col min="12" max="12" width="22.140625" customWidth="1"/>
-    <col min="13" max="13" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.265625" customWidth="1"/>
+    <col min="2" max="5" width="18.73046875" customWidth="1"/>
+    <col min="6" max="6" width="21.1328125" customWidth="1"/>
+    <col min="7" max="11" width="18.73046875" customWidth="1"/>
+    <col min="12" max="12" width="22.1328125" customWidth="1"/>
+    <col min="13" max="13" width="18.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="42" t="s">
         <v>39</v>
       </c>
@@ -8911,7 +9762,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="42" t="s">
         <v>40</v>
       </c>
@@ -8952,7 +9803,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="42" t="s">
         <v>41</v>
       </c>
@@ -8993,7 +9844,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -9034,7 +9885,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>2000</v>
       </c>
@@ -9051,7 +9902,7 @@
       <c r="L5" s="11"/>
       <c r="M5" s="11"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <f t="shared" ref="A6:A32" si="0">A5+1</f>
         <v>2001</v>
@@ -9069,7 +9920,7 @@
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>2002</v>
@@ -9087,7 +9938,7 @@
       <c r="L7" s="11"/>
       <c r="M7" s="11"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>2003</v>
@@ -9105,7 +9956,7 @@
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>2004</v>
@@ -9123,7 +9974,7 @@
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>2005</v>
@@ -9141,7 +9992,7 @@
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>2006</v>
@@ -9159,7 +10010,7 @@
       <c r="L11" s="11"/>
       <c r="M11" s="11"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>2007</v>
@@ -9177,7 +10028,7 @@
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>2008</v>
@@ -9195,7 +10046,7 @@
       <c r="L13" s="11"/>
       <c r="M13" s="11"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>2009</v>
@@ -9213,7 +10064,7 @@
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>2010</v>
@@ -9231,7 +10082,7 @@
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>2011</v>
@@ -9249,7 +10100,7 @@
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>2012</v>
@@ -9267,7 +10118,7 @@
       <c r="L17" s="11"/>
       <c r="M17" s="11"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>2013</v>
@@ -9285,7 +10136,7 @@
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>2014</v>
@@ -9303,7 +10154,7 @@
       <c r="L19" s="11"/>
       <c r="M19" s="11"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>2015</v>
@@ -9345,7 +10196,7 @@
         <v>1.3592592592592591E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>2016</v>
@@ -9387,7 +10238,7 @@
         <v>1.3592592592592591E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>2017</v>
@@ -9429,7 +10280,7 @@
         <v>1.3577546296296298E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>2018</v>
@@ -9471,7 +10322,7 @@
         <v>1.3577546296296298E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>2019</v>
@@ -9513,7 +10364,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>2020</v>
@@ -9555,7 +10406,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>2021</v>
@@ -9597,7 +10448,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>2022</v>
@@ -9639,7 +10490,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>2023</v>
@@ -9681,7 +10532,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>2024</v>
@@ -9723,7 +10574,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>2025</v>
@@ -9765,7 +10616,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>2026</v>
@@ -9807,7 +10658,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A32" s="2">
         <f t="shared" si="0"/>
         <v>2027</v>
@@ -9887,17 +10738,17 @@
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" customWidth="1"/>
-    <col min="7" max="11" width="18.7109375" customWidth="1"/>
-    <col min="12" max="12" width="22.140625" customWidth="1"/>
-    <col min="13" max="13" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.86328125" customWidth="1"/>
+    <col min="2" max="5" width="18.73046875" customWidth="1"/>
+    <col min="6" max="6" width="21.1328125" customWidth="1"/>
+    <col min="7" max="11" width="18.73046875" customWidth="1"/>
+    <col min="12" max="12" width="22.1328125" customWidth="1"/>
+    <col min="13" max="13" width="18.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="42" t="s">
         <v>39</v>
       </c>
@@ -9938,7 +10789,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="42" t="s">
         <v>40</v>
       </c>
@@ -9979,7 +10830,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="42" t="s">
         <v>41</v>
       </c>
@@ -10020,7 +10871,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -10061,7 +10912,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>2000</v>
       </c>
@@ -10078,7 +10929,7 @@
       <c r="L5" s="38"/>
       <c r="M5" s="38"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <f t="shared" ref="A6:A31" si="0">A5+1</f>
         <v>2001</v>
@@ -10108,7 +10959,7 @@
         <v>1.3629629629629632E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>2002</v>
@@ -10150,7 +11001,7 @@
         <v>1.3629629629629632E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>2003</v>
@@ -10192,7 +11043,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>2004</v>
@@ -10234,7 +11085,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>2005</v>
@@ -10276,7 +11127,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>2006</v>
@@ -10318,7 +11169,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>2007</v>
@@ -10360,7 +11211,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>2008</v>
@@ -10402,7 +11253,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>2009</v>
@@ -10444,7 +11295,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>2010</v>
@@ -10486,7 +11337,7 @@
         <v>1.3306712962962966E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>2011</v>
@@ -10528,7 +11379,7 @@
         <v>1.3306712962962966E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>2012</v>
@@ -10570,7 +11421,7 @@
         <v>1.3306712962962966E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>2013</v>
@@ -10612,7 +11463,7 @@
         <v>1.312962962962963E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>2014</v>
@@ -10654,7 +11505,7 @@
         <v>1.312962962962963E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>2015</v>
@@ -10696,7 +11547,7 @@
         <v>1.3116898148148148E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>2016</v>
@@ -10738,7 +11589,7 @@
         <v>1.3116898148148148E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>2017</v>
@@ -10780,7 +11631,7 @@
         <v>1.3116898148148148E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>2018</v>
@@ -10822,7 +11673,7 @@
         <v>1.3116898148148148E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>2019</v>
@@ -10864,7 +11715,7 @@
         <v>1.3116898148148148E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>2020</v>
@@ -10906,7 +11757,7 @@
         <v>1.3097222222222223E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>2021</v>
@@ -10948,7 +11799,7 @@
         <v>1.3097222222222223E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>2022</v>
@@ -10990,7 +11841,7 @@
         <v>1.3097222222222223E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>2023</v>
@@ -11032,7 +11883,7 @@
         <v>1.3097222222222223E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>2024</v>
@@ -11074,7 +11925,7 @@
         <v>1.3097222222222223E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>2025</v>
@@ -11116,7 +11967,7 @@
         <v>1.2931712962962962E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>2026</v>
@@ -11158,7 +12009,7 @@
         <v>1.2931712962962962E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A32" s="2">
         <f>A31+1</f>
         <v>2027</v>
@@ -11240,30 +12091,30 @@
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.59765625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.73046875" customWidth="1"/>
     <col min="15" max="16" width="19" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="22.265625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.73046875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="47.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="60" t="s">
         <v>161</v>
       </c>
@@ -11328,7 +12179,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A2" s="59" t="s">
         <v>199</v>
       </c>
@@ -11389,7 +12240,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A3" s="59" t="s">
         <v>200</v>
       </c>
@@ -11469,30 +12320,30 @@
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.59765625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.73046875" customWidth="1"/>
     <col min="15" max="16" width="19" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="22.265625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.73046875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="47.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="60" t="s">
         <v>161</v>
       </c>
@@ -11557,7 +12408,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A2" s="59" t="s">
         <v>190</v>
       </c>
@@ -11618,7 +12469,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A3" s="59" t="s">
         <v>191</v>
       </c>
@@ -11679,7 +12530,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A4" s="59" t="s">
         <v>192</v>
       </c>
@@ -11740,7 +12591,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A5" s="59" t="s">
         <v>193</v>
       </c>
@@ -11799,7 +12650,7 @@
       </c>
       <c r="U5" s="59"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A6" s="59" t="s">
         <v>194</v>
       </c>
@@ -11858,7 +12709,7 @@
       </c>
       <c r="U6" s="59"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A7" s="59" t="s">
         <v>195</v>
       </c>
@@ -11936,35 +12787,35 @@
       <selection activeCell="L6" sqref="A1:X7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.86328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.3984375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.73046875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.86328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.1328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.86328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.86328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.1328125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="24.86328125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A1" s="59" t="s">
         <v>161</v>
       </c>
@@ -12038,7 +12889,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A2" s="59" t="s">
         <v>217</v>
       </c>
@@ -12108,7 +12959,7 @@
         <v>1.9623842592592592E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A3" s="59" t="s">
         <v>218</v>
       </c>
@@ -12178,7 +13029,7 @@
         <v>1.8121527777777778E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A4" s="59" t="s">
         <v>219</v>
       </c>
@@ -12248,7 +13099,7 @@
         <v>1.9979166666666665E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A5" s="59" t="s">
         <v>220</v>
       </c>
@@ -12318,7 +13169,7 @@
         <v>1.7653935185185186E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A6" s="59" t="s">
         <v>190</v>
       </c>
@@ -12388,7 +13239,7 @@
         <v>1.8998842592592594E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A7" s="59" t="s">
         <v>191</v>
       </c>
@@ -12471,41 +13322,41 @@
   <sheetPr codeName="Tabelle10">
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:X3"/>
+  <dimension ref="A1:X9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.86328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.86328125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.59765625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.59765625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.59765625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="27" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="22" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.59765625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.265625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.59765625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="27" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A1" s="59" t="s">
         <v>161</v>
       </c>
@@ -12579,7 +13430,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A2" s="59" t="s">
         <v>215</v>
       </c>
@@ -12649,7 +13500,7 @@
         <v>1.8332175925925925E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A3" s="59" t="s">
         <v>216</v>
       </c>
@@ -12718,6 +13569,390 @@
       <c r="X3" s="62">
         <v>1.7003472222222222E-3</v>
       </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A4" s="59" t="s">
+        <v>231</v>
+      </c>
+      <c r="B4" s="59" t="s">
+        <v>182</v>
+      </c>
+      <c r="C4" s="59">
+        <v>17</v>
+      </c>
+      <c r="D4" s="59">
+        <v>17</v>
+      </c>
+      <c r="E4" s="61">
+        <v>45658</v>
+      </c>
+      <c r="F4" s="61">
+        <v>46022</v>
+      </c>
+      <c r="G4" s="61">
+        <v>45658</v>
+      </c>
+      <c r="H4" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="I4" s="59" t="s">
+        <v>179</v>
+      </c>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59">
+        <v>10</v>
+      </c>
+      <c r="M4" s="62">
+        <f>Tabelle1!E14</f>
+        <v>4.0282407407407411E-4</v>
+      </c>
+      <c r="N4" s="62">
+        <f>Tabelle1!E16</f>
+        <v>6.3721064814814814E-4</v>
+      </c>
+      <c r="O4" s="62">
+        <f>Tabelle1!E15</f>
+        <v>8.6561342592592593E-4</v>
+      </c>
+      <c r="P4" s="62">
+        <f>Tabelle1!E17</f>
+        <v>7.2594907407407417E-4</v>
+      </c>
+      <c r="Q4" s="62">
+        <f>Tabelle1!E19</f>
+        <v>1.7947569444444445E-3</v>
+      </c>
+      <c r="R4" s="62">
+        <f>Tabelle1!E18</f>
+        <v>1.6421064814814814E-3</v>
+      </c>
+      <c r="S4" s="62"/>
+      <c r="T4" s="62"/>
+      <c r="U4" s="62"/>
+      <c r="V4" s="62"/>
+      <c r="W4" s="62"/>
+      <c r="X4" s="62"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A5" s="59" t="s">
+        <v>231</v>
+      </c>
+      <c r="B5" s="59" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" s="59">
+        <v>16</v>
+      </c>
+      <c r="D5" s="59">
+        <v>16</v>
+      </c>
+      <c r="E5" s="61">
+        <v>45658</v>
+      </c>
+      <c r="F5" s="61">
+        <v>46022</v>
+      </c>
+      <c r="G5" s="61">
+        <v>45658</v>
+      </c>
+      <c r="H5" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="I5" s="59" t="s">
+        <v>179</v>
+      </c>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59">
+        <v>10</v>
+      </c>
+      <c r="M5" s="62">
+        <f>Tabelle1!D14</f>
+        <v>4.072800925925926E-4</v>
+      </c>
+      <c r="N5" s="62">
+        <f>Tabelle1!D16</f>
+        <v>6.4344907407407417E-4</v>
+      </c>
+      <c r="O5" s="62">
+        <f>Tabelle1!D15</f>
+        <v>8.7821759259259276E-4</v>
+      </c>
+      <c r="P5" s="62">
+        <f>Tabelle1!D17</f>
+        <v>7.4160879629629642E-4</v>
+      </c>
+      <c r="Q5" s="62">
+        <f>Tabelle1!D19</f>
+        <v>1.8160185185185185E-3</v>
+      </c>
+      <c r="R5" s="62">
+        <f>Tabelle1!D18</f>
+        <v>1.6614583333333334E-3</v>
+      </c>
+      <c r="S5" s="62"/>
+      <c r="T5" s="62"/>
+      <c r="U5" s="62"/>
+      <c r="V5" s="62"/>
+      <c r="W5" s="62"/>
+      <c r="X5" s="62"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A6" s="59" t="s">
+        <v>231</v>
+      </c>
+      <c r="B6" s="59" t="s">
+        <v>182</v>
+      </c>
+      <c r="C6" s="59">
+        <v>12</v>
+      </c>
+      <c r="D6" s="59">
+        <v>15</v>
+      </c>
+      <c r="E6" s="61">
+        <v>45658</v>
+      </c>
+      <c r="F6" s="61">
+        <v>46022</v>
+      </c>
+      <c r="G6" s="61">
+        <v>45658</v>
+      </c>
+      <c r="H6" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="I6" s="59" t="s">
+        <v>179</v>
+      </c>
+      <c r="J6" s="59"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="59">
+        <v>10</v>
+      </c>
+      <c r="M6" s="62">
+        <f>Tabelle1!C14</f>
+        <v>4.1122685185185186E-4</v>
+      </c>
+      <c r="N6" s="62">
+        <f>Tabelle1!C16</f>
+        <v>6.4930555555555564E-4</v>
+      </c>
+      <c r="O6" s="62">
+        <f>Tabelle1!C15</f>
+        <v>8.899305555555557E-4</v>
+      </c>
+      <c r="P6" s="62">
+        <f>Tabelle1!C17</f>
+        <v>7.5599537037037052E-4</v>
+      </c>
+      <c r="Q6" s="62">
+        <f>Tabelle1!C19</f>
+        <v>1.835752314814815E-3</v>
+      </c>
+      <c r="R6" s="62">
+        <f>Tabelle1!C18</f>
+        <v>1.6792824074074075E-3</v>
+      </c>
+      <c r="S6" s="62"/>
+      <c r="T6" s="62"/>
+      <c r="U6" s="62"/>
+      <c r="V6" s="62"/>
+      <c r="W6" s="62"/>
+      <c r="X6" s="62"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A7" s="59" t="s">
+        <v>235</v>
+      </c>
+      <c r="B7" s="59" t="s">
+        <v>164</v>
+      </c>
+      <c r="C7" s="59">
+        <v>17</v>
+      </c>
+      <c r="D7" s="59">
+        <v>17</v>
+      </c>
+      <c r="E7" s="61">
+        <v>45658</v>
+      </c>
+      <c r="F7" s="61">
+        <v>46022</v>
+      </c>
+      <c r="G7" s="61">
+        <v>45658</v>
+      </c>
+      <c r="H7" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="I7" s="59" t="s">
+        <v>179</v>
+      </c>
+      <c r="J7" s="59"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="59">
+        <v>10</v>
+      </c>
+      <c r="M7" s="62">
+        <f>Tabelle1!K14</f>
+        <v>4.9831018518518529E-4</v>
+      </c>
+      <c r="N7" s="62">
+        <f>Tabelle1!K16</f>
+        <v>7.4988425925925928E-4</v>
+      </c>
+      <c r="O7" s="62">
+        <f>Tabelle1!K15</f>
+        <v>1.0141898148148148E-3</v>
+      </c>
+      <c r="P7" s="62">
+        <f>Tabelle1!K17</f>
+        <v>8.3289351851851851E-4</v>
+      </c>
+      <c r="Q7" s="62">
+        <f>Tabelle1!K19</f>
+        <v>1.9631944444444445E-3</v>
+      </c>
+      <c r="R7" s="62">
+        <f>Tabelle1!K18</f>
+        <v>1.7831712962962964E-3</v>
+      </c>
+      <c r="S7" s="62"/>
+      <c r="T7" s="62"/>
+      <c r="U7" s="62"/>
+      <c r="V7" s="62"/>
+      <c r="W7" s="62"/>
+      <c r="X7" s="62"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A8" s="59" t="s">
+        <v>235</v>
+      </c>
+      <c r="B8" s="59" t="s">
+        <v>164</v>
+      </c>
+      <c r="C8" s="59">
+        <v>16</v>
+      </c>
+      <c r="D8" s="59">
+        <v>16</v>
+      </c>
+      <c r="E8" s="61">
+        <v>45658</v>
+      </c>
+      <c r="F8" s="61">
+        <v>46022</v>
+      </c>
+      <c r="G8" s="61">
+        <v>45658</v>
+      </c>
+      <c r="H8" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="I8" s="59" t="s">
+        <v>179</v>
+      </c>
+      <c r="J8" s="59"/>
+      <c r="K8" s="59"/>
+      <c r="L8" s="59">
+        <v>10</v>
+      </c>
+      <c r="M8" s="62">
+        <f>Tabelle1!J14</f>
+        <v>5.0836805555555563E-4</v>
+      </c>
+      <c r="N8" s="62">
+        <f>Tabelle1!J16</f>
+        <v>7.5841435185185202E-4</v>
+      </c>
+      <c r="O8" s="62">
+        <f>Tabelle1!J15</f>
+        <v>1.0323958333333335E-3</v>
+      </c>
+      <c r="P8" s="62">
+        <f>Tabelle1!J17</f>
+        <v>8.4511574074074068E-4</v>
+      </c>
+      <c r="Q8" s="62">
+        <f>Tabelle1!J19</f>
+        <v>1.9777083333333335E-3</v>
+      </c>
+      <c r="R8" s="62">
+        <f>Tabelle1!J18</f>
+        <v>1.7899189814814817E-3</v>
+      </c>
+      <c r="S8" s="62"/>
+      <c r="T8" s="62"/>
+      <c r="U8" s="62"/>
+      <c r="V8" s="62"/>
+      <c r="W8" s="62"/>
+      <c r="X8" s="62"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A9" s="59" t="s">
+        <v>235</v>
+      </c>
+      <c r="B9" s="59" t="s">
+        <v>164</v>
+      </c>
+      <c r="C9" s="59">
+        <v>12</v>
+      </c>
+      <c r="D9" s="59">
+        <v>15</v>
+      </c>
+      <c r="E9" s="61">
+        <v>45658</v>
+      </c>
+      <c r="F9" s="61">
+        <v>46022</v>
+      </c>
+      <c r="G9" s="61">
+        <v>45658</v>
+      </c>
+      <c r="H9" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="I9" s="59" t="s">
+        <v>179</v>
+      </c>
+      <c r="J9" s="59"/>
+      <c r="K9" s="59"/>
+      <c r="L9" s="59">
+        <v>10</v>
+      </c>
+      <c r="M9" s="62">
+        <f>Tabelle1!I14</f>
+        <v>5.1791666666666663E-4</v>
+      </c>
+      <c r="N9" s="62">
+        <f>Tabelle1!I16</f>
+        <v>7.6630787037037043E-4</v>
+      </c>
+      <c r="O9" s="62">
+        <f>Tabelle1!I15</f>
+        <v>1.049201388888889E-3</v>
+      </c>
+      <c r="P9" s="62">
+        <f>Tabelle1!I17</f>
+        <v>8.563194444444446E-4</v>
+      </c>
+      <c r="Q9" s="62">
+        <f>Tabelle1!I19</f>
+        <v>1.9912037037037038E-3</v>
+      </c>
+      <c r="R9" s="62">
+        <f>Tabelle1!I18</f>
+        <v>1.7961574074074073E-3</v>
+      </c>
+      <c r="S9" s="62"/>
+      <c r="T9" s="62"/>
+      <c r="U9" s="62"/>
+      <c r="V9" s="62"/>
+      <c r="W9" s="62"/>
+      <c r="X9" s="62"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -12728,6 +13963,531 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A13DA696-49DD-4BFA-98FE-5C7770404E50}">
+  <dimension ref="B3:L37"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="34.6640625" customWidth="1"/>
+    <col min="8" max="8" width="39.53125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>229</v>
+      </c>
+      <c r="H3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B4" s="66" t="s">
+        <v>224</v>
+      </c>
+      <c r="C4" s="69">
+        <v>2010</v>
+      </c>
+      <c r="D4" s="69">
+        <v>2009</v>
+      </c>
+      <c r="E4" s="69">
+        <v>2008</v>
+      </c>
+      <c r="H4" s="66" t="s">
+        <v>224</v>
+      </c>
+      <c r="I4" s="69">
+        <v>2010</v>
+      </c>
+      <c r="J4" s="69">
+        <v>2009</v>
+      </c>
+      <c r="K4" s="69">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B5" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="68">
+        <v>3.7384259259259255E-4</v>
+      </c>
+      <c r="D5" s="68">
+        <v>3.7025462962962961E-4</v>
+      </c>
+      <c r="E5" s="68">
+        <v>3.6620370370370371E-4</v>
+      </c>
+      <c r="H5" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="I5" s="68">
+        <v>4.708333333333333E-4</v>
+      </c>
+      <c r="J5" s="68">
+        <v>4.621527777777778E-4</v>
+      </c>
+      <c r="K5" s="68">
+        <v>4.5300925925925928E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B6" s="67" t="s">
+        <v>225</v>
+      </c>
+      <c r="C6" s="68">
+        <v>8.0902777777777787E-4</v>
+      </c>
+      <c r="D6" s="68">
+        <v>7.9837962962962968E-4</v>
+      </c>
+      <c r="E6" s="68">
+        <v>7.869212962962962E-4</v>
+      </c>
+      <c r="H6" s="67" t="s">
+        <v>225</v>
+      </c>
+      <c r="I6" s="68">
+        <v>9.5381944444444442E-4</v>
+      </c>
+      <c r="J6" s="68">
+        <v>9.3854166666666673E-4</v>
+      </c>
+      <c r="K6" s="68">
+        <v>9.2199074074074069E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B7" s="67" t="s">
+        <v>226</v>
+      </c>
+      <c r="C7" s="68">
+        <v>5.9027777777777778E-4</v>
+      </c>
+      <c r="D7" s="68">
+        <v>5.8495370370370374E-4</v>
+      </c>
+      <c r="E7" s="68">
+        <v>5.7928240740740737E-4</v>
+      </c>
+      <c r="H7" s="67" t="s">
+        <v>226</v>
+      </c>
+      <c r="I7" s="68">
+        <v>6.9664351851851853E-4</v>
+      </c>
+      <c r="J7" s="68">
+        <v>6.8946759259259265E-4</v>
+      </c>
+      <c r="K7" s="68">
+        <v>6.8171296296296296E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B8" s="67" t="s">
+        <v>227</v>
+      </c>
+      <c r="C8" s="68">
+        <v>6.8726851851851859E-4</v>
+      </c>
+      <c r="D8" s="68">
+        <v>6.7418981481481486E-4</v>
+      </c>
+      <c r="E8" s="68">
+        <v>6.5995370370370372E-4</v>
+      </c>
+      <c r="H8" s="67" t="s">
+        <v>227</v>
+      </c>
+      <c r="I8" s="68">
+        <v>7.7847222222222228E-4</v>
+      </c>
+      <c r="J8" s="68">
+        <v>7.6828703703703694E-4</v>
+      </c>
+      <c r="K8" s="68">
+        <v>7.571759259259259E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B9" s="67" t="s">
+        <v>228</v>
+      </c>
+      <c r="C9" s="68">
+        <v>1.5266203703703705E-3</v>
+      </c>
+      <c r="D9" s="68">
+        <v>1.5104166666666666E-3</v>
+      </c>
+      <c r="E9" s="68">
+        <v>1.4928240740740739E-3</v>
+      </c>
+      <c r="H9" s="67" t="s">
+        <v>228</v>
+      </c>
+      <c r="I9" s="68">
+        <v>1.6328703703703702E-3</v>
+      </c>
+      <c r="J9" s="68">
+        <v>1.6271990740740741E-3</v>
+      </c>
+      <c r="K9" s="68">
+        <v>1.6210648148148148E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B10" s="67" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="68">
+        <v>1.6688657407407407E-3</v>
+      </c>
+      <c r="D10" s="68">
+        <v>1.6509259259259257E-3</v>
+      </c>
+      <c r="E10" s="68">
+        <v>1.6315972222222222E-3</v>
+      </c>
+      <c r="H10" s="67" t="s">
+        <v>232</v>
+      </c>
+      <c r="I10" s="68">
+        <v>1.8101851851851853E-3</v>
+      </c>
+      <c r="J10" s="68">
+        <v>1.7979166666666666E-3</v>
+      </c>
+      <c r="K10" s="68">
+        <v>1.784722222222222E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B12" t="s">
+        <v>230</v>
+      </c>
+      <c r="F12">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H12" t="s">
+        <v>234</v>
+      </c>
+      <c r="L12">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B13" s="66" t="s">
+        <v>224</v>
+      </c>
+      <c r="C13" s="69">
+        <v>2010</v>
+      </c>
+      <c r="D13" s="69">
+        <v>2009</v>
+      </c>
+      <c r="E13" s="69">
+        <v>2008</v>
+      </c>
+      <c r="H13" s="66" t="s">
+        <v>224</v>
+      </c>
+      <c r="I13" s="69">
+        <v>2010</v>
+      </c>
+      <c r="J13" s="69">
+        <v>2009</v>
+      </c>
+      <c r="K13" s="69">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B14" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="68">
+        <f>C5*$F$12</f>
+        <v>4.1122685185185186E-4</v>
+      </c>
+      <c r="D14" s="68">
+        <f t="shared" ref="D14:E14" si="0">D5*$F$12</f>
+        <v>4.072800925925926E-4</v>
+      </c>
+      <c r="E14" s="68">
+        <f t="shared" si="0"/>
+        <v>4.0282407407407411E-4</v>
+      </c>
+      <c r="H14" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14" s="68">
+        <f>I5*$L$12</f>
+        <v>5.1791666666666663E-4</v>
+      </c>
+      <c r="J14" s="68">
+        <f t="shared" ref="J14:K14" si="1">J5*$L$12</f>
+        <v>5.0836805555555563E-4</v>
+      </c>
+      <c r="K14" s="68">
+        <f t="shared" si="1"/>
+        <v>4.9831018518518529E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B15" s="67" t="s">
+        <v>225</v>
+      </c>
+      <c r="C15" s="68">
+        <f t="shared" ref="C15:E15" si="2">C6*$F$12</f>
+        <v>8.899305555555557E-4</v>
+      </c>
+      <c r="D15" s="68">
+        <f t="shared" si="2"/>
+        <v>8.7821759259259276E-4</v>
+      </c>
+      <c r="E15" s="68">
+        <f t="shared" si="2"/>
+        <v>8.6561342592592593E-4</v>
+      </c>
+      <c r="H15" s="67" t="s">
+        <v>225</v>
+      </c>
+      <c r="I15" s="68">
+        <f t="shared" ref="I15:K15" si="3">I6*$L$12</f>
+        <v>1.049201388888889E-3</v>
+      </c>
+      <c r="J15" s="68">
+        <f t="shared" si="3"/>
+        <v>1.0323958333333335E-3</v>
+      </c>
+      <c r="K15" s="68">
+        <f t="shared" si="3"/>
+        <v>1.0141898148148148E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B16" s="67" t="s">
+        <v>226</v>
+      </c>
+      <c r="C16" s="68">
+        <f t="shared" ref="C16:E16" si="4">C7*$F$12</f>
+        <v>6.4930555555555564E-4</v>
+      </c>
+      <c r="D16" s="68">
+        <f t="shared" si="4"/>
+        <v>6.4344907407407417E-4</v>
+      </c>
+      <c r="E16" s="68">
+        <f t="shared" si="4"/>
+        <v>6.3721064814814814E-4</v>
+      </c>
+      <c r="H16" s="67" t="s">
+        <v>226</v>
+      </c>
+      <c r="I16" s="68">
+        <f t="shared" ref="I16:K16" si="5">I7*$L$12</f>
+        <v>7.6630787037037043E-4</v>
+      </c>
+      <c r="J16" s="68">
+        <f t="shared" si="5"/>
+        <v>7.5841435185185202E-4</v>
+      </c>
+      <c r="K16" s="68">
+        <f t="shared" si="5"/>
+        <v>7.4988425925925928E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B17" s="67" t="s">
+        <v>227</v>
+      </c>
+      <c r="C17" s="68">
+        <f t="shared" ref="C17:E17" si="6">C8*$F$12</f>
+        <v>7.5599537037037052E-4</v>
+      </c>
+      <c r="D17" s="68">
+        <f t="shared" si="6"/>
+        <v>7.4160879629629642E-4</v>
+      </c>
+      <c r="E17" s="68">
+        <f t="shared" si="6"/>
+        <v>7.2594907407407417E-4</v>
+      </c>
+      <c r="H17" s="67" t="s">
+        <v>227</v>
+      </c>
+      <c r="I17" s="68">
+        <f t="shared" ref="I17:K17" si="7">I8*$L$12</f>
+        <v>8.563194444444446E-4</v>
+      </c>
+      <c r="J17" s="68">
+        <f t="shared" si="7"/>
+        <v>8.4511574074074068E-4</v>
+      </c>
+      <c r="K17" s="68">
+        <f t="shared" si="7"/>
+        <v>8.3289351851851851E-4</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B18" s="67" t="s">
+        <v>228</v>
+      </c>
+      <c r="C18" s="68">
+        <f t="shared" ref="C18:E19" si="8">C9*$F$12</f>
+        <v>1.6792824074074075E-3</v>
+      </c>
+      <c r="D18" s="68">
+        <f t="shared" si="8"/>
+        <v>1.6614583333333334E-3</v>
+      </c>
+      <c r="E18" s="68">
+        <f t="shared" si="8"/>
+        <v>1.6421064814814814E-3</v>
+      </c>
+      <c r="H18" s="67" t="s">
+        <v>228</v>
+      </c>
+      <c r="I18" s="68">
+        <f t="shared" ref="I18:K18" si="9">I9*$L$12</f>
+        <v>1.7961574074074073E-3</v>
+      </c>
+      <c r="J18" s="68">
+        <f t="shared" si="9"/>
+        <v>1.7899189814814817E-3</v>
+      </c>
+      <c r="K18" s="68">
+        <f t="shared" si="9"/>
+        <v>1.7831712962962964E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B19" s="67" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="68">
+        <f t="shared" si="8"/>
+        <v>1.835752314814815E-3</v>
+      </c>
+      <c r="D19" s="68">
+        <f t="shared" si="8"/>
+        <v>1.8160185185185185E-3</v>
+      </c>
+      <c r="E19" s="68">
+        <f t="shared" si="8"/>
+        <v>1.7947569444444445E-3</v>
+      </c>
+      <c r="H19" s="67" t="s">
+        <v>4</v>
+      </c>
+      <c r="I19" s="68">
+        <f t="shared" ref="I19:K19" si="10">I10*$L$12</f>
+        <v>1.9912037037037038E-3</v>
+      </c>
+      <c r="J19" s="68">
+        <f t="shared" si="10"/>
+        <v>1.9777083333333335E-3</v>
+      </c>
+      <c r="K19" s="68">
+        <f t="shared" si="10"/>
+        <v>1.9631944444444445E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B22" s="66"/>
+      <c r="C22" s="69"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="69"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B23" s="67"/>
+      <c r="C23" s="68"/>
+      <c r="D23" s="68"/>
+      <c r="E23" s="68"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B24" s="67"/>
+      <c r="C24" s="68"/>
+      <c r="D24" s="68"/>
+      <c r="E24" s="68"/>
+    </row>
+    <row r="25" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B25" s="67"/>
+      <c r="C25" s="68"/>
+      <c r="D25" s="68"/>
+      <c r="E25" s="68"/>
+    </row>
+    <row r="26" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B26" s="67"/>
+      <c r="C26" s="68"/>
+      <c r="D26" s="68"/>
+      <c r="E26" s="68"/>
+    </row>
+    <row r="27" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B27" s="67"/>
+      <c r="C27" s="68"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="68"/>
+    </row>
+    <row r="28" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B28" s="67"/>
+      <c r="C28" s="68"/>
+      <c r="D28" s="68"/>
+      <c r="E28" s="68"/>
+    </row>
+    <row r="31" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B31" s="66"/>
+      <c r="C31" s="69"/>
+      <c r="D31" s="69"/>
+      <c r="E31" s="69"/>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.45">
+      <c r="B32" s="67"/>
+      <c r="C32" s="68"/>
+      <c r="D32" s="68"/>
+      <c r="E32" s="68"/>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B33" s="67"/>
+      <c r="C33" s="68"/>
+      <c r="D33" s="68"/>
+      <c r="E33" s="68"/>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B34" s="67"/>
+      <c r="C34" s="68"/>
+      <c r="D34" s="68"/>
+      <c r="E34" s="68"/>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B35" s="67"/>
+      <c r="C35" s="68"/>
+      <c r="D35" s="68"/>
+      <c r="E35" s="68"/>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B36" s="67"/>
+      <c r="C36" s="68"/>
+      <c r="D36" s="68"/>
+      <c r="E36" s="68"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B37" s="67"/>
+      <c r="C37" s="68"/>
+      <c r="D37" s="68"/>
+      <c r="E37" s="68"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3E1FA05-76A3-4AE3-B1B5-E78B06AE489F}">
   <sheetPr codeName="Tabelle3">
     <tabColor theme="1"/>
@@ -12738,15 +14498,15 @@
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
-    <col min="2" max="13" width="18.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.86328125" style="1" customWidth="1"/>
+    <col min="2" max="13" width="18.73046875" style="1" customWidth="1"/>
     <col min="14" max="14" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="11.42578125" style="1"/>
+    <col min="15" max="16384" width="11.3984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="18">
         <v>2024</v>
       </c>
@@ -12790,7 +14550,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
@@ -12846,7 +14606,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -12902,7 +14662,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="19" t="s">
         <v>8</v>
       </c>
@@ -12958,7 +14718,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" s="64" t="s">
         <v>13</v>
       </c>
@@ -12976,7 +14736,7 @@
       <c r="M7" s="64"/>
       <c r="N7" s="64"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" s="64"/>
       <c r="B8" s="64"/>
       <c r="C8" s="64"/>
@@ -12992,7 +14752,7 @@
       <c r="M8" s="64"/>
       <c r="N8" s="64"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" s="20" t="s">
         <v>6</v>
       </c>
@@ -13046,7 +14806,7 @@
       </c>
       <c r="N9" s="21"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" s="20" t="s">
         <v>7</v>
       </c>
@@ -13100,7 +14860,7 @@
       </c>
       <c r="N10" s="21"/>
     </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="22" t="s">
         <v>8</v>
       </c>
@@ -13154,7 +14914,7 @@
       </c>
       <c r="N11" s="23"/>
     </row>
-    <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="63" t="s">
         <v>14</v>
       </c>
@@ -13175,7 +14935,7 @@
       <c r="M14"/>
       <c r="N14"/>
     </row>
-    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="63"/>
       <c r="B15" s="63"/>
       <c r="C15" s="63"/>
@@ -13190,7 +14950,7 @@
       <c r="M15"/>
       <c r="N15"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -13225,7 +14985,7 @@
       <c r="M16"/>
       <c r="N16"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A17" s="8" t="s">
         <v>19</v>
       </c>
@@ -13260,7 +15020,7 @@
       <c r="M17"/>
       <c r="N17"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>19</v>
       </c>
@@ -13293,7 +15053,7 @@
       <c r="M18"/>
       <c r="N18"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A19" s="8" t="s">
         <v>22</v>
       </c>
@@ -13326,7 +15086,7 @@
       <c r="M19"/>
       <c r="N19"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A20" s="9" t="s">
         <v>24</v>
       </c>
@@ -13357,7 +15117,7 @@
       <c r="M20"/>
       <c r="N20"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A21" s="8" t="s">
         <v>22</v>
       </c>
@@ -13384,7 +15144,7 @@
       <c r="M21"/>
       <c r="N21"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
         <v>19</v>
       </c>
@@ -13407,7 +15167,7 @@
       <c r="I22" s="33"/>
       <c r="L22" s="41"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A23" s="8" t="s">
         <v>19</v>
       </c>
@@ -13430,50 +15190,50 @@
       <c r="I23" s="33"/>
       <c r="L23" s="40"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
       <c r="H24" s="33"/>
       <c r="I24" s="33"/>
       <c r="L24" s="41"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
       <c r="H25" s="33"/>
       <c r="I25" s="33"/>
       <c r="L25" s="40"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L26" s="41"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L27" s="40"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L28" s="41"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L29" s="40"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L30" s="41"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L31" s="40"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L32" s="41"/>
     </row>
-    <row r="33" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L33" s="40"/>
     </row>
-    <row r="34" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L34" s="41"/>
     </row>
-    <row r="35" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L35" s="33"/>
     </row>
-    <row r="36" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L36" s="41"/>
     </row>
-    <row r="37" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L37" s="33"/>
     </row>
   </sheetData>
@@ -13486,800 +15246,4 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7831D901-68D8-4F92-82B6-BCB1A3899285}">
-  <sheetPr codeName="Tabelle4">
-    <tabColor theme="4"/>
-  </sheetPr>
-  <dimension ref="A1:N39"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
-    <col min="2" max="13" width="18.7109375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="11.42578125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="18">
-        <v>2025</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="26" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(B$1))*86400,2)</f>
-        <v>44.41</v>
-      </c>
-      <c r="C2" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(C$1))*86400,2)</f>
-        <v>65.53</v>
-      </c>
-      <c r="D2" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(D$1))*86400,2)</f>
-        <v>93.26</v>
-      </c>
-      <c r="E2" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(E$1))*86400,2)</f>
-        <v>75.900000000000006</v>
-      </c>
-      <c r="F2" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(F$1))*86400,2)</f>
-        <v>189.05</v>
-      </c>
-      <c r="G2" s="27">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(G$1))*86400,2)</f>
-        <v>164.57</v>
-      </c>
-      <c r="H2" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(H$1))*86400,2)</f>
-        <v>38.799999999999997</v>
-      </c>
-      <c r="I2" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(I$1))*86400,2)</f>
-        <v>61.05</v>
-      </c>
-      <c r="J2" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(J$1))*86400,2)</f>
-        <v>79.22</v>
-      </c>
-      <c r="K2" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(K$1))*86400,2)</f>
-        <v>66.430000000000007</v>
-      </c>
-      <c r="L2" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(L$1))*86400,2)</f>
-        <v>168.79</v>
-      </c>
-      <c r="M2" s="15">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N2-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(M$1))*86400,2)</f>
-        <v>155.07</v>
-      </c>
-      <c r="N2" s="2">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="16">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(B$1))*86400,2)</f>
-        <v>43.12</v>
-      </c>
-      <c r="C3" s="16">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(C$1))*86400,2)</f>
-        <v>63.63</v>
-      </c>
-      <c r="D3" s="16">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(D$1))*86400,2)</f>
-        <v>90.56</v>
-      </c>
-      <c r="E3" s="16">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(E$1))*86400,2)</f>
-        <v>73.7</v>
-      </c>
-      <c r="F3" s="16">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(F$1))*86400,2)</f>
-        <v>183.57</v>
-      </c>
-      <c r="G3" s="28">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(G$1))*86400,2)</f>
-        <v>159.79</v>
-      </c>
-      <c r="H3" s="16">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(H$1))*86400,2)</f>
-        <v>37.68</v>
-      </c>
-      <c r="I3" s="16">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(I$1))*86400,2)</f>
-        <v>59.28</v>
-      </c>
-      <c r="J3" s="16">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(J$1))*86400,2)</f>
-        <v>76.92</v>
-      </c>
-      <c r="K3" s="16">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(K$1))*86400,2)</f>
-        <v>64.5</v>
-      </c>
-      <c r="L3" s="16">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(L$1))*86400,2)</f>
-        <v>163.9</v>
-      </c>
-      <c r="M3" s="17">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N3-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Youth[],COLUMN(M$1))*86400,2)</f>
-        <v>150.57</v>
-      </c>
-      <c r="N3" s="2">
-        <v>730</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(B$1))*86400,2)</f>
-        <v>41.76</v>
-      </c>
-      <c r="C4" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(C$1))*86400,2)</f>
-        <v>62.97</v>
-      </c>
-      <c r="D4" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(D$1))*86400,2)</f>
-        <v>84.9</v>
-      </c>
-      <c r="E4" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(E$1))*86400,2)</f>
-        <v>70.760000000000005</v>
-      </c>
-      <c r="F4" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(F$1))*86400,2)</f>
-        <v>173.81</v>
-      </c>
-      <c r="G4" s="27">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(G$1))*86400,2)</f>
-        <v>155.68</v>
-      </c>
-      <c r="H4" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(H$1))*86400,2)</f>
-        <v>34.83</v>
-      </c>
-      <c r="I4" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(I$1))*86400,2)</f>
-        <v>56.25</v>
-      </c>
-      <c r="J4" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(J$1))*86400,2)</f>
-        <v>73.650000000000006</v>
-      </c>
-      <c r="K4" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(K$1))*86400,2)</f>
-        <v>62.47</v>
-      </c>
-      <c r="L4" s="14">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(L$1))*86400,2)</f>
-        <v>157.09</v>
-      </c>
-      <c r="M4" s="15">
-        <f>ROUND(((2001/934)-((2001/934)^2+($N4-2534)/467)^(1/2))*VLOOKUP($A$1-1,WR_Open[],COLUMN(M$1))*86400,2)</f>
-        <v>144.54</v>
-      </c>
-      <c r="N4" s="2">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" s="64" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="64"/>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="64"/>
-      <c r="F7" s="64"/>
-      <c r="G7" s="64"/>
-      <c r="H7" s="64"/>
-      <c r="I7" s="64"/>
-      <c r="J7" s="64"/>
-      <c r="K7" s="64"/>
-      <c r="L7" s="64"/>
-      <c r="M7" s="64"/>
-      <c r="N7" s="64"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="64"/>
-      <c r="B8" s="64"/>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="64"/>
-      <c r="F8" s="64"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="64"/>
-      <c r="I8" s="64"/>
-      <c r="J8" s="64"/>
-      <c r="K8" s="64"/>
-      <c r="L8" s="64"/>
-      <c r="M8" s="64"/>
-      <c r="N8" s="64"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="31" t="str">
-        <f t="shared" ref="B9" si="0">CONCATENATE(ROUNDDOWN(B2/60,0),":",TEXT(B2-(60*ROUNDDOWN(B2/60,0)),"00,00"))</f>
-        <v>0:44,41</v>
-      </c>
-      <c r="C9" s="31" t="str">
-        <f>CONCATENATE(ROUNDDOWN(C2/60,0),":",TEXT(C2-(60*ROUNDDOWN(C2/60,0)),"00,00"))</f>
-        <v>1:05,53</v>
-      </c>
-      <c r="D9" s="31" t="str">
-        <f t="shared" ref="D9:M9" si="1">CONCATENATE(ROUNDDOWN(D2/60,0),":",TEXT(D2-(60*ROUNDDOWN(D2/60,0)),"00,00"))</f>
-        <v>1:33,26</v>
-      </c>
-      <c r="E9" s="31" t="str">
-        <f t="shared" si="1"/>
-        <v>1:15,90</v>
-      </c>
-      <c r="F9" s="31" t="str">
-        <f t="shared" si="1"/>
-        <v>3:09,05</v>
-      </c>
-      <c r="G9" s="32" t="str">
-        <f t="shared" si="1"/>
-        <v>2:44,57</v>
-      </c>
-      <c r="H9" s="31" t="str">
-        <f t="shared" si="1"/>
-        <v>0:38,80</v>
-      </c>
-      <c r="I9" s="31" t="str">
-        <f t="shared" si="1"/>
-        <v>1:01,05</v>
-      </c>
-      <c r="J9" s="31" t="str">
-        <f t="shared" si="1"/>
-        <v>1:19,22</v>
-      </c>
-      <c r="K9" s="31" t="str">
-        <f t="shared" si="1"/>
-        <v>1:06,43</v>
-      </c>
-      <c r="L9" s="31" t="str">
-        <f t="shared" si="1"/>
-        <v>2:48,79</v>
-      </c>
-      <c r="M9" s="31" t="str">
-        <f t="shared" si="1"/>
-        <v>2:35,07</v>
-      </c>
-      <c r="N9" s="21"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="24" t="str">
-        <f t="shared" ref="B10:M10" si="2">CONCATENATE(ROUNDDOWN(B3/60,0),":",TEXT(B3-(60*ROUNDDOWN(B3/60,0)),"00,00"))</f>
-        <v>0:43,12</v>
-      </c>
-      <c r="C10" s="24" t="str">
-        <f t="shared" si="2"/>
-        <v>1:03,63</v>
-      </c>
-      <c r="D10" s="24" t="str">
-        <f t="shared" si="2"/>
-        <v>1:30,56</v>
-      </c>
-      <c r="E10" s="24" t="str">
-        <f t="shared" si="2"/>
-        <v>1:13,70</v>
-      </c>
-      <c r="F10" s="24" t="str">
-        <f t="shared" si="2"/>
-        <v>3:03,57</v>
-      </c>
-      <c r="G10" s="29" t="str">
-        <f t="shared" si="2"/>
-        <v>2:39,79</v>
-      </c>
-      <c r="H10" s="24" t="str">
-        <f t="shared" si="2"/>
-        <v>0:37,68</v>
-      </c>
-      <c r="I10" s="24" t="str">
-        <f t="shared" si="2"/>
-        <v>0:59,28</v>
-      </c>
-      <c r="J10" s="24" t="str">
-        <f t="shared" si="2"/>
-        <v>1:16,92</v>
-      </c>
-      <c r="K10" s="24" t="str">
-        <f t="shared" si="2"/>
-        <v>1:04,50</v>
-      </c>
-      <c r="L10" s="24" t="str">
-        <f t="shared" si="2"/>
-        <v>2:43,90</v>
-      </c>
-      <c r="M10" s="24" t="str">
-        <f t="shared" si="2"/>
-        <v>2:30,57</v>
-      </c>
-      <c r="N10" s="21"/>
-    </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="B11" s="25" t="str">
-        <f t="shared" ref="B11:M11" si="3">CONCATENATE(ROUNDDOWN(B4/60,0),":",TEXT(B4-(60*ROUNDDOWN(B4/60,0)),"00,00"))</f>
-        <v>0:41,76</v>
-      </c>
-      <c r="C11" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>1:02,97</v>
-      </c>
-      <c r="D11" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>1:24,90</v>
-      </c>
-      <c r="E11" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>1:10,76</v>
-      </c>
-      <c r="F11" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>2:53,81</v>
-      </c>
-      <c r="G11" s="30" t="str">
-        <f t="shared" si="3"/>
-        <v>2:35,68</v>
-      </c>
-      <c r="H11" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>0:34,83</v>
-      </c>
-      <c r="I11" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>0:56,25</v>
-      </c>
-      <c r="J11" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>1:13,65</v>
-      </c>
-      <c r="K11" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>1:02,47</v>
-      </c>
-      <c r="L11" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>2:37,09</v>
-      </c>
-      <c r="M11" s="25" t="str">
-        <f t="shared" si="3"/>
-        <v>2:24,54</v>
-      </c>
-      <c r="N11" s="23"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="63" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="63"/>
-      <c r="C14" s="63"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="63"/>
-      <c r="H14" s="65" t="s">
-        <v>35</v>
-      </c>
-      <c r="I14" s="65"/>
-      <c r="J14" s="65"/>
-      <c r="L14" s="65" t="s">
-        <v>36</v>
-      </c>
-      <c r="M14"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="63"/>
-      <c r="B15" s="63"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="63"/>
-      <c r="H15" s="65"/>
-      <c r="I15" s="65"/>
-      <c r="J15" s="65"/>
-      <c r="L15" s="65"/>
-      <c r="M15"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="M16"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="8">
-        <v>15</v>
-      </c>
-      <c r="C17" s="8">
-        <v>18</v>
-      </c>
-      <c r="D17" s="8">
-        <v>3</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H17" s="34" t="s">
-        <v>88</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="J17" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="L17" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="M17"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" s="9">
-        <v>13</v>
-      </c>
-      <c r="C18" s="9">
-        <v>14</v>
-      </c>
-      <c r="D18" s="9">
-        <v>1</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F18" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H18" s="35" t="s">
-        <v>89</v>
-      </c>
-      <c r="I18" s="35" t="s">
-        <v>31</v>
-      </c>
-      <c r="J18" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="L18" s="38"/>
-      <c r="M18"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B19" s="8">
-        <v>12</v>
-      </c>
-      <c r="C19" s="8">
-        <v>18</v>
-      </c>
-      <c r="D19" s="8">
-        <v>16</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F19" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="H19" s="34" t="s">
-        <v>90</v>
-      </c>
-      <c r="I19" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="J19" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="L19" s="36"/>
-      <c r="M19"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="9">
-        <v>12</v>
-      </c>
-      <c r="C20" s="9">
-        <v>18</v>
-      </c>
-      <c r="D20" s="9">
-        <v>10</v>
-      </c>
-      <c r="E20" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H20" s="35" t="s">
-        <v>91</v>
-      </c>
-      <c r="I20" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="J20" s="35"/>
-      <c r="L20" s="38"/>
-      <c r="M20"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="8">
-        <v>12</v>
-      </c>
-      <c r="C21" s="8">
-        <v>100</v>
-      </c>
-      <c r="D21" s="8">
-        <v>8</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H21" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="I21" s="34" t="s">
-        <v>31</v>
-      </c>
-      <c r="J21" s="34" t="s">
-        <v>26</v>
-      </c>
-      <c r="L21" s="36"/>
-      <c r="M21"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" s="9">
-        <v>17</v>
-      </c>
-      <c r="C22" s="9">
-        <v>18</v>
-      </c>
-      <c r="D22" s="9">
-        <v>1</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="H22" s="40" t="s">
-        <v>93</v>
-      </c>
-      <c r="I22" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="J22" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="L22" s="39"/>
-      <c r="M22"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23" s="8">
-        <v>19</v>
-      </c>
-      <c r="C23" s="8">
-        <v>100</v>
-      </c>
-      <c r="D23" s="8">
-        <v>4</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F23" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="H23" s="41" t="s">
-        <v>94</v>
-      </c>
-      <c r="I23" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="J23" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="L23" s="37"/>
-      <c r="M23"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H24" s="40"/>
-      <c r="I24" s="40"/>
-      <c r="J24" s="40"/>
-      <c r="L24" s="39"/>
-      <c r="M24"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="H25" s="33"/>
-      <c r="I25" s="33"/>
-      <c r="L25" s="37"/>
-      <c r="M25"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L26" s="39"/>
-      <c r="M26"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L27" s="37"/>
-      <c r="M27"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L28" s="39"/>
-      <c r="M28"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L29" s="37"/>
-      <c r="M29"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L30" s="39"/>
-      <c r="M30"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L31" s="37"/>
-      <c r="M31"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="L32" s="39"/>
-      <c r="M32"/>
-    </row>
-    <row r="33" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="L33" s="37"/>
-      <c r="M33"/>
-    </row>
-    <row r="34" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="L34" s="39"/>
-      <c r="M34"/>
-    </row>
-    <row r="35" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="M35"/>
-    </row>
-    <row r="36" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="L36" s="39"/>
-      <c r="M36"/>
-    </row>
-    <row r="37" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="M37"/>
-    </row>
-    <row r="38" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="H38"/>
-      <c r="I38"/>
-      <c r="J38"/>
-      <c r="K38"/>
-      <c r="L38"/>
-      <c r="M38"/>
-    </row>
-    <row r="39" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="H39"/>
-      <c r="I39"/>
-      <c r="J39"/>
-      <c r="K39"/>
-      <c r="L39"/>
-      <c r="M39"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A7:N8"/>
-    <mergeCell ref="A14:F15"/>
-    <mergeCell ref="H14:J15"/>
-    <mergeCell ref="L14:L15"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Quali ende bis 2026
</commit_message>
<xml_diff>
--- a/web/utilities/records_kriterien.xlsx
+++ b/web/utilities/records_kriterien.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgna\Documents\GitHub\Lifesaving_Baden\web\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B848911A-46E0-40F5-B959-1D8076048383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{606D5193-BE97-4DFD-B5E0-AA0EA72B087C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="6" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
   </bookViews>
@@ -13325,8 +13325,8 @@
   </sheetPr>
   <dimension ref="A1:X12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4:X8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -13588,7 +13588,7 @@
         <v>45658</v>
       </c>
       <c r="F4" s="61">
-        <v>46022</v>
+        <v>46387</v>
       </c>
       <c r="G4" s="61">
         <v>45658</v>
@@ -13664,7 +13664,7 @@
         <v>45658</v>
       </c>
       <c r="F5" s="61">
-        <v>46022</v>
+        <v>46387</v>
       </c>
       <c r="G5" s="61">
         <v>45658</v>
@@ -13740,7 +13740,7 @@
         <v>45658</v>
       </c>
       <c r="F6" s="61">
-        <v>46022</v>
+        <v>46387</v>
       </c>
       <c r="G6" s="61">
         <v>45658</v>
@@ -13816,7 +13816,7 @@
         <v>45658</v>
       </c>
       <c r="F7" s="61">
-        <v>46022</v>
+        <v>46387</v>
       </c>
       <c r="G7" s="61">
         <v>45658</v>
@@ -13892,7 +13892,7 @@
         <v>45658</v>
       </c>
       <c r="F8" s="61">
-        <v>46022</v>
+        <v>46387</v>
       </c>
       <c r="G8" s="61">
         <v>45658</v>
@@ -13968,7 +13968,7 @@
         <v>45658</v>
       </c>
       <c r="F9" s="61">
-        <v>46022</v>
+        <v>46387</v>
       </c>
       <c r="G9" s="61">
         <v>45658</v>

</xml_diff>

<commit_message>
Tabellen verschmelzung JRP und OMS JA bei DEM... warum werden die angezeigt???
</commit_message>
<xml_diff>
--- a/web/utilities/records_kriterien.xlsx
+++ b/web/utilities/records_kriterien.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgna\Documents\GitHub\Lifesaving_Baden\web\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09C9167-0B48-41CB-8197-7F13F5038504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5871D699-98AC-4B15-B629-87D0C7F71EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="6" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="5" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
   </bookViews>
   <sheets>
     <sheet name="DR" sheetId="9" r:id="rId1"/>
@@ -12088,7 +12088,7 @@
   </sheetPr>
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
@@ -12784,8 +12784,8 @@
   </sheetPr>
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L6" sqref="A1:X7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -12916,7 +12916,7 @@
         <v>178</v>
       </c>
       <c r="I2" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J2" s="59"/>
       <c r="K2" s="59"/>
@@ -12986,7 +12986,7 @@
         <v>178</v>
       </c>
       <c r="I3" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J3" s="59"/>
       <c r="K3" s="59"/>
@@ -13056,7 +13056,7 @@
         <v>178</v>
       </c>
       <c r="I4" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J4" s="59"/>
       <c r="K4" s="59"/>
@@ -13126,7 +13126,7 @@
         <v>178</v>
       </c>
       <c r="I5" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J5" s="59"/>
       <c r="K5" s="59"/>
@@ -13196,7 +13196,7 @@
         <v>178</v>
       </c>
       <c r="I6" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J6" s="59"/>
       <c r="K6" s="59"/>
@@ -13266,7 +13266,7 @@
         <v>178</v>
       </c>
       <c r="I7" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="J7" s="59"/>
       <c r="K7" s="59"/>
@@ -13325,8 +13325,8 @@
   </sheetPr>
   <dimension ref="A1:X12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4:X9"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
oms deaktiviert außer beim OMS
</commit_message>
<xml_diff>
--- a/web/utilities/records_kriterien.xlsx
+++ b/web/utilities/records_kriterien.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgna\Documents\GitHub\Lifesaving_Baden\web\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5871D699-98AC-4B15-B629-87D0C7F71EEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27686831-6BFF-402B-B4F6-43ABE3AAE32A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="5" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
   </bookViews>
@@ -12089,7 +12089,7 @@
   <dimension ref="A1:U3"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -12209,7 +12209,7 @@
         <v>178</v>
       </c>
       <c r="J2" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="K2" s="59"/>
       <c r="L2" s="59"/>
@@ -12270,7 +12270,7 @@
         <v>178</v>
       </c>
       <c r="J3" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="K3" s="59"/>
       <c r="L3" s="59"/>
@@ -12318,7 +12318,7 @@
   <dimension ref="A1:U7"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -12438,7 +12438,7 @@
         <v>178</v>
       </c>
       <c r="J2" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="K2" s="59"/>
       <c r="L2" s="59"/>
@@ -12499,7 +12499,7 @@
         <v>178</v>
       </c>
       <c r="J3" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="K3" s="59"/>
       <c r="L3" s="59"/>
@@ -12560,7 +12560,7 @@
         <v>178</v>
       </c>
       <c r="J4" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="K4" s="59"/>
       <c r="L4" s="59"/>
@@ -12621,7 +12621,7 @@
         <v>178</v>
       </c>
       <c r="J5" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="K5" s="59"/>
       <c r="L5" s="59"/>
@@ -12680,7 +12680,7 @@
         <v>178</v>
       </c>
       <c r="J6" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="K6" s="59"/>
       <c r="L6" s="59"/>
@@ -12739,7 +12739,7 @@
         <v>178</v>
       </c>
       <c r="J7" s="59" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="K7" s="59"/>
       <c r="L7" s="59"/>

</xml_diff>

<commit_message>
New Tabel for Standartabweichung
</commit_message>
<xml_diff>
--- a/web/utilities/records_kriterien.xlsx
+++ b/web/utilities/records_kriterien.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgna\Documents\GitHub\Lifesaving_Baden\web\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6E63697-3764-40A1-B36A-F770F954392D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43BE5C89-43F2-489C-9A3A-8BD38956CB5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="6" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
   </bookViews>
@@ -220,7 +220,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="236">
   <si>
     <t>50m Retten</t>
   </si>
@@ -925,6 +925,9 @@
   </si>
   <si>
     <t>NK2-W (10% / 15%Test)</t>
+  </si>
+  <si>
+    <t>AK15 W Normfenster 0,8</t>
   </si>
 </sst>
 </file>
@@ -4054,8 +4057,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}" name="JRP_konfig" displayName="JRP_konfig" ref="A1:X9" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
-  <autoFilter ref="A1:X9" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}" name="JRP_konfig" displayName="JRP_konfig" ref="A1:X10" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+  <autoFilter ref="A1:X10" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -13323,7 +13326,7 @@
   <dimension ref="A1:X12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:A9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -14060,6 +14063,82 @@
         <v>1.877800925925926E-3</v>
       </c>
     </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A10" s="59" t="s">
+        <v>235</v>
+      </c>
+      <c r="B10" s="59" t="s">
+        <v>164</v>
+      </c>
+      <c r="C10" s="59">
+        <v>13</v>
+      </c>
+      <c r="D10" s="59">
+        <v>16</v>
+      </c>
+      <c r="E10" s="61">
+        <v>45658</v>
+      </c>
+      <c r="F10" s="61">
+        <v>46023</v>
+      </c>
+      <c r="G10" s="61">
+        <v>45658</v>
+      </c>
+      <c r="H10" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="I10" s="59" t="s">
+        <v>179</v>
+      </c>
+      <c r="J10" s="59"/>
+      <c r="K10" s="59"/>
+      <c r="L10" s="59">
+        <v>10</v>
+      </c>
+      <c r="M10" s="62">
+        <v>5.4239999999999996E-4</v>
+      </c>
+      <c r="N10" s="62">
+        <v>8.5547824074074072E-4</v>
+      </c>
+      <c r="O10" s="62">
+        <v>1.0492013888888888E-3</v>
+      </c>
+      <c r="P10" s="62">
+        <v>8.7188888888888895E-4</v>
+      </c>
+      <c r="Q10" s="62">
+        <v>1.9712916666666668E-3</v>
+      </c>
+      <c r="R10" s="62">
+        <v>1.9267870370370367E-3</v>
+      </c>
+      <c r="S10" s="62">
+        <f>JRP_konfig[[#This Row],[PZ1 - 50m Retten]]</f>
+        <v>5.4239999999999996E-4</v>
+      </c>
+      <c r="T10" s="62">
+        <f>JRP_konfig[[#This Row],[PZ1 - 50m Retten]]</f>
+        <v>5.4239999999999996E-4</v>
+      </c>
+      <c r="U10" s="62">
+        <f>JRP_konfig[[#This Row],[PZ1 - 50m Retten]]</f>
+        <v>5.4239999999999996E-4</v>
+      </c>
+      <c r="V10" s="62">
+        <f>JRP_konfig[[#This Row],[PZ1 - 50m Retten]]</f>
+        <v>5.4239999999999996E-4</v>
+      </c>
+      <c r="W10" s="62">
+        <f>JRP_konfig[[#This Row],[PZ1 - 50m Retten]]</f>
+        <v>5.4239999999999996E-4</v>
+      </c>
+      <c r="X10" s="62">
+        <f>JRP_konfig[[#This Row],[PZ1 - 50m Retten]]</f>
+        <v>5.4239999999999996E-4</v>
+      </c>
+    </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.45">
       <c r="S12" s="67"/>
       <c r="T12" s="67"/>
@@ -14080,8 +14159,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A13DA696-49DD-4BFA-98FE-5C7770404E50}">
   <dimension ref="B3:L37"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3:L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -14517,6 +14596,7 @@
       <c r="C22" s="66"/>
       <c r="D22" s="66"/>
       <c r="E22" s="66"/>
+      <c r="I22" s="67"/>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.45">
       <c r="B23" s="64"/>

</xml_diff>

<commit_message>
new info in jrp
</commit_message>
<xml_diff>
--- a/web/utilities/records_kriterien.xlsx
+++ b/web/utilities/records_kriterien.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgna\Documents\GitHub\Lifesaving_Baden\web\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57B646E-2661-477F-B272-DB53D473297C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3966BFD-24CD-4B61-A25E-0CBA54ADDAAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="6" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="7" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
   </bookViews>
   <sheets>
     <sheet name="DR" sheetId="9" r:id="rId1"/>
@@ -1388,6 +1388,7 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1397,7 +1398,6 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -8341,38 +8341,38 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A7" s="69" t="s">
+      <c r="A7" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="69"/>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
-      <c r="H7" s="69"/>
-      <c r="I7" s="69"/>
-      <c r="J7" s="69"/>
-      <c r="K7" s="69"/>
-      <c r="L7" s="69"/>
-      <c r="M7" s="69"/>
-      <c r="N7" s="69"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="70"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="70"/>
+      <c r="M7" s="70"/>
+      <c r="N7" s="70"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A8" s="69"/>
-      <c r="B8" s="69"/>
-      <c r="C8" s="69"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="69"/>
-      <c r="G8" s="69"/>
-      <c r="H8" s="69"/>
-      <c r="I8" s="69"/>
-      <c r="J8" s="69"/>
-      <c r="K8" s="69"/>
-      <c r="L8" s="69"/>
-      <c r="M8" s="69"/>
-      <c r="N8" s="69"/>
+      <c r="A8" s="70"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
+      <c r="F8" s="70"/>
+      <c r="G8" s="70"/>
+      <c r="H8" s="70"/>
+      <c r="I8" s="70"/>
+      <c r="J8" s="70"/>
+      <c r="K8" s="70"/>
+      <c r="L8" s="70"/>
+      <c r="M8" s="70"/>
+      <c r="N8" s="70"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" s="20" t="s">
@@ -8537,35 +8537,35 @@
       <c r="N11" s="23"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A14" s="68" t="s">
+      <c r="A14" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="68"/>
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="68"/>
-      <c r="H14" s="70" t="s">
+      <c r="B14" s="69"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
+      <c r="H14" s="71" t="s">
         <v>35</v>
       </c>
-      <c r="I14" s="70"/>
-      <c r="J14" s="70"/>
-      <c r="L14" s="70" t="s">
+      <c r="I14" s="71"/>
+      <c r="J14" s="71"/>
+      <c r="L14" s="71" t="s">
         <v>36</v>
       </c>
       <c r="M14"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A15" s="68"/>
-      <c r="B15" s="68"/>
-      <c r="C15" s="68"/>
-      <c r="D15" s="68"/>
-      <c r="E15" s="68"/>
-      <c r="F15" s="68"/>
-      <c r="H15" s="70"/>
-      <c r="I15" s="70"/>
-      <c r="J15" s="70"/>
-      <c r="L15" s="70"/>
+      <c r="A15" s="69"/>
+      <c r="B15" s="69"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="69"/>
+      <c r="H15" s="71"/>
+      <c r="I15" s="71"/>
+      <c r="J15" s="71"/>
+      <c r="L15" s="71"/>
       <c r="M15"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.45">
@@ -9137,38 +9137,38 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A7" s="69" t="s">
+      <c r="A7" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="69"/>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
-      <c r="H7" s="69"/>
-      <c r="I7" s="69"/>
-      <c r="J7" s="69"/>
-      <c r="K7" s="69"/>
-      <c r="L7" s="69"/>
-      <c r="M7" s="69"/>
-      <c r="N7" s="69"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="70"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="70"/>
+      <c r="M7" s="70"/>
+      <c r="N7" s="70"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A8" s="69"/>
-      <c r="B8" s="69"/>
-      <c r="C8" s="69"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="69"/>
-      <c r="G8" s="69"/>
-      <c r="H8" s="69"/>
-      <c r="I8" s="69"/>
-      <c r="J8" s="69"/>
-      <c r="K8" s="69"/>
-      <c r="L8" s="69"/>
-      <c r="M8" s="69"/>
-      <c r="N8" s="69"/>
+      <c r="A8" s="70"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
+      <c r="F8" s="70"/>
+      <c r="G8" s="70"/>
+      <c r="H8" s="70"/>
+      <c r="I8" s="70"/>
+      <c r="J8" s="70"/>
+      <c r="K8" s="70"/>
+      <c r="L8" s="70"/>
+      <c r="M8" s="70"/>
+      <c r="N8" s="70"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" s="20" t="s">
@@ -9333,35 +9333,35 @@
       <c r="N11" s="23"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A14" s="68" t="s">
+      <c r="A14" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="68"/>
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="68"/>
-      <c r="H14" s="70" t="s">
+      <c r="B14" s="69"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
+      <c r="H14" s="71" t="s">
         <v>35</v>
       </c>
-      <c r="I14" s="70"/>
-      <c r="J14" s="70"/>
-      <c r="L14" s="70" t="s">
+      <c r="I14" s="71"/>
+      <c r="J14" s="71"/>
+      <c r="L14" s="71" t="s">
         <v>36</v>
       </c>
       <c r="M14"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A15" s="68"/>
-      <c r="B15" s="68"/>
-      <c r="C15" s="68"/>
-      <c r="D15" s="68"/>
-      <c r="E15" s="68"/>
-      <c r="F15" s="68"/>
-      <c r="H15" s="70"/>
-      <c r="I15" s="70"/>
-      <c r="J15" s="70"/>
-      <c r="L15" s="70"/>
+      <c r="A15" s="69"/>
+      <c r="B15" s="69"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="69"/>
+      <c r="H15" s="71"/>
+      <c r="I15" s="71"/>
+      <c r="J15" s="71"/>
+      <c r="L15" s="71"/>
       <c r="M15"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.45">
@@ -13323,8 +13323,8 @@
   </sheetPr>
   <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -14081,8 +14081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A13DA696-49DD-4BFA-98FE-5C7770404E50}">
   <dimension ref="B3:Q37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -14150,20 +14150,14 @@
       <c r="K5" s="65">
         <v>4.5300925925925928E-4</v>
       </c>
-      <c r="M5" s="67">
-        <f>I5-J5</f>
-        <v>8.680555555555503E-6</v>
-      </c>
-      <c r="N5" s="67">
-        <f t="shared" ref="N5:N10" si="0">J5-K5</f>
-        <v>9.1435185185185174E-6</v>
-      </c>
-      <c r="P5" s="71">
+      <c r="M5" s="67"/>
+      <c r="N5" s="67"/>
+      <c r="P5" s="68">
         <f>(100-100/I5*J5)</f>
         <v>1.8436578171091327</v>
       </c>
-      <c r="Q5" s="71">
-        <f t="shared" ref="Q5:Q10" si="1">(100-100/J5*K5)</f>
+      <c r="Q5" s="68">
+        <f t="shared" ref="Q5:Q10" si="0">(100-100/J5*K5)</f>
         <v>1.9784623090408218</v>
       </c>
     </row>
@@ -14192,20 +14186,14 @@
       <c r="K6" s="65">
         <v>9.2199074074074069E-4</v>
       </c>
-      <c r="M6" s="67">
-        <f t="shared" ref="M6:M10" si="2">I6-J6</f>
-        <v>1.5277777777777685E-5</v>
-      </c>
-      <c r="N6" s="67">
+      <c r="M6" s="67"/>
+      <c r="N6" s="67"/>
+      <c r="P6" s="68">
+        <f t="shared" ref="P6:P10" si="1">(100-100/I6*J6)</f>
+        <v>1.6017473607571873</v>
+      </c>
+      <c r="Q6" s="68">
         <f t="shared" si="0"/>
-        <v>1.6550925925926043E-5</v>
-      </c>
-      <c r="P6" s="71">
-        <f t="shared" ref="P6:P10" si="3">(100-100/I6*J6)</f>
-        <v>1.6017473607571873</v>
-      </c>
-      <c r="Q6" s="71">
-        <f t="shared" si="1"/>
         <v>1.7634726846713704</v>
       </c>
     </row>
@@ -14234,20 +14222,14 @@
       <c r="K7" s="65">
         <v>6.8171296296296296E-4</v>
       </c>
-      <c r="M7" s="67">
-        <f t="shared" si="2"/>
-        <v>7.1759259259258825E-6</v>
-      </c>
-      <c r="N7" s="67">
+      <c r="M7" s="67"/>
+      <c r="N7" s="67"/>
+      <c r="P7" s="68">
+        <f t="shared" si="1"/>
+        <v>1.0300714404386042</v>
+      </c>
+      <c r="Q7" s="68">
         <f t="shared" si="0"/>
-        <v>7.7546296296296911E-6</v>
-      </c>
-      <c r="P7" s="71">
-        <f t="shared" si="3"/>
-        <v>1.0300714404386042</v>
-      </c>
-      <c r="Q7" s="71">
-        <f t="shared" si="1"/>
         <v>1.1247272116837337</v>
       </c>
     </row>
@@ -14276,20 +14258,14 @@
       <c r="K8" s="65">
         <v>7.571759259259259E-4</v>
       </c>
-      <c r="M8" s="67">
-        <f t="shared" si="2"/>
-        <v>1.018518518518534E-5</v>
-      </c>
-      <c r="N8" s="67">
+      <c r="M8" s="67"/>
+      <c r="N8" s="67"/>
+      <c r="P8" s="68">
+        <f t="shared" si="1"/>
+        <v>1.3083556348498604</v>
+      </c>
+      <c r="Q8" s="68">
         <f t="shared" si="0"/>
-        <v>1.1111111111111044E-5</v>
-      </c>
-      <c r="P8" s="71">
-        <f t="shared" si="3"/>
-        <v>1.3083556348498604</v>
-      </c>
-      <c r="Q8" s="71">
-        <f t="shared" si="1"/>
         <v>1.4462187405844986</v>
       </c>
     </row>
@@ -14318,20 +14294,14 @@
       <c r="K9" s="65">
         <v>1.6210648148148148E-3</v>
       </c>
-      <c r="M9" s="67">
-        <f t="shared" si="2"/>
-        <v>5.6712962962961536E-6</v>
-      </c>
-      <c r="N9" s="67">
+      <c r="M9" s="67"/>
+      <c r="N9" s="67"/>
+      <c r="P9" s="68">
+        <f t="shared" si="1"/>
+        <v>0.3473206691239028</v>
+      </c>
+      <c r="Q9" s="68">
         <f t="shared" si="0"/>
-        <v>6.1342592592593306E-6</v>
-      </c>
-      <c r="P9" s="71">
-        <f t="shared" si="3"/>
-        <v>0.3473206691239028</v>
-      </c>
-      <c r="Q9" s="71">
-        <f t="shared" si="1"/>
         <v>0.37698271569813357</v>
       </c>
     </row>
@@ -14360,20 +14330,14 @@
       <c r="K10" s="65">
         <v>1.784722222222222E-3</v>
       </c>
-      <c r="M10" s="67">
-        <f t="shared" si="2"/>
-        <v>1.2268518518518661E-5</v>
-      </c>
-      <c r="N10" s="67">
+      <c r="M10" s="67"/>
+      <c r="N10" s="67"/>
+      <c r="P10" s="68">
+        <f t="shared" si="1"/>
+        <v>0.67774936061381652</v>
+      </c>
+      <c r="Q10" s="68">
         <f t="shared" si="0"/>
-        <v>1.3194444444444581E-5</v>
-      </c>
-      <c r="P10" s="71">
-        <f t="shared" si="3"/>
-        <v>0.67774936061381652</v>
-      </c>
-      <c r="Q10" s="71">
-        <f t="shared" si="1"/>
         <v>0.73387408265740817</v>
       </c>
     </row>
@@ -14420,11 +14384,11 @@
         <v>4.4861111111111105E-4</v>
       </c>
       <c r="D14" s="65">
-        <f t="shared" ref="D14:E14" si="4">D5*$F14</f>
+        <f t="shared" ref="D14:E14" si="2">D5*$F14</f>
         <v>4.4430555555555553E-4</v>
       </c>
       <c r="E14" s="65">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>4.3944444444444445E-4</v>
       </c>
       <c r="F14">
@@ -14438,11 +14402,11 @@
         <v>5.1791666666666663E-4</v>
       </c>
       <c r="J14" s="65">
-        <f t="shared" ref="J14:K14" si="5">J5*$L14</f>
+        <f t="shared" ref="J14:K14" si="3">J5*$L14</f>
         <v>5.0836805555555563E-4</v>
       </c>
       <c r="K14" s="65">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>4.9831018518518529E-4</v>
       </c>
       <c r="L14">
@@ -14454,15 +14418,15 @@
         <v>225</v>
       </c>
       <c r="C15" s="65">
-        <f t="shared" ref="C15:E15" si="6">C6*$F15</f>
+        <f t="shared" ref="C15:E15" si="4">C6*$F15</f>
         <v>9.7083333333333342E-4</v>
       </c>
       <c r="D15" s="65">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>9.5805555555555553E-4</v>
       </c>
       <c r="E15" s="65">
-        <f t="shared" si="6"/>
+        <f t="shared" si="4"/>
         <v>9.4430555555555544E-4</v>
       </c>
       <c r="F15">
@@ -14472,15 +14436,15 @@
         <v>225</v>
       </c>
       <c r="I15" s="65">
-        <f t="shared" ref="I15:K15" si="7">I6*$L15</f>
+        <f t="shared" ref="I15:K15" si="5">I6*$L15</f>
         <v>1.096892361111111E-3</v>
       </c>
       <c r="J15" s="65">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1.0793229166666666E-3</v>
       </c>
       <c r="K15" s="65">
-        <f t="shared" si="7"/>
+        <f t="shared" si="5"/>
         <v>1.0602893518518518E-3</v>
       </c>
       <c r="L15">
@@ -14492,15 +14456,15 @@
         <v>226</v>
       </c>
       <c r="C16" s="65">
-        <f t="shared" ref="C16:E16" si="8">C7*$F16</f>
+        <f t="shared" ref="C16:E16" si="6">C7*$F16</f>
         <v>7.0833333333333328E-4</v>
       </c>
       <c r="D16" s="65">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>7.0194444444444449E-4</v>
       </c>
       <c r="E16" s="65">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>6.951388888888888E-4</v>
       </c>
       <c r="F16">
@@ -14510,15 +14474,15 @@
         <v>226</v>
       </c>
       <c r="I16" s="65">
-        <f t="shared" ref="I16:K16" si="9">I7*$L16</f>
+        <f t="shared" ref="I16:K16" si="7">I7*$L16</f>
         <v>8.3597222222222222E-4</v>
       </c>
       <c r="J16" s="65">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>8.2736111111111118E-4</v>
       </c>
       <c r="K16" s="65">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>8.1805555555555548E-4</v>
       </c>
       <c r="L16">
@@ -14530,15 +14494,15 @@
         <v>227</v>
       </c>
       <c r="C17" s="65">
-        <f t="shared" ref="C17:E17" si="10">C8*$F17</f>
+        <f t="shared" ref="C17:E17" si="8">C8*$F17</f>
         <v>8.2472222222222224E-4</v>
       </c>
       <c r="D17" s="65">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>8.0902777777777776E-4</v>
       </c>
       <c r="E17" s="65">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>7.919444444444444E-4</v>
       </c>
       <c r="F17">
@@ -14548,15 +14512,15 @@
         <v>227</v>
       </c>
       <c r="I17" s="65">
-        <f t="shared" ref="I17:K17" si="11">I8*$L17</f>
+        <f t="shared" ref="I17:K17" si="9">I8*$L17</f>
         <v>8.9524305555555559E-4</v>
       </c>
       <c r="J17" s="65">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>8.8353009259259244E-4</v>
       </c>
       <c r="K17" s="65">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>8.7075231481481476E-4</v>
       </c>
       <c r="L17">
@@ -14568,15 +14532,15 @@
         <v>228</v>
       </c>
       <c r="C18" s="65">
-        <f t="shared" ref="C18:E18" si="12">C9*$F18</f>
+        <f t="shared" ref="C18:E18" si="10">C9*$F18</f>
         <v>1.7556134259259259E-3</v>
       </c>
       <c r="D18" s="65">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>1.7369791666666664E-3</v>
       </c>
       <c r="E18" s="65">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>1.7167476851851849E-3</v>
       </c>
       <c r="F18">
@@ -14586,15 +14550,15 @@
         <v>228</v>
       </c>
       <c r="I18" s="65">
-        <f t="shared" ref="I18:K18" si="13">I9*$L18</f>
+        <f t="shared" ref="I18:K18" si="11">I9*$L18</f>
         <v>1.9186226851851851E-3</v>
       </c>
       <c r="J18" s="65">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>1.9119589120370371E-3</v>
       </c>
       <c r="K18" s="65">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>1.9047511574074075E-3</v>
       </c>
       <c r="L18">
@@ -14606,15 +14570,15 @@
         <v>4</v>
       </c>
       <c r="C19" s="65">
-        <f t="shared" ref="C19:E19" si="14">C10*$F19</f>
+        <f t="shared" ref="C19:E19" si="12">C10*$F19</f>
         <v>1.9191956018518516E-3</v>
       </c>
       <c r="D19" s="65">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>1.8985648148148143E-3</v>
       </c>
       <c r="E19" s="65">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>1.8763368055555554E-3</v>
       </c>
       <c r="F19">
@@ -14624,15 +14588,15 @@
         <v>4</v>
       </c>
       <c r="I19" s="65">
-        <f t="shared" ref="I19:K19" si="15">I10*$L19</f>
+        <f t="shared" ref="I19:K19" si="13">I10*$L19</f>
         <v>2.0636111111111111E-3</v>
       </c>
       <c r="J19" s="65">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>2.0496249999999998E-3</v>
       </c>
       <c r="K19" s="65">
-        <f t="shared" si="15"/>
+        <f t="shared" si="13"/>
         <v>2.0345833333333331E-3</v>
       </c>
       <c r="L19">
@@ -14961,38 +14925,38 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A7" s="69" t="s">
+      <c r="A7" s="70" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="69"/>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
-      <c r="H7" s="69"/>
-      <c r="I7" s="69"/>
-      <c r="J7" s="69"/>
-      <c r="K7" s="69"/>
-      <c r="L7" s="69"/>
-      <c r="M7" s="69"/>
-      <c r="N7" s="69"/>
+      <c r="B7" s="70"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="70"/>
+      <c r="H7" s="70"/>
+      <c r="I7" s="70"/>
+      <c r="J7" s="70"/>
+      <c r="K7" s="70"/>
+      <c r="L7" s="70"/>
+      <c r="M7" s="70"/>
+      <c r="N7" s="70"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A8" s="69"/>
-      <c r="B8" s="69"/>
-      <c r="C8" s="69"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="69"/>
-      <c r="G8" s="69"/>
-      <c r="H8" s="69"/>
-      <c r="I8" s="69"/>
-      <c r="J8" s="69"/>
-      <c r="K8" s="69"/>
-      <c r="L8" s="69"/>
-      <c r="M8" s="69"/>
-      <c r="N8" s="69"/>
+      <c r="A8" s="70"/>
+      <c r="B8" s="70"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="70"/>
+      <c r="E8" s="70"/>
+      <c r="F8" s="70"/>
+      <c r="G8" s="70"/>
+      <c r="H8" s="70"/>
+      <c r="I8" s="70"/>
+      <c r="J8" s="70"/>
+      <c r="K8" s="70"/>
+      <c r="L8" s="70"/>
+      <c r="M8" s="70"/>
+      <c r="N8" s="70"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" s="20" t="s">
@@ -15157,38 +15121,38 @@
       <c r="N11" s="23"/>
     </row>
     <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="68" t="s">
+      <c r="A14" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="68"/>
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="68"/>
+      <c r="B14" s="69"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
       <c r="G14"/>
-      <c r="H14" s="70" t="s">
+      <c r="H14" s="71" t="s">
         <v>35</v>
       </c>
-      <c r="I14" s="70"/>
-      <c r="J14" s="70"/>
-      <c r="L14" s="70" t="s">
+      <c r="I14" s="71"/>
+      <c r="J14" s="71"/>
+      <c r="L14" s="71" t="s">
         <v>36</v>
       </c>
       <c r="M14"/>
       <c r="N14"/>
     </row>
     <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="68"/>
-      <c r="B15" s="68"/>
-      <c r="C15" s="68"/>
-      <c r="D15" s="68"/>
-      <c r="E15" s="68"/>
-      <c r="F15" s="68"/>
+      <c r="A15" s="69"/>
+      <c r="B15" s="69"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="69"/>
       <c r="G15"/>
-      <c r="H15" s="70"/>
-      <c r="I15" s="70"/>
-      <c r="J15" s="70"/>
-      <c r="L15" s="70"/>
+      <c r="H15" s="71"/>
+      <c r="I15" s="71"/>
+      <c r="J15" s="71"/>
+      <c r="L15" s="71"/>
       <c r="M15"/>
       <c r="N15"/>
     </row>

</xml_diff>

<commit_message>
test 25m krit change
</commit_message>
<xml_diff>
--- a/web/utilities/records_kriterien.xlsx
+++ b/web/utilities/records_kriterien.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgna\Documents\GitHub\Lifesaving_Baden\web\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3966BFD-24CD-4B61-A25E-0CBA54ADDAAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{012F10C0-542A-4A80-93AE-E17DA9C4FD8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="7" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="6" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
   </bookViews>
   <sheets>
     <sheet name="DR" sheetId="9" r:id="rId1"/>
@@ -220,7 +220,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="236">
   <si>
     <t>50m Retten</t>
   </si>
@@ -925,6 +925,9 @@
   </si>
   <si>
     <t>NK2-W (10-20%) ind</t>
+  </si>
+  <si>
+    <t>Test</t>
   </si>
 </sst>
 </file>
@@ -4055,8 +4058,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}" name="JRP_konfig" displayName="JRP_konfig" ref="A1:X9" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
-  <autoFilter ref="A1:X9" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}" name="JRP_konfig" displayName="JRP_konfig" ref="A1:X11" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+  <autoFilter ref="A1:X11" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -13321,10 +13324,10 @@
   <sheetPr codeName="Tabelle10">
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:X10"/>
+  <dimension ref="A1:X11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -14062,12 +14065,148 @@
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="S10" s="67"/>
-      <c r="T10" s="67"/>
-      <c r="U10" s="67"/>
-      <c r="V10" s="67"/>
-      <c r="W10" s="67"/>
-      <c r="X10" s="67"/>
+      <c r="A10" s="59" t="s">
+        <v>235</v>
+      </c>
+      <c r="B10" s="59" t="s">
+        <v>164</v>
+      </c>
+      <c r="C10" s="59">
+        <v>15</v>
+      </c>
+      <c r="D10" s="59">
+        <v>18</v>
+      </c>
+      <c r="E10" s="61">
+        <v>45658</v>
+      </c>
+      <c r="F10" s="61">
+        <v>46174</v>
+      </c>
+      <c r="G10" s="61">
+        <v>45658</v>
+      </c>
+      <c r="H10" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="I10" s="59" t="s">
+        <v>179</v>
+      </c>
+      <c r="J10" s="59">
+        <v>25</v>
+      </c>
+      <c r="K10" s="59"/>
+      <c r="L10" s="59">
+        <v>10</v>
+      </c>
+      <c r="M10" s="62">
+        <v>4.6817129629629634E-4</v>
+      </c>
+      <c r="N10" s="62">
+        <v>7.4872685185185188E-4</v>
+      </c>
+      <c r="O10" s="62">
+        <v>9.9224537037037033E-4</v>
+      </c>
+      <c r="P10" s="62">
+        <v>7.8888888888888889E-4</v>
+      </c>
+      <c r="Q10" s="62">
+        <v>1.9605324074074074E-3</v>
+      </c>
+      <c r="R10" s="62">
+        <v>1.7837962962962963E-3</v>
+      </c>
+      <c r="S10" s="62">
+        <v>4.803240740740741E-4</v>
+      </c>
+      <c r="T10" s="62">
+        <v>7.8599537037037039E-4</v>
+      </c>
+      <c r="U10" s="62">
+        <v>1.0240740740740742E-3</v>
+      </c>
+      <c r="V10" s="62">
+        <v>8.2766203703703712E-4</v>
+      </c>
+      <c r="W10" s="62">
+        <v>2.0114583333333334E-3</v>
+      </c>
+      <c r="X10" s="62">
+        <v>1.8332175925925925E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A11" s="59" t="s">
+        <v>235</v>
+      </c>
+      <c r="B11" s="59" t="s">
+        <v>164</v>
+      </c>
+      <c r="C11" s="59">
+        <v>15</v>
+      </c>
+      <c r="D11" s="59">
+        <v>18</v>
+      </c>
+      <c r="E11" s="61">
+        <v>45658</v>
+      </c>
+      <c r="F11" s="61">
+        <v>46174</v>
+      </c>
+      <c r="G11" s="61">
+        <v>45658</v>
+      </c>
+      <c r="H11" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="I11" s="59" t="s">
+        <v>179</v>
+      </c>
+      <c r="J11" s="59">
+        <v>50</v>
+      </c>
+      <c r="K11" s="59"/>
+      <c r="L11" s="59">
+        <v>10</v>
+      </c>
+      <c r="M11" s="62">
+        <v>4.6817129629629634E-4</v>
+      </c>
+      <c r="N11" s="62">
+        <v>7.4872685185185188E-4</v>
+      </c>
+      <c r="O11" s="62">
+        <v>9.9224537037037033E-4</v>
+      </c>
+      <c r="P11" s="62">
+        <v>7.8888888888888889E-4</v>
+      </c>
+      <c r="Q11" s="62">
+        <v>1.9605324074074074E-3</v>
+      </c>
+      <c r="R11" s="62">
+        <v>1.7837962962962963E-3</v>
+      </c>
+      <c r="S11" s="62">
+        <v>4.803240740740741E-4</v>
+      </c>
+      <c r="T11" s="62">
+        <v>7.8599537037037039E-4</v>
+      </c>
+      <c r="U11" s="62">
+        <v>1.0240740740740742E-3</v>
+      </c>
+      <c r="V11" s="62">
+        <v>8.2766203703703712E-4</v>
+      </c>
+      <c r="W11" s="62">
+        <v>2.0114583333333334E-3</v>
+      </c>
+      <c r="X11" s="62">
+        <v>1.8332175925925925E-3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -14081,7 +14220,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A13DA696-49DD-4BFA-98FE-5C7770404E50}">
   <dimension ref="B3:Q37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
test mit dif times
</commit_message>
<xml_diff>
--- a/web/utilities/records_kriterien.xlsx
+++ b/web/utilities/records_kriterien.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgna\Documents\GitHub\Lifesaving_Baden\web\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{012F10C0-542A-4A80-93AE-E17DA9C4FD8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F9E0A7-5753-489A-9E7E-64EB47C46DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="6" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
   </bookViews>
@@ -13326,8 +13326,8 @@
   </sheetPr>
   <dimension ref="A1:X11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -14172,40 +14172,52 @@
         <v>10</v>
       </c>
       <c r="M11" s="62">
-        <v>4.6817129629629634E-4</v>
+        <f>M10*1.1</f>
+        <v>5.1498842592592601E-4</v>
       </c>
       <c r="N11" s="62">
-        <v>7.4872685185185188E-4</v>
+        <f t="shared" ref="N11:X11" si="6">N10*1.1</f>
+        <v>8.2359953703703718E-4</v>
       </c>
       <c r="O11" s="62">
-        <v>9.9224537037037033E-4</v>
+        <f t="shared" si="6"/>
+        <v>1.0914699074074075E-3</v>
       </c>
       <c r="P11" s="62">
-        <v>7.8888888888888889E-4</v>
+        <f t="shared" si="6"/>
+        <v>8.6777777777777786E-4</v>
       </c>
       <c r="Q11" s="62">
-        <v>1.9605324074074074E-3</v>
+        <f t="shared" si="6"/>
+        <v>2.1565856481481484E-3</v>
       </c>
       <c r="R11" s="62">
-        <v>1.7837962962962963E-3</v>
+        <f t="shared" si="6"/>
+        <v>1.9621759259259262E-3</v>
       </c>
       <c r="S11" s="62">
-        <v>4.803240740740741E-4</v>
+        <f t="shared" si="6"/>
+        <v>5.2835648148148154E-4</v>
       </c>
       <c r="T11" s="62">
-        <v>7.8599537037037039E-4</v>
+        <f t="shared" si="6"/>
+        <v>8.6459490740740746E-4</v>
       </c>
       <c r="U11" s="62">
-        <v>1.0240740740740742E-3</v>
+        <f t="shared" si="6"/>
+        <v>1.1264814814814818E-3</v>
       </c>
       <c r="V11" s="62">
-        <v>8.2766203703703712E-4</v>
+        <f t="shared" si="6"/>
+        <v>9.1042824074074095E-4</v>
       </c>
       <c r="W11" s="62">
-        <v>2.0114583333333334E-3</v>
+        <f t="shared" si="6"/>
+        <v>2.212604166666667E-3</v>
       </c>
       <c r="X11" s="62">
-        <v>1.8332175925925925E-3</v>
+        <f t="shared" si="6"/>
+        <v>2.0165393518518518E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Meta in Tab PZ infos JRP
</commit_message>
<xml_diff>
--- a/web/utilities/records_kriterien.xlsx
+++ b/web/utilities/records_kriterien.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgna\Documents\GitHub\Lifesaving_Baden\web\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01F9E0A7-5753-489A-9E7E-64EB47C46DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92797006-DE96-4DF3-8B23-046C06D3DF36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="6" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
   </bookViews>
@@ -4058,8 +4058,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}" name="JRP_konfig" displayName="JRP_konfig" ref="A1:X11" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
-  <autoFilter ref="A1:X11" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}" name="JRP_konfig" displayName="JRP_konfig" ref="A1:X12" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
+  <autoFilter ref="A1:X12" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -13324,10 +13324,10 @@
   <sheetPr codeName="Tabelle10">
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:X11"/>
+  <dimension ref="A1:X12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -14220,6 +14220,32 @@
         <v>2.0165393518518518E-3</v>
       </c>
     </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A12" s="59"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="61"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="59"/>
+      <c r="J12" s="59"/>
+      <c r="K12" s="59"/>
+      <c r="L12" s="59"/>
+      <c r="M12" s="62"/>
+      <c r="N12" s="62"/>
+      <c r="O12" s="62"/>
+      <c r="P12" s="62"/>
+      <c r="Q12" s="62"/>
+      <c r="R12" s="62"/>
+      <c r="S12" s="62"/>
+      <c r="T12" s="62"/>
+      <c r="U12" s="62"/>
+      <c r="V12" s="62"/>
+      <c r="W12" s="62"/>
+      <c r="X12" s="62"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -14233,7 +14259,7 @@
   <dimension ref="B3:Q37"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
bis 6 / 10 nominiert
</commit_message>
<xml_diff>
--- a/web/utilities/records_kriterien.xlsx
+++ b/web/utilities/records_kriterien.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgna\Documents\GitHub\Lifesaving_Baden\web\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39D0693-B613-44E4-AABF-3CD019BF5876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D29FB73-FBD6-4160-A66B-5422857C127C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="6" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
   </bookViews>
@@ -220,7 +220,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1114" uniqueCount="275">
   <si>
     <t>50m Retten</t>
   </si>
@@ -1035,10 +1035,16 @@
     <t>NK1 +27,5% Frauen</t>
   </si>
   <si>
-    <t>NK1 +30% Mäner</t>
+    <t>NK1 +13% Mäner (bis 10 nominiert)</t>
   </si>
   <si>
-    <t>NK1 +30% Frauen</t>
+    <t>NK1 +18% Frauen (bis 10 nominiert)</t>
+  </si>
+  <si>
+    <t>NK2 +30% Mäner  (bis 6 nominiert)</t>
+  </si>
+  <si>
+    <t>NK2 +30% Frauen  (bis 6 nominiert)</t>
   </si>
 </sst>
 </file>
@@ -1521,96 +1527,6 @@
   </cellStyles>
   <dxfs count="194">
     <dxf>
-      <font>
-        <color theme="6"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="164" formatCode="m:ss.00"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1702,6 +1618,96 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4"/>
+      </font>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="m:ss.00"/>
@@ -4002,10 +4008,10 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>JRP!$M$2:$M$105</c:f>
+              <c:f>JRP!$M$2:$M$109</c:f>
               <c:numCache>
                 <c:formatCode>m:ss.00</c:formatCode>
-                <c:ptCount val="104"/>
+                <c:ptCount val="108"/>
                 <c:pt idx="0">
                   <c:v>4.6817129629629634E-4</c:v>
                 </c:pt>
@@ -4103,22 +4109,22 @@
                   <c:v>5.7677083333333332E-4</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4.5775462962962962E-4</c:v>
+                  <c:v>4.5043055555555553E-4</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>4.6281828703703703E-4</c:v>
+                  <c:v>4.5541319444444443E-4</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>4.6730324074074068E-4</c:v>
+                  <c:v>4.5982638888888885E-4</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>5.6626157407407406E-4</c:v>
+                  <c:v>5.3455092592592595E-4</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>5.7769097222222228E-4</c:v>
+                  <c:v>5.4534027777777773E-4</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>5.8854166666666668E-4</c:v>
+                  <c:v>5.5558333333333328E-4</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>4.6690972222222218E-4</c:v>
@@ -4301,22 +4307,34 @@
                   <c:v>5.2475694444444445E-4</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>4.6944444444444442E-4</c:v>
+                  <c:v>4.0805555555555549E-4</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>4.6523148148148151E-4</c:v>
+                  <c:v>4.043935185185185E-4</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>4.5244212962962968E-4</c:v>
+                  <c:v>3.9327662037037033E-4</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>5.73263888888889E-4</c:v>
+                  <c:v>5.2034722222222228E-4</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>5.6393518518518522E-4</c:v>
+                  <c:v>5.118796296296296E-4</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>5.3504629629629627E-4</c:v>
+                  <c:v>4.8565740740740736E-4</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>4.5043055555555553E-4</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>4.5541319444444443E-4</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>4.5982638888888885E-4</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>5.3455092592592595E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4355,10 +4373,10 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>JRP!$N$2:$N$105</c:f>
+              <c:f>JRP!$N$2:$N$109</c:f>
               <c:numCache>
                 <c:formatCode>m:ss.00</c:formatCode>
-                <c:ptCount val="104"/>
+                <c:ptCount val="108"/>
                 <c:pt idx="0">
                   <c:v>7.4872685185185188E-4</c:v>
                 </c:pt>
@@ -4456,22 +4474,22 @@
                   <c:v>8.5338831018518522E-4</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>7.2410300925925919E-4</c:v>
+                  <c:v>7.1251736111111103E-4</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>7.311921296296297E-4</c:v>
+                  <c:v>7.1949305555555558E-4</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>7.378472222222222E-4</c:v>
+                  <c:v>7.2604166666666661E-4</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>8.521412037037037E-4</c:v>
+                  <c:v>8.0442129629629624E-4</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>8.6183449074074081E-4</c:v>
+                  <c:v>8.1357175925925933E-4</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>8.7080439814814811E-4</c:v>
+                  <c:v>8.2203935185185179E-4</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>7.3858506944444438E-4</c:v>
@@ -4654,22 +4672,34 @@
                   <c:v>8.2373263888888882E-4</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>7.4328703703703709E-4</c:v>
+                  <c:v>6.4608796296296289E-4</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>7.3726851851851861E-4</c:v>
+                  <c:v>6.4085648148148151E-4</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>7.1846064814814819E-4</c:v>
+                  <c:v>6.2450810185185179E-4</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>8.7313657407407414E-4</c:v>
+                  <c:v>7.9253935185185189E-4</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>8.6501157407407403E-4</c:v>
+                  <c:v>7.8516435185185178E-4</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>8.3988425925925929E-4</c:v>
+                  <c:v>7.6235648148148148E-4</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>7.1251736111111103E-4</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>7.1949305555555558E-4</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>7.2604166666666661E-4</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>8.0442129629629624E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4708,10 +4738,10 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>JRP!$O$2:$O$105</c:f>
+              <c:f>JRP!$O$2:$O$109</c:f>
               <c:numCache>
                 <c:formatCode>m:ss.00</c:formatCode>
-                <c:ptCount val="104"/>
+                <c:ptCount val="108"/>
                 <c:pt idx="0">
                   <c:v>9.9224537037037033E-4</c:v>
                 </c:pt>
@@ -4809,22 +4839,22 @@
                   <c:v>1.1684288194444446E-3</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>9.8365162037037019E-4</c:v>
+                  <c:v>9.6791319444444431E-4</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>9.9797453703703702E-4</c:v>
+                  <c:v>9.8200694444444442E-4</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.0112847222222224E-3</c:v>
+                  <c:v>9.9510416666666671E-4</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1.1524884259259259E-3</c:v>
+                  <c:v>1.0879490740740739E-3</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.1731770833333334E-3</c:v>
+                  <c:v>1.1074791666666668E-3</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1.1922743055555556E-3</c:v>
+                  <c:v>1.1255069444444444E-3</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>1.0033246527777777E-3</c:v>
@@ -5007,22 +5037,34 @@
                   <c:v>1.0799131944444445E-3</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>1.0034375E-3</c:v>
+                  <c:v>8.7221874999999995E-4</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>9.9155092592592611E-4</c:v>
+                  <c:v>8.6188657407407405E-4</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>9.5453703703703705E-4</c:v>
+                  <c:v>8.2971296296296287E-4</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>1.1704513888888888E-3</c:v>
+                  <c:v>1.062409722222222E-3</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>1.1534490740740741E-3</c:v>
+                  <c:v>1.0469768518518517E-3</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>1.101087962962963E-3</c:v>
+                  <c:v>9.9944907407407404E-4</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>9.6791319444444431E-4</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>9.8200694444444442E-4</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>9.9510416666666671E-4</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>1.0879490740740739E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5061,10 +5103,10 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>JRP!$P$2:$P$105</c:f>
+              <c:f>JRP!$P$2:$P$109</c:f>
               <c:numCache>
                 <c:formatCode>m:ss.00</c:formatCode>
-                <c:ptCount val="104"/>
+                <c:ptCount val="108"/>
                 <c:pt idx="0">
                   <c:v>7.8888888888888889E-4</c:v>
                 </c:pt>
@@ -5162,22 +5204,22 @@
                   <c:v>9.5362847222222236E-4</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>8.2494212962962968E-4</c:v>
+                  <c:v>8.1174305555555557E-4</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>8.427372685185186E-4</c:v>
+                  <c:v>8.2925347222222222E-4</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>8.5908564814814821E-4</c:v>
+                  <c:v>8.4534027777777786E-4</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>9.4646990740740737E-4</c:v>
+                  <c:v>8.9346759259259251E-4</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>9.6035879629629618E-4</c:v>
+                  <c:v>9.065787037037035E-4</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>9.730902777777778E-4</c:v>
+                  <c:v>9.1859722222222223E-4</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>8.4144097222222216E-4</c:v>
@@ -5360,22 +5402,34 @@
                   <c:v>9.0046875000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>8.3371527777777773E-4</c:v>
+                  <c:v>7.2469097222222206E-4</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>8.1927083333333331E-4</c:v>
+                  <c:v>7.1213541666666658E-4</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>7.7473379629629626E-4</c:v>
+                  <c:v>6.7342245370370364E-4</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>9.6537037037037034E-4</c:v>
+                  <c:v>8.7625925925925914E-4</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>9.5378472222222229E-4</c:v>
+                  <c:v>8.6574305555555547E-4</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>9.181250000000001E-4</c:v>
+                  <c:v>8.3337500000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>8.1174305555555557E-4</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>8.2925347222222222E-4</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>8.4534027777777786E-4</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>8.9346759259259251E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5414,10 +5468,10 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>JRP!$Q$2:$Q$105</c:f>
+              <c:f>JRP!$Q$2:$Q$109</c:f>
               <c:numCache>
                 <c:formatCode>m:ss.00</c:formatCode>
-                <c:ptCount val="104"/>
+                <c:ptCount val="108"/>
                 <c:pt idx="0">
                   <c:v>1.9605324074074074E-3</c:v>
                 </c:pt>
@@ -5515,22 +5569,22 @@
                   <c:v>2.217476851851852E-3</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.0394965277777777E-3</c:v>
+                  <c:v>2.0068645833333332E-3</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.0636574074074073E-3</c:v>
+                  <c:v>2.0306388888888887E-3</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.0860821759259261E-3</c:v>
+                  <c:v>2.052704861111111E-3</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.2309027777777774E-3</c:v>
+                  <c:v>2.1059722222222218E-3</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2.2473958333333335E-3</c:v>
+                  <c:v>2.1215416666666665E-3</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2.2627314814814815E-3</c:v>
+                  <c:v>2.1360185185185184E-3</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>2.0802864583333333E-3</c:v>
@@ -5713,22 +5767,34 @@
                   <c:v>2.1965711805555553E-3</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>2.0881250000000001E-3</c:v>
+                  <c:v>1.8150624999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>2.0678125000000002E-3</c:v>
+                  <c:v>1.79740625E-3</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>2.0049189814814817E-3</c:v>
+                  <c:v>1.7427372685185185E-3</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>2.2975694444444445E-3</c:v>
+                  <c:v>2.0854861111111109E-3</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>2.2834259259259262E-3</c:v>
+                  <c:v>2.0726481481481481E-3</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>2.2396412037037038E-3</c:v>
+                  <c:v>2.0329050925925922E-3</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>2.0068645833333332E-3</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>2.0306388888888887E-3</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>2.052704861111111E-3</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>2.1059722222222218E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5767,10 +5833,10 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>JRP!$R$2:$R$105</c:f>
+              <c:f>JRP!$R$2:$R$109</c:f>
               <c:numCache>
                 <c:formatCode>m:ss.00</c:formatCode>
-                <c:ptCount val="104"/>
+                <c:ptCount val="108"/>
                 <c:pt idx="0">
                   <c:v>1.7837962962962963E-3</c:v>
                 </c:pt>
@@ -5868,22 +5934,22 @@
                   <c:v>2.0002662037037038E-3</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.8660300925925923E-3</c:v>
+                  <c:v>1.8361736111111109E-3</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1.8880208333333333E-3</c:v>
+                  <c:v>1.8578124999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.9082754629629632E-3</c:v>
+                  <c:v>1.8777430555555557E-3</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.0263310185185185E-3</c:v>
+                  <c:v>1.9128564814814813E-3</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2.0339988425925925E-3</c:v>
+                  <c:v>1.9200949074074073E-3</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2.0410879629629629E-3</c:v>
+                  <c:v>1.9267870370370367E-3</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>1.9033506944444441E-3</c:v>
@@ -6066,22 +6132,34 @@
                   <c:v>2.0296701388888886E-3</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>1.9107291666666667E-3</c:v>
+                  <c:v>1.660864583333333E-3</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>1.8922222222222224E-3</c:v>
+                  <c:v>1.6447777777777778E-3</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>1.8350462962962962E-3</c:v>
+                  <c:v>1.5950787037037034E-3</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>2.0968518518518523E-3</c:v>
+                  <c:v>1.9032962962962964E-3</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>2.090231481481482E-3</c:v>
+                  <c:v>1.8972870370370372E-3</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>2.0694675925925924E-3</c:v>
+                  <c:v>1.8784398148148146E-3</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>1.8361736111111109E-3</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>1.8578124999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>1.8777430555555557E-3</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>1.9128564814814813E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6124,10 +6202,10 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>JRP!$S$2:$S$105</c:f>
+              <c:f>JRP!$S$2:$S$109</c:f>
               <c:numCache>
                 <c:formatCode>m:ss.00</c:formatCode>
-                <c:ptCount val="104"/>
+                <c:ptCount val="108"/>
                 <c:pt idx="0">
                   <c:v>4.803240740740741E-4</c:v>
                 </c:pt>
@@ -6225,22 +6303,22 @@
                   <c:v>5.7677083333333332E-4</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>4.5775462962962962E-4</c:v>
+                  <c:v>4.5043055555555553E-4</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>4.6281828703703703E-4</c:v>
+                  <c:v>4.5541319444444443E-4</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>4.6730324074074068E-4</c:v>
+                  <c:v>4.5982638888888885E-4</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>5.6626157407407406E-4</c:v>
+                  <c:v>5.3455092592592595E-4</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>5.7769097222222228E-4</c:v>
+                  <c:v>5.4534027777777773E-4</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>5.8854166666666668E-4</c:v>
+                  <c:v>5.5558333333333328E-4</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>4.6690972222222218E-4</c:v>
@@ -6423,22 +6501,34 @@
                   <c:v>5.2475694444444445E-4</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>4.6944444444444442E-4</c:v>
+                  <c:v>4.0805555555555549E-4</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>4.6523148148148151E-4</c:v>
+                  <c:v>4.043935185185185E-4</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>4.5244212962962968E-4</c:v>
+                  <c:v>3.9327662037037033E-4</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>5.73263888888889E-4</c:v>
+                  <c:v>5.2034722222222228E-4</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>5.6393518518518522E-4</c:v>
+                  <c:v>5.118796296296296E-4</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>5.3504629629629627E-4</c:v>
+                  <c:v>4.8565740740740736E-4</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>4.5043055555555553E-4</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>4.5541319444444443E-4</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>4.5982638888888885E-4</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>5.3455092592592595E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6481,10 +6571,10 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>JRP!$T$2:$T$105</c:f>
+              <c:f>JRP!$T$2:$T$109</c:f>
               <c:numCache>
                 <c:formatCode>m:ss.00</c:formatCode>
-                <c:ptCount val="104"/>
+                <c:ptCount val="108"/>
                 <c:pt idx="0">
                   <c:v>7.8599537037037039E-4</c:v>
                 </c:pt>
@@ -6582,22 +6672,22 @@
                   <c:v>8.5338831018518522E-4</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>7.2410300925925919E-4</c:v>
+                  <c:v>7.1251736111111103E-4</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>7.311921296296297E-4</c:v>
+                  <c:v>7.1949305555555558E-4</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>7.378472222222222E-4</c:v>
+                  <c:v>7.2604166666666661E-4</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>8.521412037037037E-4</c:v>
+                  <c:v>8.0442129629629624E-4</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>8.6183449074074081E-4</c:v>
+                  <c:v>8.1357175925925933E-4</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>8.7080439814814811E-4</c:v>
+                  <c:v>8.2203935185185179E-4</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>7.3858506944444438E-4</c:v>
@@ -6780,22 +6870,34 @@
                   <c:v>8.2373263888888882E-4</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>7.4328703703703709E-4</c:v>
+                  <c:v>6.4608796296296289E-4</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>7.3726851851851861E-4</c:v>
+                  <c:v>6.4085648148148151E-4</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>7.1846064814814819E-4</c:v>
+                  <c:v>6.2450810185185179E-4</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>8.7313657407407414E-4</c:v>
+                  <c:v>7.9253935185185189E-4</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>8.6501157407407403E-4</c:v>
+                  <c:v>7.8516435185185178E-4</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>8.3988425925925929E-4</c:v>
+                  <c:v>7.6235648148148148E-4</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>7.1251736111111103E-4</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>7.1949305555555558E-4</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>7.2604166666666661E-4</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>8.0442129629629624E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6838,10 +6940,10 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>JRP!$U$2:$U$105</c:f>
+              <c:f>JRP!$U$2:$U$109</c:f>
               <c:numCache>
                 <c:formatCode>m:ss.00</c:formatCode>
-                <c:ptCount val="104"/>
+                <c:ptCount val="108"/>
                 <c:pt idx="0">
                   <c:v>1.0240740740740742E-3</c:v>
                 </c:pt>
@@ -6939,22 +7041,22 @@
                   <c:v>1.1684288194444446E-3</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>9.8365162037037019E-4</c:v>
+                  <c:v>9.6791319444444431E-4</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>9.9797453703703702E-4</c:v>
+                  <c:v>9.8200694444444442E-4</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.0112847222222224E-3</c:v>
+                  <c:v>9.9510416666666671E-4</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1.1524884259259259E-3</c:v>
+                  <c:v>1.0879490740740739E-3</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>1.1731770833333334E-3</c:v>
+                  <c:v>1.1074791666666668E-3</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>1.1922743055555556E-3</c:v>
+                  <c:v>1.1255069444444444E-3</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>1.0033246527777777E-3</c:v>
@@ -7137,22 +7239,34 @@
                   <c:v>1.0799131944444445E-3</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>1.0034375E-3</c:v>
+                  <c:v>8.7221874999999995E-4</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>9.9155092592592611E-4</c:v>
+                  <c:v>8.6188657407407405E-4</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>9.5453703703703705E-4</c:v>
+                  <c:v>8.2971296296296287E-4</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>1.1704513888888888E-3</c:v>
+                  <c:v>1.062409722222222E-3</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>1.1534490740740741E-3</c:v>
+                  <c:v>1.0469768518518517E-3</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>1.101087962962963E-3</c:v>
+                  <c:v>9.9944907407407404E-4</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>9.6791319444444431E-4</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>9.8200694444444442E-4</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>9.9510416666666671E-4</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>1.0879490740740739E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7195,10 +7309,10 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>JRP!$V$2:$V$105</c:f>
+              <c:f>JRP!$V$2:$V$109</c:f>
               <c:numCache>
                 <c:formatCode>m:ss.00</c:formatCode>
-                <c:ptCount val="104"/>
+                <c:ptCount val="108"/>
                 <c:pt idx="0">
                   <c:v>8.2766203703703712E-4</c:v>
                 </c:pt>
@@ -7296,22 +7410,22 @@
                   <c:v>9.5362847222222236E-4</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>8.2494212962962968E-4</c:v>
+                  <c:v>8.1174305555555557E-4</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>8.427372685185186E-4</c:v>
+                  <c:v>8.2925347222222222E-4</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>8.5908564814814821E-4</c:v>
+                  <c:v>8.4534027777777786E-4</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>9.4646990740740737E-4</c:v>
+                  <c:v>8.9346759259259251E-4</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>9.6035879629629618E-4</c:v>
+                  <c:v>9.065787037037035E-4</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>9.730902777777778E-4</c:v>
+                  <c:v>9.1859722222222223E-4</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>8.4144097222222216E-4</c:v>
@@ -7494,22 +7608,34 @@
                   <c:v>9.0046875000000001E-4</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>8.3371527777777773E-4</c:v>
+                  <c:v>7.2469097222222206E-4</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>8.1927083333333331E-4</c:v>
+                  <c:v>7.1213541666666658E-4</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>7.7473379629629626E-4</c:v>
+                  <c:v>6.7342245370370364E-4</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>9.6537037037037034E-4</c:v>
+                  <c:v>8.7625925925925914E-4</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>9.5378472222222229E-4</c:v>
+                  <c:v>8.6574305555555547E-4</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>9.181250000000001E-4</c:v>
+                  <c:v>8.3337500000000002E-4</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>8.1174305555555557E-4</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>8.2925347222222222E-4</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>8.4534027777777786E-4</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>8.9346759259259251E-4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7552,10 +7678,10 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>JRP!$W$2:$W$105</c:f>
+              <c:f>JRP!$W$2:$W$109</c:f>
               <c:numCache>
                 <c:formatCode>m:ss.00</c:formatCode>
-                <c:ptCount val="104"/>
+                <c:ptCount val="108"/>
                 <c:pt idx="0">
                   <c:v>2.0114583333333334E-3</c:v>
                 </c:pt>
@@ -7653,22 +7779,22 @@
                   <c:v>2.217476851851852E-3</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.0394965277777777E-3</c:v>
+                  <c:v>2.0068645833333332E-3</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.0636574074074073E-3</c:v>
+                  <c:v>2.0306388888888887E-3</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.0860821759259261E-3</c:v>
+                  <c:v>2.052704861111111E-3</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.2309027777777774E-3</c:v>
+                  <c:v>2.1059722222222218E-3</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2.2473958333333335E-3</c:v>
+                  <c:v>2.1215416666666665E-3</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2.2627314814814815E-3</c:v>
+                  <c:v>2.1360185185185184E-3</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>2.0802864583333333E-3</c:v>
@@ -7851,22 +7977,34 @@
                   <c:v>2.1965711805555553E-3</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>2.0881250000000001E-3</c:v>
+                  <c:v>1.8150624999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>2.0678125000000002E-3</c:v>
+                  <c:v>1.79740625E-3</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>2.0049189814814817E-3</c:v>
+                  <c:v>1.7427372685185185E-3</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>2.2975694444444445E-3</c:v>
+                  <c:v>2.0854861111111109E-3</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>2.2834259259259262E-3</c:v>
+                  <c:v>2.0726481481481481E-3</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>2.2396412037037038E-3</c:v>
+                  <c:v>2.0329050925925922E-3</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>2.0068645833333332E-3</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>2.0306388888888887E-3</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>2.052704861111111E-3</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>2.1059722222222218E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7909,10 +8047,10 @@
           </c:marker>
           <c:yVal>
             <c:numRef>
-              <c:f>JRP!$X$2:$X$105</c:f>
+              <c:f>JRP!$X$2:$X$109</c:f>
               <c:numCache>
                 <c:formatCode>m:ss.00</c:formatCode>
-                <c:ptCount val="104"/>
+                <c:ptCount val="108"/>
                 <c:pt idx="0">
                   <c:v>1.8332175925925925E-3</c:v>
                 </c:pt>
@@ -8010,22 +8148,22 @@
                   <c:v>2.0002662037037038E-3</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.8660300925925923E-3</c:v>
+                  <c:v>1.8361736111111109E-3</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>1.8880208333333333E-3</c:v>
+                  <c:v>1.8578124999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>1.9082754629629632E-3</c:v>
+                  <c:v>1.8777430555555557E-3</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.0263310185185185E-3</c:v>
+                  <c:v>1.9128564814814813E-3</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2.0339988425925925E-3</c:v>
+                  <c:v>1.9200949074074073E-3</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2.0410879629629629E-3</c:v>
+                  <c:v>1.9267870370370367E-3</c:v>
                 </c:pt>
                 <c:pt idx="38">
                   <c:v>1.9033506944444441E-3</c:v>
@@ -8208,22 +8346,34 @@
                   <c:v>2.0296701388888886E-3</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>1.9107291666666667E-3</c:v>
+                  <c:v>1.660864583333333E-3</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>1.8922222222222224E-3</c:v>
+                  <c:v>1.6447777777777778E-3</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>1.8350462962962962E-3</c:v>
+                  <c:v>1.5950787037037034E-3</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>2.0968518518518523E-3</c:v>
+                  <c:v>1.9032962962962964E-3</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>2.090231481481482E-3</c:v>
+                  <c:v>1.8972870370370372E-3</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>2.0694675925925924E-3</c:v>
+                  <c:v>1.8784398148148146E-3</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>1.8361736111111109E-3</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>1.8578124999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>1.8777430555555557E-3</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>1.9128564814814813E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9014,15 +9164,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>1058223</xdr:colOff>
-      <xdr:row>105</xdr:row>
-      <xdr:rowOff>95547</xdr:rowOff>
+      <xdr:colOff>1246837</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>104978</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>744899</xdr:colOff>
-      <xdr:row>143</xdr:row>
-      <xdr:rowOff>151946</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>169627</xdr:colOff>
+      <xdr:row>149</xdr:row>
+      <xdr:rowOff>161377</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9297,8 +9447,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}" name="JRP_konfig" displayName="JRP_konfig" ref="A1:X105" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
-  <autoFilter ref="A1:X105" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}" name="JRP_konfig" displayName="JRP_konfig" ref="A1:X111" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+  <autoFilter ref="A1:X111" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -9325,30 +9475,30 @@
     <filterColumn colId="23" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{021DA6E1-2C93-4474-9720-B6F016186D61}" name="Tabellen Name" dataDxfId="41"/>
-    <tableColumn id="2" xr3:uid="{733C1722-A9C9-4830-A9E2-FE62E96BCD98}" name="Geschlecht" dataDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{80C0BF46-0E43-4947-BF86-B808C324772A}" name="Mindest Alter" dataDxfId="39"/>
-    <tableColumn id="4" xr3:uid="{DBA2A923-EEB7-43F9-A1A3-E78624448FB9}" name="Maximales Alter" dataDxfId="38"/>
-    <tableColumn id="5" xr3:uid="{3FDEE18A-328D-45AE-907D-69A916A93345}" name="Qualizeitraum anfang" dataDxfId="37"/>
-    <tableColumn id="6" xr3:uid="{BE002D7F-575F-4B60-9251-C71D93F59045}" name="Qualizeitraum Ende" dataDxfId="36"/>
-    <tableColumn id="7" xr3:uid="{208ABD57-DE4B-41D6-B9FC-93F2D8966E8D}" name="Letzter Wettkampf am" dataDxfId="35"/>
-    <tableColumn id="8" xr3:uid="{30C9697C-6550-4996-ADDB-7FEE5325B794}" name="Landesverband" dataDxfId="34"/>
-    <tableColumn id="9" xr3:uid="{ED2DAB77-EF46-4D8B-B8E4-90412E32E277}" name="OMS" dataDxfId="33"/>
-    <tableColumn id="10" xr3:uid="{AD534940-A91B-4A6E-9606-E3F3E517D401}" name="Pool-Länge" dataDxfId="32"/>
-    <tableColumn id="11" xr3:uid="{11F9D5D5-72FE-42CA-8624-01D513B4140F}" name="Regelwerk" dataDxfId="31"/>
-    <tableColumn id="12" xr3:uid="{3907872B-5438-4FBF-A045-3EF9EAACFC47}" name="Seiten Anzahl" dataDxfId="30"/>
-    <tableColumn id="13" xr3:uid="{FC821324-3638-40C0-BA1E-069B44E23C7A}" name="PZ1 - 50m Retten" dataDxfId="29"/>
-    <tableColumn id="14" xr3:uid="{70529619-443E-40D3-88C1-3E0F00BB2A50}" name="PZ1 - 100m Retten" dataDxfId="28"/>
-    <tableColumn id="15" xr3:uid="{EFA92FD2-C23F-42B3-83DC-5036513F19AF}" name="PZ1 - 100m Kombi" dataDxfId="27"/>
-    <tableColumn id="16" xr3:uid="{03309E52-8CF3-4E90-9EE6-A818901C3B32}" name="PZ1 - 100m Lifesaver" dataDxfId="26"/>
-    <tableColumn id="17" xr3:uid="{00B22013-AA11-4C17-9250-22060AE4B0A8}" name="PZ1 - 200m Super-Lifesaver" dataDxfId="25"/>
-    <tableColumn id="18" xr3:uid="{7E3508A9-0422-4561-A23E-53E613259B24}" name="PZ1 - 200m Hindernis" dataDxfId="24"/>
-    <tableColumn id="19" xr3:uid="{5CEA435F-F34B-4D8D-88D0-F5EBFF18B713}" name="PZ2 - 50m Retten" dataDxfId="23"/>
-    <tableColumn id="20" xr3:uid="{8585BE62-F7C4-4D5D-B287-052B43B08610}" name="PZ2 - 100m Retten" dataDxfId="22"/>
-    <tableColumn id="21" xr3:uid="{D981758B-ADAD-4E36-B787-0B0FDA808CA2}" name="PZ2 - 100m Kombi" dataDxfId="21"/>
-    <tableColumn id="22" xr3:uid="{1D4970A8-D22F-4962-934C-AEA295ED687A}" name="PZ2 - 100m Lifesaver" dataDxfId="20"/>
-    <tableColumn id="23" xr3:uid="{BE394430-C58F-4690-9615-44475E5AF9F8}" name="PZ2 - 200m Super-Lifesaver" dataDxfId="19"/>
-    <tableColumn id="24" xr3:uid="{A7036B1A-99CE-4F7C-AAB8-12E8B2696202}" name="PZ2 - 200m Hindernis" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{021DA6E1-2C93-4474-9720-B6F016186D61}" name="Tabellen Name" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{733C1722-A9C9-4830-A9E2-FE62E96BCD98}" name="Geschlecht" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{80C0BF46-0E43-4947-BF86-B808C324772A}" name="Mindest Alter" dataDxfId="21"/>
+    <tableColumn id="4" xr3:uid="{DBA2A923-EEB7-43F9-A1A3-E78624448FB9}" name="Maximales Alter" dataDxfId="20"/>
+    <tableColumn id="5" xr3:uid="{3FDEE18A-328D-45AE-907D-69A916A93345}" name="Qualizeitraum anfang" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{BE002D7F-575F-4B60-9251-C71D93F59045}" name="Qualizeitraum Ende" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{208ABD57-DE4B-41D6-B9FC-93F2D8966E8D}" name="Letzter Wettkampf am" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{30C9697C-6550-4996-ADDB-7FEE5325B794}" name="Landesverband" dataDxfId="16"/>
+    <tableColumn id="9" xr3:uid="{ED2DAB77-EF46-4D8B-B8E4-90412E32E277}" name="OMS" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{AD534940-A91B-4A6E-9606-E3F3E517D401}" name="Pool-Länge" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{11F9D5D5-72FE-42CA-8624-01D513B4140F}" name="Regelwerk" dataDxfId="13"/>
+    <tableColumn id="12" xr3:uid="{3907872B-5438-4FBF-A045-3EF9EAACFC47}" name="Seiten Anzahl" dataDxfId="12"/>
+    <tableColumn id="13" xr3:uid="{FC821324-3638-40C0-BA1E-069B44E23C7A}" name="PZ1 - 50m Retten" dataDxfId="11"/>
+    <tableColumn id="14" xr3:uid="{70529619-443E-40D3-88C1-3E0F00BB2A50}" name="PZ1 - 100m Retten" dataDxfId="10"/>
+    <tableColumn id="15" xr3:uid="{EFA92FD2-C23F-42B3-83DC-5036513F19AF}" name="PZ1 - 100m Kombi" dataDxfId="9"/>
+    <tableColumn id="16" xr3:uid="{03309E52-8CF3-4E90-9EE6-A818901C3B32}" name="PZ1 - 100m Lifesaver" dataDxfId="8"/>
+    <tableColumn id="17" xr3:uid="{00B22013-AA11-4C17-9250-22060AE4B0A8}" name="PZ1 - 200m Super-Lifesaver" dataDxfId="7"/>
+    <tableColumn id="18" xr3:uid="{7E3508A9-0422-4561-A23E-53E613259B24}" name="PZ1 - 200m Hindernis" dataDxfId="6"/>
+    <tableColumn id="19" xr3:uid="{5CEA435F-F34B-4D8D-88D0-F5EBFF18B713}" name="PZ2 - 50m Retten" dataDxfId="5"/>
+    <tableColumn id="20" xr3:uid="{8585BE62-F7C4-4D5D-B287-052B43B08610}" name="PZ2 - 100m Retten" dataDxfId="4"/>
+    <tableColumn id="21" xr3:uid="{D981758B-ADAD-4E36-B787-0B0FDA808CA2}" name="PZ2 - 100m Kombi" dataDxfId="3"/>
+    <tableColumn id="22" xr3:uid="{1D4970A8-D22F-4962-934C-AEA295ED687A}" name="PZ2 - 100m Lifesaver" dataDxfId="2"/>
+    <tableColumn id="23" xr3:uid="{BE394430-C58F-4690-9615-44475E5AF9F8}" name="PZ2 - 200m Super-Lifesaver" dataDxfId="1"/>
+    <tableColumn id="24" xr3:uid="{A7036B1A-99CE-4F7C-AAB8-12E8B2696202}" name="PZ2 - 200m Hindernis" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -13293,52 +13443,52 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B5:G31">
-    <cfRule type="expression" dxfId="17" priority="15">
+    <cfRule type="expression" dxfId="43" priority="15">
       <formula>B5&lt;&gt;B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:M31">
-    <cfRule type="expression" dxfId="16" priority="14">
+    <cfRule type="expression" dxfId="42" priority="14">
       <formula>H5&lt;&gt;H4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N5:S31">
-    <cfRule type="expression" dxfId="15" priority="13">
+    <cfRule type="expression" dxfId="41" priority="13">
       <formula>N5&lt;&gt;N4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T5:Y31">
-    <cfRule type="expression" dxfId="14" priority="12">
+    <cfRule type="expression" dxfId="40" priority="12">
       <formula>T5&lt;&gt;T4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z5:AE31">
-    <cfRule type="expression" dxfId="13" priority="9">
+    <cfRule type="expression" dxfId="39" priority="9">
       <formula>Z5&lt;&gt;Z4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF5:AK31">
-    <cfRule type="expression" dxfId="12" priority="8">
+    <cfRule type="expression" dxfId="38" priority="8">
       <formula>AF5&lt;&gt;AF4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL5:AN31">
-    <cfRule type="expression" dxfId="11" priority="6">
+    <cfRule type="expression" dxfId="37" priority="6">
       <formula>AL5&lt;&gt;AL4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO5:AQ31">
-    <cfRule type="expression" dxfId="10" priority="5">
+    <cfRule type="expression" dxfId="36" priority="5">
       <formula>AO5&lt;&gt;AO4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR5:AT31">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="35" priority="2">
       <formula>AR5&lt;&gt;AR4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU5:AW31">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="34" priority="1">
       <formula>AU5&lt;&gt;AU4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15943,22 +16093,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B6:G6">
-    <cfRule type="expression" dxfId="7" priority="20">
+    <cfRule type="expression" dxfId="33" priority="20">
       <formula>B6&lt;&gt;B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:G32">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="32" priority="1">
       <formula>B7&lt;&gt;B6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:M6">
-    <cfRule type="expression" dxfId="5" priority="22">
+    <cfRule type="expression" dxfId="31" priority="22">
       <formula>H6&lt;&gt;H4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:M32">
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="30" priority="2">
       <formula>H7&lt;&gt;H6</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17294,22 +17444,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B6:G6">
-    <cfRule type="expression" dxfId="3" priority="19">
+    <cfRule type="expression" dxfId="29" priority="19">
       <formula>B6&lt;&gt;B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:G32">
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="28" priority="2">
       <formula>B7&lt;&gt;B6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:M6">
-    <cfRule type="expression" dxfId="1" priority="20">
+    <cfRule type="expression" dxfId="27" priority="20">
       <formula>H6&lt;&gt;H4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:M32">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="26" priority="1">
       <formula>H7&lt;&gt;H6</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18563,10 +18713,10 @@
   <sheetPr codeName="Tabelle10">
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:X108"/>
+  <dimension ref="A1:X111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="101" workbookViewId="0">
-      <selection activeCell="C54" sqref="C54"/>
+    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="101" workbookViewId="0">
+      <selection activeCell="D106" sqref="D106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -20946,51 +21096,51 @@
       </c>
       <c r="M34" s="62">
         <f>NK!E14</f>
-        <v>4.5775462962962962E-4</v>
+        <v>4.5043055555555553E-4</v>
       </c>
       <c r="N34" s="62">
         <f>NK!E16</f>
-        <v>7.2410300925925919E-4</v>
+        <v>7.1251736111111103E-4</v>
       </c>
       <c r="O34" s="62">
         <f>NK!E15</f>
-        <v>9.8365162037037019E-4</v>
+        <v>9.6791319444444431E-4</v>
       </c>
       <c r="P34" s="62">
         <f>NK!E17</f>
-        <v>8.2494212962962968E-4</v>
+        <v>8.1174305555555557E-4</v>
       </c>
       <c r="Q34" s="62">
         <f>NK!E19</f>
-        <v>2.0394965277777777E-3</v>
+        <v>2.0068645833333332E-3</v>
       </c>
       <c r="R34" s="62">
         <f>NK!E18</f>
-        <v>1.8660300925925923E-3</v>
+        <v>1.8361736111111109E-3</v>
       </c>
       <c r="S34" s="62">
         <f>M34</f>
-        <v>4.5775462962962962E-4</v>
+        <v>4.5043055555555553E-4</v>
       </c>
       <c r="T34" s="62">
         <f t="shared" ref="T34:T39" si="0">N34</f>
-        <v>7.2410300925925919E-4</v>
+        <v>7.1251736111111103E-4</v>
       </c>
       <c r="U34" s="62">
         <f t="shared" ref="U34:U39" si="1">O34</f>
-        <v>9.8365162037037019E-4</v>
+        <v>9.6791319444444431E-4</v>
       </c>
       <c r="V34" s="62">
         <f t="shared" ref="V34:V39" si="2">P34</f>
-        <v>8.2494212962962968E-4</v>
+        <v>8.1174305555555557E-4</v>
       </c>
       <c r="W34" s="62">
         <f t="shared" ref="W34:W39" si="3">Q34</f>
-        <v>2.0394965277777777E-3</v>
+        <v>2.0068645833333332E-3</v>
       </c>
       <c r="X34" s="62">
         <f t="shared" ref="X34:X39" si="4">R34</f>
-        <v>1.8660300925925923E-3</v>
+        <v>1.8361736111111109E-3</v>
       </c>
     </row>
     <row r="35" spans="1:24" x14ac:dyDescent="0.45">
@@ -21028,51 +21178,51 @@
       </c>
       <c r="M35" s="62">
         <f>NK!D14</f>
-        <v>4.6281828703703703E-4</v>
+        <v>4.5541319444444443E-4</v>
       </c>
       <c r="N35" s="62">
         <f>NK!D16</f>
-        <v>7.311921296296297E-4</v>
+        <v>7.1949305555555558E-4</v>
       </c>
       <c r="O35" s="62">
         <f>NK!D15</f>
-        <v>9.9797453703703702E-4</v>
+        <v>9.8200694444444442E-4</v>
       </c>
       <c r="P35" s="62">
         <f>NK!D17</f>
-        <v>8.427372685185186E-4</v>
+        <v>8.2925347222222222E-4</v>
       </c>
       <c r="Q35" s="62">
         <f>NK!D19</f>
-        <v>2.0636574074074073E-3</v>
+        <v>2.0306388888888887E-3</v>
       </c>
       <c r="R35" s="62">
         <f>NK!D18</f>
-        <v>1.8880208333333333E-3</v>
+        <v>1.8578124999999999E-3</v>
       </c>
       <c r="S35" s="62">
         <f t="shared" ref="S35:S39" si="5">M35</f>
-        <v>4.6281828703703703E-4</v>
+        <v>4.5541319444444443E-4</v>
       </c>
       <c r="T35" s="62">
         <f t="shared" si="0"/>
-        <v>7.311921296296297E-4</v>
+        <v>7.1949305555555558E-4</v>
       </c>
       <c r="U35" s="62">
         <f t="shared" si="1"/>
-        <v>9.9797453703703702E-4</v>
+        <v>9.8200694444444442E-4</v>
       </c>
       <c r="V35" s="62">
         <f t="shared" si="2"/>
-        <v>8.427372685185186E-4</v>
+        <v>8.2925347222222222E-4</v>
       </c>
       <c r="W35" s="62">
         <f t="shared" si="3"/>
-        <v>2.0636574074074073E-3</v>
+        <v>2.0306388888888887E-3</v>
       </c>
       <c r="X35" s="62">
         <f t="shared" si="4"/>
-        <v>1.8880208333333333E-3</v>
+        <v>1.8578124999999999E-3</v>
       </c>
     </row>
     <row r="36" spans="1:24" x14ac:dyDescent="0.45">
@@ -21110,51 +21260,51 @@
       </c>
       <c r="M36" s="62">
         <f>NK!C14</f>
-        <v>4.6730324074074068E-4</v>
+        <v>4.5982638888888885E-4</v>
       </c>
       <c r="N36" s="62">
         <f>NK!C16</f>
-        <v>7.378472222222222E-4</v>
+        <v>7.2604166666666661E-4</v>
       </c>
       <c r="O36" s="62">
         <f>NK!C15</f>
-        <v>1.0112847222222224E-3</v>
+        <v>9.9510416666666671E-4</v>
       </c>
       <c r="P36" s="62">
         <f>NK!C17</f>
-        <v>8.5908564814814821E-4</v>
+        <v>8.4534027777777786E-4</v>
       </c>
       <c r="Q36" s="62">
         <f>NK!C19</f>
-        <v>2.0860821759259261E-3</v>
+        <v>2.052704861111111E-3</v>
       </c>
       <c r="R36" s="62">
         <f>NK!C18</f>
-        <v>1.9082754629629632E-3</v>
+        <v>1.8777430555555557E-3</v>
       </c>
       <c r="S36" s="62">
         <f t="shared" si="5"/>
-        <v>4.6730324074074068E-4</v>
+        <v>4.5982638888888885E-4</v>
       </c>
       <c r="T36" s="62">
         <f t="shared" si="0"/>
-        <v>7.378472222222222E-4</v>
+        <v>7.2604166666666661E-4</v>
       </c>
       <c r="U36" s="62">
         <f t="shared" si="1"/>
-        <v>1.0112847222222224E-3</v>
+        <v>9.9510416666666671E-4</v>
       </c>
       <c r="V36" s="62">
         <f t="shared" si="2"/>
-        <v>8.5908564814814821E-4</v>
+        <v>8.4534027777777786E-4</v>
       </c>
       <c r="W36" s="62">
         <f t="shared" si="3"/>
-        <v>2.0860821759259261E-3</v>
+        <v>2.052704861111111E-3</v>
       </c>
       <c r="X36" s="62">
         <f t="shared" si="4"/>
-        <v>1.9082754629629632E-3</v>
+        <v>1.8777430555555557E-3</v>
       </c>
     </row>
     <row r="37" spans="1:24" x14ac:dyDescent="0.45">
@@ -21192,51 +21342,51 @@
       </c>
       <c r="M37" s="62">
         <f>NK!K14</f>
-        <v>5.6626157407407406E-4</v>
+        <v>5.3455092592592595E-4</v>
       </c>
       <c r="N37" s="62">
         <f>NK!K16</f>
-        <v>8.521412037037037E-4</v>
+        <v>8.0442129629629624E-4</v>
       </c>
       <c r="O37" s="62">
         <f>NK!K15</f>
-        <v>1.1524884259259259E-3</v>
+        <v>1.0879490740740739E-3</v>
       </c>
       <c r="P37" s="62">
         <f>NK!K17</f>
-        <v>9.4646990740740737E-4</v>
+        <v>8.9346759259259251E-4</v>
       </c>
       <c r="Q37" s="62">
         <f>NK!K19</f>
-        <v>2.2309027777777774E-3</v>
+        <v>2.1059722222222218E-3</v>
       </c>
       <c r="R37" s="62">
         <f>NK!K18</f>
-        <v>2.0263310185185185E-3</v>
+        <v>1.9128564814814813E-3</v>
       </c>
       <c r="S37" s="62">
         <f t="shared" si="5"/>
-        <v>5.6626157407407406E-4</v>
+        <v>5.3455092592592595E-4</v>
       </c>
       <c r="T37" s="62">
         <f t="shared" si="0"/>
-        <v>8.521412037037037E-4</v>
+        <v>8.0442129629629624E-4</v>
       </c>
       <c r="U37" s="62">
         <f t="shared" si="1"/>
-        <v>1.1524884259259259E-3</v>
+        <v>1.0879490740740739E-3</v>
       </c>
       <c r="V37" s="62">
         <f t="shared" si="2"/>
-        <v>9.4646990740740737E-4</v>
+        <v>8.9346759259259251E-4</v>
       </c>
       <c r="W37" s="62">
         <f t="shared" si="3"/>
-        <v>2.2309027777777774E-3</v>
+        <v>2.1059722222222218E-3</v>
       </c>
       <c r="X37" s="62">
         <f t="shared" si="4"/>
-        <v>2.0263310185185185E-3</v>
+        <v>1.9128564814814813E-3</v>
       </c>
     </row>
     <row r="38" spans="1:24" x14ac:dyDescent="0.45">
@@ -21274,51 +21424,51 @@
       </c>
       <c r="M38" s="62">
         <f>NK!J14</f>
-        <v>5.7769097222222228E-4</v>
+        <v>5.4534027777777773E-4</v>
       </c>
       <c r="N38" s="62">
         <f>NK!J16</f>
-        <v>8.6183449074074081E-4</v>
+        <v>8.1357175925925933E-4</v>
       </c>
       <c r="O38" s="62">
         <f>NK!J15</f>
-        <v>1.1731770833333334E-3</v>
+        <v>1.1074791666666668E-3</v>
       </c>
       <c r="P38" s="62">
         <f>NK!J17</f>
-        <v>9.6035879629629618E-4</v>
+        <v>9.065787037037035E-4</v>
       </c>
       <c r="Q38" s="62">
         <f>NK!J19</f>
-        <v>2.2473958333333335E-3</v>
+        <v>2.1215416666666665E-3</v>
       </c>
       <c r="R38" s="62">
         <f>NK!J18</f>
-        <v>2.0339988425925925E-3</v>
+        <v>1.9200949074074073E-3</v>
       </c>
       <c r="S38" s="62">
         <f t="shared" si="5"/>
-        <v>5.7769097222222228E-4</v>
+        <v>5.4534027777777773E-4</v>
       </c>
       <c r="T38" s="62">
         <f t="shared" si="0"/>
-        <v>8.6183449074074081E-4</v>
+        <v>8.1357175925925933E-4</v>
       </c>
       <c r="U38" s="62">
         <f t="shared" si="1"/>
-        <v>1.1731770833333334E-3</v>
+        <v>1.1074791666666668E-3</v>
       </c>
       <c r="V38" s="62">
         <f t="shared" si="2"/>
-        <v>9.6035879629629618E-4</v>
+        <v>9.065787037037035E-4</v>
       </c>
       <c r="W38" s="62">
         <f t="shared" si="3"/>
-        <v>2.2473958333333335E-3</v>
+        <v>2.1215416666666665E-3</v>
       </c>
       <c r="X38" s="62">
         <f t="shared" si="4"/>
-        <v>2.0339988425925925E-3</v>
+        <v>1.9200949074074073E-3</v>
       </c>
     </row>
     <row r="39" spans="1:24" x14ac:dyDescent="0.45">
@@ -21356,51 +21506,51 @@
       </c>
       <c r="M39" s="62">
         <f>NK!I14</f>
-        <v>5.8854166666666668E-4</v>
+        <v>5.5558333333333328E-4</v>
       </c>
       <c r="N39" s="62">
         <f>NK!I16</f>
-        <v>8.7080439814814811E-4</v>
+        <v>8.2203935185185179E-4</v>
       </c>
       <c r="O39" s="62">
         <f>NK!I15</f>
-        <v>1.1922743055555556E-3</v>
+        <v>1.1255069444444444E-3</v>
       </c>
       <c r="P39" s="62">
         <f>NK!I17</f>
-        <v>9.730902777777778E-4</v>
+        <v>9.1859722222222223E-4</v>
       </c>
       <c r="Q39" s="62">
         <f>NK!I19</f>
-        <v>2.2627314814814815E-3</v>
+        <v>2.1360185185185184E-3</v>
       </c>
       <c r="R39" s="62">
         <f>NK!I18</f>
-        <v>2.0410879629629629E-3</v>
+        <v>1.9267870370370367E-3</v>
       </c>
       <c r="S39" s="62">
         <f t="shared" si="5"/>
-        <v>5.8854166666666668E-4</v>
+        <v>5.5558333333333328E-4</v>
       </c>
       <c r="T39" s="62">
         <f t="shared" si="0"/>
-        <v>8.7080439814814811E-4</v>
+        <v>8.2203935185185179E-4</v>
       </c>
       <c r="U39" s="62">
         <f t="shared" si="1"/>
-        <v>1.1922743055555556E-3</v>
+        <v>1.1255069444444444E-3</v>
       </c>
       <c r="V39" s="62">
         <f t="shared" si="2"/>
-        <v>9.730902777777778E-4</v>
+        <v>9.1859722222222223E-4</v>
       </c>
       <c r="W39" s="62">
         <f t="shared" si="3"/>
-        <v>2.2627314814814815E-3</v>
+        <v>2.1360185185185184E-3</v>
       </c>
       <c r="X39" s="62">
         <f t="shared" si="4"/>
-        <v>2.0410879629629629E-3</v>
+        <v>1.9267870370370367E-3</v>
       </c>
     </row>
     <row r="40" spans="1:24" x14ac:dyDescent="0.45">
@@ -22299,23 +22449,23 @@
         <v>3.9722222222222226E-4</v>
       </c>
       <c r="T52" s="62">
-        <f t="shared" ref="T52:T105" si="7">N52</f>
+        <f t="shared" ref="T52:T111" si="7">N52</f>
         <v>6.2893518518518528E-4</v>
       </c>
       <c r="U52" s="62">
-        <f t="shared" ref="U52:U105" si="8">O52</f>
+        <f t="shared" ref="U52:U111" si="8">O52</f>
         <v>8.490625000000001E-4</v>
       </c>
       <c r="V52" s="62">
-        <f t="shared" ref="V52:V105" si="9">P52</f>
+        <f t="shared" ref="V52:V111" si="9">P52</f>
         <v>7.0545138888888882E-4</v>
       </c>
       <c r="W52" s="62">
-        <f t="shared" ref="W52:W105" si="10">Q52</f>
+        <f t="shared" ref="W52:W111" si="10">Q52</f>
         <v>1.7668750000000002E-3</v>
       </c>
       <c r="X52" s="62">
-        <f t="shared" ref="X52:X105" si="11">R52</f>
+        <f t="shared" ref="X52:X111" si="11">R52</f>
         <v>1.6167708333333333E-3</v>
       </c>
     </row>
@@ -25926,51 +26076,51 @@
       </c>
       <c r="M100" s="62">
         <f>NK!$R$14</f>
-        <v>4.6944444444444442E-4</v>
+        <v>4.0805555555555549E-4</v>
       </c>
       <c r="N100" s="62">
         <f>NK!$R$16</f>
-        <v>7.4328703703703709E-4</v>
+        <v>6.4608796296296289E-4</v>
       </c>
       <c r="O100" s="62">
         <f>NK!$R$15</f>
-        <v>1.0034375E-3</v>
+        <v>8.7221874999999995E-4</v>
       </c>
       <c r="P100" s="62">
         <f>NK!$R$17</f>
-        <v>8.3371527777777773E-4</v>
+        <v>7.2469097222222206E-4</v>
       </c>
       <c r="Q100" s="62">
         <f>NK!$R$19</f>
-        <v>2.0881250000000001E-3</v>
+        <v>1.8150624999999998E-3</v>
       </c>
       <c r="R100" s="62">
         <f>NK!$R$18</f>
-        <v>1.9107291666666667E-3</v>
+        <v>1.660864583333333E-3</v>
       </c>
       <c r="S100" s="62">
         <f>M100</f>
-        <v>4.6944444444444442E-4</v>
+        <v>4.0805555555555549E-4</v>
       </c>
       <c r="T100" s="62">
         <f t="shared" si="7"/>
-        <v>7.4328703703703709E-4</v>
+        <v>6.4608796296296289E-4</v>
       </c>
       <c r="U100" s="62">
         <f t="shared" si="8"/>
-        <v>1.0034375E-3</v>
+        <v>8.7221874999999995E-4</v>
       </c>
       <c r="V100" s="62">
         <f t="shared" si="9"/>
-        <v>8.3371527777777773E-4</v>
+        <v>7.2469097222222206E-4</v>
       </c>
       <c r="W100" s="62">
         <f t="shared" si="10"/>
-        <v>2.0881250000000001E-3</v>
+        <v>1.8150624999999998E-3</v>
       </c>
       <c r="X100" s="62">
         <f t="shared" si="11"/>
-        <v>1.9107291666666667E-3</v>
+        <v>1.660864583333333E-3</v>
       </c>
     </row>
     <row r="101" spans="1:24" x14ac:dyDescent="0.45">
@@ -26008,51 +26158,51 @@
       </c>
       <c r="M101" s="62">
         <f>NK!$S$14</f>
-        <v>4.6523148148148151E-4</v>
+        <v>4.043935185185185E-4</v>
       </c>
       <c r="N101" s="62">
         <f>NK!$S$16</f>
-        <v>7.3726851851851861E-4</v>
+        <v>6.4085648148148151E-4</v>
       </c>
       <c r="O101" s="62">
         <f>NK!$S$15</f>
-        <v>9.9155092592592611E-4</v>
+        <v>8.6188657407407405E-4</v>
       </c>
       <c r="P101" s="62">
         <f>NK!$S$17</f>
-        <v>8.1927083333333331E-4</v>
+        <v>7.1213541666666658E-4</v>
       </c>
       <c r="Q101" s="62">
         <f>NK!$S$19</f>
-        <v>2.0678125000000002E-3</v>
+        <v>1.79740625E-3</v>
       </c>
       <c r="R101" s="62">
         <f>NK!$S$18</f>
-        <v>1.8922222222222224E-3</v>
+        <v>1.6447777777777778E-3</v>
       </c>
       <c r="S101" s="62">
         <f t="shared" ref="S101:S105" si="12">M101</f>
-        <v>4.6523148148148151E-4</v>
+        <v>4.043935185185185E-4</v>
       </c>
       <c r="T101" s="62">
         <f t="shared" si="7"/>
-        <v>7.3726851851851861E-4</v>
+        <v>6.4085648148148151E-4</v>
       </c>
       <c r="U101" s="62">
         <f t="shared" si="8"/>
-        <v>9.9155092592592611E-4</v>
+        <v>8.6188657407407405E-4</v>
       </c>
       <c r="V101" s="62">
         <f t="shared" si="9"/>
-        <v>8.1927083333333331E-4</v>
+        <v>7.1213541666666658E-4</v>
       </c>
       <c r="W101" s="62">
         <f t="shared" si="10"/>
-        <v>2.0678125000000002E-3</v>
+        <v>1.79740625E-3</v>
       </c>
       <c r="X101" s="62">
         <f t="shared" si="11"/>
-        <v>1.8922222222222224E-3</v>
+        <v>1.6447777777777778E-3</v>
       </c>
     </row>
     <row r="102" spans="1:24" x14ac:dyDescent="0.45">
@@ -26090,51 +26240,51 @@
       </c>
       <c r="M102" s="62">
         <f>NK!$T$14</f>
-        <v>4.5244212962962968E-4</v>
+        <v>3.9327662037037033E-4</v>
       </c>
       <c r="N102" s="62">
         <f>NK!$T$16</f>
-        <v>7.1846064814814819E-4</v>
+        <v>6.2450810185185179E-4</v>
       </c>
       <c r="O102" s="62">
         <f>NK!$T$15</f>
-        <v>9.5453703703703705E-4</v>
+        <v>8.2971296296296287E-4</v>
       </c>
       <c r="P102" s="62">
         <f>NK!$T$17</f>
-        <v>7.7473379629629626E-4</v>
+        <v>6.7342245370370364E-4</v>
       </c>
       <c r="Q102" s="62">
         <f>NK!$T$19</f>
-        <v>2.0049189814814817E-3</v>
+        <v>1.7427372685185185E-3</v>
       </c>
       <c r="R102" s="62">
         <f>NK!$T$18</f>
-        <v>1.8350462962962962E-3</v>
+        <v>1.5950787037037034E-3</v>
       </c>
       <c r="S102" s="62">
         <f t="shared" si="12"/>
-        <v>4.5244212962962968E-4</v>
+        <v>3.9327662037037033E-4</v>
       </c>
       <c r="T102" s="62">
         <f t="shared" si="7"/>
-        <v>7.1846064814814819E-4</v>
+        <v>6.2450810185185179E-4</v>
       </c>
       <c r="U102" s="62">
         <f t="shared" si="8"/>
-        <v>9.5453703703703705E-4</v>
+        <v>8.2971296296296287E-4</v>
       </c>
       <c r="V102" s="62">
         <f t="shared" si="9"/>
-        <v>7.7473379629629626E-4</v>
+        <v>6.7342245370370364E-4</v>
       </c>
       <c r="W102" s="62">
         <f t="shared" si="10"/>
-        <v>2.0049189814814817E-3</v>
+        <v>1.7427372685185185E-3</v>
       </c>
       <c r="X102" s="62">
         <f t="shared" si="11"/>
-        <v>1.8350462962962962E-3</v>
+        <v>1.5950787037037034E-3</v>
       </c>
     </row>
     <row r="103" spans="1:24" x14ac:dyDescent="0.45">
@@ -26172,51 +26322,51 @@
       </c>
       <c r="M103" s="62">
         <f>NK!$X$14</f>
-        <v>5.73263888888889E-4</v>
+        <v>5.2034722222222228E-4</v>
       </c>
       <c r="N103" s="62">
         <f>NK!$X$16</f>
-        <v>8.7313657407407414E-4</v>
+        <v>7.9253935185185189E-4</v>
       </c>
       <c r="O103" s="62">
         <f>NK!$X$15</f>
-        <v>1.1704513888888888E-3</v>
+        <v>1.062409722222222E-3</v>
       </c>
       <c r="P103" s="62">
         <f>NK!$X$17</f>
-        <v>9.6537037037037034E-4</v>
+        <v>8.7625925925925914E-4</v>
       </c>
       <c r="Q103" s="62">
         <f>NK!$X$19</f>
-        <v>2.2975694444444445E-3</v>
+        <v>2.0854861111111109E-3</v>
       </c>
       <c r="R103" s="62">
         <f>NK!$X$18</f>
-        <v>2.0968518518518523E-3</v>
+        <v>1.9032962962962964E-3</v>
       </c>
       <c r="S103" s="62">
         <f t="shared" si="12"/>
-        <v>5.73263888888889E-4</v>
+        <v>5.2034722222222228E-4</v>
       </c>
       <c r="T103" s="62">
         <f t="shared" si="7"/>
-        <v>8.7313657407407414E-4</v>
+        <v>7.9253935185185189E-4</v>
       </c>
       <c r="U103" s="62">
         <f t="shared" si="8"/>
-        <v>1.1704513888888888E-3</v>
+        <v>1.062409722222222E-3</v>
       </c>
       <c r="V103" s="62">
         <f t="shared" si="9"/>
-        <v>9.6537037037037034E-4</v>
+        <v>8.7625925925925914E-4</v>
       </c>
       <c r="W103" s="62">
         <f t="shared" si="10"/>
-        <v>2.2975694444444445E-3</v>
+        <v>2.0854861111111109E-3</v>
       </c>
       <c r="X103" s="62">
         <f t="shared" si="11"/>
-        <v>2.0968518518518523E-3</v>
+        <v>1.9032962962962964E-3</v>
       </c>
     </row>
     <row r="104" spans="1:24" x14ac:dyDescent="0.45">
@@ -26254,51 +26404,51 @@
       </c>
       <c r="M104" s="62">
         <f>NK!$Y$14</f>
-        <v>5.6393518518518522E-4</v>
+        <v>5.118796296296296E-4</v>
       </c>
       <c r="N104" s="62">
         <f>NK!$Y$16</f>
-        <v>8.6501157407407403E-4</v>
+        <v>7.8516435185185178E-4</v>
       </c>
       <c r="O104" s="62">
         <f>NK!$Y$15</f>
-        <v>1.1534490740740741E-3</v>
+        <v>1.0469768518518517E-3</v>
       </c>
       <c r="P104" s="62">
         <f>NK!$Y$17</f>
-        <v>9.5378472222222229E-4</v>
+        <v>8.6574305555555547E-4</v>
       </c>
       <c r="Q104" s="62">
         <f>NK!$Y$19</f>
-        <v>2.2834259259259262E-3</v>
+        <v>2.0726481481481481E-3</v>
       </c>
       <c r="R104" s="62">
         <f>NK!$Y$18</f>
-        <v>2.090231481481482E-3</v>
+        <v>1.8972870370370372E-3</v>
       </c>
       <c r="S104" s="62">
         <f t="shared" si="12"/>
-        <v>5.6393518518518522E-4</v>
+        <v>5.118796296296296E-4</v>
       </c>
       <c r="T104" s="62">
         <f t="shared" si="7"/>
-        <v>8.6501157407407403E-4</v>
+        <v>7.8516435185185178E-4</v>
       </c>
       <c r="U104" s="62">
         <f t="shared" si="8"/>
-        <v>1.1534490740740741E-3</v>
+        <v>1.0469768518518517E-3</v>
       </c>
       <c r="V104" s="62">
         <f t="shared" si="9"/>
-        <v>9.5378472222222229E-4</v>
+        <v>8.6574305555555547E-4</v>
       </c>
       <c r="W104" s="62">
         <f t="shared" si="10"/>
-        <v>2.2834259259259262E-3</v>
+        <v>2.0726481481481481E-3</v>
       </c>
       <c r="X104" s="62">
         <f t="shared" si="11"/>
-        <v>2.090231481481482E-3</v>
+        <v>1.8972870370370372E-3</v>
       </c>
     </row>
     <row r="105" spans="1:24" x14ac:dyDescent="0.45">
@@ -26336,130 +26486,508 @@
       </c>
       <c r="M105" s="62">
         <f>NK!$Z$14</f>
-        <v>5.3504629629629627E-4</v>
+        <v>4.8565740740740736E-4</v>
       </c>
       <c r="N105" s="62">
         <f>NK!$Z$16</f>
-        <v>8.3988425925925929E-4</v>
+        <v>7.6235648148148148E-4</v>
       </c>
       <c r="O105" s="62">
         <f>NK!$Z$15</f>
-        <v>1.101087962962963E-3</v>
+        <v>9.9944907407407404E-4</v>
       </c>
       <c r="P105" s="62">
         <f>NK!$Z$17</f>
-        <v>9.181250000000001E-4</v>
+        <v>8.3337500000000002E-4</v>
       </c>
       <c r="Q105" s="62">
         <f>NK!$Z$19</f>
-        <v>2.2396412037037038E-3</v>
+        <v>2.0329050925925922E-3</v>
       </c>
       <c r="R105" s="62">
         <f>NK!$Z$18</f>
-        <v>2.0694675925925924E-3</v>
+        <v>1.8784398148148146E-3</v>
       </c>
       <c r="S105" s="62">
         <f t="shared" si="12"/>
-        <v>5.3504629629629627E-4</v>
+        <v>4.8565740740740736E-4</v>
       </c>
       <c r="T105" s="62">
         <f t="shared" si="7"/>
-        <v>8.3988425925925929E-4</v>
+        <v>7.6235648148148148E-4</v>
       </c>
       <c r="U105" s="62">
         <f t="shared" si="8"/>
-        <v>1.101087962962963E-3</v>
+        <v>9.9944907407407404E-4</v>
       </c>
       <c r="V105" s="62">
         <f t="shared" si="9"/>
-        <v>9.181250000000001E-4</v>
+        <v>8.3337500000000002E-4</v>
       </c>
       <c r="W105" s="62">
         <f t="shared" si="10"/>
-        <v>2.2396412037037038E-3</v>
+        <v>2.0329050925925922E-3</v>
       </c>
       <c r="X105" s="62">
         <f t="shared" si="11"/>
-        <v>2.0694675925925924E-3</v>
+        <v>1.8784398148148146E-3</v>
       </c>
     </row>
     <row r="106" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A106" s="59"/>
-      <c r="B106" s="59"/>
-      <c r="C106" s="59"/>
-      <c r="D106" s="59"/>
-      <c r="E106" s="61"/>
-      <c r="F106" s="61"/>
-      <c r="G106" s="61"/>
-      <c r="H106" s="59"/>
-      <c r="I106" s="59"/>
+      <c r="A106" s="59" t="s">
+        <v>273</v>
+      </c>
+      <c r="B106" s="59" t="s">
+        <v>182</v>
+      </c>
+      <c r="C106" s="59">
+        <v>19</v>
+      </c>
+      <c r="D106" s="59">
+        <v>19</v>
+      </c>
+      <c r="E106" s="61">
+        <v>45658</v>
+      </c>
+      <c r="F106" s="61">
+        <v>46174</v>
+      </c>
+      <c r="G106" s="61">
+        <v>45658</v>
+      </c>
+      <c r="H106" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="I106" s="59" t="s">
+        <v>180</v>
+      </c>
       <c r="J106" s="59"/>
       <c r="K106" s="59"/>
-      <c r="L106" s="59"/>
-      <c r="M106" s="62"/>
-      <c r="N106" s="62"/>
-      <c r="O106" s="62"/>
-      <c r="P106" s="62"/>
-      <c r="Q106" s="62"/>
-      <c r="R106" s="62"/>
-      <c r="S106" s="62"/>
-      <c r="T106" s="62"/>
-      <c r="U106" s="62"/>
-      <c r="V106" s="62"/>
-      <c r="W106" s="62"/>
-      <c r="X106" s="62"/>
+      <c r="L106" s="59">
+        <v>10</v>
+      </c>
+      <c r="M106" s="62">
+        <v>4.5043055555555553E-4</v>
+      </c>
+      <c r="N106" s="62">
+        <v>7.1251736111111103E-4</v>
+      </c>
+      <c r="O106" s="62">
+        <v>9.6791319444444431E-4</v>
+      </c>
+      <c r="P106" s="62">
+        <v>8.1174305555555557E-4</v>
+      </c>
+      <c r="Q106" s="62">
+        <v>2.0068645833333332E-3</v>
+      </c>
+      <c r="R106" s="62">
+        <v>1.8361736111111109E-3</v>
+      </c>
+      <c r="S106" s="62">
+        <f t="shared" ref="S106:X111" si="13">M106</f>
+        <v>4.5043055555555553E-4</v>
+      </c>
+      <c r="T106" s="62">
+        <f t="shared" si="7"/>
+        <v>7.1251736111111103E-4</v>
+      </c>
+      <c r="U106" s="62">
+        <f t="shared" si="8"/>
+        <v>9.6791319444444431E-4</v>
+      </c>
+      <c r="V106" s="62">
+        <f t="shared" si="9"/>
+        <v>8.1174305555555557E-4</v>
+      </c>
+      <c r="W106" s="62">
+        <f t="shared" si="10"/>
+        <v>2.0068645833333332E-3</v>
+      </c>
+      <c r="X106" s="62">
+        <f t="shared" si="11"/>
+        <v>1.8361736111111109E-3</v>
+      </c>
     </row>
     <row r="107" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A107" s="59"/>
-      <c r="B107" s="59"/>
-      <c r="C107" s="59"/>
-      <c r="D107" s="59"/>
-      <c r="E107" s="61"/>
-      <c r="F107" s="61"/>
-      <c r="G107" s="61"/>
-      <c r="H107" s="59"/>
-      <c r="I107" s="59"/>
+      <c r="A107" s="59" t="s">
+        <v>273</v>
+      </c>
+      <c r="B107" s="59" t="s">
+        <v>182</v>
+      </c>
+      <c r="C107" s="59">
+        <v>20</v>
+      </c>
+      <c r="D107" s="59">
+        <v>22</v>
+      </c>
+      <c r="E107" s="61">
+        <v>45658</v>
+      </c>
+      <c r="F107" s="61">
+        <v>46174</v>
+      </c>
+      <c r="G107" s="61">
+        <v>45658</v>
+      </c>
+      <c r="H107" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="I107" s="59" t="s">
+        <v>180</v>
+      </c>
       <c r="J107" s="59"/>
       <c r="K107" s="59"/>
-      <c r="L107" s="59"/>
-      <c r="M107" s="62"/>
-      <c r="N107" s="62"/>
-      <c r="O107" s="62"/>
-      <c r="P107" s="62"/>
-      <c r="Q107" s="62"/>
-      <c r="R107" s="62"/>
-      <c r="S107" s="62"/>
-      <c r="T107" s="62"/>
-      <c r="U107" s="62"/>
-      <c r="V107" s="62"/>
-      <c r="W107" s="62"/>
-      <c r="X107" s="62"/>
+      <c r="L107" s="59">
+        <v>10</v>
+      </c>
+      <c r="M107" s="62">
+        <v>4.5541319444444443E-4</v>
+      </c>
+      <c r="N107" s="62">
+        <v>7.1949305555555558E-4</v>
+      </c>
+      <c r="O107" s="62">
+        <v>9.8200694444444442E-4</v>
+      </c>
+      <c r="P107" s="62">
+        <v>8.2925347222222222E-4</v>
+      </c>
+      <c r="Q107" s="62">
+        <v>2.0306388888888887E-3</v>
+      </c>
+      <c r="R107" s="62">
+        <v>1.8578124999999999E-3</v>
+      </c>
+      <c r="S107" s="62">
+        <f t="shared" si="13"/>
+        <v>4.5541319444444443E-4</v>
+      </c>
+      <c r="T107" s="62">
+        <f t="shared" si="7"/>
+        <v>7.1949305555555558E-4</v>
+      </c>
+      <c r="U107" s="62">
+        <f t="shared" si="8"/>
+        <v>9.8200694444444442E-4</v>
+      </c>
+      <c r="V107" s="62">
+        <f t="shared" si="9"/>
+        <v>8.2925347222222222E-4</v>
+      </c>
+      <c r="W107" s="62">
+        <f t="shared" si="10"/>
+        <v>2.0306388888888887E-3</v>
+      </c>
+      <c r="X107" s="62">
+        <f t="shared" si="11"/>
+        <v>1.8578124999999999E-3</v>
+      </c>
     </row>
     <row r="108" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A108" s="59"/>
-      <c r="B108" s="59"/>
-      <c r="C108" s="59"/>
-      <c r="D108" s="59"/>
-      <c r="E108" s="61"/>
-      <c r="F108" s="61"/>
-      <c r="G108" s="61"/>
-      <c r="H108" s="59"/>
-      <c r="I108" s="59"/>
+      <c r="A108" s="59" t="s">
+        <v>273</v>
+      </c>
+      <c r="B108" s="59" t="s">
+        <v>182</v>
+      </c>
+      <c r="C108" s="59">
+        <v>23</v>
+      </c>
+      <c r="D108" s="59">
+        <v>40</v>
+      </c>
+      <c r="E108" s="61">
+        <v>45658</v>
+      </c>
+      <c r="F108" s="61">
+        <v>46174</v>
+      </c>
+      <c r="G108" s="61">
+        <v>45658</v>
+      </c>
+      <c r="H108" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="I108" s="59" t="s">
+        <v>180</v>
+      </c>
       <c r="J108" s="59"/>
       <c r="K108" s="59"/>
-      <c r="L108" s="59"/>
-      <c r="M108" s="62"/>
-      <c r="N108" s="62"/>
-      <c r="O108" s="62"/>
-      <c r="P108" s="62"/>
-      <c r="Q108" s="62"/>
-      <c r="R108" s="62"/>
-      <c r="S108" s="62"/>
-      <c r="T108" s="62"/>
-      <c r="U108" s="62"/>
-      <c r="V108" s="62"/>
-      <c r="W108" s="62"/>
-      <c r="X108" s="62"/>
+      <c r="L108" s="59">
+        <v>10</v>
+      </c>
+      <c r="M108" s="62">
+        <v>4.5982638888888885E-4</v>
+      </c>
+      <c r="N108" s="62">
+        <v>7.2604166666666661E-4</v>
+      </c>
+      <c r="O108" s="62">
+        <v>9.9510416666666671E-4</v>
+      </c>
+      <c r="P108" s="62">
+        <v>8.4534027777777786E-4</v>
+      </c>
+      <c r="Q108" s="62">
+        <v>2.052704861111111E-3</v>
+      </c>
+      <c r="R108" s="62">
+        <v>1.8777430555555557E-3</v>
+      </c>
+      <c r="S108" s="62">
+        <f t="shared" si="13"/>
+        <v>4.5982638888888885E-4</v>
+      </c>
+      <c r="T108" s="62">
+        <f t="shared" si="7"/>
+        <v>7.2604166666666661E-4</v>
+      </c>
+      <c r="U108" s="62">
+        <f t="shared" si="8"/>
+        <v>9.9510416666666671E-4</v>
+      </c>
+      <c r="V108" s="62">
+        <f t="shared" si="9"/>
+        <v>8.4534027777777786E-4</v>
+      </c>
+      <c r="W108" s="62">
+        <f t="shared" si="10"/>
+        <v>2.052704861111111E-3</v>
+      </c>
+      <c r="X108" s="62">
+        <f t="shared" si="11"/>
+        <v>1.8777430555555557E-3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A109" s="59" t="s">
+        <v>274</v>
+      </c>
+      <c r="B109" s="59" t="s">
+        <v>164</v>
+      </c>
+      <c r="C109" s="59">
+        <v>19</v>
+      </c>
+      <c r="D109" s="59">
+        <v>19</v>
+      </c>
+      <c r="E109" s="61">
+        <v>45658</v>
+      </c>
+      <c r="F109" s="61">
+        <v>46174</v>
+      </c>
+      <c r="G109" s="61">
+        <v>45658</v>
+      </c>
+      <c r="H109" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="I109" s="59" t="s">
+        <v>180</v>
+      </c>
+      <c r="J109" s="59"/>
+      <c r="K109" s="59"/>
+      <c r="L109" s="59">
+        <v>10</v>
+      </c>
+      <c r="M109" s="62">
+        <v>5.3455092592592595E-4</v>
+      </c>
+      <c r="N109" s="62">
+        <v>8.0442129629629624E-4</v>
+      </c>
+      <c r="O109" s="62">
+        <v>1.0879490740740739E-3</v>
+      </c>
+      <c r="P109" s="62">
+        <v>8.9346759259259251E-4</v>
+      </c>
+      <c r="Q109" s="62">
+        <v>2.1059722222222218E-3</v>
+      </c>
+      <c r="R109" s="62">
+        <v>1.9128564814814813E-3</v>
+      </c>
+      <c r="S109" s="62">
+        <f t="shared" si="13"/>
+        <v>5.3455092592592595E-4</v>
+      </c>
+      <c r="T109" s="62">
+        <f t="shared" si="7"/>
+        <v>8.0442129629629624E-4</v>
+      </c>
+      <c r="U109" s="62">
+        <f t="shared" si="8"/>
+        <v>1.0879490740740739E-3</v>
+      </c>
+      <c r="V109" s="62">
+        <f t="shared" si="9"/>
+        <v>8.9346759259259251E-4</v>
+      </c>
+      <c r="W109" s="62">
+        <f t="shared" si="10"/>
+        <v>2.1059722222222218E-3</v>
+      </c>
+      <c r="X109" s="62">
+        <f t="shared" si="11"/>
+        <v>1.9128564814814813E-3</v>
+      </c>
+    </row>
+    <row r="110" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A110" s="59" t="s">
+        <v>274</v>
+      </c>
+      <c r="B110" s="59" t="s">
+        <v>164</v>
+      </c>
+      <c r="C110" s="59">
+        <v>20</v>
+      </c>
+      <c r="D110" s="59">
+        <v>22</v>
+      </c>
+      <c r="E110" s="61">
+        <v>45658</v>
+      </c>
+      <c r="F110" s="61">
+        <v>46174</v>
+      </c>
+      <c r="G110" s="61">
+        <v>45658</v>
+      </c>
+      <c r="H110" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="I110" s="59" t="s">
+        <v>180</v>
+      </c>
+      <c r="J110" s="59"/>
+      <c r="K110" s="59"/>
+      <c r="L110" s="59">
+        <v>10</v>
+      </c>
+      <c r="M110" s="62">
+        <v>5.4534027777777773E-4</v>
+      </c>
+      <c r="N110" s="62">
+        <v>8.1357175925925933E-4</v>
+      </c>
+      <c r="O110" s="62">
+        <v>1.1074791666666668E-3</v>
+      </c>
+      <c r="P110" s="62">
+        <v>9.065787037037035E-4</v>
+      </c>
+      <c r="Q110" s="62">
+        <v>2.1215416666666665E-3</v>
+      </c>
+      <c r="R110" s="62">
+        <v>1.9200949074074073E-3</v>
+      </c>
+      <c r="S110" s="62">
+        <f t="shared" si="13"/>
+        <v>5.4534027777777773E-4</v>
+      </c>
+      <c r="T110" s="62">
+        <f t="shared" si="7"/>
+        <v>8.1357175925925933E-4</v>
+      </c>
+      <c r="U110" s="62">
+        <f t="shared" si="8"/>
+        <v>1.1074791666666668E-3</v>
+      </c>
+      <c r="V110" s="62">
+        <f t="shared" si="9"/>
+        <v>9.065787037037035E-4</v>
+      </c>
+      <c r="W110" s="62">
+        <f t="shared" si="10"/>
+        <v>2.1215416666666665E-3</v>
+      </c>
+      <c r="X110" s="62">
+        <f t="shared" si="11"/>
+        <v>1.9200949074074073E-3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A111" s="59" t="s">
+        <v>274</v>
+      </c>
+      <c r="B111" s="59" t="s">
+        <v>164</v>
+      </c>
+      <c r="C111" s="59">
+        <v>23</v>
+      </c>
+      <c r="D111" s="59">
+        <v>40</v>
+      </c>
+      <c r="E111" s="61">
+        <v>45658</v>
+      </c>
+      <c r="F111" s="61">
+        <v>46174</v>
+      </c>
+      <c r="G111" s="61">
+        <v>45658</v>
+      </c>
+      <c r="H111" s="59" t="s">
+        <v>178</v>
+      </c>
+      <c r="I111" s="59" t="s">
+        <v>180</v>
+      </c>
+      <c r="J111" s="59"/>
+      <c r="K111" s="59"/>
+      <c r="L111" s="59">
+        <v>10</v>
+      </c>
+      <c r="M111" s="62">
+        <v>5.5558333333333328E-4</v>
+      </c>
+      <c r="N111" s="62">
+        <v>8.2203935185185179E-4</v>
+      </c>
+      <c r="O111" s="62">
+        <v>1.1255069444444444E-3</v>
+      </c>
+      <c r="P111" s="62">
+        <v>9.1859722222222223E-4</v>
+      </c>
+      <c r="Q111" s="62">
+        <v>2.1360185185185184E-3</v>
+      </c>
+      <c r="R111" s="62">
+        <v>1.9267870370370367E-3</v>
+      </c>
+      <c r="S111" s="62">
+        <f t="shared" si="13"/>
+        <v>5.5558333333333328E-4</v>
+      </c>
+      <c r="T111" s="62">
+        <f t="shared" si="7"/>
+        <v>8.2203935185185179E-4</v>
+      </c>
+      <c r="U111" s="62">
+        <f t="shared" si="8"/>
+        <v>1.1255069444444444E-3</v>
+      </c>
+      <c r="V111" s="62">
+        <f t="shared" si="9"/>
+        <v>9.1859722222222223E-4</v>
+      </c>
+      <c r="W111" s="62">
+        <f t="shared" si="10"/>
+        <v>2.1360185185185184E-3</v>
+      </c>
+      <c r="X111" s="62">
+        <f t="shared" si="11"/>
+        <v>1.9267870370370367E-3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -26474,8 +27002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A13DA696-49DD-4BFA-98FE-5C7770404E50}">
   <dimension ref="B3:AA37"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="W20" sqref="W20"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -26938,72 +27466,72 @@
       </c>
       <c r="C14" s="65">
         <f>C5*$F14</f>
-        <v>4.6730324074074068E-4</v>
+        <v>4.5982638888888885E-4</v>
       </c>
       <c r="D14" s="65">
         <f t="shared" ref="D14:E14" si="0">D5*$F14</f>
-        <v>4.6281828703703703E-4</v>
+        <v>4.5541319444444443E-4</v>
       </c>
       <c r="E14" s="65">
         <f t="shared" si="0"/>
-        <v>4.5775462962962962E-4</v>
+        <v>4.5043055555555553E-4</v>
       </c>
       <c r="F14">
-        <v>1.25</v>
+        <v>1.23</v>
       </c>
       <c r="H14" s="64" t="s">
         <v>0</v>
       </c>
       <c r="I14" s="65">
         <f>I5*$L14</f>
-        <v>5.8854166666666668E-4</v>
+        <v>5.5558333333333328E-4</v>
       </c>
       <c r="J14" s="65">
         <f t="shared" ref="J14:K14" si="1">J5*$L14</f>
-        <v>5.7769097222222228E-4</v>
+        <v>5.4534027777777773E-4</v>
       </c>
       <c r="K14" s="65">
         <f t="shared" si="1"/>
-        <v>5.6626157407407406E-4</v>
+        <v>5.3455092592592595E-4</v>
       </c>
       <c r="L14">
-        <v>1.25</v>
+        <v>1.18</v>
       </c>
       <c r="Q14" s="64" t="s">
         <v>0</v>
       </c>
       <c r="R14" s="65">
         <f t="shared" ref="R14:T19" si="2">R5*$U14</f>
-        <v>4.6944444444444442E-4</v>
+        <v>4.0805555555555549E-4</v>
       </c>
       <c r="S14" s="65">
         <f t="shared" si="2"/>
-        <v>4.6523148148148151E-4</v>
+        <v>4.043935185185185E-4</v>
       </c>
       <c r="T14" s="65">
         <f t="shared" si="2"/>
-        <v>4.5244212962962968E-4</v>
+        <v>3.9327662037037033E-4</v>
       </c>
       <c r="U14">
-        <v>1.3</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="W14" s="64" t="s">
         <v>0</v>
       </c>
       <c r="X14" s="65">
         <f>X5*$AA14</f>
-        <v>5.73263888888889E-4</v>
+        <v>5.2034722222222228E-4</v>
       </c>
       <c r="Y14" s="65">
         <f t="shared" ref="Y14:Z14" si="3">Y5*$AA14</f>
-        <v>5.6393518518518522E-4</v>
+        <v>5.118796296296296E-4</v>
       </c>
       <c r="Z14" s="65">
         <f t="shared" si="3"/>
-        <v>5.3504629629629627E-4</v>
+        <v>4.8565740740740736E-4</v>
       </c>
       <c r="AA14">
-        <v>1.3</v>
+        <v>1.18</v>
       </c>
     </row>
     <row r="15" spans="2:27" x14ac:dyDescent="0.45">
@@ -27012,72 +27540,72 @@
       </c>
       <c r="C15" s="65">
         <f t="shared" ref="C15:E15" si="4">C6*$F15</f>
-        <v>1.0112847222222224E-3</v>
+        <v>9.9510416666666671E-4</v>
       </c>
       <c r="D15" s="65">
         <f t="shared" si="4"/>
-        <v>9.9797453703703702E-4</v>
+        <v>9.8200694444444442E-4</v>
       </c>
       <c r="E15" s="65">
         <f t="shared" si="4"/>
-        <v>9.8365162037037019E-4</v>
+        <v>9.6791319444444431E-4</v>
       </c>
       <c r="F15">
-        <v>1.25</v>
+        <v>1.23</v>
       </c>
       <c r="H15" s="64" t="s">
         <v>223</v>
       </c>
       <c r="I15" s="65">
         <f t="shared" ref="I15:K15" si="5">I6*$L15</f>
-        <v>1.1922743055555556E-3</v>
+        <v>1.1255069444444444E-3</v>
       </c>
       <c r="J15" s="65">
         <f t="shared" si="5"/>
-        <v>1.1731770833333334E-3</v>
+        <v>1.1074791666666668E-3</v>
       </c>
       <c r="K15" s="65">
         <f t="shared" si="5"/>
-        <v>1.1524884259259259E-3</v>
+        <v>1.0879490740740739E-3</v>
       </c>
       <c r="L15">
-        <v>1.25</v>
+        <v>1.18</v>
       </c>
       <c r="Q15" s="64" t="s">
         <v>223</v>
       </c>
       <c r="R15" s="65">
         <f t="shared" si="2"/>
-        <v>1.0034375E-3</v>
+        <v>8.7221874999999995E-4</v>
       </c>
       <c r="S15" s="65">
         <f t="shared" si="2"/>
-        <v>9.9155092592592611E-4</v>
+        <v>8.6188657407407405E-4</v>
       </c>
       <c r="T15" s="65">
         <f t="shared" si="2"/>
-        <v>9.5453703703703705E-4</v>
+        <v>8.2971296296296287E-4</v>
       </c>
       <c r="U15">
-        <v>1.3</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="W15" s="64" t="s">
         <v>223</v>
       </c>
       <c r="X15" s="65">
         <f t="shared" ref="X15:Z15" si="6">X6*$AA15</f>
-        <v>1.1704513888888888E-3</v>
+        <v>1.062409722222222E-3</v>
       </c>
       <c r="Y15" s="65">
         <f t="shared" si="6"/>
-        <v>1.1534490740740741E-3</v>
+        <v>1.0469768518518517E-3</v>
       </c>
       <c r="Z15" s="65">
         <f t="shared" si="6"/>
-        <v>1.101087962962963E-3</v>
+        <v>9.9944907407407404E-4</v>
       </c>
       <c r="AA15">
-        <v>1.3</v>
+        <v>1.18</v>
       </c>
     </row>
     <row r="16" spans="2:27" x14ac:dyDescent="0.45">
@@ -27086,72 +27614,72 @@
       </c>
       <c r="C16" s="65">
         <f t="shared" ref="C16:E16" si="7">C7*$F16</f>
-        <v>7.378472222222222E-4</v>
+        <v>7.2604166666666661E-4</v>
       </c>
       <c r="D16" s="65">
         <f t="shared" si="7"/>
-        <v>7.311921296296297E-4</v>
+        <v>7.1949305555555558E-4</v>
       </c>
       <c r="E16" s="65">
         <f t="shared" si="7"/>
-        <v>7.2410300925925919E-4</v>
+        <v>7.1251736111111103E-4</v>
       </c>
       <c r="F16">
-        <v>1.25</v>
+        <v>1.23</v>
       </c>
       <c r="H16" s="64" t="s">
         <v>224</v>
       </c>
       <c r="I16" s="65">
         <f t="shared" ref="I16:K16" si="8">I7*$L16</f>
-        <v>8.7080439814814811E-4</v>
+        <v>8.2203935185185179E-4</v>
       </c>
       <c r="J16" s="65">
         <f t="shared" si="8"/>
-        <v>8.6183449074074081E-4</v>
+        <v>8.1357175925925933E-4</v>
       </c>
       <c r="K16" s="65">
         <f t="shared" si="8"/>
-        <v>8.521412037037037E-4</v>
+        <v>8.0442129629629624E-4</v>
       </c>
       <c r="L16">
-        <v>1.25</v>
+        <v>1.18</v>
       </c>
       <c r="Q16" s="64" t="s">
         <v>224</v>
       </c>
       <c r="R16" s="65">
         <f t="shared" si="2"/>
-        <v>7.4328703703703709E-4</v>
+        <v>6.4608796296296289E-4</v>
       </c>
       <c r="S16" s="65">
         <f t="shared" si="2"/>
-        <v>7.3726851851851861E-4</v>
+        <v>6.4085648148148151E-4</v>
       </c>
       <c r="T16" s="65">
         <f t="shared" si="2"/>
-        <v>7.1846064814814819E-4</v>
+        <v>6.2450810185185179E-4</v>
       </c>
       <c r="U16">
-        <v>1.3</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="W16" s="64" t="s">
         <v>224</v>
       </c>
       <c r="X16" s="65">
         <f t="shared" ref="X16:Z16" si="9">X7*$AA16</f>
-        <v>8.7313657407407414E-4</v>
+        <v>7.9253935185185189E-4</v>
       </c>
       <c r="Y16" s="65">
         <f t="shared" si="9"/>
-        <v>8.6501157407407403E-4</v>
+        <v>7.8516435185185178E-4</v>
       </c>
       <c r="Z16" s="65">
         <f t="shared" si="9"/>
-        <v>8.3988425925925929E-4</v>
+        <v>7.6235648148148148E-4</v>
       </c>
       <c r="AA16">
-        <v>1.3</v>
+        <v>1.18</v>
       </c>
     </row>
     <row r="17" spans="2:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -27160,72 +27688,72 @@
       </c>
       <c r="C17" s="65">
         <f t="shared" ref="C17:E17" si="10">C8*$F17</f>
-        <v>8.5908564814814821E-4</v>
+        <v>8.4534027777777786E-4</v>
       </c>
       <c r="D17" s="65">
         <f t="shared" si="10"/>
-        <v>8.427372685185186E-4</v>
+        <v>8.2925347222222222E-4</v>
       </c>
       <c r="E17" s="65">
         <f t="shared" si="10"/>
-        <v>8.2494212962962968E-4</v>
+        <v>8.1174305555555557E-4</v>
       </c>
       <c r="F17">
-        <v>1.25</v>
+        <v>1.23</v>
       </c>
       <c r="H17" s="64" t="s">
         <v>225</v>
       </c>
       <c r="I17" s="65">
         <f t="shared" ref="I17:K17" si="11">I8*$L17</f>
-        <v>9.730902777777778E-4</v>
+        <v>9.1859722222222223E-4</v>
       </c>
       <c r="J17" s="65">
         <f t="shared" si="11"/>
-        <v>9.6035879629629618E-4</v>
+        <v>9.065787037037035E-4</v>
       </c>
       <c r="K17" s="65">
         <f t="shared" si="11"/>
-        <v>9.4646990740740737E-4</v>
+        <v>8.9346759259259251E-4</v>
       </c>
       <c r="L17">
-        <v>1.25</v>
+        <v>1.18</v>
       </c>
       <c r="Q17" s="64" t="s">
         <v>225</v>
       </c>
       <c r="R17" s="65">
         <f t="shared" si="2"/>
-        <v>8.3371527777777773E-4</v>
+        <v>7.2469097222222206E-4</v>
       </c>
       <c r="S17" s="65">
         <f t="shared" si="2"/>
-        <v>8.1927083333333331E-4</v>
+        <v>7.1213541666666658E-4</v>
       </c>
       <c r="T17" s="65">
         <f t="shared" si="2"/>
-        <v>7.7473379629629626E-4</v>
+        <v>6.7342245370370364E-4</v>
       </c>
       <c r="U17">
-        <v>1.3</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="W17" s="64" t="s">
         <v>225</v>
       </c>
       <c r="X17" s="65">
         <f t="shared" ref="X17:Z17" si="12">X8*$AA17</f>
-        <v>9.6537037037037034E-4</v>
+        <v>8.7625925925925914E-4</v>
       </c>
       <c r="Y17" s="65">
         <f t="shared" si="12"/>
-        <v>9.5378472222222229E-4</v>
+        <v>8.6574305555555547E-4</v>
       </c>
       <c r="Z17" s="65">
         <f t="shared" si="12"/>
-        <v>9.181250000000001E-4</v>
+        <v>8.3337500000000002E-4</v>
       </c>
       <c r="AA17">
-        <v>1.3</v>
+        <v>1.18</v>
       </c>
     </row>
     <row r="18" spans="2:27" x14ac:dyDescent="0.45">
@@ -27234,72 +27762,72 @@
       </c>
       <c r="C18" s="65">
         <f t="shared" ref="C18:E18" si="13">C9*$F18</f>
-        <v>1.9082754629629632E-3</v>
+        <v>1.8777430555555557E-3</v>
       </c>
       <c r="D18" s="65">
         <f t="shared" si="13"/>
-        <v>1.8880208333333333E-3</v>
+        <v>1.8578124999999999E-3</v>
       </c>
       <c r="E18" s="65">
         <f t="shared" si="13"/>
-        <v>1.8660300925925923E-3</v>
+        <v>1.8361736111111109E-3</v>
       </c>
       <c r="F18">
-        <v>1.25</v>
+        <v>1.23</v>
       </c>
       <c r="H18" s="64" t="s">
         <v>226</v>
       </c>
       <c r="I18" s="65">
         <f t="shared" ref="I18:K18" si="14">I9*$L18</f>
-        <v>2.0410879629629629E-3</v>
+        <v>1.9267870370370367E-3</v>
       </c>
       <c r="J18" s="65">
         <f t="shared" si="14"/>
-        <v>2.0339988425925925E-3</v>
+        <v>1.9200949074074073E-3</v>
       </c>
       <c r="K18" s="65">
         <f t="shared" si="14"/>
-        <v>2.0263310185185185E-3</v>
+        <v>1.9128564814814813E-3</v>
       </c>
       <c r="L18">
-        <v>1.25</v>
+        <v>1.18</v>
       </c>
       <c r="Q18" s="64" t="s">
         <v>226</v>
       </c>
       <c r="R18" s="65">
         <f t="shared" si="2"/>
-        <v>1.9107291666666667E-3</v>
+        <v>1.660864583333333E-3</v>
       </c>
       <c r="S18" s="65">
         <f t="shared" si="2"/>
-        <v>1.8922222222222224E-3</v>
+        <v>1.6447777777777778E-3</v>
       </c>
       <c r="T18" s="65">
         <f t="shared" si="2"/>
-        <v>1.8350462962962962E-3</v>
+        <v>1.5950787037037034E-3</v>
       </c>
       <c r="U18">
-        <v>1.3</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="W18" s="64" t="s">
         <v>226</v>
       </c>
       <c r="X18" s="65">
         <f t="shared" ref="X18:Z18" si="15">X9*$AA18</f>
-        <v>2.0968518518518523E-3</v>
+        <v>1.9032962962962964E-3</v>
       </c>
       <c r="Y18" s="65">
         <f t="shared" si="15"/>
-        <v>2.090231481481482E-3</v>
+        <v>1.8972870370370372E-3</v>
       </c>
       <c r="Z18" s="65">
         <f t="shared" si="15"/>
-        <v>2.0694675925925924E-3</v>
+        <v>1.8784398148148146E-3</v>
       </c>
       <c r="AA18">
-        <v>1.3</v>
+        <v>1.18</v>
       </c>
     </row>
     <row r="19" spans="2:27" x14ac:dyDescent="0.45">
@@ -27308,72 +27836,72 @@
       </c>
       <c r="C19" s="65">
         <f t="shared" ref="C19:E19" si="16">C10*$F19</f>
-        <v>2.0860821759259261E-3</v>
+        <v>2.052704861111111E-3</v>
       </c>
       <c r="D19" s="65">
         <f t="shared" si="16"/>
-        <v>2.0636574074074073E-3</v>
+        <v>2.0306388888888887E-3</v>
       </c>
       <c r="E19" s="65">
         <f t="shared" si="16"/>
-        <v>2.0394965277777777E-3</v>
+        <v>2.0068645833333332E-3</v>
       </c>
       <c r="F19">
-        <v>1.25</v>
+        <v>1.23</v>
       </c>
       <c r="H19" s="64" t="s">
         <v>4</v>
       </c>
       <c r="I19" s="65">
         <f t="shared" ref="I19:K19" si="17">I10*$L19</f>
-        <v>2.2627314814814815E-3</v>
+        <v>2.1360185185185184E-3</v>
       </c>
       <c r="J19" s="65">
         <f t="shared" si="17"/>
-        <v>2.2473958333333335E-3</v>
+        <v>2.1215416666666665E-3</v>
       </c>
       <c r="K19" s="65">
         <f t="shared" si="17"/>
-        <v>2.2309027777777774E-3</v>
+        <v>2.1059722222222218E-3</v>
       </c>
       <c r="L19">
-        <v>1.25</v>
+        <v>1.18</v>
       </c>
       <c r="Q19" s="64" t="s">
         <v>4</v>
       </c>
       <c r="R19" s="65">
         <f t="shared" si="2"/>
-        <v>2.0881250000000001E-3</v>
+        <v>1.8150624999999998E-3</v>
       </c>
       <c r="S19" s="65">
         <f t="shared" si="2"/>
-        <v>2.0678125000000002E-3</v>
+        <v>1.79740625E-3</v>
       </c>
       <c r="T19" s="65">
         <f t="shared" si="2"/>
-        <v>2.0049189814814817E-3</v>
+        <v>1.7427372685185185E-3</v>
       </c>
       <c r="U19">
-        <v>1.3</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="W19" s="64" t="s">
         <v>4</v>
       </c>
       <c r="X19" s="65">
         <f t="shared" ref="X19:Z19" si="18">X10*$AA19</f>
-        <v>2.2975694444444445E-3</v>
+        <v>2.0854861111111109E-3</v>
       </c>
       <c r="Y19" s="65">
         <f t="shared" si="18"/>
-        <v>2.2834259259259262E-3</v>
+        <v>2.0726481481481481E-3</v>
       </c>
       <c r="Z19" s="65">
         <f t="shared" si="18"/>
-        <v>2.2396412037037038E-3</v>
+        <v>2.0329050925925922E-3</v>
       </c>
       <c r="AA19">
-        <v>1.3</v>
+        <v>1.18</v>
       </c>
     </row>
     <row r="22" spans="2:27" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Rek Krit anpassen auf 6 / 8
</commit_message>
<xml_diff>
--- a/web/utilities/records_kriterien.xlsx
+++ b/web/utilities/records_kriterien.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgna\Documents\GitHub\Lifesaving_Baden\web\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A65A675-AC2D-4AF2-B9C5-1960DA778743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3A6B6D-28D3-429D-9596-6897B79B869C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="6" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="7" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
   </bookViews>
   <sheets>
     <sheet name="DR" sheetId="9" r:id="rId1"/>
@@ -1023,16 +1023,16 @@
     <t>&lt;2005</t>
   </si>
   <si>
-    <t>NK2 +10% Mäner</t>
-  </si>
-  <si>
-    <t>NK2 +10% Frauen</t>
-  </si>
-  <si>
-    <t>NK1 +10% Mäner</t>
-  </si>
-  <si>
-    <t>NK1 +10% Frauen</t>
+    <t>NK2 +18% Mäner</t>
+  </si>
+  <si>
+    <t>NK2 +18% Frauen</t>
+  </si>
+  <si>
+    <t>NK1 +13% Mäner</t>
+  </si>
+  <si>
+    <t>NK1 +13% Frauen</t>
   </si>
 </sst>
 </file>
@@ -1515,6 +1515,96 @@
   </cellStyles>
   <dxfs count="194">
     <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="6"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4"/>
+      </font>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="m:ss.00"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1606,96 +1696,6 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4"/>
-      </font>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="m:ss.00"/>
@@ -4166,7 +4166,7 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}" name="JRP_konfig" displayName="JRP_konfig" ref="A1:X99" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}" name="JRP_konfig" displayName="JRP_konfig" ref="A1:X99" totalsRowShown="0" headerRowDxfId="43" dataDxfId="42">
   <autoFilter ref="A1:X99" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4194,30 +4194,30 @@
     <filterColumn colId="23" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{021DA6E1-2C93-4474-9720-B6F016186D61}" name="Tabellen Name" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{733C1722-A9C9-4830-A9E2-FE62E96BCD98}" name="Geschlecht" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{80C0BF46-0E43-4947-BF86-B808C324772A}" name="Mindest Alter" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{DBA2A923-EEB7-43F9-A1A3-E78624448FB9}" name="Maximales Alter" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{3FDEE18A-328D-45AE-907D-69A916A93345}" name="Qualizeitraum anfang" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{BE002D7F-575F-4B60-9251-C71D93F59045}" name="Qualizeitraum Ende" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{208ABD57-DE4B-41D6-B9FC-93F2D8966E8D}" name="Letzter Wettkampf am" dataDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{30C9697C-6550-4996-ADDB-7FEE5325B794}" name="Landesverband" dataDxfId="16"/>
-    <tableColumn id="9" xr3:uid="{ED2DAB77-EF46-4D8B-B8E4-90412E32E277}" name="OMS" dataDxfId="15"/>
-    <tableColumn id="10" xr3:uid="{AD534940-A91B-4A6E-9606-E3F3E517D401}" name="Pool-Länge" dataDxfId="14"/>
-    <tableColumn id="11" xr3:uid="{11F9D5D5-72FE-42CA-8624-01D513B4140F}" name="Regelwerk" dataDxfId="13"/>
-    <tableColumn id="12" xr3:uid="{3907872B-5438-4FBF-A045-3EF9EAACFC47}" name="Seiten Anzahl" dataDxfId="12"/>
-    <tableColumn id="13" xr3:uid="{FC821324-3638-40C0-BA1E-069B44E23C7A}" name="PZ1 - 50m Retten" dataDxfId="11"/>
-    <tableColumn id="14" xr3:uid="{70529619-443E-40D3-88C1-3E0F00BB2A50}" name="PZ1 - 100m Retten" dataDxfId="10"/>
-    <tableColumn id="15" xr3:uid="{EFA92FD2-C23F-42B3-83DC-5036513F19AF}" name="PZ1 - 100m Kombi" dataDxfId="9"/>
-    <tableColumn id="16" xr3:uid="{03309E52-8CF3-4E90-9EE6-A818901C3B32}" name="PZ1 - 100m Lifesaver" dataDxfId="8"/>
-    <tableColumn id="17" xr3:uid="{00B22013-AA11-4C17-9250-22060AE4B0A8}" name="PZ1 - 200m Super-Lifesaver" dataDxfId="7"/>
-    <tableColumn id="18" xr3:uid="{7E3508A9-0422-4561-A23E-53E613259B24}" name="PZ1 - 200m Hindernis" dataDxfId="6"/>
-    <tableColumn id="19" xr3:uid="{5CEA435F-F34B-4D8D-88D0-F5EBFF18B713}" name="PZ2 - 50m Retten" dataDxfId="5"/>
-    <tableColumn id="20" xr3:uid="{8585BE62-F7C4-4D5D-B287-052B43B08610}" name="PZ2 - 100m Retten" dataDxfId="4"/>
-    <tableColumn id="21" xr3:uid="{D981758B-ADAD-4E36-B787-0B0FDA808CA2}" name="PZ2 - 100m Kombi" dataDxfId="3"/>
-    <tableColumn id="22" xr3:uid="{1D4970A8-D22F-4962-934C-AEA295ED687A}" name="PZ2 - 100m Lifesaver" dataDxfId="2"/>
-    <tableColumn id="23" xr3:uid="{BE394430-C58F-4690-9615-44475E5AF9F8}" name="PZ2 - 200m Super-Lifesaver" dataDxfId="1"/>
-    <tableColumn id="24" xr3:uid="{A7036B1A-99CE-4F7C-AAB8-12E8B2696202}" name="PZ2 - 200m Hindernis" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{021DA6E1-2C93-4474-9720-B6F016186D61}" name="Tabellen Name" dataDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{733C1722-A9C9-4830-A9E2-FE62E96BCD98}" name="Geschlecht" dataDxfId="40"/>
+    <tableColumn id="3" xr3:uid="{80C0BF46-0E43-4947-BF86-B808C324772A}" name="Mindest Alter" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{DBA2A923-EEB7-43F9-A1A3-E78624448FB9}" name="Maximales Alter" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{3FDEE18A-328D-45AE-907D-69A916A93345}" name="Qualizeitraum anfang" dataDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{BE002D7F-575F-4B60-9251-C71D93F59045}" name="Qualizeitraum Ende" dataDxfId="36"/>
+    <tableColumn id="7" xr3:uid="{208ABD57-DE4B-41D6-B9FC-93F2D8966E8D}" name="Letzter Wettkampf am" dataDxfId="35"/>
+    <tableColumn id="8" xr3:uid="{30C9697C-6550-4996-ADDB-7FEE5325B794}" name="Landesverband" dataDxfId="34"/>
+    <tableColumn id="9" xr3:uid="{ED2DAB77-EF46-4D8B-B8E4-90412E32E277}" name="OMS" dataDxfId="33"/>
+    <tableColumn id="10" xr3:uid="{AD534940-A91B-4A6E-9606-E3F3E517D401}" name="Pool-Länge" dataDxfId="32"/>
+    <tableColumn id="11" xr3:uid="{11F9D5D5-72FE-42CA-8624-01D513B4140F}" name="Regelwerk" dataDxfId="31"/>
+    <tableColumn id="12" xr3:uid="{3907872B-5438-4FBF-A045-3EF9EAACFC47}" name="Seiten Anzahl" dataDxfId="30"/>
+    <tableColumn id="13" xr3:uid="{FC821324-3638-40C0-BA1E-069B44E23C7A}" name="PZ1 - 50m Retten" dataDxfId="29"/>
+    <tableColumn id="14" xr3:uid="{70529619-443E-40D3-88C1-3E0F00BB2A50}" name="PZ1 - 100m Retten" dataDxfId="28"/>
+    <tableColumn id="15" xr3:uid="{EFA92FD2-C23F-42B3-83DC-5036513F19AF}" name="PZ1 - 100m Kombi" dataDxfId="27"/>
+    <tableColumn id="16" xr3:uid="{03309E52-8CF3-4E90-9EE6-A818901C3B32}" name="PZ1 - 100m Lifesaver" dataDxfId="26"/>
+    <tableColumn id="17" xr3:uid="{00B22013-AA11-4C17-9250-22060AE4B0A8}" name="PZ1 - 200m Super-Lifesaver" dataDxfId="25"/>
+    <tableColumn id="18" xr3:uid="{7E3508A9-0422-4561-A23E-53E613259B24}" name="PZ1 - 200m Hindernis" dataDxfId="24"/>
+    <tableColumn id="19" xr3:uid="{5CEA435F-F34B-4D8D-88D0-F5EBFF18B713}" name="PZ2 - 50m Retten" dataDxfId="23"/>
+    <tableColumn id="20" xr3:uid="{8585BE62-F7C4-4D5D-B287-052B43B08610}" name="PZ2 - 100m Retten" dataDxfId="22"/>
+    <tableColumn id="21" xr3:uid="{D981758B-ADAD-4E36-B787-0B0FDA808CA2}" name="PZ2 - 100m Kombi" dataDxfId="21"/>
+    <tableColumn id="22" xr3:uid="{1D4970A8-D22F-4962-934C-AEA295ED687A}" name="PZ2 - 100m Lifesaver" dataDxfId="20"/>
+    <tableColumn id="23" xr3:uid="{BE394430-C58F-4690-9615-44475E5AF9F8}" name="PZ2 - 200m Super-Lifesaver" dataDxfId="19"/>
+    <tableColumn id="24" xr3:uid="{A7036B1A-99CE-4F7C-AAB8-12E8B2696202}" name="PZ2 - 200m Hindernis" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8162,52 +8162,52 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B5:G31">
-    <cfRule type="expression" dxfId="43" priority="15">
+    <cfRule type="expression" dxfId="17" priority="15">
       <formula>B5&lt;&gt;B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:M31">
-    <cfRule type="expression" dxfId="42" priority="14">
+    <cfRule type="expression" dxfId="16" priority="14">
       <formula>H5&lt;&gt;H4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N5:S31">
-    <cfRule type="expression" dxfId="41" priority="13">
+    <cfRule type="expression" dxfId="15" priority="13">
       <formula>N5&lt;&gt;N4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T5:Y31">
-    <cfRule type="expression" dxfId="40" priority="12">
+    <cfRule type="expression" dxfId="14" priority="12">
       <formula>T5&lt;&gt;T4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z5:AE31">
-    <cfRule type="expression" dxfId="39" priority="9">
+    <cfRule type="expression" dxfId="13" priority="9">
       <formula>Z5&lt;&gt;Z4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF5:AK31">
-    <cfRule type="expression" dxfId="38" priority="8">
+    <cfRule type="expression" dxfId="12" priority="8">
       <formula>AF5&lt;&gt;AF4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL5:AN31">
-    <cfRule type="expression" dxfId="37" priority="6">
+    <cfRule type="expression" dxfId="11" priority="6">
       <formula>AL5&lt;&gt;AL4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO5:AQ31">
-    <cfRule type="expression" dxfId="36" priority="5">
+    <cfRule type="expression" dxfId="10" priority="5">
       <formula>AO5&lt;&gt;AO4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR5:AT31">
-    <cfRule type="expression" dxfId="35" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>AR5&lt;&gt;AR4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU5:AW31">
-    <cfRule type="expression" dxfId="34" priority="1">
+    <cfRule type="expression" dxfId="8" priority="1">
       <formula>AU5&lt;&gt;AU4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10812,22 +10812,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B6:G6">
-    <cfRule type="expression" dxfId="33" priority="20">
+    <cfRule type="expression" dxfId="7" priority="20">
       <formula>B6&lt;&gt;B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:G32">
-    <cfRule type="expression" dxfId="32" priority="1">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>B7&lt;&gt;B6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:M6">
-    <cfRule type="expression" dxfId="31" priority="22">
+    <cfRule type="expression" dxfId="5" priority="22">
       <formula>H6&lt;&gt;H4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:M32">
-    <cfRule type="expression" dxfId="30" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>H7&lt;&gt;H6</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12163,22 +12163,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B6:G6">
-    <cfRule type="expression" dxfId="29" priority="19">
+    <cfRule type="expression" dxfId="3" priority="19">
       <formula>B6&lt;&gt;B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:G32">
-    <cfRule type="expression" dxfId="28" priority="2">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula>B7&lt;&gt;B6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:M6">
-    <cfRule type="expression" dxfId="27" priority="20">
+    <cfRule type="expression" dxfId="1" priority="20">
       <formula>H6&lt;&gt;H4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:M32">
-    <cfRule type="expression" dxfId="26" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>H7&lt;&gt;H6</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13434,8 +13434,8 @@
   </sheetPr>
   <dimension ref="A1:X99"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="46" workbookViewId="0">
-      <selection activeCell="O46" sqref="O46"/>
+    <sheetView zoomScale="46" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -13715,51 +13715,51 @@
       </c>
       <c r="M4" s="62">
         <f>NK!E14</f>
-        <v>4.1059027777777784E-4</v>
+        <v>4.4045138888888888E-4</v>
       </c>
       <c r="N4" s="62">
         <f>NK!E16</f>
-        <v>6.4841435185185195E-4</v>
+        <v>6.9557175925925928E-4</v>
       </c>
       <c r="O4" s="62">
         <f>NK!E15</f>
-        <v>8.8114583333333361E-4</v>
+        <v>9.4522916666666681E-4</v>
       </c>
       <c r="P4" s="62">
         <f>NK!E17</f>
-        <v>7.3498842592592593E-4</v>
+        <v>7.884421296296295E-4</v>
       </c>
       <c r="Q4" s="62">
         <f>NK!E19</f>
-        <v>1.828368055555556E-3</v>
+        <v>1.961340277777778E-3</v>
       </c>
       <c r="R4" s="62">
         <f>NK!E18</f>
-        <v>1.6699884259259259E-3</v>
+        <v>1.7914421296296294E-3</v>
       </c>
       <c r="S4" s="62">
         <f>M4</f>
-        <v>4.1059027777777784E-4</v>
+        <v>4.4045138888888888E-4</v>
       </c>
       <c r="T4" s="62">
         <f t="shared" ref="T4:T9" si="0">N4</f>
-        <v>6.4841435185185195E-4</v>
+        <v>6.9557175925925928E-4</v>
       </c>
       <c r="U4" s="62">
         <f t="shared" ref="U4:U9" si="1">O4</f>
-        <v>8.8114583333333361E-4</v>
+        <v>9.4522916666666681E-4</v>
       </c>
       <c r="V4" s="62">
         <f t="shared" ref="V4:V9" si="2">P4</f>
-        <v>7.3498842592592593E-4</v>
+        <v>7.884421296296295E-4</v>
       </c>
       <c r="W4" s="62">
         <f t="shared" ref="W4:W9" si="3">Q4</f>
-        <v>1.828368055555556E-3</v>
+        <v>1.961340277777778E-3</v>
       </c>
       <c r="X4" s="62">
         <f t="shared" ref="X4:X9" si="4">R4</f>
-        <v>1.6699884259259259E-3</v>
+        <v>1.7914421296296294E-3</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.45">
@@ -13797,51 +13797,51 @@
       </c>
       <c r="M5" s="62">
         <f>NK!D14</f>
-        <v>4.2344907407407414E-4</v>
+        <v>4.5424537037037037E-4</v>
       </c>
       <c r="N5" s="62">
         <f>NK!D16</f>
-        <v>6.6700231481481493E-4</v>
+        <v>7.1551157407407403E-4</v>
       </c>
       <c r="O5" s="62">
         <f>NK!D15</f>
-        <v>9.1666666666666676E-4</v>
+        <v>9.8333333333333324E-4</v>
       </c>
       <c r="P5" s="62">
         <f>NK!D17</f>
-        <v>7.6325231481481491E-4</v>
+        <v>8.1876157407407407E-4</v>
       </c>
       <c r="Q5" s="62">
         <f>NK!D19</f>
-        <v>1.8871875E-3</v>
+        <v>2.0244374999999998E-3</v>
       </c>
       <c r="R5" s="62">
         <f>NK!D18</f>
-        <v>1.7209143518518517E-3</v>
+        <v>1.8460717592592589E-3</v>
       </c>
       <c r="S5" s="62">
         <f t="shared" ref="S5:S9" si="5">M5</f>
-        <v>4.2344907407407414E-4</v>
+        <v>4.5424537037037037E-4</v>
       </c>
       <c r="T5" s="62">
         <f t="shared" si="0"/>
-        <v>6.6700231481481493E-4</v>
+        <v>7.1551157407407403E-4</v>
       </c>
       <c r="U5" s="62">
         <f t="shared" si="1"/>
-        <v>9.1666666666666676E-4</v>
+        <v>9.8333333333333324E-4</v>
       </c>
       <c r="V5" s="62">
         <f t="shared" si="2"/>
-        <v>7.6325231481481491E-4</v>
+        <v>8.1876157407407407E-4</v>
       </c>
       <c r="W5" s="62">
         <f t="shared" si="3"/>
-        <v>1.8871875E-3</v>
+        <v>2.0244374999999998E-3</v>
       </c>
       <c r="X5" s="62">
         <f t="shared" si="4"/>
-        <v>1.7209143518518517E-3</v>
+        <v>1.8460717592592589E-3</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.45">
@@ -13879,51 +13879,51 @@
       </c>
       <c r="M6" s="62">
         <f>NK!C14</f>
-        <v>4.3210648148148145E-4</v>
+        <v>4.6353240740740735E-4</v>
       </c>
       <c r="N6" s="62">
         <f>NK!C16</f>
-        <v>6.7973379629629644E-4</v>
+        <v>7.2916898148148146E-4</v>
       </c>
       <c r="O6" s="62">
         <f>NK!C15</f>
-        <v>9.3283564814814813E-4</v>
+        <v>1.0006782407407406E-3</v>
       </c>
       <c r="P6" s="62">
         <f>NK!C17</f>
-        <v>7.826041666666668E-4</v>
+        <v>8.3952083333333329E-4</v>
       </c>
       <c r="Q6" s="62">
         <f>NK!C19</f>
-        <v>1.9272916666666668E-3</v>
+        <v>2.067458333333333E-3</v>
       </c>
       <c r="R6" s="62">
         <f>NK!C18</f>
-        <v>1.7556712962962966E-3</v>
+        <v>1.8833564814814815E-3</v>
       </c>
       <c r="S6" s="62">
         <f t="shared" si="5"/>
-        <v>4.3210648148148145E-4</v>
+        <v>4.6353240740740735E-4</v>
       </c>
       <c r="T6" s="62">
         <f t="shared" si="0"/>
-        <v>6.7973379629629644E-4</v>
+        <v>7.2916898148148146E-4</v>
       </c>
       <c r="U6" s="62">
         <f t="shared" si="1"/>
-        <v>9.3283564814814813E-4</v>
+        <v>1.0006782407407406E-3</v>
       </c>
       <c r="V6" s="62">
         <f t="shared" si="2"/>
-        <v>7.826041666666668E-4</v>
+        <v>8.3952083333333329E-4</v>
       </c>
       <c r="W6" s="62">
         <f t="shared" si="3"/>
-        <v>1.9272916666666668E-3</v>
+        <v>2.067458333333333E-3</v>
       </c>
       <c r="X6" s="62">
         <f t="shared" si="4"/>
-        <v>1.7556712962962966E-3</v>
+        <v>1.8833564814814815E-3</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.45">
@@ -13961,51 +13961,51 @@
       </c>
       <c r="M7" s="62">
         <f>NK!K14</f>
-        <v>5.0136574074074081E-4</v>
+        <v>5.3782870370370367E-4</v>
       </c>
       <c r="N7" s="62">
         <f>NK!K16</f>
-        <v>7.5879629629629637E-4</v>
+        <v>8.139814814814815E-4</v>
       </c>
       <c r="O7" s="62">
         <f>NK!K15</f>
-        <v>1.0281944444444446E-3</v>
+        <v>1.1029722222222222E-3</v>
       </c>
       <c r="P7" s="62">
         <f>NK!K17</f>
-        <v>8.4142361111111126E-4</v>
+        <v>9.026180555555556E-4</v>
       </c>
       <c r="Q7" s="62">
         <f>NK!K19</f>
-        <v>1.9887847222222225E-3</v>
+        <v>2.1334236111111111E-3</v>
       </c>
       <c r="R7" s="62">
         <f>NK!K18</f>
-        <v>1.8017592592592595E-3</v>
+        <v>1.9327962962962962E-3</v>
       </c>
       <c r="S7" s="62">
         <f t="shared" si="5"/>
-        <v>5.0136574074074081E-4</v>
+        <v>5.3782870370370367E-4</v>
       </c>
       <c r="T7" s="62">
         <f t="shared" si="0"/>
-        <v>7.5879629629629637E-4</v>
+        <v>8.139814814814815E-4</v>
       </c>
       <c r="U7" s="62">
         <f t="shared" si="1"/>
-        <v>1.0281944444444446E-3</v>
+        <v>1.1029722222222222E-3</v>
       </c>
       <c r="V7" s="62">
         <f t="shared" si="2"/>
-        <v>8.4142361111111126E-4</v>
+        <v>9.026180555555556E-4</v>
       </c>
       <c r="W7" s="62">
         <f t="shared" si="3"/>
-        <v>1.9887847222222225E-3</v>
+        <v>2.1334236111111111E-3</v>
       </c>
       <c r="X7" s="62">
         <f t="shared" si="4"/>
-        <v>1.8017592592592595E-3</v>
+        <v>1.9327962962962962E-3</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.45">
@@ -14043,51 +14043,51 @@
       </c>
       <c r="M8" s="62">
         <f>NK!J14</f>
-        <v>5.1371527777777776E-4</v>
+        <v>5.5107638888888882E-4</v>
       </c>
       <c r="N8" s="62">
         <f>NK!J16</f>
-        <v>7.7407407407407405E-4</v>
+        <v>8.3037037037037031E-4</v>
       </c>
       <c r="O8" s="62">
         <f>NK!J15</f>
-        <v>1.0661342592592593E-3</v>
+        <v>1.1436712962962963E-3</v>
       </c>
       <c r="P8" s="62">
         <f>NK!J17</f>
-        <v>8.6013888888888902E-4</v>
+        <v>9.2269444444444441E-4</v>
       </c>
       <c r="Q8" s="62">
         <f>NK!J19</f>
-        <v>2.0334722222222225E-3</v>
+        <v>2.1813611111111109E-3</v>
       </c>
       <c r="R8" s="62">
         <f>NK!J18</f>
-        <v>1.8291319444444449E-3</v>
+        <v>1.9621597222222223E-3</v>
       </c>
       <c r="S8" s="62">
         <f t="shared" si="5"/>
-        <v>5.1371527777777776E-4</v>
+        <v>5.5107638888888882E-4</v>
       </c>
       <c r="T8" s="62">
         <f t="shared" si="0"/>
-        <v>7.7407407407407405E-4</v>
+        <v>8.3037037037037031E-4</v>
       </c>
       <c r="U8" s="62">
         <f t="shared" si="1"/>
-        <v>1.0661342592592593E-3</v>
+        <v>1.1436712962962963E-3</v>
       </c>
       <c r="V8" s="62">
         <f t="shared" si="2"/>
-        <v>8.6013888888888902E-4</v>
+        <v>9.2269444444444441E-4</v>
       </c>
       <c r="W8" s="62">
         <f t="shared" si="3"/>
-        <v>2.0334722222222225E-3</v>
+        <v>2.1813611111111109E-3</v>
       </c>
       <c r="X8" s="62">
         <f t="shared" si="4"/>
-        <v>1.8291319444444449E-3</v>
+        <v>1.9621597222222223E-3</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.45">
@@ -14125,51 +14125,51 @@
       </c>
       <c r="M9" s="62">
         <f>NK!I14</f>
-        <v>5.2517361111111113E-4</v>
+        <v>5.6336805555555545E-4</v>
       </c>
       <c r="N9" s="62">
         <f>NK!I16</f>
-        <v>7.8807870370370381E-4</v>
+        <v>8.4539351851851843E-4</v>
       </c>
       <c r="O9" s="62">
         <f>NK!I15</f>
-        <v>1.1039467592592594E-3</v>
+        <v>1.1842337962962963E-3</v>
       </c>
       <c r="P9" s="62">
         <f>NK!I17</f>
-        <v>8.7745370370370386E-4</v>
+        <v>9.4126851851851858E-4</v>
       </c>
       <c r="Q9" s="62">
         <f>NK!I19</f>
-        <v>2.0780324074074078E-3</v>
+        <v>2.2291620370370369E-3</v>
       </c>
       <c r="R9" s="62">
         <f>NK!I18</f>
-        <v>1.8566319444444444E-3</v>
+        <v>1.9916597222222219E-3</v>
       </c>
       <c r="S9" s="62">
         <f t="shared" si="5"/>
-        <v>5.2517361111111113E-4</v>
+        <v>5.6336805555555545E-4</v>
       </c>
       <c r="T9" s="62">
         <f t="shared" si="0"/>
-        <v>7.8807870370370381E-4</v>
+        <v>8.4539351851851843E-4</v>
       </c>
       <c r="U9" s="62">
         <f t="shared" si="1"/>
-        <v>1.1039467592592594E-3</v>
+        <v>1.1842337962962963E-3</v>
       </c>
       <c r="V9" s="62">
         <f t="shared" si="2"/>
-        <v>8.7745370370370386E-4</v>
+        <v>9.4126851851851858E-4</v>
       </c>
       <c r="W9" s="62">
         <f t="shared" si="3"/>
-        <v>2.0780324074074078E-3</v>
+        <v>2.2291620370370369E-3</v>
       </c>
       <c r="X9" s="62">
         <f t="shared" si="4"/>
-        <v>1.8566319444444444E-3</v>
+        <v>1.9916597222222219E-3</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.45">
@@ -14207,51 +14207,51 @@
       </c>
       <c r="M10" s="62">
         <f>NK!$R$14</f>
-        <v>3.9722222222222226E-4</v>
+        <v>4.0805555555555549E-4</v>
       </c>
       <c r="N10" s="62">
         <f>NK!$R$16</f>
-        <v>6.2893518518518528E-4</v>
+        <v>6.4608796296296289E-4</v>
       </c>
       <c r="O10" s="62">
         <f>NK!$R$15</f>
-        <v>8.490625000000001E-4</v>
+        <v>8.7221874999999995E-4</v>
       </c>
       <c r="P10" s="62">
         <f>NK!$R$17</f>
-        <v>7.0545138888888882E-4</v>
+        <v>7.2469097222222206E-4</v>
       </c>
       <c r="Q10" s="62">
         <f>NK!$R$19</f>
-        <v>1.7668750000000002E-3</v>
+        <v>1.8150624999999998E-3</v>
       </c>
       <c r="R10" s="62">
         <f>NK!$R$18</f>
-        <v>1.6167708333333333E-3</v>
+        <v>1.660864583333333E-3</v>
       </c>
       <c r="S10" s="62">
         <f>M10</f>
-        <v>3.9722222222222226E-4</v>
+        <v>4.0805555555555549E-4</v>
       </c>
       <c r="T10" s="62">
         <f t="shared" ref="T10:T15" si="6">N10</f>
-        <v>6.2893518518518528E-4</v>
+        <v>6.4608796296296289E-4</v>
       </c>
       <c r="U10" s="62">
         <f t="shared" ref="U10:U15" si="7">O10</f>
-        <v>8.490625000000001E-4</v>
+        <v>8.7221874999999995E-4</v>
       </c>
       <c r="V10" s="62">
         <f t="shared" ref="V10:V15" si="8">P10</f>
-        <v>7.0545138888888882E-4</v>
+        <v>7.2469097222222206E-4</v>
       </c>
       <c r="W10" s="62">
         <f t="shared" ref="W10:W15" si="9">Q10</f>
-        <v>1.7668750000000002E-3</v>
+        <v>1.8150624999999998E-3</v>
       </c>
       <c r="X10" s="62">
         <f t="shared" ref="X10:X15" si="10">R10</f>
-        <v>1.6167708333333333E-3</v>
+        <v>1.660864583333333E-3</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.45">
@@ -14289,51 +14289,51 @@
       </c>
       <c r="M11" s="62">
         <f>NK!$S$14</f>
-        <v>3.8589120370370372E-4</v>
+        <v>3.9641550925925923E-4</v>
       </c>
       <c r="N11" s="62">
         <f>NK!$S$16</f>
-        <v>6.1225694444444446E-4</v>
+        <v>6.2895486111111106E-4</v>
       </c>
       <c r="O11" s="62">
         <f>NK!$S$15</f>
-        <v>8.2207175925925926E-4</v>
+        <v>8.4449189814814803E-4</v>
       </c>
       <c r="P11" s="62">
         <f>NK!$S$17</f>
-        <v>6.807523148148148E-4</v>
+        <v>6.9931828703703692E-4</v>
       </c>
       <c r="Q11" s="62">
         <f>NK!$S$19</f>
-        <v>1.7496875000000002E-3</v>
+        <v>1.79740625E-3</v>
       </c>
       <c r="R11" s="62">
         <f>NK!$S$18</f>
-        <v>1.5714467592592596E-3</v>
+        <v>1.6143043981481481E-3</v>
       </c>
       <c r="S11" s="62">
         <f t="shared" ref="S11:S15" si="11">M11</f>
-        <v>3.8589120370370372E-4</v>
+        <v>3.9641550925925923E-4</v>
       </c>
       <c r="T11" s="62">
         <f t="shared" si="6"/>
-        <v>6.1225694444444446E-4</v>
+        <v>6.2895486111111106E-4</v>
       </c>
       <c r="U11" s="62">
         <f t="shared" si="7"/>
-        <v>8.2207175925925926E-4</v>
+        <v>8.4449189814814803E-4</v>
       </c>
       <c r="V11" s="62">
         <f t="shared" si="8"/>
-        <v>6.807523148148148E-4</v>
+        <v>6.9931828703703692E-4</v>
       </c>
       <c r="W11" s="62">
         <f t="shared" si="9"/>
-        <v>1.7496875000000002E-3</v>
+        <v>1.79740625E-3</v>
       </c>
       <c r="X11" s="62">
         <f t="shared" si="10"/>
-        <v>1.5714467592592596E-3</v>
+        <v>1.6143043981481481E-3</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.45">
@@ -14371,51 +14371,51 @@
       </c>
       <c r="M12" s="62">
         <f>NK!$T$14</f>
-        <v>3.7290509259259265E-4</v>
+        <v>3.8307523148148147E-4</v>
       </c>
       <c r="N12" s="62">
         <f>NK!$T$16</f>
-        <v>5.9328703703703703E-4</v>
+        <v>6.0946759259259255E-4</v>
       </c>
       <c r="O12" s="62">
         <f>NK!$T$15</f>
-        <v>7.9113425925925933E-4</v>
+        <v>8.1271064814814802E-4</v>
       </c>
       <c r="P12" s="62">
         <f>NK!$T$17</f>
-        <v>6.5248842592592594E-4</v>
+        <v>6.7028356481481474E-4</v>
       </c>
       <c r="Q12" s="62">
         <f>NK!$T$19</f>
-        <v>1.6964699074074076E-3</v>
+        <v>1.7427372685185185E-3</v>
       </c>
       <c r="R12" s="62">
         <f>NK!$T$18</f>
-        <v>1.5197569444444445E-3</v>
+        <v>1.5612048611111109E-3</v>
       </c>
       <c r="S12" s="62">
         <f t="shared" si="11"/>
-        <v>3.7290509259259265E-4</v>
+        <v>3.8307523148148147E-4</v>
       </c>
       <c r="T12" s="62">
         <f t="shared" si="6"/>
-        <v>5.9328703703703703E-4</v>
+        <v>6.0946759259259255E-4</v>
       </c>
       <c r="U12" s="62">
         <f t="shared" si="7"/>
-        <v>7.9113425925925933E-4</v>
+        <v>8.1271064814814802E-4</v>
       </c>
       <c r="V12" s="62">
         <f t="shared" si="8"/>
-        <v>6.5248842592592594E-4</v>
+        <v>6.7028356481481474E-4</v>
       </c>
       <c r="W12" s="62">
         <f t="shared" si="9"/>
-        <v>1.6964699074074076E-3</v>
+        <v>1.7427372685185185E-3</v>
       </c>
       <c r="X12" s="62">
         <f t="shared" si="10"/>
-        <v>1.5197569444444445E-3</v>
+        <v>1.5612048611111109E-3</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.45">
@@ -14453,51 +14453,51 @@
       </c>
       <c r="M13" s="62">
         <f>NK!$X$14</f>
-        <v>4.8506944444444455E-4</v>
+        <v>4.9829861111111114E-4</v>
       </c>
       <c r="N13" s="62">
         <f>NK!$X$16</f>
-        <v>7.3880787037037046E-4</v>
+        <v>7.5895717592592594E-4</v>
       </c>
       <c r="O13" s="62">
         <f>NK!$X$15</f>
-        <v>9.9038194444444434E-4</v>
+        <v>1.0173923611111108E-3</v>
       </c>
       <c r="P13" s="62">
         <f>NK!$X$17</f>
-        <v>8.1685185185185192E-4</v>
+        <v>8.3912962962962945E-4</v>
       </c>
       <c r="Q13" s="62">
         <f>NK!$X$19</f>
-        <v>1.9440972222222223E-3</v>
+        <v>1.9971180555555554E-3</v>
       </c>
       <c r="R13" s="62">
         <f>NK!$X$18</f>
-        <v>1.7742592592592597E-3</v>
+        <v>1.8226481481481483E-3</v>
       </c>
       <c r="S13" s="62">
         <f t="shared" si="11"/>
-        <v>4.8506944444444455E-4</v>
+        <v>4.9829861111111114E-4</v>
       </c>
       <c r="T13" s="62">
         <f t="shared" si="6"/>
-        <v>7.3880787037037046E-4</v>
+        <v>7.5895717592592594E-4</v>
       </c>
       <c r="U13" s="62">
         <f t="shared" si="7"/>
-        <v>9.9038194444444434E-4</v>
+        <v>1.0173923611111108E-3</v>
       </c>
       <c r="V13" s="62">
         <f t="shared" si="8"/>
-        <v>8.1685185185185192E-4</v>
+        <v>8.3912962962962945E-4</v>
       </c>
       <c r="W13" s="62">
         <f t="shared" si="9"/>
-        <v>1.9440972222222223E-3</v>
+        <v>1.9971180555555554E-3</v>
       </c>
       <c r="X13" s="62">
         <f t="shared" si="10"/>
-        <v>1.7742592592592597E-3</v>
+        <v>1.8226481481481483E-3</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.45">
@@ -14535,51 +14535,51 @@
       </c>
       <c r="M14" s="62">
         <f>NK!$Y$14</f>
-        <v>4.6253472222222225E-4</v>
+        <v>4.7514930555555554E-4</v>
       </c>
       <c r="N14" s="62">
         <f>NK!$Y$16</f>
-        <v>7.1054398148148149E-4</v>
+        <v>7.2992245370370366E-4</v>
       </c>
       <c r="O14" s="62">
         <f>NK!$Y$15</f>
-        <v>9.4556712962962975E-4</v>
+        <v>9.7135532407407403E-4</v>
       </c>
       <c r="P14" s="62">
         <f>NK!$Y$17</f>
-        <v>7.8247685185185191E-4</v>
+        <v>8.0381712962962959E-4</v>
       </c>
       <c r="Q14" s="62">
         <f>NK!$Y$19</f>
-        <v>1.8892245370370371E-3</v>
+        <v>1.9407488425925922E-3</v>
       </c>
       <c r="R14" s="62">
         <f>NK!$Y$18</f>
-        <v>1.7398842592592594E-3</v>
+        <v>1.7873356481481479E-3</v>
       </c>
       <c r="S14" s="62">
         <f t="shared" si="11"/>
-        <v>4.6253472222222225E-4</v>
+        <v>4.7514930555555554E-4</v>
       </c>
       <c r="T14" s="62">
         <f t="shared" si="6"/>
-        <v>7.1054398148148149E-4</v>
+        <v>7.2992245370370366E-4</v>
       </c>
       <c r="U14" s="62">
         <f t="shared" si="7"/>
-        <v>9.4556712962962975E-4</v>
+        <v>9.7135532407407403E-4</v>
       </c>
       <c r="V14" s="62">
         <f t="shared" si="8"/>
-        <v>7.8247685185185191E-4</v>
+        <v>8.0381712962962959E-4</v>
       </c>
       <c r="W14" s="62">
         <f t="shared" si="9"/>
-        <v>1.8892245370370371E-3</v>
+        <v>1.9407488425925922E-3</v>
       </c>
       <c r="X14" s="62">
         <f t="shared" si="10"/>
-        <v>1.7398842592592594E-3</v>
+        <v>1.7873356481481479E-3</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.45">
@@ -14617,51 +14617,51 @@
       </c>
       <c r="M15" s="62">
         <f>NK!$Z$14</f>
-        <v>4.4598379629629632E-4</v>
+        <v>4.5814699074074068E-4</v>
       </c>
       <c r="N15" s="62">
         <f>NK!$Z$16</f>
-        <v>6.8991898148148157E-4</v>
+        <v>7.0873495370370361E-4</v>
       </c>
       <c r="O15" s="62">
         <f>NK!$Z$15</f>
-        <v>9.1271990740740745E-4</v>
+        <v>9.376122685185184E-4</v>
       </c>
       <c r="P15" s="62">
         <f>NK!$Z$17</f>
-        <v>7.5726851851851856E-4</v>
+        <v>7.779212962962962E-4</v>
       </c>
       <c r="Q15" s="62">
         <f>NK!$Z$19</f>
-        <v>1.8491203703703705E-3</v>
+        <v>1.8995509259259258E-3</v>
       </c>
       <c r="R15" s="62">
         <f>NK!$Z$18</f>
-        <v>1.7148032407407409E-3</v>
+        <v>1.7615706018518516E-3</v>
       </c>
       <c r="S15" s="62">
         <f t="shared" si="11"/>
-        <v>4.4598379629629632E-4</v>
+        <v>4.5814699074074068E-4</v>
       </c>
       <c r="T15" s="62">
         <f t="shared" si="6"/>
-        <v>6.8991898148148157E-4</v>
+        <v>7.0873495370370361E-4</v>
       </c>
       <c r="U15" s="62">
         <f t="shared" si="7"/>
-        <v>9.1271990740740745E-4</v>
+        <v>9.376122685185184E-4</v>
       </c>
       <c r="V15" s="62">
         <f t="shared" si="8"/>
-        <v>7.5726851851851856E-4</v>
+        <v>7.779212962962962E-4</v>
       </c>
       <c r="W15" s="62">
         <f t="shared" si="9"/>
-        <v>1.8491203703703705E-3</v>
+        <v>1.8995509259259258E-3</v>
       </c>
       <c r="X15" s="62">
         <f t="shared" si="10"/>
-        <v>1.7148032407407409E-3</v>
+        <v>1.7615706018518516E-3</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.45">
@@ -20556,7 +20556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A13DA696-49DD-4BFA-98FE-5C7770404E50}">
   <dimension ref="B3:AA37"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AA14" sqref="AA14:AA19"/>
     </sheetView>
   </sheetViews>
@@ -21020,72 +21020,72 @@
       </c>
       <c r="C14" s="65">
         <f>C5*$F14</f>
-        <v>4.3210648148148145E-4</v>
+        <v>4.6353240740740735E-4</v>
       </c>
       <c r="D14" s="65">
         <f t="shared" ref="D14:E14" si="0">D5*$F14</f>
-        <v>4.2344907407407414E-4</v>
+        <v>4.5424537037037037E-4</v>
       </c>
       <c r="E14" s="65">
         <f t="shared" si="0"/>
-        <v>4.1059027777777784E-4</v>
+        <v>4.4045138888888888E-4</v>
       </c>
       <c r="F14">
-        <v>1.1000000000000001</v>
+        <v>1.18</v>
       </c>
       <c r="H14" s="64" t="s">
         <v>0</v>
       </c>
       <c r="I14" s="65">
         <f>I5*$L14</f>
-        <v>5.2517361111111113E-4</v>
+        <v>5.6336805555555545E-4</v>
       </c>
       <c r="J14" s="65">
         <f t="shared" ref="J14:K14" si="1">J5*$L14</f>
-        <v>5.1371527777777776E-4</v>
+        <v>5.5107638888888882E-4</v>
       </c>
       <c r="K14" s="65">
         <f t="shared" si="1"/>
-        <v>5.0136574074074081E-4</v>
+        <v>5.3782870370370367E-4</v>
       </c>
       <c r="L14">
-        <v>1.1000000000000001</v>
+        <v>1.18</v>
       </c>
       <c r="Q14" s="64" t="s">
         <v>0</v>
       </c>
       <c r="R14" s="65">
         <f t="shared" ref="R14:T19" si="2">R5*$U14</f>
-        <v>3.9722222222222226E-4</v>
+        <v>4.0805555555555549E-4</v>
       </c>
       <c r="S14" s="65">
         <f t="shared" si="2"/>
-        <v>3.8589120370370372E-4</v>
+        <v>3.9641550925925923E-4</v>
       </c>
       <c r="T14" s="65">
         <f t="shared" si="2"/>
-        <v>3.7290509259259265E-4</v>
+        <v>3.8307523148148147E-4</v>
       </c>
       <c r="U14">
-        <v>1.1000000000000001</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="W14" s="64" t="s">
         <v>0</v>
       </c>
       <c r="X14" s="65">
         <f>X5*$AA14</f>
-        <v>4.8506944444444455E-4</v>
+        <v>4.9829861111111114E-4</v>
       </c>
       <c r="Y14" s="65">
         <f t="shared" ref="Y14:Z14" si="3">Y5*$AA14</f>
-        <v>4.6253472222222225E-4</v>
+        <v>4.7514930555555554E-4</v>
       </c>
       <c r="Z14" s="65">
         <f t="shared" si="3"/>
-        <v>4.4598379629629632E-4</v>
+        <v>4.5814699074074068E-4</v>
       </c>
       <c r="AA14">
-        <v>1.1000000000000001</v>
+        <v>1.1299999999999999</v>
       </c>
     </row>
     <row r="15" spans="2:27" x14ac:dyDescent="0.45">
@@ -21094,72 +21094,72 @@
       </c>
       <c r="C15" s="65">
         <f t="shared" ref="C15:E15" si="4">C6*$F15</f>
-        <v>9.3283564814814813E-4</v>
+        <v>1.0006782407407406E-3</v>
       </c>
       <c r="D15" s="65">
         <f t="shared" si="4"/>
-        <v>9.1666666666666676E-4</v>
+        <v>9.8333333333333324E-4</v>
       </c>
       <c r="E15" s="65">
         <f t="shared" si="4"/>
-        <v>8.8114583333333361E-4</v>
+        <v>9.4522916666666681E-4</v>
       </c>
       <c r="F15">
-        <v>1.1000000000000001</v>
+        <v>1.18</v>
       </c>
       <c r="H15" s="64" t="s">
         <v>223</v>
       </c>
       <c r="I15" s="65">
         <f t="shared" ref="I15:K15" si="5">I6*$L15</f>
-        <v>1.1039467592592594E-3</v>
+        <v>1.1842337962962963E-3</v>
       </c>
       <c r="J15" s="65">
         <f t="shared" si="5"/>
-        <v>1.0661342592592593E-3</v>
+        <v>1.1436712962962963E-3</v>
       </c>
       <c r="K15" s="65">
         <f t="shared" si="5"/>
-        <v>1.0281944444444446E-3</v>
+        <v>1.1029722222222222E-3</v>
       </c>
       <c r="L15">
-        <v>1.1000000000000001</v>
+        <v>1.18</v>
       </c>
       <c r="Q15" s="64" t="s">
         <v>223</v>
       </c>
       <c r="R15" s="65">
         <f t="shared" si="2"/>
-        <v>8.490625000000001E-4</v>
+        <v>8.7221874999999995E-4</v>
       </c>
       <c r="S15" s="65">
         <f t="shared" si="2"/>
-        <v>8.2207175925925926E-4</v>
+        <v>8.4449189814814803E-4</v>
       </c>
       <c r="T15" s="65">
         <f t="shared" si="2"/>
-        <v>7.9113425925925933E-4</v>
+        <v>8.1271064814814802E-4</v>
       </c>
       <c r="U15">
-        <v>1.1000000000000001</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="W15" s="64" t="s">
         <v>223</v>
       </c>
       <c r="X15" s="65">
         <f t="shared" ref="X15:Z15" si="6">X6*$AA15</f>
-        <v>9.9038194444444434E-4</v>
+        <v>1.0173923611111108E-3</v>
       </c>
       <c r="Y15" s="65">
         <f t="shared" si="6"/>
-        <v>9.4556712962962975E-4</v>
+        <v>9.7135532407407403E-4</v>
       </c>
       <c r="Z15" s="65">
         <f t="shared" si="6"/>
-        <v>9.1271990740740745E-4</v>
+        <v>9.376122685185184E-4</v>
       </c>
       <c r="AA15">
-        <v>1.1000000000000001</v>
+        <v>1.1299999999999999</v>
       </c>
     </row>
     <row r="16" spans="2:27" x14ac:dyDescent="0.45">
@@ -21168,72 +21168,72 @@
       </c>
       <c r="C16" s="65">
         <f t="shared" ref="C16:E16" si="7">C7*$F16</f>
-        <v>6.7973379629629644E-4</v>
+        <v>7.2916898148148146E-4</v>
       </c>
       <c r="D16" s="65">
         <f t="shared" si="7"/>
-        <v>6.6700231481481493E-4</v>
+        <v>7.1551157407407403E-4</v>
       </c>
       <c r="E16" s="65">
         <f t="shared" si="7"/>
-        <v>6.4841435185185195E-4</v>
+        <v>6.9557175925925928E-4</v>
       </c>
       <c r="F16">
-        <v>1.1000000000000001</v>
+        <v>1.18</v>
       </c>
       <c r="H16" s="64" t="s">
         <v>224</v>
       </c>
       <c r="I16" s="65">
         <f t="shared" ref="I16:K16" si="8">I7*$L16</f>
-        <v>7.8807870370370381E-4</v>
+        <v>8.4539351851851843E-4</v>
       </c>
       <c r="J16" s="65">
         <f t="shared" si="8"/>
-        <v>7.7407407407407405E-4</v>
+        <v>8.3037037037037031E-4</v>
       </c>
       <c r="K16" s="65">
         <f t="shared" si="8"/>
-        <v>7.5879629629629637E-4</v>
+        <v>8.139814814814815E-4</v>
       </c>
       <c r="L16">
-        <v>1.1000000000000001</v>
+        <v>1.18</v>
       </c>
       <c r="Q16" s="64" t="s">
         <v>224</v>
       </c>
       <c r="R16" s="65">
         <f t="shared" si="2"/>
-        <v>6.2893518518518528E-4</v>
+        <v>6.4608796296296289E-4</v>
       </c>
       <c r="S16" s="65">
         <f t="shared" si="2"/>
-        <v>6.1225694444444446E-4</v>
+        <v>6.2895486111111106E-4</v>
       </c>
       <c r="T16" s="65">
         <f t="shared" si="2"/>
-        <v>5.9328703703703703E-4</v>
+        <v>6.0946759259259255E-4</v>
       </c>
       <c r="U16">
-        <v>1.1000000000000001</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="W16" s="64" t="s">
         <v>224</v>
       </c>
       <c r="X16" s="65">
         <f t="shared" ref="X16:Z16" si="9">X7*$AA16</f>
-        <v>7.3880787037037046E-4</v>
+        <v>7.5895717592592594E-4</v>
       </c>
       <c r="Y16" s="65">
         <f>Y7*$AA16</f>
-        <v>7.1054398148148149E-4</v>
+        <v>7.2992245370370366E-4</v>
       </c>
       <c r="Z16" s="65">
         <f t="shared" si="9"/>
-        <v>6.8991898148148157E-4</v>
+        <v>7.0873495370370361E-4</v>
       </c>
       <c r="AA16">
-        <v>1.1000000000000001</v>
+        <v>1.1299999999999999</v>
       </c>
     </row>
     <row r="17" spans="2:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -21242,72 +21242,72 @@
       </c>
       <c r="C17" s="65">
         <f t="shared" ref="C17:E17" si="10">C8*$F17</f>
-        <v>7.826041666666668E-4</v>
+        <v>8.3952083333333329E-4</v>
       </c>
       <c r="D17" s="65">
         <f t="shared" si="10"/>
-        <v>7.6325231481481491E-4</v>
+        <v>8.1876157407407407E-4</v>
       </c>
       <c r="E17" s="65">
         <f t="shared" si="10"/>
-        <v>7.3498842592592593E-4</v>
+        <v>7.884421296296295E-4</v>
       </c>
       <c r="F17">
-        <v>1.1000000000000001</v>
+        <v>1.18</v>
       </c>
       <c r="H17" s="64" t="s">
         <v>225</v>
       </c>
       <c r="I17" s="65">
         <f t="shared" ref="I17:K17" si="11">I8*$L17</f>
-        <v>8.7745370370370386E-4</v>
+        <v>9.4126851851851858E-4</v>
       </c>
       <c r="J17" s="65">
         <f t="shared" si="11"/>
-        <v>8.6013888888888902E-4</v>
+        <v>9.2269444444444441E-4</v>
       </c>
       <c r="K17" s="65">
         <f t="shared" si="11"/>
-        <v>8.4142361111111126E-4</v>
+        <v>9.026180555555556E-4</v>
       </c>
       <c r="L17">
-        <v>1.1000000000000001</v>
+        <v>1.18</v>
       </c>
       <c r="Q17" s="64" t="s">
         <v>225</v>
       </c>
       <c r="R17" s="65">
         <f t="shared" si="2"/>
-        <v>7.0545138888888882E-4</v>
+        <v>7.2469097222222206E-4</v>
       </c>
       <c r="S17" s="65">
         <f t="shared" si="2"/>
-        <v>6.807523148148148E-4</v>
+        <v>6.9931828703703692E-4</v>
       </c>
       <c r="T17" s="65">
         <f t="shared" si="2"/>
-        <v>6.5248842592592594E-4</v>
+        <v>6.7028356481481474E-4</v>
       </c>
       <c r="U17">
-        <v>1.1000000000000001</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="W17" s="64" t="s">
         <v>225</v>
       </c>
       <c r="X17" s="65">
         <f t="shared" ref="X17:Z17" si="12">X8*$AA17</f>
-        <v>8.1685185185185192E-4</v>
+        <v>8.3912962962962945E-4</v>
       </c>
       <c r="Y17" s="65">
         <f>Y8*$AA17</f>
-        <v>7.8247685185185191E-4</v>
+        <v>8.0381712962962959E-4</v>
       </c>
       <c r="Z17" s="65">
         <f t="shared" si="12"/>
-        <v>7.5726851851851856E-4</v>
+        <v>7.779212962962962E-4</v>
       </c>
       <c r="AA17">
-        <v>1.1000000000000001</v>
+        <v>1.1299999999999999</v>
       </c>
     </row>
     <row r="18" spans="2:27" x14ac:dyDescent="0.45">
@@ -21316,72 +21316,72 @@
       </c>
       <c r="C18" s="65">
         <f t="shared" ref="C18:E18" si="13">C9*$F18</f>
-        <v>1.7556712962962966E-3</v>
+        <v>1.8833564814814815E-3</v>
       </c>
       <c r="D18" s="65">
         <f t="shared" si="13"/>
-        <v>1.7209143518518517E-3</v>
+        <v>1.8460717592592589E-3</v>
       </c>
       <c r="E18" s="65">
         <f t="shared" si="13"/>
-        <v>1.6699884259259259E-3</v>
+        <v>1.7914421296296294E-3</v>
       </c>
       <c r="F18">
-        <v>1.1000000000000001</v>
+        <v>1.18</v>
       </c>
       <c r="H18" s="64" t="s">
         <v>226</v>
       </c>
       <c r="I18" s="65">
         <f t="shared" ref="I18:K18" si="14">I9*$L18</f>
-        <v>1.8566319444444444E-3</v>
+        <v>1.9916597222222219E-3</v>
       </c>
       <c r="J18" s="65">
         <f t="shared" si="14"/>
-        <v>1.8291319444444449E-3</v>
+        <v>1.9621597222222223E-3</v>
       </c>
       <c r="K18" s="65">
         <f t="shared" si="14"/>
-        <v>1.8017592592592595E-3</v>
+        <v>1.9327962962962962E-3</v>
       </c>
       <c r="L18">
-        <v>1.1000000000000001</v>
+        <v>1.18</v>
       </c>
       <c r="Q18" s="64" t="s">
         <v>226</v>
       </c>
       <c r="R18" s="65">
         <f t="shared" si="2"/>
-        <v>1.6167708333333333E-3</v>
+        <v>1.660864583333333E-3</v>
       </c>
       <c r="S18" s="65">
         <f t="shared" si="2"/>
-        <v>1.5714467592592596E-3</v>
+        <v>1.6143043981481481E-3</v>
       </c>
       <c r="T18" s="65">
         <f t="shared" si="2"/>
-        <v>1.5197569444444445E-3</v>
+        <v>1.5612048611111109E-3</v>
       </c>
       <c r="U18">
-        <v>1.1000000000000001</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="W18" s="64" t="s">
         <v>226</v>
       </c>
       <c r="X18" s="65">
         <f t="shared" ref="X18:Z18" si="15">X9*$AA18</f>
-        <v>1.7742592592592597E-3</v>
+        <v>1.8226481481481483E-3</v>
       </c>
       <c r="Y18" s="65">
         <f t="shared" si="15"/>
-        <v>1.7398842592592594E-3</v>
+        <v>1.7873356481481479E-3</v>
       </c>
       <c r="Z18" s="65">
         <f t="shared" si="15"/>
-        <v>1.7148032407407409E-3</v>
+        <v>1.7615706018518516E-3</v>
       </c>
       <c r="AA18">
-        <v>1.1000000000000001</v>
+        <v>1.1299999999999999</v>
       </c>
     </row>
     <row r="19" spans="2:27" x14ac:dyDescent="0.45">
@@ -21390,72 +21390,72 @@
       </c>
       <c r="C19" s="65">
         <f t="shared" ref="C19:E19" si="16">C10*$F19</f>
-        <v>1.9272916666666668E-3</v>
+        <v>2.067458333333333E-3</v>
       </c>
       <c r="D19" s="65">
         <f t="shared" si="16"/>
-        <v>1.8871875E-3</v>
+        <v>2.0244374999999998E-3</v>
       </c>
       <c r="E19" s="65">
         <f t="shared" si="16"/>
-        <v>1.828368055555556E-3</v>
+        <v>1.961340277777778E-3</v>
       </c>
       <c r="F19">
-        <v>1.1000000000000001</v>
+        <v>1.18</v>
       </c>
       <c r="H19" s="64" t="s">
         <v>4</v>
       </c>
       <c r="I19" s="65">
         <f t="shared" ref="I19:K19" si="17">I10*$L19</f>
-        <v>2.0780324074074078E-3</v>
+        <v>2.2291620370370369E-3</v>
       </c>
       <c r="J19" s="65">
         <f t="shared" si="17"/>
-        <v>2.0334722222222225E-3</v>
+        <v>2.1813611111111109E-3</v>
       </c>
       <c r="K19" s="65">
         <f t="shared" si="17"/>
-        <v>1.9887847222222225E-3</v>
+        <v>2.1334236111111111E-3</v>
       </c>
       <c r="L19">
-        <v>1.1000000000000001</v>
+        <v>1.18</v>
       </c>
       <c r="Q19" s="64" t="s">
         <v>4</v>
       </c>
       <c r="R19" s="65">
         <f t="shared" si="2"/>
-        <v>1.7668750000000002E-3</v>
+        <v>1.8150624999999998E-3</v>
       </c>
       <c r="S19" s="65">
         <f t="shared" si="2"/>
-        <v>1.7496875000000002E-3</v>
+        <v>1.79740625E-3</v>
       </c>
       <c r="T19" s="65">
         <f t="shared" si="2"/>
-        <v>1.6964699074074076E-3</v>
+        <v>1.7427372685185185E-3</v>
       </c>
       <c r="U19">
-        <v>1.1000000000000001</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="W19" s="64" t="s">
         <v>4</v>
       </c>
       <c r="X19" s="65">
         <f t="shared" ref="X19:Z19" si="18">X10*$AA19</f>
-        <v>1.9440972222222223E-3</v>
+        <v>1.9971180555555554E-3</v>
       </c>
       <c r="Y19" s="65">
         <f t="shared" si="18"/>
-        <v>1.8892245370370371E-3</v>
+        <v>1.9407488425925922E-3</v>
       </c>
       <c r="Z19" s="65">
         <f t="shared" si="18"/>
-        <v>1.8491203703703705E-3</v>
+        <v>1.8995509259259258E-3</v>
       </c>
       <c r="AA19">
-        <v>1.1000000000000001</v>
+        <v>1.1299999999999999</v>
       </c>
     </row>
     <row r="22" spans="2:27" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Neue anpassung a krits
</commit_message>
<xml_diff>
--- a/web/utilities/records_kriterien.xlsx
+++ b/web/utilities/records_kriterien.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgna\Documents\GitHub\Lifesaving_Baden\web\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3A6B6D-28D3-429D-9596-6897B79B869C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75132DDE-FA4F-4D18-83DE-ADB365B2505B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="7" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="6" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
   </bookViews>
   <sheets>
     <sheet name="DR" sheetId="9" r:id="rId1"/>
@@ -1023,16 +1023,16 @@
     <t>&lt;2005</t>
   </si>
   <si>
-    <t>NK2 +18% Mäner</t>
-  </si>
-  <si>
     <t>NK2 +18% Frauen</t>
   </si>
   <si>
-    <t>NK1 +13% Mäner</t>
-  </si>
-  <si>
-    <t>NK1 +13% Frauen</t>
+    <t>NK2 +19% Mäner</t>
+  </si>
+  <si>
+    <t>NK1 +14% Mäner</t>
+  </si>
+  <si>
+    <t>NK1 +21% Frauen</t>
   </si>
 </sst>
 </file>
@@ -13434,7 +13434,7 @@
   </sheetPr>
   <dimension ref="A1:X99"/>
   <sheetViews>
-    <sheetView zoomScale="46" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="46" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -13682,7 +13682,7 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A4" s="59" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B4" s="59" t="s">
         <v>182</v>
@@ -13715,56 +13715,56 @@
       </c>
       <c r="M4" s="62">
         <f>NK!E14</f>
-        <v>4.4045138888888888E-4</v>
+        <v>4.4418402777777777E-4</v>
       </c>
       <c r="N4" s="62">
         <f>NK!E16</f>
-        <v>6.9557175925925928E-4</v>
+        <v>7.0146643518518518E-4</v>
       </c>
       <c r="O4" s="62">
         <f>NK!E15</f>
-        <v>9.4522916666666681E-4</v>
+        <v>9.532395833333335E-4</v>
       </c>
       <c r="P4" s="62">
         <f>NK!E17</f>
-        <v>7.884421296296295E-4</v>
+        <v>7.951238425925925E-4</v>
       </c>
       <c r="Q4" s="62">
         <f>NK!E19</f>
-        <v>1.961340277777778E-3</v>
+        <v>1.9779618055555557E-3</v>
       </c>
       <c r="R4" s="62">
         <f>NK!E18</f>
-        <v>1.7914421296296294E-3</v>
+        <v>1.8066238425925923E-3</v>
       </c>
       <c r="S4" s="62">
         <f>M4</f>
-        <v>4.4045138888888888E-4</v>
+        <v>4.4418402777777777E-4</v>
       </c>
       <c r="T4" s="62">
         <f t="shared" ref="T4:T9" si="0">N4</f>
-        <v>6.9557175925925928E-4</v>
+        <v>7.0146643518518518E-4</v>
       </c>
       <c r="U4" s="62">
         <f t="shared" ref="U4:U9" si="1">O4</f>
-        <v>9.4522916666666681E-4</v>
+        <v>9.532395833333335E-4</v>
       </c>
       <c r="V4" s="62">
         <f t="shared" ref="V4:V9" si="2">P4</f>
-        <v>7.884421296296295E-4</v>
+        <v>7.951238425925925E-4</v>
       </c>
       <c r="W4" s="62">
         <f t="shared" ref="W4:W9" si="3">Q4</f>
-        <v>1.961340277777778E-3</v>
+        <v>1.9779618055555557E-3</v>
       </c>
       <c r="X4" s="62">
         <f t="shared" ref="X4:X9" si="4">R4</f>
-        <v>1.7914421296296294E-3</v>
+        <v>1.8066238425925923E-3</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A5" s="59" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B5" s="59" t="s">
         <v>182</v>
@@ -13797,56 +13797,56 @@
       </c>
       <c r="M5" s="62">
         <f>NK!D14</f>
-        <v>4.5424537037037037E-4</v>
+        <v>4.5809490740740739E-4</v>
       </c>
       <c r="N5" s="62">
         <f>NK!D16</f>
-        <v>7.1551157407407403E-4</v>
+        <v>7.2157523148148146E-4</v>
       </c>
       <c r="O5" s="62">
         <f>NK!D15</f>
-        <v>9.8333333333333324E-4</v>
+        <v>9.9166666666666674E-4</v>
       </c>
       <c r="P5" s="62">
         <f>NK!D17</f>
-        <v>8.1876157407407407E-4</v>
+        <v>8.2570023148148151E-4</v>
       </c>
       <c r="Q5" s="62">
         <f>NK!D19</f>
-        <v>2.0244374999999998E-3</v>
+        <v>2.04159375E-3</v>
       </c>
       <c r="R5" s="62">
         <f>NK!D18</f>
-        <v>1.8460717592592589E-3</v>
+        <v>1.8617164351851848E-3</v>
       </c>
       <c r="S5" s="62">
         <f t="shared" ref="S5:S9" si="5">M5</f>
-        <v>4.5424537037037037E-4</v>
+        <v>4.5809490740740739E-4</v>
       </c>
       <c r="T5" s="62">
         <f t="shared" si="0"/>
-        <v>7.1551157407407403E-4</v>
+        <v>7.2157523148148146E-4</v>
       </c>
       <c r="U5" s="62">
         <f t="shared" si="1"/>
-        <v>9.8333333333333324E-4</v>
+        <v>9.9166666666666674E-4</v>
       </c>
       <c r="V5" s="62">
         <f t="shared" si="2"/>
-        <v>8.1876157407407407E-4</v>
+        <v>8.2570023148148151E-4</v>
       </c>
       <c r="W5" s="62">
         <f t="shared" si="3"/>
-        <v>2.0244374999999998E-3</v>
+        <v>2.04159375E-3</v>
       </c>
       <c r="X5" s="62">
         <f t="shared" si="4"/>
-        <v>1.8460717592592589E-3</v>
+        <v>1.8617164351851848E-3</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A6" s="59" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="B6" s="59" t="s">
         <v>182</v>
@@ -13879,56 +13879,56 @@
       </c>
       <c r="M6" s="62">
         <f>NK!C14</f>
-        <v>4.6353240740740735E-4</v>
+        <v>4.6746064814814805E-4</v>
       </c>
       <c r="N6" s="62">
         <f>NK!C16</f>
-        <v>7.2916898148148146E-4</v>
+        <v>7.3534837962962963E-4</v>
       </c>
       <c r="O6" s="62">
         <f>NK!C15</f>
-        <v>1.0006782407407406E-3</v>
+        <v>1.0091585648148147E-3</v>
       </c>
       <c r="P6" s="62">
         <f>NK!C17</f>
-        <v>8.3952083333333329E-4</v>
+        <v>8.4663541666666665E-4</v>
       </c>
       <c r="Q6" s="62">
         <f>NK!C19</f>
-        <v>2.067458333333333E-3</v>
+        <v>2.0849791666666664E-3</v>
       </c>
       <c r="R6" s="62">
         <f>NK!C18</f>
-        <v>1.8833564814814815E-3</v>
+        <v>1.8993171296296297E-3</v>
       </c>
       <c r="S6" s="62">
         <f t="shared" si="5"/>
-        <v>4.6353240740740735E-4</v>
+        <v>4.6746064814814805E-4</v>
       </c>
       <c r="T6" s="62">
         <f t="shared" si="0"/>
-        <v>7.2916898148148146E-4</v>
+        <v>7.3534837962962963E-4</v>
       </c>
       <c r="U6" s="62">
         <f t="shared" si="1"/>
-        <v>1.0006782407407406E-3</v>
+        <v>1.0091585648148147E-3</v>
       </c>
       <c r="V6" s="62">
         <f t="shared" si="2"/>
-        <v>8.3952083333333329E-4</v>
+        <v>8.4663541666666665E-4</v>
       </c>
       <c r="W6" s="62">
         <f t="shared" si="3"/>
-        <v>2.067458333333333E-3</v>
+        <v>2.0849791666666664E-3</v>
       </c>
       <c r="X6" s="62">
         <f t="shared" si="4"/>
-        <v>1.8833564814814815E-3</v>
+        <v>1.8993171296296297E-3</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A7" s="59" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B7" s="59" t="s">
         <v>164</v>
@@ -14010,7 +14010,7 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A8" s="59" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B8" s="59" t="s">
         <v>164</v>
@@ -14092,7 +14092,7 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A9" s="59" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B9" s="59" t="s">
         <v>164</v>
@@ -14207,51 +14207,51 @@
       </c>
       <c r="M10" s="62">
         <f>NK!$R$14</f>
-        <v>4.0805555555555549E-4</v>
+        <v>4.1166666666666663E-4</v>
       </c>
       <c r="N10" s="62">
         <f>NK!$R$16</f>
-        <v>6.4608796296296289E-4</v>
+        <v>6.5180555555555554E-4</v>
       </c>
       <c r="O10" s="62">
         <f>NK!$R$15</f>
-        <v>8.7221874999999995E-4</v>
+        <v>8.7993749999999997E-4</v>
       </c>
       <c r="P10" s="62">
         <f>NK!$R$17</f>
-        <v>7.2469097222222206E-4</v>
+        <v>7.3110416666666647E-4</v>
       </c>
       <c r="Q10" s="62">
         <f>NK!$R$19</f>
-        <v>1.8150624999999998E-3</v>
+        <v>1.8311249999999999E-3</v>
       </c>
       <c r="R10" s="62">
         <f>NK!$R$18</f>
-        <v>1.660864583333333E-3</v>
+        <v>1.6755624999999998E-3</v>
       </c>
       <c r="S10" s="62">
         <f>M10</f>
-        <v>4.0805555555555549E-4</v>
+        <v>4.1166666666666663E-4</v>
       </c>
       <c r="T10" s="62">
         <f t="shared" ref="T10:T15" si="6">N10</f>
-        <v>6.4608796296296289E-4</v>
+        <v>6.5180555555555554E-4</v>
       </c>
       <c r="U10" s="62">
         <f t="shared" ref="U10:U15" si="7">O10</f>
-        <v>8.7221874999999995E-4</v>
+        <v>8.7993749999999997E-4</v>
       </c>
       <c r="V10" s="62">
         <f t="shared" ref="V10:V15" si="8">P10</f>
-        <v>7.2469097222222206E-4</v>
+        <v>7.3110416666666647E-4</v>
       </c>
       <c r="W10" s="62">
         <f t="shared" ref="W10:W15" si="9">Q10</f>
-        <v>1.8150624999999998E-3</v>
+        <v>1.8311249999999999E-3</v>
       </c>
       <c r="X10" s="62">
         <f t="shared" ref="X10:X15" si="10">R10</f>
-        <v>1.660864583333333E-3</v>
+        <v>1.6755624999999998E-3</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.45">
@@ -14289,51 +14289,51 @@
       </c>
       <c r="M11" s="62">
         <f>NK!$S$14</f>
-        <v>3.9641550925925923E-4</v>
+        <v>3.9992361111111104E-4</v>
       </c>
       <c r="N11" s="62">
         <f>NK!$S$16</f>
-        <v>6.2895486111111106E-4</v>
+        <v>6.3452083333333329E-4</v>
       </c>
       <c r="O11" s="62">
         <f>NK!$S$15</f>
-        <v>8.4449189814814803E-4</v>
+        <v>8.5196527777777766E-4</v>
       </c>
       <c r="P11" s="62">
         <f>NK!$S$17</f>
-        <v>6.9931828703703692E-4</v>
+        <v>7.0550694444444437E-4</v>
       </c>
       <c r="Q11" s="62">
         <f>NK!$S$19</f>
-        <v>1.79740625E-3</v>
+        <v>1.8133124999999998E-3</v>
       </c>
       <c r="R11" s="62">
         <f>NK!$S$18</f>
-        <v>1.6143043981481481E-3</v>
+        <v>1.6285902777777778E-3</v>
       </c>
       <c r="S11" s="62">
         <f t="shared" ref="S11:S15" si="11">M11</f>
-        <v>3.9641550925925923E-4</v>
+        <v>3.9992361111111104E-4</v>
       </c>
       <c r="T11" s="62">
         <f t="shared" si="6"/>
-        <v>6.2895486111111106E-4</v>
+        <v>6.3452083333333329E-4</v>
       </c>
       <c r="U11" s="62">
         <f t="shared" si="7"/>
-        <v>8.4449189814814803E-4</v>
+        <v>8.5196527777777766E-4</v>
       </c>
       <c r="V11" s="62">
         <f t="shared" si="8"/>
-        <v>6.9931828703703692E-4</v>
+        <v>7.0550694444444437E-4</v>
       </c>
       <c r="W11" s="62">
         <f t="shared" si="9"/>
-        <v>1.79740625E-3</v>
+        <v>1.8133124999999998E-3</v>
       </c>
       <c r="X11" s="62">
         <f t="shared" si="10"/>
-        <v>1.6143043981481481E-3</v>
+        <v>1.6285902777777778E-3</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.45">
@@ -14371,51 +14371,51 @@
       </c>
       <c r="M12" s="62">
         <f>NK!$T$14</f>
-        <v>3.8307523148148147E-4</v>
+        <v>3.8646527777777773E-4</v>
       </c>
       <c r="N12" s="62">
         <f>NK!$T$16</f>
-        <v>6.0946759259259255E-4</v>
+        <v>6.1486111111111106E-4</v>
       </c>
       <c r="O12" s="62">
         <f>NK!$T$15</f>
-        <v>8.1271064814814802E-4</v>
+        <v>8.1990277777777769E-4</v>
       </c>
       <c r="P12" s="62">
         <f>NK!$T$17</f>
-        <v>6.7028356481481474E-4</v>
+        <v>6.7621527777777775E-4</v>
       </c>
       <c r="Q12" s="62">
         <f>NK!$T$19</f>
-        <v>1.7427372685185185E-3</v>
+        <v>1.7581597222222222E-3</v>
       </c>
       <c r="R12" s="62">
         <f>NK!$T$18</f>
-        <v>1.5612048611111109E-3</v>
+        <v>1.5750208333333332E-3</v>
       </c>
       <c r="S12" s="62">
         <f t="shared" si="11"/>
-        <v>3.8307523148148147E-4</v>
+        <v>3.8646527777777773E-4</v>
       </c>
       <c r="T12" s="62">
         <f t="shared" si="6"/>
-        <v>6.0946759259259255E-4</v>
+        <v>6.1486111111111106E-4</v>
       </c>
       <c r="U12" s="62">
         <f t="shared" si="7"/>
-        <v>8.1271064814814802E-4</v>
+        <v>8.1990277777777769E-4</v>
       </c>
       <c r="V12" s="62">
         <f t="shared" si="8"/>
-        <v>6.7028356481481474E-4</v>
+        <v>6.7621527777777775E-4</v>
       </c>
       <c r="W12" s="62">
         <f t="shared" si="9"/>
-        <v>1.7427372685185185E-3</v>
+        <v>1.7581597222222222E-3</v>
       </c>
       <c r="X12" s="62">
         <f t="shared" si="10"/>
-        <v>1.5612048611111109E-3</v>
+        <v>1.5750208333333332E-3</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.45">
@@ -14453,51 +14453,51 @@
       </c>
       <c r="M13" s="62">
         <f>NK!$X$14</f>
-        <v>4.9829861111111114E-4</v>
+        <v>5.3357638888888888E-4</v>
       </c>
       <c r="N13" s="62">
         <f>NK!$X$16</f>
-        <v>7.5895717592592594E-4</v>
+        <v>8.1268865740740748E-4</v>
       </c>
       <c r="O13" s="62">
         <f>NK!$X$15</f>
-        <v>1.0173923611111108E-3</v>
+        <v>1.0894201388888887E-3</v>
       </c>
       <c r="P13" s="62">
         <f>NK!$X$17</f>
-        <v>8.3912962962962945E-4</v>
+        <v>8.9853703703703699E-4</v>
       </c>
       <c r="Q13" s="62">
         <f>NK!$X$19</f>
-        <v>1.9971180555555554E-3</v>
+        <v>2.1385069444444442E-3</v>
       </c>
       <c r="R13" s="62">
         <f>NK!$X$18</f>
-        <v>1.8226481481481483E-3</v>
+        <v>1.9516851851851854E-3</v>
       </c>
       <c r="S13" s="62">
         <f t="shared" si="11"/>
-        <v>4.9829861111111114E-4</v>
+        <v>5.3357638888888888E-4</v>
       </c>
       <c r="T13" s="62">
         <f t="shared" si="6"/>
-        <v>7.5895717592592594E-4</v>
+        <v>8.1268865740740748E-4</v>
       </c>
       <c r="U13" s="62">
         <f t="shared" si="7"/>
-        <v>1.0173923611111108E-3</v>
+        <v>1.0894201388888887E-3</v>
       </c>
       <c r="V13" s="62">
         <f t="shared" si="8"/>
-        <v>8.3912962962962945E-4</v>
+        <v>8.9853703703703699E-4</v>
       </c>
       <c r="W13" s="62">
         <f t="shared" si="9"/>
-        <v>1.9971180555555554E-3</v>
+        <v>2.1385069444444442E-3</v>
       </c>
       <c r="X13" s="62">
         <f t="shared" si="10"/>
-        <v>1.8226481481481483E-3</v>
+        <v>1.9516851851851854E-3</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.45">
@@ -14535,51 +14535,51 @@
       </c>
       <c r="M14" s="62">
         <f>NK!$Y$14</f>
-        <v>4.7514930555555554E-4</v>
+        <v>5.0878819444444441E-4</v>
       </c>
       <c r="N14" s="62">
         <f>NK!$Y$16</f>
-        <v>7.2992245370370366E-4</v>
+        <v>7.8159837962962959E-4</v>
       </c>
       <c r="O14" s="62">
         <f>NK!$Y$15</f>
-        <v>9.7135532407407403E-4</v>
+        <v>1.0401238425925925E-3</v>
       </c>
       <c r="P14" s="62">
         <f>NK!$Y$17</f>
-        <v>8.0381712962962959E-4</v>
+        <v>8.6072453703703701E-4</v>
       </c>
       <c r="Q14" s="62">
         <f>NK!$Y$19</f>
-        <v>1.9407488425925922E-3</v>
+        <v>2.0781469907407406E-3</v>
       </c>
       <c r="R14" s="62">
         <f>NK!$Y$18</f>
-        <v>1.7873356481481479E-3</v>
+        <v>1.9138726851851851E-3</v>
       </c>
       <c r="S14" s="62">
         <f t="shared" si="11"/>
-        <v>4.7514930555555554E-4</v>
+        <v>5.0878819444444441E-4</v>
       </c>
       <c r="T14" s="62">
         <f t="shared" si="6"/>
-        <v>7.2992245370370366E-4</v>
+        <v>7.8159837962962959E-4</v>
       </c>
       <c r="U14" s="62">
         <f t="shared" si="7"/>
-        <v>9.7135532407407403E-4</v>
+        <v>1.0401238425925925E-3</v>
       </c>
       <c r="V14" s="62">
         <f t="shared" si="8"/>
-        <v>8.0381712962962959E-4</v>
+        <v>8.6072453703703701E-4</v>
       </c>
       <c r="W14" s="62">
         <f t="shared" si="9"/>
-        <v>1.9407488425925922E-3</v>
+        <v>2.0781469907407406E-3</v>
       </c>
       <c r="X14" s="62">
         <f t="shared" si="10"/>
-        <v>1.7873356481481479E-3</v>
+        <v>1.9138726851851851E-3</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.45">
@@ -14617,51 +14617,51 @@
       </c>
       <c r="M15" s="62">
         <f>NK!$Z$14</f>
-        <v>4.5814699074074068E-4</v>
+        <v>4.9058217592592589E-4</v>
       </c>
       <c r="N15" s="62">
         <f>NK!$Z$16</f>
-        <v>7.0873495370370361E-4</v>
+        <v>7.5891087962962956E-4</v>
       </c>
       <c r="O15" s="62">
         <f>NK!$Z$15</f>
-        <v>9.376122685185184E-4</v>
+        <v>1.0039918981481482E-3</v>
       </c>
       <c r="P15" s="62">
         <f>NK!$Z$17</f>
-        <v>7.779212962962962E-4</v>
+        <v>8.3299537037037033E-4</v>
       </c>
       <c r="Q15" s="62">
         <f>NK!$Z$19</f>
-        <v>1.8995509259259258E-3</v>
+        <v>2.0340324074074076E-3</v>
       </c>
       <c r="R15" s="62">
         <f>NK!$Z$18</f>
-        <v>1.7615706018518516E-3</v>
+        <v>1.8862835648148148E-3</v>
       </c>
       <c r="S15" s="62">
         <f t="shared" si="11"/>
-        <v>4.5814699074074068E-4</v>
+        <v>4.9058217592592589E-4</v>
       </c>
       <c r="T15" s="62">
         <f t="shared" si="6"/>
-        <v>7.0873495370370361E-4</v>
+        <v>7.5891087962962956E-4</v>
       </c>
       <c r="U15" s="62">
         <f t="shared" si="7"/>
-        <v>9.376122685185184E-4</v>
+        <v>1.0039918981481482E-3</v>
       </c>
       <c r="V15" s="62">
         <f t="shared" si="8"/>
-        <v>7.779212962962962E-4</v>
+        <v>8.3299537037037033E-4</v>
       </c>
       <c r="W15" s="62">
         <f t="shared" si="9"/>
-        <v>1.8995509259259258E-3</v>
+        <v>2.0340324074074076E-3</v>
       </c>
       <c r="X15" s="62">
         <f t="shared" si="10"/>
-        <v>1.7615706018518516E-3</v>
+        <v>1.8862835648148148E-3</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.45">
@@ -20556,8 +20556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A13DA696-49DD-4BFA-98FE-5C7770404E50}">
   <dimension ref="B3:AA37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA14" sqref="AA14:AA19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AA14" sqref="AA14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -21020,18 +21020,18 @@
       </c>
       <c r="C14" s="65">
         <f>C5*$F14</f>
-        <v>4.6353240740740735E-4</v>
+        <v>4.6746064814814805E-4</v>
       </c>
       <c r="D14" s="65">
         <f t="shared" ref="D14:E14" si="0">D5*$F14</f>
-        <v>4.5424537037037037E-4</v>
+        <v>4.5809490740740739E-4</v>
       </c>
       <c r="E14" s="65">
         <f t="shared" si="0"/>
-        <v>4.4045138888888888E-4</v>
+        <v>4.4418402777777777E-4</v>
       </c>
       <c r="F14">
-        <v>1.18</v>
+        <v>1.19</v>
       </c>
       <c r="H14" s="64" t="s">
         <v>0</v>
@@ -21056,36 +21056,36 @@
       </c>
       <c r="R14" s="65">
         <f t="shared" ref="R14:T19" si="2">R5*$U14</f>
-        <v>4.0805555555555549E-4</v>
+        <v>4.1166666666666663E-4</v>
       </c>
       <c r="S14" s="65">
         <f t="shared" si="2"/>
-        <v>3.9641550925925923E-4</v>
+        <v>3.9992361111111104E-4</v>
       </c>
       <c r="T14" s="65">
         <f t="shared" si="2"/>
-        <v>3.8307523148148147E-4</v>
+        <v>3.8646527777777773E-4</v>
       </c>
       <c r="U14">
-        <v>1.1299999999999999</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="W14" s="64" t="s">
         <v>0</v>
       </c>
       <c r="X14" s="65">
         <f>X5*$AA14</f>
-        <v>4.9829861111111114E-4</v>
+        <v>5.3357638888888888E-4</v>
       </c>
       <c r="Y14" s="65">
         <f t="shared" ref="Y14:Z14" si="3">Y5*$AA14</f>
-        <v>4.7514930555555554E-4</v>
+        <v>5.0878819444444441E-4</v>
       </c>
       <c r="Z14" s="65">
         <f t="shared" si="3"/>
-        <v>4.5814699074074068E-4</v>
+        <v>4.9058217592592589E-4</v>
       </c>
       <c r="AA14">
-        <v>1.1299999999999999</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="15" spans="2:27" x14ac:dyDescent="0.45">
@@ -21094,18 +21094,18 @@
       </c>
       <c r="C15" s="65">
         <f t="shared" ref="C15:E15" si="4">C6*$F15</f>
-        <v>1.0006782407407406E-3</v>
+        <v>1.0091585648148147E-3</v>
       </c>
       <c r="D15" s="65">
         <f t="shared" si="4"/>
-        <v>9.8333333333333324E-4</v>
+        <v>9.9166666666666674E-4</v>
       </c>
       <c r="E15" s="65">
         <f t="shared" si="4"/>
-        <v>9.4522916666666681E-4</v>
+        <v>9.532395833333335E-4</v>
       </c>
       <c r="F15">
-        <v>1.18</v>
+        <v>1.19</v>
       </c>
       <c r="H15" s="64" t="s">
         <v>223</v>
@@ -21130,36 +21130,36 @@
       </c>
       <c r="R15" s="65">
         <f t="shared" si="2"/>
-        <v>8.7221874999999995E-4</v>
+        <v>8.7993749999999997E-4</v>
       </c>
       <c r="S15" s="65">
         <f t="shared" si="2"/>
-        <v>8.4449189814814803E-4</v>
+        <v>8.5196527777777766E-4</v>
       </c>
       <c r="T15" s="65">
         <f t="shared" si="2"/>
-        <v>8.1271064814814802E-4</v>
+        <v>8.1990277777777769E-4</v>
       </c>
       <c r="U15">
-        <v>1.1299999999999999</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="W15" s="64" t="s">
         <v>223</v>
       </c>
       <c r="X15" s="65">
         <f t="shared" ref="X15:Z15" si="6">X6*$AA15</f>
-        <v>1.0173923611111108E-3</v>
+        <v>1.0894201388888887E-3</v>
       </c>
       <c r="Y15" s="65">
         <f t="shared" si="6"/>
-        <v>9.7135532407407403E-4</v>
+        <v>1.0401238425925925E-3</v>
       </c>
       <c r="Z15" s="65">
         <f t="shared" si="6"/>
-        <v>9.376122685185184E-4</v>
+        <v>1.0039918981481482E-3</v>
       </c>
       <c r="AA15">
-        <v>1.1299999999999999</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="16" spans="2:27" x14ac:dyDescent="0.45">
@@ -21168,18 +21168,18 @@
       </c>
       <c r="C16" s="65">
         <f t="shared" ref="C16:E16" si="7">C7*$F16</f>
-        <v>7.2916898148148146E-4</v>
+        <v>7.3534837962962963E-4</v>
       </c>
       <c r="D16" s="65">
         <f t="shared" si="7"/>
-        <v>7.1551157407407403E-4</v>
+        <v>7.2157523148148146E-4</v>
       </c>
       <c r="E16" s="65">
         <f t="shared" si="7"/>
-        <v>6.9557175925925928E-4</v>
+        <v>7.0146643518518518E-4</v>
       </c>
       <c r="F16">
-        <v>1.18</v>
+        <v>1.19</v>
       </c>
       <c r="H16" s="64" t="s">
         <v>224</v>
@@ -21204,36 +21204,36 @@
       </c>
       <c r="R16" s="65">
         <f t="shared" si="2"/>
-        <v>6.4608796296296289E-4</v>
+        <v>6.5180555555555554E-4</v>
       </c>
       <c r="S16" s="65">
         <f t="shared" si="2"/>
-        <v>6.2895486111111106E-4</v>
+        <v>6.3452083333333329E-4</v>
       </c>
       <c r="T16" s="65">
         <f t="shared" si="2"/>
-        <v>6.0946759259259255E-4</v>
+        <v>6.1486111111111106E-4</v>
       </c>
       <c r="U16">
-        <v>1.1299999999999999</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="W16" s="64" t="s">
         <v>224</v>
       </c>
       <c r="X16" s="65">
         <f t="shared" ref="X16:Z16" si="9">X7*$AA16</f>
-        <v>7.5895717592592594E-4</v>
+        <v>8.1268865740740748E-4</v>
       </c>
       <c r="Y16" s="65">
         <f>Y7*$AA16</f>
-        <v>7.2992245370370366E-4</v>
+        <v>7.8159837962962959E-4</v>
       </c>
       <c r="Z16" s="65">
         <f t="shared" si="9"/>
-        <v>7.0873495370370361E-4</v>
+        <v>7.5891087962962956E-4</v>
       </c>
       <c r="AA16">
-        <v>1.1299999999999999</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="17" spans="2:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -21242,18 +21242,18 @@
       </c>
       <c r="C17" s="65">
         <f t="shared" ref="C17:E17" si="10">C8*$F17</f>
-        <v>8.3952083333333329E-4</v>
+        <v>8.4663541666666665E-4</v>
       </c>
       <c r="D17" s="65">
         <f t="shared" si="10"/>
-        <v>8.1876157407407407E-4</v>
+        <v>8.2570023148148151E-4</v>
       </c>
       <c r="E17" s="65">
         <f t="shared" si="10"/>
-        <v>7.884421296296295E-4</v>
+        <v>7.951238425925925E-4</v>
       </c>
       <c r="F17">
-        <v>1.18</v>
+        <v>1.19</v>
       </c>
       <c r="H17" s="64" t="s">
         <v>225</v>
@@ -21278,36 +21278,36 @@
       </c>
       <c r="R17" s="65">
         <f t="shared" si="2"/>
-        <v>7.2469097222222206E-4</v>
+        <v>7.3110416666666647E-4</v>
       </c>
       <c r="S17" s="65">
         <f t="shared" si="2"/>
-        <v>6.9931828703703692E-4</v>
+        <v>7.0550694444444437E-4</v>
       </c>
       <c r="T17" s="65">
         <f t="shared" si="2"/>
-        <v>6.7028356481481474E-4</v>
+        <v>6.7621527777777775E-4</v>
       </c>
       <c r="U17">
-        <v>1.1299999999999999</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="W17" s="64" t="s">
         <v>225</v>
       </c>
       <c r="X17" s="65">
         <f t="shared" ref="X17:Z17" si="12">X8*$AA17</f>
-        <v>8.3912962962962945E-4</v>
+        <v>8.9853703703703699E-4</v>
       </c>
       <c r="Y17" s="65">
         <f>Y8*$AA17</f>
-        <v>8.0381712962962959E-4</v>
+        <v>8.6072453703703701E-4</v>
       </c>
       <c r="Z17" s="65">
         <f t="shared" si="12"/>
-        <v>7.779212962962962E-4</v>
+        <v>8.3299537037037033E-4</v>
       </c>
       <c r="AA17">
-        <v>1.1299999999999999</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="18" spans="2:27" x14ac:dyDescent="0.45">
@@ -21316,18 +21316,18 @@
       </c>
       <c r="C18" s="65">
         <f t="shared" ref="C18:E18" si="13">C9*$F18</f>
-        <v>1.8833564814814815E-3</v>
+        <v>1.8993171296296297E-3</v>
       </c>
       <c r="D18" s="65">
         <f t="shared" si="13"/>
-        <v>1.8460717592592589E-3</v>
+        <v>1.8617164351851848E-3</v>
       </c>
       <c r="E18" s="65">
         <f t="shared" si="13"/>
-        <v>1.7914421296296294E-3</v>
+        <v>1.8066238425925923E-3</v>
       </c>
       <c r="F18">
-        <v>1.18</v>
+        <v>1.19</v>
       </c>
       <c r="H18" s="64" t="s">
         <v>226</v>
@@ -21352,36 +21352,36 @@
       </c>
       <c r="R18" s="65">
         <f t="shared" si="2"/>
-        <v>1.660864583333333E-3</v>
+        <v>1.6755624999999998E-3</v>
       </c>
       <c r="S18" s="65">
         <f t="shared" si="2"/>
-        <v>1.6143043981481481E-3</v>
+        <v>1.6285902777777778E-3</v>
       </c>
       <c r="T18" s="65">
         <f t="shared" si="2"/>
-        <v>1.5612048611111109E-3</v>
+        <v>1.5750208333333332E-3</v>
       </c>
       <c r="U18">
-        <v>1.1299999999999999</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="W18" s="64" t="s">
         <v>226</v>
       </c>
       <c r="X18" s="65">
         <f t="shared" ref="X18:Z18" si="15">X9*$AA18</f>
-        <v>1.8226481481481483E-3</v>
+        <v>1.9516851851851854E-3</v>
       </c>
       <c r="Y18" s="65">
         <f t="shared" si="15"/>
-        <v>1.7873356481481479E-3</v>
+        <v>1.9138726851851851E-3</v>
       </c>
       <c r="Z18" s="65">
         <f t="shared" si="15"/>
-        <v>1.7615706018518516E-3</v>
+        <v>1.8862835648148148E-3</v>
       </c>
       <c r="AA18">
-        <v>1.1299999999999999</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="19" spans="2:27" x14ac:dyDescent="0.45">
@@ -21390,18 +21390,18 @@
       </c>
       <c r="C19" s="65">
         <f t="shared" ref="C19:E19" si="16">C10*$F19</f>
-        <v>2.067458333333333E-3</v>
+        <v>2.0849791666666664E-3</v>
       </c>
       <c r="D19" s="65">
         <f t="shared" si="16"/>
-        <v>2.0244374999999998E-3</v>
+        <v>2.04159375E-3</v>
       </c>
       <c r="E19" s="65">
         <f t="shared" si="16"/>
-        <v>1.961340277777778E-3</v>
+        <v>1.9779618055555557E-3</v>
       </c>
       <c r="F19">
-        <v>1.18</v>
+        <v>1.19</v>
       </c>
       <c r="H19" s="64" t="s">
         <v>4</v>
@@ -21426,36 +21426,36 @@
       </c>
       <c r="R19" s="65">
         <f t="shared" si="2"/>
-        <v>1.8150624999999998E-3</v>
+        <v>1.8311249999999999E-3</v>
       </c>
       <c r="S19" s="65">
         <f t="shared" si="2"/>
-        <v>1.79740625E-3</v>
+        <v>1.8133124999999998E-3</v>
       </c>
       <c r="T19" s="65">
         <f t="shared" si="2"/>
-        <v>1.7427372685185185E-3</v>
+        <v>1.7581597222222222E-3</v>
       </c>
       <c r="U19">
-        <v>1.1299999999999999</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="W19" s="64" t="s">
         <v>4</v>
       </c>
       <c r="X19" s="65">
         <f t="shared" ref="X19:Z19" si="18">X10*$AA19</f>
-        <v>1.9971180555555554E-3</v>
+        <v>2.1385069444444442E-3</v>
       </c>
       <c r="Y19" s="65">
         <f t="shared" si="18"/>
-        <v>1.9407488425925922E-3</v>
+        <v>2.0781469907407406E-3</v>
       </c>
       <c r="Z19" s="65">
         <f t="shared" si="18"/>
-        <v>1.8995509259259258E-3</v>
+        <v>2.0340324074074076E-3</v>
       </c>
       <c r="AA19">
-        <v>1.1299999999999999</v>
+        <v>1.21</v>
       </c>
     </row>
     <row r="22" spans="2:27" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
kleine anpassungen Kalender! Gleich Dynamisierung mit excel
</commit_message>
<xml_diff>
--- a/web/utilities/records_kriterien.xlsx
+++ b/web/utilities/records_kriterien.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgna\Documents\GitHub\Lifesaving_Baden\web\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0A3D19-F657-40F0-B300-5340DD37E0F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7412C3B3-4A7B-4AB6-BDF4-5C1DC445D931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13335" firstSheet="1" activeTab="7" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="7" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
   </bookViews>
   <sheets>
     <sheet name="DR" sheetId="9" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="BP" sheetId="11" r:id="rId5"/>
     <sheet name="DEM" sheetId="12" r:id="rId6"/>
     <sheet name="JRP" sheetId="13" r:id="rId7"/>
-    <sheet name="Kalender LK" sheetId="15" r:id="rId8"/>
+    <sheet name="LK Kalender" sheetId="15" r:id="rId8"/>
     <sheet name="NK" sheetId="14" r:id="rId9"/>
     <sheet name="2024" sheetId="6" r:id="rId10"/>
     <sheet name="2025" sheetId="5" r:id="rId11"/>
@@ -221,7 +221,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="301">
   <si>
     <t>50m Retten</t>
   </si>
@@ -1057,19 +1057,73 @@
     <t>ort</t>
   </si>
   <si>
-    <t>info</t>
-  </si>
-  <si>
     <t>Kadertraining LK1</t>
   </si>
   <si>
-    <t>+ Beach Flags</t>
-  </si>
-  <si>
     <t>Fächerbad, Karlsruhe</t>
   </si>
   <si>
     <t>LK1</t>
+  </si>
+  <si>
+    <t>meta</t>
+  </si>
+  <si>
+    <t>50m Bahn, Treffpunkt 9:15 im Foyer</t>
+  </si>
+  <si>
+    <t>Kadertraining LK2</t>
+  </si>
+  <si>
+    <t>Warm Up, 50m Bahn, Cool Down, Treffpunkt 11:30 im Foyer</t>
+  </si>
+  <si>
+    <t>LK2</t>
+  </si>
+  <si>
+    <t>WarmUp, Beach Flags, 50m Bahn, Cool down, Treffpunkt: 12:00 Uhr im Foyer</t>
+  </si>
+  <si>
+    <t>JRP und LMS Vorbereitung. (Ocean &amp; Pool)</t>
+  </si>
+  <si>
+    <t>Buchtzigsee, Ettlingen &amp; Fächerbad, Karlsruhe</t>
+  </si>
+  <si>
+    <t>50m Bahn, Treffpunkt 12:45 im Foyer</t>
+  </si>
+  <si>
+    <t>Junioren Rettungspokal</t>
+  </si>
+  <si>
+    <t>(Nominierungswettkampf)</t>
+  </si>
+  <si>
+    <t>Paderborn/Lippstadt</t>
+  </si>
+  <si>
+    <t>Trainingslehrgang LK3</t>
+  </si>
+  <si>
+    <t>Tageslehrgang für LK3 und deren Heimtrainer zu den neuen Disziplinen. (Noch nicht fix)</t>
+  </si>
+  <si>
+    <t>Hallenbad Oberhausen-Rheinhausen</t>
+  </si>
+  <si>
+    <t>LK3</t>
+  </si>
+  <si>
+    <t>18. Bodensee Pokal</t>
+  </si>
+  <si>
+    <t>Internationaler Wettkampf für Baden, Württemberg, Bayern, Österreich, Schweiz. (Nominierungswettkampf)</t>
+  </si>
+  <si>
+    <t>Stuttgart, RheinNeckar Park</t>
+  </si>
+  <si>
+    <t>LK1 / LK2 / LK3</t>
   </si>
 </sst>
 </file>
@@ -1537,6 +1591,9 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1546,28 +1603,15 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="199">
+  <dxfs count="200">
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <font>
+        <color theme="4"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1658,6 +1702,21 @@
       <font>
         <color theme="4"/>
       </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="m:ss.00"/>
@@ -3975,102 +4034,102 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2C5E83EE-6B6F-478A-9C90-A846A1A76536}" name="WR_Open4" displayName="WR_Open4" ref="A4:AW31" totalsRowShown="0" headerRowDxfId="198" headerRowBorderDxfId="197" tableBorderDxfId="196">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2C5E83EE-6B6F-478A-9C90-A846A1A76536}" name="WR_Open4" displayName="WR_Open4" ref="A4:AW31" totalsRowShown="0" headerRowDxfId="199" headerRowBorderDxfId="198" tableBorderDxfId="197">
   <autoFilter ref="A4:AW31" xr:uid="{2C5E83EE-6B6F-478A-9C90-A846A1A76536}"/>
   <tableColumns count="49">
-    <tableColumn id="1" xr3:uid="{7C0C4105-A61A-4B8D-9129-EDC4F18765AF}" name="WR-Open" dataDxfId="195">
+    <tableColumn id="1" xr3:uid="{7C0C4105-A61A-4B8D-9129-EDC4F18765AF}" name="WR-Open" dataDxfId="196">
       <calculatedColumnFormula>A4+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{516F5612-F85F-413F-9012-E235F415E34B}" name="50m Retten - offen - W" dataDxfId="194"/>
-    <tableColumn id="3" xr3:uid="{BC9ACAC9-0D45-42FD-B596-D19FBE3A4D83}" name="100m Retten - offen - W" dataDxfId="193"/>
-    <tableColumn id="4" xr3:uid="{CB6DBE59-EB65-43F0-93E7-0BDC3F82832B}" name="100m Kombi - offen - W" dataDxfId="192"/>
-    <tableColumn id="5" xr3:uid="{AA603C60-6831-4C14-A8CD-0AA050DA7551}" name="100m Lifesaver - offen - W" dataDxfId="191"/>
-    <tableColumn id="6" xr3:uid="{7920F147-7717-4582-940A-2610F7D310CA}" name="200m Superlifesaver - offen - W" dataDxfId="190"/>
-    <tableColumn id="7" xr3:uid="{04E21F1D-AC8D-4A1B-9B43-59B8F7901673}" name="200m Hindernis - offen - W" dataDxfId="189"/>
-    <tableColumn id="8" xr3:uid="{40E8A083-653A-48A8-9B37-0A2D850B7829}" name="50m Retten - offen - M" dataDxfId="188"/>
-    <tableColumn id="9" xr3:uid="{863824A9-134F-4189-BB14-225AE224FC44}" name="100m Retten - offen - M" dataDxfId="187"/>
+    <tableColumn id="2" xr3:uid="{516F5612-F85F-413F-9012-E235F415E34B}" name="50m Retten - offen - W" dataDxfId="195"/>
+    <tableColumn id="3" xr3:uid="{BC9ACAC9-0D45-42FD-B596-D19FBE3A4D83}" name="100m Retten - offen - W" dataDxfId="194"/>
+    <tableColumn id="4" xr3:uid="{CB6DBE59-EB65-43F0-93E7-0BDC3F82832B}" name="100m Kombi - offen - W" dataDxfId="193"/>
+    <tableColumn id="5" xr3:uid="{AA603C60-6831-4C14-A8CD-0AA050DA7551}" name="100m Lifesaver - offen - W" dataDxfId="192"/>
+    <tableColumn id="6" xr3:uid="{7920F147-7717-4582-940A-2610F7D310CA}" name="200m Superlifesaver - offen - W" dataDxfId="191"/>
+    <tableColumn id="7" xr3:uid="{04E21F1D-AC8D-4A1B-9B43-59B8F7901673}" name="200m Hindernis - offen - W" dataDxfId="190"/>
+    <tableColumn id="8" xr3:uid="{40E8A083-653A-48A8-9B37-0A2D850B7829}" name="50m Retten - offen - M" dataDxfId="189"/>
+    <tableColumn id="9" xr3:uid="{863824A9-134F-4189-BB14-225AE224FC44}" name="100m Retten - offen - M" dataDxfId="188"/>
     <tableColumn id="10" xr3:uid="{598FC6AE-DEA2-4475-9A35-CDCB8C81496A}" name="100m Kombi - offen - M"/>
     <tableColumn id="11" xr3:uid="{9FC50B37-0D51-422E-A268-A6506D4F3854}" name="100m Lifesaver - offen - M"/>
     <tableColumn id="12" xr3:uid="{B8D2552B-5D82-442A-98F0-E47D5C5F6728}" name="200m Superlifesaver - offen - M"/>
-    <tableColumn id="13" xr3:uid="{5A5E9873-0C5F-4508-AF6B-4974E0526D84}" name="200m Hindernis - offen - M" dataDxfId="186"/>
-    <tableColumn id="14" xr3:uid="{FA907992-7FCE-4CAD-8CF2-F5BEBC9B3756}" name="50m Retten - 17/18 - W" dataDxfId="185"/>
-    <tableColumn id="15" xr3:uid="{76B63DC0-CB67-48F4-9B5A-D22902F59334}" name="100m Retten - 17/18 - W" dataDxfId="184"/>
-    <tableColumn id="16" xr3:uid="{614A2419-51B1-44C0-8469-ADBFB078B81A}" name="100m Kombi -17/18 - W" dataDxfId="183"/>
-    <tableColumn id="17" xr3:uid="{2EC953EE-367D-4524-A25E-8DE3B8168E34}" name="100m Lifesaver - 17/18 - W" dataDxfId="182"/>
-    <tableColumn id="18" xr3:uid="{25711867-9BD7-4197-9094-A21392411249}" name="200m Superlifesaver - 17/18 - W" dataDxfId="181"/>
-    <tableColumn id="19" xr3:uid="{262DB142-CFB1-45C3-9332-7273CACD1B62}" name="200m Hindernis - 17/18 - W" dataDxfId="180"/>
-    <tableColumn id="20" xr3:uid="{938BA45A-8244-4637-8A14-DF49CD91A945}" name="50m Retten - 17/18 - M" dataDxfId="179"/>
-    <tableColumn id="21" xr3:uid="{737E28D8-900F-4A98-95FE-EE7B0AFDEE90}" name="100m Retten - 17/18 - M" dataDxfId="178"/>
-    <tableColumn id="22" xr3:uid="{330BD3A8-061C-45E2-ADDB-40C2F346772F}" name="100m Kombi - 17/18 - M" dataDxfId="177"/>
-    <tableColumn id="23" xr3:uid="{0CADDE90-A167-4E1D-8D33-8624E5E1A4E2}" name="100m Lifesaver - 17/18 - M" dataDxfId="176"/>
-    <tableColumn id="24" xr3:uid="{FCF9F42C-1291-4985-9D37-B9DE2DAA5DCB}" name="200m Superlifesaver - 17/18 - M" dataDxfId="175"/>
-    <tableColumn id="25" xr3:uid="{4E5397B2-F924-4F48-AE69-AF6D650AF88D}" name="200m Hindernis - 17/18 - M" dataDxfId="174"/>
-    <tableColumn id="26" xr3:uid="{0A78315A-BFDC-43EE-A66F-48B301F66508}" name="50m Retten - 15/16 - W" dataDxfId="173"/>
-    <tableColumn id="27" xr3:uid="{D3FCF8BD-6C76-450D-80C0-CC0519A79731}" name="100m Retten - 15/16 - W" dataDxfId="172"/>
-    <tableColumn id="28" xr3:uid="{6BE7937E-D62D-47CD-95DE-1730304B0DF3}" name="100m Kombi - 15/16 - W" dataDxfId="171"/>
-    <tableColumn id="29" xr3:uid="{098BA5BE-5AF6-4187-89B6-534498F24C51}" name="100m Lifesaver -  15/16 - W" dataDxfId="170"/>
-    <tableColumn id="30" xr3:uid="{2A6822CF-143C-4BF7-A440-5777527BE512}" name="200m Superlifesaver -  15/16 - W" dataDxfId="169"/>
-    <tableColumn id="31" xr3:uid="{541C7145-CDEA-4E4E-9E7A-A4F05BA6C3E5}" name="200m Hindernis -  15/16 - W" dataDxfId="168"/>
-    <tableColumn id="32" xr3:uid="{342C4488-8C61-42E6-87A9-C75BD8EB7452}" name="50m Retten - 15/16 - M" dataDxfId="167"/>
-    <tableColumn id="33" xr3:uid="{857B1D46-7D20-47F7-AB9B-732D50346E32}" name="100m Retten - 15/16 - M" dataDxfId="166"/>
-    <tableColumn id="34" xr3:uid="{4C8A2EB4-804B-45F1-A768-9A6958957F8B}" name="100m Kombi -15/16 - M" dataDxfId="165"/>
-    <tableColumn id="35" xr3:uid="{26C75B4F-21EC-4EB0-A9A9-54BC80140672}" name="100m Lifesaver - 15/16 - M" dataDxfId="164"/>
-    <tableColumn id="36" xr3:uid="{DBBB2A23-1A06-429A-A5D1-A547EF5EC16F}" name="200m Superlifesaver - 15/16 - M" dataDxfId="163"/>
-    <tableColumn id="37" xr3:uid="{84061231-CAE5-427A-87F5-6DDBA99F77D2}" name="200m Hindernis - 15/16 - M" dataDxfId="162"/>
-    <tableColumn id="38" xr3:uid="{878CCA80-A742-4B3C-90C9-E93BB814201B}" name="50m Retten - 13/14 - W" dataDxfId="161"/>
-    <tableColumn id="39" xr3:uid="{A1F57102-61CF-4784-8DE2-0B8F32D5D699}" name="50m Retten mit Flossen - 13/14 - W" dataDxfId="160"/>
-    <tableColumn id="40" xr3:uid="{0F6BAF78-3D79-42A9-9FED-E6D0E335A920}" name="100m Hindernis - 13/14 - W" dataDxfId="159"/>
-    <tableColumn id="41" xr3:uid="{EB748A68-E10D-4D76-B315-8FDB3AC33C8D}" name="50m Retten - 13/14 - M" dataDxfId="158"/>
-    <tableColumn id="42" xr3:uid="{C7B04167-6430-40F0-9A0F-D0D0BE2F9C77}" name="50m Retten mit Flossen - 13/14 - M" dataDxfId="157"/>
-    <tableColumn id="43" xr3:uid="{48704BB7-A853-445A-8CDC-8D8F86C2B66A}" name="100m Hindernis - 13/14 - M" dataDxfId="156"/>
-    <tableColumn id="44" xr3:uid="{9605FE9A-F41C-4A5F-A59C-B7A9D45C460F}" name="50m Flossen - 12 - W" dataDxfId="155"/>
-    <tableColumn id="45" xr3:uid="{4C9DBF61-35B1-4BC2-8272-526E0AFAAFFB}" name="50m komb. Schwimmen - 12 - W" dataDxfId="154"/>
-    <tableColumn id="46" xr3:uid="{CF433C95-C272-48F9-98CD-7E3C8DBB6F2C}" name="50m Hindernis - 12 - W" dataDxfId="153"/>
-    <tableColumn id="47" xr3:uid="{FADB7411-DB43-4B14-B9E8-D74CA1BA18B8}" name="50m Flossen - 12 - M" dataDxfId="152"/>
-    <tableColumn id="48" xr3:uid="{02936F84-1D82-48AC-8D7C-6D2954D68A06}" name="50m komb. Schwimmen - 12 - M" dataDxfId="151"/>
-    <tableColumn id="49" xr3:uid="{7FD9BD11-0597-4E07-8DA5-DB53384197F5}" name="50m Hindernis - 12 - M" dataDxfId="150"/>
+    <tableColumn id="13" xr3:uid="{5A5E9873-0C5F-4508-AF6B-4974E0526D84}" name="200m Hindernis - offen - M" dataDxfId="187"/>
+    <tableColumn id="14" xr3:uid="{FA907992-7FCE-4CAD-8CF2-F5BEBC9B3756}" name="50m Retten - 17/18 - W" dataDxfId="186"/>
+    <tableColumn id="15" xr3:uid="{76B63DC0-CB67-48F4-9B5A-D22902F59334}" name="100m Retten - 17/18 - W" dataDxfId="185"/>
+    <tableColumn id="16" xr3:uid="{614A2419-51B1-44C0-8469-ADBFB078B81A}" name="100m Kombi -17/18 - W" dataDxfId="184"/>
+    <tableColumn id="17" xr3:uid="{2EC953EE-367D-4524-A25E-8DE3B8168E34}" name="100m Lifesaver - 17/18 - W" dataDxfId="183"/>
+    <tableColumn id="18" xr3:uid="{25711867-9BD7-4197-9094-A21392411249}" name="200m Superlifesaver - 17/18 - W" dataDxfId="182"/>
+    <tableColumn id="19" xr3:uid="{262DB142-CFB1-45C3-9332-7273CACD1B62}" name="200m Hindernis - 17/18 - W" dataDxfId="181"/>
+    <tableColumn id="20" xr3:uid="{938BA45A-8244-4637-8A14-DF49CD91A945}" name="50m Retten - 17/18 - M" dataDxfId="180"/>
+    <tableColumn id="21" xr3:uid="{737E28D8-900F-4A98-95FE-EE7B0AFDEE90}" name="100m Retten - 17/18 - M" dataDxfId="179"/>
+    <tableColumn id="22" xr3:uid="{330BD3A8-061C-45E2-ADDB-40C2F346772F}" name="100m Kombi - 17/18 - M" dataDxfId="178"/>
+    <tableColumn id="23" xr3:uid="{0CADDE90-A167-4E1D-8D33-8624E5E1A4E2}" name="100m Lifesaver - 17/18 - M" dataDxfId="177"/>
+    <tableColumn id="24" xr3:uid="{FCF9F42C-1291-4985-9D37-B9DE2DAA5DCB}" name="200m Superlifesaver - 17/18 - M" dataDxfId="176"/>
+    <tableColumn id="25" xr3:uid="{4E5397B2-F924-4F48-AE69-AF6D650AF88D}" name="200m Hindernis - 17/18 - M" dataDxfId="175"/>
+    <tableColumn id="26" xr3:uid="{0A78315A-BFDC-43EE-A66F-48B301F66508}" name="50m Retten - 15/16 - W" dataDxfId="174"/>
+    <tableColumn id="27" xr3:uid="{D3FCF8BD-6C76-450D-80C0-CC0519A79731}" name="100m Retten - 15/16 - W" dataDxfId="173"/>
+    <tableColumn id="28" xr3:uid="{6BE7937E-D62D-47CD-95DE-1730304B0DF3}" name="100m Kombi - 15/16 - W" dataDxfId="172"/>
+    <tableColumn id="29" xr3:uid="{098BA5BE-5AF6-4187-89B6-534498F24C51}" name="100m Lifesaver -  15/16 - W" dataDxfId="171"/>
+    <tableColumn id="30" xr3:uid="{2A6822CF-143C-4BF7-A440-5777527BE512}" name="200m Superlifesaver -  15/16 - W" dataDxfId="170"/>
+    <tableColumn id="31" xr3:uid="{541C7145-CDEA-4E4E-9E7A-A4F05BA6C3E5}" name="200m Hindernis -  15/16 - W" dataDxfId="169"/>
+    <tableColumn id="32" xr3:uid="{342C4488-8C61-42E6-87A9-C75BD8EB7452}" name="50m Retten - 15/16 - M" dataDxfId="168"/>
+    <tableColumn id="33" xr3:uid="{857B1D46-7D20-47F7-AB9B-732D50346E32}" name="100m Retten - 15/16 - M" dataDxfId="167"/>
+    <tableColumn id="34" xr3:uid="{4C8A2EB4-804B-45F1-A768-9A6958957F8B}" name="100m Kombi -15/16 - M" dataDxfId="166"/>
+    <tableColumn id="35" xr3:uid="{26C75B4F-21EC-4EB0-A9A9-54BC80140672}" name="100m Lifesaver - 15/16 - M" dataDxfId="165"/>
+    <tableColumn id="36" xr3:uid="{DBBB2A23-1A06-429A-A5D1-A547EF5EC16F}" name="200m Superlifesaver - 15/16 - M" dataDxfId="164"/>
+    <tableColumn id="37" xr3:uid="{84061231-CAE5-427A-87F5-6DDBA99F77D2}" name="200m Hindernis - 15/16 - M" dataDxfId="163"/>
+    <tableColumn id="38" xr3:uid="{878CCA80-A742-4B3C-90C9-E93BB814201B}" name="50m Retten - 13/14 - W" dataDxfId="162"/>
+    <tableColumn id="39" xr3:uid="{A1F57102-61CF-4784-8DE2-0B8F32D5D699}" name="50m Retten mit Flossen - 13/14 - W" dataDxfId="161"/>
+    <tableColumn id="40" xr3:uid="{0F6BAF78-3D79-42A9-9FED-E6D0E335A920}" name="100m Hindernis - 13/14 - W" dataDxfId="160"/>
+    <tableColumn id="41" xr3:uid="{EB748A68-E10D-4D76-B315-8FDB3AC33C8D}" name="50m Retten - 13/14 - M" dataDxfId="159"/>
+    <tableColumn id="42" xr3:uid="{C7B04167-6430-40F0-9A0F-D0D0BE2F9C77}" name="50m Retten mit Flossen - 13/14 - M" dataDxfId="158"/>
+    <tableColumn id="43" xr3:uid="{48704BB7-A853-445A-8CDC-8D8F86C2B66A}" name="100m Hindernis - 13/14 - M" dataDxfId="157"/>
+    <tableColumn id="44" xr3:uid="{9605FE9A-F41C-4A5F-A59C-B7A9D45C460F}" name="50m Flossen - 12 - W" dataDxfId="156"/>
+    <tableColumn id="45" xr3:uid="{4C9DBF61-35B1-4BC2-8272-526E0AFAAFFB}" name="50m komb. Schwimmen - 12 - W" dataDxfId="155"/>
+    <tableColumn id="46" xr3:uid="{CF433C95-C272-48F9-98CD-7E3C8DBB6F2C}" name="50m Hindernis - 12 - W" dataDxfId="154"/>
+    <tableColumn id="47" xr3:uid="{FADB7411-DB43-4B14-B9E8-D74CA1BA18B8}" name="50m Flossen - 12 - M" dataDxfId="153"/>
+    <tableColumn id="48" xr3:uid="{02936F84-1D82-48AC-8D7C-6D2954D68A06}" name="50m komb. Schwimmen - 12 - M" dataDxfId="152"/>
+    <tableColumn id="49" xr3:uid="{7FD9BD11-0597-4E07-8DA5-DB53384197F5}" name="50m Hindernis - 12 - M" dataDxfId="151"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4234D44E-A2BE-4790-B589-1A8CC19B714E}" name="WR_Youth" displayName="WR_Youth" ref="A4:M32" totalsRowShown="0" headerRowDxfId="149" dataDxfId="147" headerRowBorderDxfId="148" tableBorderDxfId="146">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4234D44E-A2BE-4790-B589-1A8CC19B714E}" name="WR_Youth" displayName="WR_Youth" ref="A4:M32" totalsRowShown="0" headerRowDxfId="150" dataDxfId="148" headerRowBorderDxfId="149" tableBorderDxfId="147">
   <autoFilter ref="A4:M32" xr:uid="{4234D44E-A2BE-4790-B589-1A8CC19B714E}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{848E691A-41B0-42DD-B122-FB6DF43CB3EF}" name="WR-Youth" dataDxfId="145"/>
-    <tableColumn id="2" xr3:uid="{2FE43F18-485B-46A9-8946-FBC5FDAE5A8E}" name="50m Retten" dataDxfId="144"/>
-    <tableColumn id="3" xr3:uid="{CA5C3ABF-02E6-442B-868B-95B293B231D3}" name="100m Retten" dataDxfId="143"/>
-    <tableColumn id="4" xr3:uid="{7A6BBA52-2145-464D-8C04-B2CCFC1A90DC}" name="100m Kombi" dataDxfId="142"/>
-    <tableColumn id="5" xr3:uid="{21F420C9-E788-49EE-88F6-E37963ED31CF}" name="100m Lifesaver" dataDxfId="141"/>
-    <tableColumn id="6" xr3:uid="{CB87B7CD-8A9C-4775-A4D7-4D267F43FD1A}" name="200m Superlifesaver" dataDxfId="140"/>
-    <tableColumn id="7" xr3:uid="{2DC7F290-B564-4851-85AE-D211DA701B32}" name="200m Hindernis" dataDxfId="139"/>
-    <tableColumn id="8" xr3:uid="{8112783D-8796-4D6A-8414-AC675D745697}" name="50m Retten2" dataDxfId="138"/>
-    <tableColumn id="9" xr3:uid="{4E818CD4-8725-495D-9D1D-1AFCED9181F5}" name="100m Retten2" dataDxfId="137"/>
-    <tableColumn id="10" xr3:uid="{28C05A91-E302-40A9-B50A-ECF997F129FC}" name="100m Kombi2" dataDxfId="136"/>
-    <tableColumn id="11" xr3:uid="{D56FB9F2-45BF-4EC9-A84C-8A5FB59F2F05}" name="100m Lifesaver2" dataDxfId="135"/>
-    <tableColumn id="12" xr3:uid="{540169C0-2A40-4794-A872-F7DF8A887BF2}" name="200m Superlifesaver2" dataDxfId="134"/>
-    <tableColumn id="13" xr3:uid="{D104CB67-B55A-4C81-87E5-0AC758DD22A4}" name="200m Hindernis2" dataDxfId="133"/>
+    <tableColumn id="1" xr3:uid="{848E691A-41B0-42DD-B122-FB6DF43CB3EF}" name="WR-Youth" dataDxfId="146"/>
+    <tableColumn id="2" xr3:uid="{2FE43F18-485B-46A9-8946-FBC5FDAE5A8E}" name="50m Retten" dataDxfId="145"/>
+    <tableColumn id="3" xr3:uid="{CA5C3ABF-02E6-442B-868B-95B293B231D3}" name="100m Retten" dataDxfId="144"/>
+    <tableColumn id="4" xr3:uid="{7A6BBA52-2145-464D-8C04-B2CCFC1A90DC}" name="100m Kombi" dataDxfId="143"/>
+    <tableColumn id="5" xr3:uid="{21F420C9-E788-49EE-88F6-E37963ED31CF}" name="100m Lifesaver" dataDxfId="142"/>
+    <tableColumn id="6" xr3:uid="{CB87B7CD-8A9C-4775-A4D7-4D267F43FD1A}" name="200m Superlifesaver" dataDxfId="141"/>
+    <tableColumn id="7" xr3:uid="{2DC7F290-B564-4851-85AE-D211DA701B32}" name="200m Hindernis" dataDxfId="140"/>
+    <tableColumn id="8" xr3:uid="{8112783D-8796-4D6A-8414-AC675D745697}" name="50m Retten2" dataDxfId="139"/>
+    <tableColumn id="9" xr3:uid="{4E818CD4-8725-495D-9D1D-1AFCED9181F5}" name="100m Retten2" dataDxfId="138"/>
+    <tableColumn id="10" xr3:uid="{28C05A91-E302-40A9-B50A-ECF997F129FC}" name="100m Kombi2" dataDxfId="137"/>
+    <tableColumn id="11" xr3:uid="{D56FB9F2-45BF-4EC9-A84C-8A5FB59F2F05}" name="100m Lifesaver2" dataDxfId="136"/>
+    <tableColumn id="12" xr3:uid="{540169C0-2A40-4794-A872-F7DF8A887BF2}" name="200m Superlifesaver2" dataDxfId="135"/>
+    <tableColumn id="13" xr3:uid="{D104CB67-B55A-4C81-87E5-0AC758DD22A4}" name="200m Hindernis2" dataDxfId="134"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E2D2F97B-7645-4066-8AB3-F35CF6E035EB}" name="WR_Open" displayName="WR_Open" ref="A4:M32" totalsRowShown="0" headerRowDxfId="132" headerRowBorderDxfId="131" tableBorderDxfId="130">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E2D2F97B-7645-4066-8AB3-F35CF6E035EB}" name="WR_Open" displayName="WR_Open" ref="A4:M32" totalsRowShown="0" headerRowDxfId="133" headerRowBorderDxfId="132" tableBorderDxfId="131">
   <autoFilter ref="A4:M32" xr:uid="{E2D2F97B-7645-4066-8AB3-F35CF6E035EB}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{AE73402B-B27E-4B29-8DCF-30B7FC1855EF}" name="WR-Open" dataDxfId="129">
+    <tableColumn id="1" xr3:uid="{AE73402B-B27E-4B29-8DCF-30B7FC1855EF}" name="WR-Open" dataDxfId="130">
       <calculatedColumnFormula>A4+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{EA3EAC1F-184E-4A28-B3E3-08DE12F138EF}" name="50m Retten" dataDxfId="128"/>
-    <tableColumn id="3" xr3:uid="{E0305A3F-6087-4F8C-8B64-153E1ACAA32E}" name="100m Retten" dataDxfId="127"/>
-    <tableColumn id="4" xr3:uid="{F0B7AC37-315E-49AA-855C-7955D2B43A76}" name="100m Kombi" dataDxfId="126"/>
-    <tableColumn id="5" xr3:uid="{B5E690AB-DB7D-4864-8916-89D2A68C4128}" name="100m Lifesaver" dataDxfId="125"/>
-    <tableColumn id="6" xr3:uid="{D89BAF4D-36AE-4C73-9320-9C5736F02F8A}" name="200m Superlifesaver" dataDxfId="124"/>
-    <tableColumn id="7" xr3:uid="{58AE7517-1A90-459F-A7D2-B95265D217E7}" name="200m Hindernis" dataDxfId="123"/>
-    <tableColumn id="8" xr3:uid="{13A189FB-E897-4A1F-A001-525F61E9CFFF}" name="50m Retten2" dataDxfId="122"/>
-    <tableColumn id="9" xr3:uid="{36418AC5-46B8-400F-BD2E-D329CF4F92CD}" name="100m Retten2" dataDxfId="121"/>
+    <tableColumn id="2" xr3:uid="{EA3EAC1F-184E-4A28-B3E3-08DE12F138EF}" name="50m Retten" dataDxfId="129"/>
+    <tableColumn id="3" xr3:uid="{E0305A3F-6087-4F8C-8B64-153E1ACAA32E}" name="100m Retten" dataDxfId="128"/>
+    <tableColumn id="4" xr3:uid="{F0B7AC37-315E-49AA-855C-7955D2B43A76}" name="100m Kombi" dataDxfId="127"/>
+    <tableColumn id="5" xr3:uid="{B5E690AB-DB7D-4864-8916-89D2A68C4128}" name="100m Lifesaver" dataDxfId="126"/>
+    <tableColumn id="6" xr3:uid="{D89BAF4D-36AE-4C73-9320-9C5736F02F8A}" name="200m Superlifesaver" dataDxfId="125"/>
+    <tableColumn id="7" xr3:uid="{58AE7517-1A90-459F-A7D2-B95265D217E7}" name="200m Hindernis" dataDxfId="124"/>
+    <tableColumn id="8" xr3:uid="{13A189FB-E897-4A1F-A001-525F61E9CFFF}" name="50m Retten2" dataDxfId="123"/>
+    <tableColumn id="9" xr3:uid="{36418AC5-46B8-400F-BD2E-D329CF4F92CD}" name="100m Retten2" dataDxfId="122"/>
     <tableColumn id="10" xr3:uid="{06A35C2D-7313-472B-BC1F-4F2FB1D14782}" name="100m Kombi2"/>
     <tableColumn id="11" xr3:uid="{89966D0D-9131-4245-A7BE-1A7384D5ADA0}" name="100m Lifesaver2"/>
     <tableColumn id="12" xr3:uid="{D9D6CF56-869C-4DDE-9886-572D4E523A8F}" name="200m Superlifesaver2"/>
@@ -4081,7 +4140,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CF3D303A-A04B-42DD-A44E-CEB6CECB77A4}" name="DP_konfig" displayName="DP_konfig" ref="A1:U3" totalsRowShown="0" headerRowDxfId="120" dataDxfId="119">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CF3D303A-A04B-42DD-A44E-CEB6CECB77A4}" name="DP_konfig" displayName="DP_konfig" ref="A1:U3" totalsRowShown="0" headerRowDxfId="121" dataDxfId="120">
   <autoFilter ref="A1:U3" xr:uid="{CF3D303A-A04B-42DD-A44E-CEB6CECB77A4}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4106,64 +4165,64 @@
     <filterColumn colId="20" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="21">
-    <tableColumn id="1" xr3:uid="{58D628F0-061E-4A82-8362-CDB37A2E7C60}" name="Tabellen Name" dataDxfId="118"/>
-    <tableColumn id="2" xr3:uid="{2F302F6C-F8AF-4FDE-AB08-6F30F9671015}" name="Geschlecht" dataDxfId="117"/>
-    <tableColumn id="3" xr3:uid="{4D91FBF9-386D-43DD-90D0-B49823FDB629}" name="Mindest alter" dataDxfId="116"/>
-    <tableColumn id="4" xr3:uid="{4126AAC6-AF2F-446C-B4EA-D86ACFD9FAC2}" name="Maximales Alter" dataDxfId="115"/>
-    <tableColumn id="5" xr3:uid="{8A10890A-A299-4B09-AC72-0E9AE9238AF3}" name="Qualizeitraum anfang" dataDxfId="114"/>
-    <tableColumn id="6" xr3:uid="{FBCD1C13-FC82-429B-8DE1-0C5A455FDAB8}" name="Qualizeitraum Ende" dataDxfId="113"/>
-    <tableColumn id="7" xr3:uid="{1DCCAC9B-BC46-468E-A3CE-57576C2FF11D}" name="Letzter Wettkampf am" dataDxfId="112"/>
-    <tableColumn id="8" xr3:uid="{9A6E47EE-ABD8-4A1E-87D3-9D286E4C124F}" name="Wertung" dataDxfId="111"/>
-    <tableColumn id="9" xr3:uid="{09E848D2-ED17-49C7-9775-CBF17D20DFC0}" name="Landesverband" dataDxfId="110"/>
-    <tableColumn id="10" xr3:uid="{70ABB713-23F6-4FCF-920E-3CB0CD451446}" name="OMS" dataDxfId="109"/>
-    <tableColumn id="11" xr3:uid="{9C108A1C-E6AB-4C13-9C1D-0FA8944A39A3}" name="Pool-Länge" dataDxfId="108"/>
-    <tableColumn id="12" xr3:uid="{087948DD-430D-48F1-906D-4F4EF4B46053}" name="Regelwerk" dataDxfId="107"/>
-    <tableColumn id="13" xr3:uid="{BF42D9C0-F77D-4971-A67E-32B0246C72C3}" name="Referenz" dataDxfId="106"/>
-    <tableColumn id="19" xr3:uid="{AFFB84E8-B398-4E99-805B-9A247071A040}" name="Referenz Jahr" dataDxfId="105"/>
-    <tableColumn id="20" xr3:uid="{0A59A474-DFBB-4437-8EFF-70284AFD9934}" name="Mindest Punktzahl" dataDxfId="104"/>
-    <tableColumn id="21" xr3:uid="{198BD231-EEF3-43C9-AD9B-39B4B7E9B337}" name="Mindest Disziplinen" dataDxfId="103"/>
-    <tableColumn id="14" xr3:uid="{443CD4F6-A2B2-480B-BB35-DCEEBC531727}" name="3-Kampf Regel" dataDxfId="102"/>
-    <tableColumn id="15" xr3:uid="{70116160-7666-42B1-92AC-FAC2620E6A60}" name="Anzahl Nominierte" dataDxfId="101"/>
-    <tableColumn id="16" xr3:uid="{0EFD0A46-D12B-4AB0-907C-08E5D9F282E0}" name="Anzahl Nachrücker" dataDxfId="100"/>
-    <tableColumn id="17" xr3:uid="{AA5430A0-8ED8-40E8-B7F8-DA25E4E8790F}" name="Seiten Anzahl" dataDxfId="99"/>
-    <tableColumn id="18" xr3:uid="{16F699D9-2741-43F3-AD5F-826A568EFEAC}" name="Absagen" dataDxfId="98"/>
+    <tableColumn id="1" xr3:uid="{58D628F0-061E-4A82-8362-CDB37A2E7C60}" name="Tabellen Name" dataDxfId="119"/>
+    <tableColumn id="2" xr3:uid="{2F302F6C-F8AF-4FDE-AB08-6F30F9671015}" name="Geschlecht" dataDxfId="118"/>
+    <tableColumn id="3" xr3:uid="{4D91FBF9-386D-43DD-90D0-B49823FDB629}" name="Mindest alter" dataDxfId="117"/>
+    <tableColumn id="4" xr3:uid="{4126AAC6-AF2F-446C-B4EA-D86ACFD9FAC2}" name="Maximales Alter" dataDxfId="116"/>
+    <tableColumn id="5" xr3:uid="{8A10890A-A299-4B09-AC72-0E9AE9238AF3}" name="Qualizeitraum anfang" dataDxfId="115"/>
+    <tableColumn id="6" xr3:uid="{FBCD1C13-FC82-429B-8DE1-0C5A455FDAB8}" name="Qualizeitraum Ende" dataDxfId="114"/>
+    <tableColumn id="7" xr3:uid="{1DCCAC9B-BC46-468E-A3CE-57576C2FF11D}" name="Letzter Wettkampf am" dataDxfId="113"/>
+    <tableColumn id="8" xr3:uid="{9A6E47EE-ABD8-4A1E-87D3-9D286E4C124F}" name="Wertung" dataDxfId="112"/>
+    <tableColumn id="9" xr3:uid="{09E848D2-ED17-49C7-9775-CBF17D20DFC0}" name="Landesverband" dataDxfId="111"/>
+    <tableColumn id="10" xr3:uid="{70ABB713-23F6-4FCF-920E-3CB0CD451446}" name="OMS" dataDxfId="110"/>
+    <tableColumn id="11" xr3:uid="{9C108A1C-E6AB-4C13-9C1D-0FA8944A39A3}" name="Pool-Länge" dataDxfId="109"/>
+    <tableColumn id="12" xr3:uid="{087948DD-430D-48F1-906D-4F4EF4B46053}" name="Regelwerk" dataDxfId="108"/>
+    <tableColumn id="13" xr3:uid="{BF42D9C0-F77D-4971-A67E-32B0246C72C3}" name="Referenz" dataDxfId="107"/>
+    <tableColumn id="19" xr3:uid="{AFFB84E8-B398-4E99-805B-9A247071A040}" name="Referenz Jahr" dataDxfId="106"/>
+    <tableColumn id="20" xr3:uid="{0A59A474-DFBB-4437-8EFF-70284AFD9934}" name="Mindest Punktzahl" dataDxfId="105"/>
+    <tableColumn id="21" xr3:uid="{198BD231-EEF3-43C9-AD9B-39B4B7E9B337}" name="Mindest Disziplinen" dataDxfId="104"/>
+    <tableColumn id="14" xr3:uid="{443CD4F6-A2B2-480B-BB35-DCEEBC531727}" name="3-Kampf Regel" dataDxfId="103"/>
+    <tableColumn id="15" xr3:uid="{70116160-7666-42B1-92AC-FAC2620E6A60}" name="Anzahl Nominierte" dataDxfId="102"/>
+    <tableColumn id="16" xr3:uid="{0EFD0A46-D12B-4AB0-907C-08E5D9F282E0}" name="Anzahl Nachrücker" dataDxfId="101"/>
+    <tableColumn id="17" xr3:uid="{AA5430A0-8ED8-40E8-B7F8-DA25E4E8790F}" name="Seiten Anzahl" dataDxfId="100"/>
+    <tableColumn id="18" xr3:uid="{16F699D9-2741-43F3-AD5F-826A568EFEAC}" name="Absagen" dataDxfId="99"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CDBF6724-48A1-41AB-94B5-CC35C54BB15C}" name="BP_konfig" displayName="BP_konfig" ref="A1:U7" totalsRowShown="0" headerRowDxfId="97" dataDxfId="96">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CDBF6724-48A1-41AB-94B5-CC35C54BB15C}" name="BP_konfig" displayName="BP_konfig" ref="A1:U7" totalsRowShown="0" headerRowDxfId="98" dataDxfId="97">
   <autoFilter ref="A1:U7" xr:uid="{CDBF6724-48A1-41AB-94B5-CC35C54BB15C}"/>
   <tableColumns count="21">
-    <tableColumn id="1" xr3:uid="{E1FB3D0C-B874-4874-BACC-6872CF171957}" name="Tabellen Name" dataDxfId="95"/>
-    <tableColumn id="2" xr3:uid="{FFDD2777-2097-450C-B020-F133CF643855}" name="Geschlecht" dataDxfId="94"/>
-    <tableColumn id="3" xr3:uid="{8CF52BE2-8020-48BD-A36D-63F13A1878DE}" name="Mindest alter" dataDxfId="93"/>
-    <tableColumn id="4" xr3:uid="{FD3A030F-CD97-4B6F-8E8C-BC2E67D79F1D}" name="Maximales Alter" dataDxfId="92"/>
-    <tableColumn id="5" xr3:uid="{3E22B645-D77C-4509-B031-9914FCB91599}" name="Qualizeitraum anfang" dataDxfId="91"/>
-    <tableColumn id="6" xr3:uid="{AE299324-3C1C-4063-ADF9-54555A161734}" name="Qualizeitraum Ende" dataDxfId="90"/>
-    <tableColumn id="7" xr3:uid="{DCC178B3-11FC-4C53-BBC6-C2FDA2C89857}" name="Letzter Wettkampf am" dataDxfId="89"/>
-    <tableColumn id="8" xr3:uid="{2811DB01-60A5-4BE4-B6F9-A806398A602A}" name="Wertung" dataDxfId="88"/>
-    <tableColumn id="9" xr3:uid="{0C16DAFE-847D-4E9E-9604-3A7D9FE924D0}" name="Landesverband" dataDxfId="87"/>
-    <tableColumn id="10" xr3:uid="{7A8A4101-A553-4BD5-9116-9AA5876B9401}" name="OMS" dataDxfId="86"/>
-    <tableColumn id="11" xr3:uid="{9807C9BD-6499-45F6-ACE0-4D13D64EF675}" name="Pool-Länge" dataDxfId="85"/>
-    <tableColumn id="12" xr3:uid="{13D336DD-650F-4F2C-836F-361CA1528F6D}" name="Regelwerk" dataDxfId="84"/>
-    <tableColumn id="13" xr3:uid="{66660E2D-ADF2-4FB5-8A13-004F826EE908}" name="Referenz" dataDxfId="83"/>
-    <tableColumn id="19" xr3:uid="{D72EDF8B-ECC3-4FF7-ABE6-B60BCE4A5E26}" name="Referenz Jahr" dataDxfId="82"/>
-    <tableColumn id="20" xr3:uid="{7B18E667-70F7-4BC1-AB1B-21C019F2AA89}" name="Mindest Punktzahl" dataDxfId="81"/>
-    <tableColumn id="21" xr3:uid="{FC185946-681B-42A6-AB1A-FC1EABB668C5}" name="Mindest Disziplinen" dataDxfId="80"/>
-    <tableColumn id="14" xr3:uid="{6A2676FD-2EC7-4C41-A35E-A1597A38F932}" name="3-Kampf Regel" dataDxfId="79"/>
-    <tableColumn id="15" xr3:uid="{718E0917-4F83-4A2B-832F-EBB16D5E21BF}" name="Anzahl Nominierte" dataDxfId="78"/>
-    <tableColumn id="16" xr3:uid="{5C66A461-D647-4E00-A81C-FD7AD44D7CC2}" name="Anzahl Nachrücker" dataDxfId="77"/>
-    <tableColumn id="17" xr3:uid="{D434BDEC-293B-4B4E-A5E9-479438960A03}" name="Seiten Anzahl" dataDxfId="76"/>
-    <tableColumn id="18" xr3:uid="{80908229-9247-473F-81C0-9C9D4C12FF06}" name="Absagen" dataDxfId="75"/>
+    <tableColumn id="1" xr3:uid="{E1FB3D0C-B874-4874-BACC-6872CF171957}" name="Tabellen Name" dataDxfId="96"/>
+    <tableColumn id="2" xr3:uid="{FFDD2777-2097-450C-B020-F133CF643855}" name="Geschlecht" dataDxfId="95"/>
+    <tableColumn id="3" xr3:uid="{8CF52BE2-8020-48BD-A36D-63F13A1878DE}" name="Mindest alter" dataDxfId="94"/>
+    <tableColumn id="4" xr3:uid="{FD3A030F-CD97-4B6F-8E8C-BC2E67D79F1D}" name="Maximales Alter" dataDxfId="93"/>
+    <tableColumn id="5" xr3:uid="{3E22B645-D77C-4509-B031-9914FCB91599}" name="Qualizeitraum anfang" dataDxfId="92"/>
+    <tableColumn id="6" xr3:uid="{AE299324-3C1C-4063-ADF9-54555A161734}" name="Qualizeitraum Ende" dataDxfId="91"/>
+    <tableColumn id="7" xr3:uid="{DCC178B3-11FC-4C53-BBC6-C2FDA2C89857}" name="Letzter Wettkampf am" dataDxfId="90"/>
+    <tableColumn id="8" xr3:uid="{2811DB01-60A5-4BE4-B6F9-A806398A602A}" name="Wertung" dataDxfId="89"/>
+    <tableColumn id="9" xr3:uid="{0C16DAFE-847D-4E9E-9604-3A7D9FE924D0}" name="Landesverband" dataDxfId="88"/>
+    <tableColumn id="10" xr3:uid="{7A8A4101-A553-4BD5-9116-9AA5876B9401}" name="OMS" dataDxfId="87"/>
+    <tableColumn id="11" xr3:uid="{9807C9BD-6499-45F6-ACE0-4D13D64EF675}" name="Pool-Länge" dataDxfId="86"/>
+    <tableColumn id="12" xr3:uid="{13D336DD-650F-4F2C-836F-361CA1528F6D}" name="Regelwerk" dataDxfId="85"/>
+    <tableColumn id="13" xr3:uid="{66660E2D-ADF2-4FB5-8A13-004F826EE908}" name="Referenz" dataDxfId="84"/>
+    <tableColumn id="19" xr3:uid="{D72EDF8B-ECC3-4FF7-ABE6-B60BCE4A5E26}" name="Referenz Jahr" dataDxfId="83"/>
+    <tableColumn id="20" xr3:uid="{7B18E667-70F7-4BC1-AB1B-21C019F2AA89}" name="Mindest Punktzahl" dataDxfId="82"/>
+    <tableColumn id="21" xr3:uid="{FC185946-681B-42A6-AB1A-FC1EABB668C5}" name="Mindest Disziplinen" dataDxfId="81"/>
+    <tableColumn id="14" xr3:uid="{6A2676FD-2EC7-4C41-A35E-A1597A38F932}" name="3-Kampf Regel" dataDxfId="80"/>
+    <tableColumn id="15" xr3:uid="{718E0917-4F83-4A2B-832F-EBB16D5E21BF}" name="Anzahl Nominierte" dataDxfId="79"/>
+    <tableColumn id="16" xr3:uid="{5C66A461-D647-4E00-A81C-FD7AD44D7CC2}" name="Anzahl Nachrücker" dataDxfId="78"/>
+    <tableColumn id="17" xr3:uid="{D434BDEC-293B-4B4E-A5E9-479438960A03}" name="Seiten Anzahl" dataDxfId="77"/>
+    <tableColumn id="18" xr3:uid="{80908229-9247-473F-81C0-9C9D4C12FF06}" name="Absagen" dataDxfId="76"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{16F87202-5A6A-4E2F-B973-3CE7EC2566C1}" name="DEM_konfig" displayName="DEM_konfig" ref="A1:X7" totalsRowShown="0" headerRowDxfId="74" dataDxfId="73">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{16F87202-5A6A-4E2F-B973-3CE7EC2566C1}" name="DEM_konfig" displayName="DEM_konfig" ref="A1:X7" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74">
   <autoFilter ref="A1:X7" xr:uid="{16F87202-5A6A-4E2F-B973-3CE7EC2566C1}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4191,37 +4250,37 @@
     <filterColumn colId="23" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{4847B567-64E1-4AC3-8C4B-EFCF3F00CC6C}" name="Tabellen Name" dataDxfId="72"/>
-    <tableColumn id="2" xr3:uid="{6346FF3B-B334-4CD8-8B23-F2347E29C536}" name="Geschlecht" dataDxfId="71"/>
-    <tableColumn id="3" xr3:uid="{E793B48A-BC8A-439F-8AAF-6FD08104A619}" name="Mindest Alter" dataDxfId="70"/>
-    <tableColumn id="4" xr3:uid="{01A62C29-2F75-4107-A431-F69230BCCD0C}" name="Maximales Alter" dataDxfId="69"/>
-    <tableColumn id="5" xr3:uid="{B7E4DE90-7856-4A0C-9063-61414D7F227C}" name="Qualizeitraum anfang" dataDxfId="68"/>
-    <tableColumn id="6" xr3:uid="{B00F7CD1-82CB-42B9-A396-89F79EF419CA}" name="Qualizeitraum Ende" dataDxfId="67"/>
-    <tableColumn id="7" xr3:uid="{9E50DDE5-12E3-4BCB-801C-FBABCE309F0E}" name="Letzter Wettkampf am" dataDxfId="66"/>
-    <tableColumn id="8" xr3:uid="{57E68247-0FF2-48D8-8ACD-AB057E576A21}" name="Landesverband" dataDxfId="65"/>
-    <tableColumn id="9" xr3:uid="{EBAA439D-F69A-4C2A-8193-9AE08F1E57B8}" name="OMS" dataDxfId="64"/>
-    <tableColumn id="10" xr3:uid="{BBD11E7F-3DDF-428A-B005-4A40E6FA78DC}" name="Pool-Länge" dataDxfId="63"/>
-    <tableColumn id="11" xr3:uid="{6AE38DCA-A084-4F3D-A6A4-4E76E3E2CBC6}" name="Regelwerk" dataDxfId="62"/>
-    <tableColumn id="12" xr3:uid="{7F7470AD-5502-4CEE-BB4C-44BA308E61D7}" name="Seiten Anzahl" dataDxfId="61"/>
-    <tableColumn id="13" xr3:uid="{F416CBFA-4C9D-45CD-9BA7-E4BC57A08BC2}" name="PZ1 - 50m Retten" dataDxfId="60"/>
-    <tableColumn id="14" xr3:uid="{7117DBCA-0DA7-462C-84FE-0DC7E33B124C}" name="PZ1 - 100m Retten" dataDxfId="59"/>
-    <tableColumn id="15" xr3:uid="{E8630E91-DC30-4822-9E53-6D65487C3670}" name="PZ1 - 100m Kombi" dataDxfId="58"/>
-    <tableColumn id="16" xr3:uid="{4B3AA225-E042-430F-8259-D176887B4528}" name="PZ1 - 100m Lifesaver" dataDxfId="57"/>
-    <tableColumn id="17" xr3:uid="{798674BD-98CE-4531-BDFF-6AB06253AD7C}" name="PZ1 - 200m Super-Lifesaver" dataDxfId="56"/>
-    <tableColumn id="18" xr3:uid="{8809BB71-D58B-4E8B-A442-D0EB9A65A25D}" name="PZ1 - 200m Hindernis" dataDxfId="55"/>
-    <tableColumn id="19" xr3:uid="{93DCF463-806B-4117-B4E3-1FFAE976B37C}" name="PZ2 - 50m Retten" dataDxfId="54"/>
-    <tableColumn id="20" xr3:uid="{A514C961-559E-462F-B143-BA30974C0129}" name="PZ2 - 100m Retten" dataDxfId="53"/>
-    <tableColumn id="21" xr3:uid="{F1CF6143-45FE-498D-93D6-36F26D2F3C0B}" name="PZ2 - 100m Kombi" dataDxfId="52"/>
-    <tableColumn id="22" xr3:uid="{E90962FC-C214-467F-841F-40DF60E41456}" name="PZ2 - 100m Lifesaver" dataDxfId="51"/>
-    <tableColumn id="23" xr3:uid="{7FBC6334-C4C8-4B38-9F59-30ED95A44379}" name="PZ2 - 200m Super-Lifesaver" dataDxfId="50"/>
-    <tableColumn id="24" xr3:uid="{231BFF86-8F3A-4BA1-B25E-28175D9EDFA9}" name="PZ2 - 200m Hindernis" dataDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{4847B567-64E1-4AC3-8C4B-EFCF3F00CC6C}" name="Tabellen Name" dataDxfId="73"/>
+    <tableColumn id="2" xr3:uid="{6346FF3B-B334-4CD8-8B23-F2347E29C536}" name="Geschlecht" dataDxfId="72"/>
+    <tableColumn id="3" xr3:uid="{E793B48A-BC8A-439F-8AAF-6FD08104A619}" name="Mindest Alter" dataDxfId="71"/>
+    <tableColumn id="4" xr3:uid="{01A62C29-2F75-4107-A431-F69230BCCD0C}" name="Maximales Alter" dataDxfId="70"/>
+    <tableColumn id="5" xr3:uid="{B7E4DE90-7856-4A0C-9063-61414D7F227C}" name="Qualizeitraum anfang" dataDxfId="69"/>
+    <tableColumn id="6" xr3:uid="{B00F7CD1-82CB-42B9-A396-89F79EF419CA}" name="Qualizeitraum Ende" dataDxfId="68"/>
+    <tableColumn id="7" xr3:uid="{9E50DDE5-12E3-4BCB-801C-FBABCE309F0E}" name="Letzter Wettkampf am" dataDxfId="67"/>
+    <tableColumn id="8" xr3:uid="{57E68247-0FF2-48D8-8ACD-AB057E576A21}" name="Landesverband" dataDxfId="66"/>
+    <tableColumn id="9" xr3:uid="{EBAA439D-F69A-4C2A-8193-9AE08F1E57B8}" name="OMS" dataDxfId="65"/>
+    <tableColumn id="10" xr3:uid="{BBD11E7F-3DDF-428A-B005-4A40E6FA78DC}" name="Pool-Länge" dataDxfId="64"/>
+    <tableColumn id="11" xr3:uid="{6AE38DCA-A084-4F3D-A6A4-4E76E3E2CBC6}" name="Regelwerk" dataDxfId="63"/>
+    <tableColumn id="12" xr3:uid="{7F7470AD-5502-4CEE-BB4C-44BA308E61D7}" name="Seiten Anzahl" dataDxfId="62"/>
+    <tableColumn id="13" xr3:uid="{F416CBFA-4C9D-45CD-9BA7-E4BC57A08BC2}" name="PZ1 - 50m Retten" dataDxfId="61"/>
+    <tableColumn id="14" xr3:uid="{7117DBCA-0DA7-462C-84FE-0DC7E33B124C}" name="PZ1 - 100m Retten" dataDxfId="60"/>
+    <tableColumn id="15" xr3:uid="{E8630E91-DC30-4822-9E53-6D65487C3670}" name="PZ1 - 100m Kombi" dataDxfId="59"/>
+    <tableColumn id="16" xr3:uid="{4B3AA225-E042-430F-8259-D176887B4528}" name="PZ1 - 100m Lifesaver" dataDxfId="58"/>
+    <tableColumn id="17" xr3:uid="{798674BD-98CE-4531-BDFF-6AB06253AD7C}" name="PZ1 - 200m Super-Lifesaver" dataDxfId="57"/>
+    <tableColumn id="18" xr3:uid="{8809BB71-D58B-4E8B-A442-D0EB9A65A25D}" name="PZ1 - 200m Hindernis" dataDxfId="56"/>
+    <tableColumn id="19" xr3:uid="{93DCF463-806B-4117-B4E3-1FFAE976B37C}" name="PZ2 - 50m Retten" dataDxfId="55"/>
+    <tableColumn id="20" xr3:uid="{A514C961-559E-462F-B143-BA30974C0129}" name="PZ2 - 100m Retten" dataDxfId="54"/>
+    <tableColumn id="21" xr3:uid="{F1CF6143-45FE-498D-93D6-36F26D2F3C0B}" name="PZ2 - 100m Kombi" dataDxfId="53"/>
+    <tableColumn id="22" xr3:uid="{E90962FC-C214-467F-841F-40DF60E41456}" name="PZ2 - 100m Lifesaver" dataDxfId="52"/>
+    <tableColumn id="23" xr3:uid="{7FBC6334-C4C8-4B38-9F59-30ED95A44379}" name="PZ2 - 200m Super-Lifesaver" dataDxfId="51"/>
+    <tableColumn id="24" xr3:uid="{231BFF86-8F3A-4BA1-B25E-28175D9EDFA9}" name="PZ2 - 200m Hindernis" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}" name="JRP_konfig" displayName="JRP_konfig" ref="A1:X99" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}" name="JRP_konfig" displayName="JRP_konfig" ref="A1:X99" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
   <autoFilter ref="A1:X99" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4249,45 +4308,45 @@
     <filterColumn colId="23" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{021DA6E1-2C93-4474-9720-B6F016186D61}" name="Tabellen Name" dataDxfId="46"/>
-    <tableColumn id="2" xr3:uid="{733C1722-A9C9-4830-A9E2-FE62E96BCD98}" name="Geschlecht" dataDxfId="45"/>
-    <tableColumn id="3" xr3:uid="{80C0BF46-0E43-4947-BF86-B808C324772A}" name="Mindest Alter" dataDxfId="44"/>
-    <tableColumn id="4" xr3:uid="{DBA2A923-EEB7-43F9-A1A3-E78624448FB9}" name="Maximales Alter" dataDxfId="43"/>
-    <tableColumn id="5" xr3:uid="{3FDEE18A-328D-45AE-907D-69A916A93345}" name="Qualizeitraum anfang" dataDxfId="42"/>
-    <tableColumn id="6" xr3:uid="{BE002D7F-575F-4B60-9251-C71D93F59045}" name="Qualizeitraum Ende" dataDxfId="41"/>
-    <tableColumn id="7" xr3:uid="{208ABD57-DE4B-41D6-B9FC-93F2D8966E8D}" name="Letzter Wettkampf am" dataDxfId="40"/>
-    <tableColumn id="8" xr3:uid="{30C9697C-6550-4996-ADDB-7FEE5325B794}" name="Landesverband" dataDxfId="39"/>
-    <tableColumn id="9" xr3:uid="{ED2DAB77-EF46-4D8B-B8E4-90412E32E277}" name="OMS" dataDxfId="38"/>
-    <tableColumn id="10" xr3:uid="{AD534940-A91B-4A6E-9606-E3F3E517D401}" name="Pool-Länge" dataDxfId="37"/>
-    <tableColumn id="11" xr3:uid="{11F9D5D5-72FE-42CA-8624-01D513B4140F}" name="Regelwerk" dataDxfId="36"/>
-    <tableColumn id="12" xr3:uid="{3907872B-5438-4FBF-A045-3EF9EAACFC47}" name="Seiten Anzahl" dataDxfId="35"/>
-    <tableColumn id="13" xr3:uid="{FC821324-3638-40C0-BA1E-069B44E23C7A}" name="PZ1 - 50m Retten" dataDxfId="34"/>
-    <tableColumn id="14" xr3:uid="{70529619-443E-40D3-88C1-3E0F00BB2A50}" name="PZ1 - 100m Retten" dataDxfId="33"/>
-    <tableColumn id="15" xr3:uid="{EFA92FD2-C23F-42B3-83DC-5036513F19AF}" name="PZ1 - 100m Kombi" dataDxfId="32"/>
-    <tableColumn id="16" xr3:uid="{03309E52-8CF3-4E90-9EE6-A818901C3B32}" name="PZ1 - 100m Lifesaver" dataDxfId="31"/>
-    <tableColumn id="17" xr3:uid="{00B22013-AA11-4C17-9250-22060AE4B0A8}" name="PZ1 - 200m Super-Lifesaver" dataDxfId="30"/>
-    <tableColumn id="18" xr3:uid="{7E3508A9-0422-4561-A23E-53E613259B24}" name="PZ1 - 200m Hindernis" dataDxfId="29"/>
-    <tableColumn id="19" xr3:uid="{5CEA435F-F34B-4D8D-88D0-F5EBFF18B713}" name="PZ2 - 50m Retten" dataDxfId="28"/>
-    <tableColumn id="20" xr3:uid="{8585BE62-F7C4-4D5D-B287-052B43B08610}" name="PZ2 - 100m Retten" dataDxfId="27"/>
-    <tableColumn id="21" xr3:uid="{D981758B-ADAD-4E36-B787-0B0FDA808CA2}" name="PZ2 - 100m Kombi" dataDxfId="26"/>
-    <tableColumn id="22" xr3:uid="{1D4970A8-D22F-4962-934C-AEA295ED687A}" name="PZ2 - 100m Lifesaver" dataDxfId="25"/>
-    <tableColumn id="23" xr3:uid="{BE394430-C58F-4690-9615-44475E5AF9F8}" name="PZ2 - 200m Super-Lifesaver" dataDxfId="24"/>
-    <tableColumn id="24" xr3:uid="{A7036B1A-99CE-4F7C-AAB8-12E8B2696202}" name="PZ2 - 200m Hindernis" dataDxfId="23"/>
+    <tableColumn id="1" xr3:uid="{021DA6E1-2C93-4474-9720-B6F016186D61}" name="Tabellen Name" dataDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{733C1722-A9C9-4830-A9E2-FE62E96BCD98}" name="Geschlecht" dataDxfId="46"/>
+    <tableColumn id="3" xr3:uid="{80C0BF46-0E43-4947-BF86-B808C324772A}" name="Mindest Alter" dataDxfId="45"/>
+    <tableColumn id="4" xr3:uid="{DBA2A923-EEB7-43F9-A1A3-E78624448FB9}" name="Maximales Alter" dataDxfId="44"/>
+    <tableColumn id="5" xr3:uid="{3FDEE18A-328D-45AE-907D-69A916A93345}" name="Qualizeitraum anfang" dataDxfId="43"/>
+    <tableColumn id="6" xr3:uid="{BE002D7F-575F-4B60-9251-C71D93F59045}" name="Qualizeitraum Ende" dataDxfId="42"/>
+    <tableColumn id="7" xr3:uid="{208ABD57-DE4B-41D6-B9FC-93F2D8966E8D}" name="Letzter Wettkampf am" dataDxfId="41"/>
+    <tableColumn id="8" xr3:uid="{30C9697C-6550-4996-ADDB-7FEE5325B794}" name="Landesverband" dataDxfId="40"/>
+    <tableColumn id="9" xr3:uid="{ED2DAB77-EF46-4D8B-B8E4-90412E32E277}" name="OMS" dataDxfId="39"/>
+    <tableColumn id="10" xr3:uid="{AD534940-A91B-4A6E-9606-E3F3E517D401}" name="Pool-Länge" dataDxfId="38"/>
+    <tableColumn id="11" xr3:uid="{11F9D5D5-72FE-42CA-8624-01D513B4140F}" name="Regelwerk" dataDxfId="37"/>
+    <tableColumn id="12" xr3:uid="{3907872B-5438-4FBF-A045-3EF9EAACFC47}" name="Seiten Anzahl" dataDxfId="36"/>
+    <tableColumn id="13" xr3:uid="{FC821324-3638-40C0-BA1E-069B44E23C7A}" name="PZ1 - 50m Retten" dataDxfId="35"/>
+    <tableColumn id="14" xr3:uid="{70529619-443E-40D3-88C1-3E0F00BB2A50}" name="PZ1 - 100m Retten" dataDxfId="34"/>
+    <tableColumn id="15" xr3:uid="{EFA92FD2-C23F-42B3-83DC-5036513F19AF}" name="PZ1 - 100m Kombi" dataDxfId="33"/>
+    <tableColumn id="16" xr3:uid="{03309E52-8CF3-4E90-9EE6-A818901C3B32}" name="PZ1 - 100m Lifesaver" dataDxfId="32"/>
+    <tableColumn id="17" xr3:uid="{00B22013-AA11-4C17-9250-22060AE4B0A8}" name="PZ1 - 200m Super-Lifesaver" dataDxfId="31"/>
+    <tableColumn id="18" xr3:uid="{7E3508A9-0422-4561-A23E-53E613259B24}" name="PZ1 - 200m Hindernis" dataDxfId="30"/>
+    <tableColumn id="19" xr3:uid="{5CEA435F-F34B-4D8D-88D0-F5EBFF18B713}" name="PZ2 - 50m Retten" dataDxfId="29"/>
+    <tableColumn id="20" xr3:uid="{8585BE62-F7C4-4D5D-B287-052B43B08610}" name="PZ2 - 100m Retten" dataDxfId="28"/>
+    <tableColumn id="21" xr3:uid="{D981758B-ADAD-4E36-B787-0B0FDA808CA2}" name="PZ2 - 100m Kombi" dataDxfId="27"/>
+    <tableColumn id="22" xr3:uid="{1D4970A8-D22F-4962-934C-AEA295ED687A}" name="PZ2 - 100m Lifesaver" dataDxfId="26"/>
+    <tableColumn id="23" xr3:uid="{BE394430-C58F-4690-9615-44475E5AF9F8}" name="PZ2 - 200m Super-Lifesaver" dataDxfId="25"/>
+    <tableColumn id="24" xr3:uid="{A7036B1A-99CE-4F7C-AAB8-12E8B2696202}" name="PZ2 - 200m Hindernis" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{888CE7BE-8313-44C0-AE38-83992EABD44D}" name="Tabelle7" displayName="Tabelle7" ref="A1:H3" totalsRowShown="0">
-  <autoFilter ref="A1:H3" xr:uid="{888CE7BE-8313-44C0-AE38-83992EABD44D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{888CE7BE-8313-44C0-AE38-83992EABD44D}" name="LK_Kalender" displayName="LK_Kalender" ref="A1:H10" totalsRowShown="0">
+  <autoFilter ref="A1:H10" xr:uid="{888CE7BE-8313-44C0-AE38-83992EABD44D}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{B26B9E90-F378-41EF-B35E-CE240017E4BE}" name="datum von" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{B26B9E90-F378-41EF-B35E-CE240017E4BE}" name="datum von" dataDxfId="23"/>
     <tableColumn id="2" xr3:uid="{38211212-0A92-428C-895C-E4CA68F52818}" name="datum bis"/>
-    <tableColumn id="3" xr3:uid="{66E541C6-0A5E-4B2D-9B89-5E52F449A4A6}" name="uhrzeit von" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{D93C06A2-29AD-4073-8E3C-A685B4474CC8}" name="uhrzeit bis" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{C5C3979C-B528-44E8-A5A6-36F020A6034F}" name="titel" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{9DC09E1D-44FD-40ED-9EBE-86A8E61C38B2}" name="info" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{66E541C6-0A5E-4B2D-9B89-5E52F449A4A6}" name="uhrzeit von" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{D93C06A2-29AD-4073-8E3C-A685B4474CC8}" name="uhrzeit bis" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{C5C3979C-B528-44E8-A5A6-36F020A6034F}" name="titel" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{9DC09E1D-44FD-40ED-9EBE-86A8E61C38B2}" name="meta" dataDxfId="19"/>
     <tableColumn id="7" xr3:uid="{E7E62A34-7A76-4361-937D-F4DE76E6E7CC}" name="ort"/>
     <tableColumn id="8" xr3:uid="{84F02734-FC16-406B-ACCA-0CCDF547D94C}" name="kader"/>
   </tableColumns>
@@ -8234,52 +8293,52 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B5:G31">
-    <cfRule type="expression" dxfId="22" priority="15">
+    <cfRule type="expression" dxfId="18" priority="15">
       <formula>B5&lt;&gt;B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:M31">
-    <cfRule type="expression" dxfId="21" priority="14">
+    <cfRule type="expression" dxfId="17" priority="14">
       <formula>H5&lt;&gt;H4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N5:S31">
-    <cfRule type="expression" dxfId="20" priority="13">
+    <cfRule type="expression" dxfId="16" priority="13">
       <formula>N5&lt;&gt;N4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T5:Y31">
-    <cfRule type="expression" dxfId="19" priority="12">
+    <cfRule type="expression" dxfId="15" priority="12">
       <formula>T5&lt;&gt;T4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z5:AE31">
-    <cfRule type="expression" dxfId="18" priority="9">
+    <cfRule type="expression" dxfId="14" priority="9">
       <formula>Z5&lt;&gt;Z4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF5:AK31">
-    <cfRule type="expression" dxfId="17" priority="8">
+    <cfRule type="expression" dxfId="13" priority="8">
       <formula>AF5&lt;&gt;AF4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL5:AN31">
-    <cfRule type="expression" dxfId="16" priority="6">
+    <cfRule type="expression" dxfId="12" priority="6">
       <formula>AL5&lt;&gt;AL4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO5:AQ31">
-    <cfRule type="expression" dxfId="15" priority="5">
+    <cfRule type="expression" dxfId="11" priority="5">
       <formula>AO5&lt;&gt;AO4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR5:AT31">
-    <cfRule type="expression" dxfId="14" priority="2">
+    <cfRule type="expression" dxfId="10" priority="2">
       <formula>AR5&lt;&gt;AR4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU5:AW31">
-    <cfRule type="expression" dxfId="13" priority="1">
+    <cfRule type="expression" dxfId="9" priority="1">
       <formula>AU5&lt;&gt;AU4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8524,38 +8583,38 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="71"/>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="71"/>
-      <c r="J7" s="71"/>
-      <c r="K7" s="71"/>
-      <c r="L7" s="71"/>
-      <c r="M7" s="71"/>
-      <c r="N7" s="71"/>
+      <c r="B7" s="74"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="74"/>
+      <c r="L7" s="74"/>
+      <c r="M7" s="74"/>
+      <c r="N7" s="74"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A8" s="71"/>
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="71"/>
-      <c r="H8" s="71"/>
-      <c r="I8" s="71"/>
-      <c r="J8" s="71"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="71"/>
-      <c r="M8" s="71"/>
-      <c r="N8" s="71"/>
+      <c r="A8" s="74"/>
+      <c r="B8" s="74"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="74"/>
+      <c r="G8" s="74"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="74"/>
+      <c r="K8" s="74"/>
+      <c r="L8" s="74"/>
+      <c r="M8" s="74"/>
+      <c r="N8" s="74"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" s="20" t="s">
@@ -8720,38 +8779,38 @@
       <c r="N11" s="23"/>
     </row>
     <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="70" t="s">
+      <c r="A14" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="70"/>
-      <c r="C14" s="70"/>
-      <c r="D14" s="70"/>
-      <c r="E14" s="70"/>
-      <c r="F14" s="70"/>
+      <c r="B14" s="73"/>
+      <c r="C14" s="73"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="73"/>
       <c r="G14"/>
-      <c r="H14" s="72" t="s">
+      <c r="H14" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="I14" s="72"/>
-      <c r="J14" s="72"/>
-      <c r="L14" s="72" t="s">
+      <c r="I14" s="75"/>
+      <c r="J14" s="75"/>
+      <c r="L14" s="75" t="s">
         <v>36</v>
       </c>
       <c r="M14"/>
       <c r="N14"/>
     </row>
     <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="70"/>
-      <c r="B15" s="70"/>
-      <c r="C15" s="70"/>
-      <c r="D15" s="70"/>
-      <c r="E15" s="70"/>
-      <c r="F15" s="70"/>
+      <c r="A15" s="73"/>
+      <c r="B15" s="73"/>
+      <c r="C15" s="73"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="73"/>
       <c r="G15"/>
-      <c r="H15" s="72"/>
-      <c r="I15" s="72"/>
-      <c r="J15" s="72"/>
-      <c r="L15" s="72"/>
+      <c r="H15" s="75"/>
+      <c r="I15" s="75"/>
+      <c r="J15" s="75"/>
+      <c r="L15" s="75"/>
       <c r="M15"/>
       <c r="N15"/>
     </row>
@@ -9285,38 +9344,38 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="71"/>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="71"/>
-      <c r="J7" s="71"/>
-      <c r="K7" s="71"/>
-      <c r="L7" s="71"/>
-      <c r="M7" s="71"/>
-      <c r="N7" s="71"/>
+      <c r="B7" s="74"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="74"/>
+      <c r="L7" s="74"/>
+      <c r="M7" s="74"/>
+      <c r="N7" s="74"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A8" s="71"/>
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="71"/>
-      <c r="H8" s="71"/>
-      <c r="I8" s="71"/>
-      <c r="J8" s="71"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="71"/>
-      <c r="M8" s="71"/>
-      <c r="N8" s="71"/>
+      <c r="A8" s="74"/>
+      <c r="B8" s="74"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="74"/>
+      <c r="G8" s="74"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="74"/>
+      <c r="K8" s="74"/>
+      <c r="L8" s="74"/>
+      <c r="M8" s="74"/>
+      <c r="N8" s="74"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" s="20" t="s">
@@ -9481,35 +9540,35 @@
       <c r="N11" s="23"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A14" s="70" t="s">
+      <c r="A14" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="70"/>
-      <c r="C14" s="70"/>
-      <c r="D14" s="70"/>
-      <c r="E14" s="70"/>
-      <c r="F14" s="70"/>
-      <c r="H14" s="72" t="s">
+      <c r="B14" s="73"/>
+      <c r="C14" s="73"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="73"/>
+      <c r="H14" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="I14" s="72"/>
-      <c r="J14" s="72"/>
-      <c r="L14" s="72" t="s">
+      <c r="I14" s="75"/>
+      <c r="J14" s="75"/>
+      <c r="L14" s="75" t="s">
         <v>36</v>
       </c>
       <c r="M14"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A15" s="70"/>
-      <c r="B15" s="70"/>
-      <c r="C15" s="70"/>
-      <c r="D15" s="70"/>
-      <c r="E15" s="70"/>
-      <c r="F15" s="70"/>
-      <c r="H15" s="72"/>
-      <c r="I15" s="72"/>
-      <c r="J15" s="72"/>
-      <c r="L15" s="72"/>
+      <c r="A15" s="73"/>
+      <c r="B15" s="73"/>
+      <c r="C15" s="73"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="73"/>
+      <c r="H15" s="75"/>
+      <c r="I15" s="75"/>
+      <c r="J15" s="75"/>
+      <c r="L15" s="75"/>
       <c r="M15"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.45">
@@ -10081,38 +10140,38 @@
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="71"/>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="71"/>
-      <c r="J7" s="71"/>
-      <c r="K7" s="71"/>
-      <c r="L7" s="71"/>
-      <c r="M7" s="71"/>
-      <c r="N7" s="71"/>
+      <c r="B7" s="74"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="74"/>
+      <c r="E7" s="74"/>
+      <c r="F7" s="74"/>
+      <c r="G7" s="74"/>
+      <c r="H7" s="74"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="74"/>
+      <c r="K7" s="74"/>
+      <c r="L7" s="74"/>
+      <c r="M7" s="74"/>
+      <c r="N7" s="74"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A8" s="71"/>
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="71"/>
-      <c r="H8" s="71"/>
-      <c r="I8" s="71"/>
-      <c r="J8" s="71"/>
-      <c r="K8" s="71"/>
-      <c r="L8" s="71"/>
-      <c r="M8" s="71"/>
-      <c r="N8" s="71"/>
+      <c r="A8" s="74"/>
+      <c r="B8" s="74"/>
+      <c r="C8" s="74"/>
+      <c r="D8" s="74"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="74"/>
+      <c r="G8" s="74"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="74"/>
+      <c r="K8" s="74"/>
+      <c r="L8" s="74"/>
+      <c r="M8" s="74"/>
+      <c r="N8" s="74"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" s="20" t="s">
@@ -10277,35 +10336,35 @@
       <c r="N11" s="23"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A14" s="70" t="s">
+      <c r="A14" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="70"/>
-      <c r="C14" s="70"/>
-      <c r="D14" s="70"/>
-      <c r="E14" s="70"/>
-      <c r="F14" s="70"/>
-      <c r="H14" s="72" t="s">
+      <c r="B14" s="73"/>
+      <c r="C14" s="73"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="73"/>
+      <c r="H14" s="75" t="s">
         <v>35</v>
       </c>
-      <c r="I14" s="72"/>
-      <c r="J14" s="72"/>
-      <c r="L14" s="72" t="s">
+      <c r="I14" s="75"/>
+      <c r="J14" s="75"/>
+      <c r="L14" s="75" t="s">
         <v>36</v>
       </c>
       <c r="M14"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.45">
-      <c r="A15" s="70"/>
-      <c r="B15" s="70"/>
-      <c r="C15" s="70"/>
-      <c r="D15" s="70"/>
-      <c r="E15" s="70"/>
-      <c r="F15" s="70"/>
-      <c r="H15" s="72"/>
-      <c r="I15" s="72"/>
-      <c r="J15" s="72"/>
-      <c r="L15" s="72"/>
+      <c r="A15" s="73"/>
+      <c r="B15" s="73"/>
+      <c r="C15" s="73"/>
+      <c r="D15" s="73"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="73"/>
+      <c r="H15" s="75"/>
+      <c r="I15" s="75"/>
+      <c r="J15" s="75"/>
+      <c r="L15" s="75"/>
       <c r="M15"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.45">
@@ -11645,22 +11704,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B6:G6">
-    <cfRule type="expression" dxfId="12" priority="20">
+    <cfRule type="expression" dxfId="8" priority="20">
       <formula>B6&lt;&gt;B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:G32">
-    <cfRule type="expression" dxfId="11" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>B7&lt;&gt;B6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:M6">
-    <cfRule type="expression" dxfId="10" priority="22">
+    <cfRule type="expression" dxfId="6" priority="22">
       <formula>H6&lt;&gt;H4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:M32">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>H7&lt;&gt;H6</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12996,22 +13055,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B6:G6">
-    <cfRule type="expression" dxfId="8" priority="19">
+    <cfRule type="expression" dxfId="4" priority="19">
       <formula>B6&lt;&gt;B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:G32">
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>B7&lt;&gt;B6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:M6">
-    <cfRule type="expression" dxfId="6" priority="20">
+    <cfRule type="expression" dxfId="2" priority="20">
       <formula>H6&lt;&gt;H4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:M32">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>H7&lt;&gt;H6</formula>
     </cfRule>
   </conditionalFormatting>
@@ -21390,20 +21449,21 @@
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="10.86328125" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" customWidth="1"/>
-    <col min="4" max="4" width="10.796875" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.9296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="84.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
@@ -21423,7 +21483,7 @@
         <v>275</v>
       </c>
       <c r="F1" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="G1" t="s">
         <v>277</v>
@@ -21433,38 +21493,221 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A2" s="73">
+      <c r="A2" s="70">
         <v>46075</v>
       </c>
-      <c r="C2" s="74">
-        <v>0.45833333333333331</v>
-      </c>
-      <c r="D2" s="74">
+      <c r="C2" s="71">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="D2" s="71">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E2" s="72" t="s">
+        <v>278</v>
+      </c>
+      <c r="F2" s="72" t="s">
+        <v>282</v>
+      </c>
+      <c r="G2" t="s">
+        <v>279</v>
+      </c>
+      <c r="H2" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" s="70">
+        <v>46075</v>
+      </c>
+      <c r="C3" s="71">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D3" s="71">
+        <v>0.65625</v>
+      </c>
+      <c r="E3" s="72" t="s">
+        <v>283</v>
+      </c>
+      <c r="F3" s="72" t="s">
+        <v>284</v>
+      </c>
+      <c r="G3" t="s">
+        <v>279</v>
+      </c>
+      <c r="H3" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4" s="70">
+        <v>46124</v>
+      </c>
+      <c r="C4" s="71">
+        <v>0.38541666666666669</v>
+      </c>
+      <c r="D4" s="71">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E4" s="72" t="s">
+        <v>278</v>
+      </c>
+      <c r="F4" s="72" t="s">
+        <v>282</v>
+      </c>
+      <c r="G4" t="s">
+        <v>279</v>
+      </c>
+      <c r="H4" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" s="70">
+        <v>46124</v>
+      </c>
+      <c r="C5" s="71">
         <v>0.5</v>
       </c>
-      <c r="E2" s="75" t="s">
+      <c r="D5" s="71">
+        <v>0.65625</v>
+      </c>
+      <c r="E5" s="72" t="s">
+        <v>283</v>
+      </c>
+      <c r="F5" s="72" t="s">
+        <v>286</v>
+      </c>
+      <c r="G5" t="s">
         <v>279</v>
       </c>
-      <c r="F2" s="75" t="s">
+      <c r="H5" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A6" s="70">
+        <v>46186</v>
+      </c>
+      <c r="C6" s="71">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D6" s="71">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="E6" s="72" t="s">
+        <v>283</v>
+      </c>
+      <c r="F6" s="72" t="s">
+        <v>287</v>
+      </c>
+      <c r="G6" t="s">
+        <v>288</v>
+      </c>
+      <c r="H6" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A7" s="70">
+        <v>46187</v>
+      </c>
+      <c r="C7" s="71">
+        <v>0.53125</v>
+      </c>
+      <c r="D7" s="71">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E7" s="72" t="s">
+        <v>278</v>
+      </c>
+      <c r="F7" s="72" t="s">
+        <v>289</v>
+      </c>
+      <c r="G7" t="s">
+        <v>279</v>
+      </c>
+      <c r="H7" t="s">
         <v>280</v>
       </c>
-      <c r="G2" t="s">
-        <v>281</v>
-      </c>
-      <c r="H2" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" s="73">
-        <v>46075</v>
-      </c>
-      <c r="C3" s="74"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A8" s="70">
+        <v>46199</v>
+      </c>
+      <c r="B8" s="70">
+        <v>46204</v>
+      </c>
+      <c r="C8" s="71">
+        <v>0</v>
+      </c>
+      <c r="D8" s="71">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="E8" s="72" t="s">
+        <v>290</v>
+      </c>
+      <c r="F8" s="72" t="s">
+        <v>291</v>
+      </c>
+      <c r="G8" t="s">
+        <v>292</v>
+      </c>
+      <c r="H8" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A9" s="70">
+        <v>46207</v>
+      </c>
+      <c r="C9" s="71">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D9" s="71">
+        <v>0.75</v>
+      </c>
+      <c r="E9" s="72" t="s">
+        <v>293</v>
+      </c>
+      <c r="F9" s="72" t="s">
+        <v>294</v>
+      </c>
+      <c r="G9" t="s">
+        <v>295</v>
+      </c>
+      <c r="H9" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A10" s="70">
+        <v>46228</v>
+      </c>
+      <c r="C10" s="71">
+        <v>0</v>
+      </c>
+      <c r="D10" s="71">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="E10" s="72" t="s">
+        <v>297</v>
+      </c>
+      <c r="F10" s="72" t="s">
+        <v>298</v>
+      </c>
+      <c r="G10" t="s">
+        <v>299</v>
+      </c>
+      <c r="H10" t="s">
+        <v>300</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:H10">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$A2&lt;TODAY()</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
new times for LK
</commit_message>
<xml_diff>
--- a/web/utilities/records_kriterien.xlsx
+++ b/web/utilities/records_kriterien.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgna\Documents\GitHub\Lifesaving_Baden\web\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D53B8D5-A2C9-4A93-905F-8684BD73162B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D695A6A8-4FF6-4465-975F-81C2251A41C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="4" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="8" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
   </bookViews>
   <sheets>
     <sheet name="DR" sheetId="9" r:id="rId1"/>
@@ -1525,9 +1525,6 @@
   </cellStyles>
   <dxfs count="200">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <color theme="4"/>
       </font>
@@ -1803,6 +1800,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -4117,28 +4117,28 @@
     <tableColumn id="4" xr3:uid="{FD3A030F-CD97-4B6F-8E8C-BC2E67D79F1D}" name="Maximales Alter" dataDxfId="93"/>
     <tableColumn id="5" xr3:uid="{3E22B645-D77C-4509-B031-9914FCB91599}" name="Qualizeitraum anfang" dataDxfId="92"/>
     <tableColumn id="6" xr3:uid="{AE299324-3C1C-4063-ADF9-54555A161734}" name="Qualizeitraum Ende" dataDxfId="91"/>
-    <tableColumn id="7" xr3:uid="{DCC178B3-11FC-4C53-BBC6-C2FDA2C89857}" name="Letzter Wettkampf am" dataDxfId="0"/>
-    <tableColumn id="8" xr3:uid="{2811DB01-60A5-4BE4-B6F9-A806398A602A}" name="Wertung" dataDxfId="90"/>
-    <tableColumn id="9" xr3:uid="{0C16DAFE-847D-4E9E-9604-3A7D9FE924D0}" name="Landesverband" dataDxfId="89"/>
-    <tableColumn id="10" xr3:uid="{7A8A4101-A553-4BD5-9116-9AA5876B9401}" name="OMS" dataDxfId="88"/>
-    <tableColumn id="11" xr3:uid="{9807C9BD-6499-45F6-ACE0-4D13D64EF675}" name="Pool-Länge" dataDxfId="87"/>
-    <tableColumn id="12" xr3:uid="{13D336DD-650F-4F2C-836F-361CA1528F6D}" name="Regelwerk" dataDxfId="86"/>
-    <tableColumn id="13" xr3:uid="{66660E2D-ADF2-4FB5-8A13-004F826EE908}" name="Referenz" dataDxfId="85"/>
-    <tableColumn id="19" xr3:uid="{D72EDF8B-ECC3-4FF7-ABE6-B60BCE4A5E26}" name="Referenz Jahr" dataDxfId="84"/>
-    <tableColumn id="20" xr3:uid="{7B18E667-70F7-4BC1-AB1B-21C019F2AA89}" name="Mindest Punktzahl" dataDxfId="83"/>
-    <tableColumn id="21" xr3:uid="{FC185946-681B-42A6-AB1A-FC1EABB668C5}" name="Mindest Disziplinen" dataDxfId="82"/>
-    <tableColumn id="14" xr3:uid="{6A2676FD-2EC7-4C41-A35E-A1597A38F932}" name="3-Kampf Regel" dataDxfId="81"/>
-    <tableColumn id="15" xr3:uid="{718E0917-4F83-4A2B-832F-EBB16D5E21BF}" name="Anzahl Nominierte" dataDxfId="80"/>
-    <tableColumn id="16" xr3:uid="{5C66A461-D647-4E00-A81C-FD7AD44D7CC2}" name="Anzahl Nachrücker" dataDxfId="79"/>
-    <tableColumn id="17" xr3:uid="{D434BDEC-293B-4B4E-A5E9-479438960A03}" name="Seiten Anzahl" dataDxfId="78"/>
-    <tableColumn id="18" xr3:uid="{80908229-9247-473F-81C0-9C9D4C12FF06}" name="Absagen" dataDxfId="77"/>
+    <tableColumn id="7" xr3:uid="{DCC178B3-11FC-4C53-BBC6-C2FDA2C89857}" name="Letzter Wettkampf am" dataDxfId="90"/>
+    <tableColumn id="8" xr3:uid="{2811DB01-60A5-4BE4-B6F9-A806398A602A}" name="Wertung" dataDxfId="89"/>
+    <tableColumn id="9" xr3:uid="{0C16DAFE-847D-4E9E-9604-3A7D9FE924D0}" name="Landesverband" dataDxfId="88"/>
+    <tableColumn id="10" xr3:uid="{7A8A4101-A553-4BD5-9116-9AA5876B9401}" name="OMS" dataDxfId="87"/>
+    <tableColumn id="11" xr3:uid="{9807C9BD-6499-45F6-ACE0-4D13D64EF675}" name="Pool-Länge" dataDxfId="86"/>
+    <tableColumn id="12" xr3:uid="{13D336DD-650F-4F2C-836F-361CA1528F6D}" name="Regelwerk" dataDxfId="85"/>
+    <tableColumn id="13" xr3:uid="{66660E2D-ADF2-4FB5-8A13-004F826EE908}" name="Referenz" dataDxfId="84"/>
+    <tableColumn id="19" xr3:uid="{D72EDF8B-ECC3-4FF7-ABE6-B60BCE4A5E26}" name="Referenz Jahr" dataDxfId="83"/>
+    <tableColumn id="20" xr3:uid="{7B18E667-70F7-4BC1-AB1B-21C019F2AA89}" name="Mindest Punktzahl" dataDxfId="82"/>
+    <tableColumn id="21" xr3:uid="{FC185946-681B-42A6-AB1A-FC1EABB668C5}" name="Mindest Disziplinen" dataDxfId="81"/>
+    <tableColumn id="14" xr3:uid="{6A2676FD-2EC7-4C41-A35E-A1597A38F932}" name="3-Kampf Regel" dataDxfId="80"/>
+    <tableColumn id="15" xr3:uid="{718E0917-4F83-4A2B-832F-EBB16D5E21BF}" name="Anzahl Nominierte" dataDxfId="79"/>
+    <tableColumn id="16" xr3:uid="{5C66A461-D647-4E00-A81C-FD7AD44D7CC2}" name="Anzahl Nachrücker" dataDxfId="78"/>
+    <tableColumn id="17" xr3:uid="{D434BDEC-293B-4B4E-A5E9-479438960A03}" name="Seiten Anzahl" dataDxfId="77"/>
+    <tableColumn id="18" xr3:uid="{80908229-9247-473F-81C0-9C9D4C12FF06}" name="Absagen" dataDxfId="76"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{16F87202-5A6A-4E2F-B973-3CE7EC2566C1}" name="DEM_konfig" displayName="DEM_konfig" ref="A1:X7" totalsRowShown="0" headerRowDxfId="76" dataDxfId="75">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{16F87202-5A6A-4E2F-B973-3CE7EC2566C1}" name="DEM_konfig" displayName="DEM_konfig" ref="A1:X7" totalsRowShown="0" headerRowDxfId="75" dataDxfId="74">
   <autoFilter ref="A1:X7" xr:uid="{16F87202-5A6A-4E2F-B973-3CE7EC2566C1}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4166,37 +4166,37 @@
     <filterColumn colId="23" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{4847B567-64E1-4AC3-8C4B-EFCF3F00CC6C}" name="Tabellen Name" dataDxfId="74"/>
-    <tableColumn id="2" xr3:uid="{6346FF3B-B334-4CD8-8B23-F2347E29C536}" name="Geschlecht" dataDxfId="73"/>
-    <tableColumn id="3" xr3:uid="{E793B48A-BC8A-439F-8AAF-6FD08104A619}" name="Mindest Alter" dataDxfId="72"/>
-    <tableColumn id="4" xr3:uid="{01A62C29-2F75-4107-A431-F69230BCCD0C}" name="Maximales Alter" dataDxfId="71"/>
-    <tableColumn id="5" xr3:uid="{B7E4DE90-7856-4A0C-9063-61414D7F227C}" name="Qualizeitraum anfang" dataDxfId="70"/>
-    <tableColumn id="6" xr3:uid="{B00F7CD1-82CB-42B9-A396-89F79EF419CA}" name="Qualizeitraum Ende" dataDxfId="69"/>
-    <tableColumn id="7" xr3:uid="{9E50DDE5-12E3-4BCB-801C-FBABCE309F0E}" name="Letzter Wettkampf am" dataDxfId="68"/>
-    <tableColumn id="8" xr3:uid="{57E68247-0FF2-48D8-8ACD-AB057E576A21}" name="Landesverband" dataDxfId="67"/>
-    <tableColumn id="9" xr3:uid="{EBAA439D-F69A-4C2A-8193-9AE08F1E57B8}" name="OMS" dataDxfId="66"/>
-    <tableColumn id="10" xr3:uid="{BBD11E7F-3DDF-428A-B005-4A40E6FA78DC}" name="Pool-Länge" dataDxfId="65"/>
-    <tableColumn id="11" xr3:uid="{6AE38DCA-A084-4F3D-A6A4-4E76E3E2CBC6}" name="Regelwerk" dataDxfId="64"/>
-    <tableColumn id="12" xr3:uid="{7F7470AD-5502-4CEE-BB4C-44BA308E61D7}" name="Seiten Anzahl" dataDxfId="63"/>
-    <tableColumn id="13" xr3:uid="{F416CBFA-4C9D-45CD-9BA7-E4BC57A08BC2}" name="PZ1 - 50m Retten" dataDxfId="62"/>
-    <tableColumn id="14" xr3:uid="{7117DBCA-0DA7-462C-84FE-0DC7E33B124C}" name="PZ1 - 100m Retten" dataDxfId="61"/>
-    <tableColumn id="15" xr3:uid="{E8630E91-DC30-4822-9E53-6D65487C3670}" name="PZ1 - 100m Kombi" dataDxfId="60"/>
-    <tableColumn id="16" xr3:uid="{4B3AA225-E042-430F-8259-D176887B4528}" name="PZ1 - 100m Lifesaver" dataDxfId="59"/>
-    <tableColumn id="17" xr3:uid="{798674BD-98CE-4531-BDFF-6AB06253AD7C}" name="PZ1 - 200m Super-Lifesaver" dataDxfId="58"/>
-    <tableColumn id="18" xr3:uid="{8809BB71-D58B-4E8B-A442-D0EB9A65A25D}" name="PZ1 - 200m Hindernis" dataDxfId="57"/>
-    <tableColumn id="19" xr3:uid="{93DCF463-806B-4117-B4E3-1FFAE976B37C}" name="PZ2 - 50m Retten" dataDxfId="56"/>
-    <tableColumn id="20" xr3:uid="{A514C961-559E-462F-B143-BA30974C0129}" name="PZ2 - 100m Retten" dataDxfId="55"/>
-    <tableColumn id="21" xr3:uid="{F1CF6143-45FE-498D-93D6-36F26D2F3C0B}" name="PZ2 - 100m Kombi" dataDxfId="54"/>
-    <tableColumn id="22" xr3:uid="{E90962FC-C214-467F-841F-40DF60E41456}" name="PZ2 - 100m Lifesaver" dataDxfId="53"/>
-    <tableColumn id="23" xr3:uid="{7FBC6334-C4C8-4B38-9F59-30ED95A44379}" name="PZ2 - 200m Super-Lifesaver" dataDxfId="52"/>
-    <tableColumn id="24" xr3:uid="{231BFF86-8F3A-4BA1-B25E-28175D9EDFA9}" name="PZ2 - 200m Hindernis" dataDxfId="51"/>
+    <tableColumn id="1" xr3:uid="{4847B567-64E1-4AC3-8C4B-EFCF3F00CC6C}" name="Tabellen Name" dataDxfId="73"/>
+    <tableColumn id="2" xr3:uid="{6346FF3B-B334-4CD8-8B23-F2347E29C536}" name="Geschlecht" dataDxfId="72"/>
+    <tableColumn id="3" xr3:uid="{E793B48A-BC8A-439F-8AAF-6FD08104A619}" name="Mindest Alter" dataDxfId="71"/>
+    <tableColumn id="4" xr3:uid="{01A62C29-2F75-4107-A431-F69230BCCD0C}" name="Maximales Alter" dataDxfId="70"/>
+    <tableColumn id="5" xr3:uid="{B7E4DE90-7856-4A0C-9063-61414D7F227C}" name="Qualizeitraum anfang" dataDxfId="69"/>
+    <tableColumn id="6" xr3:uid="{B00F7CD1-82CB-42B9-A396-89F79EF419CA}" name="Qualizeitraum Ende" dataDxfId="68"/>
+    <tableColumn id="7" xr3:uid="{9E50DDE5-12E3-4BCB-801C-FBABCE309F0E}" name="Letzter Wettkampf am" dataDxfId="67"/>
+    <tableColumn id="8" xr3:uid="{57E68247-0FF2-48D8-8ACD-AB057E576A21}" name="Landesverband" dataDxfId="66"/>
+    <tableColumn id="9" xr3:uid="{EBAA439D-F69A-4C2A-8193-9AE08F1E57B8}" name="OMS" dataDxfId="65"/>
+    <tableColumn id="10" xr3:uid="{BBD11E7F-3DDF-428A-B005-4A40E6FA78DC}" name="Pool-Länge" dataDxfId="64"/>
+    <tableColumn id="11" xr3:uid="{6AE38DCA-A084-4F3D-A6A4-4E76E3E2CBC6}" name="Regelwerk" dataDxfId="63"/>
+    <tableColumn id="12" xr3:uid="{7F7470AD-5502-4CEE-BB4C-44BA308E61D7}" name="Seiten Anzahl" dataDxfId="62"/>
+    <tableColumn id="13" xr3:uid="{F416CBFA-4C9D-45CD-9BA7-E4BC57A08BC2}" name="PZ1 - 50m Retten" dataDxfId="61"/>
+    <tableColumn id="14" xr3:uid="{7117DBCA-0DA7-462C-84FE-0DC7E33B124C}" name="PZ1 - 100m Retten" dataDxfId="60"/>
+    <tableColumn id="15" xr3:uid="{E8630E91-DC30-4822-9E53-6D65487C3670}" name="PZ1 - 100m Kombi" dataDxfId="59"/>
+    <tableColumn id="16" xr3:uid="{4B3AA225-E042-430F-8259-D176887B4528}" name="PZ1 - 100m Lifesaver" dataDxfId="58"/>
+    <tableColumn id="17" xr3:uid="{798674BD-98CE-4531-BDFF-6AB06253AD7C}" name="PZ1 - 200m Super-Lifesaver" dataDxfId="57"/>
+    <tableColumn id="18" xr3:uid="{8809BB71-D58B-4E8B-A442-D0EB9A65A25D}" name="PZ1 - 200m Hindernis" dataDxfId="56"/>
+    <tableColumn id="19" xr3:uid="{93DCF463-806B-4117-B4E3-1FFAE976B37C}" name="PZ2 - 50m Retten" dataDxfId="55"/>
+    <tableColumn id="20" xr3:uid="{A514C961-559E-462F-B143-BA30974C0129}" name="PZ2 - 100m Retten" dataDxfId="54"/>
+    <tableColumn id="21" xr3:uid="{F1CF6143-45FE-498D-93D6-36F26D2F3C0B}" name="PZ2 - 100m Kombi" dataDxfId="53"/>
+    <tableColumn id="22" xr3:uid="{E90962FC-C214-467F-841F-40DF60E41456}" name="PZ2 - 100m Lifesaver" dataDxfId="52"/>
+    <tableColumn id="23" xr3:uid="{7FBC6334-C4C8-4B38-9F59-30ED95A44379}" name="PZ2 - 200m Super-Lifesaver" dataDxfId="51"/>
+    <tableColumn id="24" xr3:uid="{231BFF86-8F3A-4BA1-B25E-28175D9EDFA9}" name="PZ2 - 200m Hindernis" dataDxfId="50"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}" name="JRP_konfig" displayName="JRP_konfig" ref="A1:X15" totalsRowShown="0" headerRowDxfId="50" dataDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}" name="JRP_konfig" displayName="JRP_konfig" ref="A1:X15" totalsRowShown="0" headerRowDxfId="49" dataDxfId="48">
   <autoFilter ref="A1:X15" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4224,30 +4224,30 @@
     <filterColumn colId="23" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{021DA6E1-2C93-4474-9720-B6F016186D61}" name="Tabellen Name" dataDxfId="48"/>
-    <tableColumn id="2" xr3:uid="{733C1722-A9C9-4830-A9E2-FE62E96BCD98}" name="Geschlecht" dataDxfId="47"/>
-    <tableColumn id="3" xr3:uid="{80C0BF46-0E43-4947-BF86-B808C324772A}" name="Mindest Alter" dataDxfId="46"/>
-    <tableColumn id="4" xr3:uid="{DBA2A923-EEB7-43F9-A1A3-E78624448FB9}" name="Maximales Alter" dataDxfId="45"/>
-    <tableColumn id="5" xr3:uid="{3FDEE18A-328D-45AE-907D-69A916A93345}" name="Qualizeitraum anfang" dataDxfId="44"/>
-    <tableColumn id="6" xr3:uid="{BE002D7F-575F-4B60-9251-C71D93F59045}" name="Qualizeitraum Ende" dataDxfId="43"/>
-    <tableColumn id="7" xr3:uid="{208ABD57-DE4B-41D6-B9FC-93F2D8966E8D}" name="Letzter Wettkampf am" dataDxfId="42"/>
-    <tableColumn id="8" xr3:uid="{30C9697C-6550-4996-ADDB-7FEE5325B794}" name="Landesverband" dataDxfId="41"/>
-    <tableColumn id="9" xr3:uid="{ED2DAB77-EF46-4D8B-B8E4-90412E32E277}" name="OMS" dataDxfId="40"/>
-    <tableColumn id="10" xr3:uid="{AD534940-A91B-4A6E-9606-E3F3E517D401}" name="Pool-Länge" dataDxfId="39"/>
-    <tableColumn id="11" xr3:uid="{11F9D5D5-72FE-42CA-8624-01D513B4140F}" name="Regelwerk" dataDxfId="38"/>
-    <tableColumn id="12" xr3:uid="{3907872B-5438-4FBF-A045-3EF9EAACFC47}" name="Seiten Anzahl" dataDxfId="37"/>
-    <tableColumn id="13" xr3:uid="{FC821324-3638-40C0-BA1E-069B44E23C7A}" name="PZ1 - 50m Retten" dataDxfId="36"/>
-    <tableColumn id="14" xr3:uid="{70529619-443E-40D3-88C1-3E0F00BB2A50}" name="PZ1 - 100m Retten" dataDxfId="35"/>
-    <tableColumn id="15" xr3:uid="{EFA92FD2-C23F-42B3-83DC-5036513F19AF}" name="PZ1 - 100m Kombi" dataDxfId="34"/>
-    <tableColumn id="16" xr3:uid="{03309E52-8CF3-4E90-9EE6-A818901C3B32}" name="PZ1 - 100m Lifesaver" dataDxfId="33"/>
-    <tableColumn id="17" xr3:uid="{00B22013-AA11-4C17-9250-22060AE4B0A8}" name="PZ1 - 200m Super-Lifesaver" dataDxfId="32"/>
-    <tableColumn id="18" xr3:uid="{7E3508A9-0422-4561-A23E-53E613259B24}" name="PZ1 - 200m Hindernis" dataDxfId="31"/>
-    <tableColumn id="19" xr3:uid="{5CEA435F-F34B-4D8D-88D0-F5EBFF18B713}" name="PZ2 - 50m Retten" dataDxfId="30"/>
-    <tableColumn id="20" xr3:uid="{8585BE62-F7C4-4D5D-B287-052B43B08610}" name="PZ2 - 100m Retten" dataDxfId="29"/>
-    <tableColumn id="21" xr3:uid="{D981758B-ADAD-4E36-B787-0B0FDA808CA2}" name="PZ2 - 100m Kombi" dataDxfId="28"/>
-    <tableColumn id="22" xr3:uid="{1D4970A8-D22F-4962-934C-AEA295ED687A}" name="PZ2 - 100m Lifesaver" dataDxfId="27"/>
-    <tableColumn id="23" xr3:uid="{BE394430-C58F-4690-9615-44475E5AF9F8}" name="PZ2 - 200m Super-Lifesaver" dataDxfId="26"/>
-    <tableColumn id="24" xr3:uid="{A7036B1A-99CE-4F7C-AAB8-12E8B2696202}" name="PZ2 - 200m Hindernis" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{021DA6E1-2C93-4474-9720-B6F016186D61}" name="Tabellen Name" dataDxfId="47"/>
+    <tableColumn id="2" xr3:uid="{733C1722-A9C9-4830-A9E2-FE62E96BCD98}" name="Geschlecht" dataDxfId="46"/>
+    <tableColumn id="3" xr3:uid="{80C0BF46-0E43-4947-BF86-B808C324772A}" name="Mindest Alter" dataDxfId="45"/>
+    <tableColumn id="4" xr3:uid="{DBA2A923-EEB7-43F9-A1A3-E78624448FB9}" name="Maximales Alter" dataDxfId="44"/>
+    <tableColumn id="5" xr3:uid="{3FDEE18A-328D-45AE-907D-69A916A93345}" name="Qualizeitraum anfang" dataDxfId="43"/>
+    <tableColumn id="6" xr3:uid="{BE002D7F-575F-4B60-9251-C71D93F59045}" name="Qualizeitraum Ende" dataDxfId="42"/>
+    <tableColumn id="7" xr3:uid="{208ABD57-DE4B-41D6-B9FC-93F2D8966E8D}" name="Letzter Wettkampf am" dataDxfId="41"/>
+    <tableColumn id="8" xr3:uid="{30C9697C-6550-4996-ADDB-7FEE5325B794}" name="Landesverband" dataDxfId="40"/>
+    <tableColumn id="9" xr3:uid="{ED2DAB77-EF46-4D8B-B8E4-90412E32E277}" name="OMS" dataDxfId="39"/>
+    <tableColumn id="10" xr3:uid="{AD534940-A91B-4A6E-9606-E3F3E517D401}" name="Pool-Länge" dataDxfId="38"/>
+    <tableColumn id="11" xr3:uid="{11F9D5D5-72FE-42CA-8624-01D513B4140F}" name="Regelwerk" dataDxfId="37"/>
+    <tableColumn id="12" xr3:uid="{3907872B-5438-4FBF-A045-3EF9EAACFC47}" name="Seiten Anzahl" dataDxfId="36"/>
+    <tableColumn id="13" xr3:uid="{FC821324-3638-40C0-BA1E-069B44E23C7A}" name="PZ1 - 50m Retten" dataDxfId="35"/>
+    <tableColumn id="14" xr3:uid="{70529619-443E-40D3-88C1-3E0F00BB2A50}" name="PZ1 - 100m Retten" dataDxfId="34"/>
+    <tableColumn id="15" xr3:uid="{EFA92FD2-C23F-42B3-83DC-5036513F19AF}" name="PZ1 - 100m Kombi" dataDxfId="33"/>
+    <tableColumn id="16" xr3:uid="{03309E52-8CF3-4E90-9EE6-A818901C3B32}" name="PZ1 - 100m Lifesaver" dataDxfId="32"/>
+    <tableColumn id="17" xr3:uid="{00B22013-AA11-4C17-9250-22060AE4B0A8}" name="PZ1 - 200m Super-Lifesaver" dataDxfId="31"/>
+    <tableColumn id="18" xr3:uid="{7E3508A9-0422-4561-A23E-53E613259B24}" name="PZ1 - 200m Hindernis" dataDxfId="30"/>
+    <tableColumn id="19" xr3:uid="{5CEA435F-F34B-4D8D-88D0-F5EBFF18B713}" name="PZ2 - 50m Retten" dataDxfId="29"/>
+    <tableColumn id="20" xr3:uid="{8585BE62-F7C4-4D5D-B287-052B43B08610}" name="PZ2 - 100m Retten" dataDxfId="28"/>
+    <tableColumn id="21" xr3:uid="{D981758B-ADAD-4E36-B787-0B0FDA808CA2}" name="PZ2 - 100m Kombi" dataDxfId="27"/>
+    <tableColumn id="22" xr3:uid="{1D4970A8-D22F-4962-934C-AEA295ED687A}" name="PZ2 - 100m Lifesaver" dataDxfId="26"/>
+    <tableColumn id="23" xr3:uid="{BE394430-C58F-4690-9615-44475E5AF9F8}" name="PZ2 - 200m Super-Lifesaver" dataDxfId="25"/>
+    <tableColumn id="24" xr3:uid="{A7036B1A-99CE-4F7C-AAB8-12E8B2696202}" name="PZ2 - 200m Hindernis" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4257,12 +4257,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{888CE7BE-8313-44C0-AE38-83992EABD44D}" name="LK_Kalender" displayName="LK_Kalender" ref="A1:H10" totalsRowShown="0">
   <autoFilter ref="A1:H10" xr:uid="{888CE7BE-8313-44C0-AE38-83992EABD44D}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{B26B9E90-F378-41EF-B35E-CE240017E4BE}" name="datum von" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{B26B9E90-F378-41EF-B35E-CE240017E4BE}" name="datum von" dataDxfId="23"/>
     <tableColumn id="2" xr3:uid="{38211212-0A92-428C-895C-E4CA68F52818}" name="datum bis"/>
-    <tableColumn id="3" xr3:uid="{66E541C6-0A5E-4B2D-9B89-5E52F449A4A6}" name="uhrzeit von" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{D93C06A2-29AD-4073-8E3C-A685B4474CC8}" name="uhrzeit bis" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{C5C3979C-B528-44E8-A5A6-36F020A6034F}" name="titel" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{9DC09E1D-44FD-40ED-9EBE-86A8E61C38B2}" name="meta" dataDxfId="20"/>
+    <tableColumn id="3" xr3:uid="{66E541C6-0A5E-4B2D-9B89-5E52F449A4A6}" name="uhrzeit von" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{D93C06A2-29AD-4073-8E3C-A685B4474CC8}" name="uhrzeit bis" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{C5C3979C-B528-44E8-A5A6-36F020A6034F}" name="titel" dataDxfId="20"/>
+    <tableColumn id="6" xr3:uid="{9DC09E1D-44FD-40ED-9EBE-86A8E61C38B2}" name="meta" dataDxfId="19"/>
     <tableColumn id="7" xr3:uid="{E7E62A34-7A76-4361-937D-F4DE76E6E7CC}" name="ort"/>
     <tableColumn id="8" xr3:uid="{84F02734-FC16-406B-ACCA-0CCDF547D94C}" name="kader"/>
   </tableColumns>
@@ -8209,52 +8209,52 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B5:G31">
-    <cfRule type="expression" dxfId="19" priority="15">
+    <cfRule type="expression" dxfId="18" priority="15">
       <formula>B5&lt;&gt;B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:M31">
-    <cfRule type="expression" dxfId="18" priority="14">
+    <cfRule type="expression" dxfId="17" priority="14">
       <formula>H5&lt;&gt;H4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N5:S31">
-    <cfRule type="expression" dxfId="17" priority="13">
+    <cfRule type="expression" dxfId="16" priority="13">
       <formula>N5&lt;&gt;N4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T5:Y31">
-    <cfRule type="expression" dxfId="16" priority="12">
+    <cfRule type="expression" dxfId="15" priority="12">
       <formula>T5&lt;&gt;T4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z5:AE31">
-    <cfRule type="expression" dxfId="15" priority="9">
+    <cfRule type="expression" dxfId="14" priority="9">
       <formula>Z5&lt;&gt;Z4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF5:AK31">
-    <cfRule type="expression" dxfId="14" priority="8">
+    <cfRule type="expression" dxfId="13" priority="8">
       <formula>AF5&lt;&gt;AF4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL5:AN31">
-    <cfRule type="expression" dxfId="13" priority="6">
+    <cfRule type="expression" dxfId="12" priority="6">
       <formula>AL5&lt;&gt;AL4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO5:AQ31">
-    <cfRule type="expression" dxfId="12" priority="5">
+    <cfRule type="expression" dxfId="11" priority="5">
       <formula>AO5&lt;&gt;AO4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR5:AT31">
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="10" priority="2">
       <formula>AR5&lt;&gt;AR4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU5:AW31">
-    <cfRule type="expression" dxfId="10" priority="1">
+    <cfRule type="expression" dxfId="9" priority="1">
       <formula>AU5&lt;&gt;AU4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11620,22 +11620,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B6:G6">
-    <cfRule type="expression" dxfId="9" priority="20">
+    <cfRule type="expression" dxfId="8" priority="20">
       <formula>B6&lt;&gt;B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:G32">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>B7&lt;&gt;B6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:M6">
-    <cfRule type="expression" dxfId="7" priority="22">
+    <cfRule type="expression" dxfId="6" priority="22">
       <formula>H6&lt;&gt;H4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:M32">
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>H7&lt;&gt;H6</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12971,22 +12971,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B6:G6">
-    <cfRule type="expression" dxfId="5" priority="19">
+    <cfRule type="expression" dxfId="4" priority="19">
       <formula>B6&lt;&gt;B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:G32">
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>B7&lt;&gt;B6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:M6">
-    <cfRule type="expression" dxfId="3" priority="20">
+    <cfRule type="expression" dxfId="2" priority="20">
       <formula>H6&lt;&gt;H4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:M32">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>H7&lt;&gt;H6</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13234,7 +13234,7 @@
   </sheetPr>
   <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
@@ -14243,7 +14243,7 @@
   <dimension ref="A1:X15"/>
   <sheetViews>
     <sheetView zoomScale="83" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -14523,51 +14523,51 @@
       </c>
       <c r="M4" s="62">
         <f>NK!E14</f>
-        <v>4.4045138888888888E-4</v>
+        <v>4.4418402777777777E-4</v>
       </c>
       <c r="N4" s="62">
         <f>NK!E16</f>
-        <v>6.9557175925925928E-4</v>
+        <v>7.0146643518518518E-4</v>
       </c>
       <c r="O4" s="62">
         <f>NK!E15</f>
-        <v>9.4522916666666681E-4</v>
+        <v>9.532395833333335E-4</v>
       </c>
       <c r="P4" s="62">
         <f>NK!E17</f>
-        <v>7.884421296296295E-4</v>
+        <v>7.951238425925925E-4</v>
       </c>
       <c r="Q4" s="62">
         <f>NK!E19</f>
-        <v>1.961340277777778E-3</v>
+        <v>1.9779618055555557E-3</v>
       </c>
       <c r="R4" s="62">
         <f>NK!E18</f>
-        <v>1.7914421296296294E-3</v>
+        <v>1.8066238425925923E-3</v>
       </c>
       <c r="S4" s="62">
         <f>M4</f>
-        <v>4.4045138888888888E-4</v>
+        <v>4.4418402777777777E-4</v>
       </c>
       <c r="T4" s="62">
         <f t="shared" ref="T4:T9" si="0">N4</f>
-        <v>6.9557175925925928E-4</v>
+        <v>7.0146643518518518E-4</v>
       </c>
       <c r="U4" s="62">
         <f t="shared" ref="U4:U9" si="1">O4</f>
-        <v>9.4522916666666681E-4</v>
+        <v>9.532395833333335E-4</v>
       </c>
       <c r="V4" s="62">
         <f t="shared" ref="V4:V9" si="2">P4</f>
-        <v>7.884421296296295E-4</v>
+        <v>7.951238425925925E-4</v>
       </c>
       <c r="W4" s="62">
         <f t="shared" ref="W4:W9" si="3">Q4</f>
-        <v>1.961340277777778E-3</v>
+        <v>1.9779618055555557E-3</v>
       </c>
       <c r="X4" s="62">
         <f t="shared" ref="X4:X9" si="4">R4</f>
-        <v>1.7914421296296294E-3</v>
+        <v>1.8066238425925923E-3</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.45">
@@ -14605,51 +14605,51 @@
       </c>
       <c r="M5" s="62">
         <f>NK!D14</f>
-        <v>4.5424537037037037E-4</v>
+        <v>4.5809490740740739E-4</v>
       </c>
       <c r="N5" s="62">
         <f>NK!D16</f>
-        <v>7.1551157407407403E-4</v>
+        <v>7.2157523148148146E-4</v>
       </c>
       <c r="O5" s="62">
         <f>NK!D15</f>
-        <v>9.8333333333333324E-4</v>
+        <v>9.9166666666666674E-4</v>
       </c>
       <c r="P5" s="62">
         <f>NK!D17</f>
-        <v>8.1876157407407407E-4</v>
+        <v>8.2570023148148151E-4</v>
       </c>
       <c r="Q5" s="62">
         <f>NK!D19</f>
-        <v>2.0244374999999998E-3</v>
+        <v>2.04159375E-3</v>
       </c>
       <c r="R5" s="62">
         <f>NK!D18</f>
-        <v>1.8460717592592589E-3</v>
+        <v>1.8617164351851848E-3</v>
       </c>
       <c r="S5" s="62">
         <f t="shared" ref="S5:S9" si="5">M5</f>
-        <v>4.5424537037037037E-4</v>
+        <v>4.5809490740740739E-4</v>
       </c>
       <c r="T5" s="62">
         <f t="shared" si="0"/>
-        <v>7.1551157407407403E-4</v>
+        <v>7.2157523148148146E-4</v>
       </c>
       <c r="U5" s="62">
         <f t="shared" si="1"/>
-        <v>9.8333333333333324E-4</v>
+        <v>9.9166666666666674E-4</v>
       </c>
       <c r="V5" s="62">
         <f t="shared" si="2"/>
-        <v>8.1876157407407407E-4</v>
+        <v>8.2570023148148151E-4</v>
       </c>
       <c r="W5" s="62">
         <f t="shared" si="3"/>
-        <v>2.0244374999999998E-3</v>
+        <v>2.04159375E-3</v>
       </c>
       <c r="X5" s="62">
         <f t="shared" si="4"/>
-        <v>1.8460717592592589E-3</v>
+        <v>1.8617164351851848E-3</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.45">
@@ -14687,51 +14687,51 @@
       </c>
       <c r="M6" s="62">
         <f>NK!C14</f>
-        <v>4.6353240740740735E-4</v>
+        <v>4.6746064814814805E-4</v>
       </c>
       <c r="N6" s="62">
         <f>NK!C16</f>
-        <v>7.2916898148148146E-4</v>
+        <v>7.3534837962962963E-4</v>
       </c>
       <c r="O6" s="62">
         <f>NK!C15</f>
-        <v>1.0006782407407406E-3</v>
+        <v>1.0091585648148147E-3</v>
       </c>
       <c r="P6" s="62">
         <f>NK!C17</f>
-        <v>8.3952083333333329E-4</v>
+        <v>8.4663541666666665E-4</v>
       </c>
       <c r="Q6" s="62">
         <f>NK!C19</f>
-        <v>2.067458333333333E-3</v>
+        <v>2.0849791666666664E-3</v>
       </c>
       <c r="R6" s="62">
         <f>NK!C18</f>
-        <v>1.8833564814814815E-3</v>
+        <v>1.8993171296296297E-3</v>
       </c>
       <c r="S6" s="62">
         <f t="shared" si="5"/>
-        <v>4.6353240740740735E-4</v>
+        <v>4.6746064814814805E-4</v>
       </c>
       <c r="T6" s="62">
         <f t="shared" si="0"/>
-        <v>7.2916898148148146E-4</v>
+        <v>7.3534837962962963E-4</v>
       </c>
       <c r="U6" s="62">
         <f t="shared" si="1"/>
-        <v>1.0006782407407406E-3</v>
+        <v>1.0091585648148147E-3</v>
       </c>
       <c r="V6" s="62">
         <f t="shared" si="2"/>
-        <v>8.3952083333333329E-4</v>
+        <v>8.4663541666666665E-4</v>
       </c>
       <c r="W6" s="62">
         <f t="shared" si="3"/>
-        <v>2.067458333333333E-3</v>
+        <v>2.0849791666666664E-3</v>
       </c>
       <c r="X6" s="62">
         <f t="shared" si="4"/>
-        <v>1.8833564814814815E-3</v>
+        <v>1.8993171296296297E-3</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.45">
@@ -14769,51 +14769,51 @@
       </c>
       <c r="M7" s="62">
         <f>NK!K14</f>
-        <v>5.4694444444444441E-4</v>
+        <v>5.4238657407407404E-4</v>
       </c>
       <c r="N7" s="62">
         <f>NK!K16</f>
-        <v>8.2777777777777786E-4</v>
+        <v>8.2087962962962963E-4</v>
       </c>
       <c r="O7" s="62">
         <f>NK!K15</f>
-        <v>1.1216666666666666E-3</v>
+        <v>1.1123194444444444E-3</v>
       </c>
       <c r="P7" s="62">
         <f>NK!K17</f>
-        <v>9.1791666666666671E-4</v>
+        <v>9.1026736111111115E-4</v>
       </c>
       <c r="Q7" s="62">
         <f>NK!K19</f>
-        <v>2.1695833333333333E-3</v>
+        <v>2.1515034722222222E-3</v>
       </c>
       <c r="R7" s="62">
         <f>NK!K18</f>
-        <v>1.9655555555555555E-3</v>
+        <v>1.9491759259259258E-3</v>
       </c>
       <c r="S7" s="62">
         <f t="shared" si="5"/>
-        <v>5.4694444444444441E-4</v>
+        <v>5.4238657407407404E-4</v>
       </c>
       <c r="T7" s="62">
         <f t="shared" si="0"/>
-        <v>8.2777777777777786E-4</v>
+        <v>8.2087962962962963E-4</v>
       </c>
       <c r="U7" s="62">
         <f t="shared" si="1"/>
-        <v>1.1216666666666666E-3</v>
+        <v>1.1123194444444444E-3</v>
       </c>
       <c r="V7" s="62">
         <f t="shared" si="2"/>
-        <v>9.1791666666666671E-4</v>
+        <v>9.1026736111111115E-4</v>
       </c>
       <c r="W7" s="62">
         <f t="shared" si="3"/>
-        <v>2.1695833333333333E-3</v>
+        <v>2.1515034722222222E-3</v>
       </c>
       <c r="X7" s="62">
         <f t="shared" si="4"/>
-        <v>1.9655555555555555E-3</v>
+        <v>1.9491759259259258E-3</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.45">
@@ -14851,51 +14851,51 @@
       </c>
       <c r="M8" s="62">
         <f>NK!J14</f>
-        <v>5.6041666666666664E-4</v>
+        <v>5.5574652777777773E-4</v>
       </c>
       <c r="N8" s="62">
         <f>NK!J16</f>
-        <v>8.4444444444444443E-4</v>
+        <v>8.3740740740740737E-4</v>
       </c>
       <c r="O8" s="62">
         <f>NK!J15</f>
-        <v>1.1630555555555554E-3</v>
+        <v>1.153363425925926E-3</v>
       </c>
       <c r="P8" s="62">
         <f>NK!J17</f>
-        <v>9.3833333333333334E-4</v>
+        <v>9.3051388888888893E-4</v>
       </c>
       <c r="Q8" s="62">
         <f>NK!J19</f>
-        <v>2.2183333333333334E-3</v>
+        <v>2.1998472222222224E-3</v>
       </c>
       <c r="R8" s="62">
         <f>NK!J18</f>
-        <v>1.995416666666667E-3</v>
+        <v>1.9787881944444445E-3</v>
       </c>
       <c r="S8" s="62">
         <f t="shared" si="5"/>
-        <v>5.6041666666666664E-4</v>
+        <v>5.5574652777777773E-4</v>
       </c>
       <c r="T8" s="62">
         <f t="shared" si="0"/>
-        <v>8.4444444444444443E-4</v>
+        <v>8.3740740740740737E-4</v>
       </c>
       <c r="U8" s="62">
         <f t="shared" si="1"/>
-        <v>1.1630555555555554E-3</v>
+        <v>1.153363425925926E-3</v>
       </c>
       <c r="V8" s="62">
         <f t="shared" si="2"/>
-        <v>9.3833333333333334E-4</v>
+        <v>9.3051388888888893E-4</v>
       </c>
       <c r="W8" s="62">
         <f t="shared" si="3"/>
-        <v>2.2183333333333334E-3</v>
+        <v>2.1998472222222224E-3</v>
       </c>
       <c r="X8" s="62">
         <f t="shared" si="4"/>
-        <v>1.995416666666667E-3</v>
+        <v>1.9787881944444445E-3</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.45">
@@ -14933,51 +14933,51 @@
       </c>
       <c r="M9" s="62">
         <f>NK!I14</f>
-        <v>5.7291666666666667E-4</v>
+        <v>5.6814236111111106E-4</v>
       </c>
       <c r="N9" s="62">
         <f>NK!I16</f>
-        <v>8.5972222222222222E-4</v>
+        <v>8.5255787037037038E-4</v>
       </c>
       <c r="O9" s="62">
         <f>NK!I15</f>
-        <v>1.2043055555555557E-3</v>
+        <v>1.1942696759259261E-3</v>
       </c>
       <c r="P9" s="62">
         <f>NK!I17</f>
-        <v>9.5722222222222226E-4</v>
+        <v>9.4924537037037037E-4</v>
       </c>
       <c r="Q9" s="62">
         <f>NK!I19</f>
-        <v>2.2669444444444443E-3</v>
+        <v>2.2480532407407406E-3</v>
       </c>
       <c r="R9" s="62">
         <f>NK!I18</f>
-        <v>2.0254166666666663E-3</v>
+        <v>2.0085381944444443E-3</v>
       </c>
       <c r="S9" s="62">
         <f t="shared" si="5"/>
-        <v>5.7291666666666667E-4</v>
+        <v>5.6814236111111106E-4</v>
       </c>
       <c r="T9" s="62">
         <f t="shared" si="0"/>
-        <v>8.5972222222222222E-4</v>
+        <v>8.5255787037037038E-4</v>
       </c>
       <c r="U9" s="62">
         <f t="shared" si="1"/>
-        <v>1.2043055555555557E-3</v>
+        <v>1.1942696759259261E-3</v>
       </c>
       <c r="V9" s="62">
         <f t="shared" si="2"/>
-        <v>9.5722222222222226E-4</v>
+        <v>9.4924537037037037E-4</v>
       </c>
       <c r="W9" s="62">
         <f t="shared" si="3"/>
-        <v>2.2669444444444443E-3</v>
+        <v>2.2480532407407406E-3</v>
       </c>
       <c r="X9" s="62">
         <f t="shared" si="4"/>
-        <v>2.0254166666666663E-3</v>
+        <v>2.0085381944444443E-3</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.45">
@@ -15015,51 +15015,51 @@
       </c>
       <c r="M10" s="62">
         <f>NK!$R$14</f>
-        <v>4.2249999999999997E-4</v>
+        <v>4.152777777777777E-4</v>
       </c>
       <c r="N10" s="62">
         <f>NK!$R$16</f>
-        <v>6.6895833333333325E-4</v>
+        <v>6.5752314814814807E-4</v>
       </c>
       <c r="O10" s="62">
         <f>NK!$R$15</f>
-        <v>9.0309374999999993E-4</v>
+        <v>8.8765624999999988E-4</v>
       </c>
       <c r="P10" s="62">
         <f>NK!$R$17</f>
-        <v>7.5034374999999982E-4</v>
+        <v>7.3751736111111099E-4</v>
       </c>
       <c r="Q10" s="62">
         <f>NK!$R$19</f>
-        <v>1.8793124999999999E-3</v>
+        <v>1.8471874999999999E-3</v>
       </c>
       <c r="R10" s="62">
         <f>NK!$R$18</f>
-        <v>1.7196562499999998E-3</v>
+        <v>1.6902604166666663E-3</v>
       </c>
       <c r="S10" s="62">
         <f>M10</f>
-        <v>4.2249999999999997E-4</v>
+        <v>4.152777777777777E-4</v>
       </c>
       <c r="T10" s="62">
         <f t="shared" ref="T10:T15" si="6">N10</f>
-        <v>6.6895833333333325E-4</v>
+        <v>6.5752314814814807E-4</v>
       </c>
       <c r="U10" s="62">
         <f t="shared" ref="U10:U15" si="7">O10</f>
-        <v>9.0309374999999993E-4</v>
+        <v>8.8765624999999988E-4</v>
       </c>
       <c r="V10" s="62">
         <f t="shared" ref="V10:V15" si="8">P10</f>
-        <v>7.5034374999999982E-4</v>
+        <v>7.3751736111111099E-4</v>
       </c>
       <c r="W10" s="62">
         <f t="shared" ref="W10:W15" si="9">Q10</f>
-        <v>1.8793124999999999E-3</v>
+        <v>1.8471874999999999E-3</v>
       </c>
       <c r="X10" s="62">
         <f t="shared" ref="X10:X15" si="10">R10</f>
-        <v>1.7196562499999998E-3</v>
+        <v>1.6902604166666663E-3</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.45">
@@ -15097,51 +15097,51 @@
       </c>
       <c r="M11" s="62">
         <f>NK!$S$14</f>
-        <v>4.1044791666666665E-4</v>
+        <v>4.0343171296296291E-4</v>
       </c>
       <c r="N11" s="62">
         <f>NK!$S$16</f>
-        <v>6.5121875E-4</v>
+        <v>6.4008680555555553E-4</v>
       </c>
       <c r="O11" s="62">
         <f>NK!$S$15</f>
-        <v>8.7438541666666654E-4</v>
+        <v>8.5943865740740729E-4</v>
       </c>
       <c r="P11" s="62">
         <f>NK!$S$17</f>
-        <v>7.2407291666666659E-4</v>
+        <v>7.116956018518517E-4</v>
       </c>
       <c r="Q11" s="62">
         <f>NK!$S$19</f>
-        <v>1.8610312499999998E-3</v>
+        <v>1.8292187499999999E-3</v>
       </c>
       <c r="R11" s="62">
         <f>NK!$S$18</f>
-        <v>1.6714479166666668E-3</v>
+        <v>1.6428761574074073E-3</v>
       </c>
       <c r="S11" s="62">
         <f t="shared" ref="S11:S15" si="11">M11</f>
-        <v>4.1044791666666665E-4</v>
+        <v>4.0343171296296291E-4</v>
       </c>
       <c r="T11" s="62">
         <f t="shared" si="6"/>
-        <v>6.5121875E-4</v>
+        <v>6.4008680555555553E-4</v>
       </c>
       <c r="U11" s="62">
         <f t="shared" si="7"/>
-        <v>8.7438541666666654E-4</v>
+        <v>8.5943865740740729E-4</v>
       </c>
       <c r="V11" s="62">
         <f t="shared" si="8"/>
-        <v>7.2407291666666659E-4</v>
+        <v>7.116956018518517E-4</v>
       </c>
       <c r="W11" s="62">
         <f t="shared" si="9"/>
-        <v>1.8610312499999998E-3</v>
+        <v>1.8292187499999999E-3</v>
       </c>
       <c r="X11" s="62">
         <f t="shared" si="10"/>
-        <v>1.6714479166666668E-3</v>
+        <v>1.6428761574074073E-3</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.45">
@@ -15179,51 +15179,51 @@
       </c>
       <c r="M12" s="62">
         <f>NK!$T$14</f>
-        <v>3.9663541666666666E-4</v>
+        <v>3.8985532407407404E-4</v>
       </c>
       <c r="N12" s="62">
         <f>NK!$T$16</f>
-        <v>6.3104166666666658E-4</v>
+        <v>6.2025462962962956E-4</v>
       </c>
       <c r="O12" s="62">
         <f>NK!$T$15</f>
-        <v>8.4147916666666659E-4</v>
+        <v>8.2709490740740736E-4</v>
       </c>
       <c r="P12" s="62">
         <f>NK!$T$17</f>
-        <v>6.9401041666666656E-4</v>
+        <v>6.8214699074074065E-4</v>
       </c>
       <c r="Q12" s="62">
         <f>NK!$T$19</f>
-        <v>1.8044270833333334E-3</v>
+        <v>1.7735821759259258E-3</v>
       </c>
       <c r="R12" s="62">
         <f>NK!$T$18</f>
-        <v>1.6164687499999999E-3</v>
+        <v>1.5888368055555554E-3</v>
       </c>
       <c r="S12" s="62">
         <f t="shared" si="11"/>
-        <v>3.9663541666666666E-4</v>
+        <v>3.8985532407407404E-4</v>
       </c>
       <c r="T12" s="62">
         <f t="shared" si="6"/>
-        <v>6.3104166666666658E-4</v>
+        <v>6.2025462962962956E-4</v>
       </c>
       <c r="U12" s="62">
         <f t="shared" si="7"/>
-        <v>8.4147916666666659E-4</v>
+        <v>8.2709490740740736E-4</v>
       </c>
       <c r="V12" s="62">
         <f t="shared" si="8"/>
-        <v>6.9401041666666656E-4</v>
+        <v>6.8214699074074065E-4</v>
       </c>
       <c r="W12" s="62">
         <f t="shared" si="9"/>
-        <v>1.8044270833333334E-3</v>
+        <v>1.7735821759259258E-3</v>
       </c>
       <c r="X12" s="62">
         <f t="shared" si="10"/>
-        <v>1.6164687499999999E-3</v>
+        <v>1.5888368055555554E-3</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.45">
@@ -15261,51 +15261,51 @@
       </c>
       <c r="M13" s="62">
         <f>NK!$X$14</f>
-        <v>5.2475694444444445E-4</v>
+        <v>5.1593750000000001E-4</v>
       </c>
       <c r="N13" s="62">
         <f>NK!$X$16</f>
-        <v>7.9925578703703712E-4</v>
+        <v>7.8582291666666666E-4</v>
       </c>
       <c r="O13" s="62">
         <f>NK!$X$15</f>
-        <v>1.0714131944444443E-3</v>
+        <v>1.0534062499999999E-3</v>
       </c>
       <c r="P13" s="62">
         <f>NK!$X$17</f>
-        <v>8.8368518518518505E-4</v>
+        <v>8.6883333333333322E-4</v>
       </c>
       <c r="Q13" s="62">
         <f>NK!$X$19</f>
-        <v>2.103159722222222E-3</v>
+        <v>2.0678124999999998E-3</v>
       </c>
       <c r="R13" s="62">
         <f>NK!$X$18</f>
-        <v>1.9194259259259262E-3</v>
+        <v>1.8871666666666668E-3</v>
       </c>
       <c r="S13" s="62">
         <f t="shared" si="11"/>
-        <v>5.2475694444444445E-4</v>
+        <v>5.1593750000000001E-4</v>
       </c>
       <c r="T13" s="62">
         <f t="shared" si="6"/>
-        <v>7.9925578703703712E-4</v>
+        <v>7.8582291666666666E-4</v>
       </c>
       <c r="U13" s="62">
         <f t="shared" si="7"/>
-        <v>1.0714131944444443E-3</v>
+        <v>1.0534062499999999E-3</v>
       </c>
       <c r="V13" s="62">
         <f t="shared" si="8"/>
-        <v>8.8368518518518505E-4</v>
+        <v>8.6883333333333322E-4</v>
       </c>
       <c r="W13" s="62">
         <f t="shared" si="9"/>
-        <v>2.103159722222222E-3</v>
+        <v>2.0678124999999998E-3</v>
       </c>
       <c r="X13" s="62">
         <f t="shared" si="10"/>
-        <v>1.9194259259259262E-3</v>
+        <v>1.8871666666666668E-3</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.45">
@@ -15343,51 +15343,51 @@
       </c>
       <c r="M14" s="62">
         <f>NK!$Y$14</f>
-        <v>5.0037847222222215E-4</v>
+        <v>4.9196875E-4</v>
       </c>
       <c r="N14" s="62">
         <f>NK!$Y$16</f>
-        <v>7.6867939814814811E-4</v>
+        <v>7.5576041666666662E-4</v>
       </c>
       <c r="O14" s="62">
         <f>NK!$Y$15</f>
-        <v>1.0229317129629629E-3</v>
+        <v>1.0057395833333333E-3</v>
       </c>
       <c r="P14" s="62">
         <f>NK!$Y$17</f>
-        <v>8.4649768518518516E-4</v>
+        <v>8.322708333333333E-4</v>
       </c>
       <c r="Q14" s="62">
         <f>NK!$Y$19</f>
-        <v>2.0437974537037035E-3</v>
+        <v>2.0094479166666663E-3</v>
       </c>
       <c r="R14" s="62">
         <f>NK!$Y$18</f>
-        <v>1.8822384259259259E-3</v>
+        <v>1.8506041666666664E-3</v>
       </c>
       <c r="S14" s="62">
         <f t="shared" si="11"/>
-        <v>5.0037847222222215E-4</v>
+        <v>4.9196875E-4</v>
       </c>
       <c r="T14" s="62">
         <f t="shared" si="6"/>
-        <v>7.6867939814814811E-4</v>
+        <v>7.5576041666666662E-4</v>
       </c>
       <c r="U14" s="62">
         <f t="shared" si="7"/>
-        <v>1.0229317129629629E-3</v>
+        <v>1.0057395833333333E-3</v>
       </c>
       <c r="V14" s="62">
         <f t="shared" si="8"/>
-        <v>8.4649768518518516E-4</v>
+        <v>8.322708333333333E-4</v>
       </c>
       <c r="W14" s="62">
         <f t="shared" si="9"/>
-        <v>2.0437974537037035E-3</v>
+        <v>2.0094479166666663E-3</v>
       </c>
       <c r="X14" s="62">
         <f t="shared" si="10"/>
-        <v>1.8822384259259259E-3</v>
+        <v>1.8506041666666664E-3</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.45">
@@ -15425,51 +15425,51 @@
       </c>
       <c r="M15" s="62">
         <f>NK!$Z$14</f>
-        <v>4.8247337962962957E-4</v>
+        <v>4.7436458333333331E-4</v>
       </c>
       <c r="N15" s="62">
         <f>NK!$Z$16</f>
-        <v>7.4636689814814813E-4</v>
+        <v>7.3382291666666659E-4</v>
       </c>
       <c r="O15" s="62">
         <f>NK!$Z$15</f>
-        <v>9.8739699074074073E-4</v>
+        <v>9.7080208333333328E-4</v>
       </c>
       <c r="P15" s="62">
         <f>NK!$Z$17</f>
-        <v>8.192268518518518E-4</v>
+        <v>8.0545833333333326E-4</v>
       </c>
       <c r="Q15" s="62">
         <f>NK!$Z$19</f>
-        <v>2.0004120370370371E-3</v>
+        <v>1.9667916666666666E-3</v>
       </c>
       <c r="R15" s="62">
         <f>NK!$Z$18</f>
-        <v>1.8551053240740739E-3</v>
+        <v>1.8239270833333332E-3</v>
       </c>
       <c r="S15" s="62">
         <f t="shared" si="11"/>
-        <v>4.8247337962962957E-4</v>
+        <v>4.7436458333333331E-4</v>
       </c>
       <c r="T15" s="62">
         <f t="shared" si="6"/>
-        <v>7.4636689814814813E-4</v>
+        <v>7.3382291666666659E-4</v>
       </c>
       <c r="U15" s="62">
         <f t="shared" si="7"/>
-        <v>9.8739699074074073E-4</v>
+        <v>9.7080208333333328E-4</v>
       </c>
       <c r="V15" s="62">
         <f t="shared" si="8"/>
-        <v>8.192268518518518E-4</v>
+        <v>8.0545833333333326E-4</v>
       </c>
       <c r="W15" s="62">
         <f t="shared" si="9"/>
-        <v>2.0004120370370371E-3</v>
+        <v>1.9667916666666666E-3</v>
       </c>
       <c r="X15" s="62">
         <f t="shared" si="10"/>
-        <v>1.8551053240740739E-3</v>
+        <v>1.8239270833333332E-3</v>
       </c>
     </row>
   </sheetData>
@@ -15740,7 +15740,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:H10">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$A2&lt;TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15756,7 +15756,7 @@
   <sheetPr codeName="Tabelle12"/>
   <dimension ref="B3:AA37"/>
   <sheetViews>
-    <sheetView topLeftCell="N5" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
       <selection activeCell="AA19" sqref="AA19"/>
     </sheetView>
   </sheetViews>
@@ -16220,72 +16220,72 @@
       </c>
       <c r="C14" s="65">
         <f>C5*$F14</f>
-        <v>4.6353240740740735E-4</v>
+        <v>4.6746064814814805E-4</v>
       </c>
       <c r="D14" s="65">
         <f t="shared" ref="D14:E14" si="0">D5*$F14</f>
-        <v>4.5424537037037037E-4</v>
+        <v>4.5809490740740739E-4</v>
       </c>
       <c r="E14" s="65">
         <f t="shared" si="0"/>
-        <v>4.4045138888888888E-4</v>
+        <v>4.4418402777777777E-4</v>
       </c>
       <c r="F14">
-        <v>1.18</v>
+        <v>1.19</v>
       </c>
       <c r="H14" s="64" t="s">
         <v>0</v>
       </c>
       <c r="I14" s="65">
         <f>I5*$L14</f>
-        <v>5.7291666666666667E-4</v>
+        <v>5.6814236111111106E-4</v>
       </c>
       <c r="J14" s="65">
         <f t="shared" ref="J14:K14" si="1">J5*$L14</f>
-        <v>5.6041666666666664E-4</v>
+        <v>5.5574652777777773E-4</v>
       </c>
       <c r="K14" s="65">
         <f t="shared" si="1"/>
-        <v>5.4694444444444441E-4</v>
+        <v>5.4238657407407404E-4</v>
       </c>
       <c r="L14">
-        <v>1.2</v>
+        <v>1.19</v>
       </c>
       <c r="Q14" s="64" t="s">
         <v>0</v>
       </c>
       <c r="R14" s="65">
         <f t="shared" ref="R14:T19" si="2">R5*$U14</f>
-        <v>4.2249999999999997E-4</v>
+        <v>4.152777777777777E-4</v>
       </c>
       <c r="S14" s="65">
         <f t="shared" si="2"/>
-        <v>4.1044791666666665E-4</v>
+        <v>4.0343171296296291E-4</v>
       </c>
       <c r="T14" s="65">
         <f t="shared" si="2"/>
-        <v>3.9663541666666666E-4</v>
+        <v>3.8985532407407404E-4</v>
       </c>
       <c r="U14">
-        <v>1.17</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="W14" s="64" t="s">
         <v>0</v>
       </c>
       <c r="X14" s="65">
         <f>X5*$AA14</f>
-        <v>5.2475694444444445E-4</v>
+        <v>5.1593750000000001E-4</v>
       </c>
       <c r="Y14" s="65">
         <f t="shared" ref="Y14:Z14" si="3">Y5*$AA14</f>
-        <v>5.0037847222222215E-4</v>
+        <v>4.9196875E-4</v>
       </c>
       <c r="Z14" s="65">
         <f t="shared" si="3"/>
-        <v>4.8247337962962957E-4</v>
+        <v>4.7436458333333331E-4</v>
       </c>
       <c r="AA14">
-        <v>1.19</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="15" spans="2:27" x14ac:dyDescent="0.45">
@@ -16294,72 +16294,72 @@
       </c>
       <c r="C15" s="65">
         <f t="shared" ref="C15:E15" si="4">C6*$F15</f>
-        <v>1.0006782407407406E-3</v>
+        <v>1.0091585648148147E-3</v>
       </c>
       <c r="D15" s="65">
         <f t="shared" si="4"/>
-        <v>9.8333333333333324E-4</v>
+        <v>9.9166666666666674E-4</v>
       </c>
       <c r="E15" s="65">
         <f t="shared" si="4"/>
-        <v>9.4522916666666681E-4</v>
+        <v>9.532395833333335E-4</v>
       </c>
       <c r="F15">
-        <v>1.18</v>
+        <v>1.19</v>
       </c>
       <c r="H15" s="64" t="s">
         <v>220</v>
       </c>
       <c r="I15" s="65">
         <f t="shared" ref="I15:K15" si="5">I6*$L15</f>
-        <v>1.2043055555555557E-3</v>
+        <v>1.1942696759259261E-3</v>
       </c>
       <c r="J15" s="65">
         <f t="shared" si="5"/>
-        <v>1.1630555555555554E-3</v>
+        <v>1.153363425925926E-3</v>
       </c>
       <c r="K15" s="65">
         <f t="shared" si="5"/>
-        <v>1.1216666666666666E-3</v>
+        <v>1.1123194444444444E-3</v>
       </c>
       <c r="L15">
-        <v>1.2</v>
+        <v>1.19</v>
       </c>
       <c r="Q15" s="64" t="s">
         <v>220</v>
       </c>
       <c r="R15" s="65">
         <f t="shared" si="2"/>
-        <v>9.0309374999999993E-4</v>
+        <v>8.8765624999999988E-4</v>
       </c>
       <c r="S15" s="65">
         <f t="shared" si="2"/>
-        <v>8.7438541666666654E-4</v>
+        <v>8.5943865740740729E-4</v>
       </c>
       <c r="T15" s="65">
         <f t="shared" si="2"/>
-        <v>8.4147916666666659E-4</v>
+        <v>8.2709490740740736E-4</v>
       </c>
       <c r="U15">
-        <v>1.17</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="W15" s="64" t="s">
         <v>220</v>
       </c>
       <c r="X15" s="65">
         <f t="shared" ref="X15:Z15" si="6">X6*$AA15</f>
-        <v>1.0714131944444443E-3</v>
+        <v>1.0534062499999999E-3</v>
       </c>
       <c r="Y15" s="65">
         <f t="shared" si="6"/>
-        <v>1.0229317129629629E-3</v>
+        <v>1.0057395833333333E-3</v>
       </c>
       <c r="Z15" s="65">
         <f t="shared" si="6"/>
-        <v>9.8739699074074073E-4</v>
+        <v>9.7080208333333328E-4</v>
       </c>
       <c r="AA15">
-        <v>1.19</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="16" spans="2:27" x14ac:dyDescent="0.45">
@@ -16368,72 +16368,72 @@
       </c>
       <c r="C16" s="65">
         <f t="shared" ref="C16:E16" si="7">C7*$F16</f>
-        <v>7.2916898148148146E-4</v>
+        <v>7.3534837962962963E-4</v>
       </c>
       <c r="D16" s="65">
         <f t="shared" si="7"/>
-        <v>7.1551157407407403E-4</v>
+        <v>7.2157523148148146E-4</v>
       </c>
       <c r="E16" s="65">
         <f t="shared" si="7"/>
-        <v>6.9557175925925928E-4</v>
+        <v>7.0146643518518518E-4</v>
       </c>
       <c r="F16">
-        <v>1.18</v>
+        <v>1.19</v>
       </c>
       <c r="H16" s="64" t="s">
         <v>221</v>
       </c>
       <c r="I16" s="65">
         <f t="shared" ref="I16:K16" si="8">I7*$L16</f>
-        <v>8.5972222222222222E-4</v>
+        <v>8.5255787037037038E-4</v>
       </c>
       <c r="J16" s="65">
         <f t="shared" si="8"/>
-        <v>8.4444444444444443E-4</v>
+        <v>8.3740740740740737E-4</v>
       </c>
       <c r="K16" s="65">
         <f t="shared" si="8"/>
-        <v>8.2777777777777786E-4</v>
+        <v>8.2087962962962963E-4</v>
       </c>
       <c r="L16">
-        <v>1.2</v>
+        <v>1.19</v>
       </c>
       <c r="Q16" s="64" t="s">
         <v>221</v>
       </c>
       <c r="R16" s="65">
         <f t="shared" si="2"/>
-        <v>6.6895833333333325E-4</v>
+        <v>6.5752314814814807E-4</v>
       </c>
       <c r="S16" s="65">
         <f t="shared" si="2"/>
-        <v>6.5121875E-4</v>
+        <v>6.4008680555555553E-4</v>
       </c>
       <c r="T16" s="65">
         <f t="shared" si="2"/>
-        <v>6.3104166666666658E-4</v>
+        <v>6.2025462962962956E-4</v>
       </c>
       <c r="U16">
-        <v>1.17</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="W16" s="64" t="s">
         <v>221</v>
       </c>
       <c r="X16" s="65">
         <f t="shared" ref="X16:Z16" si="9">X7*$AA16</f>
-        <v>7.9925578703703712E-4</v>
+        <v>7.8582291666666666E-4</v>
       </c>
       <c r="Y16" s="65">
         <f>Y7*$AA16</f>
-        <v>7.6867939814814811E-4</v>
+        <v>7.5576041666666662E-4</v>
       </c>
       <c r="Z16" s="65">
         <f t="shared" si="9"/>
-        <v>7.4636689814814813E-4</v>
+        <v>7.3382291666666659E-4</v>
       </c>
       <c r="AA16">
-        <v>1.19</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="17" spans="2:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -16442,72 +16442,72 @@
       </c>
       <c r="C17" s="65">
         <f t="shared" ref="C17:E17" si="10">C8*$F17</f>
-        <v>8.3952083333333329E-4</v>
+        <v>8.4663541666666665E-4</v>
       </c>
       <c r="D17" s="65">
         <f t="shared" si="10"/>
-        <v>8.1876157407407407E-4</v>
+        <v>8.2570023148148151E-4</v>
       </c>
       <c r="E17" s="65">
         <f t="shared" si="10"/>
-        <v>7.884421296296295E-4</v>
+        <v>7.951238425925925E-4</v>
       </c>
       <c r="F17">
-        <v>1.18</v>
+        <v>1.19</v>
       </c>
       <c r="H17" s="64" t="s">
         <v>222</v>
       </c>
       <c r="I17" s="65">
         <f t="shared" ref="I17:K17" si="11">I8*$L17</f>
-        <v>9.5722222222222226E-4</v>
+        <v>9.4924537037037037E-4</v>
       </c>
       <c r="J17" s="65">
         <f t="shared" si="11"/>
-        <v>9.3833333333333334E-4</v>
+        <v>9.3051388888888893E-4</v>
       </c>
       <c r="K17" s="65">
         <f t="shared" si="11"/>
-        <v>9.1791666666666671E-4</v>
+        <v>9.1026736111111115E-4</v>
       </c>
       <c r="L17">
-        <v>1.2</v>
+        <v>1.19</v>
       </c>
       <c r="Q17" s="64" t="s">
         <v>222</v>
       </c>
       <c r="R17" s="65">
         <f t="shared" si="2"/>
-        <v>7.5034374999999982E-4</v>
+        <v>7.3751736111111099E-4</v>
       </c>
       <c r="S17" s="65">
         <f t="shared" si="2"/>
-        <v>7.2407291666666659E-4</v>
+        <v>7.116956018518517E-4</v>
       </c>
       <c r="T17" s="65">
         <f t="shared" si="2"/>
-        <v>6.9401041666666656E-4</v>
+        <v>6.8214699074074065E-4</v>
       </c>
       <c r="U17">
-        <v>1.17</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="W17" s="64" t="s">
         <v>222</v>
       </c>
       <c r="X17" s="65">
         <f t="shared" ref="X17:Z17" si="12">X8*$AA17</f>
-        <v>8.8368518518518505E-4</v>
+        <v>8.6883333333333322E-4</v>
       </c>
       <c r="Y17" s="65">
         <f>Y8*$AA17</f>
-        <v>8.4649768518518516E-4</v>
+        <v>8.322708333333333E-4</v>
       </c>
       <c r="Z17" s="65">
         <f t="shared" si="12"/>
-        <v>8.192268518518518E-4</v>
+        <v>8.0545833333333326E-4</v>
       </c>
       <c r="AA17">
-        <v>1.19</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="18" spans="2:27" x14ac:dyDescent="0.45">
@@ -16516,72 +16516,72 @@
       </c>
       <c r="C18" s="65">
         <f t="shared" ref="C18:E18" si="13">C9*$F18</f>
-        <v>1.8833564814814815E-3</v>
+        <v>1.8993171296296297E-3</v>
       </c>
       <c r="D18" s="65">
         <f t="shared" si="13"/>
-        <v>1.8460717592592589E-3</v>
+        <v>1.8617164351851848E-3</v>
       </c>
       <c r="E18" s="65">
         <f t="shared" si="13"/>
-        <v>1.7914421296296294E-3</v>
+        <v>1.8066238425925923E-3</v>
       </c>
       <c r="F18">
-        <v>1.18</v>
+        <v>1.19</v>
       </c>
       <c r="H18" s="64" t="s">
         <v>223</v>
       </c>
       <c r="I18" s="65">
         <f t="shared" ref="I18:K18" si="14">I9*$L18</f>
-        <v>2.0254166666666663E-3</v>
+        <v>2.0085381944444443E-3</v>
       </c>
       <c r="J18" s="65">
         <f t="shared" si="14"/>
-        <v>1.995416666666667E-3</v>
+        <v>1.9787881944444445E-3</v>
       </c>
       <c r="K18" s="65">
         <f t="shared" si="14"/>
-        <v>1.9655555555555555E-3</v>
+        <v>1.9491759259259258E-3</v>
       </c>
       <c r="L18">
-        <v>1.2</v>
+        <v>1.19</v>
       </c>
       <c r="Q18" s="64" t="s">
         <v>223</v>
       </c>
       <c r="R18" s="65">
         <f t="shared" si="2"/>
-        <v>1.7196562499999998E-3</v>
+        <v>1.6902604166666663E-3</v>
       </c>
       <c r="S18" s="65">
         <f t="shared" si="2"/>
-        <v>1.6714479166666668E-3</v>
+        <v>1.6428761574074073E-3</v>
       </c>
       <c r="T18" s="65">
         <f t="shared" si="2"/>
-        <v>1.6164687499999999E-3</v>
+        <v>1.5888368055555554E-3</v>
       </c>
       <c r="U18">
-        <v>1.17</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="W18" s="64" t="s">
         <v>223</v>
       </c>
       <c r="X18" s="65">
         <f t="shared" ref="X18:Z18" si="15">X9*$AA18</f>
-        <v>1.9194259259259262E-3</v>
+        <v>1.8871666666666668E-3</v>
       </c>
       <c r="Y18" s="65">
         <f t="shared" si="15"/>
-        <v>1.8822384259259259E-3</v>
+        <v>1.8506041666666664E-3</v>
       </c>
       <c r="Z18" s="65">
         <f t="shared" si="15"/>
-        <v>1.8551053240740739E-3</v>
+        <v>1.8239270833333332E-3</v>
       </c>
       <c r="AA18">
-        <v>1.19</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="19" spans="2:27" x14ac:dyDescent="0.45">
@@ -16590,72 +16590,72 @@
       </c>
       <c r="C19" s="65">
         <f t="shared" ref="C19:E19" si="16">C10*$F19</f>
-        <v>2.067458333333333E-3</v>
+        <v>2.0849791666666664E-3</v>
       </c>
       <c r="D19" s="65">
         <f t="shared" si="16"/>
-        <v>2.0244374999999998E-3</v>
+        <v>2.04159375E-3</v>
       </c>
       <c r="E19" s="65">
         <f t="shared" si="16"/>
-        <v>1.961340277777778E-3</v>
+        <v>1.9779618055555557E-3</v>
       </c>
       <c r="F19">
-        <v>1.18</v>
+        <v>1.19</v>
       </c>
       <c r="H19" s="64" t="s">
         <v>4</v>
       </c>
       <c r="I19" s="65">
         <f t="shared" ref="I19:K19" si="17">I10*$L19</f>
-        <v>2.2669444444444443E-3</v>
+        <v>2.2480532407407406E-3</v>
       </c>
       <c r="J19" s="65">
         <f t="shared" si="17"/>
-        <v>2.2183333333333334E-3</v>
+        <v>2.1998472222222224E-3</v>
       </c>
       <c r="K19" s="65">
         <f t="shared" si="17"/>
-        <v>2.1695833333333333E-3</v>
+        <v>2.1515034722222222E-3</v>
       </c>
       <c r="L19">
-        <v>1.2</v>
+        <v>1.19</v>
       </c>
       <c r="Q19" s="64" t="s">
         <v>4</v>
       </c>
       <c r="R19" s="65">
         <f t="shared" si="2"/>
-        <v>1.8793124999999999E-3</v>
+        <v>1.8471874999999999E-3</v>
       </c>
       <c r="S19" s="65">
         <f t="shared" si="2"/>
-        <v>1.8610312499999998E-3</v>
+        <v>1.8292187499999999E-3</v>
       </c>
       <c r="T19" s="65">
         <f t="shared" si="2"/>
-        <v>1.8044270833333334E-3</v>
+        <v>1.7735821759259258E-3</v>
       </c>
       <c r="U19">
-        <v>1.17</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="W19" s="64" t="s">
         <v>4</v>
       </c>
       <c r="X19" s="65">
         <f t="shared" ref="X19:Z19" si="18">X10*$AA19</f>
-        <v>2.103159722222222E-3</v>
+        <v>2.0678124999999998E-3</v>
       </c>
       <c r="Y19" s="65">
         <f t="shared" si="18"/>
-        <v>2.0437974537037035E-3</v>
+        <v>2.0094479166666663E-3</v>
       </c>
       <c r="Z19" s="65">
         <f t="shared" si="18"/>
-        <v>2.0004120370370371E-3</v>
+        <v>1.9667916666666666E-3</v>
       </c>
       <c r="AA19">
-        <v>1.19</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="22" spans="2:27" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Angleich auf 6 / 8 verfeinern
</commit_message>
<xml_diff>
--- a/web/utilities/records_kriterien.xlsx
+++ b/web/utilities/records_kriterien.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgna\Documents\GitHub\Lifesaving_Baden\web\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAC86488-4D36-41B1-A12B-8C40F0C8E1EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35AEF5D4-4DE8-41E2-BB79-3D380449978C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="8" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="6" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
   </bookViews>
   <sheets>
     <sheet name="DR" sheetId="9" r:id="rId1"/>
@@ -1030,19 +1030,19 @@
     <t>Lara Ramackers, Lina Weidmann</t>
   </si>
   <si>
-    <t>NK2 +19% Mäner</t>
-  </si>
-  <si>
     <t>NK2 % W</t>
   </si>
   <si>
-    <t>NK2 +19% Frauen</t>
-  </si>
-  <si>
-    <t>NK1 +15% Mäner</t>
-  </si>
-  <si>
-    <t>NK1 +17% Frauen</t>
+    <t>NK1 +16% Frauen</t>
+  </si>
+  <si>
+    <t>NK1 +14% Mäner</t>
+  </si>
+  <si>
+    <t>NK2 +18% Frauen</t>
+  </si>
+  <si>
+    <t>NK2 +20% Mäner</t>
   </si>
 </sst>
 </file>
@@ -14245,8 +14245,8 @@
   </sheetPr>
   <dimension ref="A1:X15"/>
   <sheetViews>
-    <sheetView zoomScale="83" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -14493,7 +14493,7 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A4" s="59" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="B4" s="59" t="s">
         <v>182</v>
@@ -14526,56 +14526,56 @@
       </c>
       <c r="M4" s="62">
         <f>NK!E14</f>
-        <v>4.4418402777777777E-4</v>
+        <v>4.4791666666666667E-4</v>
       </c>
       <c r="N4" s="62">
         <f>NK!E16</f>
-        <v>7.0146643518518518E-4</v>
+        <v>7.0736111111111108E-4</v>
       </c>
       <c r="O4" s="62">
         <f>NK!E15</f>
-        <v>9.532395833333335E-4</v>
+        <v>9.6125000000000008E-4</v>
       </c>
       <c r="P4" s="62">
         <f>NK!E17</f>
-        <v>7.951238425925925E-4</v>
+        <v>8.018055555555555E-4</v>
       </c>
       <c r="Q4" s="62">
         <f>NK!E19</f>
-        <v>1.9779618055555557E-3</v>
+        <v>1.9945833333333335E-3</v>
       </c>
       <c r="R4" s="62">
         <f>NK!E18</f>
-        <v>1.8066238425925923E-3</v>
+        <v>1.8218055555555552E-3</v>
       </c>
       <c r="S4" s="62">
         <f>M4</f>
-        <v>4.4418402777777777E-4</v>
+        <v>4.4791666666666667E-4</v>
       </c>
       <c r="T4" s="62">
         <f t="shared" ref="T4:T9" si="0">N4</f>
-        <v>7.0146643518518518E-4</v>
+        <v>7.0736111111111108E-4</v>
       </c>
       <c r="U4" s="62">
         <f t="shared" ref="U4:U9" si="1">O4</f>
-        <v>9.532395833333335E-4</v>
+        <v>9.6125000000000008E-4</v>
       </c>
       <c r="V4" s="62">
         <f t="shared" ref="V4:V9" si="2">P4</f>
-        <v>7.951238425925925E-4</v>
+        <v>8.018055555555555E-4</v>
       </c>
       <c r="W4" s="62">
         <f t="shared" ref="W4:W9" si="3">Q4</f>
-        <v>1.9779618055555557E-3</v>
+        <v>1.9945833333333335E-3</v>
       </c>
       <c r="X4" s="62">
         <f t="shared" ref="X4:X9" si="4">R4</f>
-        <v>1.8066238425925923E-3</v>
+        <v>1.8218055555555552E-3</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A5" s="59" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="B5" s="59" t="s">
         <v>182</v>
@@ -14608,56 +14608,56 @@
       </c>
       <c r="M5" s="62">
         <f>NK!D14</f>
-        <v>4.5809490740740739E-4</v>
+        <v>4.619444444444444E-4</v>
       </c>
       <c r="N5" s="62">
         <f>NK!D16</f>
-        <v>7.2157523148148146E-4</v>
+        <v>7.2763888888888889E-4</v>
       </c>
       <c r="O5" s="62">
         <f>NK!D15</f>
-        <v>9.9166666666666674E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="P5" s="62">
         <f>NK!D17</f>
-        <v>8.2570023148148151E-4</v>
+        <v>8.3263888888888895E-4</v>
       </c>
       <c r="Q5" s="62">
         <f>NK!D19</f>
-        <v>2.04159375E-3</v>
+        <v>2.0587499999999998E-3</v>
       </c>
       <c r="R5" s="62">
         <f>NK!D18</f>
-        <v>1.8617164351851848E-3</v>
+        <v>1.8773611111111107E-3</v>
       </c>
       <c r="S5" s="62">
         <f t="shared" ref="S5:S9" si="5">M5</f>
-        <v>4.5809490740740739E-4</v>
+        <v>4.619444444444444E-4</v>
       </c>
       <c r="T5" s="62">
         <f t="shared" si="0"/>
-        <v>7.2157523148148146E-4</v>
+        <v>7.2763888888888889E-4</v>
       </c>
       <c r="U5" s="62">
         <f t="shared" si="1"/>
-        <v>9.9166666666666674E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="V5" s="62">
         <f t="shared" si="2"/>
-        <v>8.2570023148148151E-4</v>
+        <v>8.3263888888888895E-4</v>
       </c>
       <c r="W5" s="62">
         <f t="shared" si="3"/>
-        <v>2.04159375E-3</v>
+        <v>2.0587499999999998E-3</v>
       </c>
       <c r="X5" s="62">
         <f t="shared" si="4"/>
-        <v>1.8617164351851848E-3</v>
+        <v>1.8773611111111107E-3</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A6" s="59" t="s">
-        <v>269</v>
+        <v>273</v>
       </c>
       <c r="B6" s="59" t="s">
         <v>182</v>
@@ -14690,56 +14690,56 @@
       </c>
       <c r="M6" s="62">
         <f>NK!C14</f>
-        <v>4.6746064814814805E-4</v>
+        <v>4.7138888888888881E-4</v>
       </c>
       <c r="N6" s="62">
         <f>NK!C16</f>
-        <v>7.3534837962962963E-4</v>
+        <v>7.415277777777778E-4</v>
       </c>
       <c r="O6" s="62">
         <f>NK!C15</f>
-        <v>1.0091585648148147E-3</v>
+        <v>1.0176388888888889E-3</v>
       </c>
       <c r="P6" s="62">
         <f>NK!C17</f>
-        <v>8.4663541666666665E-4</v>
+        <v>8.5375000000000002E-4</v>
       </c>
       <c r="Q6" s="62">
         <f>NK!C19</f>
-        <v>2.0849791666666664E-3</v>
+        <v>2.1024999999999998E-3</v>
       </c>
       <c r="R6" s="62">
         <f>NK!C18</f>
-        <v>1.8993171296296297E-3</v>
+        <v>1.9152777777777779E-3</v>
       </c>
       <c r="S6" s="62">
         <f t="shared" si="5"/>
-        <v>4.6746064814814805E-4</v>
+        <v>4.7138888888888881E-4</v>
       </c>
       <c r="T6" s="62">
         <f t="shared" si="0"/>
-        <v>7.3534837962962963E-4</v>
+        <v>7.415277777777778E-4</v>
       </c>
       <c r="U6" s="62">
         <f t="shared" si="1"/>
-        <v>1.0091585648148147E-3</v>
+        <v>1.0176388888888889E-3</v>
       </c>
       <c r="V6" s="62">
         <f t="shared" si="2"/>
-        <v>8.4663541666666665E-4</v>
+        <v>8.5375000000000002E-4</v>
       </c>
       <c r="W6" s="62">
         <f t="shared" si="3"/>
-        <v>2.0849791666666664E-3</v>
+        <v>2.1024999999999998E-3</v>
       </c>
       <c r="X6" s="62">
         <f t="shared" si="4"/>
-        <v>1.8993171296296297E-3</v>
+        <v>1.9152777777777779E-3</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A7" s="59" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B7" s="59" t="s">
         <v>164</v>
@@ -14772,56 +14772,56 @@
       </c>
       <c r="M7" s="62">
         <f>NK!K14</f>
-        <v>5.4238657407407404E-4</v>
+        <v>8.2041666666666667E-4</v>
       </c>
       <c r="N7" s="62">
         <f>NK!K16</f>
-        <v>8.2087962962962963E-4</v>
+        <v>1.2416666666666667E-3</v>
       </c>
       <c r="O7" s="62">
         <f>NK!K15</f>
-        <v>1.1123194444444444E-3</v>
+        <v>1.6825000000000002E-3</v>
       </c>
       <c r="P7" s="62">
         <f>NK!K17</f>
-        <v>9.1026736111111115E-4</v>
+        <v>1.3768750000000001E-3</v>
       </c>
       <c r="Q7" s="62">
         <f>NK!K19</f>
-        <v>2.1515034722222222E-3</v>
+        <v>3.2543749999999999E-3</v>
       </c>
       <c r="R7" s="62">
         <f>NK!K18</f>
-        <v>1.9491759259259258E-3</v>
+        <v>2.9483333333333336E-3</v>
       </c>
       <c r="S7" s="62">
         <f t="shared" si="5"/>
-        <v>5.4238657407407404E-4</v>
+        <v>8.2041666666666667E-4</v>
       </c>
       <c r="T7" s="62">
         <f t="shared" si="0"/>
-        <v>8.2087962962962963E-4</v>
+        <v>1.2416666666666667E-3</v>
       </c>
       <c r="U7" s="62">
         <f t="shared" si="1"/>
-        <v>1.1123194444444444E-3</v>
+        <v>1.6825000000000002E-3</v>
       </c>
       <c r="V7" s="62">
         <f t="shared" si="2"/>
-        <v>9.1026736111111115E-4</v>
+        <v>1.3768750000000001E-3</v>
       </c>
       <c r="W7" s="62">
         <f t="shared" si="3"/>
-        <v>2.1515034722222222E-3</v>
+        <v>3.2543749999999999E-3</v>
       </c>
       <c r="X7" s="62">
         <f t="shared" si="4"/>
-        <v>1.9491759259259258E-3</v>
+        <v>2.9483333333333336E-3</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A8" s="59" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B8" s="59" t="s">
         <v>164</v>
@@ -14854,56 +14854,56 @@
       </c>
       <c r="M8" s="62">
         <f>NK!J14</f>
-        <v>5.5574652777777773E-4</v>
+        <v>8.4062500000000001E-4</v>
       </c>
       <c r="N8" s="62">
         <f>NK!J16</f>
-        <v>8.3740740740740737E-4</v>
+        <v>1.2666666666666666E-3</v>
       </c>
       <c r="O8" s="62">
         <f>NK!J15</f>
-        <v>1.153363425925926E-3</v>
+        <v>1.7445833333333334E-3</v>
       </c>
       <c r="P8" s="62">
         <f>NK!J17</f>
-        <v>9.3051388888888893E-4</v>
+        <v>1.4075000000000001E-3</v>
       </c>
       <c r="Q8" s="62">
         <f>NK!J19</f>
-        <v>2.1998472222222224E-3</v>
+        <v>3.3275000000000002E-3</v>
       </c>
       <c r="R8" s="62">
         <f>NK!J18</f>
-        <v>1.9787881944444445E-3</v>
+        <v>2.9931250000000006E-3</v>
       </c>
       <c r="S8" s="62">
         <f t="shared" si="5"/>
-        <v>5.5574652777777773E-4</v>
+        <v>8.4062500000000001E-4</v>
       </c>
       <c r="T8" s="62">
         <f t="shared" si="0"/>
-        <v>8.3740740740740737E-4</v>
+        <v>1.2666666666666666E-3</v>
       </c>
       <c r="U8" s="62">
         <f t="shared" si="1"/>
-        <v>1.153363425925926E-3</v>
+        <v>1.7445833333333334E-3</v>
       </c>
       <c r="V8" s="62">
         <f t="shared" si="2"/>
-        <v>9.3051388888888893E-4</v>
+        <v>1.4075000000000001E-3</v>
       </c>
       <c r="W8" s="62">
         <f t="shared" si="3"/>
-        <v>2.1998472222222224E-3</v>
+        <v>3.3275000000000002E-3</v>
       </c>
       <c r="X8" s="62">
         <f t="shared" si="4"/>
-        <v>1.9787881944444445E-3</v>
+        <v>2.9931250000000006E-3</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A9" s="59" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B9" s="59" t="s">
         <v>164</v>
@@ -14936,56 +14936,56 @@
       </c>
       <c r="M9" s="62">
         <f>NK!I14</f>
-        <v>5.6814236111111106E-4</v>
+        <v>8.59375E-4</v>
       </c>
       <c r="N9" s="62">
         <f>NK!I16</f>
-        <v>8.5255787037037038E-4</v>
+        <v>1.2895833333333333E-3</v>
       </c>
       <c r="O9" s="62">
         <f>NK!I15</f>
-        <v>1.1942696759259261E-3</v>
+        <v>1.8064583333333335E-3</v>
       </c>
       <c r="P9" s="62">
         <f>NK!I17</f>
-        <v>9.4924537037037037E-4</v>
+        <v>1.4358333333333334E-3</v>
       </c>
       <c r="Q9" s="62">
         <f>NK!I19</f>
-        <v>2.2480532407407406E-3</v>
+        <v>3.400416666666667E-3</v>
       </c>
       <c r="R9" s="62">
         <f>NK!I18</f>
-        <v>2.0085381944444443E-3</v>
+        <v>3.038125E-3</v>
       </c>
       <c r="S9" s="62">
         <f t="shared" si="5"/>
-        <v>5.6814236111111106E-4</v>
+        <v>8.59375E-4</v>
       </c>
       <c r="T9" s="62">
         <f t="shared" si="0"/>
-        <v>8.5255787037037038E-4</v>
+        <v>1.2895833333333333E-3</v>
       </c>
       <c r="U9" s="62">
         <f t="shared" si="1"/>
-        <v>1.1942696759259261E-3</v>
+        <v>1.8064583333333335E-3</v>
       </c>
       <c r="V9" s="62">
         <f t="shared" si="2"/>
-        <v>9.4924537037037037E-4</v>
+        <v>1.4358333333333334E-3</v>
       </c>
       <c r="W9" s="62">
         <f t="shared" si="3"/>
-        <v>2.2480532407407406E-3</v>
+        <v>3.400416666666667E-3</v>
       </c>
       <c r="X9" s="62">
         <f t="shared" si="4"/>
-        <v>2.0085381944444443E-3</v>
+        <v>3.038125E-3</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A10" s="59" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B10" s="59" t="s">
         <v>182</v>
@@ -15018,56 +15018,56 @@
       </c>
       <c r="M10" s="62">
         <f>NK!$R$14</f>
-        <v>4.152777777777777E-4</v>
+        <v>4.1166666666666663E-4</v>
       </c>
       <c r="N10" s="62">
         <f>NK!$R$16</f>
-        <v>6.5752314814814807E-4</v>
+        <v>6.5180555555555554E-4</v>
       </c>
       <c r="O10" s="62">
         <f>NK!$R$15</f>
-        <v>8.8765624999999988E-4</v>
+        <v>8.7993749999999997E-4</v>
       </c>
       <c r="P10" s="62">
         <f>NK!$R$17</f>
-        <v>7.3751736111111099E-4</v>
+        <v>7.3110416666666647E-4</v>
       </c>
       <c r="Q10" s="62">
         <f>NK!$R$19</f>
-        <v>1.8471874999999999E-3</v>
+        <v>1.8311249999999999E-3</v>
       </c>
       <c r="R10" s="62">
         <f>NK!$R$18</f>
-        <v>1.6902604166666663E-3</v>
+        <v>1.6755624999999998E-3</v>
       </c>
       <c r="S10" s="62">
         <f>M10</f>
-        <v>4.152777777777777E-4</v>
+        <v>4.1166666666666663E-4</v>
       </c>
       <c r="T10" s="62">
         <f t="shared" ref="T10:T15" si="6">N10</f>
-        <v>6.5752314814814807E-4</v>
+        <v>6.5180555555555554E-4</v>
       </c>
       <c r="U10" s="62">
         <f t="shared" ref="U10:U15" si="7">O10</f>
-        <v>8.8765624999999988E-4</v>
+        <v>8.7993749999999997E-4</v>
       </c>
       <c r="V10" s="62">
         <f t="shared" ref="V10:V15" si="8">P10</f>
-        <v>7.3751736111111099E-4</v>
+        <v>7.3110416666666647E-4</v>
       </c>
       <c r="W10" s="62">
         <f t="shared" ref="W10:W15" si="9">Q10</f>
-        <v>1.8471874999999999E-3</v>
+        <v>1.8311249999999999E-3</v>
       </c>
       <c r="X10" s="62">
         <f t="shared" ref="X10:X15" si="10">R10</f>
-        <v>1.6902604166666663E-3</v>
+        <v>1.6755624999999998E-3</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A11" s="59" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B11" s="59" t="s">
         <v>182</v>
@@ -15100,56 +15100,56 @@
       </c>
       <c r="M11" s="62">
         <f>NK!$S$14</f>
-        <v>4.0343171296296291E-4</v>
+        <v>3.9992361111111104E-4</v>
       </c>
       <c r="N11" s="62">
         <f>NK!$S$16</f>
-        <v>6.4008680555555553E-4</v>
+        <v>6.3452083333333329E-4</v>
       </c>
       <c r="O11" s="62">
         <f>NK!$S$15</f>
-        <v>8.5943865740740729E-4</v>
+        <v>8.5196527777777766E-4</v>
       </c>
       <c r="P11" s="62">
         <f>NK!$S$17</f>
-        <v>7.116956018518517E-4</v>
+        <v>7.0550694444444437E-4</v>
       </c>
       <c r="Q11" s="62">
         <f>NK!$S$19</f>
-        <v>1.8292187499999999E-3</v>
+        <v>1.8133124999999998E-3</v>
       </c>
       <c r="R11" s="62">
         <f>NK!$S$18</f>
-        <v>1.6428761574074073E-3</v>
+        <v>1.6285902777777778E-3</v>
       </c>
       <c r="S11" s="62">
         <f t="shared" ref="S11:S15" si="11">M11</f>
-        <v>4.0343171296296291E-4</v>
+        <v>3.9992361111111104E-4</v>
       </c>
       <c r="T11" s="62">
         <f t="shared" si="6"/>
-        <v>6.4008680555555553E-4</v>
+        <v>6.3452083333333329E-4</v>
       </c>
       <c r="U11" s="62">
         <f t="shared" si="7"/>
-        <v>8.5943865740740729E-4</v>
+        <v>8.5196527777777766E-4</v>
       </c>
       <c r="V11" s="62">
         <f t="shared" si="8"/>
-        <v>7.116956018518517E-4</v>
+        <v>7.0550694444444437E-4</v>
       </c>
       <c r="W11" s="62">
         <f t="shared" si="9"/>
-        <v>1.8292187499999999E-3</v>
+        <v>1.8133124999999998E-3</v>
       </c>
       <c r="X11" s="62">
         <f t="shared" si="10"/>
-        <v>1.6428761574074073E-3</v>
+        <v>1.6285902777777778E-3</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A12" s="59" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B12" s="59" t="s">
         <v>182</v>
@@ -15182,56 +15182,56 @@
       </c>
       <c r="M12" s="62">
         <f>NK!$T$14</f>
-        <v>3.8985532407407404E-4</v>
+        <v>3.8646527777777773E-4</v>
       </c>
       <c r="N12" s="62">
         <f>NK!$T$16</f>
-        <v>6.2025462962962956E-4</v>
+        <v>6.1486111111111106E-4</v>
       </c>
       <c r="O12" s="62">
         <f>NK!$T$15</f>
-        <v>8.2709490740740736E-4</v>
+        <v>8.1990277777777769E-4</v>
       </c>
       <c r="P12" s="62">
         <f>NK!$T$17</f>
-        <v>6.8214699074074065E-4</v>
+        <v>6.7621527777777775E-4</v>
       </c>
       <c r="Q12" s="62">
         <f>NK!$T$19</f>
-        <v>1.7735821759259258E-3</v>
+        <v>1.7581597222222222E-3</v>
       </c>
       <c r="R12" s="62">
         <f>NK!$T$18</f>
-        <v>1.5888368055555554E-3</v>
+        <v>1.5750208333333332E-3</v>
       </c>
       <c r="S12" s="62">
         <f t="shared" si="11"/>
-        <v>3.8985532407407404E-4</v>
+        <v>3.8646527777777773E-4</v>
       </c>
       <c r="T12" s="62">
         <f t="shared" si="6"/>
-        <v>6.2025462962962956E-4</v>
+        <v>6.1486111111111106E-4</v>
       </c>
       <c r="U12" s="62">
         <f t="shared" si="7"/>
-        <v>8.2709490740740736E-4</v>
+        <v>8.1990277777777769E-4</v>
       </c>
       <c r="V12" s="62">
         <f t="shared" si="8"/>
-        <v>6.8214699074074065E-4</v>
+        <v>6.7621527777777775E-4</v>
       </c>
       <c r="W12" s="62">
         <f t="shared" si="9"/>
-        <v>1.7735821759259258E-3</v>
+        <v>1.7581597222222222E-3</v>
       </c>
       <c r="X12" s="62">
         <f t="shared" si="10"/>
-        <v>1.5888368055555554E-3</v>
+        <v>1.5750208333333332E-3</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A13" s="59" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B13" s="59" t="s">
         <v>164</v>
@@ -15264,56 +15264,56 @@
       </c>
       <c r="M13" s="62">
         <f>NK!$X$14</f>
-        <v>5.1593750000000001E-4</v>
+        <v>5.1152777777777774E-4</v>
       </c>
       <c r="N13" s="62">
         <f>NK!$X$16</f>
-        <v>7.8582291666666666E-4</v>
+        <v>7.7910648148148153E-4</v>
       </c>
       <c r="O13" s="62">
         <f>NK!$X$15</f>
-        <v>1.0534062499999999E-3</v>
+        <v>1.0444027777777776E-3</v>
       </c>
       <c r="P13" s="62">
         <f>NK!$X$17</f>
-        <v>8.6883333333333322E-4</v>
+        <v>8.614074074074073E-4</v>
       </c>
       <c r="Q13" s="62">
         <f>NK!$X$19</f>
-        <v>2.0678124999999998E-3</v>
+        <v>2.0501388888888887E-3</v>
       </c>
       <c r="R13" s="62">
         <f>NK!$X$18</f>
-        <v>1.8871666666666668E-3</v>
+        <v>1.8710370370370372E-3</v>
       </c>
       <c r="S13" s="62">
         <f t="shared" si="11"/>
-        <v>5.1593750000000001E-4</v>
+        <v>5.1152777777777774E-4</v>
       </c>
       <c r="T13" s="62">
         <f t="shared" si="6"/>
-        <v>7.8582291666666666E-4</v>
+        <v>7.7910648148148153E-4</v>
       </c>
       <c r="U13" s="62">
         <f t="shared" si="7"/>
-        <v>1.0534062499999999E-3</v>
+        <v>1.0444027777777776E-3</v>
       </c>
       <c r="V13" s="62">
         <f t="shared" si="8"/>
-        <v>8.6883333333333322E-4</v>
+        <v>8.614074074074073E-4</v>
       </c>
       <c r="W13" s="62">
         <f t="shared" si="9"/>
-        <v>2.0678124999999998E-3</v>
+        <v>2.0501388888888887E-3</v>
       </c>
       <c r="X13" s="62">
         <f t="shared" si="10"/>
-        <v>1.8871666666666668E-3</v>
+        <v>1.8710370370370372E-3</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A14" s="59" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B14" s="59" t="s">
         <v>164</v>
@@ -15346,56 +15346,56 @@
       </c>
       <c r="M14" s="62">
         <f>NK!$Y$14</f>
-        <v>4.9196875E-4</v>
+        <v>4.8776388888888887E-4</v>
       </c>
       <c r="N14" s="62">
         <f>NK!$Y$16</f>
-        <v>7.5576041666666662E-4</v>
+        <v>7.4930092592592583E-4</v>
       </c>
       <c r="O14" s="62">
         <f>NK!$Y$15</f>
-        <v>1.0057395833333333E-3</v>
+        <v>9.9714351851851852E-4</v>
       </c>
       <c r="P14" s="62">
         <f>NK!$Y$17</f>
-        <v>8.322708333333333E-4</v>
+        <v>8.2515740740740737E-4</v>
       </c>
       <c r="Q14" s="62">
         <f>NK!$Y$19</f>
-        <v>2.0094479166666663E-3</v>
+        <v>1.992273148148148E-3</v>
       </c>
       <c r="R14" s="62">
         <f>NK!$Y$18</f>
-        <v>1.8506041666666664E-3</v>
+        <v>1.8347870370370369E-3</v>
       </c>
       <c r="S14" s="62">
         <f t="shared" si="11"/>
-        <v>4.9196875E-4</v>
+        <v>4.8776388888888887E-4</v>
       </c>
       <c r="T14" s="62">
         <f t="shared" si="6"/>
-        <v>7.5576041666666662E-4</v>
+        <v>7.4930092592592583E-4</v>
       </c>
       <c r="U14" s="62">
         <f t="shared" si="7"/>
-        <v>1.0057395833333333E-3</v>
+        <v>9.9714351851851852E-4</v>
       </c>
       <c r="V14" s="62">
         <f t="shared" si="8"/>
-        <v>8.322708333333333E-4</v>
+        <v>8.2515740740740737E-4</v>
       </c>
       <c r="W14" s="62">
         <f t="shared" si="9"/>
-        <v>2.0094479166666663E-3</v>
+        <v>1.992273148148148E-3</v>
       </c>
       <c r="X14" s="62">
         <f t="shared" si="10"/>
-        <v>1.8506041666666664E-3</v>
+        <v>1.8347870370370369E-3</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A15" s="59" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B15" s="59" t="s">
         <v>164</v>
@@ -15428,51 +15428,51 @@
       </c>
       <c r="M15" s="62">
         <f>NK!$Z$14</f>
-        <v>4.7436458333333331E-4</v>
+        <v>4.7031018518518515E-4</v>
       </c>
       <c r="N15" s="62">
         <f>NK!$Z$16</f>
-        <v>7.3382291666666659E-4</v>
+        <v>7.2755092592592587E-4</v>
       </c>
       <c r="O15" s="62">
         <f>NK!$Z$15</f>
-        <v>9.7080208333333328E-4</v>
+        <v>9.6250462962962956E-4</v>
       </c>
       <c r="P15" s="62">
         <f>NK!$Z$17</f>
-        <v>8.0545833333333326E-4</v>
+        <v>7.9857407407407394E-4</v>
       </c>
       <c r="Q15" s="62">
         <f>NK!$Z$19</f>
-        <v>1.9667916666666666E-3</v>
+        <v>1.9499814814814814E-3</v>
       </c>
       <c r="R15" s="62">
         <f>NK!$Z$18</f>
-        <v>1.8239270833333332E-3</v>
+        <v>1.8083379629629628E-3</v>
       </c>
       <c r="S15" s="62">
         <f t="shared" si="11"/>
-        <v>4.7436458333333331E-4</v>
+        <v>4.7031018518518515E-4</v>
       </c>
       <c r="T15" s="62">
         <f t="shared" si="6"/>
-        <v>7.3382291666666659E-4</v>
+        <v>7.2755092592592587E-4</v>
       </c>
       <c r="U15" s="62">
         <f t="shared" si="7"/>
-        <v>9.7080208333333328E-4</v>
+        <v>9.6250462962962956E-4</v>
       </c>
       <c r="V15" s="62">
         <f t="shared" si="8"/>
-        <v>8.0545833333333326E-4</v>
+        <v>7.9857407407407394E-4</v>
       </c>
       <c r="W15" s="62">
         <f t="shared" si="9"/>
-        <v>1.9667916666666666E-3</v>
+        <v>1.9499814814814814E-3</v>
       </c>
       <c r="X15" s="62">
         <f t="shared" si="10"/>
-        <v>1.8239270833333332E-3</v>
+        <v>1.8083379629629628E-3</v>
       </c>
     </row>
   </sheetData>
@@ -15759,8 +15759,8 @@
   <sheetPr codeName="Tabelle12"/>
   <dimension ref="B3:AA37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="AA19" sqref="AA19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -16158,7 +16158,7 @@
         <v>227</v>
       </c>
       <c r="H12" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="Q12" t="s">
         <v>230</v>
@@ -16223,72 +16223,72 @@
       </c>
       <c r="C14" s="65">
         <f>C5*$F14</f>
-        <v>4.6746064814814805E-4</v>
+        <v>4.7138888888888881E-4</v>
       </c>
       <c r="D14" s="65">
         <f t="shared" ref="D14:E14" si="0">D5*$F14</f>
-        <v>4.5809490740740739E-4</v>
+        <v>4.619444444444444E-4</v>
       </c>
       <c r="E14" s="65">
         <f t="shared" si="0"/>
-        <v>4.4418402777777777E-4</v>
+        <v>4.4791666666666667E-4</v>
       </c>
       <c r="F14">
-        <v>1.19</v>
+        <v>1.2</v>
       </c>
       <c r="H14" s="64" t="s">
         <v>0</v>
       </c>
       <c r="I14" s="65">
         <f>I5*$L14</f>
-        <v>5.6814236111111106E-4</v>
+        <v>8.59375E-4</v>
       </c>
       <c r="J14" s="65">
         <f t="shared" ref="J14:K14" si="1">J5*$L14</f>
-        <v>5.5574652777777773E-4</v>
+        <v>8.4062500000000001E-4</v>
       </c>
       <c r="K14" s="65">
         <f t="shared" si="1"/>
-        <v>5.4238657407407404E-4</v>
+        <v>8.2041666666666667E-4</v>
       </c>
       <c r="L14">
-        <v>1.19</v>
+        <v>1.8</v>
       </c>
       <c r="Q14" s="64" t="s">
         <v>0</v>
       </c>
       <c r="R14" s="65">
         <f t="shared" ref="R14:T19" si="2">R5*$U14</f>
-        <v>4.152777777777777E-4</v>
+        <v>4.1166666666666663E-4</v>
       </c>
       <c r="S14" s="65">
         <f t="shared" si="2"/>
-        <v>4.0343171296296291E-4</v>
+        <v>3.9992361111111104E-4</v>
       </c>
       <c r="T14" s="65">
         <f t="shared" si="2"/>
-        <v>3.8985532407407404E-4</v>
+        <v>3.8646527777777773E-4</v>
       </c>
       <c r="U14">
-        <v>1.1499999999999999</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="W14" s="64" t="s">
         <v>0</v>
       </c>
       <c r="X14" s="65">
         <f>X5*$AA14</f>
-        <v>5.1593750000000001E-4</v>
+        <v>5.1152777777777774E-4</v>
       </c>
       <c r="Y14" s="65">
         <f t="shared" ref="Y14:Z14" si="3">Y5*$AA14</f>
-        <v>4.9196875E-4</v>
+        <v>4.8776388888888887E-4</v>
       </c>
       <c r="Z14" s="65">
         <f t="shared" si="3"/>
-        <v>4.7436458333333331E-4</v>
+        <v>4.7031018518518515E-4</v>
       </c>
       <c r="AA14">
-        <v>1.17</v>
+        <v>1.1599999999999999</v>
       </c>
     </row>
     <row r="15" spans="2:27" x14ac:dyDescent="0.45">
@@ -16297,72 +16297,72 @@
       </c>
       <c r="C15" s="65">
         <f t="shared" ref="C15:E15" si="4">C6*$F15</f>
-        <v>1.0091585648148147E-3</v>
+        <v>1.0176388888888889E-3</v>
       </c>
       <c r="D15" s="65">
         <f t="shared" si="4"/>
-        <v>9.9166666666666674E-4</v>
+        <v>1E-3</v>
       </c>
       <c r="E15" s="65">
         <f t="shared" si="4"/>
-        <v>9.532395833333335E-4</v>
+        <v>9.6125000000000008E-4</v>
       </c>
       <c r="F15">
-        <v>1.19</v>
+        <v>1.2</v>
       </c>
       <c r="H15" s="64" t="s">
         <v>220</v>
       </c>
       <c r="I15" s="65">
         <f t="shared" ref="I15:K15" si="5">I6*$L15</f>
-        <v>1.1942696759259261E-3</v>
+        <v>1.8064583333333335E-3</v>
       </c>
       <c r="J15" s="65">
         <f t="shared" si="5"/>
-        <v>1.153363425925926E-3</v>
+        <v>1.7445833333333334E-3</v>
       </c>
       <c r="K15" s="65">
         <f t="shared" si="5"/>
-        <v>1.1123194444444444E-3</v>
+        <v>1.6825000000000002E-3</v>
       </c>
       <c r="L15">
-        <v>1.19</v>
+        <v>1.8</v>
       </c>
       <c r="Q15" s="64" t="s">
         <v>220</v>
       </c>
       <c r="R15" s="65">
         <f t="shared" si="2"/>
-        <v>8.8765624999999988E-4</v>
+        <v>8.7993749999999997E-4</v>
       </c>
       <c r="S15" s="65">
         <f t="shared" si="2"/>
-        <v>8.5943865740740729E-4</v>
+        <v>8.5196527777777766E-4</v>
       </c>
       <c r="T15" s="65">
         <f t="shared" si="2"/>
-        <v>8.2709490740740736E-4</v>
+        <v>8.1990277777777769E-4</v>
       </c>
       <c r="U15">
-        <v>1.1499999999999999</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="W15" s="64" t="s">
         <v>220</v>
       </c>
       <c r="X15" s="65">
         <f t="shared" ref="X15:Z15" si="6">X6*$AA15</f>
-        <v>1.0534062499999999E-3</v>
+        <v>1.0444027777777776E-3</v>
       </c>
       <c r="Y15" s="65">
         <f t="shared" si="6"/>
-        <v>1.0057395833333333E-3</v>
+        <v>9.9714351851851852E-4</v>
       </c>
       <c r="Z15" s="65">
         <f t="shared" si="6"/>
-        <v>9.7080208333333328E-4</v>
+        <v>9.6250462962962956E-4</v>
       </c>
       <c r="AA15">
-        <v>1.17</v>
+        <v>1.1599999999999999</v>
       </c>
     </row>
     <row r="16" spans="2:27" x14ac:dyDescent="0.45">
@@ -16371,72 +16371,72 @@
       </c>
       <c r="C16" s="65">
         <f t="shared" ref="C16:E16" si="7">C7*$F16</f>
-        <v>7.3534837962962963E-4</v>
+        <v>7.415277777777778E-4</v>
       </c>
       <c r="D16" s="65">
         <f t="shared" si="7"/>
-        <v>7.2157523148148146E-4</v>
+        <v>7.2763888888888889E-4</v>
       </c>
       <c r="E16" s="65">
         <f t="shared" si="7"/>
-        <v>7.0146643518518518E-4</v>
+        <v>7.0736111111111108E-4</v>
       </c>
       <c r="F16">
-        <v>1.19</v>
+        <v>1.2</v>
       </c>
       <c r="H16" s="64" t="s">
         <v>221</v>
       </c>
       <c r="I16" s="65">
         <f t="shared" ref="I16:K16" si="8">I7*$L16</f>
-        <v>8.5255787037037038E-4</v>
+        <v>1.2895833333333333E-3</v>
       </c>
       <c r="J16" s="65">
         <f t="shared" si="8"/>
-        <v>8.3740740740740737E-4</v>
+        <v>1.2666666666666666E-3</v>
       </c>
       <c r="K16" s="65">
         <f t="shared" si="8"/>
-        <v>8.2087962962962963E-4</v>
+        <v>1.2416666666666667E-3</v>
       </c>
       <c r="L16">
-        <v>1.19</v>
+        <v>1.8</v>
       </c>
       <c r="Q16" s="64" t="s">
         <v>221</v>
       </c>
       <c r="R16" s="65">
         <f t="shared" si="2"/>
-        <v>6.5752314814814807E-4</v>
+        <v>6.5180555555555554E-4</v>
       </c>
       <c r="S16" s="65">
         <f t="shared" si="2"/>
-        <v>6.4008680555555553E-4</v>
+        <v>6.3452083333333329E-4</v>
       </c>
       <c r="T16" s="65">
         <f t="shared" si="2"/>
-        <v>6.2025462962962956E-4</v>
+        <v>6.1486111111111106E-4</v>
       </c>
       <c r="U16">
-        <v>1.1499999999999999</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="W16" s="64" t="s">
         <v>221</v>
       </c>
       <c r="X16" s="65">
         <f t="shared" ref="X16:Z16" si="9">X7*$AA16</f>
-        <v>7.8582291666666666E-4</v>
+        <v>7.7910648148148153E-4</v>
       </c>
       <c r="Y16" s="65">
         <f>Y7*$AA16</f>
-        <v>7.5576041666666662E-4</v>
+        <v>7.4930092592592583E-4</v>
       </c>
       <c r="Z16" s="65">
         <f t="shared" si="9"/>
-        <v>7.3382291666666659E-4</v>
+        <v>7.2755092592592587E-4</v>
       </c>
       <c r="AA16">
-        <v>1.17</v>
+        <v>1.1599999999999999</v>
       </c>
     </row>
     <row r="17" spans="2:27" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -16445,72 +16445,72 @@
       </c>
       <c r="C17" s="65">
         <f t="shared" ref="C17:E17" si="10">C8*$F17</f>
-        <v>8.4663541666666665E-4</v>
+        <v>8.5375000000000002E-4</v>
       </c>
       <c r="D17" s="65">
         <f t="shared" si="10"/>
-        <v>8.2570023148148151E-4</v>
+        <v>8.3263888888888895E-4</v>
       </c>
       <c r="E17" s="65">
         <f t="shared" si="10"/>
-        <v>7.951238425925925E-4</v>
+        <v>8.018055555555555E-4</v>
       </c>
       <c r="F17">
-        <v>1.19</v>
+        <v>1.2</v>
       </c>
       <c r="H17" s="64" t="s">
         <v>222</v>
       </c>
       <c r="I17" s="65">
         <f t="shared" ref="I17:K17" si="11">I8*$L17</f>
-        <v>9.4924537037037037E-4</v>
+        <v>1.4358333333333334E-3</v>
       </c>
       <c r="J17" s="65">
         <f t="shared" si="11"/>
-        <v>9.3051388888888893E-4</v>
+        <v>1.4075000000000001E-3</v>
       </c>
       <c r="K17" s="65">
         <f t="shared" si="11"/>
-        <v>9.1026736111111115E-4</v>
+        <v>1.3768750000000001E-3</v>
       </c>
       <c r="L17">
-        <v>1.19</v>
+        <v>1.8</v>
       </c>
       <c r="Q17" s="64" t="s">
         <v>222</v>
       </c>
       <c r="R17" s="65">
         <f t="shared" si="2"/>
-        <v>7.3751736111111099E-4</v>
+        <v>7.3110416666666647E-4</v>
       </c>
       <c r="S17" s="65">
         <f t="shared" si="2"/>
-        <v>7.116956018518517E-4</v>
+        <v>7.0550694444444437E-4</v>
       </c>
       <c r="T17" s="65">
         <f t="shared" si="2"/>
-        <v>6.8214699074074065E-4</v>
+        <v>6.7621527777777775E-4</v>
       </c>
       <c r="U17">
-        <v>1.1499999999999999</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="W17" s="64" t="s">
         <v>222</v>
       </c>
       <c r="X17" s="65">
         <f t="shared" ref="X17:Z17" si="12">X8*$AA17</f>
-        <v>8.6883333333333322E-4</v>
+        <v>8.614074074074073E-4</v>
       </c>
       <c r="Y17" s="65">
         <f>Y8*$AA17</f>
-        <v>8.322708333333333E-4</v>
+        <v>8.2515740740740737E-4</v>
       </c>
       <c r="Z17" s="65">
         <f t="shared" si="12"/>
-        <v>8.0545833333333326E-4</v>
+        <v>7.9857407407407394E-4</v>
       </c>
       <c r="AA17">
-        <v>1.17</v>
+        <v>1.1599999999999999</v>
       </c>
     </row>
     <row r="18" spans="2:27" x14ac:dyDescent="0.45">
@@ -16519,72 +16519,72 @@
       </c>
       <c r="C18" s="65">
         <f t="shared" ref="C18:E18" si="13">C9*$F18</f>
-        <v>1.8993171296296297E-3</v>
+        <v>1.9152777777777779E-3</v>
       </c>
       <c r="D18" s="65">
         <f t="shared" si="13"/>
-        <v>1.8617164351851848E-3</v>
+        <v>1.8773611111111107E-3</v>
       </c>
       <c r="E18" s="65">
         <f t="shared" si="13"/>
-        <v>1.8066238425925923E-3</v>
+        <v>1.8218055555555552E-3</v>
       </c>
       <c r="F18">
-        <v>1.19</v>
+        <v>1.2</v>
       </c>
       <c r="H18" s="64" t="s">
         <v>223</v>
       </c>
       <c r="I18" s="65">
         <f t="shared" ref="I18:K18" si="14">I9*$L18</f>
-        <v>2.0085381944444443E-3</v>
+        <v>3.038125E-3</v>
       </c>
       <c r="J18" s="65">
         <f t="shared" si="14"/>
-        <v>1.9787881944444445E-3</v>
+        <v>2.9931250000000006E-3</v>
       </c>
       <c r="K18" s="65">
         <f t="shared" si="14"/>
-        <v>1.9491759259259258E-3</v>
+        <v>2.9483333333333336E-3</v>
       </c>
       <c r="L18">
-        <v>1.19</v>
+        <v>1.8</v>
       </c>
       <c r="Q18" s="64" t="s">
         <v>223</v>
       </c>
       <c r="R18" s="65">
         <f t="shared" si="2"/>
-        <v>1.6902604166666663E-3</v>
+        <v>1.6755624999999998E-3</v>
       </c>
       <c r="S18" s="65">
         <f t="shared" si="2"/>
-        <v>1.6428761574074073E-3</v>
+        <v>1.6285902777777778E-3</v>
       </c>
       <c r="T18" s="65">
         <f t="shared" si="2"/>
-        <v>1.5888368055555554E-3</v>
+        <v>1.5750208333333332E-3</v>
       </c>
       <c r="U18">
-        <v>1.1499999999999999</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="W18" s="64" t="s">
         <v>223</v>
       </c>
       <c r="X18" s="65">
         <f t="shared" ref="X18:Z18" si="15">X9*$AA18</f>
-        <v>1.8871666666666668E-3</v>
+        <v>1.8710370370370372E-3</v>
       </c>
       <c r="Y18" s="65">
         <f t="shared" si="15"/>
-        <v>1.8506041666666664E-3</v>
+        <v>1.8347870370370369E-3</v>
       </c>
       <c r="Z18" s="65">
         <f t="shared" si="15"/>
-        <v>1.8239270833333332E-3</v>
+        <v>1.8083379629629628E-3</v>
       </c>
       <c r="AA18">
-        <v>1.17</v>
+        <v>1.1599999999999999</v>
       </c>
     </row>
     <row r="19" spans="2:27" x14ac:dyDescent="0.45">
@@ -16593,72 +16593,72 @@
       </c>
       <c r="C19" s="65">
         <f t="shared" ref="C19:E19" si="16">C10*$F19</f>
-        <v>2.0849791666666664E-3</v>
+        <v>2.1024999999999998E-3</v>
       </c>
       <c r="D19" s="65">
         <f t="shared" si="16"/>
-        <v>2.04159375E-3</v>
+        <v>2.0587499999999998E-3</v>
       </c>
       <c r="E19" s="65">
         <f t="shared" si="16"/>
-        <v>1.9779618055555557E-3</v>
+        <v>1.9945833333333335E-3</v>
       </c>
       <c r="F19">
-        <v>1.19</v>
+        <v>1.2</v>
       </c>
       <c r="H19" s="64" t="s">
         <v>4</v>
       </c>
       <c r="I19" s="65">
         <f t="shared" ref="I19:K19" si="17">I10*$L19</f>
-        <v>2.2480532407407406E-3</v>
+        <v>3.400416666666667E-3</v>
       </c>
       <c r="J19" s="65">
         <f t="shared" si="17"/>
-        <v>2.1998472222222224E-3</v>
+        <v>3.3275000000000002E-3</v>
       </c>
       <c r="K19" s="65">
         <f t="shared" si="17"/>
-        <v>2.1515034722222222E-3</v>
+        <v>3.2543749999999999E-3</v>
       </c>
       <c r="L19">
-        <v>1.19</v>
+        <v>1.8</v>
       </c>
       <c r="Q19" s="64" t="s">
         <v>4</v>
       </c>
       <c r="R19" s="65">
         <f t="shared" si="2"/>
-        <v>1.8471874999999999E-3</v>
+        <v>1.8311249999999999E-3</v>
       </c>
       <c r="S19" s="65">
         <f t="shared" si="2"/>
-        <v>1.8292187499999999E-3</v>
+        <v>1.8133124999999998E-3</v>
       </c>
       <c r="T19" s="65">
         <f t="shared" si="2"/>
-        <v>1.7735821759259258E-3</v>
+        <v>1.7581597222222222E-3</v>
       </c>
       <c r="U19">
-        <v>1.1499999999999999</v>
+        <v>1.1399999999999999</v>
       </c>
       <c r="W19" s="64" t="s">
         <v>4</v>
       </c>
       <c r="X19" s="65">
         <f t="shared" ref="X19:Z19" si="18">X10*$AA19</f>
-        <v>2.0678124999999998E-3</v>
+        <v>2.0501388888888887E-3</v>
       </c>
       <c r="Y19" s="65">
         <f t="shared" si="18"/>
-        <v>2.0094479166666663E-3</v>
+        <v>1.992273148148148E-3</v>
       </c>
       <c r="Z19" s="65">
         <f t="shared" si="18"/>
-        <v>1.9667916666666666E-3</v>
+        <v>1.9499814814814814E-3</v>
       </c>
       <c r="AA19">
-        <v>1.17</v>
+        <v>1.1599999999999999</v>
       </c>
     </row>
     <row r="22" spans="2:27" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Kalender korrektur / Landeskader style napassung
</commit_message>
<xml_diff>
--- a/web/utilities/records_kriterien.xlsx
+++ b/web/utilities/records_kriterien.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29725"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgna\Documents\GitHub\Lifesaving_Baden\web\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9D9E425-DB7B-46B8-BCE8-3AFE602DA79F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1C2E2CE-B097-4FB5-AA3F-F38EB8A3E25B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" tabRatio="687" firstSheet="1" activeTab="6" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="687" firstSheet="1" activeTab="7" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
   </bookViews>
   <sheets>
     <sheet name="DR" sheetId="9" r:id="rId1"/>
@@ -937,9 +937,6 @@
     <t>Kadertraining LK2</t>
   </si>
   <si>
-    <t>LK2</t>
-  </si>
-  <si>
     <t>WarmUp, Beach Flags, 50m Bahn, Cool down, Treffpunkt: 12:00 Uhr im Foyer</t>
   </si>
   <si>
@@ -1052,6 +1049,9 @@
   </si>
   <si>
     <t>LK2 - Weiblich</t>
+  </si>
+  <si>
+    <t>LK2 / (LK1 - Junioren)</t>
   </si>
 </sst>
 </file>
@@ -1888,13 +1888,16 @@
     <xf numFmtId="0" fontId="17" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1906,6 +1909,15 @@
     <xf numFmtId="0" fontId="17" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1915,10 +1927,13 @@
     <xf numFmtId="0" fontId="17" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1930,14 +1945,8 @@
     <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1981,15 +1990,6 @@
     <xf numFmtId="0" fontId="20" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2004,57 +2004,7 @@
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="207">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="202">
     <dxf>
       <font>
         <color theme="0" tint="-0.24994659260841701"/>
@@ -2360,6 +2310,75 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -4408,75 +4427,6 @@
       </fill>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4491,102 +4441,102 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2C5E83EE-6B6F-478A-9C90-A846A1A76536}" name="WR_Open4" displayName="WR_Open4" ref="A4:AW31" totalsRowShown="0" headerRowDxfId="183" headerRowBorderDxfId="182" tableBorderDxfId="181">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2C5E83EE-6B6F-478A-9C90-A846A1A76536}" name="WR_Open4" displayName="WR_Open4" ref="A4:AW31" totalsRowShown="0" headerRowDxfId="201" headerRowBorderDxfId="200" tableBorderDxfId="199">
   <autoFilter ref="A4:AW31" xr:uid="{2C5E83EE-6B6F-478A-9C90-A846A1A76536}"/>
   <tableColumns count="49">
-    <tableColumn id="1" xr3:uid="{7C0C4105-A61A-4B8D-9129-EDC4F18765AF}" name="WR-Open" dataDxfId="180">
+    <tableColumn id="1" xr3:uid="{7C0C4105-A61A-4B8D-9129-EDC4F18765AF}" name="WR-Open" dataDxfId="198">
       <calculatedColumnFormula>A4+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{516F5612-F85F-413F-9012-E235F415E34B}" name="50m Retten - offen - W" dataDxfId="179"/>
-    <tableColumn id="3" xr3:uid="{BC9ACAC9-0D45-42FD-B596-D19FBE3A4D83}" name="100m Retten - offen - W" dataDxfId="178"/>
-    <tableColumn id="4" xr3:uid="{CB6DBE59-EB65-43F0-93E7-0BDC3F82832B}" name="100m Kombi - offen - W" dataDxfId="177"/>
-    <tableColumn id="5" xr3:uid="{AA603C60-6831-4C14-A8CD-0AA050DA7551}" name="100m Lifesaver - offen - W" dataDxfId="176"/>
-    <tableColumn id="6" xr3:uid="{7920F147-7717-4582-940A-2610F7D310CA}" name="200m Superlifesaver - offen - W" dataDxfId="175"/>
-    <tableColumn id="7" xr3:uid="{04E21F1D-AC8D-4A1B-9B43-59B8F7901673}" name="200m Hindernis - offen - W" dataDxfId="174"/>
-    <tableColumn id="8" xr3:uid="{40E8A083-653A-48A8-9B37-0A2D850B7829}" name="50m Retten - offen - M" dataDxfId="173"/>
-    <tableColumn id="9" xr3:uid="{863824A9-134F-4189-BB14-225AE224FC44}" name="100m Retten - offen - M" dataDxfId="172"/>
+    <tableColumn id="2" xr3:uid="{516F5612-F85F-413F-9012-E235F415E34B}" name="50m Retten - offen - W" dataDxfId="197"/>
+    <tableColumn id="3" xr3:uid="{BC9ACAC9-0D45-42FD-B596-D19FBE3A4D83}" name="100m Retten - offen - W" dataDxfId="196"/>
+    <tableColumn id="4" xr3:uid="{CB6DBE59-EB65-43F0-93E7-0BDC3F82832B}" name="100m Kombi - offen - W" dataDxfId="195"/>
+    <tableColumn id="5" xr3:uid="{AA603C60-6831-4C14-A8CD-0AA050DA7551}" name="100m Lifesaver - offen - W" dataDxfId="194"/>
+    <tableColumn id="6" xr3:uid="{7920F147-7717-4582-940A-2610F7D310CA}" name="200m Superlifesaver - offen - W" dataDxfId="193"/>
+    <tableColumn id="7" xr3:uid="{04E21F1D-AC8D-4A1B-9B43-59B8F7901673}" name="200m Hindernis - offen - W" dataDxfId="192"/>
+    <tableColumn id="8" xr3:uid="{40E8A083-653A-48A8-9B37-0A2D850B7829}" name="50m Retten - offen - M" dataDxfId="191"/>
+    <tableColumn id="9" xr3:uid="{863824A9-134F-4189-BB14-225AE224FC44}" name="100m Retten - offen - M" dataDxfId="190"/>
     <tableColumn id="10" xr3:uid="{598FC6AE-DEA2-4475-9A35-CDCB8C81496A}" name="100m Kombi - offen - M"/>
     <tableColumn id="11" xr3:uid="{9FC50B37-0D51-422E-A268-A6506D4F3854}" name="100m Lifesaver - offen - M"/>
     <tableColumn id="12" xr3:uid="{B8D2552B-5D82-442A-98F0-E47D5C5F6728}" name="200m Superlifesaver - offen - M"/>
-    <tableColumn id="13" xr3:uid="{5A5E9873-0C5F-4508-AF6B-4974E0526D84}" name="200m Hindernis - offen - M" dataDxfId="171"/>
-    <tableColumn id="14" xr3:uid="{FA907992-7FCE-4CAD-8CF2-F5BEBC9B3756}" name="50m Retten - 17/18 - W" dataDxfId="170"/>
-    <tableColumn id="15" xr3:uid="{76B63DC0-CB67-48F4-9B5A-D22902F59334}" name="100m Retten - 17/18 - W" dataDxfId="169"/>
-    <tableColumn id="16" xr3:uid="{614A2419-51B1-44C0-8469-ADBFB078B81A}" name="100m Kombi -17/18 - W" dataDxfId="168"/>
-    <tableColumn id="17" xr3:uid="{2EC953EE-367D-4524-A25E-8DE3B8168E34}" name="100m Lifesaver - 17/18 - W" dataDxfId="167"/>
-    <tableColumn id="18" xr3:uid="{25711867-9BD7-4197-9094-A21392411249}" name="200m Superlifesaver - 17/18 - W" dataDxfId="166"/>
-    <tableColumn id="19" xr3:uid="{262DB142-CFB1-45C3-9332-7273CACD1B62}" name="200m Hindernis - 17/18 - W" dataDxfId="165"/>
-    <tableColumn id="20" xr3:uid="{938BA45A-8244-4637-8A14-DF49CD91A945}" name="50m Retten - 17/18 - M" dataDxfId="164"/>
-    <tableColumn id="21" xr3:uid="{737E28D8-900F-4A98-95FE-EE7B0AFDEE90}" name="100m Retten - 17/18 - M" dataDxfId="163"/>
-    <tableColumn id="22" xr3:uid="{330BD3A8-061C-45E2-ADDB-40C2F346772F}" name="100m Kombi - 17/18 - M" dataDxfId="162"/>
-    <tableColumn id="23" xr3:uid="{0CADDE90-A167-4E1D-8D33-8624E5E1A4E2}" name="100m Lifesaver - 17/18 - M" dataDxfId="161"/>
-    <tableColumn id="24" xr3:uid="{FCF9F42C-1291-4985-9D37-B9DE2DAA5DCB}" name="200m Superlifesaver - 17/18 - M" dataDxfId="160"/>
-    <tableColumn id="25" xr3:uid="{4E5397B2-F924-4F48-AE69-AF6D650AF88D}" name="200m Hindernis - 17/18 - M" dataDxfId="159"/>
-    <tableColumn id="26" xr3:uid="{0A78315A-BFDC-43EE-A66F-48B301F66508}" name="50m Retten - 15/16 - W" dataDxfId="158"/>
-    <tableColumn id="27" xr3:uid="{D3FCF8BD-6C76-450D-80C0-CC0519A79731}" name="100m Retten - 15/16 - W" dataDxfId="157"/>
-    <tableColumn id="28" xr3:uid="{6BE7937E-D62D-47CD-95DE-1730304B0DF3}" name="100m Kombi - 15/16 - W" dataDxfId="156"/>
-    <tableColumn id="29" xr3:uid="{098BA5BE-5AF6-4187-89B6-534498F24C51}" name="100m Lifesaver -  15/16 - W" dataDxfId="155"/>
-    <tableColumn id="30" xr3:uid="{2A6822CF-143C-4BF7-A440-5777527BE512}" name="200m Superlifesaver -  15/16 - W" dataDxfId="154"/>
-    <tableColumn id="31" xr3:uid="{541C7145-CDEA-4E4E-9E7A-A4F05BA6C3E5}" name="200m Hindernis -  15/16 - W" dataDxfId="153"/>
-    <tableColumn id="32" xr3:uid="{342C4488-8C61-42E6-87A9-C75BD8EB7452}" name="50m Retten - 15/16 - M" dataDxfId="152"/>
-    <tableColumn id="33" xr3:uid="{857B1D46-7D20-47F7-AB9B-732D50346E32}" name="100m Retten - 15/16 - M" dataDxfId="151"/>
-    <tableColumn id="34" xr3:uid="{4C8A2EB4-804B-45F1-A768-9A6958957F8B}" name="100m Kombi -15/16 - M" dataDxfId="150"/>
-    <tableColumn id="35" xr3:uid="{26C75B4F-21EC-4EB0-A9A9-54BC80140672}" name="100m Lifesaver - 15/16 - M" dataDxfId="149"/>
-    <tableColumn id="36" xr3:uid="{DBBB2A23-1A06-429A-A5D1-A547EF5EC16F}" name="200m Superlifesaver - 15/16 - M" dataDxfId="148"/>
-    <tableColumn id="37" xr3:uid="{84061231-CAE5-427A-87F5-6DDBA99F77D2}" name="200m Hindernis - 15/16 - M" dataDxfId="147"/>
-    <tableColumn id="38" xr3:uid="{878CCA80-A742-4B3C-90C9-E93BB814201B}" name="50m Retten - 13/14 - W" dataDxfId="146"/>
-    <tableColumn id="39" xr3:uid="{A1F57102-61CF-4784-8DE2-0B8F32D5D699}" name="50m Retten mit Flossen - 13/14 - W" dataDxfId="145"/>
-    <tableColumn id="40" xr3:uid="{0F6BAF78-3D79-42A9-9FED-E6D0E335A920}" name="100m Hindernis - 13/14 - W" dataDxfId="144"/>
-    <tableColumn id="41" xr3:uid="{EB748A68-E10D-4D76-B315-8FDB3AC33C8D}" name="50m Retten - 13/14 - M" dataDxfId="143"/>
-    <tableColumn id="42" xr3:uid="{C7B04167-6430-40F0-9A0F-D0D0BE2F9C77}" name="50m Retten mit Flossen - 13/14 - M" dataDxfId="142"/>
-    <tableColumn id="43" xr3:uid="{48704BB7-A853-445A-8CDC-8D8F86C2B66A}" name="100m Hindernis - 13/14 - M" dataDxfId="141"/>
-    <tableColumn id="44" xr3:uid="{9605FE9A-F41C-4A5F-A59C-B7A9D45C460F}" name="50m Flossen - 12 - W" dataDxfId="140"/>
-    <tableColumn id="45" xr3:uid="{4C9DBF61-35B1-4BC2-8272-526E0AFAAFFB}" name="50m komb. Schwimmen - 12 - W" dataDxfId="139"/>
-    <tableColumn id="46" xr3:uid="{CF433C95-C272-48F9-98CD-7E3C8DBB6F2C}" name="50m Hindernis - 12 - W" dataDxfId="138"/>
-    <tableColumn id="47" xr3:uid="{FADB7411-DB43-4B14-B9E8-D74CA1BA18B8}" name="50m Flossen - 12 - M" dataDxfId="137"/>
-    <tableColumn id="48" xr3:uid="{02936F84-1D82-48AC-8D7C-6D2954D68A06}" name="50m komb. Schwimmen - 12 - M" dataDxfId="136"/>
-    <tableColumn id="49" xr3:uid="{7FD9BD11-0597-4E07-8DA5-DB53384197F5}" name="50m Hindernis - 12 - M" dataDxfId="135"/>
+    <tableColumn id="13" xr3:uid="{5A5E9873-0C5F-4508-AF6B-4974E0526D84}" name="200m Hindernis - offen - M" dataDxfId="189"/>
+    <tableColumn id="14" xr3:uid="{FA907992-7FCE-4CAD-8CF2-F5BEBC9B3756}" name="50m Retten - 17/18 - W" dataDxfId="188"/>
+    <tableColumn id="15" xr3:uid="{76B63DC0-CB67-48F4-9B5A-D22902F59334}" name="100m Retten - 17/18 - W" dataDxfId="187"/>
+    <tableColumn id="16" xr3:uid="{614A2419-51B1-44C0-8469-ADBFB078B81A}" name="100m Kombi -17/18 - W" dataDxfId="186"/>
+    <tableColumn id="17" xr3:uid="{2EC953EE-367D-4524-A25E-8DE3B8168E34}" name="100m Lifesaver - 17/18 - W" dataDxfId="185"/>
+    <tableColumn id="18" xr3:uid="{25711867-9BD7-4197-9094-A21392411249}" name="200m Superlifesaver - 17/18 - W" dataDxfId="184"/>
+    <tableColumn id="19" xr3:uid="{262DB142-CFB1-45C3-9332-7273CACD1B62}" name="200m Hindernis - 17/18 - W" dataDxfId="183"/>
+    <tableColumn id="20" xr3:uid="{938BA45A-8244-4637-8A14-DF49CD91A945}" name="50m Retten - 17/18 - M" dataDxfId="182"/>
+    <tableColumn id="21" xr3:uid="{737E28D8-900F-4A98-95FE-EE7B0AFDEE90}" name="100m Retten - 17/18 - M" dataDxfId="181"/>
+    <tableColumn id="22" xr3:uid="{330BD3A8-061C-45E2-ADDB-40C2F346772F}" name="100m Kombi - 17/18 - M" dataDxfId="180"/>
+    <tableColumn id="23" xr3:uid="{0CADDE90-A167-4E1D-8D33-8624E5E1A4E2}" name="100m Lifesaver - 17/18 - M" dataDxfId="179"/>
+    <tableColumn id="24" xr3:uid="{FCF9F42C-1291-4985-9D37-B9DE2DAA5DCB}" name="200m Superlifesaver - 17/18 - M" dataDxfId="178"/>
+    <tableColumn id="25" xr3:uid="{4E5397B2-F924-4F48-AE69-AF6D650AF88D}" name="200m Hindernis - 17/18 - M" dataDxfId="177"/>
+    <tableColumn id="26" xr3:uid="{0A78315A-BFDC-43EE-A66F-48B301F66508}" name="50m Retten - 15/16 - W" dataDxfId="176"/>
+    <tableColumn id="27" xr3:uid="{D3FCF8BD-6C76-450D-80C0-CC0519A79731}" name="100m Retten - 15/16 - W" dataDxfId="175"/>
+    <tableColumn id="28" xr3:uid="{6BE7937E-D62D-47CD-95DE-1730304B0DF3}" name="100m Kombi - 15/16 - W" dataDxfId="174"/>
+    <tableColumn id="29" xr3:uid="{098BA5BE-5AF6-4187-89B6-534498F24C51}" name="100m Lifesaver -  15/16 - W" dataDxfId="173"/>
+    <tableColumn id="30" xr3:uid="{2A6822CF-143C-4BF7-A440-5777527BE512}" name="200m Superlifesaver -  15/16 - W" dataDxfId="172"/>
+    <tableColumn id="31" xr3:uid="{541C7145-CDEA-4E4E-9E7A-A4F05BA6C3E5}" name="200m Hindernis -  15/16 - W" dataDxfId="171"/>
+    <tableColumn id="32" xr3:uid="{342C4488-8C61-42E6-87A9-C75BD8EB7452}" name="50m Retten - 15/16 - M" dataDxfId="170"/>
+    <tableColumn id="33" xr3:uid="{857B1D46-7D20-47F7-AB9B-732D50346E32}" name="100m Retten - 15/16 - M" dataDxfId="169"/>
+    <tableColumn id="34" xr3:uid="{4C8A2EB4-804B-45F1-A768-9A6958957F8B}" name="100m Kombi -15/16 - M" dataDxfId="168"/>
+    <tableColumn id="35" xr3:uid="{26C75B4F-21EC-4EB0-A9A9-54BC80140672}" name="100m Lifesaver - 15/16 - M" dataDxfId="167"/>
+    <tableColumn id="36" xr3:uid="{DBBB2A23-1A06-429A-A5D1-A547EF5EC16F}" name="200m Superlifesaver - 15/16 - M" dataDxfId="166"/>
+    <tableColumn id="37" xr3:uid="{84061231-CAE5-427A-87F5-6DDBA99F77D2}" name="200m Hindernis - 15/16 - M" dataDxfId="165"/>
+    <tableColumn id="38" xr3:uid="{878CCA80-A742-4B3C-90C9-E93BB814201B}" name="50m Retten - 13/14 - W" dataDxfId="164"/>
+    <tableColumn id="39" xr3:uid="{A1F57102-61CF-4784-8DE2-0B8F32D5D699}" name="50m Retten mit Flossen - 13/14 - W" dataDxfId="163"/>
+    <tableColumn id="40" xr3:uid="{0F6BAF78-3D79-42A9-9FED-E6D0E335A920}" name="100m Hindernis - 13/14 - W" dataDxfId="162"/>
+    <tableColumn id="41" xr3:uid="{EB748A68-E10D-4D76-B315-8FDB3AC33C8D}" name="50m Retten - 13/14 - M" dataDxfId="161"/>
+    <tableColumn id="42" xr3:uid="{C7B04167-6430-40F0-9A0F-D0D0BE2F9C77}" name="50m Retten mit Flossen - 13/14 - M" dataDxfId="160"/>
+    <tableColumn id="43" xr3:uid="{48704BB7-A853-445A-8CDC-8D8F86C2B66A}" name="100m Hindernis - 13/14 - M" dataDxfId="159"/>
+    <tableColumn id="44" xr3:uid="{9605FE9A-F41C-4A5F-A59C-B7A9D45C460F}" name="50m Flossen - 12 - W" dataDxfId="158"/>
+    <tableColumn id="45" xr3:uid="{4C9DBF61-35B1-4BC2-8272-526E0AFAAFFB}" name="50m komb. Schwimmen - 12 - W" dataDxfId="157"/>
+    <tableColumn id="46" xr3:uid="{CF433C95-C272-48F9-98CD-7E3C8DBB6F2C}" name="50m Hindernis - 12 - W" dataDxfId="156"/>
+    <tableColumn id="47" xr3:uid="{FADB7411-DB43-4B14-B9E8-D74CA1BA18B8}" name="50m Flossen - 12 - M" dataDxfId="155"/>
+    <tableColumn id="48" xr3:uid="{02936F84-1D82-48AC-8D7C-6D2954D68A06}" name="50m komb. Schwimmen - 12 - M" dataDxfId="154"/>
+    <tableColumn id="49" xr3:uid="{7FD9BD11-0597-4E07-8DA5-DB53384197F5}" name="50m Hindernis - 12 - M" dataDxfId="153"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4234D44E-A2BE-4790-B589-1A8CC19B714E}" name="WR_Youth" displayName="WR_Youth" ref="A4:M32" totalsRowShown="0" headerRowDxfId="134" dataDxfId="132" headerRowBorderDxfId="133" tableBorderDxfId="131">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4234D44E-A2BE-4790-B589-1A8CC19B714E}" name="WR_Youth" displayName="WR_Youth" ref="A4:M32" totalsRowShown="0" headerRowDxfId="152" dataDxfId="150" headerRowBorderDxfId="151" tableBorderDxfId="149">
   <autoFilter ref="A4:M32" xr:uid="{4234D44E-A2BE-4790-B589-1A8CC19B714E}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{848E691A-41B0-42DD-B122-FB6DF43CB3EF}" name="WR-Youth" dataDxfId="130"/>
-    <tableColumn id="2" xr3:uid="{2FE43F18-485B-46A9-8946-FBC5FDAE5A8E}" name="50m Retten" dataDxfId="129"/>
-    <tableColumn id="3" xr3:uid="{CA5C3ABF-02E6-442B-868B-95B293B231D3}" name="100m Retten" dataDxfId="128"/>
-    <tableColumn id="4" xr3:uid="{7A6BBA52-2145-464D-8C04-B2CCFC1A90DC}" name="100m Kombi" dataDxfId="127"/>
-    <tableColumn id="5" xr3:uid="{21F420C9-E788-49EE-88F6-E37963ED31CF}" name="100m Lifesaver" dataDxfId="126"/>
-    <tableColumn id="6" xr3:uid="{CB87B7CD-8A9C-4775-A4D7-4D267F43FD1A}" name="200m Superlifesaver" dataDxfId="125"/>
-    <tableColumn id="7" xr3:uid="{2DC7F290-B564-4851-85AE-D211DA701B32}" name="200m Hindernis" dataDxfId="124"/>
-    <tableColumn id="8" xr3:uid="{8112783D-8796-4D6A-8414-AC675D745697}" name="50m Retten2" dataDxfId="123"/>
-    <tableColumn id="9" xr3:uid="{4E818CD4-8725-495D-9D1D-1AFCED9181F5}" name="100m Retten2" dataDxfId="122"/>
-    <tableColumn id="10" xr3:uid="{28C05A91-E302-40A9-B50A-ECF997F129FC}" name="100m Kombi2" dataDxfId="121"/>
-    <tableColumn id="11" xr3:uid="{D56FB9F2-45BF-4EC9-A84C-8A5FB59F2F05}" name="100m Lifesaver2" dataDxfId="120"/>
-    <tableColumn id="12" xr3:uid="{540169C0-2A40-4794-A872-F7DF8A887BF2}" name="200m Superlifesaver2" dataDxfId="119"/>
-    <tableColumn id="13" xr3:uid="{D104CB67-B55A-4C81-87E5-0AC758DD22A4}" name="200m Hindernis2" dataDxfId="118"/>
+    <tableColumn id="1" xr3:uid="{848E691A-41B0-42DD-B122-FB6DF43CB3EF}" name="WR-Youth" dataDxfId="148"/>
+    <tableColumn id="2" xr3:uid="{2FE43F18-485B-46A9-8946-FBC5FDAE5A8E}" name="50m Retten" dataDxfId="147"/>
+    <tableColumn id="3" xr3:uid="{CA5C3ABF-02E6-442B-868B-95B293B231D3}" name="100m Retten" dataDxfId="146"/>
+    <tableColumn id="4" xr3:uid="{7A6BBA52-2145-464D-8C04-B2CCFC1A90DC}" name="100m Kombi" dataDxfId="145"/>
+    <tableColumn id="5" xr3:uid="{21F420C9-E788-49EE-88F6-E37963ED31CF}" name="100m Lifesaver" dataDxfId="144"/>
+    <tableColumn id="6" xr3:uid="{CB87B7CD-8A9C-4775-A4D7-4D267F43FD1A}" name="200m Superlifesaver" dataDxfId="143"/>
+    <tableColumn id="7" xr3:uid="{2DC7F290-B564-4851-85AE-D211DA701B32}" name="200m Hindernis" dataDxfId="142"/>
+    <tableColumn id="8" xr3:uid="{8112783D-8796-4D6A-8414-AC675D745697}" name="50m Retten2" dataDxfId="141"/>
+    <tableColumn id="9" xr3:uid="{4E818CD4-8725-495D-9D1D-1AFCED9181F5}" name="100m Retten2" dataDxfId="140"/>
+    <tableColumn id="10" xr3:uid="{28C05A91-E302-40A9-B50A-ECF997F129FC}" name="100m Kombi2" dataDxfId="139"/>
+    <tableColumn id="11" xr3:uid="{D56FB9F2-45BF-4EC9-A84C-8A5FB59F2F05}" name="100m Lifesaver2" dataDxfId="138"/>
+    <tableColumn id="12" xr3:uid="{540169C0-2A40-4794-A872-F7DF8A887BF2}" name="200m Superlifesaver2" dataDxfId="137"/>
+    <tableColumn id="13" xr3:uid="{D104CB67-B55A-4C81-87E5-0AC758DD22A4}" name="200m Hindernis2" dataDxfId="136"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E2D2F97B-7645-4066-8AB3-F35CF6E035EB}" name="WR_Open" displayName="WR_Open" ref="A4:M32" totalsRowShown="0" headerRowDxfId="117" headerRowBorderDxfId="116" tableBorderDxfId="115">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E2D2F97B-7645-4066-8AB3-F35CF6E035EB}" name="WR_Open" displayName="WR_Open" ref="A4:M32" totalsRowShown="0" headerRowDxfId="135" headerRowBorderDxfId="134" tableBorderDxfId="133">
   <autoFilter ref="A4:M32" xr:uid="{E2D2F97B-7645-4066-8AB3-F35CF6E035EB}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{AE73402B-B27E-4B29-8DCF-30B7FC1855EF}" name="WR-Open" dataDxfId="114">
+    <tableColumn id="1" xr3:uid="{AE73402B-B27E-4B29-8DCF-30B7FC1855EF}" name="WR-Open" dataDxfId="132">
       <calculatedColumnFormula>A4+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{EA3EAC1F-184E-4A28-B3E3-08DE12F138EF}" name="50m Retten" dataDxfId="113"/>
-    <tableColumn id="3" xr3:uid="{E0305A3F-6087-4F8C-8B64-153E1ACAA32E}" name="100m Retten" dataDxfId="112"/>
-    <tableColumn id="4" xr3:uid="{F0B7AC37-315E-49AA-855C-7955D2B43A76}" name="100m Kombi" dataDxfId="111"/>
-    <tableColumn id="5" xr3:uid="{B5E690AB-DB7D-4864-8916-89D2A68C4128}" name="100m Lifesaver" dataDxfId="110"/>
-    <tableColumn id="6" xr3:uid="{D89BAF4D-36AE-4C73-9320-9C5736F02F8A}" name="200m Superlifesaver" dataDxfId="109"/>
-    <tableColumn id="7" xr3:uid="{58AE7517-1A90-459F-A7D2-B95265D217E7}" name="200m Hindernis" dataDxfId="108"/>
-    <tableColumn id="8" xr3:uid="{13A189FB-E897-4A1F-A001-525F61E9CFFF}" name="50m Retten2" dataDxfId="107"/>
-    <tableColumn id="9" xr3:uid="{36418AC5-46B8-400F-BD2E-D329CF4F92CD}" name="100m Retten2" dataDxfId="106"/>
+    <tableColumn id="2" xr3:uid="{EA3EAC1F-184E-4A28-B3E3-08DE12F138EF}" name="50m Retten" dataDxfId="131"/>
+    <tableColumn id="3" xr3:uid="{E0305A3F-6087-4F8C-8B64-153E1ACAA32E}" name="100m Retten" dataDxfId="130"/>
+    <tableColumn id="4" xr3:uid="{F0B7AC37-315E-49AA-855C-7955D2B43A76}" name="100m Kombi" dataDxfId="129"/>
+    <tableColumn id="5" xr3:uid="{B5E690AB-DB7D-4864-8916-89D2A68C4128}" name="100m Lifesaver" dataDxfId="128"/>
+    <tableColumn id="6" xr3:uid="{D89BAF4D-36AE-4C73-9320-9C5736F02F8A}" name="200m Superlifesaver" dataDxfId="127"/>
+    <tableColumn id="7" xr3:uid="{58AE7517-1A90-459F-A7D2-B95265D217E7}" name="200m Hindernis" dataDxfId="126"/>
+    <tableColumn id="8" xr3:uid="{13A189FB-E897-4A1F-A001-525F61E9CFFF}" name="50m Retten2" dataDxfId="125"/>
+    <tableColumn id="9" xr3:uid="{36418AC5-46B8-400F-BD2E-D329CF4F92CD}" name="100m Retten2" dataDxfId="124"/>
     <tableColumn id="10" xr3:uid="{06A35C2D-7313-472B-BC1F-4F2FB1D14782}" name="100m Kombi2"/>
     <tableColumn id="11" xr3:uid="{89966D0D-9131-4245-A7BE-1A7384D5ADA0}" name="100m Lifesaver2"/>
     <tableColumn id="12" xr3:uid="{D9D6CF56-869C-4DDE-9886-572D4E523A8F}" name="200m Superlifesaver2"/>
@@ -4597,7 +4547,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CF3D303A-A04B-42DD-A44E-CEB6CECB77A4}" name="DP_konfig" displayName="DP_konfig" ref="A1:U3" totalsRowShown="0" headerRowDxfId="206" dataDxfId="205">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CF3D303A-A04B-42DD-A44E-CEB6CECB77A4}" name="DP_konfig" displayName="DP_konfig" ref="A1:U3" totalsRowShown="0" headerRowDxfId="123" dataDxfId="122">
   <autoFilter ref="A1:U3" xr:uid="{CF3D303A-A04B-42DD-A44E-CEB6CECB77A4}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4622,64 +4572,64 @@
     <filterColumn colId="20" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="21">
-    <tableColumn id="1" xr3:uid="{58D628F0-061E-4A82-8362-CDB37A2E7C60}" name="Tabellen Name" dataDxfId="204"/>
-    <tableColumn id="2" xr3:uid="{2F302F6C-F8AF-4FDE-AB08-6F30F9671015}" name="Geschlecht" dataDxfId="203"/>
-    <tableColumn id="3" xr3:uid="{4D91FBF9-386D-43DD-90D0-B49823FDB629}" name="Mindest alter" dataDxfId="202"/>
-    <tableColumn id="4" xr3:uid="{4126AAC6-AF2F-446C-B4EA-D86ACFD9FAC2}" name="Maximales Alter" dataDxfId="201"/>
-    <tableColumn id="5" xr3:uid="{8A10890A-A299-4B09-AC72-0E9AE9238AF3}" name="Qualizeitraum anfang" dataDxfId="200"/>
-    <tableColumn id="6" xr3:uid="{FBCD1C13-FC82-429B-8DE1-0C5A455FDAB8}" name="Qualizeitraum Ende" dataDxfId="199"/>
-    <tableColumn id="7" xr3:uid="{1DCCAC9B-BC46-468E-A3CE-57576C2FF11D}" name="Letzter Wettkampf am" dataDxfId="198"/>
-    <tableColumn id="8" xr3:uid="{9A6E47EE-ABD8-4A1E-87D3-9D286E4C124F}" name="Wertung" dataDxfId="197"/>
-    <tableColumn id="9" xr3:uid="{09E848D2-ED17-49C7-9775-CBF17D20DFC0}" name="Landesverband" dataDxfId="196"/>
-    <tableColumn id="10" xr3:uid="{70ABB713-23F6-4FCF-920E-3CB0CD451446}" name="OMS" dataDxfId="195"/>
-    <tableColumn id="11" xr3:uid="{9C108A1C-E6AB-4C13-9C1D-0FA8944A39A3}" name="Pool-Länge" dataDxfId="194"/>
-    <tableColumn id="12" xr3:uid="{087948DD-430D-48F1-906D-4F4EF4B46053}" name="Regelwerk" dataDxfId="193"/>
-    <tableColumn id="13" xr3:uid="{BF42D9C0-F77D-4971-A67E-32B0246C72C3}" name="Referenz" dataDxfId="192"/>
-    <tableColumn id="19" xr3:uid="{AFFB84E8-B398-4E99-805B-9A247071A040}" name="Referenz Jahr" dataDxfId="191"/>
-    <tableColumn id="20" xr3:uid="{0A59A474-DFBB-4437-8EFF-70284AFD9934}" name="Mindest Punktzahl" dataDxfId="190"/>
-    <tableColumn id="21" xr3:uid="{198BD231-EEF3-43C9-AD9B-39B4B7E9B337}" name="Mindest Disziplinen" dataDxfId="189"/>
-    <tableColumn id="14" xr3:uid="{443CD4F6-A2B2-480B-BB35-DCEEBC531727}" name="3-Kampf Regel" dataDxfId="188"/>
-    <tableColumn id="15" xr3:uid="{70116160-7666-42B1-92AC-FAC2620E6A60}" name="Anzahl Nominierte" dataDxfId="187"/>
-    <tableColumn id="16" xr3:uid="{0EFD0A46-D12B-4AB0-907C-08E5D9F282E0}" name="Anzahl Nachrücker" dataDxfId="186"/>
-    <tableColumn id="17" xr3:uid="{AA5430A0-8ED8-40E8-B7F8-DA25E4E8790F}" name="Seiten Anzahl" dataDxfId="185"/>
-    <tableColumn id="18" xr3:uid="{16F699D9-2741-43F3-AD5F-826A568EFEAC}" name="Absagen" dataDxfId="184"/>
+    <tableColumn id="1" xr3:uid="{58D628F0-061E-4A82-8362-CDB37A2E7C60}" name="Tabellen Name" dataDxfId="121"/>
+    <tableColumn id="2" xr3:uid="{2F302F6C-F8AF-4FDE-AB08-6F30F9671015}" name="Geschlecht" dataDxfId="120"/>
+    <tableColumn id="3" xr3:uid="{4D91FBF9-386D-43DD-90D0-B49823FDB629}" name="Mindest alter" dataDxfId="119"/>
+    <tableColumn id="4" xr3:uid="{4126AAC6-AF2F-446C-B4EA-D86ACFD9FAC2}" name="Maximales Alter" dataDxfId="118"/>
+    <tableColumn id="5" xr3:uid="{8A10890A-A299-4B09-AC72-0E9AE9238AF3}" name="Qualizeitraum anfang" dataDxfId="117"/>
+    <tableColumn id="6" xr3:uid="{FBCD1C13-FC82-429B-8DE1-0C5A455FDAB8}" name="Qualizeitraum Ende" dataDxfId="116"/>
+    <tableColumn id="7" xr3:uid="{1DCCAC9B-BC46-468E-A3CE-57576C2FF11D}" name="Letzter Wettkampf am" dataDxfId="115"/>
+    <tableColumn id="8" xr3:uid="{9A6E47EE-ABD8-4A1E-87D3-9D286E4C124F}" name="Wertung" dataDxfId="114"/>
+    <tableColumn id="9" xr3:uid="{09E848D2-ED17-49C7-9775-CBF17D20DFC0}" name="Landesverband" dataDxfId="113"/>
+    <tableColumn id="10" xr3:uid="{70ABB713-23F6-4FCF-920E-3CB0CD451446}" name="OMS" dataDxfId="112"/>
+    <tableColumn id="11" xr3:uid="{9C108A1C-E6AB-4C13-9C1D-0FA8944A39A3}" name="Pool-Länge" dataDxfId="111"/>
+    <tableColumn id="12" xr3:uid="{087948DD-430D-48F1-906D-4F4EF4B46053}" name="Regelwerk" dataDxfId="110"/>
+    <tableColumn id="13" xr3:uid="{BF42D9C0-F77D-4971-A67E-32B0246C72C3}" name="Referenz" dataDxfId="109"/>
+    <tableColumn id="19" xr3:uid="{AFFB84E8-B398-4E99-805B-9A247071A040}" name="Referenz Jahr" dataDxfId="108"/>
+    <tableColumn id="20" xr3:uid="{0A59A474-DFBB-4437-8EFF-70284AFD9934}" name="Mindest Punktzahl" dataDxfId="107"/>
+    <tableColumn id="21" xr3:uid="{198BD231-EEF3-43C9-AD9B-39B4B7E9B337}" name="Mindest Disziplinen" dataDxfId="106"/>
+    <tableColumn id="14" xr3:uid="{443CD4F6-A2B2-480B-BB35-DCEEBC531727}" name="3-Kampf Regel" dataDxfId="105"/>
+    <tableColumn id="15" xr3:uid="{70116160-7666-42B1-92AC-FAC2620E6A60}" name="Anzahl Nominierte" dataDxfId="104"/>
+    <tableColumn id="16" xr3:uid="{0EFD0A46-D12B-4AB0-907C-08E5D9F282E0}" name="Anzahl Nachrücker" dataDxfId="103"/>
+    <tableColumn id="17" xr3:uid="{AA5430A0-8ED8-40E8-B7F8-DA25E4E8790F}" name="Seiten Anzahl" dataDxfId="102"/>
+    <tableColumn id="18" xr3:uid="{16F699D9-2741-43F3-AD5F-826A568EFEAC}" name="Absagen" dataDxfId="101"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CDBF6724-48A1-41AB-94B5-CC35C54BB15C}" name="BP_konfig" displayName="BP_konfig" ref="A1:U7" totalsRowShown="0" headerRowDxfId="105" dataDxfId="104">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CDBF6724-48A1-41AB-94B5-CC35C54BB15C}" name="BP_konfig" displayName="BP_konfig" ref="A1:U7" totalsRowShown="0" headerRowDxfId="100" dataDxfId="99">
   <autoFilter ref="A1:U7" xr:uid="{CDBF6724-48A1-41AB-94B5-CC35C54BB15C}"/>
   <tableColumns count="21">
-    <tableColumn id="1" xr3:uid="{E1FB3D0C-B874-4874-BACC-6872CF171957}" name="Tabellen Name" dataDxfId="103"/>
-    <tableColumn id="2" xr3:uid="{FFDD2777-2097-450C-B020-F133CF643855}" name="Geschlecht" dataDxfId="102"/>
-    <tableColumn id="3" xr3:uid="{8CF52BE2-8020-48BD-A36D-63F13A1878DE}" name="Mindest alter" dataDxfId="101"/>
-    <tableColumn id="4" xr3:uid="{FD3A030F-CD97-4B6F-8E8C-BC2E67D79F1D}" name="Maximales Alter" dataDxfId="100"/>
-    <tableColumn id="5" xr3:uid="{3E22B645-D77C-4509-B031-9914FCB91599}" name="Qualizeitraum anfang" dataDxfId="99"/>
-    <tableColumn id="6" xr3:uid="{AE299324-3C1C-4063-ADF9-54555A161734}" name="Qualizeitraum Ende" dataDxfId="98"/>
-    <tableColumn id="7" xr3:uid="{DCC178B3-11FC-4C53-BBC6-C2FDA2C89857}" name="Letzter Wettkampf am" dataDxfId="97"/>
-    <tableColumn id="8" xr3:uid="{2811DB01-60A5-4BE4-B6F9-A806398A602A}" name="Wertung" dataDxfId="96"/>
-    <tableColumn id="9" xr3:uid="{0C16DAFE-847D-4E9E-9604-3A7D9FE924D0}" name="Landesverband" dataDxfId="95"/>
-    <tableColumn id="10" xr3:uid="{7A8A4101-A553-4BD5-9116-9AA5876B9401}" name="OMS" dataDxfId="94"/>
-    <tableColumn id="11" xr3:uid="{9807C9BD-6499-45F6-ACE0-4D13D64EF675}" name="Pool-Länge" dataDxfId="93"/>
-    <tableColumn id="12" xr3:uid="{13D336DD-650F-4F2C-836F-361CA1528F6D}" name="Regelwerk" dataDxfId="92"/>
-    <tableColumn id="13" xr3:uid="{66660E2D-ADF2-4FB5-8A13-004F826EE908}" name="Referenz" dataDxfId="91"/>
-    <tableColumn id="19" xr3:uid="{D72EDF8B-ECC3-4FF7-ABE6-B60BCE4A5E26}" name="Referenz Jahr" dataDxfId="90"/>
-    <tableColumn id="20" xr3:uid="{7B18E667-70F7-4BC1-AB1B-21C019F2AA89}" name="Mindest Punktzahl" dataDxfId="89"/>
-    <tableColumn id="21" xr3:uid="{FC185946-681B-42A6-AB1A-FC1EABB668C5}" name="Mindest Disziplinen" dataDxfId="88"/>
-    <tableColumn id="14" xr3:uid="{6A2676FD-2EC7-4C41-A35E-A1597A38F932}" name="3-Kampf Regel" dataDxfId="87"/>
-    <tableColumn id="15" xr3:uid="{718E0917-4F83-4A2B-832F-EBB16D5E21BF}" name="Anzahl Nominierte" dataDxfId="86"/>
-    <tableColumn id="16" xr3:uid="{5C66A461-D647-4E00-A81C-FD7AD44D7CC2}" name="Anzahl Nachrücker" dataDxfId="85"/>
-    <tableColumn id="17" xr3:uid="{D434BDEC-293B-4B4E-A5E9-479438960A03}" name="Seiten Anzahl" dataDxfId="84"/>
-    <tableColumn id="18" xr3:uid="{80908229-9247-473F-81C0-9C9D4C12FF06}" name="Absagen" dataDxfId="83"/>
+    <tableColumn id="1" xr3:uid="{E1FB3D0C-B874-4874-BACC-6872CF171957}" name="Tabellen Name" dataDxfId="98"/>
+    <tableColumn id="2" xr3:uid="{FFDD2777-2097-450C-B020-F133CF643855}" name="Geschlecht" dataDxfId="97"/>
+    <tableColumn id="3" xr3:uid="{8CF52BE2-8020-48BD-A36D-63F13A1878DE}" name="Mindest alter" dataDxfId="96"/>
+    <tableColumn id="4" xr3:uid="{FD3A030F-CD97-4B6F-8E8C-BC2E67D79F1D}" name="Maximales Alter" dataDxfId="95"/>
+    <tableColumn id="5" xr3:uid="{3E22B645-D77C-4509-B031-9914FCB91599}" name="Qualizeitraum anfang" dataDxfId="94"/>
+    <tableColumn id="6" xr3:uid="{AE299324-3C1C-4063-ADF9-54555A161734}" name="Qualizeitraum Ende" dataDxfId="93"/>
+    <tableColumn id="7" xr3:uid="{DCC178B3-11FC-4C53-BBC6-C2FDA2C89857}" name="Letzter Wettkampf am" dataDxfId="92"/>
+    <tableColumn id="8" xr3:uid="{2811DB01-60A5-4BE4-B6F9-A806398A602A}" name="Wertung" dataDxfId="91"/>
+    <tableColumn id="9" xr3:uid="{0C16DAFE-847D-4E9E-9604-3A7D9FE924D0}" name="Landesverband" dataDxfId="90"/>
+    <tableColumn id="10" xr3:uid="{7A8A4101-A553-4BD5-9116-9AA5876B9401}" name="OMS" dataDxfId="89"/>
+    <tableColumn id="11" xr3:uid="{9807C9BD-6499-45F6-ACE0-4D13D64EF675}" name="Pool-Länge" dataDxfId="88"/>
+    <tableColumn id="12" xr3:uid="{13D336DD-650F-4F2C-836F-361CA1528F6D}" name="Regelwerk" dataDxfId="87"/>
+    <tableColumn id="13" xr3:uid="{66660E2D-ADF2-4FB5-8A13-004F826EE908}" name="Referenz" dataDxfId="86"/>
+    <tableColumn id="19" xr3:uid="{D72EDF8B-ECC3-4FF7-ABE6-B60BCE4A5E26}" name="Referenz Jahr" dataDxfId="85"/>
+    <tableColumn id="20" xr3:uid="{7B18E667-70F7-4BC1-AB1B-21C019F2AA89}" name="Mindest Punktzahl" dataDxfId="84"/>
+    <tableColumn id="21" xr3:uid="{FC185946-681B-42A6-AB1A-FC1EABB668C5}" name="Mindest Disziplinen" dataDxfId="83"/>
+    <tableColumn id="14" xr3:uid="{6A2676FD-2EC7-4C41-A35E-A1597A38F932}" name="3-Kampf Regel" dataDxfId="82"/>
+    <tableColumn id="15" xr3:uid="{718E0917-4F83-4A2B-832F-EBB16D5E21BF}" name="Anzahl Nominierte" dataDxfId="81"/>
+    <tableColumn id="16" xr3:uid="{5C66A461-D647-4E00-A81C-FD7AD44D7CC2}" name="Anzahl Nachrücker" dataDxfId="80"/>
+    <tableColumn id="17" xr3:uid="{D434BDEC-293B-4B4E-A5E9-479438960A03}" name="Seiten Anzahl" dataDxfId="79"/>
+    <tableColumn id="18" xr3:uid="{80908229-9247-473F-81C0-9C9D4C12FF06}" name="Absagen" dataDxfId="78"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{16F87202-5A6A-4E2F-B973-3CE7EC2566C1}" name="DEM_konfig" displayName="DEM_konfig" ref="A1:X7" totalsRowShown="0" headerRowDxfId="82" dataDxfId="81">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{16F87202-5A6A-4E2F-B973-3CE7EC2566C1}" name="DEM_konfig" displayName="DEM_konfig" ref="A1:X7" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76">
   <autoFilter ref="A1:X7" xr:uid="{16F87202-5A6A-4E2F-B973-3CE7EC2566C1}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4707,37 +4657,37 @@
     <filterColumn colId="23" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{4847B567-64E1-4AC3-8C4B-EFCF3F00CC6C}" name="Tabellen Name" dataDxfId="80"/>
-    <tableColumn id="2" xr3:uid="{6346FF3B-B334-4CD8-8B23-F2347E29C536}" name="Geschlecht" dataDxfId="79"/>
-    <tableColumn id="3" xr3:uid="{E793B48A-BC8A-439F-8AAF-6FD08104A619}" name="Mindest Alter" dataDxfId="78"/>
-    <tableColumn id="4" xr3:uid="{01A62C29-2F75-4107-A431-F69230BCCD0C}" name="Maximales Alter" dataDxfId="77"/>
-    <tableColumn id="5" xr3:uid="{B7E4DE90-7856-4A0C-9063-61414D7F227C}" name="Qualizeitraum anfang" dataDxfId="76"/>
-    <tableColumn id="6" xr3:uid="{B00F7CD1-82CB-42B9-A396-89F79EF419CA}" name="Qualizeitraum Ende" dataDxfId="75"/>
-    <tableColumn id="7" xr3:uid="{9E50DDE5-12E3-4BCB-801C-FBABCE309F0E}" name="Letzter Wettkampf am" dataDxfId="74"/>
-    <tableColumn id="8" xr3:uid="{57E68247-0FF2-48D8-8ACD-AB057E576A21}" name="Landesverband" dataDxfId="73"/>
-    <tableColumn id="9" xr3:uid="{EBAA439D-F69A-4C2A-8193-9AE08F1E57B8}" name="OMS" dataDxfId="72"/>
-    <tableColumn id="10" xr3:uid="{BBD11E7F-3DDF-428A-B005-4A40E6FA78DC}" name="Pool-Länge" dataDxfId="71"/>
-    <tableColumn id="11" xr3:uid="{6AE38DCA-A084-4F3D-A6A4-4E76E3E2CBC6}" name="Regelwerk" dataDxfId="70"/>
-    <tableColumn id="12" xr3:uid="{7F7470AD-5502-4CEE-BB4C-44BA308E61D7}" name="Seiten Anzahl" dataDxfId="69"/>
-    <tableColumn id="13" xr3:uid="{F416CBFA-4C9D-45CD-9BA7-E4BC57A08BC2}" name="PZ1 - 50m Retten" dataDxfId="68"/>
-    <tableColumn id="14" xr3:uid="{7117DBCA-0DA7-462C-84FE-0DC7E33B124C}" name="PZ1 - 100m Retten" dataDxfId="67"/>
-    <tableColumn id="15" xr3:uid="{E8630E91-DC30-4822-9E53-6D65487C3670}" name="PZ1 - 100m Kombi" dataDxfId="66"/>
-    <tableColumn id="16" xr3:uid="{4B3AA225-E042-430F-8259-D176887B4528}" name="PZ1 - 100m Lifesaver" dataDxfId="65"/>
-    <tableColumn id="17" xr3:uid="{798674BD-98CE-4531-BDFF-6AB06253AD7C}" name="PZ1 - 200m Super-Lifesaver" dataDxfId="64"/>
-    <tableColumn id="18" xr3:uid="{8809BB71-D58B-4E8B-A442-D0EB9A65A25D}" name="PZ1 - 200m Hindernis" dataDxfId="63"/>
-    <tableColumn id="19" xr3:uid="{93DCF463-806B-4117-B4E3-1FFAE976B37C}" name="PZ2 - 50m Retten" dataDxfId="62"/>
-    <tableColumn id="20" xr3:uid="{A514C961-559E-462F-B143-BA30974C0129}" name="PZ2 - 100m Retten" dataDxfId="61"/>
-    <tableColumn id="21" xr3:uid="{F1CF6143-45FE-498D-93D6-36F26D2F3C0B}" name="PZ2 - 100m Kombi" dataDxfId="60"/>
-    <tableColumn id="22" xr3:uid="{E90962FC-C214-467F-841F-40DF60E41456}" name="PZ2 - 100m Lifesaver" dataDxfId="59"/>
-    <tableColumn id="23" xr3:uid="{7FBC6334-C4C8-4B38-9F59-30ED95A44379}" name="PZ2 - 200m Super-Lifesaver" dataDxfId="58"/>
-    <tableColumn id="24" xr3:uid="{231BFF86-8F3A-4BA1-B25E-28175D9EDFA9}" name="PZ2 - 200m Hindernis" dataDxfId="57"/>
+    <tableColumn id="1" xr3:uid="{4847B567-64E1-4AC3-8C4B-EFCF3F00CC6C}" name="Tabellen Name" dataDxfId="75"/>
+    <tableColumn id="2" xr3:uid="{6346FF3B-B334-4CD8-8B23-F2347E29C536}" name="Geschlecht" dataDxfId="74"/>
+    <tableColumn id="3" xr3:uid="{E793B48A-BC8A-439F-8AAF-6FD08104A619}" name="Mindest Alter" dataDxfId="73"/>
+    <tableColumn id="4" xr3:uid="{01A62C29-2F75-4107-A431-F69230BCCD0C}" name="Maximales Alter" dataDxfId="72"/>
+    <tableColumn id="5" xr3:uid="{B7E4DE90-7856-4A0C-9063-61414D7F227C}" name="Qualizeitraum anfang" dataDxfId="71"/>
+    <tableColumn id="6" xr3:uid="{B00F7CD1-82CB-42B9-A396-89F79EF419CA}" name="Qualizeitraum Ende" dataDxfId="70"/>
+    <tableColumn id="7" xr3:uid="{9E50DDE5-12E3-4BCB-801C-FBABCE309F0E}" name="Letzter Wettkampf am" dataDxfId="69"/>
+    <tableColumn id="8" xr3:uid="{57E68247-0FF2-48D8-8ACD-AB057E576A21}" name="Landesverband" dataDxfId="68"/>
+    <tableColumn id="9" xr3:uid="{EBAA439D-F69A-4C2A-8193-9AE08F1E57B8}" name="OMS" dataDxfId="67"/>
+    <tableColumn id="10" xr3:uid="{BBD11E7F-3DDF-428A-B005-4A40E6FA78DC}" name="Pool-Länge" dataDxfId="66"/>
+    <tableColumn id="11" xr3:uid="{6AE38DCA-A084-4F3D-A6A4-4E76E3E2CBC6}" name="Regelwerk" dataDxfId="65"/>
+    <tableColumn id="12" xr3:uid="{7F7470AD-5502-4CEE-BB4C-44BA308E61D7}" name="Seiten Anzahl" dataDxfId="64"/>
+    <tableColumn id="13" xr3:uid="{F416CBFA-4C9D-45CD-9BA7-E4BC57A08BC2}" name="PZ1 - 50m Retten" dataDxfId="63"/>
+    <tableColumn id="14" xr3:uid="{7117DBCA-0DA7-462C-84FE-0DC7E33B124C}" name="PZ1 - 100m Retten" dataDxfId="62"/>
+    <tableColumn id="15" xr3:uid="{E8630E91-DC30-4822-9E53-6D65487C3670}" name="PZ1 - 100m Kombi" dataDxfId="61"/>
+    <tableColumn id="16" xr3:uid="{4B3AA225-E042-430F-8259-D176887B4528}" name="PZ1 - 100m Lifesaver" dataDxfId="60"/>
+    <tableColumn id="17" xr3:uid="{798674BD-98CE-4531-BDFF-6AB06253AD7C}" name="PZ1 - 200m Super-Lifesaver" dataDxfId="59"/>
+    <tableColumn id="18" xr3:uid="{8809BB71-D58B-4E8B-A442-D0EB9A65A25D}" name="PZ1 - 200m Hindernis" dataDxfId="58"/>
+    <tableColumn id="19" xr3:uid="{93DCF463-806B-4117-B4E3-1FFAE976B37C}" name="PZ2 - 50m Retten" dataDxfId="57"/>
+    <tableColumn id="20" xr3:uid="{A514C961-559E-462F-B143-BA30974C0129}" name="PZ2 - 100m Retten" dataDxfId="56"/>
+    <tableColumn id="21" xr3:uid="{F1CF6143-45FE-498D-93D6-36F26D2F3C0B}" name="PZ2 - 100m Kombi" dataDxfId="55"/>
+    <tableColumn id="22" xr3:uid="{E90962FC-C214-467F-841F-40DF60E41456}" name="PZ2 - 100m Lifesaver" dataDxfId="54"/>
+    <tableColumn id="23" xr3:uid="{7FBC6334-C4C8-4B38-9F59-30ED95A44379}" name="PZ2 - 200m Super-Lifesaver" dataDxfId="53"/>
+    <tableColumn id="24" xr3:uid="{231BFF86-8F3A-4BA1-B25E-28175D9EDFA9}" name="PZ2 - 200m Hindernis" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}" name="JRP_konfig" displayName="JRP_konfig" ref="A1:X15" totalsRowShown="0" headerRowDxfId="56" dataDxfId="55">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}" name="JRP_konfig" displayName="JRP_konfig" ref="A1:X15" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
   <autoFilter ref="A1:X15" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4765,30 +4715,30 @@
     <filterColumn colId="23" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{021DA6E1-2C93-4474-9720-B6F016186D61}" name="Tabellen Name" dataDxfId="54"/>
-    <tableColumn id="2" xr3:uid="{733C1722-A9C9-4830-A9E2-FE62E96BCD98}" name="Geschlecht" dataDxfId="53"/>
-    <tableColumn id="3" xr3:uid="{80C0BF46-0E43-4947-BF86-B808C324772A}" name="Mindest Alter" dataDxfId="52"/>
-    <tableColumn id="4" xr3:uid="{DBA2A923-EEB7-43F9-A1A3-E78624448FB9}" name="Maximales Alter" dataDxfId="51"/>
-    <tableColumn id="5" xr3:uid="{3FDEE18A-328D-45AE-907D-69A916A93345}" name="Qualizeitraum anfang" dataDxfId="50"/>
-    <tableColumn id="6" xr3:uid="{BE002D7F-575F-4B60-9251-C71D93F59045}" name="Qualizeitraum Ende" dataDxfId="49"/>
-    <tableColumn id="7" xr3:uid="{208ABD57-DE4B-41D6-B9FC-93F2D8966E8D}" name="Letzter Wettkampf am" dataDxfId="48"/>
-    <tableColumn id="8" xr3:uid="{30C9697C-6550-4996-ADDB-7FEE5325B794}" name="Landesverband" dataDxfId="47"/>
-    <tableColumn id="9" xr3:uid="{ED2DAB77-EF46-4D8B-B8E4-90412E32E277}" name="OMS" dataDxfId="46"/>
-    <tableColumn id="10" xr3:uid="{AD534940-A91B-4A6E-9606-E3F3E517D401}" name="Pool-Länge" dataDxfId="45"/>
-    <tableColumn id="11" xr3:uid="{11F9D5D5-72FE-42CA-8624-01D513B4140F}" name="Regelwerk" dataDxfId="44"/>
-    <tableColumn id="12" xr3:uid="{3907872B-5438-4FBF-A045-3EF9EAACFC47}" name="Seiten Anzahl" dataDxfId="43"/>
-    <tableColumn id="13" xr3:uid="{FC821324-3638-40C0-BA1E-069B44E23C7A}" name="PZ1 - 50m Retten" dataDxfId="42"/>
-    <tableColumn id="14" xr3:uid="{70529619-443E-40D3-88C1-3E0F00BB2A50}" name="PZ1 - 100m Retten" dataDxfId="41"/>
-    <tableColumn id="15" xr3:uid="{EFA92FD2-C23F-42B3-83DC-5036513F19AF}" name="PZ1 - 100m Kombi" dataDxfId="40"/>
-    <tableColumn id="16" xr3:uid="{03309E52-8CF3-4E90-9EE6-A818901C3B32}" name="PZ1 - 100m Lifesaver" dataDxfId="39"/>
-    <tableColumn id="17" xr3:uid="{00B22013-AA11-4C17-9250-22060AE4B0A8}" name="PZ1 - 200m Super-Lifesaver" dataDxfId="38"/>
-    <tableColumn id="18" xr3:uid="{7E3508A9-0422-4561-A23E-53E613259B24}" name="PZ1 - 200m Hindernis" dataDxfId="37"/>
-    <tableColumn id="19" xr3:uid="{5CEA435F-F34B-4D8D-88D0-F5EBFF18B713}" name="PZ2 - 50m Retten" dataDxfId="36"/>
-    <tableColumn id="20" xr3:uid="{8585BE62-F7C4-4D5D-B287-052B43B08610}" name="PZ2 - 100m Retten" dataDxfId="35"/>
-    <tableColumn id="21" xr3:uid="{D981758B-ADAD-4E36-B787-0B0FDA808CA2}" name="PZ2 - 100m Kombi" dataDxfId="34"/>
-    <tableColumn id="22" xr3:uid="{1D4970A8-D22F-4962-934C-AEA295ED687A}" name="PZ2 - 100m Lifesaver" dataDxfId="33"/>
-    <tableColumn id="23" xr3:uid="{BE394430-C58F-4690-9615-44475E5AF9F8}" name="PZ2 - 200m Super-Lifesaver" dataDxfId="32"/>
-    <tableColumn id="24" xr3:uid="{A7036B1A-99CE-4F7C-AAB8-12E8B2696202}" name="PZ2 - 200m Hindernis" dataDxfId="31"/>
+    <tableColumn id="1" xr3:uid="{021DA6E1-2C93-4474-9720-B6F016186D61}" name="Tabellen Name" dataDxfId="49"/>
+    <tableColumn id="2" xr3:uid="{733C1722-A9C9-4830-A9E2-FE62E96BCD98}" name="Geschlecht" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{80C0BF46-0E43-4947-BF86-B808C324772A}" name="Mindest Alter" dataDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{DBA2A923-EEB7-43F9-A1A3-E78624448FB9}" name="Maximales Alter" dataDxfId="46"/>
+    <tableColumn id="5" xr3:uid="{3FDEE18A-328D-45AE-907D-69A916A93345}" name="Qualizeitraum anfang" dataDxfId="45"/>
+    <tableColumn id="6" xr3:uid="{BE002D7F-575F-4B60-9251-C71D93F59045}" name="Qualizeitraum Ende" dataDxfId="44"/>
+    <tableColumn id="7" xr3:uid="{208ABD57-DE4B-41D6-B9FC-93F2D8966E8D}" name="Letzter Wettkampf am" dataDxfId="43"/>
+    <tableColumn id="8" xr3:uid="{30C9697C-6550-4996-ADDB-7FEE5325B794}" name="Landesverband" dataDxfId="42"/>
+    <tableColumn id="9" xr3:uid="{ED2DAB77-EF46-4D8B-B8E4-90412E32E277}" name="OMS" dataDxfId="41"/>
+    <tableColumn id="10" xr3:uid="{AD534940-A91B-4A6E-9606-E3F3E517D401}" name="Pool-Länge" dataDxfId="40"/>
+    <tableColumn id="11" xr3:uid="{11F9D5D5-72FE-42CA-8624-01D513B4140F}" name="Regelwerk" dataDxfId="39"/>
+    <tableColumn id="12" xr3:uid="{3907872B-5438-4FBF-A045-3EF9EAACFC47}" name="Seiten Anzahl" dataDxfId="38"/>
+    <tableColumn id="13" xr3:uid="{FC821324-3638-40C0-BA1E-069B44E23C7A}" name="PZ1 - 50m Retten" dataDxfId="37"/>
+    <tableColumn id="14" xr3:uid="{70529619-443E-40D3-88C1-3E0F00BB2A50}" name="PZ1 - 100m Retten" dataDxfId="36"/>
+    <tableColumn id="15" xr3:uid="{EFA92FD2-C23F-42B3-83DC-5036513F19AF}" name="PZ1 - 100m Kombi" dataDxfId="35"/>
+    <tableColumn id="16" xr3:uid="{03309E52-8CF3-4E90-9EE6-A818901C3B32}" name="PZ1 - 100m Lifesaver" dataDxfId="34"/>
+    <tableColumn id="17" xr3:uid="{00B22013-AA11-4C17-9250-22060AE4B0A8}" name="PZ1 - 200m Super-Lifesaver" dataDxfId="33"/>
+    <tableColumn id="18" xr3:uid="{7E3508A9-0422-4561-A23E-53E613259B24}" name="PZ1 - 200m Hindernis" dataDxfId="32"/>
+    <tableColumn id="19" xr3:uid="{5CEA435F-F34B-4D8D-88D0-F5EBFF18B713}" name="PZ2 - 50m Retten" dataDxfId="31"/>
+    <tableColumn id="20" xr3:uid="{8585BE62-F7C4-4D5D-B287-052B43B08610}" name="PZ2 - 100m Retten" dataDxfId="30"/>
+    <tableColumn id="21" xr3:uid="{D981758B-ADAD-4E36-B787-0B0FDA808CA2}" name="PZ2 - 100m Kombi" dataDxfId="29"/>
+    <tableColumn id="22" xr3:uid="{1D4970A8-D22F-4962-934C-AEA295ED687A}" name="PZ2 - 100m Lifesaver" dataDxfId="28"/>
+    <tableColumn id="23" xr3:uid="{BE394430-C58F-4690-9615-44475E5AF9F8}" name="PZ2 - 200m Super-Lifesaver" dataDxfId="27"/>
+    <tableColumn id="24" xr3:uid="{A7036B1A-99CE-4F7C-AAB8-12E8B2696202}" name="PZ2 - 200m Hindernis" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4798,12 +4748,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{888CE7BE-8313-44C0-AE38-83992EABD44D}" name="LK_Kalender" displayName="LK_Kalender" ref="A1:H10" totalsRowShown="0">
   <autoFilter ref="A1:H10" xr:uid="{888CE7BE-8313-44C0-AE38-83992EABD44D}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{B26B9E90-F378-41EF-B35E-CE240017E4BE}" name="datum von" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{B26B9E90-F378-41EF-B35E-CE240017E4BE}" name="datum von" dataDxfId="25"/>
     <tableColumn id="2" xr3:uid="{38211212-0A92-428C-895C-E4CA68F52818}" name="datum bis"/>
-    <tableColumn id="3" xr3:uid="{66E541C6-0A5E-4B2D-9B89-5E52F449A4A6}" name="uhrzeit von" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{D93C06A2-29AD-4073-8E3C-A685B4474CC8}" name="uhrzeit bis" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{C5C3979C-B528-44E8-A5A6-36F020A6034F}" name="titel" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{9DC09E1D-44FD-40ED-9EBE-86A8E61C38B2}" name="meta" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{66E541C6-0A5E-4B2D-9B89-5E52F449A4A6}" name="uhrzeit von" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{D93C06A2-29AD-4073-8E3C-A685B4474CC8}" name="uhrzeit bis" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{C5C3979C-B528-44E8-A5A6-36F020A6034F}" name="titel" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{9DC09E1D-44FD-40ED-9EBE-86A8E61C38B2}" name="meta" dataDxfId="21"/>
     <tableColumn id="7" xr3:uid="{E7E62A34-7A76-4361-937D-F4DE76E6E7CC}" name="ort"/>
     <tableColumn id="8" xr3:uid="{84F02734-FC16-406B-ACCA-0CCDF547D94C}" name="kader"/>
   </tableColumns>
@@ -5135,9 +5085,9 @@
       <selection activeCell="Y25" sqref="Y25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.265625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>39</v>
       </c>
@@ -5206,7 +5156,7 @@
       <c r="AV1" s="44"/>
       <c r="AW1" s="44"/>
     </row>
-    <row r="2" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
         <v>40</v>
       </c>
@@ -5273,7 +5223,7 @@
       <c r="AV2" s="45"/>
       <c r="AW2" s="45"/>
     </row>
-    <row r="3" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">
         <v>101</v>
       </c>
@@ -5334,7 +5284,7 @@
       <c r="AV3" s="45"/>
       <c r="AW3" s="45"/>
     </row>
-    <row r="4" spans="1:49" s="53" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:49" s="53" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="49" t="s">
         <v>10</v>
       </c>
@@ -5483,7 +5433,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2000</v>
       </c>
@@ -5536,7 +5486,7 @@
       <c r="AV5" s="10"/>
       <c r="AW5" s="10"/>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f t="shared" ref="A6:A31" si="0">A5+1</f>
         <v>2001</v>
@@ -5614,7 +5564,7 @@
       <c r="AV6" s="11"/>
       <c r="AW6" s="11"/>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>2002</v>
@@ -5692,7 +5642,7 @@
       <c r="AV7" s="10"/>
       <c r="AW7" s="10"/>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>2003</v>
@@ -5770,7 +5720,7 @@
       <c r="AV8" s="11"/>
       <c r="AW8" s="11"/>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>2004</v>
@@ -5848,7 +5798,7 @@
       <c r="AV9" s="10"/>
       <c r="AW9" s="10"/>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>2005</v>
@@ -5926,7 +5876,7 @@
       <c r="AV10" s="11"/>
       <c r="AW10" s="11"/>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>2006</v>
@@ -6004,7 +5954,7 @@
       <c r="AV11" s="10"/>
       <c r="AW11" s="10"/>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>2007</v>
@@ -6126,7 +6076,7 @@
         <v>3.5995370370370369E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>2008</v>
@@ -6248,7 +6198,7 @@
         <v>3.5995370370370369E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>2009</v>
@@ -6370,7 +6320,7 @@
         <v>3.5995370370370369E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>2010</v>
@@ -6492,7 +6442,7 @@
         <v>3.5995370370370369E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>2011</v>
@@ -6626,7 +6576,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>2012</v>
@@ -6760,7 +6710,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>2013</v>
@@ -6894,7 +6844,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>2014</v>
@@ -7028,7 +6978,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>2015</v>
@@ -7162,7 +7112,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>2016</v>
@@ -7296,7 +7246,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>2017</v>
@@ -7430,7 +7380,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>2018</v>
@@ -7564,7 +7514,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>2019</v>
@@ -7698,7 +7648,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>2020</v>
@@ -7848,7 +7798,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>2021</v>
@@ -7998,7 +7948,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>2022</v>
@@ -8148,7 +8098,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>2023</v>
@@ -8298,7 +8248,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>2024</v>
@@ -8448,7 +8398,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>2025</v>
@@ -8598,7 +8548,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>2026</v>
@@ -8750,52 +8700,52 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B5:G31">
-    <cfRule type="expression" dxfId="25" priority="15">
+    <cfRule type="expression" dxfId="20" priority="15">
       <formula>B5&lt;&gt;B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:M31">
-    <cfRule type="expression" dxfId="24" priority="14">
+    <cfRule type="expression" dxfId="19" priority="14">
       <formula>H5&lt;&gt;H4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N5:S31">
-    <cfRule type="expression" dxfId="23" priority="13">
+    <cfRule type="expression" dxfId="18" priority="13">
       <formula>N5&lt;&gt;N4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T5:Y31">
-    <cfRule type="expression" dxfId="22" priority="12">
+    <cfRule type="expression" dxfId="17" priority="12">
       <formula>T5&lt;&gt;T4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z5:AE31">
-    <cfRule type="expression" dxfId="21" priority="9">
+    <cfRule type="expression" dxfId="16" priority="9">
       <formula>Z5&lt;&gt;Z4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF5:AK31">
-    <cfRule type="expression" dxfId="20" priority="8">
+    <cfRule type="expression" dxfId="15" priority="8">
       <formula>AF5&lt;&gt;AF4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AL5:AN31">
-    <cfRule type="expression" dxfId="19" priority="6">
+    <cfRule type="expression" dxfId="14" priority="6">
       <formula>AL5&lt;&gt;AL4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AO5:AQ31">
-    <cfRule type="expression" dxfId="18" priority="5">
+    <cfRule type="expression" dxfId="13" priority="5">
       <formula>AO5&lt;&gt;AO4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AR5:AT31">
-    <cfRule type="expression" dxfId="17" priority="2">
+    <cfRule type="expression" dxfId="12" priority="2">
       <formula>AR5&lt;&gt;AR4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AU5:AW31">
-    <cfRule type="expression" dxfId="16" priority="1">
+    <cfRule type="expression" dxfId="11" priority="1">
       <formula>AU5&lt;&gt;AU4</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8819,15 +8769,15 @@
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.86328125" style="1" customWidth="1"/>
-    <col min="2" max="13" width="18.73046875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
+    <col min="2" max="13" width="18.7109375" style="1" customWidth="1"/>
     <col min="14" max="14" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="11.3984375" style="1"/>
+    <col min="15" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18">
         <v>2024</v>
       </c>
@@ -8871,7 +8821,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
@@ -8927,7 +8877,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -8983,7 +8933,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>8</v>
       </c>
@@ -9039,7 +8989,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="175" t="s">
         <v>13</v>
       </c>
@@ -9057,7 +9007,7 @@
       <c r="M7" s="175"/>
       <c r="N7" s="175"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="175"/>
       <c r="B8" s="175"/>
       <c r="C8" s="175"/>
@@ -9073,7 +9023,7 @@
       <c r="M8" s="175"/>
       <c r="N8" s="175"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>6</v>
       </c>
@@ -9127,7 +9077,7 @@
       </c>
       <c r="N9" s="21"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>7</v>
       </c>
@@ -9181,7 +9131,7 @@
       </c>
       <c r="N10" s="21"/>
     </row>
-    <row r="11" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>8</v>
       </c>
@@ -9235,7 +9185,7 @@
       </c>
       <c r="N11" s="23"/>
     </row>
-    <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="174" t="s">
         <v>14</v>
       </c>
@@ -9256,7 +9206,7 @@
       <c r="M14"/>
       <c r="N14"/>
     </row>
-    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="174"/>
       <c r="B15" s="174"/>
       <c r="C15" s="174"/>
@@ -9271,7 +9221,7 @@
       <c r="M15"/>
       <c r="N15"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -9306,7 +9256,7 @@
       <c r="M16"/>
       <c r="N16"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>19</v>
       </c>
@@ -9341,7 +9291,7 @@
       <c r="M17"/>
       <c r="N17"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>19</v>
       </c>
@@ -9374,7 +9324,7 @@
       <c r="M18"/>
       <c r="N18"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>22</v>
       </c>
@@ -9407,7 +9357,7 @@
       <c r="M19"/>
       <c r="N19"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>24</v>
       </c>
@@ -9438,7 +9388,7 @@
       <c r="M20"/>
       <c r="N20"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>22</v>
       </c>
@@ -9465,7 +9415,7 @@
       <c r="M21"/>
       <c r="N21"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>19</v>
       </c>
@@ -9488,7 +9438,7 @@
       <c r="I22" s="33"/>
       <c r="L22" s="41"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>19</v>
       </c>
@@ -9511,50 +9461,50 @@
       <c r="I23" s="33"/>
       <c r="L23" s="40"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H24" s="33"/>
       <c r="I24" s="33"/>
       <c r="L24" s="41"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H25" s="33"/>
       <c r="I25" s="33"/>
       <c r="L25" s="40"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L26" s="41"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L27" s="40"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L28" s="41"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L29" s="40"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L30" s="41"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L31" s="40"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L32" s="41"/>
     </row>
-    <row r="33" spans="12:12" x14ac:dyDescent="0.45">
+    <row r="33" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L33" s="40"/>
     </row>
-    <row r="34" spans="12:12" x14ac:dyDescent="0.45">
+    <row r="34" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L34" s="41"/>
     </row>
-    <row r="35" spans="12:12" x14ac:dyDescent="0.45">
+    <row r="35" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L35" s="33"/>
     </row>
-    <row r="36" spans="12:12" x14ac:dyDescent="0.45">
+    <row r="36" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L36" s="41"/>
     </row>
-    <row r="37" spans="12:12" x14ac:dyDescent="0.45">
+    <row r="37" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L37" s="33"/>
     </row>
   </sheetData>
@@ -9580,15 +9530,15 @@
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.86328125" style="1" customWidth="1"/>
-    <col min="2" max="13" width="18.73046875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
+    <col min="2" max="13" width="18.7109375" style="1" customWidth="1"/>
     <col min="14" max="14" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="11.3984375" style="1"/>
+    <col min="15" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18">
         <v>2025</v>
       </c>
@@ -9632,7 +9582,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
@@ -9688,7 +9638,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -9744,7 +9694,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>8</v>
       </c>
@@ -9800,7 +9750,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="175" t="s">
         <v>13</v>
       </c>
@@ -9818,7 +9768,7 @@
       <c r="M7" s="175"/>
       <c r="N7" s="175"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="175"/>
       <c r="B8" s="175"/>
       <c r="C8" s="175"/>
@@ -9834,7 +9784,7 @@
       <c r="M8" s="175"/>
       <c r="N8" s="175"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>6</v>
       </c>
@@ -9888,7 +9838,7 @@
       </c>
       <c r="N9" s="21"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>7</v>
       </c>
@@ -9942,7 +9892,7 @@
       </c>
       <c r="N10" s="21"/>
     </row>
-    <row r="11" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>8</v>
       </c>
@@ -9996,7 +9946,7 @@
       </c>
       <c r="N11" s="23"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="174" t="s">
         <v>14</v>
       </c>
@@ -10015,7 +9965,7 @@
       </c>
       <c r="M14"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="174"/>
       <c r="B15" s="174"/>
       <c r="C15" s="174"/>
@@ -10028,7 +9978,7 @@
       <c r="L15" s="176"/>
       <c r="M15"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -10061,7 +10011,7 @@
       </c>
       <c r="M16"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>28</v>
       </c>
@@ -10094,7 +10044,7 @@
       </c>
       <c r="M17"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>28</v>
       </c>
@@ -10125,7 +10075,7 @@
       <c r="L18" s="38"/>
       <c r="M18"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>29</v>
       </c>
@@ -10156,7 +10106,7 @@
       <c r="L19" s="36"/>
       <c r="M19"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>30</v>
       </c>
@@ -10185,7 +10135,7 @@
       <c r="L20" s="38"/>
       <c r="M20"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>29</v>
       </c>
@@ -10216,7 +10166,7 @@
       <c r="L21" s="36"/>
       <c r="M21"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>28</v>
       </c>
@@ -10247,7 +10197,7 @@
       <c r="L22" s="39"/>
       <c r="M22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>28</v>
       </c>
@@ -10278,66 +10228,66 @@
       <c r="L23" s="37"/>
       <c r="M23"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H24" s="40"/>
       <c r="I24" s="40"/>
       <c r="J24" s="40"/>
       <c r="L24" s="39"/>
       <c r="M24"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H25" s="33"/>
       <c r="I25" s="33"/>
       <c r="L25" s="37"/>
       <c r="M25"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L26" s="39"/>
       <c r="M26"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L27" s="37"/>
       <c r="M27"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L28" s="39"/>
       <c r="M28"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L29" s="37"/>
       <c r="M29"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L30" s="39"/>
       <c r="M30"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L31" s="37"/>
       <c r="M31"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L32" s="39"/>
       <c r="M32"/>
     </row>
-    <row r="33" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="33" spans="8:13" x14ac:dyDescent="0.25">
       <c r="L33" s="37"/>
       <c r="M33"/>
     </row>
-    <row r="34" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="34" spans="8:13" x14ac:dyDescent="0.25">
       <c r="L34" s="39"/>
       <c r="M34"/>
     </row>
-    <row r="35" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="35" spans="8:13" x14ac:dyDescent="0.25">
       <c r="M35"/>
     </row>
-    <row r="36" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="36" spans="8:13" x14ac:dyDescent="0.25">
       <c r="L36" s="39"/>
       <c r="M36"/>
     </row>
-    <row r="37" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="37" spans="8:13" x14ac:dyDescent="0.25">
       <c r="M37"/>
     </row>
-    <row r="38" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="38" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H38"/>
       <c r="I38"/>
       <c r="J38"/>
@@ -10345,7 +10295,7 @@
       <c r="L38"/>
       <c r="M38"/>
     </row>
-    <row r="39" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="39" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H39"/>
       <c r="I39"/>
       <c r="J39"/>
@@ -10376,15 +10326,15 @@
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.86328125" style="1" customWidth="1"/>
-    <col min="2" max="13" width="18.73046875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
+    <col min="2" max="13" width="18.7109375" style="1" customWidth="1"/>
     <col min="14" max="14" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="11.3984375" style="1"/>
+    <col min="15" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18">
         <v>2026</v>
       </c>
@@ -10428,7 +10378,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
@@ -10484,7 +10434,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -10540,7 +10490,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>8</v>
       </c>
@@ -10596,7 +10546,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="175" t="s">
         <v>13</v>
       </c>
@@ -10614,7 +10564,7 @@
       <c r="M7" s="175"/>
       <c r="N7" s="175"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="175"/>
       <c r="B8" s="175"/>
       <c r="C8" s="175"/>
@@ -10630,7 +10580,7 @@
       <c r="M8" s="175"/>
       <c r="N8" s="175"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>6</v>
       </c>
@@ -10684,7 +10634,7 @@
       </c>
       <c r="N9" s="21"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>7</v>
       </c>
@@ -10738,7 +10688,7 @@
       </c>
       <c r="N10" s="21"/>
     </row>
-    <row r="11" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>8</v>
       </c>
@@ -10792,7 +10742,7 @@
       </c>
       <c r="N11" s="23"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="174" t="s">
         <v>14</v>
       </c>
@@ -10811,7 +10761,7 @@
       </c>
       <c r="M14"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="174"/>
       <c r="B15" s="174"/>
       <c r="C15" s="174"/>
@@ -10824,7 +10774,7 @@
       <c r="L15" s="176"/>
       <c r="M15"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -10857,7 +10807,7 @@
       </c>
       <c r="M16"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>28</v>
       </c>
@@ -10890,7 +10840,7 @@
       </c>
       <c r="M17"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>28</v>
       </c>
@@ -10921,7 +10871,7 @@
       <c r="L18" s="38"/>
       <c r="M18"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>29</v>
       </c>
@@ -10952,7 +10902,7 @@
       <c r="L19" s="36"/>
       <c r="M19"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>30</v>
       </c>
@@ -10981,7 +10931,7 @@
       <c r="L20" s="38"/>
       <c r="M20"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>29</v>
       </c>
@@ -11012,7 +10962,7 @@
       <c r="L21" s="36"/>
       <c r="M21"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>28</v>
       </c>
@@ -11043,7 +10993,7 @@
       <c r="L22" s="39"/>
       <c r="M22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>28</v>
       </c>
@@ -11074,66 +11024,66 @@
       <c r="L23" s="37"/>
       <c r="M23"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H24" s="40"/>
       <c r="I24" s="40"/>
       <c r="J24" s="40"/>
       <c r="L24" s="39"/>
       <c r="M24"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H25" s="33"/>
       <c r="I25" s="33"/>
       <c r="L25" s="37"/>
       <c r="M25"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L26" s="39"/>
       <c r="M26"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L27" s="37"/>
       <c r="M27"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L28" s="39"/>
       <c r="M28"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L29" s="37"/>
       <c r="M29"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L30" s="39"/>
       <c r="M30"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L31" s="37"/>
       <c r="M31"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L32" s="39"/>
       <c r="M32"/>
     </row>
-    <row r="33" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="33" spans="8:13" x14ac:dyDescent="0.25">
       <c r="L33" s="37"/>
       <c r="M33"/>
     </row>
-    <row r="34" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="34" spans="8:13" x14ac:dyDescent="0.25">
       <c r="L34" s="39"/>
       <c r="M34"/>
     </row>
-    <row r="35" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="35" spans="8:13" x14ac:dyDescent="0.25">
       <c r="M35"/>
     </row>
-    <row r="36" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="36" spans="8:13" x14ac:dyDescent="0.25">
       <c r="L36" s="39"/>
       <c r="M36"/>
     </row>
-    <row r="37" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="37" spans="8:13" x14ac:dyDescent="0.25">
       <c r="M37"/>
     </row>
-    <row r="38" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="38" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H38"/>
       <c r="I38"/>
       <c r="J38"/>
@@ -11141,7 +11091,7 @@
       <c r="L38"/>
       <c r="M38"/>
     </row>
-    <row r="39" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="39" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H39"/>
       <c r="I39"/>
       <c r="J39"/>
@@ -11170,17 +11120,17 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.265625" customWidth="1"/>
-    <col min="2" max="5" width="18.73046875" customWidth="1"/>
-    <col min="6" max="6" width="21.1328125" customWidth="1"/>
-    <col min="7" max="11" width="18.73046875" customWidth="1"/>
-    <col min="12" max="12" width="22.1328125" customWidth="1"/>
-    <col min="13" max="13" width="18.73046875" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="7" max="11" width="18.7109375" customWidth="1"/>
+    <col min="12" max="12" width="22.140625" customWidth="1"/>
+    <col min="13" max="13" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>39</v>
       </c>
@@ -11221,7 +11171,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
         <v>40</v>
       </c>
@@ -11262,7 +11212,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">
         <v>41</v>
       </c>
@@ -11303,7 +11253,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -11344,7 +11294,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2000</v>
       </c>
@@ -11361,7 +11311,7 @@
       <c r="L5" s="11"/>
       <c r="M5" s="11"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f t="shared" ref="A6:A32" si="0">A5+1</f>
         <v>2001</v>
@@ -11379,7 +11329,7 @@
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>2002</v>
@@ -11397,7 +11347,7 @@
       <c r="L7" s="11"/>
       <c r="M7" s="11"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>2003</v>
@@ -11415,7 +11365,7 @@
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>2004</v>
@@ -11433,7 +11383,7 @@
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>2005</v>
@@ -11451,7 +11401,7 @@
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>2006</v>
@@ -11469,7 +11419,7 @@
       <c r="L11" s="11"/>
       <c r="M11" s="11"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>2007</v>
@@ -11487,7 +11437,7 @@
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>2008</v>
@@ -11505,7 +11455,7 @@
       <c r="L13" s="11"/>
       <c r="M13" s="11"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>2009</v>
@@ -11523,7 +11473,7 @@
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>2010</v>
@@ -11541,7 +11491,7 @@
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>2011</v>
@@ -11559,7 +11509,7 @@
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>2012</v>
@@ -11577,7 +11527,7 @@
       <c r="L17" s="11"/>
       <c r="M17" s="11"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>2013</v>
@@ -11595,7 +11545,7 @@
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>2014</v>
@@ -11613,7 +11563,7 @@
       <c r="L19" s="11"/>
       <c r="M19" s="11"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>2015</v>
@@ -11655,7 +11605,7 @@
         <v>1.3592592592592591E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>2016</v>
@@ -11697,7 +11647,7 @@
         <v>1.3592592592592591E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>2017</v>
@@ -11739,7 +11689,7 @@
         <v>1.3577546296296298E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>2018</v>
@@ -11781,7 +11731,7 @@
         <v>1.3577546296296298E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>2019</v>
@@ -11823,7 +11773,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>2020</v>
@@ -11865,7 +11815,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>2021</v>
@@ -11907,7 +11857,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>2022</v>
@@ -11949,7 +11899,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>2023</v>
@@ -11991,7 +11941,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>2024</v>
@@ -12033,7 +11983,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>2025</v>
@@ -12075,7 +12025,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>2026</v>
@@ -12117,7 +12067,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <f t="shared" si="0"/>
         <v>2027</v>
@@ -12161,22 +12111,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B6:G6">
-    <cfRule type="expression" dxfId="15" priority="20">
+    <cfRule type="expression" dxfId="10" priority="20">
       <formula>B6&lt;&gt;B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:G32">
-    <cfRule type="expression" dxfId="14" priority="1">
+    <cfRule type="expression" dxfId="9" priority="1">
       <formula>B7&lt;&gt;B6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:M6">
-    <cfRule type="expression" dxfId="13" priority="22">
+    <cfRule type="expression" dxfId="8" priority="22">
       <formula>H6&lt;&gt;H4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:M32">
-    <cfRule type="expression" dxfId="12" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>H7&lt;&gt;H6</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12197,17 +12147,17 @@
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.86328125" customWidth="1"/>
-    <col min="2" max="5" width="18.73046875" customWidth="1"/>
-    <col min="6" max="6" width="21.1328125" customWidth="1"/>
-    <col min="7" max="11" width="18.73046875" customWidth="1"/>
-    <col min="12" max="12" width="22.1328125" customWidth="1"/>
-    <col min="13" max="13" width="18.73046875" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="7" max="11" width="18.7109375" customWidth="1"/>
+    <col min="12" max="12" width="22.140625" customWidth="1"/>
+    <col min="13" max="13" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>39</v>
       </c>
@@ -12248,7 +12198,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
         <v>40</v>
       </c>
@@ -12289,7 +12239,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">
         <v>41</v>
       </c>
@@ -12330,7 +12280,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -12371,7 +12321,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2000</v>
       </c>
@@ -12388,7 +12338,7 @@
       <c r="L5" s="38"/>
       <c r="M5" s="38"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f t="shared" ref="A6:A31" si="0">A5+1</f>
         <v>2001</v>
@@ -12418,7 +12368,7 @@
         <v>1.3629629629629632E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>2002</v>
@@ -12460,7 +12410,7 @@
         <v>1.3629629629629632E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>2003</v>
@@ -12502,7 +12452,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>2004</v>
@@ -12544,7 +12494,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>2005</v>
@@ -12586,7 +12536,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>2006</v>
@@ -12628,7 +12578,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>2007</v>
@@ -12670,7 +12620,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>2008</v>
@@ -12712,7 +12662,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>2009</v>
@@ -12754,7 +12704,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>2010</v>
@@ -12796,7 +12746,7 @@
         <v>1.3306712962962966E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>2011</v>
@@ -12838,7 +12788,7 @@
         <v>1.3306712962962966E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>2012</v>
@@ -12880,7 +12830,7 @@
         <v>1.3306712962962966E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>2013</v>
@@ -12922,7 +12872,7 @@
         <v>1.312962962962963E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>2014</v>
@@ -12964,7 +12914,7 @@
         <v>1.312962962962963E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>2015</v>
@@ -13006,7 +12956,7 @@
         <v>1.3116898148148148E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>2016</v>
@@ -13048,7 +12998,7 @@
         <v>1.3116898148148148E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>2017</v>
@@ -13090,7 +13040,7 @@
         <v>1.3116898148148148E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>2018</v>
@@ -13132,7 +13082,7 @@
         <v>1.3116898148148148E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>2019</v>
@@ -13174,7 +13124,7 @@
         <v>1.3116898148148148E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>2020</v>
@@ -13216,7 +13166,7 @@
         <v>1.3097222222222223E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>2021</v>
@@ -13258,7 +13208,7 @@
         <v>1.3097222222222223E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>2022</v>
@@ -13300,7 +13250,7 @@
         <v>1.3097222222222223E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>2023</v>
@@ -13342,7 +13292,7 @@
         <v>1.3097222222222223E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>2024</v>
@@ -13384,7 +13334,7 @@
         <v>1.3097222222222223E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>2025</v>
@@ -13426,7 +13376,7 @@
         <v>1.2931712962962962E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>2026</v>
@@ -13468,7 +13418,7 @@
         <v>1.2931712962962962E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <f>A31+1</f>
         <v>2027</v>
@@ -13512,22 +13462,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B6:G6">
-    <cfRule type="expression" dxfId="11" priority="19">
+    <cfRule type="expression" dxfId="6" priority="19">
       <formula>B6&lt;&gt;B4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B7:G32">
-    <cfRule type="expression" dxfId="10" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>B7&lt;&gt;B6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:M6">
-    <cfRule type="expression" dxfId="9" priority="20">
+    <cfRule type="expression" dxfId="4" priority="20">
       <formula>H6&lt;&gt;H4</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H7:M32">
-    <cfRule type="expression" dxfId="8" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>H7&lt;&gt;H6</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13550,30 +13500,30 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.73046875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.73046875" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
     <col min="15" max="16" width="19" customWidth="1"/>
-    <col min="17" max="17" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="22.265625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.73046875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="47.265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="47.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="60" t="s">
         <v>161</v>
       </c>
@@ -13638,7 +13588,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="59" t="s">
         <v>197</v>
       </c>
@@ -13699,7 +13649,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="59" t="s">
         <v>198</v>
       </c>
@@ -13779,30 +13729,30 @@
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.73046875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.73046875" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
     <col min="15" max="16" width="19" customWidth="1"/>
-    <col min="17" max="17" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="22.265625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.73046875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="47.265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="47.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="60" t="s">
         <v>161</v>
       </c>
@@ -13867,7 +13817,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="59" t="s">
         <v>189</v>
       </c>
@@ -13881,7 +13831,7 @@
         <v>50</v>
       </c>
       <c r="E2" s="59" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F2" s="59" t="s">
         <v>195</v>
@@ -13928,7 +13878,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="59" t="s">
         <v>190</v>
       </c>
@@ -13942,7 +13892,7 @@
         <v>50</v>
       </c>
       <c r="E3" s="59" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F3" s="59" t="s">
         <v>195</v>
@@ -13989,7 +13939,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
         <v>191</v>
       </c>
@@ -14003,7 +13953,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="59" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F4" s="59" t="s">
         <v>195</v>
@@ -14047,10 +13997,10 @@
         <v>10</v>
       </c>
       <c r="U4" s="59" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
         <v>192</v>
       </c>
@@ -14064,7 +14014,7 @@
         <v>18</v>
       </c>
       <c r="E5" s="59" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F5" s="59" t="s">
         <v>195</v>
@@ -14109,7 +14059,7 @@
       </c>
       <c r="U5" s="59"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="59" t="s">
         <v>193</v>
       </c>
@@ -14123,7 +14073,7 @@
         <v>16</v>
       </c>
       <c r="E6" s="59" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F6" s="59" t="s">
         <v>195</v>
@@ -14168,7 +14118,7 @@
       </c>
       <c r="U6" s="59"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="59" t="s">
         <v>194</v>
       </c>
@@ -14182,7 +14132,7 @@
         <v>16</v>
       </c>
       <c r="E7" s="59" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="F7" s="59" t="s">
         <v>195</v>
@@ -14246,35 +14196,35 @@
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.86328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.73046875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.86328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.73046875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.3984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.1328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.86328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.86328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.3984375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.1328125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="24.86328125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.86328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="59" t="s">
         <v>161</v>
       </c>
@@ -14348,7 +14298,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="59" t="s">
         <v>212</v>
       </c>
@@ -14418,7 +14368,7 @@
         <v>1.9623842592592592E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="59" t="s">
         <v>213</v>
       </c>
@@ -14488,7 +14438,7 @@
         <v>1.8121527777777778E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
         <v>214</v>
       </c>
@@ -14558,7 +14508,7 @@
         <v>1.9979166666666665E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
         <v>215</v>
       </c>
@@ -14628,7 +14578,7 @@
         <v>1.7653935185185186E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="59" t="s">
         <v>189</v>
       </c>
@@ -14698,7 +14648,7 @@
         <v>1.8998842592592594E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="59" t="s">
         <v>190</v>
       </c>
@@ -14783,39 +14733,39 @@
   </sheetPr>
   <dimension ref="A1:X15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
+    <sheetView zoomScale="83" workbookViewId="0">
       <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.73046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.59765625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.265625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.59765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="27" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="22" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.59765625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.265625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21.59765625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="27" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="59" t="s">
         <v>161</v>
       </c>
@@ -14889,7 +14839,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="59" t="s">
         <v>223</v>
       </c>
@@ -14959,7 +14909,7 @@
         <v>1.8332175925925925E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="59" t="s">
         <v>224</v>
       </c>
@@ -15029,9 +14979,9 @@
         <v>1.7003472222222222E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B4" s="59" t="s">
         <v>182</v>
@@ -15105,9 +15055,9 @@
         <v>3.9324537037037035E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B5" s="59" t="s">
         <v>182</v>
@@ -15181,9 +15131,9 @@
         <v>4.0693981481481478E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="59" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B6" s="59" t="s">
         <v>182</v>
@@ -15257,9 +15207,9 @@
         <v>4.1888888888888884E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="59" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B7" s="59" t="s">
         <v>164</v>
@@ -15333,9 +15283,9 @@
         <v>4.7436458333333331E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="59" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B8" s="59" t="s">
         <v>164</v>
@@ -15409,9 +15359,9 @@
         <v>4.9196875E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="59" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B9" s="59" t="s">
         <v>164</v>
@@ -15485,9 +15435,9 @@
         <v>5.1593750000000001E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="59" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B10" s="59" t="s">
         <v>182</v>
@@ -15561,9 +15511,9 @@
         <v>4.4791666666666667E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="59" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B11" s="59" t="s">
         <v>182</v>
@@ -15637,9 +15587,9 @@
         <v>4.619444444444444E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="59" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B12" s="59" t="s">
         <v>182</v>
@@ -15713,9 +15663,9 @@
         <v>4.7138888888888881E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="59" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B13" s="59" t="s">
         <v>164</v>
@@ -15789,9 +15739,9 @@
         <v>5.3782870370370367E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="59" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B14" s="59" t="s">
         <v>164</v>
@@ -15865,9 +15815,9 @@
         <v>5.5107638888888882E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="59" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B15" s="59" t="s">
         <v>164</v>
@@ -15956,22 +15906,22 @@
   </sheetPr>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.9296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="84.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="84.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>225</v>
       </c>
@@ -15997,7 +15947,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="70">
         <v>46075</v>
       </c>
@@ -16020,7 +15970,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="70">
         <v>46075</v>
       </c>
@@ -16034,16 +15984,16 @@
         <v>237</v>
       </c>
       <c r="F3" s="72" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G3" t="s">
         <v>233</v>
       </c>
       <c r="H3" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="70">
         <v>46124</v>
       </c>
@@ -16066,7 +16016,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="70">
         <v>46124</v>
       </c>
@@ -16080,16 +16030,16 @@
         <v>237</v>
       </c>
       <c r="F5" s="72" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G5" t="s">
         <v>233</v>
       </c>
       <c r="H5" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="70">
         <v>46186</v>
       </c>
@@ -16103,16 +16053,16 @@
         <v>237</v>
       </c>
       <c r="F6" s="72" t="s">
+        <v>239</v>
+      </c>
+      <c r="G6" t="s">
         <v>240</v>
       </c>
-      <c r="G6" t="s">
-        <v>241</v>
-      </c>
       <c r="H6" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="70">
         <v>46187</v>
       </c>
@@ -16126,7 +16076,7 @@
         <v>232</v>
       </c>
       <c r="F7" s="72" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G7" t="s">
         <v>233</v>
@@ -16135,12 +16085,12 @@
         <v>234</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="70">
         <v>46199</v>
       </c>
       <c r="B8" s="70">
-        <v>46204</v>
+        <v>46203</v>
       </c>
       <c r="C8" s="71">
         <v>0</v>
@@ -16149,19 +16099,19 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="E8" s="72" t="s">
+        <v>242</v>
+      </c>
+      <c r="F8" s="72" t="s">
         <v>243</v>
       </c>
-      <c r="F8" s="72" t="s">
+      <c r="G8" t="s">
         <v>244</v>
       </c>
-      <c r="G8" t="s">
-        <v>245</v>
-      </c>
       <c r="H8" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="70">
         <v>46207</v>
       </c>
@@ -16172,19 +16122,19 @@
         <v>0.75</v>
       </c>
       <c r="E9" s="72" t="s">
+        <v>245</v>
+      </c>
+      <c r="F9" s="72" t="s">
         <v>246</v>
       </c>
-      <c r="F9" s="72" t="s">
+      <c r="G9" t="s">
         <v>247</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>248</v>
       </c>
-      <c r="H9" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="70">
         <v>46228</v>
       </c>
@@ -16195,21 +16145,21 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="E10" s="72" t="s">
+        <v>249</v>
+      </c>
+      <c r="F10" s="72" t="s">
         <v>250</v>
       </c>
-      <c r="F10" s="72" t="s">
+      <c r="G10" t="s">
         <v>251</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>252</v>
-      </c>
-      <c r="H10" t="s">
-        <v>253</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:H10">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>$A2&lt;TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16229,147 +16179,147 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" customWidth="1"/>
-    <col min="2" max="2" width="32.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="26" width="9.59765625" customWidth="1"/>
-    <col min="28" max="28" width="32.3984375" bestFit="1" customWidth="1"/>
-    <col min="29" max="52" width="4.59765625" customWidth="1"/>
-    <col min="54" max="54" width="32.3984375" bestFit="1" customWidth="1"/>
-    <col min="55" max="78" width="9.59765625" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="26" width="9.5703125" customWidth="1"/>
+    <col min="28" max="28" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="52" width="4.5703125" customWidth="1"/>
+    <col min="54" max="54" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="55" max="78" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="140">
+    <row r="1" spans="1:78" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="159">
         <v>2025</v>
       </c>
       <c r="B1" s="79" t="str">
         <f ca="1">CONCATENATE("in: ",YEAR(TODAY())-1," für: ", YEAR(TODAY()))</f>
         <v>in: 2025 für: 2026</v>
       </c>
-      <c r="C1" s="141" t="s">
+      <c r="C1" s="140" t="s">
+        <v>256</v>
+      </c>
+      <c r="D1" s="140"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="144" t="s">
         <v>257</v>
       </c>
-      <c r="D1" s="141"/>
-      <c r="E1" s="142"/>
-      <c r="F1" s="143" t="s">
+      <c r="G1" s="145"/>
+      <c r="H1" s="145"/>
+      <c r="I1" s="145"/>
+      <c r="J1" s="146"/>
+      <c r="K1" s="150" t="s">
+        <v>261</v>
+      </c>
+      <c r="L1" s="151"/>
+      <c r="M1" s="151"/>
+      <c r="N1" s="152"/>
+      <c r="O1" s="142" t="s">
         <v>258</v>
       </c>
-      <c r="G1" s="144"/>
-      <c r="H1" s="144"/>
-      <c r="I1" s="144"/>
-      <c r="J1" s="145"/>
-      <c r="K1" s="146" t="s">
+      <c r="P1" s="142"/>
+      <c r="Q1" s="143"/>
+      <c r="R1" s="156" t="s">
+        <v>259</v>
+      </c>
+      <c r="S1" s="157"/>
+      <c r="T1" s="157"/>
+      <c r="U1" s="157"/>
+      <c r="V1" s="158"/>
+      <c r="W1" s="153" t="s">
         <v>262</v>
       </c>
-      <c r="L1" s="147"/>
-      <c r="M1" s="147"/>
-      <c r="N1" s="148"/>
-      <c r="O1" s="149" t="s">
-        <v>259</v>
-      </c>
-      <c r="P1" s="149"/>
-      <c r="Q1" s="150"/>
-      <c r="R1" s="151" t="s">
-        <v>260</v>
-      </c>
-      <c r="S1" s="152"/>
-      <c r="T1" s="152"/>
-      <c r="U1" s="152"/>
-      <c r="V1" s="153"/>
-      <c r="W1" s="154" t="s">
-        <v>263</v>
-      </c>
-      <c r="X1" s="155"/>
-      <c r="Y1" s="155"/>
-      <c r="Z1" s="156"/>
+      <c r="X1" s="154"/>
+      <c r="Y1" s="154"/>
+      <c r="Z1" s="155"/>
       <c r="AA1"/>
       <c r="AB1" s="79" t="str">
         <f ca="1">CONCATENATE("in: ",YEAR(TODAY())-1," für: ", YEAR(TODAY()))</f>
         <v>in: 2025 für: 2026</v>
       </c>
-      <c r="AC1" s="157" t="s">
+      <c r="AC1" s="160" t="s">
+        <v>263</v>
+      </c>
+      <c r="AD1" s="160"/>
+      <c r="AE1" s="161"/>
+      <c r="AF1" s="162" t="s">
         <v>264</v>
       </c>
-      <c r="AD1" s="157"/>
-      <c r="AE1" s="158"/>
-      <c r="AF1" s="159" t="s">
+      <c r="AG1" s="163"/>
+      <c r="AH1" s="163"/>
+      <c r="AI1" s="163"/>
+      <c r="AJ1" s="164"/>
+      <c r="AK1" s="165" t="s">
         <v>265</v>
       </c>
-      <c r="AG1" s="160"/>
-      <c r="AH1" s="160"/>
-      <c r="AI1" s="160"/>
-      <c r="AJ1" s="161"/>
-      <c r="AK1" s="162" t="s">
+      <c r="AL1" s="166"/>
+      <c r="AM1" s="166"/>
+      <c r="AN1" s="167"/>
+      <c r="AO1" s="168" t="s">
         <v>266</v>
       </c>
-      <c r="AL1" s="163"/>
-      <c r="AM1" s="163"/>
-      <c r="AN1" s="164"/>
-      <c r="AO1" s="165" t="s">
+      <c r="AP1" s="169"/>
+      <c r="AQ1" s="170"/>
+      <c r="AR1" s="171" t="s">
         <v>267</v>
       </c>
-      <c r="AP1" s="166"/>
-      <c r="AQ1" s="167"/>
-      <c r="AR1" s="168" t="s">
+      <c r="AS1" s="172"/>
+      <c r="AT1" s="172"/>
+      <c r="AU1" s="172"/>
+      <c r="AV1" s="173"/>
+      <c r="AW1" s="147" t="s">
         <v>268</v>
       </c>
-      <c r="AS1" s="169"/>
-      <c r="AT1" s="169"/>
-      <c r="AU1" s="169"/>
-      <c r="AV1" s="170"/>
-      <c r="AW1" s="171" t="s">
-        <v>269</v>
-      </c>
-      <c r="AX1" s="172"/>
-      <c r="AY1" s="172"/>
-      <c r="AZ1" s="173"/>
+      <c r="AX1" s="148"/>
+      <c r="AY1" s="148"/>
+      <c r="AZ1" s="149"/>
       <c r="BB1" s="79" t="str">
         <f ca="1">CONCATENATE("in: ",YEAR(TODAY())-1," für: ", YEAR(TODAY()))</f>
         <v>in: 2025 für: 2026</v>
       </c>
-      <c r="BC1" s="141" t="s">
+      <c r="BC1" s="140" t="s">
+        <v>269</v>
+      </c>
+      <c r="BD1" s="140"/>
+      <c r="BE1" s="141"/>
+      <c r="BF1" s="144" t="s">
         <v>270</v>
       </c>
-      <c r="BD1" s="141"/>
-      <c r="BE1" s="142"/>
-      <c r="BF1" s="143" t="s">
+      <c r="BG1" s="145"/>
+      <c r="BH1" s="145"/>
+      <c r="BI1" s="145"/>
+      <c r="BJ1" s="146"/>
+      <c r="BK1" s="150" t="s">
         <v>271</v>
       </c>
-      <c r="BG1" s="144"/>
-      <c r="BH1" s="144"/>
-      <c r="BI1" s="144"/>
-      <c r="BJ1" s="145"/>
-      <c r="BK1" s="146" t="s">
+      <c r="BL1" s="151"/>
+      <c r="BM1" s="151"/>
+      <c r="BN1" s="152"/>
+      <c r="BO1" s="142" t="s">
+        <v>258</v>
+      </c>
+      <c r="BP1" s="142"/>
+      <c r="BQ1" s="143"/>
+      <c r="BR1" s="156" t="s">
+        <v>259</v>
+      </c>
+      <c r="BS1" s="157"/>
+      <c r="BT1" s="157"/>
+      <c r="BU1" s="157"/>
+      <c r="BV1" s="158"/>
+      <c r="BW1" s="153" t="s">
         <v>272</v>
       </c>
-      <c r="BL1" s="147"/>
-      <c r="BM1" s="147"/>
-      <c r="BN1" s="148"/>
-      <c r="BO1" s="149" t="s">
-        <v>259</v>
-      </c>
-      <c r="BP1" s="149"/>
-      <c r="BQ1" s="150"/>
-      <c r="BR1" s="151" t="s">
+      <c r="BX1" s="154"/>
+      <c r="BY1" s="154"/>
+      <c r="BZ1" s="155"/>
+    </row>
+    <row r="2" spans="1:78" s="128" customFormat="1" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="159"/>
+      <c r="B2" s="80" t="s">
         <v>260</v>
-      </c>
-      <c r="BS1" s="152"/>
-      <c r="BT1" s="152"/>
-      <c r="BU1" s="152"/>
-      <c r="BV1" s="153"/>
-      <c r="BW1" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="BX1" s="155"/>
-      <c r="BY1" s="155"/>
-      <c r="BZ1" s="156"/>
-    </row>
-    <row r="2" spans="1:78" s="128" customFormat="1" ht="21.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="140"/>
-      <c r="B2" s="80" t="s">
-        <v>261</v>
       </c>
       <c r="C2" s="75" t="str">
         <f ca="1">CONCATENATE("≤",YEAR(TODAY())-15-1)</f>
@@ -16469,7 +16419,7 @@
       </c>
       <c r="AA2"/>
       <c r="AB2" s="80" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AC2" s="114" t="str">
         <f ca="1">CONCATENATE("≤",YEAR(TODAY())-15)</f>
@@ -16568,7 +16518,7 @@
         <v>2002-1986</v>
       </c>
       <c r="BB2" s="80" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="BC2" s="92" t="str">
         <f ca="1">CONCATENATE("≤",YEAR(TODAY())-15-1)</f>
@@ -16667,8 +16617,8 @@
         <v>2001-1985</v>
       </c>
     </row>
-    <row r="3" spans="1:78" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="140"/>
+    <row r="3" spans="1:78" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="159"/>
       <c r="B3" s="81" t="s">
         <v>0</v>
       </c>
@@ -16920,8 +16870,8 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:78" x14ac:dyDescent="0.45">
-      <c r="A4" s="140"/>
+    <row r="4" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="A4" s="159"/>
       <c r="B4" s="81" t="s">
         <v>219</v>
       </c>
@@ -17172,8 +17122,8 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:78" x14ac:dyDescent="0.45">
-      <c r="A5" s="140"/>
+    <row r="5" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="A5" s="159"/>
       <c r="B5" s="81" t="s">
         <v>220</v>
       </c>
@@ -17424,8 +17374,8 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:78" x14ac:dyDescent="0.45">
-      <c r="A6" s="140"/>
+    <row r="6" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="A6" s="159"/>
       <c r="B6" s="81" t="s">
         <v>221</v>
       </c>
@@ -17676,8 +17626,8 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:78" x14ac:dyDescent="0.45">
-      <c r="A7" s="140"/>
+    <row r="7" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="A7" s="159"/>
       <c r="B7" s="81" t="s">
         <v>222</v>
       </c>
@@ -17928,8 +17878,8 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:78" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="140"/>
+    <row r="8" spans="1:78" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="159"/>
       <c r="B8" s="84" t="s">
         <v>4</v>
       </c>
@@ -18180,136 +18130,136 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:78" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
-    <row r="10" spans="1:78" ht="18" x14ac:dyDescent="0.45">
-      <c r="A10" s="140">
+    <row r="9" spans="1:78" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:78" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="159">
         <v>2026</v>
       </c>
       <c r="B10" s="79" t="str">
         <f ca="1">CONCATENATE("in: ",YEAR(TODAY())," für: ", YEAR(TODAY())+1)</f>
         <v>in: 2026 für: 2027</v>
       </c>
-      <c r="C10" s="141" t="s">
+      <c r="C10" s="140" t="s">
+        <v>256</v>
+      </c>
+      <c r="D10" s="140"/>
+      <c r="E10" s="141"/>
+      <c r="F10" s="144" t="s">
         <v>257</v>
       </c>
-      <c r="D10" s="141"/>
-      <c r="E10" s="142"/>
-      <c r="F10" s="143" t="s">
+      <c r="G10" s="145"/>
+      <c r="H10" s="145"/>
+      <c r="I10" s="145"/>
+      <c r="J10" s="146"/>
+      <c r="K10" s="150" t="s">
+        <v>261</v>
+      </c>
+      <c r="L10" s="151"/>
+      <c r="M10" s="151"/>
+      <c r="N10" s="152"/>
+      <c r="O10" s="142" t="s">
         <v>258</v>
       </c>
-      <c r="G10" s="144"/>
-      <c r="H10" s="144"/>
-      <c r="I10" s="144"/>
-      <c r="J10" s="145"/>
-      <c r="K10" s="146" t="s">
+      <c r="P10" s="142"/>
+      <c r="Q10" s="143"/>
+      <c r="R10" s="156" t="s">
+        <v>259</v>
+      </c>
+      <c r="S10" s="157"/>
+      <c r="T10" s="157"/>
+      <c r="U10" s="157"/>
+      <c r="V10" s="158"/>
+      <c r="W10" s="153" t="s">
         <v>262</v>
       </c>
-      <c r="L10" s="147"/>
-      <c r="M10" s="147"/>
-      <c r="N10" s="148"/>
-      <c r="O10" s="149" t="s">
-        <v>259</v>
-      </c>
-      <c r="P10" s="149"/>
-      <c r="Q10" s="150"/>
-      <c r="R10" s="151" t="s">
-        <v>260</v>
-      </c>
-      <c r="S10" s="152"/>
-      <c r="T10" s="152"/>
-      <c r="U10" s="152"/>
-      <c r="V10" s="153"/>
-      <c r="W10" s="154" t="s">
-        <v>263</v>
-      </c>
-      <c r="X10" s="155"/>
-      <c r="Y10" s="155"/>
-      <c r="Z10" s="156"/>
+      <c r="X10" s="154"/>
+      <c r="Y10" s="154"/>
+      <c r="Z10" s="155"/>
       <c r="AB10" s="79" t="str">
         <f ca="1">CONCATENATE("in: ",YEAR(TODAY())," für: ", YEAR(TODAY())+1)</f>
         <v>in: 2026 für: 2027</v>
       </c>
-      <c r="AC10" s="157" t="s">
+      <c r="AC10" s="160" t="s">
+        <v>263</v>
+      </c>
+      <c r="AD10" s="160"/>
+      <c r="AE10" s="161"/>
+      <c r="AF10" s="162" t="s">
         <v>264</v>
       </c>
-      <c r="AD10" s="157"/>
-      <c r="AE10" s="158"/>
-      <c r="AF10" s="159" t="s">
+      <c r="AG10" s="163"/>
+      <c r="AH10" s="163"/>
+      <c r="AI10" s="163"/>
+      <c r="AJ10" s="164"/>
+      <c r="AK10" s="165" t="s">
         <v>265</v>
       </c>
-      <c r="AG10" s="160"/>
-      <c r="AH10" s="160"/>
-      <c r="AI10" s="160"/>
-      <c r="AJ10" s="161"/>
-      <c r="AK10" s="162" t="s">
+      <c r="AL10" s="166"/>
+      <c r="AM10" s="166"/>
+      <c r="AN10" s="167"/>
+      <c r="AO10" s="168" t="s">
         <v>266</v>
       </c>
-      <c r="AL10" s="163"/>
-      <c r="AM10" s="163"/>
-      <c r="AN10" s="164"/>
-      <c r="AO10" s="165" t="s">
+      <c r="AP10" s="169"/>
+      <c r="AQ10" s="170"/>
+      <c r="AR10" s="171" t="s">
         <v>267</v>
       </c>
-      <c r="AP10" s="166"/>
-      <c r="AQ10" s="167"/>
-      <c r="AR10" s="168" t="s">
+      <c r="AS10" s="172"/>
+      <c r="AT10" s="172"/>
+      <c r="AU10" s="172"/>
+      <c r="AV10" s="173"/>
+      <c r="AW10" s="147" t="s">
         <v>268</v>
       </c>
-      <c r="AS10" s="169"/>
-      <c r="AT10" s="169"/>
-      <c r="AU10" s="169"/>
-      <c r="AV10" s="170"/>
-      <c r="AW10" s="171" t="s">
-        <v>269</v>
-      </c>
-      <c r="AX10" s="172"/>
-      <c r="AY10" s="172"/>
-      <c r="AZ10" s="173"/>
+      <c r="AX10" s="148"/>
+      <c r="AY10" s="148"/>
+      <c r="AZ10" s="149"/>
       <c r="BB10" s="79" t="str">
         <f ca="1">CONCATENATE("in: ",YEAR(TODAY())," für: ", YEAR(TODAY())+1)</f>
         <v>in: 2026 für: 2027</v>
       </c>
-      <c r="BC10" s="141" t="s">
+      <c r="BC10" s="140" t="s">
+        <v>269</v>
+      </c>
+      <c r="BD10" s="140"/>
+      <c r="BE10" s="141"/>
+      <c r="BF10" s="144" t="s">
         <v>270</v>
       </c>
-      <c r="BD10" s="141"/>
-      <c r="BE10" s="142"/>
-      <c r="BF10" s="143" t="s">
+      <c r="BG10" s="145"/>
+      <c r="BH10" s="145"/>
+      <c r="BI10" s="145"/>
+      <c r="BJ10" s="146"/>
+      <c r="BK10" s="150" t="s">
         <v>271</v>
       </c>
-      <c r="BG10" s="144"/>
-      <c r="BH10" s="144"/>
-      <c r="BI10" s="144"/>
-      <c r="BJ10" s="145"/>
-      <c r="BK10" s="146" t="s">
+      <c r="BL10" s="151"/>
+      <c r="BM10" s="151"/>
+      <c r="BN10" s="152"/>
+      <c r="BO10" s="142" t="s">
+        <v>258</v>
+      </c>
+      <c r="BP10" s="142"/>
+      <c r="BQ10" s="143"/>
+      <c r="BR10" s="156" t="s">
+        <v>259</v>
+      </c>
+      <c r="BS10" s="157"/>
+      <c r="BT10" s="157"/>
+      <c r="BU10" s="157"/>
+      <c r="BV10" s="158"/>
+      <c r="BW10" s="153" t="s">
         <v>272</v>
       </c>
-      <c r="BL10" s="147"/>
-      <c r="BM10" s="147"/>
-      <c r="BN10" s="148"/>
-      <c r="BO10" s="149" t="s">
-        <v>259</v>
-      </c>
-      <c r="BP10" s="149"/>
-      <c r="BQ10" s="150"/>
-      <c r="BR10" s="151" t="s">
+      <c r="BX10" s="154"/>
+      <c r="BY10" s="154"/>
+      <c r="BZ10" s="155"/>
+    </row>
+    <row r="11" spans="1:78" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="159"/>
+      <c r="B11" s="80" t="s">
         <v>260</v>
-      </c>
-      <c r="BS10" s="152"/>
-      <c r="BT10" s="152"/>
-      <c r="BU10" s="152"/>
-      <c r="BV10" s="153"/>
-      <c r="BW10" s="154" t="s">
-        <v>273</v>
-      </c>
-      <c r="BX10" s="155"/>
-      <c r="BY10" s="155"/>
-      <c r="BZ10" s="156"/>
-    </row>
-    <row r="11" spans="1:78" ht="21.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="140"/>
-      <c r="B11" s="80" t="s">
-        <v>261</v>
       </c>
       <c r="C11" s="92" t="str">
         <f ca="1">CONCATENATE("≤",YEAR(TODAY())-15)</f>
@@ -18409,7 +18359,7 @@
       </c>
       <c r="AA11" s="73"/>
       <c r="AB11" s="80" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="AC11" s="114" t="str">
         <f ca="1">CONCATENATE("≤",YEAR(TODAY())-15)</f>
@@ -18508,7 +18458,7 @@
         <v>2002-1986</v>
       </c>
       <c r="BB11" s="80" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="BC11" s="92" t="str">
         <f ca="1">CONCATENATE("≤",YEAR(TODAY())-15-1)</f>
@@ -18607,8 +18557,8 @@
         <v>2001-1985</v>
       </c>
     </row>
-    <row r="12" spans="1:78" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="140"/>
+    <row r="12" spans="1:78" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="159"/>
       <c r="B12" s="81" t="s">
         <v>0</v>
       </c>
@@ -18859,8 +18809,8 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:78" x14ac:dyDescent="0.45">
-      <c r="A13" s="140"/>
+    <row r="13" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="A13" s="159"/>
       <c r="B13" s="81" t="s">
         <v>219</v>
       </c>
@@ -19111,8 +19061,8 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:78" x14ac:dyDescent="0.45">
-      <c r="A14" s="140"/>
+    <row r="14" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="A14" s="159"/>
       <c r="B14" s="81" t="s">
         <v>220</v>
       </c>
@@ -19363,8 +19313,8 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:78" x14ac:dyDescent="0.45">
-      <c r="A15" s="140"/>
+    <row r="15" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="A15" s="159"/>
       <c r="B15" s="81" t="s">
         <v>221</v>
       </c>
@@ -19615,8 +19565,8 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="140"/>
+    <row r="16" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="159"/>
       <c r="B16" s="81" t="s">
         <v>222</v>
       </c>
@@ -19867,8 +19817,8 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:78" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="140"/>
+    <row r="17" spans="1:78" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="159"/>
       <c r="B17" s="84" t="s">
         <v>4</v>
       </c>
@@ -20119,7 +20069,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:78" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:78" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C18" s="64"/>
       <c r="O18" s="64"/>
       <c r="T18" s="67"/>
@@ -20128,7 +20078,7 @@
       <c r="X18" s="64"/>
       <c r="AD18" s="64"/>
     </row>
-    <row r="21" spans="1:78" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:78" x14ac:dyDescent="0.25">
       <c r="C21" s="63"/>
       <c r="D21" s="66"/>
       <c r="E21" s="66"/>
@@ -20148,7 +20098,7 @@
       <c r="AF21" s="69"/>
       <c r="AG21" s="69"/>
     </row>
-    <row r="22" spans="1:78" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:78" x14ac:dyDescent="0.25">
       <c r="C22" s="64"/>
       <c r="D22" s="65"/>
       <c r="E22" s="65"/>
@@ -20168,7 +20118,7 @@
       <c r="AF22" s="65"/>
       <c r="AG22" s="65"/>
     </row>
-    <row r="23" spans="1:78" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:78" x14ac:dyDescent="0.25">
       <c r="C23" s="64"/>
       <c r="D23" s="65"/>
       <c r="E23" s="65"/>
@@ -20188,7 +20138,7 @@
       <c r="AF23" s="65"/>
       <c r="AG23" s="65"/>
     </row>
-    <row r="24" spans="1:78" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:78" x14ac:dyDescent="0.25">
       <c r="C24" s="64"/>
       <c r="D24" s="65"/>
       <c r="E24" s="65"/>
@@ -20208,7 +20158,7 @@
       <c r="AF24" s="65"/>
       <c r="AG24" s="65"/>
     </row>
-    <row r="25" spans="1:78" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:78" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="64"/>
       <c r="D25" s="65"/>
       <c r="E25" s="65"/>
@@ -20228,7 +20178,7 @@
       <c r="AF25" s="65"/>
       <c r="AG25" s="65"/>
     </row>
-    <row r="26" spans="1:78" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:78" x14ac:dyDescent="0.25">
       <c r="C26" s="64"/>
       <c r="D26" s="65"/>
       <c r="E26" s="65"/>
@@ -20248,7 +20198,7 @@
       <c r="AF26" s="65"/>
       <c r="AG26" s="65"/>
     </row>
-    <row r="27" spans="1:78" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:78" x14ac:dyDescent="0.25">
       <c r="C27" s="64"/>
       <c r="D27" s="65"/>
       <c r="E27" s="65"/>
@@ -20268,7 +20218,7 @@
       <c r="AF27" s="65"/>
       <c r="AG27" s="65"/>
     </row>
-    <row r="30" spans="1:78" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:78" x14ac:dyDescent="0.25">
       <c r="C30" s="63"/>
       <c r="D30" s="66"/>
       <c r="E30" s="66"/>
@@ -20277,7 +20227,7 @@
       <c r="H30" s="66"/>
       <c r="P30" s="67"/>
     </row>
-    <row r="31" spans="1:78" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:78" x14ac:dyDescent="0.25">
       <c r="C31" s="64"/>
       <c r="D31" s="65"/>
       <c r="E31" s="65"/>
@@ -20285,7 +20235,7 @@
       <c r="G31" s="65"/>
       <c r="H31" s="65"/>
     </row>
-    <row r="40" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="40" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C40" s="64"/>
       <c r="D40" s="65"/>
       <c r="E40" s="65"/>
@@ -20293,7 +20243,7 @@
       <c r="G40" s="65"/>
       <c r="H40" s="65"/>
     </row>
-    <row r="41" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="41" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C41" s="64"/>
       <c r="D41" s="65"/>
       <c r="E41" s="65"/>
@@ -20301,7 +20251,7 @@
       <c r="G41" s="65"/>
       <c r="H41" s="65"/>
     </row>
-    <row r="42" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="42" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C42" s="64"/>
       <c r="D42" s="65"/>
       <c r="E42" s="65"/>
@@ -20309,7 +20259,7 @@
       <c r="G42" s="65"/>
       <c r="H42" s="65"/>
     </row>
-    <row r="43" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="43" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C43" s="64"/>
       <c r="D43" s="65"/>
       <c r="E43" s="65"/>
@@ -20317,7 +20267,7 @@
       <c r="G43" s="65"/>
       <c r="H43" s="65"/>
     </row>
-    <row r="44" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="44" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C44" s="64"/>
       <c r="D44" s="65"/>
       <c r="E44" s="65"/>
@@ -20325,7 +20275,7 @@
       <c r="G44" s="65"/>
       <c r="H44" s="65"/>
     </row>
-    <row r="45" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="45" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C45" s="64"/>
       <c r="D45" s="65"/>
       <c r="E45" s="65"/>
@@ -20335,28 +20285,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="O10:Q10"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="F10:J10"/>
-    <mergeCell ref="AW10:AZ10"/>
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="W10:Z10"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="R1:V1"/>
-    <mergeCell ref="W1:Z1"/>
-    <mergeCell ref="R10:V10"/>
-    <mergeCell ref="BO10:BQ10"/>
-    <mergeCell ref="BR10:BV10"/>
-    <mergeCell ref="BW10:BZ10"/>
-    <mergeCell ref="BC1:BE1"/>
-    <mergeCell ref="BF1:BJ1"/>
-    <mergeCell ref="BK1:BN1"/>
-    <mergeCell ref="BO1:BQ1"/>
-    <mergeCell ref="BR1:BV1"/>
-    <mergeCell ref="BW1:BZ1"/>
     <mergeCell ref="A1:A8"/>
     <mergeCell ref="A10:A17"/>
     <mergeCell ref="BC10:BE10"/>
@@ -20373,14 +20301,36 @@
     <mergeCell ref="AK10:AN10"/>
     <mergeCell ref="AO10:AQ10"/>
     <mergeCell ref="AR10:AV10"/>
+    <mergeCell ref="BO10:BQ10"/>
+    <mergeCell ref="BR10:BV10"/>
+    <mergeCell ref="BW10:BZ10"/>
+    <mergeCell ref="BC1:BE1"/>
+    <mergeCell ref="BF1:BJ1"/>
+    <mergeCell ref="BK1:BN1"/>
+    <mergeCell ref="BO1:BQ1"/>
+    <mergeCell ref="BR1:BV1"/>
+    <mergeCell ref="BW1:BZ1"/>
+    <mergeCell ref="AW10:AZ10"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="W10:Z10"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="R1:V1"/>
+    <mergeCell ref="W1:Z1"/>
+    <mergeCell ref="R10:V10"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="O10:Q10"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="F10:J10"/>
   </mergeCells>
   <conditionalFormatting sqref="AC3:AZ8">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AC12:AZ17">
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Kader krit für 2026 in JRP
</commit_message>
<xml_diff>
--- a/web/utilities/records_kriterien.xlsx
+++ b/web/utilities/records_kriterien.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29725"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgna\Documents\GitHub\Lifesaving_Baden\web\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBCB48CC-3C5E-4D9F-BD55-D0751163FDB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB7094BB-C166-4C75-935B-60CA9C5DA3B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="687" firstSheet="1" activeTab="7" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" tabRatio="687" firstSheet="1" activeTab="6" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
   </bookViews>
   <sheets>
     <sheet name="DR" sheetId="9" r:id="rId1"/>
@@ -1888,13 +1888,16 @@
     <xf numFmtId="0" fontId="17" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1906,6 +1909,15 @@
     <xf numFmtId="0" fontId="17" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1914,6 +1926,27 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1955,39 +1988,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2109,21 +2109,6 @@
       <font>
         <color theme="4"/>
       </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="25" formatCode="hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="m:ss.00"/>
@@ -4427,6 +4412,21 @@
       </fill>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="25" formatCode="hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4441,102 +4441,102 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2C5E83EE-6B6F-478A-9C90-A846A1A76536}" name="WR_Open4" displayName="WR_Open4" ref="A4:AW31" totalsRowShown="0" headerRowDxfId="201" headerRowBorderDxfId="200" tableBorderDxfId="199">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2C5E83EE-6B6F-478A-9C90-A846A1A76536}" name="WR_Open4" displayName="WR_Open4" ref="A4:AW31" totalsRowShown="0" headerRowDxfId="196" headerRowBorderDxfId="195" tableBorderDxfId="194">
   <autoFilter ref="A4:AW31" xr:uid="{2C5E83EE-6B6F-478A-9C90-A846A1A76536}"/>
   <tableColumns count="49">
-    <tableColumn id="1" xr3:uid="{7C0C4105-A61A-4B8D-9129-EDC4F18765AF}" name="WR-Open" dataDxfId="198">
+    <tableColumn id="1" xr3:uid="{7C0C4105-A61A-4B8D-9129-EDC4F18765AF}" name="WR-Open" dataDxfId="193">
       <calculatedColumnFormula>A4+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{516F5612-F85F-413F-9012-E235F415E34B}" name="50m Retten - offen - W" dataDxfId="197"/>
-    <tableColumn id="3" xr3:uid="{BC9ACAC9-0D45-42FD-B596-D19FBE3A4D83}" name="100m Retten - offen - W" dataDxfId="196"/>
-    <tableColumn id="4" xr3:uid="{CB6DBE59-EB65-43F0-93E7-0BDC3F82832B}" name="100m Kombi - offen - W" dataDxfId="195"/>
-    <tableColumn id="5" xr3:uid="{AA603C60-6831-4C14-A8CD-0AA050DA7551}" name="100m Lifesaver - offen - W" dataDxfId="194"/>
-    <tableColumn id="6" xr3:uid="{7920F147-7717-4582-940A-2610F7D310CA}" name="200m Superlifesaver - offen - W" dataDxfId="193"/>
-    <tableColumn id="7" xr3:uid="{04E21F1D-AC8D-4A1B-9B43-59B8F7901673}" name="200m Hindernis - offen - W" dataDxfId="192"/>
-    <tableColumn id="8" xr3:uid="{40E8A083-653A-48A8-9B37-0A2D850B7829}" name="50m Retten - offen - M" dataDxfId="191"/>
-    <tableColumn id="9" xr3:uid="{863824A9-134F-4189-BB14-225AE224FC44}" name="100m Retten - offen - M" dataDxfId="190"/>
+    <tableColumn id="2" xr3:uid="{516F5612-F85F-413F-9012-E235F415E34B}" name="50m Retten - offen - W" dataDxfId="192"/>
+    <tableColumn id="3" xr3:uid="{BC9ACAC9-0D45-42FD-B596-D19FBE3A4D83}" name="100m Retten - offen - W" dataDxfId="191"/>
+    <tableColumn id="4" xr3:uid="{CB6DBE59-EB65-43F0-93E7-0BDC3F82832B}" name="100m Kombi - offen - W" dataDxfId="190"/>
+    <tableColumn id="5" xr3:uid="{AA603C60-6831-4C14-A8CD-0AA050DA7551}" name="100m Lifesaver - offen - W" dataDxfId="189"/>
+    <tableColumn id="6" xr3:uid="{7920F147-7717-4582-940A-2610F7D310CA}" name="200m Superlifesaver - offen - W" dataDxfId="188"/>
+    <tableColumn id="7" xr3:uid="{04E21F1D-AC8D-4A1B-9B43-59B8F7901673}" name="200m Hindernis - offen - W" dataDxfId="187"/>
+    <tableColumn id="8" xr3:uid="{40E8A083-653A-48A8-9B37-0A2D850B7829}" name="50m Retten - offen - M" dataDxfId="186"/>
+    <tableColumn id="9" xr3:uid="{863824A9-134F-4189-BB14-225AE224FC44}" name="100m Retten - offen - M" dataDxfId="185"/>
     <tableColumn id="10" xr3:uid="{598FC6AE-DEA2-4475-9A35-CDCB8C81496A}" name="100m Kombi - offen - M"/>
     <tableColumn id="11" xr3:uid="{9FC50B37-0D51-422E-A268-A6506D4F3854}" name="100m Lifesaver - offen - M"/>
     <tableColumn id="12" xr3:uid="{B8D2552B-5D82-442A-98F0-E47D5C5F6728}" name="200m Superlifesaver - offen - M"/>
-    <tableColumn id="13" xr3:uid="{5A5E9873-0C5F-4508-AF6B-4974E0526D84}" name="200m Hindernis - offen - M" dataDxfId="189"/>
-    <tableColumn id="14" xr3:uid="{FA907992-7FCE-4CAD-8CF2-F5BEBC9B3756}" name="50m Retten - 17/18 - W" dataDxfId="188"/>
-    <tableColumn id="15" xr3:uid="{76B63DC0-CB67-48F4-9B5A-D22902F59334}" name="100m Retten - 17/18 - W" dataDxfId="187"/>
-    <tableColumn id="16" xr3:uid="{614A2419-51B1-44C0-8469-ADBFB078B81A}" name="100m Kombi -17/18 - W" dataDxfId="186"/>
-    <tableColumn id="17" xr3:uid="{2EC953EE-367D-4524-A25E-8DE3B8168E34}" name="100m Lifesaver - 17/18 - W" dataDxfId="185"/>
-    <tableColumn id="18" xr3:uid="{25711867-9BD7-4197-9094-A21392411249}" name="200m Superlifesaver - 17/18 - W" dataDxfId="184"/>
-    <tableColumn id="19" xr3:uid="{262DB142-CFB1-45C3-9332-7273CACD1B62}" name="200m Hindernis - 17/18 - W" dataDxfId="183"/>
-    <tableColumn id="20" xr3:uid="{938BA45A-8244-4637-8A14-DF49CD91A945}" name="50m Retten - 17/18 - M" dataDxfId="182"/>
-    <tableColumn id="21" xr3:uid="{737E28D8-900F-4A98-95FE-EE7B0AFDEE90}" name="100m Retten - 17/18 - M" dataDxfId="181"/>
-    <tableColumn id="22" xr3:uid="{330BD3A8-061C-45E2-ADDB-40C2F346772F}" name="100m Kombi - 17/18 - M" dataDxfId="180"/>
-    <tableColumn id="23" xr3:uid="{0CADDE90-A167-4E1D-8D33-8624E5E1A4E2}" name="100m Lifesaver - 17/18 - M" dataDxfId="179"/>
-    <tableColumn id="24" xr3:uid="{FCF9F42C-1291-4985-9D37-B9DE2DAA5DCB}" name="200m Superlifesaver - 17/18 - M" dataDxfId="178"/>
-    <tableColumn id="25" xr3:uid="{4E5397B2-F924-4F48-AE69-AF6D650AF88D}" name="200m Hindernis - 17/18 - M" dataDxfId="177"/>
-    <tableColumn id="26" xr3:uid="{0A78315A-BFDC-43EE-A66F-48B301F66508}" name="50m Retten - 15/16 - W" dataDxfId="176"/>
-    <tableColumn id="27" xr3:uid="{D3FCF8BD-6C76-450D-80C0-CC0519A79731}" name="100m Retten - 15/16 - W" dataDxfId="175"/>
-    <tableColumn id="28" xr3:uid="{6BE7937E-D62D-47CD-95DE-1730304B0DF3}" name="100m Kombi - 15/16 - W" dataDxfId="174"/>
-    <tableColumn id="29" xr3:uid="{098BA5BE-5AF6-4187-89B6-534498F24C51}" name="100m Lifesaver -  15/16 - W" dataDxfId="173"/>
-    <tableColumn id="30" xr3:uid="{2A6822CF-143C-4BF7-A440-5777527BE512}" name="200m Superlifesaver -  15/16 - W" dataDxfId="172"/>
-    <tableColumn id="31" xr3:uid="{541C7145-CDEA-4E4E-9E7A-A4F05BA6C3E5}" name="200m Hindernis -  15/16 - W" dataDxfId="171"/>
-    <tableColumn id="32" xr3:uid="{342C4488-8C61-42E6-87A9-C75BD8EB7452}" name="50m Retten - 15/16 - M" dataDxfId="170"/>
-    <tableColumn id="33" xr3:uid="{857B1D46-7D20-47F7-AB9B-732D50346E32}" name="100m Retten - 15/16 - M" dataDxfId="169"/>
-    <tableColumn id="34" xr3:uid="{4C8A2EB4-804B-45F1-A768-9A6958957F8B}" name="100m Kombi -15/16 - M" dataDxfId="168"/>
-    <tableColumn id="35" xr3:uid="{26C75B4F-21EC-4EB0-A9A9-54BC80140672}" name="100m Lifesaver - 15/16 - M" dataDxfId="167"/>
-    <tableColumn id="36" xr3:uid="{DBBB2A23-1A06-429A-A5D1-A547EF5EC16F}" name="200m Superlifesaver - 15/16 - M" dataDxfId="166"/>
-    <tableColumn id="37" xr3:uid="{84061231-CAE5-427A-87F5-6DDBA99F77D2}" name="200m Hindernis - 15/16 - M" dataDxfId="165"/>
-    <tableColumn id="38" xr3:uid="{878CCA80-A742-4B3C-90C9-E93BB814201B}" name="50m Retten - 13/14 - W" dataDxfId="164"/>
-    <tableColumn id="39" xr3:uid="{A1F57102-61CF-4784-8DE2-0B8F32D5D699}" name="50m Retten mit Flossen - 13/14 - W" dataDxfId="163"/>
-    <tableColumn id="40" xr3:uid="{0F6BAF78-3D79-42A9-9FED-E6D0E335A920}" name="100m Hindernis - 13/14 - W" dataDxfId="162"/>
-    <tableColumn id="41" xr3:uid="{EB748A68-E10D-4D76-B315-8FDB3AC33C8D}" name="50m Retten - 13/14 - M" dataDxfId="161"/>
-    <tableColumn id="42" xr3:uid="{C7B04167-6430-40F0-9A0F-D0D0BE2F9C77}" name="50m Retten mit Flossen - 13/14 - M" dataDxfId="160"/>
-    <tableColumn id="43" xr3:uid="{48704BB7-A853-445A-8CDC-8D8F86C2B66A}" name="100m Hindernis - 13/14 - M" dataDxfId="159"/>
-    <tableColumn id="44" xr3:uid="{9605FE9A-F41C-4A5F-A59C-B7A9D45C460F}" name="50m Flossen - 12 - W" dataDxfId="158"/>
-    <tableColumn id="45" xr3:uid="{4C9DBF61-35B1-4BC2-8272-526E0AFAAFFB}" name="50m komb. Schwimmen - 12 - W" dataDxfId="157"/>
-    <tableColumn id="46" xr3:uid="{CF433C95-C272-48F9-98CD-7E3C8DBB6F2C}" name="50m Hindernis - 12 - W" dataDxfId="156"/>
-    <tableColumn id="47" xr3:uid="{FADB7411-DB43-4B14-B9E8-D74CA1BA18B8}" name="50m Flossen - 12 - M" dataDxfId="155"/>
-    <tableColumn id="48" xr3:uid="{02936F84-1D82-48AC-8D7C-6D2954D68A06}" name="50m komb. Schwimmen - 12 - M" dataDxfId="154"/>
-    <tableColumn id="49" xr3:uid="{7FD9BD11-0597-4E07-8DA5-DB53384197F5}" name="50m Hindernis - 12 - M" dataDxfId="153"/>
+    <tableColumn id="13" xr3:uid="{5A5E9873-0C5F-4508-AF6B-4974E0526D84}" name="200m Hindernis - offen - M" dataDxfId="184"/>
+    <tableColumn id="14" xr3:uid="{FA907992-7FCE-4CAD-8CF2-F5BEBC9B3756}" name="50m Retten - 17/18 - W" dataDxfId="183"/>
+    <tableColumn id="15" xr3:uid="{76B63DC0-CB67-48F4-9B5A-D22902F59334}" name="100m Retten - 17/18 - W" dataDxfId="182"/>
+    <tableColumn id="16" xr3:uid="{614A2419-51B1-44C0-8469-ADBFB078B81A}" name="100m Kombi -17/18 - W" dataDxfId="181"/>
+    <tableColumn id="17" xr3:uid="{2EC953EE-367D-4524-A25E-8DE3B8168E34}" name="100m Lifesaver - 17/18 - W" dataDxfId="180"/>
+    <tableColumn id="18" xr3:uid="{25711867-9BD7-4197-9094-A21392411249}" name="200m Superlifesaver - 17/18 - W" dataDxfId="179"/>
+    <tableColumn id="19" xr3:uid="{262DB142-CFB1-45C3-9332-7273CACD1B62}" name="200m Hindernis - 17/18 - W" dataDxfId="178"/>
+    <tableColumn id="20" xr3:uid="{938BA45A-8244-4637-8A14-DF49CD91A945}" name="50m Retten - 17/18 - M" dataDxfId="177"/>
+    <tableColumn id="21" xr3:uid="{737E28D8-900F-4A98-95FE-EE7B0AFDEE90}" name="100m Retten - 17/18 - M" dataDxfId="176"/>
+    <tableColumn id="22" xr3:uid="{330BD3A8-061C-45E2-ADDB-40C2F346772F}" name="100m Kombi - 17/18 - M" dataDxfId="175"/>
+    <tableColumn id="23" xr3:uid="{0CADDE90-A167-4E1D-8D33-8624E5E1A4E2}" name="100m Lifesaver - 17/18 - M" dataDxfId="174"/>
+    <tableColumn id="24" xr3:uid="{FCF9F42C-1291-4985-9D37-B9DE2DAA5DCB}" name="200m Superlifesaver - 17/18 - M" dataDxfId="173"/>
+    <tableColumn id="25" xr3:uid="{4E5397B2-F924-4F48-AE69-AF6D650AF88D}" name="200m Hindernis - 17/18 - M" dataDxfId="172"/>
+    <tableColumn id="26" xr3:uid="{0A78315A-BFDC-43EE-A66F-48B301F66508}" name="50m Retten - 15/16 - W" dataDxfId="171"/>
+    <tableColumn id="27" xr3:uid="{D3FCF8BD-6C76-450D-80C0-CC0519A79731}" name="100m Retten - 15/16 - W" dataDxfId="170"/>
+    <tableColumn id="28" xr3:uid="{6BE7937E-D62D-47CD-95DE-1730304B0DF3}" name="100m Kombi - 15/16 - W" dataDxfId="169"/>
+    <tableColumn id="29" xr3:uid="{098BA5BE-5AF6-4187-89B6-534498F24C51}" name="100m Lifesaver -  15/16 - W" dataDxfId="168"/>
+    <tableColumn id="30" xr3:uid="{2A6822CF-143C-4BF7-A440-5777527BE512}" name="200m Superlifesaver -  15/16 - W" dataDxfId="167"/>
+    <tableColumn id="31" xr3:uid="{541C7145-CDEA-4E4E-9E7A-A4F05BA6C3E5}" name="200m Hindernis -  15/16 - W" dataDxfId="166"/>
+    <tableColumn id="32" xr3:uid="{342C4488-8C61-42E6-87A9-C75BD8EB7452}" name="50m Retten - 15/16 - M" dataDxfId="165"/>
+    <tableColumn id="33" xr3:uid="{857B1D46-7D20-47F7-AB9B-732D50346E32}" name="100m Retten - 15/16 - M" dataDxfId="164"/>
+    <tableColumn id="34" xr3:uid="{4C8A2EB4-804B-45F1-A768-9A6958957F8B}" name="100m Kombi -15/16 - M" dataDxfId="163"/>
+    <tableColumn id="35" xr3:uid="{26C75B4F-21EC-4EB0-A9A9-54BC80140672}" name="100m Lifesaver - 15/16 - M" dataDxfId="162"/>
+    <tableColumn id="36" xr3:uid="{DBBB2A23-1A06-429A-A5D1-A547EF5EC16F}" name="200m Superlifesaver - 15/16 - M" dataDxfId="161"/>
+    <tableColumn id="37" xr3:uid="{84061231-CAE5-427A-87F5-6DDBA99F77D2}" name="200m Hindernis - 15/16 - M" dataDxfId="160"/>
+    <tableColumn id="38" xr3:uid="{878CCA80-A742-4B3C-90C9-E93BB814201B}" name="50m Retten - 13/14 - W" dataDxfId="159"/>
+    <tableColumn id="39" xr3:uid="{A1F57102-61CF-4784-8DE2-0B8F32D5D699}" name="50m Retten mit Flossen - 13/14 - W" dataDxfId="158"/>
+    <tableColumn id="40" xr3:uid="{0F6BAF78-3D79-42A9-9FED-E6D0E335A920}" name="100m Hindernis - 13/14 - W" dataDxfId="157"/>
+    <tableColumn id="41" xr3:uid="{EB748A68-E10D-4D76-B315-8FDB3AC33C8D}" name="50m Retten - 13/14 - M" dataDxfId="156"/>
+    <tableColumn id="42" xr3:uid="{C7B04167-6430-40F0-9A0F-D0D0BE2F9C77}" name="50m Retten mit Flossen - 13/14 - M" dataDxfId="155"/>
+    <tableColumn id="43" xr3:uid="{48704BB7-A853-445A-8CDC-8D8F86C2B66A}" name="100m Hindernis - 13/14 - M" dataDxfId="154"/>
+    <tableColumn id="44" xr3:uid="{9605FE9A-F41C-4A5F-A59C-B7A9D45C460F}" name="50m Flossen - 12 - W" dataDxfId="153"/>
+    <tableColumn id="45" xr3:uid="{4C9DBF61-35B1-4BC2-8272-526E0AFAAFFB}" name="50m komb. Schwimmen - 12 - W" dataDxfId="152"/>
+    <tableColumn id="46" xr3:uid="{CF433C95-C272-48F9-98CD-7E3C8DBB6F2C}" name="50m Hindernis - 12 - W" dataDxfId="151"/>
+    <tableColumn id="47" xr3:uid="{FADB7411-DB43-4B14-B9E8-D74CA1BA18B8}" name="50m Flossen - 12 - M" dataDxfId="150"/>
+    <tableColumn id="48" xr3:uid="{02936F84-1D82-48AC-8D7C-6D2954D68A06}" name="50m komb. Schwimmen - 12 - M" dataDxfId="149"/>
+    <tableColumn id="49" xr3:uid="{7FD9BD11-0597-4E07-8DA5-DB53384197F5}" name="50m Hindernis - 12 - M" dataDxfId="148"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4234D44E-A2BE-4790-B589-1A8CC19B714E}" name="WR_Youth" displayName="WR_Youth" ref="A4:M32" totalsRowShown="0" headerRowDxfId="152" dataDxfId="150" headerRowBorderDxfId="151" tableBorderDxfId="149">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4234D44E-A2BE-4790-B589-1A8CC19B714E}" name="WR_Youth" displayName="WR_Youth" ref="A4:M32" totalsRowShown="0" headerRowDxfId="147" dataDxfId="145" headerRowBorderDxfId="146" tableBorderDxfId="144">
   <autoFilter ref="A4:M32" xr:uid="{4234D44E-A2BE-4790-B589-1A8CC19B714E}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{848E691A-41B0-42DD-B122-FB6DF43CB3EF}" name="WR-Youth" dataDxfId="148"/>
-    <tableColumn id="2" xr3:uid="{2FE43F18-485B-46A9-8946-FBC5FDAE5A8E}" name="50m Retten" dataDxfId="147"/>
-    <tableColumn id="3" xr3:uid="{CA5C3ABF-02E6-442B-868B-95B293B231D3}" name="100m Retten" dataDxfId="146"/>
-    <tableColumn id="4" xr3:uid="{7A6BBA52-2145-464D-8C04-B2CCFC1A90DC}" name="100m Kombi" dataDxfId="145"/>
-    <tableColumn id="5" xr3:uid="{21F420C9-E788-49EE-88F6-E37963ED31CF}" name="100m Lifesaver" dataDxfId="144"/>
-    <tableColumn id="6" xr3:uid="{CB87B7CD-8A9C-4775-A4D7-4D267F43FD1A}" name="200m Superlifesaver" dataDxfId="143"/>
-    <tableColumn id="7" xr3:uid="{2DC7F290-B564-4851-85AE-D211DA701B32}" name="200m Hindernis" dataDxfId="142"/>
-    <tableColumn id="8" xr3:uid="{8112783D-8796-4D6A-8414-AC675D745697}" name="50m Retten2" dataDxfId="141"/>
-    <tableColumn id="9" xr3:uid="{4E818CD4-8725-495D-9D1D-1AFCED9181F5}" name="100m Retten2" dataDxfId="140"/>
-    <tableColumn id="10" xr3:uid="{28C05A91-E302-40A9-B50A-ECF997F129FC}" name="100m Kombi2" dataDxfId="139"/>
-    <tableColumn id="11" xr3:uid="{D56FB9F2-45BF-4EC9-A84C-8A5FB59F2F05}" name="100m Lifesaver2" dataDxfId="138"/>
-    <tableColumn id="12" xr3:uid="{540169C0-2A40-4794-A872-F7DF8A887BF2}" name="200m Superlifesaver2" dataDxfId="137"/>
-    <tableColumn id="13" xr3:uid="{D104CB67-B55A-4C81-87E5-0AC758DD22A4}" name="200m Hindernis2" dataDxfId="136"/>
+    <tableColumn id="1" xr3:uid="{848E691A-41B0-42DD-B122-FB6DF43CB3EF}" name="WR-Youth" dataDxfId="143"/>
+    <tableColumn id="2" xr3:uid="{2FE43F18-485B-46A9-8946-FBC5FDAE5A8E}" name="50m Retten" dataDxfId="142"/>
+    <tableColumn id="3" xr3:uid="{CA5C3ABF-02E6-442B-868B-95B293B231D3}" name="100m Retten" dataDxfId="141"/>
+    <tableColumn id="4" xr3:uid="{7A6BBA52-2145-464D-8C04-B2CCFC1A90DC}" name="100m Kombi" dataDxfId="140"/>
+    <tableColumn id="5" xr3:uid="{21F420C9-E788-49EE-88F6-E37963ED31CF}" name="100m Lifesaver" dataDxfId="139"/>
+    <tableColumn id="6" xr3:uid="{CB87B7CD-8A9C-4775-A4D7-4D267F43FD1A}" name="200m Superlifesaver" dataDxfId="138"/>
+    <tableColumn id="7" xr3:uid="{2DC7F290-B564-4851-85AE-D211DA701B32}" name="200m Hindernis" dataDxfId="137"/>
+    <tableColumn id="8" xr3:uid="{8112783D-8796-4D6A-8414-AC675D745697}" name="50m Retten2" dataDxfId="136"/>
+    <tableColumn id="9" xr3:uid="{4E818CD4-8725-495D-9D1D-1AFCED9181F5}" name="100m Retten2" dataDxfId="135"/>
+    <tableColumn id="10" xr3:uid="{28C05A91-E302-40A9-B50A-ECF997F129FC}" name="100m Kombi2" dataDxfId="134"/>
+    <tableColumn id="11" xr3:uid="{D56FB9F2-45BF-4EC9-A84C-8A5FB59F2F05}" name="100m Lifesaver2" dataDxfId="133"/>
+    <tableColumn id="12" xr3:uid="{540169C0-2A40-4794-A872-F7DF8A887BF2}" name="200m Superlifesaver2" dataDxfId="132"/>
+    <tableColumn id="13" xr3:uid="{D104CB67-B55A-4C81-87E5-0AC758DD22A4}" name="200m Hindernis2" dataDxfId="131"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E2D2F97B-7645-4066-8AB3-F35CF6E035EB}" name="WR_Open" displayName="WR_Open" ref="A4:M32" totalsRowShown="0" headerRowDxfId="135" headerRowBorderDxfId="134" tableBorderDxfId="133">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E2D2F97B-7645-4066-8AB3-F35CF6E035EB}" name="WR_Open" displayName="WR_Open" ref="A4:M32" totalsRowShown="0" headerRowDxfId="130" headerRowBorderDxfId="129" tableBorderDxfId="128">
   <autoFilter ref="A4:M32" xr:uid="{E2D2F97B-7645-4066-8AB3-F35CF6E035EB}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{AE73402B-B27E-4B29-8DCF-30B7FC1855EF}" name="WR-Open" dataDxfId="132">
+    <tableColumn id="1" xr3:uid="{AE73402B-B27E-4B29-8DCF-30B7FC1855EF}" name="WR-Open" dataDxfId="127">
       <calculatedColumnFormula>A4+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{EA3EAC1F-184E-4A28-B3E3-08DE12F138EF}" name="50m Retten" dataDxfId="131"/>
-    <tableColumn id="3" xr3:uid="{E0305A3F-6087-4F8C-8B64-153E1ACAA32E}" name="100m Retten" dataDxfId="130"/>
-    <tableColumn id="4" xr3:uid="{F0B7AC37-315E-49AA-855C-7955D2B43A76}" name="100m Kombi" dataDxfId="129"/>
-    <tableColumn id="5" xr3:uid="{B5E690AB-DB7D-4864-8916-89D2A68C4128}" name="100m Lifesaver" dataDxfId="128"/>
-    <tableColumn id="6" xr3:uid="{D89BAF4D-36AE-4C73-9320-9C5736F02F8A}" name="200m Superlifesaver" dataDxfId="127"/>
-    <tableColumn id="7" xr3:uid="{58AE7517-1A90-459F-A7D2-B95265D217E7}" name="200m Hindernis" dataDxfId="126"/>
-    <tableColumn id="8" xr3:uid="{13A189FB-E897-4A1F-A001-525F61E9CFFF}" name="50m Retten2" dataDxfId="125"/>
-    <tableColumn id="9" xr3:uid="{36418AC5-46B8-400F-BD2E-D329CF4F92CD}" name="100m Retten2" dataDxfId="124"/>
+    <tableColumn id="2" xr3:uid="{EA3EAC1F-184E-4A28-B3E3-08DE12F138EF}" name="50m Retten" dataDxfId="126"/>
+    <tableColumn id="3" xr3:uid="{E0305A3F-6087-4F8C-8B64-153E1ACAA32E}" name="100m Retten" dataDxfId="125"/>
+    <tableColumn id="4" xr3:uid="{F0B7AC37-315E-49AA-855C-7955D2B43A76}" name="100m Kombi" dataDxfId="124"/>
+    <tableColumn id="5" xr3:uid="{B5E690AB-DB7D-4864-8916-89D2A68C4128}" name="100m Lifesaver" dataDxfId="123"/>
+    <tableColumn id="6" xr3:uid="{D89BAF4D-36AE-4C73-9320-9C5736F02F8A}" name="200m Superlifesaver" dataDxfId="122"/>
+    <tableColumn id="7" xr3:uid="{58AE7517-1A90-459F-A7D2-B95265D217E7}" name="200m Hindernis" dataDxfId="121"/>
+    <tableColumn id="8" xr3:uid="{13A189FB-E897-4A1F-A001-525F61E9CFFF}" name="50m Retten2" dataDxfId="120"/>
+    <tableColumn id="9" xr3:uid="{36418AC5-46B8-400F-BD2E-D329CF4F92CD}" name="100m Retten2" dataDxfId="119"/>
     <tableColumn id="10" xr3:uid="{06A35C2D-7313-472B-BC1F-4F2FB1D14782}" name="100m Kombi2"/>
     <tableColumn id="11" xr3:uid="{89966D0D-9131-4245-A7BE-1A7384D5ADA0}" name="100m Lifesaver2"/>
     <tableColumn id="12" xr3:uid="{D9D6CF56-869C-4DDE-9886-572D4E523A8F}" name="200m Superlifesaver2"/>
@@ -4547,7 +4547,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CF3D303A-A04B-42DD-A44E-CEB6CECB77A4}" name="DP_konfig" displayName="DP_konfig" ref="A1:U3" totalsRowShown="0" headerRowDxfId="123" dataDxfId="122">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CF3D303A-A04B-42DD-A44E-CEB6CECB77A4}" name="DP_konfig" displayName="DP_konfig" ref="A1:U3" totalsRowShown="0" headerRowDxfId="118" dataDxfId="117">
   <autoFilter ref="A1:U3" xr:uid="{CF3D303A-A04B-42DD-A44E-CEB6CECB77A4}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4572,64 +4572,64 @@
     <filterColumn colId="20" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="21">
-    <tableColumn id="1" xr3:uid="{58D628F0-061E-4A82-8362-CDB37A2E7C60}" name="Tabellen Name" dataDxfId="121"/>
-    <tableColumn id="2" xr3:uid="{2F302F6C-F8AF-4FDE-AB08-6F30F9671015}" name="Geschlecht" dataDxfId="120"/>
-    <tableColumn id="3" xr3:uid="{4D91FBF9-386D-43DD-90D0-B49823FDB629}" name="Mindest alter" dataDxfId="119"/>
-    <tableColumn id="4" xr3:uid="{4126AAC6-AF2F-446C-B4EA-D86ACFD9FAC2}" name="Maximales Alter" dataDxfId="118"/>
-    <tableColumn id="5" xr3:uid="{8A10890A-A299-4B09-AC72-0E9AE9238AF3}" name="Qualizeitraum anfang" dataDxfId="117"/>
-    <tableColumn id="6" xr3:uid="{FBCD1C13-FC82-429B-8DE1-0C5A455FDAB8}" name="Qualizeitraum Ende" dataDxfId="116"/>
-    <tableColumn id="7" xr3:uid="{1DCCAC9B-BC46-468E-A3CE-57576C2FF11D}" name="Letzter Wettkampf am" dataDxfId="115"/>
-    <tableColumn id="8" xr3:uid="{9A6E47EE-ABD8-4A1E-87D3-9D286E4C124F}" name="Wertung" dataDxfId="114"/>
-    <tableColumn id="9" xr3:uid="{09E848D2-ED17-49C7-9775-CBF17D20DFC0}" name="Landesverband" dataDxfId="113"/>
-    <tableColumn id="10" xr3:uid="{70ABB713-23F6-4FCF-920E-3CB0CD451446}" name="OMS" dataDxfId="112"/>
-    <tableColumn id="11" xr3:uid="{9C108A1C-E6AB-4C13-9C1D-0FA8944A39A3}" name="Pool-Länge" dataDxfId="111"/>
-    <tableColumn id="12" xr3:uid="{087948DD-430D-48F1-906D-4F4EF4B46053}" name="Regelwerk" dataDxfId="110"/>
-    <tableColumn id="13" xr3:uid="{BF42D9C0-F77D-4971-A67E-32B0246C72C3}" name="Referenz" dataDxfId="109"/>
-    <tableColumn id="19" xr3:uid="{AFFB84E8-B398-4E99-805B-9A247071A040}" name="Referenz Jahr" dataDxfId="108"/>
-    <tableColumn id="20" xr3:uid="{0A59A474-DFBB-4437-8EFF-70284AFD9934}" name="Mindest Punktzahl" dataDxfId="107"/>
-    <tableColumn id="21" xr3:uid="{198BD231-EEF3-43C9-AD9B-39B4B7E9B337}" name="Mindest Disziplinen" dataDxfId="106"/>
-    <tableColumn id="14" xr3:uid="{443CD4F6-A2B2-480B-BB35-DCEEBC531727}" name="3-Kampf Regel" dataDxfId="105"/>
-    <tableColumn id="15" xr3:uid="{70116160-7666-42B1-92AC-FAC2620E6A60}" name="Anzahl Nominierte" dataDxfId="104"/>
-    <tableColumn id="16" xr3:uid="{0EFD0A46-D12B-4AB0-907C-08E5D9F282E0}" name="Anzahl Nachrücker" dataDxfId="103"/>
-    <tableColumn id="17" xr3:uid="{AA5430A0-8ED8-40E8-B7F8-DA25E4E8790F}" name="Seiten Anzahl" dataDxfId="102"/>
-    <tableColumn id="18" xr3:uid="{16F699D9-2741-43F3-AD5F-826A568EFEAC}" name="Absagen" dataDxfId="101"/>
+    <tableColumn id="1" xr3:uid="{58D628F0-061E-4A82-8362-CDB37A2E7C60}" name="Tabellen Name" dataDxfId="116"/>
+    <tableColumn id="2" xr3:uid="{2F302F6C-F8AF-4FDE-AB08-6F30F9671015}" name="Geschlecht" dataDxfId="115"/>
+    <tableColumn id="3" xr3:uid="{4D91FBF9-386D-43DD-90D0-B49823FDB629}" name="Mindest alter" dataDxfId="114"/>
+    <tableColumn id="4" xr3:uid="{4126AAC6-AF2F-446C-B4EA-D86ACFD9FAC2}" name="Maximales Alter" dataDxfId="113"/>
+    <tableColumn id="5" xr3:uid="{8A10890A-A299-4B09-AC72-0E9AE9238AF3}" name="Qualizeitraum anfang" dataDxfId="112"/>
+    <tableColumn id="6" xr3:uid="{FBCD1C13-FC82-429B-8DE1-0C5A455FDAB8}" name="Qualizeitraum Ende" dataDxfId="111"/>
+    <tableColumn id="7" xr3:uid="{1DCCAC9B-BC46-468E-A3CE-57576C2FF11D}" name="Letzter Wettkampf am" dataDxfId="110"/>
+    <tableColumn id="8" xr3:uid="{9A6E47EE-ABD8-4A1E-87D3-9D286E4C124F}" name="Wertung" dataDxfId="109"/>
+    <tableColumn id="9" xr3:uid="{09E848D2-ED17-49C7-9775-CBF17D20DFC0}" name="Landesverband" dataDxfId="108"/>
+    <tableColumn id="10" xr3:uid="{70ABB713-23F6-4FCF-920E-3CB0CD451446}" name="OMS" dataDxfId="107"/>
+    <tableColumn id="11" xr3:uid="{9C108A1C-E6AB-4C13-9C1D-0FA8944A39A3}" name="Pool-Länge" dataDxfId="106"/>
+    <tableColumn id="12" xr3:uid="{087948DD-430D-48F1-906D-4F4EF4B46053}" name="Regelwerk" dataDxfId="105"/>
+    <tableColumn id="13" xr3:uid="{BF42D9C0-F77D-4971-A67E-32B0246C72C3}" name="Referenz" dataDxfId="104"/>
+    <tableColumn id="19" xr3:uid="{AFFB84E8-B398-4E99-805B-9A247071A040}" name="Referenz Jahr" dataDxfId="103"/>
+    <tableColumn id="20" xr3:uid="{0A59A474-DFBB-4437-8EFF-70284AFD9934}" name="Mindest Punktzahl" dataDxfId="102"/>
+    <tableColumn id="21" xr3:uid="{198BD231-EEF3-43C9-AD9B-39B4B7E9B337}" name="Mindest Disziplinen" dataDxfId="101"/>
+    <tableColumn id="14" xr3:uid="{443CD4F6-A2B2-480B-BB35-DCEEBC531727}" name="3-Kampf Regel" dataDxfId="100"/>
+    <tableColumn id="15" xr3:uid="{70116160-7666-42B1-92AC-FAC2620E6A60}" name="Anzahl Nominierte" dataDxfId="99"/>
+    <tableColumn id="16" xr3:uid="{0EFD0A46-D12B-4AB0-907C-08E5D9F282E0}" name="Anzahl Nachrücker" dataDxfId="98"/>
+    <tableColumn id="17" xr3:uid="{AA5430A0-8ED8-40E8-B7F8-DA25E4E8790F}" name="Seiten Anzahl" dataDxfId="97"/>
+    <tableColumn id="18" xr3:uid="{16F699D9-2741-43F3-AD5F-826A568EFEAC}" name="Absagen" dataDxfId="96"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CDBF6724-48A1-41AB-94B5-CC35C54BB15C}" name="BP_konfig" displayName="BP_konfig" ref="A1:U7" totalsRowShown="0" headerRowDxfId="100" dataDxfId="99">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CDBF6724-48A1-41AB-94B5-CC35C54BB15C}" name="BP_konfig" displayName="BP_konfig" ref="A1:U7" totalsRowShown="0" headerRowDxfId="95" dataDxfId="94">
   <autoFilter ref="A1:U7" xr:uid="{CDBF6724-48A1-41AB-94B5-CC35C54BB15C}"/>
   <tableColumns count="21">
-    <tableColumn id="1" xr3:uid="{E1FB3D0C-B874-4874-BACC-6872CF171957}" name="Tabellen Name" dataDxfId="98"/>
-    <tableColumn id="2" xr3:uid="{FFDD2777-2097-450C-B020-F133CF643855}" name="Geschlecht" dataDxfId="97"/>
-    <tableColumn id="3" xr3:uid="{8CF52BE2-8020-48BD-A36D-63F13A1878DE}" name="Mindest alter" dataDxfId="96"/>
-    <tableColumn id="4" xr3:uid="{FD3A030F-CD97-4B6F-8E8C-BC2E67D79F1D}" name="Maximales Alter" dataDxfId="95"/>
-    <tableColumn id="5" xr3:uid="{3E22B645-D77C-4509-B031-9914FCB91599}" name="Qualizeitraum anfang" dataDxfId="94"/>
-    <tableColumn id="6" xr3:uid="{AE299324-3C1C-4063-ADF9-54555A161734}" name="Qualizeitraum Ende" dataDxfId="93"/>
-    <tableColumn id="7" xr3:uid="{DCC178B3-11FC-4C53-BBC6-C2FDA2C89857}" name="Letzter Wettkampf am" dataDxfId="92"/>
-    <tableColumn id="8" xr3:uid="{2811DB01-60A5-4BE4-B6F9-A806398A602A}" name="Wertung" dataDxfId="91"/>
-    <tableColumn id="9" xr3:uid="{0C16DAFE-847D-4E9E-9604-3A7D9FE924D0}" name="Landesverband" dataDxfId="90"/>
-    <tableColumn id="10" xr3:uid="{7A8A4101-A553-4BD5-9116-9AA5876B9401}" name="OMS" dataDxfId="89"/>
-    <tableColumn id="11" xr3:uid="{9807C9BD-6499-45F6-ACE0-4D13D64EF675}" name="Pool-Länge" dataDxfId="88"/>
-    <tableColumn id="12" xr3:uid="{13D336DD-650F-4F2C-836F-361CA1528F6D}" name="Regelwerk" dataDxfId="87"/>
-    <tableColumn id="13" xr3:uid="{66660E2D-ADF2-4FB5-8A13-004F826EE908}" name="Referenz" dataDxfId="86"/>
-    <tableColumn id="19" xr3:uid="{D72EDF8B-ECC3-4FF7-ABE6-B60BCE4A5E26}" name="Referenz Jahr" dataDxfId="85"/>
-    <tableColumn id="20" xr3:uid="{7B18E667-70F7-4BC1-AB1B-21C019F2AA89}" name="Mindest Punktzahl" dataDxfId="84"/>
-    <tableColumn id="21" xr3:uid="{FC185946-681B-42A6-AB1A-FC1EABB668C5}" name="Mindest Disziplinen" dataDxfId="83"/>
-    <tableColumn id="14" xr3:uid="{6A2676FD-2EC7-4C41-A35E-A1597A38F932}" name="3-Kampf Regel" dataDxfId="82"/>
-    <tableColumn id="15" xr3:uid="{718E0917-4F83-4A2B-832F-EBB16D5E21BF}" name="Anzahl Nominierte" dataDxfId="81"/>
-    <tableColumn id="16" xr3:uid="{5C66A461-D647-4E00-A81C-FD7AD44D7CC2}" name="Anzahl Nachrücker" dataDxfId="80"/>
-    <tableColumn id="17" xr3:uid="{D434BDEC-293B-4B4E-A5E9-479438960A03}" name="Seiten Anzahl" dataDxfId="79"/>
-    <tableColumn id="18" xr3:uid="{80908229-9247-473F-81C0-9C9D4C12FF06}" name="Absagen" dataDxfId="78"/>
+    <tableColumn id="1" xr3:uid="{E1FB3D0C-B874-4874-BACC-6872CF171957}" name="Tabellen Name" dataDxfId="93"/>
+    <tableColumn id="2" xr3:uid="{FFDD2777-2097-450C-B020-F133CF643855}" name="Geschlecht" dataDxfId="92"/>
+    <tableColumn id="3" xr3:uid="{8CF52BE2-8020-48BD-A36D-63F13A1878DE}" name="Mindest alter" dataDxfId="91"/>
+    <tableColumn id="4" xr3:uid="{FD3A030F-CD97-4B6F-8E8C-BC2E67D79F1D}" name="Maximales Alter" dataDxfId="90"/>
+    <tableColumn id="5" xr3:uid="{3E22B645-D77C-4509-B031-9914FCB91599}" name="Qualizeitraum anfang" dataDxfId="89"/>
+    <tableColumn id="6" xr3:uid="{AE299324-3C1C-4063-ADF9-54555A161734}" name="Qualizeitraum Ende" dataDxfId="88"/>
+    <tableColumn id="7" xr3:uid="{DCC178B3-11FC-4C53-BBC6-C2FDA2C89857}" name="Letzter Wettkampf am" dataDxfId="87"/>
+    <tableColumn id="8" xr3:uid="{2811DB01-60A5-4BE4-B6F9-A806398A602A}" name="Wertung" dataDxfId="86"/>
+    <tableColumn id="9" xr3:uid="{0C16DAFE-847D-4E9E-9604-3A7D9FE924D0}" name="Landesverband" dataDxfId="85"/>
+    <tableColumn id="10" xr3:uid="{7A8A4101-A553-4BD5-9116-9AA5876B9401}" name="OMS" dataDxfId="84"/>
+    <tableColumn id="11" xr3:uid="{9807C9BD-6499-45F6-ACE0-4D13D64EF675}" name="Pool-Länge" dataDxfId="83"/>
+    <tableColumn id="12" xr3:uid="{13D336DD-650F-4F2C-836F-361CA1528F6D}" name="Regelwerk" dataDxfId="82"/>
+    <tableColumn id="13" xr3:uid="{66660E2D-ADF2-4FB5-8A13-004F826EE908}" name="Referenz" dataDxfId="81"/>
+    <tableColumn id="19" xr3:uid="{D72EDF8B-ECC3-4FF7-ABE6-B60BCE4A5E26}" name="Referenz Jahr" dataDxfId="80"/>
+    <tableColumn id="20" xr3:uid="{7B18E667-70F7-4BC1-AB1B-21C019F2AA89}" name="Mindest Punktzahl" dataDxfId="79"/>
+    <tableColumn id="21" xr3:uid="{FC185946-681B-42A6-AB1A-FC1EABB668C5}" name="Mindest Disziplinen" dataDxfId="78"/>
+    <tableColumn id="14" xr3:uid="{6A2676FD-2EC7-4C41-A35E-A1597A38F932}" name="3-Kampf Regel" dataDxfId="77"/>
+    <tableColumn id="15" xr3:uid="{718E0917-4F83-4A2B-832F-EBB16D5E21BF}" name="Anzahl Nominierte" dataDxfId="76"/>
+    <tableColumn id="16" xr3:uid="{5C66A461-D647-4E00-A81C-FD7AD44D7CC2}" name="Anzahl Nachrücker" dataDxfId="75"/>
+    <tableColumn id="17" xr3:uid="{D434BDEC-293B-4B4E-A5E9-479438960A03}" name="Seiten Anzahl" dataDxfId="74"/>
+    <tableColumn id="18" xr3:uid="{80908229-9247-473F-81C0-9C9D4C12FF06}" name="Absagen" dataDxfId="73"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{16F87202-5A6A-4E2F-B973-3CE7EC2566C1}" name="DEM_konfig" displayName="DEM_konfig" ref="A1:X7" totalsRowShown="0" headerRowDxfId="77" dataDxfId="76">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{16F87202-5A6A-4E2F-B973-3CE7EC2566C1}" name="DEM_konfig" displayName="DEM_konfig" ref="A1:X7" totalsRowShown="0" headerRowDxfId="72" dataDxfId="71">
   <autoFilter ref="A1:X7" xr:uid="{16F87202-5A6A-4E2F-B973-3CE7EC2566C1}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4657,37 +4657,37 @@
     <filterColumn colId="23" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{4847B567-64E1-4AC3-8C4B-EFCF3F00CC6C}" name="Tabellen Name" dataDxfId="75"/>
-    <tableColumn id="2" xr3:uid="{6346FF3B-B334-4CD8-8B23-F2347E29C536}" name="Geschlecht" dataDxfId="74"/>
-    <tableColumn id="3" xr3:uid="{E793B48A-BC8A-439F-8AAF-6FD08104A619}" name="Mindest Alter" dataDxfId="73"/>
-    <tableColumn id="4" xr3:uid="{01A62C29-2F75-4107-A431-F69230BCCD0C}" name="Maximales Alter" dataDxfId="72"/>
-    <tableColumn id="5" xr3:uid="{B7E4DE90-7856-4A0C-9063-61414D7F227C}" name="Qualizeitraum anfang" dataDxfId="71"/>
-    <tableColumn id="6" xr3:uid="{B00F7CD1-82CB-42B9-A396-89F79EF419CA}" name="Qualizeitraum Ende" dataDxfId="70"/>
-    <tableColumn id="7" xr3:uid="{9E50DDE5-12E3-4BCB-801C-FBABCE309F0E}" name="Letzter Wettkampf am" dataDxfId="69"/>
-    <tableColumn id="8" xr3:uid="{57E68247-0FF2-48D8-8ACD-AB057E576A21}" name="Landesverband" dataDxfId="68"/>
-    <tableColumn id="9" xr3:uid="{EBAA439D-F69A-4C2A-8193-9AE08F1E57B8}" name="OMS" dataDxfId="67"/>
-    <tableColumn id="10" xr3:uid="{BBD11E7F-3DDF-428A-B005-4A40E6FA78DC}" name="Pool-Länge" dataDxfId="66"/>
-    <tableColumn id="11" xr3:uid="{6AE38DCA-A084-4F3D-A6A4-4E76E3E2CBC6}" name="Regelwerk" dataDxfId="65"/>
-    <tableColumn id="12" xr3:uid="{7F7470AD-5502-4CEE-BB4C-44BA308E61D7}" name="Seiten Anzahl" dataDxfId="64"/>
-    <tableColumn id="13" xr3:uid="{F416CBFA-4C9D-45CD-9BA7-E4BC57A08BC2}" name="PZ1 - 50m Retten" dataDxfId="63"/>
-    <tableColumn id="14" xr3:uid="{7117DBCA-0DA7-462C-84FE-0DC7E33B124C}" name="PZ1 - 100m Retten" dataDxfId="62"/>
-    <tableColumn id="15" xr3:uid="{E8630E91-DC30-4822-9E53-6D65487C3670}" name="PZ1 - 100m Kombi" dataDxfId="61"/>
-    <tableColumn id="16" xr3:uid="{4B3AA225-E042-430F-8259-D176887B4528}" name="PZ1 - 100m Lifesaver" dataDxfId="60"/>
-    <tableColumn id="17" xr3:uid="{798674BD-98CE-4531-BDFF-6AB06253AD7C}" name="PZ1 - 200m Super-Lifesaver" dataDxfId="59"/>
-    <tableColumn id="18" xr3:uid="{8809BB71-D58B-4E8B-A442-D0EB9A65A25D}" name="PZ1 - 200m Hindernis" dataDxfId="58"/>
-    <tableColumn id="19" xr3:uid="{93DCF463-806B-4117-B4E3-1FFAE976B37C}" name="PZ2 - 50m Retten" dataDxfId="57"/>
-    <tableColumn id="20" xr3:uid="{A514C961-559E-462F-B143-BA30974C0129}" name="PZ2 - 100m Retten" dataDxfId="56"/>
-    <tableColumn id="21" xr3:uid="{F1CF6143-45FE-498D-93D6-36F26D2F3C0B}" name="PZ2 - 100m Kombi" dataDxfId="55"/>
-    <tableColumn id="22" xr3:uid="{E90962FC-C214-467F-841F-40DF60E41456}" name="PZ2 - 100m Lifesaver" dataDxfId="54"/>
-    <tableColumn id="23" xr3:uid="{7FBC6334-C4C8-4B38-9F59-30ED95A44379}" name="PZ2 - 200m Super-Lifesaver" dataDxfId="53"/>
-    <tableColumn id="24" xr3:uid="{231BFF86-8F3A-4BA1-B25E-28175D9EDFA9}" name="PZ2 - 200m Hindernis" dataDxfId="52"/>
+    <tableColumn id="1" xr3:uid="{4847B567-64E1-4AC3-8C4B-EFCF3F00CC6C}" name="Tabellen Name" dataDxfId="70"/>
+    <tableColumn id="2" xr3:uid="{6346FF3B-B334-4CD8-8B23-F2347E29C536}" name="Geschlecht" dataDxfId="69"/>
+    <tableColumn id="3" xr3:uid="{E793B48A-BC8A-439F-8AAF-6FD08104A619}" name="Mindest Alter" dataDxfId="68"/>
+    <tableColumn id="4" xr3:uid="{01A62C29-2F75-4107-A431-F69230BCCD0C}" name="Maximales Alter" dataDxfId="67"/>
+    <tableColumn id="5" xr3:uid="{B7E4DE90-7856-4A0C-9063-61414D7F227C}" name="Qualizeitraum anfang" dataDxfId="66"/>
+    <tableColumn id="6" xr3:uid="{B00F7CD1-82CB-42B9-A396-89F79EF419CA}" name="Qualizeitraum Ende" dataDxfId="65"/>
+    <tableColumn id="7" xr3:uid="{9E50DDE5-12E3-4BCB-801C-FBABCE309F0E}" name="Letzter Wettkampf am" dataDxfId="64"/>
+    <tableColumn id="8" xr3:uid="{57E68247-0FF2-48D8-8ACD-AB057E576A21}" name="Landesverband" dataDxfId="63"/>
+    <tableColumn id="9" xr3:uid="{EBAA439D-F69A-4C2A-8193-9AE08F1E57B8}" name="OMS" dataDxfId="62"/>
+    <tableColumn id="10" xr3:uid="{BBD11E7F-3DDF-428A-B005-4A40E6FA78DC}" name="Pool-Länge" dataDxfId="61"/>
+    <tableColumn id="11" xr3:uid="{6AE38DCA-A084-4F3D-A6A4-4E76E3E2CBC6}" name="Regelwerk" dataDxfId="60"/>
+    <tableColumn id="12" xr3:uid="{7F7470AD-5502-4CEE-BB4C-44BA308E61D7}" name="Seiten Anzahl" dataDxfId="59"/>
+    <tableColumn id="13" xr3:uid="{F416CBFA-4C9D-45CD-9BA7-E4BC57A08BC2}" name="PZ1 - 50m Retten" dataDxfId="58"/>
+    <tableColumn id="14" xr3:uid="{7117DBCA-0DA7-462C-84FE-0DC7E33B124C}" name="PZ1 - 100m Retten" dataDxfId="57"/>
+    <tableColumn id="15" xr3:uid="{E8630E91-DC30-4822-9E53-6D65487C3670}" name="PZ1 - 100m Kombi" dataDxfId="56"/>
+    <tableColumn id="16" xr3:uid="{4B3AA225-E042-430F-8259-D176887B4528}" name="PZ1 - 100m Lifesaver" dataDxfId="55"/>
+    <tableColumn id="17" xr3:uid="{798674BD-98CE-4531-BDFF-6AB06253AD7C}" name="PZ1 - 200m Super-Lifesaver" dataDxfId="54"/>
+    <tableColumn id="18" xr3:uid="{8809BB71-D58B-4E8B-A442-D0EB9A65A25D}" name="PZ1 - 200m Hindernis" dataDxfId="53"/>
+    <tableColumn id="19" xr3:uid="{93DCF463-806B-4117-B4E3-1FFAE976B37C}" name="PZ2 - 50m Retten" dataDxfId="52"/>
+    <tableColumn id="20" xr3:uid="{A514C961-559E-462F-B143-BA30974C0129}" name="PZ2 - 100m Retten" dataDxfId="51"/>
+    <tableColumn id="21" xr3:uid="{F1CF6143-45FE-498D-93D6-36F26D2F3C0B}" name="PZ2 - 100m Kombi" dataDxfId="50"/>
+    <tableColumn id="22" xr3:uid="{E90962FC-C214-467F-841F-40DF60E41456}" name="PZ2 - 100m Lifesaver" dataDxfId="49"/>
+    <tableColumn id="23" xr3:uid="{7FBC6334-C4C8-4B38-9F59-30ED95A44379}" name="PZ2 - 200m Super-Lifesaver" dataDxfId="48"/>
+    <tableColumn id="24" xr3:uid="{231BFF86-8F3A-4BA1-B25E-28175D9EDFA9}" name="PZ2 - 200m Hindernis" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}" name="JRP_konfig" displayName="JRP_konfig" ref="A1:X15" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}" name="JRP_konfig" displayName="JRP_konfig" ref="A1:X15" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
   <autoFilter ref="A1:X15" xr:uid="{D7CDEF11-F813-469D-9DE0-678961AB7005}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4715,30 +4715,30 @@
     <filterColumn colId="23" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="24">
-    <tableColumn id="1" xr3:uid="{021DA6E1-2C93-4474-9720-B6F016186D61}" name="Tabellen Name" dataDxfId="49"/>
-    <tableColumn id="2" xr3:uid="{733C1722-A9C9-4830-A9E2-FE62E96BCD98}" name="Geschlecht" dataDxfId="48"/>
-    <tableColumn id="3" xr3:uid="{80C0BF46-0E43-4947-BF86-B808C324772A}" name="Mindest Alter" dataDxfId="47"/>
-    <tableColumn id="4" xr3:uid="{DBA2A923-EEB7-43F9-A1A3-E78624448FB9}" name="Maximales Alter" dataDxfId="46"/>
-    <tableColumn id="5" xr3:uid="{3FDEE18A-328D-45AE-907D-69A916A93345}" name="Qualizeitraum anfang" dataDxfId="45"/>
-    <tableColumn id="6" xr3:uid="{BE002D7F-575F-4B60-9251-C71D93F59045}" name="Qualizeitraum Ende" dataDxfId="44"/>
-    <tableColumn id="7" xr3:uid="{208ABD57-DE4B-41D6-B9FC-93F2D8966E8D}" name="Letzter Wettkampf am" dataDxfId="43"/>
-    <tableColumn id="8" xr3:uid="{30C9697C-6550-4996-ADDB-7FEE5325B794}" name="Landesverband" dataDxfId="42"/>
-    <tableColumn id="9" xr3:uid="{ED2DAB77-EF46-4D8B-B8E4-90412E32E277}" name="OMS" dataDxfId="41"/>
-    <tableColumn id="10" xr3:uid="{AD534940-A91B-4A6E-9606-E3F3E517D401}" name="Pool-Länge" dataDxfId="40"/>
-    <tableColumn id="11" xr3:uid="{11F9D5D5-72FE-42CA-8624-01D513B4140F}" name="Regelwerk" dataDxfId="39"/>
-    <tableColumn id="12" xr3:uid="{3907872B-5438-4FBF-A045-3EF9EAACFC47}" name="Seiten Anzahl" dataDxfId="38"/>
-    <tableColumn id="13" xr3:uid="{FC821324-3638-40C0-BA1E-069B44E23C7A}" name="PZ1 - 50m Retten" dataDxfId="37"/>
-    <tableColumn id="14" xr3:uid="{70529619-443E-40D3-88C1-3E0F00BB2A50}" name="PZ1 - 100m Retten" dataDxfId="36"/>
-    <tableColumn id="15" xr3:uid="{EFA92FD2-C23F-42B3-83DC-5036513F19AF}" name="PZ1 - 100m Kombi" dataDxfId="35"/>
-    <tableColumn id="16" xr3:uid="{03309E52-8CF3-4E90-9EE6-A818901C3B32}" name="PZ1 - 100m Lifesaver" dataDxfId="34"/>
-    <tableColumn id="17" xr3:uid="{00B22013-AA11-4C17-9250-22060AE4B0A8}" name="PZ1 - 200m Super-Lifesaver" dataDxfId="33"/>
-    <tableColumn id="18" xr3:uid="{7E3508A9-0422-4561-A23E-53E613259B24}" name="PZ1 - 200m Hindernis" dataDxfId="32"/>
-    <tableColumn id="19" xr3:uid="{5CEA435F-F34B-4D8D-88D0-F5EBFF18B713}" name="PZ2 - 50m Retten" dataDxfId="31"/>
-    <tableColumn id="20" xr3:uid="{8585BE62-F7C4-4D5D-B287-052B43B08610}" name="PZ2 - 100m Retten" dataDxfId="30"/>
-    <tableColumn id="21" xr3:uid="{D981758B-ADAD-4E36-B787-0B0FDA808CA2}" name="PZ2 - 100m Kombi" dataDxfId="29"/>
-    <tableColumn id="22" xr3:uid="{1D4970A8-D22F-4962-934C-AEA295ED687A}" name="PZ2 - 100m Lifesaver" dataDxfId="28"/>
-    <tableColumn id="23" xr3:uid="{BE394430-C58F-4690-9615-44475E5AF9F8}" name="PZ2 - 200m Super-Lifesaver" dataDxfId="27"/>
-    <tableColumn id="24" xr3:uid="{A7036B1A-99CE-4F7C-AAB8-12E8B2696202}" name="PZ2 - 200m Hindernis" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{021DA6E1-2C93-4474-9720-B6F016186D61}" name="Tabellen Name" dataDxfId="44"/>
+    <tableColumn id="2" xr3:uid="{733C1722-A9C9-4830-A9E2-FE62E96BCD98}" name="Geschlecht" dataDxfId="43"/>
+    <tableColumn id="3" xr3:uid="{80C0BF46-0E43-4947-BF86-B808C324772A}" name="Mindest Alter" dataDxfId="42"/>
+    <tableColumn id="4" xr3:uid="{DBA2A923-EEB7-43F9-A1A3-E78624448FB9}" name="Maximales Alter" dataDxfId="41"/>
+    <tableColumn id="5" xr3:uid="{3FDEE18A-328D-45AE-907D-69A916A93345}" name="Qualizeitraum anfang" dataDxfId="40"/>
+    <tableColumn id="6" xr3:uid="{BE002D7F-575F-4B60-9251-C71D93F59045}" name="Qualizeitraum Ende" dataDxfId="39"/>
+    <tableColumn id="7" xr3:uid="{208ABD57-DE4B-41D6-B9FC-93F2D8966E8D}" name="Letzter Wettkampf am" dataDxfId="38"/>
+    <tableColumn id="8" xr3:uid="{30C9697C-6550-4996-ADDB-7FEE5325B794}" name="Landesverband" dataDxfId="37"/>
+    <tableColumn id="9" xr3:uid="{ED2DAB77-EF46-4D8B-B8E4-90412E32E277}" name="OMS" dataDxfId="36"/>
+    <tableColumn id="10" xr3:uid="{AD534940-A91B-4A6E-9606-E3F3E517D401}" name="Pool-Länge" dataDxfId="35"/>
+    <tableColumn id="11" xr3:uid="{11F9D5D5-72FE-42CA-8624-01D513B4140F}" name="Regelwerk" dataDxfId="34"/>
+    <tableColumn id="12" xr3:uid="{3907872B-5438-4FBF-A045-3EF9EAACFC47}" name="Seiten Anzahl" dataDxfId="33"/>
+    <tableColumn id="13" xr3:uid="{FC821324-3638-40C0-BA1E-069B44E23C7A}" name="PZ1 - 50m Retten" dataDxfId="32"/>
+    <tableColumn id="14" xr3:uid="{70529619-443E-40D3-88C1-3E0F00BB2A50}" name="PZ1 - 100m Retten" dataDxfId="31"/>
+    <tableColumn id="15" xr3:uid="{EFA92FD2-C23F-42B3-83DC-5036513F19AF}" name="PZ1 - 100m Kombi" dataDxfId="30"/>
+    <tableColumn id="16" xr3:uid="{03309E52-8CF3-4E90-9EE6-A818901C3B32}" name="PZ1 - 100m Lifesaver" dataDxfId="29"/>
+    <tableColumn id="17" xr3:uid="{00B22013-AA11-4C17-9250-22060AE4B0A8}" name="PZ1 - 200m Super-Lifesaver" dataDxfId="28"/>
+    <tableColumn id="18" xr3:uid="{7E3508A9-0422-4561-A23E-53E613259B24}" name="PZ1 - 200m Hindernis" dataDxfId="27"/>
+    <tableColumn id="19" xr3:uid="{5CEA435F-F34B-4D8D-88D0-F5EBFF18B713}" name="PZ2 - 50m Retten" dataDxfId="26"/>
+    <tableColumn id="20" xr3:uid="{8585BE62-F7C4-4D5D-B287-052B43B08610}" name="PZ2 - 100m Retten" dataDxfId="25"/>
+    <tableColumn id="21" xr3:uid="{D981758B-ADAD-4E36-B787-0B0FDA808CA2}" name="PZ2 - 100m Kombi" dataDxfId="24"/>
+    <tableColumn id="22" xr3:uid="{1D4970A8-D22F-4962-934C-AEA295ED687A}" name="PZ2 - 100m Lifesaver" dataDxfId="23"/>
+    <tableColumn id="23" xr3:uid="{BE394430-C58F-4690-9615-44475E5AF9F8}" name="PZ2 - 200m Super-Lifesaver" dataDxfId="22"/>
+    <tableColumn id="24" xr3:uid="{A7036B1A-99CE-4F7C-AAB8-12E8B2696202}" name="PZ2 - 200m Hindernis" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4748,12 +4748,12 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{888CE7BE-8313-44C0-AE38-83992EABD44D}" name="LK_Kalender" displayName="LK_Kalender" ref="A1:H10" totalsRowShown="0">
   <autoFilter ref="A1:H10" xr:uid="{888CE7BE-8313-44C0-AE38-83992EABD44D}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{B26B9E90-F378-41EF-B35E-CE240017E4BE}" name="datum von" dataDxfId="25"/>
+    <tableColumn id="1" xr3:uid="{B26B9E90-F378-41EF-B35E-CE240017E4BE}" name="datum von" dataDxfId="201"/>
     <tableColumn id="2" xr3:uid="{38211212-0A92-428C-895C-E4CA68F52818}" name="datum bis"/>
-    <tableColumn id="3" xr3:uid="{66E541C6-0A5E-4B2D-9B89-5E52F449A4A6}" name="uhrzeit von" dataDxfId="24"/>
-    <tableColumn id="4" xr3:uid="{D93C06A2-29AD-4073-8E3C-A685B4474CC8}" name="uhrzeit bis" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{C5C3979C-B528-44E8-A5A6-36F020A6034F}" name="titel" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{9DC09E1D-44FD-40ED-9EBE-86A8E61C38B2}" name="meta" dataDxfId="21"/>
+    <tableColumn id="3" xr3:uid="{66E541C6-0A5E-4B2D-9B89-5E52F449A4A6}" name="uhrzeit von" dataDxfId="200"/>
+    <tableColumn id="4" xr3:uid="{D93C06A2-29AD-4073-8E3C-A685B4474CC8}" name="uhrzeit bis" dataDxfId="199"/>
+    <tableColumn id="5" xr3:uid="{C5C3979C-B528-44E8-A5A6-36F020A6034F}" name="titel" dataDxfId="198"/>
+    <tableColumn id="6" xr3:uid="{9DC09E1D-44FD-40ED-9EBE-86A8E61C38B2}" name="meta" dataDxfId="197"/>
     <tableColumn id="7" xr3:uid="{E7E62A34-7A76-4361-937D-F4DE76E6E7CC}" name="ort"/>
     <tableColumn id="8" xr3:uid="{84F02734-FC16-406B-ACCA-0CCDF547D94C}" name="kader"/>
   </tableColumns>
@@ -5085,9 +5085,9 @@
       <selection activeCell="Y25" sqref="Y25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.265625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="42" t="s">
         <v>39</v>
       </c>
@@ -5156,7 +5156,7 @@
       <c r="AV1" s="44"/>
       <c r="AW1" s="44"/>
     </row>
-    <row r="2" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="42" t="s">
         <v>40</v>
       </c>
@@ -5223,7 +5223,7 @@
       <c r="AV2" s="45"/>
       <c r="AW2" s="45"/>
     </row>
-    <row r="3" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="42" t="s">
         <v>101</v>
       </c>
@@ -5284,7 +5284,7 @@
       <c r="AV3" s="45"/>
       <c r="AW3" s="45"/>
     </row>
-    <row r="4" spans="1:49" s="53" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:49" s="53" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="49" t="s">
         <v>10</v>
       </c>
@@ -5433,7 +5433,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>2000</v>
       </c>
@@ -5486,7 +5486,7 @@
       <c r="AV5" s="10"/>
       <c r="AW5" s="10"/>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <f t="shared" ref="A6:A31" si="0">A5+1</f>
         <v>2001</v>
@@ -5564,7 +5564,7 @@
       <c r="AV6" s="11"/>
       <c r="AW6" s="11"/>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>2002</v>
@@ -5642,7 +5642,7 @@
       <c r="AV7" s="10"/>
       <c r="AW7" s="10"/>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>2003</v>
@@ -5720,7 +5720,7 @@
       <c r="AV8" s="11"/>
       <c r="AW8" s="11"/>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>2004</v>
@@ -5798,7 +5798,7 @@
       <c r="AV9" s="10"/>
       <c r="AW9" s="10"/>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>2005</v>
@@ -5876,7 +5876,7 @@
       <c r="AV10" s="11"/>
       <c r="AW10" s="11"/>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>2006</v>
@@ -5954,7 +5954,7 @@
       <c r="AV11" s="10"/>
       <c r="AW11" s="10"/>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>2007</v>
@@ -6076,7 +6076,7 @@
         <v>3.5995370370370369E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>2008</v>
@@ -6198,7 +6198,7 @@
         <v>3.5995370370370369E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>2009</v>
@@ -6320,7 +6320,7 @@
         <v>3.5995370370370369E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>2010</v>
@@ -6442,7 +6442,7 @@
         <v>3.5995370370370369E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>2011</v>
@@ -6576,7 +6576,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>2012</v>
@@ -6710,7 +6710,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>2013</v>
@@ -6844,7 +6844,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>2014</v>
@@ -6978,7 +6978,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>2015</v>
@@ -7112,7 +7112,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>2016</v>
@@ -7246,7 +7246,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>2017</v>
@@ -7380,7 +7380,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>2018</v>
@@ -7514,7 +7514,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>2019</v>
@@ -7648,7 +7648,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>2020</v>
@@ -7798,7 +7798,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>2021</v>
@@ -7948,7 +7948,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>2022</v>
@@ -8098,7 +8098,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>2023</v>
@@ -8248,7 +8248,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>2024</v>
@@ -8398,7 +8398,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>2025</v>
@@ -8548,7 +8548,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:49" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:49" x14ac:dyDescent="0.45">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>2026</v>
@@ -8769,15 +8769,15 @@
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
-    <col min="2" max="13" width="18.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.86328125" style="1" customWidth="1"/>
+    <col min="2" max="13" width="18.73046875" style="1" customWidth="1"/>
     <col min="14" max="14" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="11.42578125" style="1"/>
+    <col min="15" max="16384" width="11.3984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="18">
         <v>2024</v>
       </c>
@@ -8821,7 +8821,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
@@ -8877,7 +8877,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -8933,7 +8933,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="19" t="s">
         <v>8</v>
       </c>
@@ -8989,7 +8989,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" s="175" t="s">
         <v>13</v>
       </c>
@@ -9007,7 +9007,7 @@
       <c r="M7" s="175"/>
       <c r="N7" s="175"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" s="175"/>
       <c r="B8" s="175"/>
       <c r="C8" s="175"/>
@@ -9023,7 +9023,7 @@
       <c r="M8" s="175"/>
       <c r="N8" s="175"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" s="20" t="s">
         <v>6</v>
       </c>
@@ -9077,7 +9077,7 @@
       </c>
       <c r="N9" s="21"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" s="20" t="s">
         <v>7</v>
       </c>
@@ -9131,7 +9131,7 @@
       </c>
       <c r="N10" s="21"/>
     </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="22" t="s">
         <v>8</v>
       </c>
@@ -9185,7 +9185,7 @@
       </c>
       <c r="N11" s="23"/>
     </row>
-    <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="174" t="s">
         <v>14</v>
       </c>
@@ -9206,7 +9206,7 @@
       <c r="M14"/>
       <c r="N14"/>
     </row>
-    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="174"/>
       <c r="B15" s="174"/>
       <c r="C15" s="174"/>
@@ -9221,7 +9221,7 @@
       <c r="M15"/>
       <c r="N15"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -9256,7 +9256,7 @@
       <c r="M16"/>
       <c r="N16"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A17" s="8" t="s">
         <v>19</v>
       </c>
@@ -9291,7 +9291,7 @@
       <c r="M17"/>
       <c r="N17"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>19</v>
       </c>
@@ -9324,7 +9324,7 @@
       <c r="M18"/>
       <c r="N18"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A19" s="8" t="s">
         <v>22</v>
       </c>
@@ -9357,7 +9357,7 @@
       <c r="M19"/>
       <c r="N19"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A20" s="9" t="s">
         <v>24</v>
       </c>
@@ -9388,7 +9388,7 @@
       <c r="M20"/>
       <c r="N20"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A21" s="8" t="s">
         <v>22</v>
       </c>
@@ -9415,7 +9415,7 @@
       <c r="M21"/>
       <c r="N21"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
         <v>19</v>
       </c>
@@ -9438,7 +9438,7 @@
       <c r="I22" s="33"/>
       <c r="L22" s="41"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A23" s="8" t="s">
         <v>19</v>
       </c>
@@ -9461,50 +9461,50 @@
       <c r="I23" s="33"/>
       <c r="L23" s="40"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
       <c r="H24" s="33"/>
       <c r="I24" s="33"/>
       <c r="L24" s="41"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
       <c r="H25" s="33"/>
       <c r="I25" s="33"/>
       <c r="L25" s="40"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L26" s="41"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L27" s="40"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L28" s="41"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L29" s="40"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L30" s="41"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L31" s="40"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.45">
       <c r="L32" s="41"/>
     </row>
-    <row r="33" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L33" s="40"/>
     </row>
-    <row r="34" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L34" s="41"/>
     </row>
-    <row r="35" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L35" s="33"/>
     </row>
-    <row r="36" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L36" s="41"/>
     </row>
-    <row r="37" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="12:12" x14ac:dyDescent="0.45">
       <c r="L37" s="33"/>
     </row>
   </sheetData>
@@ -9530,15 +9530,15 @@
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
-    <col min="2" max="13" width="18.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.86328125" style="1" customWidth="1"/>
+    <col min="2" max="13" width="18.73046875" style="1" customWidth="1"/>
     <col min="14" max="14" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="11.42578125" style="1"/>
+    <col min="15" max="16384" width="11.3984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="18">
         <v>2025</v>
       </c>
@@ -9582,7 +9582,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
@@ -9638,7 +9638,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -9694,7 +9694,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="19" t="s">
         <v>8</v>
       </c>
@@ -9750,7 +9750,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" s="175" t="s">
         <v>13</v>
       </c>
@@ -9768,7 +9768,7 @@
       <c r="M7" s="175"/>
       <c r="N7" s="175"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" s="175"/>
       <c r="B8" s="175"/>
       <c r="C8" s="175"/>
@@ -9784,7 +9784,7 @@
       <c r="M8" s="175"/>
       <c r="N8" s="175"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" s="20" t="s">
         <v>6</v>
       </c>
@@ -9838,7 +9838,7 @@
       </c>
       <c r="N9" s="21"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" s="20" t="s">
         <v>7</v>
       </c>
@@ -9892,7 +9892,7 @@
       </c>
       <c r="N10" s="21"/>
     </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="22" t="s">
         <v>8</v>
       </c>
@@ -9946,7 +9946,7 @@
       </c>
       <c r="N11" s="23"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A14" s="174" t="s">
         <v>14</v>
       </c>
@@ -9965,7 +9965,7 @@
       </c>
       <c r="M14"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A15" s="174"/>
       <c r="B15" s="174"/>
       <c r="C15" s="174"/>
@@ -9978,7 +9978,7 @@
       <c r="L15" s="176"/>
       <c r="M15"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -10011,7 +10011,7 @@
       </c>
       <c r="M16"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="8" t="s">
         <v>28</v>
       </c>
@@ -10044,7 +10044,7 @@
       </c>
       <c r="M17"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>28</v>
       </c>
@@ -10075,7 +10075,7 @@
       <c r="L18" s="38"/>
       <c r="M18"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="8" t="s">
         <v>29</v>
       </c>
@@ -10106,7 +10106,7 @@
       <c r="L19" s="36"/>
       <c r="M19"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="9" t="s">
         <v>30</v>
       </c>
@@ -10135,7 +10135,7 @@
       <c r="L20" s="38"/>
       <c r="M20"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="8" t="s">
         <v>29</v>
       </c>
@@ -10166,7 +10166,7 @@
       <c r="L21" s="36"/>
       <c r="M21"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
         <v>28</v>
       </c>
@@ -10197,7 +10197,7 @@
       <c r="L22" s="39"/>
       <c r="M22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" s="8" t="s">
         <v>28</v>
       </c>
@@ -10228,66 +10228,66 @@
       <c r="L23" s="37"/>
       <c r="M23"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="H24" s="40"/>
       <c r="I24" s="40"/>
       <c r="J24" s="40"/>
       <c r="L24" s="39"/>
       <c r="M24"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="H25" s="33"/>
       <c r="I25" s="33"/>
       <c r="L25" s="37"/>
       <c r="M25"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L26" s="39"/>
       <c r="M26"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L27" s="37"/>
       <c r="M27"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L28" s="39"/>
       <c r="M28"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L29" s="37"/>
       <c r="M29"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L30" s="39"/>
       <c r="M30"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L31" s="37"/>
       <c r="M31"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L32" s="39"/>
       <c r="M32"/>
     </row>
-    <row r="33" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="8:13" x14ac:dyDescent="0.45">
       <c r="L33" s="37"/>
       <c r="M33"/>
     </row>
-    <row r="34" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="8:13" x14ac:dyDescent="0.45">
       <c r="L34" s="39"/>
       <c r="M34"/>
     </row>
-    <row r="35" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:13" x14ac:dyDescent="0.45">
       <c r="M35"/>
     </row>
-    <row r="36" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="8:13" x14ac:dyDescent="0.45">
       <c r="L36" s="39"/>
       <c r="M36"/>
     </row>
-    <row r="37" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="8:13" x14ac:dyDescent="0.45">
       <c r="M37"/>
     </row>
-    <row r="38" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="8:13" x14ac:dyDescent="0.45">
       <c r="H38"/>
       <c r="I38"/>
       <c r="J38"/>
@@ -10295,7 +10295,7 @@
       <c r="L38"/>
       <c r="M38"/>
     </row>
-    <row r="39" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="8:13" x14ac:dyDescent="0.45">
       <c r="H39"/>
       <c r="I39"/>
       <c r="J39"/>
@@ -10326,15 +10326,15 @@
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
-    <col min="2" max="13" width="18.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.86328125" style="1" customWidth="1"/>
+    <col min="2" max="13" width="18.73046875" style="1" customWidth="1"/>
     <col min="14" max="14" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="11.42578125" style="1"/>
+    <col min="15" max="16384" width="11.3984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="18">
         <v>2026</v>
       </c>
@@ -10378,7 +10378,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
@@ -10434,7 +10434,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -10490,7 +10490,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="19" t="s">
         <v>8</v>
       </c>
@@ -10546,7 +10546,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A7" s="175" t="s">
         <v>13</v>
       </c>
@@ -10564,7 +10564,7 @@
       <c r="M7" s="175"/>
       <c r="N7" s="175"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A8" s="175"/>
       <c r="B8" s="175"/>
       <c r="C8" s="175"/>
@@ -10580,7 +10580,7 @@
       <c r="M8" s="175"/>
       <c r="N8" s="175"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A9" s="20" t="s">
         <v>6</v>
       </c>
@@ -10634,7 +10634,7 @@
       </c>
       <c r="N9" s="21"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A10" s="20" t="s">
         <v>7</v>
       </c>
@@ -10688,7 +10688,7 @@
       </c>
       <c r="N10" s="21"/>
     </row>
-    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A11" s="22" t="s">
         <v>8</v>
       </c>
@@ -10742,7 +10742,7 @@
       </c>
       <c r="N11" s="23"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A14" s="174" t="s">
         <v>14</v>
       </c>
@@ -10761,7 +10761,7 @@
       </c>
       <c r="M14"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A15" s="174"/>
       <c r="B15" s="174"/>
       <c r="C15" s="174"/>
@@ -10774,7 +10774,7 @@
       <c r="L15" s="176"/>
       <c r="M15"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -10807,7 +10807,7 @@
       </c>
       <c r="M16"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="8" t="s">
         <v>28</v>
       </c>
@@ -10840,7 +10840,7 @@
       </c>
       <c r="M17"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="9" t="s">
         <v>28</v>
       </c>
@@ -10871,7 +10871,7 @@
       <c r="L18" s="38"/>
       <c r="M18"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="8" t="s">
         <v>29</v>
       </c>
@@ -10902,7 +10902,7 @@
       <c r="L19" s="36"/>
       <c r="M19"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="9" t="s">
         <v>30</v>
       </c>
@@ -10931,7 +10931,7 @@
       <c r="L20" s="38"/>
       <c r="M20"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="8" t="s">
         <v>29</v>
       </c>
@@ -10962,7 +10962,7 @@
       <c r="L21" s="36"/>
       <c r="M21"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
         <v>28</v>
       </c>
@@ -10993,7 +10993,7 @@
       <c r="L22" s="39"/>
       <c r="M22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" s="8" t="s">
         <v>28</v>
       </c>
@@ -11024,66 +11024,66 @@
       <c r="L23" s="37"/>
       <c r="M23"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="H24" s="40"/>
       <c r="I24" s="40"/>
       <c r="J24" s="40"/>
       <c r="L24" s="39"/>
       <c r="M24"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="H25" s="33"/>
       <c r="I25" s="33"/>
       <c r="L25" s="37"/>
       <c r="M25"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L26" s="39"/>
       <c r="M26"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L27" s="37"/>
       <c r="M27"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L28" s="39"/>
       <c r="M28"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L29" s="37"/>
       <c r="M29"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L30" s="39"/>
       <c r="M30"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L31" s="37"/>
       <c r="M31"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="L32" s="39"/>
       <c r="M32"/>
     </row>
-    <row r="33" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="8:13" x14ac:dyDescent="0.45">
       <c r="L33" s="37"/>
       <c r="M33"/>
     </row>
-    <row r="34" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="8:13" x14ac:dyDescent="0.45">
       <c r="L34" s="39"/>
       <c r="M34"/>
     </row>
-    <row r="35" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="8:13" x14ac:dyDescent="0.45">
       <c r="M35"/>
     </row>
-    <row r="36" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="8:13" x14ac:dyDescent="0.45">
       <c r="L36" s="39"/>
       <c r="M36"/>
     </row>
-    <row r="37" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="8:13" x14ac:dyDescent="0.45">
       <c r="M37"/>
     </row>
-    <row r="38" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="8:13" x14ac:dyDescent="0.45">
       <c r="H38"/>
       <c r="I38"/>
       <c r="J38"/>
@@ -11091,7 +11091,7 @@
       <c r="L38"/>
       <c r="M38"/>
     </row>
-    <row r="39" spans="8:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="8:13" x14ac:dyDescent="0.45">
       <c r="H39"/>
       <c r="I39"/>
       <c r="J39"/>
@@ -11120,17 +11120,17 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" customWidth="1"/>
-    <col min="7" max="11" width="18.7109375" customWidth="1"/>
-    <col min="12" max="12" width="22.140625" customWidth="1"/>
-    <col min="13" max="13" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="12.265625" customWidth="1"/>
+    <col min="2" max="5" width="18.73046875" customWidth="1"/>
+    <col min="6" max="6" width="21.1328125" customWidth="1"/>
+    <col min="7" max="11" width="18.73046875" customWidth="1"/>
+    <col min="12" max="12" width="22.1328125" customWidth="1"/>
+    <col min="13" max="13" width="18.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="42" t="s">
         <v>39</v>
       </c>
@@ -11171,7 +11171,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="42" t="s">
         <v>40</v>
       </c>
@@ -11212,7 +11212,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="42" t="s">
         <v>41</v>
       </c>
@@ -11253,7 +11253,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -11294,7 +11294,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>2000</v>
       </c>
@@ -11311,7 +11311,7 @@
       <c r="L5" s="11"/>
       <c r="M5" s="11"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <f t="shared" ref="A6:A32" si="0">A5+1</f>
         <v>2001</v>
@@ -11329,7 +11329,7 @@
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>2002</v>
@@ -11347,7 +11347,7 @@
       <c r="L7" s="11"/>
       <c r="M7" s="11"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>2003</v>
@@ -11365,7 +11365,7 @@
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>2004</v>
@@ -11383,7 +11383,7 @@
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>2005</v>
@@ -11401,7 +11401,7 @@
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>2006</v>
@@ -11419,7 +11419,7 @@
       <c r="L11" s="11"/>
       <c r="M11" s="11"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>2007</v>
@@ -11437,7 +11437,7 @@
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>2008</v>
@@ -11455,7 +11455,7 @@
       <c r="L13" s="11"/>
       <c r="M13" s="11"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>2009</v>
@@ -11473,7 +11473,7 @@
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>2010</v>
@@ -11491,7 +11491,7 @@
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>2011</v>
@@ -11509,7 +11509,7 @@
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>2012</v>
@@ -11527,7 +11527,7 @@
       <c r="L17" s="11"/>
       <c r="M17" s="11"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>2013</v>
@@ -11545,7 +11545,7 @@
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>2014</v>
@@ -11563,7 +11563,7 @@
       <c r="L19" s="11"/>
       <c r="M19" s="11"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>2015</v>
@@ -11605,7 +11605,7 @@
         <v>1.3592592592592591E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>2016</v>
@@ -11647,7 +11647,7 @@
         <v>1.3592592592592591E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>2017</v>
@@ -11689,7 +11689,7 @@
         <v>1.3577546296296298E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>2018</v>
@@ -11731,7 +11731,7 @@
         <v>1.3577546296296298E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>2019</v>
@@ -11773,7 +11773,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>2020</v>
@@ -11815,7 +11815,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>2021</v>
@@ -11857,7 +11857,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>2022</v>
@@ -11899,7 +11899,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>2023</v>
@@ -11941,7 +11941,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>2024</v>
@@ -11983,7 +11983,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>2025</v>
@@ -12025,7 +12025,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>2026</v>
@@ -12067,7 +12067,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A32" s="2">
         <f t="shared" si="0"/>
         <v>2027</v>
@@ -12147,17 +12147,17 @@
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.85546875" customWidth="1"/>
-    <col min="2" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="21.140625" customWidth="1"/>
-    <col min="7" max="11" width="18.7109375" customWidth="1"/>
-    <col min="12" max="12" width="22.140625" customWidth="1"/>
-    <col min="13" max="13" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="11.86328125" customWidth="1"/>
+    <col min="2" max="5" width="18.73046875" customWidth="1"/>
+    <col min="6" max="6" width="21.1328125" customWidth="1"/>
+    <col min="7" max="11" width="18.73046875" customWidth="1"/>
+    <col min="12" max="12" width="22.1328125" customWidth="1"/>
+    <col min="13" max="13" width="18.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="42" t="s">
         <v>39</v>
       </c>
@@ -12198,7 +12198,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="42" t="s">
         <v>40</v>
       </c>
@@ -12239,7 +12239,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="42" t="s">
         <v>41</v>
       </c>
@@ -12280,7 +12280,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -12321,7 +12321,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5" s="2">
         <v>2000</v>
       </c>
@@ -12338,7 +12338,7 @@
       <c r="L5" s="38"/>
       <c r="M5" s="38"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6" s="2">
         <f t="shared" ref="A6:A31" si="0">A5+1</f>
         <v>2001</v>
@@ -12368,7 +12368,7 @@
         <v>1.3629629629629632E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>2002</v>
@@ -12410,7 +12410,7 @@
         <v>1.3629629629629632E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>2003</v>
@@ -12452,7 +12452,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>2004</v>
@@ -12494,7 +12494,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>2005</v>
@@ -12536,7 +12536,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>2006</v>
@@ -12578,7 +12578,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>2007</v>
@@ -12620,7 +12620,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>2008</v>
@@ -12662,7 +12662,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>2009</v>
@@ -12704,7 +12704,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>2010</v>
@@ -12746,7 +12746,7 @@
         <v>1.3306712962962966E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>2011</v>
@@ -12788,7 +12788,7 @@
         <v>1.3306712962962966E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>2012</v>
@@ -12830,7 +12830,7 @@
         <v>1.3306712962962966E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>2013</v>
@@ -12872,7 +12872,7 @@
         <v>1.312962962962963E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>2014</v>
@@ -12914,7 +12914,7 @@
         <v>1.312962962962963E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>2015</v>
@@ -12956,7 +12956,7 @@
         <v>1.3116898148148148E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>2016</v>
@@ -12998,7 +12998,7 @@
         <v>1.3116898148148148E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>2017</v>
@@ -13040,7 +13040,7 @@
         <v>1.3116898148148148E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>2018</v>
@@ -13082,7 +13082,7 @@
         <v>1.3116898148148148E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>2019</v>
@@ -13124,7 +13124,7 @@
         <v>1.3116898148148148E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>2020</v>
@@ -13166,7 +13166,7 @@
         <v>1.3097222222222223E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>2021</v>
@@ -13208,7 +13208,7 @@
         <v>1.3097222222222223E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>2022</v>
@@ -13250,7 +13250,7 @@
         <v>1.3097222222222223E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>2023</v>
@@ -13292,7 +13292,7 @@
         <v>1.3097222222222223E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>2024</v>
@@ -13334,7 +13334,7 @@
         <v>1.3097222222222223E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>2025</v>
@@ -13376,7 +13376,7 @@
         <v>1.2931712962962962E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>2026</v>
@@ -13418,7 +13418,7 @@
         <v>1.2931712962962962E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A32" s="2">
         <f>A31+1</f>
         <v>2027</v>
@@ -13500,30 +13500,30 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.59765625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.73046875" customWidth="1"/>
     <col min="15" max="16" width="19" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="22.265625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.73046875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="47.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="60" t="s">
         <v>161</v>
       </c>
@@ -13588,7 +13588,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A2" s="59" t="s">
         <v>197</v>
       </c>
@@ -13649,7 +13649,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A3" s="59" t="s">
         <v>198</v>
       </c>
@@ -13729,30 +13729,30 @@
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.86328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.73046875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.73046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.59765625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.73046875" customWidth="1"/>
     <col min="15" max="16" width="19" customWidth="1"/>
-    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="22.265625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.73046875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="47.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="60" t="s">
         <v>161</v>
       </c>
@@ -13817,7 +13817,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A2" s="59" t="s">
         <v>189</v>
       </c>
@@ -13878,7 +13878,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A3" s="59" t="s">
         <v>190</v>
       </c>
@@ -13939,7 +13939,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A4" s="59" t="s">
         <v>191</v>
       </c>
@@ -14000,7 +14000,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A5" s="59" t="s">
         <v>192</v>
       </c>
@@ -14059,7 +14059,7 @@
       </c>
       <c r="U5" s="59"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A6" s="59" t="s">
         <v>193</v>
       </c>
@@ -14118,7 +14118,7 @@
       </c>
       <c r="U6" s="59"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
       <c r="A7" s="59" t="s">
         <v>194</v>
       </c>
@@ -14196,35 +14196,35 @@
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.86328125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.73046875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.3984375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.73046875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.86328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.1328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.86328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.86328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.1328125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.3984375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="24.86328125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A1" s="59" t="s">
         <v>161</v>
       </c>
@@ -14298,7 +14298,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A2" s="59" t="s">
         <v>212</v>
       </c>
@@ -14368,7 +14368,7 @@
         <v>1.9623842592592592E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A3" s="59" t="s">
         <v>213</v>
       </c>
@@ -14438,7 +14438,7 @@
         <v>1.8121527777777778E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A4" s="59" t="s">
         <v>214</v>
       </c>
@@ -14508,7 +14508,7 @@
         <v>1.9979166666666665E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A5" s="59" t="s">
         <v>215</v>
       </c>
@@ -14578,7 +14578,7 @@
         <v>1.7653935185185186E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A6" s="59" t="s">
         <v>189</v>
       </c>
@@ -14648,7 +14648,7 @@
         <v>1.8998842592592594E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A7" s="59" t="s">
         <v>190</v>
       </c>
@@ -14733,39 +14733,39 @@
   </sheetPr>
   <dimension ref="A1:X15"/>
   <sheetViews>
-    <sheetView zoomScale="83" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.86328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.86328125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.59765625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.59765625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.59765625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="27" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="22" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.59765625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.265625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.59765625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="27" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A1" s="59" t="s">
         <v>161</v>
       </c>
@@ -14839,7 +14839,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A2" s="59" t="s">
         <v>223</v>
       </c>
@@ -14909,7 +14909,7 @@
         <v>1.8332175925925925E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A3" s="59" t="s">
         <v>224</v>
       </c>
@@ -14979,7 +14979,7 @@
         <v>1.7003472222222222E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A4" s="59" t="s">
         <v>273</v>
       </c>
@@ -14993,13 +14993,13 @@
         <v>50</v>
       </c>
       <c r="E4" s="61">
-        <v>45658</v>
+        <v>46023</v>
       </c>
       <c r="F4" s="61">
+        <v>46371</v>
+      </c>
+      <c r="G4" s="61">
         <v>46023</v>
-      </c>
-      <c r="G4" s="61">
-        <v>45658</v>
       </c>
       <c r="H4" s="59" t="s">
         <v>178</v>
@@ -15055,7 +15055,7 @@
         <v>3.9324537037037035E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A5" s="59" t="s">
         <v>273</v>
       </c>
@@ -15069,13 +15069,13 @@
         <v>22</v>
       </c>
       <c r="E5" s="61">
-        <v>45658</v>
+        <v>46023</v>
       </c>
       <c r="F5" s="61">
+        <v>46371</v>
+      </c>
+      <c r="G5" s="61">
         <v>46023</v>
-      </c>
-      <c r="G5" s="61">
-        <v>45658</v>
       </c>
       <c r="H5" s="59" t="s">
         <v>178</v>
@@ -15131,7 +15131,7 @@
         <v>4.0693981481481478E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A6" s="59" t="s">
         <v>273</v>
       </c>
@@ -15145,13 +15145,13 @@
         <v>19</v>
       </c>
       <c r="E6" s="61">
-        <v>45658</v>
+        <v>46023</v>
       </c>
       <c r="F6" s="61">
+        <v>46371</v>
+      </c>
+      <c r="G6" s="61">
         <v>46023</v>
-      </c>
-      <c r="G6" s="61">
-        <v>45658</v>
       </c>
       <c r="H6" s="59" t="s">
         <v>178</v>
@@ -15207,7 +15207,7 @@
         <v>4.1888888888888884E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A7" s="59" t="s">
         <v>274</v>
       </c>
@@ -15221,13 +15221,13 @@
         <v>50</v>
       </c>
       <c r="E7" s="61">
-        <v>45658</v>
+        <v>46023</v>
       </c>
       <c r="F7" s="61">
+        <v>46371</v>
+      </c>
+      <c r="G7" s="61">
         <v>46023</v>
-      </c>
-      <c r="G7" s="61">
-        <v>45658</v>
       </c>
       <c r="H7" s="59" t="s">
         <v>178</v>
@@ -15283,7 +15283,7 @@
         <v>4.7436458333333331E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A8" s="59" t="s">
         <v>274</v>
       </c>
@@ -15297,13 +15297,13 @@
         <v>22</v>
       </c>
       <c r="E8" s="61">
-        <v>45658</v>
+        <v>46023</v>
       </c>
       <c r="F8" s="61">
+        <v>46371</v>
+      </c>
+      <c r="G8" s="61">
         <v>46023</v>
-      </c>
-      <c r="G8" s="61">
-        <v>45658</v>
       </c>
       <c r="H8" s="59" t="s">
         <v>178</v>
@@ -15359,7 +15359,7 @@
         <v>4.9196875E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A9" s="59" t="s">
         <v>274</v>
       </c>
@@ -15373,13 +15373,13 @@
         <v>19</v>
       </c>
       <c r="E9" s="61">
-        <v>45658</v>
+        <v>46023</v>
       </c>
       <c r="F9" s="61">
+        <v>46371</v>
+      </c>
+      <c r="G9" s="61">
         <v>46023</v>
-      </c>
-      <c r="G9" s="61">
-        <v>45658</v>
       </c>
       <c r="H9" s="59" t="s">
         <v>178</v>
@@ -15435,7 +15435,7 @@
         <v>5.1593750000000001E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A10" s="59" t="s">
         <v>269</v>
       </c>
@@ -15449,13 +15449,13 @@
         <v>18</v>
       </c>
       <c r="E10" s="61">
-        <v>45658</v>
+        <v>46023</v>
       </c>
       <c r="F10" s="61">
+        <v>46371</v>
+      </c>
+      <c r="G10" s="61">
         <v>46023</v>
-      </c>
-      <c r="G10" s="61">
-        <v>45658</v>
       </c>
       <c r="H10" s="59" t="s">
         <v>178</v>
@@ -15511,7 +15511,7 @@
         <v>4.4791666666666667E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A11" s="59" t="s">
         <v>269</v>
       </c>
@@ -15525,13 +15525,13 @@
         <v>17</v>
       </c>
       <c r="E11" s="61">
-        <v>45658</v>
+        <v>46023</v>
       </c>
       <c r="F11" s="61">
+        <v>46371</v>
+      </c>
+      <c r="G11" s="61">
         <v>46023</v>
-      </c>
-      <c r="G11" s="61">
-        <v>45658</v>
       </c>
       <c r="H11" s="59" t="s">
         <v>178</v>
@@ -15587,7 +15587,7 @@
         <v>4.619444444444444E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A12" s="59" t="s">
         <v>269</v>
       </c>
@@ -15601,13 +15601,13 @@
         <v>16</v>
       </c>
       <c r="E12" s="61">
-        <v>45658</v>
+        <v>46023</v>
       </c>
       <c r="F12" s="61">
+        <v>46371</v>
+      </c>
+      <c r="G12" s="61">
         <v>46023</v>
-      </c>
-      <c r="G12" s="61">
-        <v>45658</v>
       </c>
       <c r="H12" s="59" t="s">
         <v>178</v>
@@ -15663,7 +15663,7 @@
         <v>4.7138888888888881E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A13" s="59" t="s">
         <v>275</v>
       </c>
@@ -15677,13 +15677,13 @@
         <v>18</v>
       </c>
       <c r="E13" s="61">
-        <v>45658</v>
+        <v>46023</v>
       </c>
       <c r="F13" s="61">
+        <v>46371</v>
+      </c>
+      <c r="G13" s="61">
         <v>46023</v>
-      </c>
-      <c r="G13" s="61">
-        <v>45658</v>
       </c>
       <c r="H13" s="59" t="s">
         <v>178</v>
@@ -15739,7 +15739,7 @@
         <v>5.3782870370370367E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A14" s="59" t="s">
         <v>275</v>
       </c>
@@ -15753,13 +15753,13 @@
         <v>17</v>
       </c>
       <c r="E14" s="61">
-        <v>45658</v>
+        <v>46023</v>
       </c>
       <c r="F14" s="61">
+        <v>46371</v>
+      </c>
+      <c r="G14" s="61">
         <v>46023</v>
-      </c>
-      <c r="G14" s="61">
-        <v>45658</v>
       </c>
       <c r="H14" s="59" t="s">
         <v>178</v>
@@ -15815,7 +15815,7 @@
         <v>5.5107638888888882E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A15" s="59" t="s">
         <v>275</v>
       </c>
@@ -15829,13 +15829,13 @@
         <v>16</v>
       </c>
       <c r="E15" s="61">
-        <v>45658</v>
+        <v>46023</v>
       </c>
       <c r="F15" s="61">
+        <v>46371</v>
+      </c>
+      <c r="G15" s="61">
         <v>46023</v>
-      </c>
-      <c r="G15" s="61">
-        <v>45658</v>
       </c>
       <c r="H15" s="59" t="s">
         <v>178</v>
@@ -15906,22 +15906,22 @@
   </sheetPr>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.1328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="84.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="84.86328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.73046875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>225</v>
       </c>
@@ -15947,7 +15947,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" s="70">
         <v>46075</v>
       </c>
@@ -15970,7 +15970,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" s="70">
         <v>46075</v>
       </c>
@@ -15993,7 +15993,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" s="70">
         <v>46124</v>
       </c>
@@ -16016,7 +16016,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" s="70">
         <v>46124</v>
       </c>
@@ -16039,7 +16039,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" s="70">
         <v>46186</v>
       </c>
@@ -16062,7 +16062,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" s="70">
         <v>46187</v>
       </c>
@@ -16085,7 +16085,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" s="70">
         <v>46199</v>
       </c>
@@ -16111,7 +16111,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" s="70">
         <v>46202</v>
       </c>
@@ -16134,7 +16134,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" s="70">
         <v>46228</v>
       </c>
@@ -16179,145 +16179,145 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="5.28515625" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="26" width="9.5703125" customWidth="1"/>
-    <col min="28" max="28" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="52" width="4.5703125" customWidth="1"/>
-    <col min="54" max="54" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="55" max="78" width="9.5703125" customWidth="1"/>
+    <col min="1" max="1" width="5.265625" customWidth="1"/>
+    <col min="2" max="2" width="32.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="26" width="9.59765625" customWidth="1"/>
+    <col min="28" max="28" width="32.3984375" bestFit="1" customWidth="1"/>
+    <col min="29" max="52" width="4.59765625" customWidth="1"/>
+    <col min="54" max="54" width="32.3984375" bestFit="1" customWidth="1"/>
+    <col min="55" max="78" width="9.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="140">
+    <row r="1" spans="1:78" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="159">
         <v>2025</v>
       </c>
       <c r="B1" s="79" t="str">
         <f ca="1">CONCATENATE("in: ",YEAR(TODAY())-1," für: ", YEAR(TODAY()))</f>
         <v>in: 2025 für: 2026</v>
       </c>
-      <c r="C1" s="141" t="s">
+      <c r="C1" s="140" t="s">
         <v>256</v>
       </c>
-      <c r="D1" s="141"/>
-      <c r="E1" s="142"/>
-      <c r="F1" s="143" t="s">
+      <c r="D1" s="140"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="144" t="s">
         <v>257</v>
       </c>
-      <c r="G1" s="144"/>
-      <c r="H1" s="144"/>
-      <c r="I1" s="144"/>
-      <c r="J1" s="145"/>
-      <c r="K1" s="146" t="s">
+      <c r="G1" s="145"/>
+      <c r="H1" s="145"/>
+      <c r="I1" s="145"/>
+      <c r="J1" s="146"/>
+      <c r="K1" s="150" t="s">
         <v>261</v>
       </c>
-      <c r="L1" s="147"/>
-      <c r="M1" s="147"/>
-      <c r="N1" s="148"/>
-      <c r="O1" s="166" t="s">
+      <c r="L1" s="151"/>
+      <c r="M1" s="151"/>
+      <c r="N1" s="152"/>
+      <c r="O1" s="142" t="s">
         <v>258</v>
       </c>
-      <c r="P1" s="166"/>
-      <c r="Q1" s="167"/>
-      <c r="R1" s="168" t="s">
+      <c r="P1" s="142"/>
+      <c r="Q1" s="143"/>
+      <c r="R1" s="156" t="s">
         <v>259</v>
       </c>
-      <c r="S1" s="169"/>
-      <c r="T1" s="169"/>
-      <c r="U1" s="169"/>
-      <c r="V1" s="170"/>
-      <c r="W1" s="171" t="s">
+      <c r="S1" s="157"/>
+      <c r="T1" s="157"/>
+      <c r="U1" s="157"/>
+      <c r="V1" s="158"/>
+      <c r="W1" s="153" t="s">
         <v>262</v>
       </c>
-      <c r="X1" s="172"/>
-      <c r="Y1" s="172"/>
-      <c r="Z1" s="173"/>
+      <c r="X1" s="154"/>
+      <c r="Y1" s="154"/>
+      <c r="Z1" s="155"/>
       <c r="AA1"/>
       <c r="AB1" s="79" t="str">
         <f ca="1">CONCATENATE("in: ",YEAR(TODAY())-1," für: ", YEAR(TODAY()))</f>
         <v>in: 2025 für: 2026</v>
       </c>
-      <c r="AC1" s="149" t="s">
+      <c r="AC1" s="160" t="s">
         <v>263</v>
       </c>
-      <c r="AD1" s="149"/>
-      <c r="AE1" s="150"/>
-      <c r="AF1" s="151" t="s">
+      <c r="AD1" s="160"/>
+      <c r="AE1" s="161"/>
+      <c r="AF1" s="162" t="s">
         <v>264</v>
       </c>
-      <c r="AG1" s="152"/>
-      <c r="AH1" s="152"/>
-      <c r="AI1" s="152"/>
-      <c r="AJ1" s="153"/>
-      <c r="AK1" s="154" t="s">
+      <c r="AG1" s="163"/>
+      <c r="AH1" s="163"/>
+      <c r="AI1" s="163"/>
+      <c r="AJ1" s="164"/>
+      <c r="AK1" s="165" t="s">
         <v>265</v>
       </c>
-      <c r="AL1" s="155"/>
-      <c r="AM1" s="155"/>
-      <c r="AN1" s="156"/>
-      <c r="AO1" s="157" t="s">
+      <c r="AL1" s="166"/>
+      <c r="AM1" s="166"/>
+      <c r="AN1" s="167"/>
+      <c r="AO1" s="168" t="s">
         <v>266</v>
       </c>
-      <c r="AP1" s="158"/>
-      <c r="AQ1" s="159"/>
-      <c r="AR1" s="160" t="s">
+      <c r="AP1" s="169"/>
+      <c r="AQ1" s="170"/>
+      <c r="AR1" s="171" t="s">
         <v>267</v>
       </c>
-      <c r="AS1" s="161"/>
-      <c r="AT1" s="161"/>
-      <c r="AU1" s="161"/>
-      <c r="AV1" s="162"/>
-      <c r="AW1" s="163" t="s">
+      <c r="AS1" s="172"/>
+      <c r="AT1" s="172"/>
+      <c r="AU1" s="172"/>
+      <c r="AV1" s="173"/>
+      <c r="AW1" s="147" t="s">
         <v>268</v>
       </c>
-      <c r="AX1" s="164"/>
-      <c r="AY1" s="164"/>
-      <c r="AZ1" s="165"/>
+      <c r="AX1" s="148"/>
+      <c r="AY1" s="148"/>
+      <c r="AZ1" s="149"/>
       <c r="BB1" s="79" t="str">
         <f ca="1">CONCATENATE("in: ",YEAR(TODAY())-1," für: ", YEAR(TODAY()))</f>
         <v>in: 2025 für: 2026</v>
       </c>
-      <c r="BC1" s="141" t="s">
+      <c r="BC1" s="140" t="s">
         <v>269</v>
       </c>
-      <c r="BD1" s="141"/>
-      <c r="BE1" s="142"/>
-      <c r="BF1" s="143" t="s">
+      <c r="BD1" s="140"/>
+      <c r="BE1" s="141"/>
+      <c r="BF1" s="144" t="s">
         <v>270</v>
       </c>
-      <c r="BG1" s="144"/>
-      <c r="BH1" s="144"/>
-      <c r="BI1" s="144"/>
-      <c r="BJ1" s="145"/>
-      <c r="BK1" s="146" t="s">
+      <c r="BG1" s="145"/>
+      <c r="BH1" s="145"/>
+      <c r="BI1" s="145"/>
+      <c r="BJ1" s="146"/>
+      <c r="BK1" s="150" t="s">
         <v>271</v>
       </c>
-      <c r="BL1" s="147"/>
-      <c r="BM1" s="147"/>
-      <c r="BN1" s="148"/>
-      <c r="BO1" s="166" t="s">
+      <c r="BL1" s="151"/>
+      <c r="BM1" s="151"/>
+      <c r="BN1" s="152"/>
+      <c r="BO1" s="142" t="s">
         <v>258</v>
       </c>
-      <c r="BP1" s="166"/>
-      <c r="BQ1" s="167"/>
-      <c r="BR1" s="168" t="s">
+      <c r="BP1" s="142"/>
+      <c r="BQ1" s="143"/>
+      <c r="BR1" s="156" t="s">
         <v>259</v>
       </c>
-      <c r="BS1" s="169"/>
-      <c r="BT1" s="169"/>
-      <c r="BU1" s="169"/>
-      <c r="BV1" s="170"/>
-      <c r="BW1" s="171" t="s">
+      <c r="BS1" s="157"/>
+      <c r="BT1" s="157"/>
+      <c r="BU1" s="157"/>
+      <c r="BV1" s="158"/>
+      <c r="BW1" s="153" t="s">
         <v>272</v>
       </c>
-      <c r="BX1" s="172"/>
-      <c r="BY1" s="172"/>
-      <c r="BZ1" s="173"/>
-    </row>
-    <row r="2" spans="1:78" s="128" customFormat="1" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="140"/>
+      <c r="BX1" s="154"/>
+      <c r="BY1" s="154"/>
+      <c r="BZ1" s="155"/>
+    </row>
+    <row r="2" spans="1:78" s="128" customFormat="1" ht="21.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="159"/>
       <c r="B2" s="80" t="s">
         <v>260</v>
       </c>
@@ -16617,8 +16617,8 @@
         <v>2001-1985</v>
       </c>
     </row>
-    <row r="3" spans="1:78" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="140"/>
+    <row r="3" spans="1:78" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="159"/>
       <c r="B3" s="81" t="s">
         <v>0</v>
       </c>
@@ -16870,8 +16870,8 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="A4" s="140"/>
+    <row r="4" spans="1:78" x14ac:dyDescent="0.45">
+      <c r="A4" s="159"/>
       <c r="B4" s="81" t="s">
         <v>219</v>
       </c>
@@ -17122,8 +17122,8 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="A5" s="140"/>
+    <row r="5" spans="1:78" x14ac:dyDescent="0.45">
+      <c r="A5" s="159"/>
       <c r="B5" s="81" t="s">
         <v>220</v>
       </c>
@@ -17374,8 +17374,8 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="A6" s="140"/>
+    <row r="6" spans="1:78" x14ac:dyDescent="0.45">
+      <c r="A6" s="159"/>
       <c r="B6" s="81" t="s">
         <v>221</v>
       </c>
@@ -17626,8 +17626,8 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="A7" s="140"/>
+    <row r="7" spans="1:78" x14ac:dyDescent="0.45">
+      <c r="A7" s="159"/>
       <c r="B7" s="81" t="s">
         <v>222</v>
       </c>
@@ -17878,8 +17878,8 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:78" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="140"/>
+    <row r="8" spans="1:78" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="159"/>
       <c r="B8" s="84" t="s">
         <v>4</v>
       </c>
@@ -18130,134 +18130,134 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:78" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:78" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="140">
+    <row r="9" spans="1:78" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
+    <row r="10" spans="1:78" ht="18" x14ac:dyDescent="0.45">
+      <c r="A10" s="159">
         <v>2026</v>
       </c>
       <c r="B10" s="79" t="str">
         <f ca="1">CONCATENATE("in: ",YEAR(TODAY())," für: ", YEAR(TODAY())+1)</f>
         <v>in: 2026 für: 2027</v>
       </c>
-      <c r="C10" s="141" t="s">
+      <c r="C10" s="140" t="s">
         <v>256</v>
       </c>
-      <c r="D10" s="141"/>
-      <c r="E10" s="142"/>
-      <c r="F10" s="143" t="s">
+      <c r="D10" s="140"/>
+      <c r="E10" s="141"/>
+      <c r="F10" s="144" t="s">
         <v>257</v>
       </c>
-      <c r="G10" s="144"/>
-      <c r="H10" s="144"/>
-      <c r="I10" s="144"/>
-      <c r="J10" s="145"/>
-      <c r="K10" s="146" t="s">
+      <c r="G10" s="145"/>
+      <c r="H10" s="145"/>
+      <c r="I10" s="145"/>
+      <c r="J10" s="146"/>
+      <c r="K10" s="150" t="s">
         <v>261</v>
       </c>
-      <c r="L10" s="147"/>
-      <c r="M10" s="147"/>
-      <c r="N10" s="148"/>
-      <c r="O10" s="166" t="s">
+      <c r="L10" s="151"/>
+      <c r="M10" s="151"/>
+      <c r="N10" s="152"/>
+      <c r="O10" s="142" t="s">
         <v>258</v>
       </c>
-      <c r="P10" s="166"/>
-      <c r="Q10" s="167"/>
-      <c r="R10" s="168" t="s">
+      <c r="P10" s="142"/>
+      <c r="Q10" s="143"/>
+      <c r="R10" s="156" t="s">
         <v>259</v>
       </c>
-      <c r="S10" s="169"/>
-      <c r="T10" s="169"/>
-      <c r="U10" s="169"/>
-      <c r="V10" s="170"/>
-      <c r="W10" s="171" t="s">
+      <c r="S10" s="157"/>
+      <c r="T10" s="157"/>
+      <c r="U10" s="157"/>
+      <c r="V10" s="158"/>
+      <c r="W10" s="153" t="s">
         <v>262</v>
       </c>
-      <c r="X10" s="172"/>
-      <c r="Y10" s="172"/>
-      <c r="Z10" s="173"/>
+      <c r="X10" s="154"/>
+      <c r="Y10" s="154"/>
+      <c r="Z10" s="155"/>
       <c r="AB10" s="79" t="str">
         <f ca="1">CONCATENATE("in: ",YEAR(TODAY())," für: ", YEAR(TODAY())+1)</f>
         <v>in: 2026 für: 2027</v>
       </c>
-      <c r="AC10" s="149" t="s">
+      <c r="AC10" s="160" t="s">
         <v>263</v>
       </c>
-      <c r="AD10" s="149"/>
-      <c r="AE10" s="150"/>
-      <c r="AF10" s="151" t="s">
+      <c r="AD10" s="160"/>
+      <c r="AE10" s="161"/>
+      <c r="AF10" s="162" t="s">
         <v>264</v>
       </c>
-      <c r="AG10" s="152"/>
-      <c r="AH10" s="152"/>
-      <c r="AI10" s="152"/>
-      <c r="AJ10" s="153"/>
-      <c r="AK10" s="154" t="s">
+      <c r="AG10" s="163"/>
+      <c r="AH10" s="163"/>
+      <c r="AI10" s="163"/>
+      <c r="AJ10" s="164"/>
+      <c r="AK10" s="165" t="s">
         <v>265</v>
       </c>
-      <c r="AL10" s="155"/>
-      <c r="AM10" s="155"/>
-      <c r="AN10" s="156"/>
-      <c r="AO10" s="157" t="s">
+      <c r="AL10" s="166"/>
+      <c r="AM10" s="166"/>
+      <c r="AN10" s="167"/>
+      <c r="AO10" s="168" t="s">
         <v>266</v>
       </c>
-      <c r="AP10" s="158"/>
-      <c r="AQ10" s="159"/>
-      <c r="AR10" s="160" t="s">
+      <c r="AP10" s="169"/>
+      <c r="AQ10" s="170"/>
+      <c r="AR10" s="171" t="s">
         <v>267</v>
       </c>
-      <c r="AS10" s="161"/>
-      <c r="AT10" s="161"/>
-      <c r="AU10" s="161"/>
-      <c r="AV10" s="162"/>
-      <c r="AW10" s="163" t="s">
+      <c r="AS10" s="172"/>
+      <c r="AT10" s="172"/>
+      <c r="AU10" s="172"/>
+      <c r="AV10" s="173"/>
+      <c r="AW10" s="147" t="s">
         <v>268</v>
       </c>
-      <c r="AX10" s="164"/>
-      <c r="AY10" s="164"/>
-      <c r="AZ10" s="165"/>
+      <c r="AX10" s="148"/>
+      <c r="AY10" s="148"/>
+      <c r="AZ10" s="149"/>
       <c r="BB10" s="79" t="str">
         <f ca="1">CONCATENATE("in: ",YEAR(TODAY())," für: ", YEAR(TODAY())+1)</f>
         <v>in: 2026 für: 2027</v>
       </c>
-      <c r="BC10" s="141" t="s">
+      <c r="BC10" s="140" t="s">
         <v>269</v>
       </c>
-      <c r="BD10" s="141"/>
-      <c r="BE10" s="142"/>
-      <c r="BF10" s="143" t="s">
+      <c r="BD10" s="140"/>
+      <c r="BE10" s="141"/>
+      <c r="BF10" s="144" t="s">
         <v>270</v>
       </c>
-      <c r="BG10" s="144"/>
-      <c r="BH10" s="144"/>
-      <c r="BI10" s="144"/>
-      <c r="BJ10" s="145"/>
-      <c r="BK10" s="146" t="s">
+      <c r="BG10" s="145"/>
+      <c r="BH10" s="145"/>
+      <c r="BI10" s="145"/>
+      <c r="BJ10" s="146"/>
+      <c r="BK10" s="150" t="s">
         <v>271</v>
       </c>
-      <c r="BL10" s="147"/>
-      <c r="BM10" s="147"/>
-      <c r="BN10" s="148"/>
-      <c r="BO10" s="166" t="s">
+      <c r="BL10" s="151"/>
+      <c r="BM10" s="151"/>
+      <c r="BN10" s="152"/>
+      <c r="BO10" s="142" t="s">
         <v>258</v>
       </c>
-      <c r="BP10" s="166"/>
-      <c r="BQ10" s="167"/>
-      <c r="BR10" s="168" t="s">
+      <c r="BP10" s="142"/>
+      <c r="BQ10" s="143"/>
+      <c r="BR10" s="156" t="s">
         <v>259</v>
       </c>
-      <c r="BS10" s="169"/>
-      <c r="BT10" s="169"/>
-      <c r="BU10" s="169"/>
-      <c r="BV10" s="170"/>
-      <c r="BW10" s="171" t="s">
+      <c r="BS10" s="157"/>
+      <c r="BT10" s="157"/>
+      <c r="BU10" s="157"/>
+      <c r="BV10" s="158"/>
+      <c r="BW10" s="153" t="s">
         <v>272</v>
       </c>
-      <c r="BX10" s="172"/>
-      <c r="BY10" s="172"/>
-      <c r="BZ10" s="173"/>
-    </row>
-    <row r="11" spans="1:78" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="140"/>
+      <c r="BX10" s="154"/>
+      <c r="BY10" s="154"/>
+      <c r="BZ10" s="155"/>
+    </row>
+    <row r="11" spans="1:78" ht="21.4" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="159"/>
       <c r="B11" s="80" t="s">
         <v>260</v>
       </c>
@@ -18557,8 +18557,8 @@
         <v>2001-1985</v>
       </c>
     </row>
-    <row r="12" spans="1:78" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="140"/>
+    <row r="12" spans="1:78" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="159"/>
       <c r="B12" s="81" t="s">
         <v>0</v>
       </c>
@@ -18809,8 +18809,8 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="A13" s="140"/>
+    <row r="13" spans="1:78" x14ac:dyDescent="0.45">
+      <c r="A13" s="159"/>
       <c r="B13" s="81" t="s">
         <v>219</v>
       </c>
@@ -19061,8 +19061,8 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="A14" s="140"/>
+    <row r="14" spans="1:78" x14ac:dyDescent="0.45">
+      <c r="A14" s="159"/>
       <c r="B14" s="81" t="s">
         <v>220</v>
       </c>
@@ -19313,8 +19313,8 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:78" x14ac:dyDescent="0.25">
-      <c r="A15" s="140"/>
+    <row r="15" spans="1:78" x14ac:dyDescent="0.45">
+      <c r="A15" s="159"/>
       <c r="B15" s="81" t="s">
         <v>221</v>
       </c>
@@ -19565,8 +19565,8 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="140"/>
+    <row r="16" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="159"/>
       <c r="B16" s="81" t="s">
         <v>222</v>
       </c>
@@ -19817,8 +19817,8 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:78" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="140"/>
+    <row r="17" spans="1:78" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A17" s="159"/>
       <c r="B17" s="84" t="s">
         <v>4</v>
       </c>
@@ -20069,7 +20069,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:78" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:78" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
       <c r="C18" s="64"/>
       <c r="O18" s="64"/>
       <c r="T18" s="67"/>
@@ -20078,7 +20078,7 @@
       <c r="X18" s="64"/>
       <c r="AD18" s="64"/>
     </row>
-    <row r="21" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:78" x14ac:dyDescent="0.45">
       <c r="C21" s="63"/>
       <c r="D21" s="66"/>
       <c r="E21" s="66"/>
@@ -20098,7 +20098,7 @@
       <c r="AF21" s="69"/>
       <c r="AG21" s="69"/>
     </row>
-    <row r="22" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:78" x14ac:dyDescent="0.45">
       <c r="C22" s="64"/>
       <c r="D22" s="65"/>
       <c r="E22" s="65"/>
@@ -20118,7 +20118,7 @@
       <c r="AF22" s="65"/>
       <c r="AG22" s="65"/>
     </row>
-    <row r="23" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:78" x14ac:dyDescent="0.45">
       <c r="C23" s="64"/>
       <c r="D23" s="65"/>
       <c r="E23" s="65"/>
@@ -20138,7 +20138,7 @@
       <c r="AF23" s="65"/>
       <c r="AG23" s="65"/>
     </row>
-    <row r="24" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:78" x14ac:dyDescent="0.45">
       <c r="C24" s="64"/>
       <c r="D24" s="65"/>
       <c r="E24" s="65"/>
@@ -20158,7 +20158,7 @@
       <c r="AF24" s="65"/>
       <c r="AG24" s="65"/>
     </row>
-    <row r="25" spans="1:78" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:78" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C25" s="64"/>
       <c r="D25" s="65"/>
       <c r="E25" s="65"/>
@@ -20178,7 +20178,7 @@
       <c r="AF25" s="65"/>
       <c r="AG25" s="65"/>
     </row>
-    <row r="26" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:78" x14ac:dyDescent="0.45">
       <c r="C26" s="64"/>
       <c r="D26" s="65"/>
       <c r="E26" s="65"/>
@@ -20198,7 +20198,7 @@
       <c r="AF26" s="65"/>
       <c r="AG26" s="65"/>
     </row>
-    <row r="27" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:78" x14ac:dyDescent="0.45">
       <c r="C27" s="64"/>
       <c r="D27" s="65"/>
       <c r="E27" s="65"/>
@@ -20218,7 +20218,7 @@
       <c r="AF27" s="65"/>
       <c r="AG27" s="65"/>
     </row>
-    <row r="30" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:78" x14ac:dyDescent="0.45">
       <c r="C30" s="63"/>
       <c r="D30" s="66"/>
       <c r="E30" s="66"/>
@@ -20227,7 +20227,7 @@
       <c r="H30" s="66"/>
       <c r="P30" s="67"/>
     </row>
-    <row r="31" spans="1:78" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:78" x14ac:dyDescent="0.45">
       <c r="C31" s="64"/>
       <c r="D31" s="65"/>
       <c r="E31" s="65"/>
@@ -20235,7 +20235,7 @@
       <c r="G31" s="65"/>
       <c r="H31" s="65"/>
     </row>
-    <row r="40" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C40" s="64"/>
       <c r="D40" s="65"/>
       <c r="E40" s="65"/>
@@ -20243,7 +20243,7 @@
       <c r="G40" s="65"/>
       <c r="H40" s="65"/>
     </row>
-    <row r="41" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C41" s="64"/>
       <c r="D41" s="65"/>
       <c r="E41" s="65"/>
@@ -20251,7 +20251,7 @@
       <c r="G41" s="65"/>
       <c r="H41" s="65"/>
     </row>
-    <row r="42" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C42" s="64"/>
       <c r="D42" s="65"/>
       <c r="E42" s="65"/>
@@ -20259,7 +20259,7 @@
       <c r="G42" s="65"/>
       <c r="H42" s="65"/>
     </row>
-    <row r="43" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C43" s="64"/>
       <c r="D43" s="65"/>
       <c r="E43" s="65"/>
@@ -20267,7 +20267,7 @@
       <c r="G43" s="65"/>
       <c r="H43" s="65"/>
     </row>
-    <row r="44" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C44" s="64"/>
       <c r="D44" s="65"/>
       <c r="E44" s="65"/>
@@ -20275,7 +20275,7 @@
       <c r="G44" s="65"/>
       <c r="H44" s="65"/>
     </row>
-    <row r="45" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:8" x14ac:dyDescent="0.45">
       <c r="C45" s="64"/>
       <c r="D45" s="65"/>
       <c r="E45" s="65"/>
@@ -20285,28 +20285,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="O10:Q10"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="F10:J10"/>
-    <mergeCell ref="AW10:AZ10"/>
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="W10:Z10"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="R1:V1"/>
-    <mergeCell ref="W1:Z1"/>
-    <mergeCell ref="R10:V10"/>
-    <mergeCell ref="BO10:BQ10"/>
-    <mergeCell ref="BR10:BV10"/>
-    <mergeCell ref="BW10:BZ10"/>
-    <mergeCell ref="BC1:BE1"/>
-    <mergeCell ref="BF1:BJ1"/>
-    <mergeCell ref="BK1:BN1"/>
-    <mergeCell ref="BO1:BQ1"/>
-    <mergeCell ref="BR1:BV1"/>
-    <mergeCell ref="BW1:BZ1"/>
     <mergeCell ref="A1:A8"/>
     <mergeCell ref="A10:A17"/>
     <mergeCell ref="BC10:BE10"/>
@@ -20323,6 +20301,28 @@
     <mergeCell ref="AK10:AN10"/>
     <mergeCell ref="AO10:AQ10"/>
     <mergeCell ref="AR10:AV10"/>
+    <mergeCell ref="BO10:BQ10"/>
+    <mergeCell ref="BR10:BV10"/>
+    <mergeCell ref="BW10:BZ10"/>
+    <mergeCell ref="BC1:BE1"/>
+    <mergeCell ref="BF1:BJ1"/>
+    <mergeCell ref="BK1:BN1"/>
+    <mergeCell ref="BO1:BQ1"/>
+    <mergeCell ref="BR1:BV1"/>
+    <mergeCell ref="BW1:BZ1"/>
+    <mergeCell ref="AW10:AZ10"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="W10:Z10"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="R1:V1"/>
+    <mergeCell ref="W1:Z1"/>
+    <mergeCell ref="R10:V10"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="O10:Q10"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="F10:J10"/>
   </mergeCells>
   <conditionalFormatting sqref="AC3:AZ8">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">

</xml_diff>

<commit_message>
TITEL anpassung karussel slide
</commit_message>
<xml_diff>
--- a/web/utilities/records_kriterien.xlsx
+++ b/web/utilities/records_kriterien.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpgna\Documents\GitHub\Lifesaving_Baden\web\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B72D59-C2DF-4314-A95D-D0D5A704357A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78C7425A-B835-4F86-AA07-8832CD397A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" tabRatio="687" firstSheet="1" activeTab="5" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="687" firstSheet="1" activeTab="7" xr2:uid="{E1AB626B-3773-4829-92A5-28DD4DB7C8F8}"/>
   </bookViews>
   <sheets>
     <sheet name="DR" sheetId="9" r:id="rId1"/>
@@ -221,7 +221,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="277">
   <si>
     <t>50m Retten</t>
   </si>
@@ -961,9 +961,6 @@
     <t>Trainingslehrgang LK3</t>
   </si>
   <si>
-    <t>Tageslehrgang für LK3 und deren Heimtrainer zu den neuen Disziplinen. (Noch nicht fix)</t>
-  </si>
-  <si>
     <t>Hallenbad Oberhausen-Rheinhausen</t>
   </si>
   <si>
@@ -982,9 +979,6 @@
     <t>LK1 / LK2 / LK3</t>
   </si>
   <si>
-    <t>Warm Up, 50m Bahn, Cool Down, Theorie Lifesaver, Treffpunkt 12:10 im Foyer</t>
-  </si>
-  <si>
     <t>20.7.Jahr - 1</t>
   </si>
   <si>
@@ -1055,6 +1049,9 @@
   </si>
   <si>
     <t>TEST (LK2 - Weiblich)</t>
+  </si>
+  <si>
+    <t>Tageslehrgang für LK3 und deren Heimtrainer zu den neuen Disziplinen.</t>
   </si>
 </sst>
 </file>
@@ -1891,13 +1888,16 @@
     <xf numFmtId="0" fontId="17" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1909,6 +1909,15 @@
     <xf numFmtId="0" fontId="17" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1917,6 +1926,27 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1958,39 +1988,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2313,6 +2310,75 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -4361,75 +4427,6 @@
       </fill>
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -4444,102 +4441,102 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2C5E83EE-6B6F-478A-9C90-A846A1A76536}" name="WR_Open4" displayName="WR_Open4" ref="A4:AW31" totalsRowShown="0" headerRowDxfId="178" headerRowBorderDxfId="177" tableBorderDxfId="176">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2C5E83EE-6B6F-478A-9C90-A846A1A76536}" name="WR_Open4" displayName="WR_Open4" ref="A4:AW31" totalsRowShown="0" headerRowDxfId="201" headerRowBorderDxfId="200" tableBorderDxfId="199">
   <autoFilter ref="A4:AW31" xr:uid="{2C5E83EE-6B6F-478A-9C90-A846A1A76536}"/>
   <tableColumns count="49">
-    <tableColumn id="1" xr3:uid="{7C0C4105-A61A-4B8D-9129-EDC4F18765AF}" name="WR-Open" dataDxfId="175">
+    <tableColumn id="1" xr3:uid="{7C0C4105-A61A-4B8D-9129-EDC4F18765AF}" name="WR-Open" dataDxfId="198">
       <calculatedColumnFormula>A4+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{516F5612-F85F-413F-9012-E235F415E34B}" name="50m Retten - offen - W" dataDxfId="174"/>
-    <tableColumn id="3" xr3:uid="{BC9ACAC9-0D45-42FD-B596-D19FBE3A4D83}" name="100m Retten - offen - W" dataDxfId="173"/>
-    <tableColumn id="4" xr3:uid="{CB6DBE59-EB65-43F0-93E7-0BDC3F82832B}" name="100m Kombi - offen - W" dataDxfId="172"/>
-    <tableColumn id="5" xr3:uid="{AA603C60-6831-4C14-A8CD-0AA050DA7551}" name="100m Lifesaver - offen - W" dataDxfId="171"/>
-    <tableColumn id="6" xr3:uid="{7920F147-7717-4582-940A-2610F7D310CA}" name="200m Superlifesaver - offen - W" dataDxfId="170"/>
-    <tableColumn id="7" xr3:uid="{04E21F1D-AC8D-4A1B-9B43-59B8F7901673}" name="200m Hindernis - offen - W" dataDxfId="169"/>
-    <tableColumn id="8" xr3:uid="{40E8A083-653A-48A8-9B37-0A2D850B7829}" name="50m Retten - offen - M" dataDxfId="168"/>
-    <tableColumn id="9" xr3:uid="{863824A9-134F-4189-BB14-225AE224FC44}" name="100m Retten - offen - M" dataDxfId="167"/>
+    <tableColumn id="2" xr3:uid="{516F5612-F85F-413F-9012-E235F415E34B}" name="50m Retten - offen - W" dataDxfId="197"/>
+    <tableColumn id="3" xr3:uid="{BC9ACAC9-0D45-42FD-B596-D19FBE3A4D83}" name="100m Retten - offen - W" dataDxfId="196"/>
+    <tableColumn id="4" xr3:uid="{CB6DBE59-EB65-43F0-93E7-0BDC3F82832B}" name="100m Kombi - offen - W" dataDxfId="195"/>
+    <tableColumn id="5" xr3:uid="{AA603C60-6831-4C14-A8CD-0AA050DA7551}" name="100m Lifesaver - offen - W" dataDxfId="194"/>
+    <tableColumn id="6" xr3:uid="{7920F147-7717-4582-940A-2610F7D310CA}" name="200m Superlifesaver - offen - W" dataDxfId="193"/>
+    <tableColumn id="7" xr3:uid="{04E21F1D-AC8D-4A1B-9B43-59B8F7901673}" name="200m Hindernis - offen - W" dataDxfId="192"/>
+    <tableColumn id="8" xr3:uid="{40E8A083-653A-48A8-9B37-0A2D850B7829}" name="50m Retten - offen - M" dataDxfId="191"/>
+    <tableColumn id="9" xr3:uid="{863824A9-134F-4189-BB14-225AE224FC44}" name="100m Retten - offen - M" dataDxfId="190"/>
     <tableColumn id="10" xr3:uid="{598FC6AE-DEA2-4475-9A35-CDCB8C81496A}" name="100m Kombi - offen - M"/>
     <tableColumn id="11" xr3:uid="{9FC50B37-0D51-422E-A268-A6506D4F3854}" name="100m Lifesaver - offen - M"/>
     <tableColumn id="12" xr3:uid="{B8D2552B-5D82-442A-98F0-E47D5C5F6728}" name="200m Superlifesaver - offen - M"/>
-    <tableColumn id="13" xr3:uid="{5A5E9873-0C5F-4508-AF6B-4974E0526D84}" name="200m Hindernis - offen - M" dataDxfId="166"/>
-    <tableColumn id="14" xr3:uid="{FA907992-7FCE-4CAD-8CF2-F5BEBC9B3756}" name="50m Retten - 17/18 - W" dataDxfId="165"/>
-    <tableColumn id="15" xr3:uid="{76B63DC0-CB67-48F4-9B5A-D22902F59334}" name="100m Retten - 17/18 - W" dataDxfId="164"/>
-    <tableColumn id="16" xr3:uid="{614A2419-51B1-44C0-8469-ADBFB078B81A}" name="100m Kombi -17/18 - W" dataDxfId="163"/>
-    <tableColumn id="17" xr3:uid="{2EC953EE-367D-4524-A25E-8DE3B8168E34}" name="100m Lifesaver - 17/18 - W" dataDxfId="162"/>
-    <tableColumn id="18" xr3:uid="{25711867-9BD7-4197-9094-A21392411249}" name="200m Superlifesaver - 17/18 - W" dataDxfId="161"/>
-    <tableColumn id="19" xr3:uid="{262DB142-CFB1-45C3-9332-7273CACD1B62}" name="200m Hindernis - 17/18 - W" dataDxfId="160"/>
-    <tableColumn id="20" xr3:uid="{938BA45A-8244-4637-8A14-DF49CD91A945}" name="50m Retten - 17/18 - M" dataDxfId="159"/>
-    <tableColumn id="21" xr3:uid="{737E28D8-900F-4A98-95FE-EE7B0AFDEE90}" name="100m Retten - 17/18 - M" dataDxfId="158"/>
-    <tableColumn id="22" xr3:uid="{330BD3A8-061C-45E2-ADDB-40C2F346772F}" name="100m Kombi - 17/18 - M" dataDxfId="157"/>
-    <tableColumn id="23" xr3:uid="{0CADDE90-A167-4E1D-8D33-8624E5E1A4E2}" name="100m Lifesaver - 17/18 - M" dataDxfId="156"/>
-    <tableColumn id="24" xr3:uid="{FCF9F42C-1291-4985-9D37-B9DE2DAA5DCB}" name="200m Superlifesaver - 17/18 - M" dataDxfId="155"/>
-    <tableColumn id="25" xr3:uid="{4E5397B2-F924-4F48-AE69-AF6D650AF88D}" name="200m Hindernis - 17/18 - M" dataDxfId="154"/>
-    <tableColumn id="26" xr3:uid="{0A78315A-BFDC-43EE-A66F-48B301F66508}" name="50m Retten - 15/16 - W" dataDxfId="153"/>
-    <tableColumn id="27" xr3:uid="{D3FCF8BD-6C76-450D-80C0-CC0519A79731}" name="100m Retten - 15/16 - W" dataDxfId="152"/>
-    <tableColumn id="28" xr3:uid="{6BE7937E-D62D-47CD-95DE-1730304B0DF3}" name="100m Kombi - 15/16 - W" dataDxfId="151"/>
-    <tableColumn id="29" xr3:uid="{098BA5BE-5AF6-4187-89B6-534498F24C51}" name="100m Lifesaver -  15/16 - W" dataDxfId="150"/>
-    <tableColumn id="30" xr3:uid="{2A6822CF-143C-4BF7-A440-5777527BE512}" name="200m Superlifesaver -  15/16 - W" dataDxfId="149"/>
-    <tableColumn id="31" xr3:uid="{541C7145-CDEA-4E4E-9E7A-A4F05BA6C3E5}" name="200m Hindernis -  15/16 - W" dataDxfId="148"/>
-    <tableColumn id="32" xr3:uid="{342C4488-8C61-42E6-87A9-C75BD8EB7452}" name="50m Retten - 15/16 - M" dataDxfId="147"/>
-    <tableColumn id="33" xr3:uid="{857B1D46-7D20-47F7-AB9B-732D50346E32}" name="100m Retten - 15/16 - M" dataDxfId="146"/>
-    <tableColumn id="34" xr3:uid="{4C8A2EB4-804B-45F1-A768-9A6958957F8B}" name="100m Kombi -15/16 - M" dataDxfId="145"/>
-    <tableColumn id="35" xr3:uid="{26C75B4F-21EC-4EB0-A9A9-54BC80140672}" name="100m Lifesaver - 15/16 - M" dataDxfId="144"/>
-    <tableColumn id="36" xr3:uid="{DBBB2A23-1A06-429A-A5D1-A547EF5EC16F}" name="200m Superlifesaver - 15/16 - M" dataDxfId="143"/>
-    <tableColumn id="37" xr3:uid="{84061231-CAE5-427A-87F5-6DDBA99F77D2}" name="200m Hindernis - 15/16 - M" dataDxfId="142"/>
-    <tableColumn id="38" xr3:uid="{878CCA80-A742-4B3C-90C9-E93BB814201B}" name="50m Retten - 13/14 - W" dataDxfId="141"/>
-    <tableColumn id="39" xr3:uid="{A1F57102-61CF-4784-8DE2-0B8F32D5D699}" name="50m Retten mit Flossen - 13/14 - W" dataDxfId="140"/>
-    <tableColumn id="40" xr3:uid="{0F6BAF78-3D79-42A9-9FED-E6D0E335A920}" name="100m Hindernis - 13/14 - W" dataDxfId="139"/>
-    <tableColumn id="41" xr3:uid="{EB748A68-E10D-4D76-B315-8FDB3AC33C8D}" name="50m Retten - 13/14 - M" dataDxfId="138"/>
-    <tableColumn id="42" xr3:uid="{C7B04167-6430-40F0-9A0F-D0D0BE2F9C77}" name="50m Retten mit Flossen - 13/14 - M" dataDxfId="137"/>
-    <tableColumn id="43" xr3:uid="{48704BB7-A853-445A-8CDC-8D8F86C2B66A}" name="100m Hindernis - 13/14 - M" dataDxfId="136"/>
-    <tableColumn id="44" xr3:uid="{9605FE9A-F41C-4A5F-A59C-B7A9D45C460F}" name="50m Flossen - 12 - W" dataDxfId="135"/>
-    <tableColumn id="45" xr3:uid="{4C9DBF61-35B1-4BC2-8272-526E0AFAAFFB}" name="50m komb. Schwimmen - 12 - W" dataDxfId="134"/>
-    <tableColumn id="46" xr3:uid="{CF433C95-C272-48F9-98CD-7E3C8DBB6F2C}" name="50m Hindernis - 12 - W" dataDxfId="133"/>
-    <tableColumn id="47" xr3:uid="{FADB7411-DB43-4B14-B9E8-D74CA1BA18B8}" name="50m Flossen - 12 - M" dataDxfId="132"/>
-    <tableColumn id="48" xr3:uid="{02936F84-1D82-48AC-8D7C-6D2954D68A06}" name="50m komb. Schwimmen - 12 - M" dataDxfId="131"/>
-    <tableColumn id="49" xr3:uid="{7FD9BD11-0597-4E07-8DA5-DB53384197F5}" name="50m Hindernis - 12 - M" dataDxfId="130"/>
+    <tableColumn id="13" xr3:uid="{5A5E9873-0C5F-4508-AF6B-4974E0526D84}" name="200m Hindernis - offen - M" dataDxfId="189"/>
+    <tableColumn id="14" xr3:uid="{FA907992-7FCE-4CAD-8CF2-F5BEBC9B3756}" name="50m Retten - 17/18 - W" dataDxfId="188"/>
+    <tableColumn id="15" xr3:uid="{76B63DC0-CB67-48F4-9B5A-D22902F59334}" name="100m Retten - 17/18 - W" dataDxfId="187"/>
+    <tableColumn id="16" xr3:uid="{614A2419-51B1-44C0-8469-ADBFB078B81A}" name="100m Kombi -17/18 - W" dataDxfId="186"/>
+    <tableColumn id="17" xr3:uid="{2EC953EE-367D-4524-A25E-8DE3B8168E34}" name="100m Lifesaver - 17/18 - W" dataDxfId="185"/>
+    <tableColumn id="18" xr3:uid="{25711867-9BD7-4197-9094-A21392411249}" name="200m Superlifesaver - 17/18 - W" dataDxfId="184"/>
+    <tableColumn id="19" xr3:uid="{262DB142-CFB1-45C3-9332-7273CACD1B62}" name="200m Hindernis - 17/18 - W" dataDxfId="183"/>
+    <tableColumn id="20" xr3:uid="{938BA45A-8244-4637-8A14-DF49CD91A945}" name="50m Retten - 17/18 - M" dataDxfId="182"/>
+    <tableColumn id="21" xr3:uid="{737E28D8-900F-4A98-95FE-EE7B0AFDEE90}" name="100m Retten - 17/18 - M" dataDxfId="181"/>
+    <tableColumn id="22" xr3:uid="{330BD3A8-061C-45E2-ADDB-40C2F346772F}" name="100m Kombi - 17/18 - M" dataDxfId="180"/>
+    <tableColumn id="23" xr3:uid="{0CADDE90-A167-4E1D-8D33-8624E5E1A4E2}" name="100m Lifesaver - 17/18 - M" dataDxfId="179"/>
+    <tableColumn id="24" xr3:uid="{FCF9F42C-1291-4985-9D37-B9DE2DAA5DCB}" name="200m Superlifesaver - 17/18 - M" dataDxfId="178"/>
+    <tableColumn id="25" xr3:uid="{4E5397B2-F924-4F48-AE69-AF6D650AF88D}" name="200m Hindernis - 17/18 - M" dataDxfId="177"/>
+    <tableColumn id="26" xr3:uid="{0A78315A-BFDC-43EE-A66F-48B301F66508}" name="50m Retten - 15/16 - W" dataDxfId="176"/>
+    <tableColumn id="27" xr3:uid="{D3FCF8BD-6C76-450D-80C0-CC0519A79731}" name="100m Retten - 15/16 - W" dataDxfId="175"/>
+    <tableColumn id="28" xr3:uid="{6BE7937E-D62D-47CD-95DE-1730304B0DF3}" name="100m Kombi - 15/16 - W" dataDxfId="174"/>
+    <tableColumn id="29" xr3:uid="{098BA5BE-5AF6-4187-89B6-534498F24C51}" name="100m Lifesaver -  15/16 - W" dataDxfId="173"/>
+    <tableColumn id="30" xr3:uid="{2A6822CF-143C-4BF7-A440-5777527BE512}" name="200m Superlifesaver -  15/16 - W" dataDxfId="172"/>
+    <tableColumn id="31" xr3:uid="{541C7145-CDEA-4E4E-9E7A-A4F05BA6C3E5}" name="200m Hindernis -  15/16 - W" dataDxfId="171"/>
+    <tableColumn id="32" xr3:uid="{342C4488-8C61-42E6-87A9-C75BD8EB7452}" name="50m Retten - 15/16 - M" dataDxfId="170"/>
+    <tableColumn id="33" xr3:uid="{857B1D46-7D20-47F7-AB9B-732D50346E32}" name="100m Retten - 15/16 - M" dataDxfId="169"/>
+    <tableColumn id="34" xr3:uid="{4C8A2EB4-804B-45F1-A768-9A6958957F8B}" name="100m Kombi -15/16 - M" dataDxfId="168"/>
+    <tableColumn id="35" xr3:uid="{26C75B4F-21EC-4EB0-A9A9-54BC80140672}" name="100m Lifesaver - 15/16 - M" dataDxfId="167"/>
+    <tableColumn id="36" xr3:uid="{DBBB2A23-1A06-429A-A5D1-A547EF5EC16F}" name="200m Superlifesaver - 15/16 - M" dataDxfId="166"/>
+    <tableColumn id="37" xr3:uid="{84061231-CAE5-427A-87F5-6DDBA99F77D2}" name="200m Hindernis - 15/16 - M" dataDxfId="165"/>
+    <tableColumn id="38" xr3:uid="{878CCA80-A742-4B3C-90C9-E93BB814201B}" name="50m Retten - 13/14 - W" dataDxfId="164"/>
+    <tableColumn id="39" xr3:uid="{A1F57102-61CF-4784-8DE2-0B8F32D5D699}" name="50m Retten mit Flossen - 13/14 - W" dataDxfId="163"/>
+    <tableColumn id="40" xr3:uid="{0F6BAF78-3D79-42A9-9FED-E6D0E335A920}" name="100m Hindernis - 13/14 - W" dataDxfId="162"/>
+    <tableColumn id="41" xr3:uid="{EB748A68-E10D-4D76-B315-8FDB3AC33C8D}" name="50m Retten - 13/14 - M" dataDxfId="161"/>
+    <tableColumn id="42" xr3:uid="{C7B04167-6430-40F0-9A0F-D0D0BE2F9C77}" name="50m Retten mit Flossen - 13/14 - M" dataDxfId="160"/>
+    <tableColumn id="43" xr3:uid="{48704BB7-A853-445A-8CDC-8D8F86C2B66A}" name="100m Hindernis - 13/14 - M" dataDxfId="159"/>
+    <tableColumn id="44" xr3:uid="{9605FE9A-F41C-4A5F-A59C-B7A9D45C460F}" name="50m Flossen - 12 - W" dataDxfId="158"/>
+    <tableColumn id="45" xr3:uid="{4C9DBF61-35B1-4BC2-8272-526E0AFAAFFB}" name="50m komb. Schwimmen - 12 - W" dataDxfId="157"/>
+    <tableColumn id="46" xr3:uid="{CF433C95-C272-48F9-98CD-7E3C8DBB6F2C}" name="50m Hindernis - 12 - W" dataDxfId="156"/>
+    <tableColumn id="47" xr3:uid="{FADB7411-DB43-4B14-B9E8-D74CA1BA18B8}" name="50m Flossen - 12 - M" dataDxfId="155"/>
+    <tableColumn id="48" xr3:uid="{02936F84-1D82-48AC-8D7C-6D2954D68A06}" name="50m komb. Schwimmen - 12 - M" dataDxfId="154"/>
+    <tableColumn id="49" xr3:uid="{7FD9BD11-0597-4E07-8DA5-DB53384197F5}" name="50m Hindernis - 12 - M" dataDxfId="153"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4234D44E-A2BE-4790-B589-1A8CC19B714E}" name="WR_Youth" displayName="WR_Youth" ref="A4:M32" totalsRowShown="0" headerRowDxfId="129" dataDxfId="127" headerRowBorderDxfId="128" tableBorderDxfId="126">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{4234D44E-A2BE-4790-B589-1A8CC19B714E}" name="WR_Youth" displayName="WR_Youth" ref="A4:M32" totalsRowShown="0" headerRowDxfId="152" dataDxfId="150" headerRowBorderDxfId="151" tableBorderDxfId="149">
   <autoFilter ref="A4:M32" xr:uid="{4234D44E-A2BE-4790-B589-1A8CC19B714E}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{848E691A-41B0-42DD-B122-FB6DF43CB3EF}" name="WR-Youth" dataDxfId="125"/>
-    <tableColumn id="2" xr3:uid="{2FE43F18-485B-46A9-8946-FBC5FDAE5A8E}" name="50m Retten" dataDxfId="124"/>
-    <tableColumn id="3" xr3:uid="{CA5C3ABF-02E6-442B-868B-95B293B231D3}" name="100m Retten" dataDxfId="123"/>
-    <tableColumn id="4" xr3:uid="{7A6BBA52-2145-464D-8C04-B2CCFC1A90DC}" name="100m Kombi" dataDxfId="122"/>
-    <tableColumn id="5" xr3:uid="{21F420C9-E788-49EE-88F6-E37963ED31CF}" name="100m Lifesaver" dataDxfId="121"/>
-    <tableColumn id="6" xr3:uid="{CB87B7CD-8A9C-4775-A4D7-4D267F43FD1A}" name="200m Superlifesaver" dataDxfId="120"/>
-    <tableColumn id="7" xr3:uid="{2DC7F290-B564-4851-85AE-D211DA701B32}" name="200m Hindernis" dataDxfId="119"/>
-    <tableColumn id="8" xr3:uid="{8112783D-8796-4D6A-8414-AC675D745697}" name="50m Retten2" dataDxfId="118"/>
-    <tableColumn id="9" xr3:uid="{4E818CD4-8725-495D-9D1D-1AFCED9181F5}" name="100m Retten2" dataDxfId="117"/>
-    <tableColumn id="10" xr3:uid="{28C05A91-E302-40A9-B50A-ECF997F129FC}" name="100m Kombi2" dataDxfId="116"/>
-    <tableColumn id="11" xr3:uid="{D56FB9F2-45BF-4EC9-A84C-8A5FB59F2F05}" name="100m Lifesaver2" dataDxfId="115"/>
-    <tableColumn id="12" xr3:uid="{540169C0-2A40-4794-A872-F7DF8A887BF2}" name="200m Superlifesaver2" dataDxfId="114"/>
-    <tableColumn id="13" xr3:uid="{D104CB67-B55A-4C81-87E5-0AC758DD22A4}" name="200m Hindernis2" dataDxfId="113"/>
+    <tableColumn id="1" xr3:uid="{848E691A-41B0-42DD-B122-FB6DF43CB3EF}" name="WR-Youth" dataDxfId="148"/>
+    <tableColumn id="2" xr3:uid="{2FE43F18-485B-46A9-8946-FBC5FDAE5A8E}" name="50m Retten" dataDxfId="147"/>
+    <tableColumn id="3" xr3:uid="{CA5C3ABF-02E6-442B-868B-95B293B231D3}" name="100m Retten" dataDxfId="146"/>
+    <tableColumn id="4" xr3:uid="{7A6BBA52-2145-464D-8C04-B2CCFC1A90DC}" name="100m Kombi" dataDxfId="145"/>
+    <tableColumn id="5" xr3:uid="{21F420C9-E788-49EE-88F6-E37963ED31CF}" name="100m Lifesaver" dataDxfId="144"/>
+    <tableColumn id="6" xr3:uid="{CB87B7CD-8A9C-4775-A4D7-4D267F43FD1A}" name="200m Superlifesaver" dataDxfId="143"/>
+    <tableColumn id="7" xr3:uid="{2DC7F290-B564-4851-85AE-D211DA701B32}" name="200m Hindernis" dataDxfId="142"/>
+    <tableColumn id="8" xr3:uid="{8112783D-8796-4D6A-8414-AC675D745697}" name="50m Retten2" dataDxfId="141"/>
+    <tableColumn id="9" xr3:uid="{4E818CD4-8725-495D-9D1D-1AFCED9181F5}" name="100m Retten2" dataDxfId="140"/>
+    <tableColumn id="10" xr3:uid="{28C05A91-E302-40A9-B50A-ECF997F129FC}" name="100m Kombi2" dataDxfId="139"/>
+    <tableColumn id="11" xr3:uid="{D56FB9F2-45BF-4EC9-A84C-8A5FB59F2F05}" name="100m Lifesaver2" dataDxfId="138"/>
+    <tableColumn id="12" xr3:uid="{540169C0-2A40-4794-A872-F7DF8A887BF2}" name="200m Superlifesaver2" dataDxfId="137"/>
+    <tableColumn id="13" xr3:uid="{D104CB67-B55A-4C81-87E5-0AC758DD22A4}" name="200m Hindernis2" dataDxfId="136"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E2D2F97B-7645-4066-8AB3-F35CF6E035EB}" name="WR_Open" displayName="WR_Open" ref="A4:M32" totalsRowShown="0" headerRowDxfId="112" headerRowBorderDxfId="111" tableBorderDxfId="110">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E2D2F97B-7645-4066-8AB3-F35CF6E035EB}" name="WR_Open" displayName="WR_Open" ref="A4:M32" totalsRowShown="0" headerRowDxfId="135" headerRowBorderDxfId="134" tableBorderDxfId="133">
   <autoFilter ref="A4:M32" xr:uid="{E2D2F97B-7645-4066-8AB3-F35CF6E035EB}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{AE73402B-B27E-4B29-8DCF-30B7FC1855EF}" name="WR-Open" dataDxfId="109">
+    <tableColumn id="1" xr3:uid="{AE73402B-B27E-4B29-8DCF-30B7FC1855EF}" name="WR-Open" dataDxfId="132">
       <calculatedColumnFormula>A4+1</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{EA3EAC1F-184E-4A28-B3E3-08DE12F138EF}" name="50m Retten" dataDxfId="108"/>
-    <tableColumn id="3" xr3:uid="{E0305A3F-6087-4F8C-8B64-153E1ACAA32E}" name="100m Retten" dataDxfId="107"/>
-    <tableColumn id="4" xr3:uid="{F0B7AC37-315E-49AA-855C-7955D2B43A76}" name="100m Kombi" dataDxfId="106"/>
-    <tableColumn id="5" xr3:uid="{B5E690AB-DB7D-4864-8916-89D2A68C4128}" name="100m Lifesaver" dataDxfId="105"/>
-    <tableColumn id="6" xr3:uid="{D89BAF4D-36AE-4C73-9320-9C5736F02F8A}" name="200m Superlifesaver" dataDxfId="104"/>
-    <tableColumn id="7" xr3:uid="{58AE7517-1A90-459F-A7D2-B95265D217E7}" name="200m Hindernis" dataDxfId="103"/>
-    <tableColumn id="8" xr3:uid="{13A189FB-E897-4A1F-A001-525F61E9CFFF}" name="50m Retten2" dataDxfId="102"/>
-    <tableColumn id="9" xr3:uid="{36418AC5-46B8-400F-BD2E-D329CF4F92CD}" name="100m Retten2" dataDxfId="101"/>
+    <tableColumn id="2" xr3:uid="{EA3EAC1F-184E-4A28-B3E3-08DE12F138EF}" name="50m Retten" dataDxfId="131"/>
+    <tableColumn id="3" xr3:uid="{E0305A3F-6087-4F8C-8B64-153E1ACAA32E}" name="100m Retten" dataDxfId="130"/>
+    <tableColumn id="4" xr3:uid="{F0B7AC37-315E-49AA-855C-7955D2B43A76}" name="100m Kombi" dataDxfId="129"/>
+    <tableColumn id="5" xr3:uid="{B5E690AB-DB7D-4864-8916-89D2A68C4128}" name="100m Lifesaver" dataDxfId="128"/>
+    <tableColumn id="6" xr3:uid="{D89BAF4D-36AE-4C73-9320-9C5736F02F8A}" name="200m Superlifesaver" dataDxfId="127"/>
+    <tableColumn id="7" xr3:uid="{58AE7517-1A90-459F-A7D2-B95265D217E7}" name="200m Hindernis" dataDxfId="126"/>
+    <tableColumn id="8" xr3:uid="{13A189FB-E897-4A1F-A001-525F61E9CFFF}" name="50m Retten2" dataDxfId="125"/>
+    <tableColumn id="9" xr3:uid="{36418AC5-46B8-400F-BD2E-D329CF4F92CD}" name="100m Retten2" dataDxfId="124"/>
     <tableColumn id="10" xr3:uid="{06A35C2D-7313-472B-BC1F-4F2FB1D14782}" name="100m Kombi2"/>
     <tableColumn id="11" xr3:uid="{89966D0D-9131-4245-A7BE-1A7384D5ADA0}" name="100m Lifesaver2"/>
     <tableColumn id="12" xr3:uid="{D9D6CF56-869C-4DDE-9886-572D4E523A8F}" name="200m Superlifesaver2"/>
@@ -4550,7 +4547,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CF3D303A-A04B-42DD-A44E-CEB6CECB77A4}" name="DP_konfig" displayName="DP_konfig" ref="A1:U3" totalsRowShown="0" headerRowDxfId="100" dataDxfId="99">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{CF3D303A-A04B-42DD-A44E-CEB6CECB77A4}" name="DP_konfig" displayName="DP_konfig" ref="A1:U3" totalsRowShown="0" headerRowDxfId="123" dataDxfId="122">
   <autoFilter ref="A1:U3" xr:uid="{CF3D303A-A04B-42DD-A44E-CEB6CECB77A4}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -4575,57 +4572,57 @@
     <filterColumn colId="20" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="21">
-    <tableColumn id="1" xr3:uid="{58D628F0-061E-4A82-8362-CDB37A2E7C60}" name="Tabellen Name" dataDxfId="98"/>
-    <tableColumn id="2" xr3:uid="{2F302F6C-F8AF-4FDE-AB08-6F30F9671015}" name="Geschlecht" dataDxfId="97"/>
-    <tableColumn id="3" xr3:uid="{4D91FBF9-386D-43DD-90D0-B49823FDB629}" name="Mindest alter" dataDxfId="96"/>
-    <tableColumn id="4" xr3:uid="{4126AAC6-AF2F-446C-B4EA-D86ACFD9FAC2}" name="Maximales Alter" dataDxfId="95"/>
-    <tableColumn id="5" xr3:uid="{8A10890A-A299-4B09-AC72-0E9AE9238AF3}" name="Qualizeitraum anfang" dataDxfId="94"/>
-    <tableColumn id="6" xr3:uid="{FBCD1C13-FC82-429B-8DE1-0C5A455FDAB8}" name="Qualizeitraum Ende" dataDxfId="93"/>
-    <tableColumn id="7" xr3:uid="{1DCCAC9B-BC46-468E-A3CE-57576C2FF11D}" name="Letzter Wettkampf am" dataDxfId="92"/>
-    <tableColumn id="8" xr3:uid="{9A6E47EE-ABD8-4A1E-87D3-9D286E4C124F}" name="Wertung" dataDxfId="91"/>
-    <tableColumn id="9" xr3:uid="{09E848D2-ED17-49C7-9775-CBF17D20DFC0}" name="Landesverband" dataDxfId="90"/>
-    <tableColumn id="10" xr3:uid="{70ABB713-23F6-4FCF-920E-3CB0CD451446}" name="OMS" dataDxfId="89"/>
-    <tableColumn id="11" xr3:uid="{9C108A1C-E6AB-4C13-9C1D-0FA8944A39A3}" name="Pool-Länge" dataDxfId="88"/>
-    <tableColumn id="12" xr3:uid="{087948DD-430D-48F1-906D-4F4EF4B46053}" name="Regelwerk" dataDxfId="87"/>
-    <tableColumn id="13" xr3:uid="{BF42D9C0-F77D-4971-A67E-32B0246C72C3}" name="Referenz" dataDxfId="86"/>
-    <tableColumn id="19" xr3:uid="{AFFB84E8-B398-4E99-805B-9A247071A040}" name="Referenz Jahr" dataDxfId="85"/>
-    <tableColumn id="20" xr3:uid="{0A59A474-DFBB-4437-8EFF-70284AFD9934}" name="Mindest Punktzahl" dataDxfId="84"/>
-    <tableColumn id="21" xr3:uid="{198BD231-EEF3-43C9-AD9B-39B4B7E9B337}" name="Mindest Disziplinen" dataDxfId="83"/>
-    <tableColumn id="14" xr3:uid="{443CD4F6-A2B2-480B-BB35-DCEEBC531727}" name="3-Kampf Regel" dataDxfId="82"/>
-    <tableColumn id="15" xr3:uid="{70116160-7666-42B1-92AC-FAC2620E6A60}" name="Anzahl Nominierte" dataDxfId="81"/>
-    <tableColumn id="16" xr3:uid="{0EFD0A46-D12B-4AB0-907C-08E5D9F282E0}" name="Anzahl Nachrücker" dataDxfId="80"/>
-    <tableColumn id="17" xr3:uid="{AA5430A0-8ED8-40E8-B7F8-DA25E4E8790F}" name="Seiten Anzahl" dataDxfId="79"/>
-    <tableColumn id="18" xr3:uid="{16F699D9-2741-43F3-AD5F-826A568EFEAC}" name="Absagen" dataDxfId="78"/>
+    <tableColumn id="1" xr3:uid="{58D628F0-061E-4A82-8362-CDB37A2E7C60}" name="Tabellen Name" dataDxfId="121"/>
+    <tableColumn id="2" xr3:uid="{2F302F6C-F8AF-4FDE-AB08-6F30F9671015}" name="Geschlecht" dataDxfId="120"/>
+    <tableColumn id="3" xr3:uid="{4D91FBF9-386D-43DD-90D0-B49823FDB629}" name="Mindest alter" dataDxfId="119"/>
+    <tableColumn id="4" xr3:uid="{4126AAC6-AF2F-446C-B4EA-D86ACFD9FAC2}" name="Maximales Alter" dataDxfId="118"/>
+    <tableColumn id="5" xr3:uid="{8A10890A-A299-4B09-AC72-0E9AE9238AF3}" name="Qualizeitraum anfang" dataDxfId="117"/>
+    <tableColumn id="6" xr3:uid="{FBCD1C13-FC82-429B-8DE1-0C5A455FDAB8}" name="Qualizeitraum Ende" dataDxfId="116"/>
+    <tableColumn id="7" xr3:uid="{1DCCAC9B-BC46-468E-A3CE-57576C2FF11D}" name="Letzter Wettkampf am" dataDxfId="115"/>
+    <tableColumn id="8" xr3:uid="{9A6E47EE-ABD8-4A1E-87D3-9D286E4C124F}" name="Wertung" dataDxfId="114"/>
+    <tableColumn id="9" xr3:uid="{09E848D2-ED17-49C7-9775-CBF17D20DFC0}" name="Landesverband" dataDxfId="113"/>
+    <tableColumn id="10" xr3:uid="{70ABB713-23F6-4FCF-920E-3CB0CD451446}" name="OMS" dataDxfId="112"/>
+    <tableColumn id="11" xr3:uid="{9C108A1C-E6AB-4C13-9C1D-0FA8944A39A3}" name="Pool-Länge" dataDxfId="111"/>
+    <tableColumn id="12" xr3:uid="{087948DD-430D-48F1-906D-4F4EF4B46053}" name="Regelwerk" dataDxfId="110"/>
+    <tableColumn id="13" xr3:uid="{BF42D9C0-F77D-4971-A67E-32B0246C72C3}" name="Referenz" dataDxfId="109"/>
+    <tableColumn id="19" xr3:uid="{AFFB84E8-B398-4E99-805B-9A247071A040}" name="Referenz Jahr" dataDxfId="108"/>
+    <tableColumn id="20" xr3:uid="{0A59A474-DFBB-4437-8EFF-70284AFD9934}" name="Mindest Punktzahl" dataDxfId="107"/>
+    <tableColumn id="21" xr3:uid="{198BD231-EEF3-43C9-AD9B-39B4B7E9B337}" name="Mindest Disziplinen" dataDxfId="106"/>
+    <tableColumn id="14" xr3:uid="{443CD4F6-A2B2-480B-BB35-DCEEBC531727}" name="3-Kampf Regel" dataDxfId="105"/>
+    <tableColumn id="15" xr3:uid="{70116160-7666-42B1-92AC-FAC2620E6A60}" name="Anzahl Nominierte" dataDxfId="104"/>
+    <tableColumn id="16" xr3:uid="{0EFD0A46-D12B-4AB0-907C-08E5D9F282E0}" name="Anzahl Nachrücker" dataDxfId="103"/>
+    <tableColumn id="17" xr3:uid="{AA5430A0-8ED8-40E8-B7F8-DA25E4E8790F}" name="Seiten Anzahl" dataDxfId="102"/>
+    <tableColumn id="18" xr3:uid="{16F699D9-2741-43F3-AD5F-826A568EFEAC}" name="Absagen" dataDxfId="101"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CDBF6724-48A1-41AB-94B5-CC35C54BB15C}" name="BP_konfig" displayName="BP_konfig" ref="A1:U7" totalsRowShown="0" headerRowDxfId="201" dataDxfId="200">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{CDBF6724-48A1-41AB-94B5-CC35C54BB15C}" name="BP_konfig" displayName="BP_konfig" ref="A1:U7" totalsRowShown="0" headerRowDxfId="100" dataDxfId="99">
   <autoFilter ref="A1:U7" xr:uid="{CDBF6724-48A1-41AB-94B5-CC35C54BB15C}"/>
   <tableColumns count="21">
-    <tableColumn id="1" xr3:uid="{E1FB3D0C-B874-4874-BACC-6872CF171957}" name="Tabellen Name" dataDxfId="199"/>
-    <tableColumn id="2" xr3:uid="{FFDD2777-2097-450C-B020-F133CF643855}" name="Geschlecht" dataDxfId="198"/>
-    <tableColumn id="3" xr3:uid="{8CF52BE2-8020-48BD-A36D-63F13A1878DE}" name="Mindest alter" dataDxfId="197"/>
-    <tableColumn id="4" xr3:uid="{FD3A030F-CD97-4B6F-8E8C-BC2E67D79F1D}" name="Maximales Alter" dataDxfId="196"/>
-    <tableColumn id="5" xr3:uid="{3E22B645-D77C-4509-B031-9914FCB91599}" name="Qualizeitraum anfang" dataDxfId="195"/>
-    <tableColumn id="6" xr3:uid="{AE299324-3C1C-4063-ADF9-54555A161734}" name="Qualizeitraum Ende" dataDxfId="194"/>
-    <tableColumn id="7" xr3:uid="{DCC178B3-11FC-4C53-BBC6-C2FDA2C89857}" name="Letzter Wettkampf am" dataDxfId="193"/>
-    <tableColumn id="8" xr3:uid="{2811DB01-60A5-4BE4-B6F9-A806398A602A}" name="Wertung" dataDxfId="192"/>
-    <tableColumn id="9" xr3:uid="{0C16DAFE-847D-4E9E-9604-3A7D9FE924D0}" name="Landesverband" dataDxfId="191"/>
-    <tableColumn id="10" xr3:uid="{7A8A4101-A553-4BD5-9116-9AA5876B9401}" name="OMS" dataDxfId="190"/>
-    <tableColumn id="11" xr3:uid="{9807C9BD-6499-45F6-ACE0-4D13D64EF675}" name="Pool-Länge" dataDxfId="189"/>
-    <tableColumn id="12" xr3:uid="{13D336DD-650F-4F2C-836F-361CA1528F6D}" name="Regelwerk" dataDxfId="188"/>
-    <tableColumn id="13" xr3:uid="{66660E2D-ADF2-4FB5-8A13-004F826EE908}" name="Referenz" dataDxfId="187"/>
-    <tableColumn id="19" xr3:uid="{D72EDF8B-ECC3-4FF7-ABE6-B60BCE4A5E26}" name="Referenz Jahr" dataDxfId="186"/>
-    <tableColumn id="20" xr3:uid="{7B18E667-70F7-4BC1-AB1B-21C019F2AA89}" name="Mindest Punktzahl" dataDxfId="185"/>
-    <tableColumn id="21" xr3:uid="{FC185946-681B-42A6-AB1A-FC1EABB668C5}" name="Mindest Disziplinen" dataDxfId="184"/>
-    <tableColumn id="14" xr3:uid="{6A2676FD-2EC7-4C41-A35E-A1597A38F932}" name="3-Kampf Regel" dataDxfId="183"/>
-    <tableColumn id="15" xr3:uid="{718E0917-4F83-4A2B-832F-EBB16D5E21BF}" name="Anzahl Nominierte" dataDxfId="182"/>
-    <tableColumn id="16" xr3:uid="{5C66A461-D647-4E00-A81C-FD7AD44D7CC2}" name="Anzahl Nachrücker" dataDxfId="181"/>
-    <tableColumn id="17" xr3:uid="{D434BDEC-293B-4B4E-A5E9-479438960A03}" name="Seiten Anzahl" dataDxfId="180"/>
-    <tableColumn id="18" xr3:uid="{80908229-9247-473F-81C0-9C9D4C12FF06}" name="Absagen" dataDxfId="179"/>
+    <tableColumn id="1" xr3:uid="{E1FB3D0C-B874-4874-BACC-6872CF171957}" name="Tabellen Name" dataDxfId="98"/>
+    <tableColumn id="2" xr3:uid="{FFDD2777-2097-450C-B020-F133CF643855}" name="Geschlecht" dataDxfId="97"/>
+    <tableColumn id="3" xr3:uid="{8CF52BE2-8020-48BD-A36D-63F13A1878DE}" name="Mindest alter" dataDxfId="96"/>
+    <tableColumn id="4" xr3:uid="{FD3A030F-CD97-4B6F-8E8C-BC2E67D79F1D}" name="Maximales Alter" dataDxfId="95"/>
+    <tableColumn id="5" xr3:uid="{3E22B645-D77C-4509-B031-9914FCB91599}" name="Qualizeitraum anfang" dataDxfId="94"/>
+    <tableColumn id="6" xr3:uid="{AE299324-3C1C-4063-ADF9-54555A161734}" name="Qualizeitraum Ende" dataDxfId="93"/>
+    <tableColumn id="7" xr3:uid="{DCC178B3-11FC-4C53-BBC6-C2FDA2C89857}" name="Letzter Wettkampf am" dataDxfId="92"/>
+    <tableColumn id="8" xr3:uid="{2811DB01-60A5-4BE4-B6F9-A806398A602A}" name="Wertung" dataDxfId="91"/>
+    <tableColumn id="9" xr3:uid="{0C16DAFE-847D-4E9E-9604-3A7D9FE924D0}" name="Landesverband" dataDxfId="90"/>
+    <tableColumn id="10" xr3:uid="{7A8A4101-A553-4BD5-9116-9AA5876B9401}" name="OMS" dataDxfId="89"/>
+    <tableColumn id="11" xr3:uid="{9807C9BD-6499-45F6-ACE0-4D13D64EF675}" name="Pool-Länge" dataDxfId="88"/>
+    <tableColumn id="12" xr3:uid="{13D336DD-650F-4F2C-836F-361CA1528F6D}" name="Regelwerk" dataDxfId="87"/>
+    <tableColumn id="13" xr3:uid="{66660E2D-ADF2-4FB5-8A13-004F826EE908}" name="Referenz" dataDxfId="86"/>
+    <tableColumn id="19" xr3:uid="{D72EDF8B-ECC3-4FF7-ABE6-B60BCE4A5E26}" name="Referenz Jahr" dataDxfId="85"/>
+    <tableColumn id="20" xr3:uid="{7B18E667-70F7-4BC1-AB1B-21C019F2AA89}" name="Mindest Punktzahl" dataDxfId="84"/>
+    <tableColumn id="21" xr3:uid="{FC185946-681B-42A6-AB1A-FC1EABB668C5}" name="Mindest Disziplinen" dataDxfId="83"/>
+    <tableColumn id="14" xr3:uid="{6A2676FD-2EC7-4C41-A35E-A1597A38F932}" name="3-Kampf Regel" dataDxfId="82"/>
+    <tableColumn id="15" xr3:uid="{718E0917-4F83-4A2B-832F-EBB16D5E21BF}" name="Anzahl Nominierte" dataDxfId="81"/>
+    <tableColumn id="16" xr3:uid="{5C66A461-D647-4E00-A81C-FD7AD44D7CC2}" name="Anzahl Nachrücker" dataDxfId="80"/>
+    <tableColumn id="17" xr3:uid="{D434BDEC-293B-4B4E-A5E9-479438960A03}" name="Seiten Anzahl" dataDxfId="79"/>
+    <tableColumn id="18" xr3:uid="{80908229-9247-473F-81C0-9C9D4C12FF06}" name="Absagen" dataDxfId="78"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4748,8 +4745,8 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{888CE7BE-8313-44C0-AE38-83992EABD44D}" name="LK_Kalender" displayName="LK_Kalender" ref="A1:H10" totalsRowShown="0">
-  <autoFilter ref="A1:H10" xr:uid="{888CE7BE-8313-44C0-AE38-83992EABD44D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{888CE7BE-8313-44C0-AE38-83992EABD44D}" name="LK_Kalender" displayName="LK_Kalender" ref="A1:H8" totalsRowShown="0">
+  <autoFilter ref="A1:H8" xr:uid="{888CE7BE-8313-44C0-AE38-83992EABD44D}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{B26B9E90-F378-41EF-B35E-CE240017E4BE}" name="datum von" dataDxfId="25"/>
     <tableColumn id="2" xr3:uid="{38211212-0A92-428C-895C-E4CA68F52818}" name="datum bis"/>
@@ -5088,9 +5085,9 @@
       <selection activeCell="Y25" sqref="Y25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="15.265625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>39</v>
       </c>
@@ -5159,7 +5156,7 @@
       <c r="AV1" s="44"/>
       <c r="AW1" s="44"/>
     </row>
-    <row r="2" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
         <v>40</v>
       </c>
@@ -5226,7 +5223,7 @@
       <c r="AV2" s="45"/>
       <c r="AW2" s="45"/>
     </row>
-    <row r="3" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:49" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">
         <v>101</v>
       </c>
@@ -5287,7 +5284,7 @@
       <c r="AV3" s="45"/>
       <c r="AW3" s="45"/>
     </row>
-    <row r="4" spans="1:49" s="53" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:49" s="53" customFormat="1" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="49" t="s">
         <v>10</v>
       </c>
@@ -5436,7 +5433,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="5" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2000</v>
       </c>
@@ -5489,7 +5486,7 @@
       <c r="AV5" s="10"/>
       <c r="AW5" s="10"/>
     </row>
-    <row r="6" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f t="shared" ref="A6:A31" si="0">A5+1</f>
         <v>2001</v>
@@ -5567,7 +5564,7 @@
       <c r="AV6" s="11"/>
       <c r="AW6" s="11"/>
     </row>
-    <row r="7" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>2002</v>
@@ -5645,7 +5642,7 @@
       <c r="AV7" s="10"/>
       <c r="AW7" s="10"/>
     </row>
-    <row r="8" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>2003</v>
@@ -5723,7 +5720,7 @@
       <c r="AV8" s="11"/>
       <c r="AW8" s="11"/>
     </row>
-    <row r="9" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>2004</v>
@@ -5801,7 +5798,7 @@
       <c r="AV9" s="10"/>
       <c r="AW9" s="10"/>
     </row>
-    <row r="10" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>2005</v>
@@ -5879,7 +5876,7 @@
       <c r="AV10" s="11"/>
       <c r="AW10" s="11"/>
     </row>
-    <row r="11" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>2006</v>
@@ -5957,7 +5954,7 @@
       <c r="AV11" s="10"/>
       <c r="AW11" s="10"/>
     </row>
-    <row r="12" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>2007</v>
@@ -6079,7 +6076,7 @@
         <v>3.5995370370370369E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>2008</v>
@@ -6201,7 +6198,7 @@
         <v>3.5995370370370369E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>2009</v>
@@ -6323,7 +6320,7 @@
         <v>3.5995370370370369E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>2010</v>
@@ -6445,7 +6442,7 @@
         <v>3.5995370370370369E-4</v>
       </c>
     </row>
-    <row r="16" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>2011</v>
@@ -6579,7 +6576,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="17" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>2012</v>
@@ -6713,7 +6710,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="18" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>2013</v>
@@ -6847,7 +6844,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="19" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>2014</v>
@@ -6981,7 +6978,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="20" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>2015</v>
@@ -7115,7 +7112,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="21" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>2016</v>
@@ -7249,7 +7246,7 @@
         <v>3.5324074074074077E-4</v>
       </c>
     </row>
-    <row r="22" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>2017</v>
@@ -7383,7 +7380,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>2018</v>
@@ -7517,7 +7514,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="24" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>2019</v>
@@ -7651,7 +7648,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="25" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>2020</v>
@@ -7801,7 +7798,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="26" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>2021</v>
@@ -7951,7 +7948,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="27" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>2022</v>
@@ -8101,7 +8098,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="28" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>2023</v>
@@ -8251,7 +8248,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="29" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>2024</v>
@@ -8401,7 +8398,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="30" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>2025</v>
@@ -8551,7 +8548,7 @@
         <v>3.4745370370370372E-4</v>
       </c>
     </row>
-    <row r="31" spans="1:49" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>2026</v>
@@ -8772,15 +8769,15 @@
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.86328125" style="1" customWidth="1"/>
-    <col min="2" max="13" width="18.73046875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
+    <col min="2" max="13" width="18.7109375" style="1" customWidth="1"/>
     <col min="14" max="14" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="11.3984375" style="1"/>
+    <col min="15" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18">
         <v>2024</v>
       </c>
@@ -8824,7 +8821,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
@@ -8880,7 +8877,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -8936,7 +8933,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>8</v>
       </c>
@@ -8992,7 +8989,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="175" t="s">
         <v>13</v>
       </c>
@@ -9010,7 +9007,7 @@
       <c r="M7" s="175"/>
       <c r="N7" s="175"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="175"/>
       <c r="B8" s="175"/>
       <c r="C8" s="175"/>
@@ -9026,7 +9023,7 @@
       <c r="M8" s="175"/>
       <c r="N8" s="175"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>6</v>
       </c>
@@ -9080,7 +9077,7 @@
       </c>
       <c r="N9" s="21"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>7</v>
       </c>
@@ -9134,7 +9131,7 @@
       </c>
       <c r="N10" s="21"/>
     </row>
-    <row r="11" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>8</v>
       </c>
@@ -9188,7 +9185,7 @@
       </c>
       <c r="N11" s="23"/>
     </row>
-    <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="174" t="s">
         <v>14</v>
       </c>
@@ -9209,7 +9206,7 @@
       <c r="M14"/>
       <c r="N14"/>
     </row>
-    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="174"/>
       <c r="B15" s="174"/>
       <c r="C15" s="174"/>
@@ -9224,7 +9221,7 @@
       <c r="M15"/>
       <c r="N15"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -9259,7 +9256,7 @@
       <c r="M16"/>
       <c r="N16"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>19</v>
       </c>
@@ -9294,7 +9291,7 @@
       <c r="M17"/>
       <c r="N17"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>19</v>
       </c>
@@ -9327,7 +9324,7 @@
       <c r="M18"/>
       <c r="N18"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>22</v>
       </c>
@@ -9360,7 +9357,7 @@
       <c r="M19"/>
       <c r="N19"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>24</v>
       </c>
@@ -9391,7 +9388,7 @@
       <c r="M20"/>
       <c r="N20"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>22</v>
       </c>
@@ -9418,7 +9415,7 @@
       <c r="M21"/>
       <c r="N21"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>19</v>
       </c>
@@ -9441,7 +9438,7 @@
       <c r="I22" s="33"/>
       <c r="L22" s="41"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>19</v>
       </c>
@@ -9464,50 +9461,50 @@
       <c r="I23" s="33"/>
       <c r="L23" s="40"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H24" s="33"/>
       <c r="I24" s="33"/>
       <c r="L24" s="41"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H25" s="33"/>
       <c r="I25" s="33"/>
       <c r="L25" s="40"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L26" s="41"/>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L27" s="40"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L28" s="41"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L29" s="40"/>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L30" s="41"/>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L31" s="40"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="L32" s="41"/>
     </row>
-    <row r="33" spans="12:12" x14ac:dyDescent="0.45">
+    <row r="33" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L33" s="40"/>
     </row>
-    <row r="34" spans="12:12" x14ac:dyDescent="0.45">
+    <row r="34" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L34" s="41"/>
     </row>
-    <row r="35" spans="12:12" x14ac:dyDescent="0.45">
+    <row r="35" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L35" s="33"/>
     </row>
-    <row r="36" spans="12:12" x14ac:dyDescent="0.45">
+    <row r="36" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L36" s="41"/>
     </row>
-    <row r="37" spans="12:12" x14ac:dyDescent="0.45">
+    <row r="37" spans="12:12" x14ac:dyDescent="0.25">
       <c r="L37" s="33"/>
     </row>
   </sheetData>
@@ -9533,15 +9530,15 @@
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.86328125" style="1" customWidth="1"/>
-    <col min="2" max="13" width="18.73046875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
+    <col min="2" max="13" width="18.7109375" style="1" customWidth="1"/>
     <col min="14" max="14" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="11.3984375" style="1"/>
+    <col min="15" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18">
         <v>2025</v>
       </c>
@@ -9585,7 +9582,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
@@ -9641,7 +9638,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -9697,7 +9694,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>8</v>
       </c>
@@ -9753,7 +9750,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="175" t="s">
         <v>13</v>
       </c>
@@ -9771,7 +9768,7 @@
       <c r="M7" s="175"/>
       <c r="N7" s="175"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="175"/>
       <c r="B8" s="175"/>
       <c r="C8" s="175"/>
@@ -9787,7 +9784,7 @@
       <c r="M8" s="175"/>
       <c r="N8" s="175"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>6</v>
       </c>
@@ -9841,7 +9838,7 @@
       </c>
       <c r="N9" s="21"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>7</v>
       </c>
@@ -9895,7 +9892,7 @@
       </c>
       <c r="N10" s="21"/>
     </row>
-    <row r="11" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>8</v>
       </c>
@@ -9949,7 +9946,7 @@
       </c>
       <c r="N11" s="23"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="174" t="s">
         <v>14</v>
       </c>
@@ -9968,7 +9965,7 @@
       </c>
       <c r="M14"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="174"/>
       <c r="B15" s="174"/>
       <c r="C15" s="174"/>
@@ -9981,7 +9978,7 @@
       <c r="L15" s="176"/>
       <c r="M15"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -10014,7 +10011,7 @@
       </c>
       <c r="M16"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>28</v>
       </c>
@@ -10047,7 +10044,7 @@
       </c>
       <c r="M17"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>28</v>
       </c>
@@ -10078,7 +10075,7 @@
       <c r="L18" s="38"/>
       <c r="M18"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>29</v>
       </c>
@@ -10109,7 +10106,7 @@
       <c r="L19" s="36"/>
       <c r="M19"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>30</v>
       </c>
@@ -10138,7 +10135,7 @@
       <c r="L20" s="38"/>
       <c r="M20"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>29</v>
       </c>
@@ -10169,7 +10166,7 @@
       <c r="L21" s="36"/>
       <c r="M21"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>28</v>
       </c>
@@ -10200,7 +10197,7 @@
       <c r="L22" s="39"/>
       <c r="M22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>28</v>
       </c>
@@ -10231,66 +10228,66 @@
       <c r="L23" s="37"/>
       <c r="M23"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H24" s="40"/>
       <c r="I24" s="40"/>
       <c r="J24" s="40"/>
       <c r="L24" s="39"/>
       <c r="M24"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H25" s="33"/>
       <c r="I25" s="33"/>
       <c r="L25" s="37"/>
       <c r="M25"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L26" s="39"/>
       <c r="M26"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L27" s="37"/>
       <c r="M27"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L28" s="39"/>
       <c r="M28"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L29" s="37"/>
       <c r="M29"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L30" s="39"/>
       <c r="M30"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L31" s="37"/>
       <c r="M31"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L32" s="39"/>
       <c r="M32"/>
     </row>
-    <row r="33" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="33" spans="8:13" x14ac:dyDescent="0.25">
       <c r="L33" s="37"/>
       <c r="M33"/>
     </row>
-    <row r="34" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="34" spans="8:13" x14ac:dyDescent="0.25">
       <c r="L34" s="39"/>
       <c r="M34"/>
     </row>
-    <row r="35" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="35" spans="8:13" x14ac:dyDescent="0.25">
       <c r="M35"/>
     </row>
-    <row r="36" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="36" spans="8:13" x14ac:dyDescent="0.25">
       <c r="L36" s="39"/>
       <c r="M36"/>
     </row>
-    <row r="37" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="37" spans="8:13" x14ac:dyDescent="0.25">
       <c r="M37"/>
     </row>
-    <row r="38" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="38" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H38"/>
       <c r="I38"/>
       <c r="J38"/>
@@ -10298,7 +10295,7 @@
       <c r="L38"/>
       <c r="M38"/>
     </row>
-    <row r="39" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="39" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H39"/>
       <c r="I39"/>
       <c r="J39"/>
@@ -10329,15 +10326,15 @@
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.86328125" style="1" customWidth="1"/>
-    <col min="2" max="13" width="18.73046875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.85546875" style="1" customWidth="1"/>
+    <col min="2" max="13" width="18.7109375" style="1" customWidth="1"/>
     <col min="14" max="14" width="25" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="11.3984375" style="1"/>
+    <col min="15" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:14" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="18">
         <v>2026</v>
       </c>
@@ -10381,7 +10378,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="19" t="s">
         <v>6</v>
       </c>
@@ -10437,7 +10434,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19" t="s">
         <v>7</v>
       </c>
@@ -10493,7 +10490,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>8</v>
       </c>
@@ -10549,7 +10546,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="175" t="s">
         <v>13</v>
       </c>
@@ -10567,7 +10564,7 @@
       <c r="M7" s="175"/>
       <c r="N7" s="175"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="175"/>
       <c r="B8" s="175"/>
       <c r="C8" s="175"/>
@@ -10583,7 +10580,7 @@
       <c r="M8" s="175"/>
       <c r="N8" s="175"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="20" t="s">
         <v>6</v>
       </c>
@@ -10637,7 +10634,7 @@
       </c>
       <c r="N9" s="21"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
         <v>7</v>
       </c>
@@ -10691,7 +10688,7 @@
       </c>
       <c r="N10" s="21"/>
     </row>
-    <row r="11" spans="1:14" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="22" t="s">
         <v>8</v>
       </c>
@@ -10745,7 +10742,7 @@
       </c>
       <c r="N11" s="23"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="174" t="s">
         <v>14</v>
       </c>
@@ -10764,7 +10761,7 @@
       </c>
       <c r="M14"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="174"/>
       <c r="B15" s="174"/>
       <c r="C15" s="174"/>
@@ -10777,7 +10774,7 @@
       <c r="L15" s="176"/>
       <c r="M15"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>15</v>
       </c>
@@ -10810,7 +10807,7 @@
       </c>
       <c r="M16"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>28</v>
       </c>
@@ -10843,7 +10840,7 @@
       </c>
       <c r="M17"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>28</v>
       </c>
@@ -10874,7 +10871,7 @@
       <c r="L18" s="38"/>
       <c r="M18"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>29</v>
       </c>
@@ -10905,7 +10902,7 @@
       <c r="L19" s="36"/>
       <c r="M19"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>30</v>
       </c>
@@ -10934,7 +10931,7 @@
       <c r="L20" s="38"/>
       <c r="M20"/>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>29</v>
       </c>
@@ -10965,7 +10962,7 @@
       <c r="L21" s="36"/>
       <c r="M21"/>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="9" t="s">
         <v>28</v>
       </c>
@@ -10996,7 +10993,7 @@
       <c r="L22" s="39"/>
       <c r="M22"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>28</v>
       </c>
@@ -11027,66 +11024,66 @@
       <c r="L23" s="37"/>
       <c r="M23"/>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H24" s="40"/>
       <c r="I24" s="40"/>
       <c r="J24" s="40"/>
       <c r="L24" s="39"/>
       <c r="M24"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="H25" s="33"/>
       <c r="I25" s="33"/>
       <c r="L25" s="37"/>
       <c r="M25"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L26" s="39"/>
       <c r="M26"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L27" s="37"/>
       <c r="M27"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L28" s="39"/>
       <c r="M28"/>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L29" s="37"/>
       <c r="M29"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L30" s="39"/>
       <c r="M30"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L31" s="37"/>
       <c r="M31"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="L32" s="39"/>
       <c r="M32"/>
     </row>
-    <row r="33" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="33" spans="8:13" x14ac:dyDescent="0.25">
       <c r="L33" s="37"/>
       <c r="M33"/>
     </row>
-    <row r="34" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="34" spans="8:13" x14ac:dyDescent="0.25">
       <c r="L34" s="39"/>
       <c r="M34"/>
     </row>
-    <row r="35" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="35" spans="8:13" x14ac:dyDescent="0.25">
       <c r="M35"/>
     </row>
-    <row r="36" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="36" spans="8:13" x14ac:dyDescent="0.25">
       <c r="L36" s="39"/>
       <c r="M36"/>
     </row>
-    <row r="37" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="37" spans="8:13" x14ac:dyDescent="0.25">
       <c r="M37"/>
     </row>
-    <row r="38" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="38" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H38"/>
       <c r="I38"/>
       <c r="J38"/>
@@ -11094,7 +11091,7 @@
       <c r="L38"/>
       <c r="M38"/>
     </row>
-    <row r="39" spans="8:13" x14ac:dyDescent="0.45">
+    <row r="39" spans="8:13" x14ac:dyDescent="0.25">
       <c r="H39"/>
       <c r="I39"/>
       <c r="J39"/>
@@ -11123,17 +11120,17 @@
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.265625" customWidth="1"/>
-    <col min="2" max="5" width="18.73046875" customWidth="1"/>
-    <col min="6" max="6" width="21.1328125" customWidth="1"/>
-    <col min="7" max="11" width="18.73046875" customWidth="1"/>
-    <col min="12" max="12" width="22.1328125" customWidth="1"/>
-    <col min="13" max="13" width="18.73046875" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+    <col min="2" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="7" max="11" width="18.7109375" customWidth="1"/>
+    <col min="12" max="12" width="22.140625" customWidth="1"/>
+    <col min="13" max="13" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>39</v>
       </c>
@@ -11174,7 +11171,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
         <v>40</v>
       </c>
@@ -11215,7 +11212,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">
         <v>41</v>
       </c>
@@ -11256,7 +11253,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -11297,7 +11294,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2000</v>
       </c>
@@ -11314,7 +11311,7 @@
       <c r="L5" s="11"/>
       <c r="M5" s="11"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f t="shared" ref="A6:A32" si="0">A5+1</f>
         <v>2001</v>
@@ -11332,7 +11329,7 @@
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>2002</v>
@@ -11350,7 +11347,7 @@
       <c r="L7" s="11"/>
       <c r="M7" s="11"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>2003</v>
@@ -11368,7 +11365,7 @@
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>2004</v>
@@ -11386,7 +11383,7 @@
       <c r="L9" s="11"/>
       <c r="M9" s="11"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>2005</v>
@@ -11404,7 +11401,7 @@
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>2006</v>
@@ -11422,7 +11419,7 @@
       <c r="L11" s="11"/>
       <c r="M11" s="11"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>2007</v>
@@ -11440,7 +11437,7 @@
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>2008</v>
@@ -11458,7 +11455,7 @@
       <c r="L13" s="11"/>
       <c r="M13" s="11"/>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>2009</v>
@@ -11476,7 +11473,7 @@
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>2010</v>
@@ -11494,7 +11491,7 @@
       <c r="L15" s="11"/>
       <c r="M15" s="11"/>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>2011</v>
@@ -11512,7 +11509,7 @@
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>2012</v>
@@ -11530,7 +11527,7 @@
       <c r="L17" s="11"/>
       <c r="M17" s="11"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>2013</v>
@@ -11548,7 +11545,7 @@
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>2014</v>
@@ -11566,7 +11563,7 @@
       <c r="L19" s="11"/>
       <c r="M19" s="11"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>2015</v>
@@ -11608,7 +11605,7 @@
         <v>1.3592592592592591E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>2016</v>
@@ -11650,7 +11647,7 @@
         <v>1.3592592592592591E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>2017</v>
@@ -11692,7 +11689,7 @@
         <v>1.3577546296296298E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>2018</v>
@@ -11734,7 +11731,7 @@
         <v>1.3577546296296298E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>2019</v>
@@ -11776,7 +11773,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>2020</v>
@@ -11818,7 +11815,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>2021</v>
@@ -11860,7 +11857,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>2022</v>
@@ -11902,7 +11899,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>2023</v>
@@ -11944,7 +11941,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>2024</v>
@@ -11986,7 +11983,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>2025</v>
@@ -12028,7 +12025,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>2026</v>
@@ -12070,7 +12067,7 @@
         <v>1.3511574074074075E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <f t="shared" si="0"/>
         <v>2027</v>
@@ -12150,17 +12147,17 @@
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.86328125" customWidth="1"/>
-    <col min="2" max="5" width="18.73046875" customWidth="1"/>
-    <col min="6" max="6" width="21.1328125" customWidth="1"/>
-    <col min="7" max="11" width="18.73046875" customWidth="1"/>
-    <col min="12" max="12" width="22.1328125" customWidth="1"/>
-    <col min="13" max="13" width="18.73046875" customWidth="1"/>
+    <col min="1" max="1" width="11.85546875" customWidth="1"/>
+    <col min="2" max="5" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="21.140625" customWidth="1"/>
+    <col min="7" max="11" width="18.7109375" customWidth="1"/>
+    <col min="12" max="12" width="22.140625" customWidth="1"/>
+    <col min="13" max="13" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="42" t="s">
         <v>39</v>
       </c>
@@ -12201,7 +12198,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="42" t="s">
         <v>40</v>
       </c>
@@ -12242,7 +12239,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="42" t="s">
         <v>41</v>
       </c>
@@ -12283,7 +12280,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -12324,7 +12321,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>2000</v>
       </c>
@@ -12341,7 +12338,7 @@
       <c r="L5" s="38"/>
       <c r="M5" s="38"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <f t="shared" ref="A6:A31" si="0">A5+1</f>
         <v>2001</v>
@@ -12371,7 +12368,7 @@
         <v>1.3629629629629632E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <f t="shared" si="0"/>
         <v>2002</v>
@@ -12413,7 +12410,7 @@
         <v>1.3629629629629632E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <f t="shared" si="0"/>
         <v>2003</v>
@@ -12455,7 +12452,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <f t="shared" si="0"/>
         <v>2004</v>
@@ -12497,7 +12494,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <f t="shared" si="0"/>
         <v>2005</v>
@@ -12539,7 +12536,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <f t="shared" si="0"/>
         <v>2006</v>
@@ -12581,7 +12578,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>2007</v>
@@ -12623,7 +12620,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <f t="shared" si="0"/>
         <v>2008</v>
@@ -12665,7 +12662,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <f t="shared" si="0"/>
         <v>2009</v>
@@ -12707,7 +12704,7 @@
         <v>1.3346064814814815E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <f t="shared" si="0"/>
         <v>2010</v>
@@ -12749,7 +12746,7 @@
         <v>1.3306712962962966E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <f t="shared" si="0"/>
         <v>2011</v>
@@ -12791,7 +12788,7 @@
         <v>1.3306712962962966E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <f t="shared" si="0"/>
         <v>2012</v>
@@ -12833,7 +12830,7 @@
         <v>1.3306712962962966E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <f t="shared" si="0"/>
         <v>2013</v>
@@ -12875,7 +12872,7 @@
         <v>1.312962962962963E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <f t="shared" si="0"/>
         <v>2014</v>
@@ -12917,7 +12914,7 @@
         <v>1.312962962962963E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <f t="shared" si="0"/>
         <v>2015</v>
@@ -12959,7 +12956,7 @@
         <v>1.3116898148148148E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <f t="shared" si="0"/>
         <v>2016</v>
@@ -13001,7 +12998,7 @@
         <v>1.3116898148148148E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <f t="shared" si="0"/>
         <v>2017</v>
@@ -13043,7 +13040,7 @@
         <v>1.3116898148148148E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <f t="shared" si="0"/>
         <v>2018</v>
@@ -13085,7 +13082,7 @@
         <v>1.3116898148148148E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <f t="shared" si="0"/>
         <v>2019</v>
@@ -13127,7 +13124,7 @@
         <v>1.3116898148148148E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <f t="shared" si="0"/>
         <v>2020</v>
@@ -13169,7 +13166,7 @@
         <v>1.3097222222222223E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <f t="shared" si="0"/>
         <v>2021</v>
@@ -13211,7 +13208,7 @@
         <v>1.3097222222222223E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <f t="shared" si="0"/>
         <v>2022</v>
@@ -13253,7 +13250,7 @@
         <v>1.3097222222222223E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <f t="shared" si="0"/>
         <v>2023</v>
@@ -13295,7 +13292,7 @@
         <v>1.3097222222222223E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <f t="shared" si="0"/>
         <v>2024</v>
@@ -13337,7 +13334,7 @@
         <v>1.3097222222222223E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <f t="shared" si="0"/>
         <v>2025</v>
@@ -13379,7 +13376,7 @@
         <v>1.2931712962962962E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <f t="shared" si="0"/>
         <v>2026</v>
@@ -13421,7 +13418,7 @@
         <v>1.2931712962962962E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <f>A31+1</f>
         <v>2027</v>
@@ -13503,30 +13500,30 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.86328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.73046875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.73046875" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
     <col min="15" max="16" width="19" customWidth="1"/>
-    <col min="17" max="17" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="22.265625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.73046875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="47.265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="47.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="60" t="s">
         <v>161</v>
       </c>
@@ -13591,7 +13588,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="59" t="s">
         <v>197</v>
       </c>
@@ -13652,7 +13649,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="59" t="s">
         <v>198</v>
       </c>
@@ -13732,30 +13729,30 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.86328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="25.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.73046875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.73046875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.73046875" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
     <col min="15" max="16" width="19" customWidth="1"/>
-    <col min="17" max="17" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="22.265625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.73046875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="47.265625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="47.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:21" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="60" t="s">
         <v>161</v>
       </c>
@@ -13820,7 +13817,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="59" t="s">
         <v>189</v>
       </c>
@@ -13834,7 +13831,7 @@
         <v>50</v>
       </c>
       <c r="E2" s="59" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F2" s="59" t="s">
         <v>195</v>
@@ -13881,7 +13878,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="59" t="s">
         <v>190</v>
       </c>
@@ -13895,7 +13892,7 @@
         <v>50</v>
       </c>
       <c r="E3" s="59" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F3" s="59" t="s">
         <v>195</v>
@@ -13942,7 +13939,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
         <v>191</v>
       </c>
@@ -13956,7 +13953,7 @@
         <v>18</v>
       </c>
       <c r="E4" s="59" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F4" s="59" t="s">
         <v>195</v>
@@ -14000,10 +13997,10 @@
         <v>10</v>
       </c>
       <c r="U4" s="59" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.45">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
         <v>192</v>
       </c>
@@ -14017,7 +14014,7 @@
         <v>18</v>
       </c>
       <c r="E5" s="59" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F5" s="59" t="s">
         <v>195</v>
@@ -14062,7 +14059,7 @@
       </c>
       <c r="U5" s="59"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="59" t="s">
         <v>193</v>
       </c>
@@ -14076,7 +14073,7 @@
         <v>16</v>
       </c>
       <c r="E6" s="59" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F6" s="59" t="s">
         <v>195</v>
@@ -14121,7 +14118,7 @@
       </c>
       <c r="U6" s="59"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="59" t="s">
         <v>194</v>
       </c>
@@ -14135,7 +14132,7 @@
         <v>16</v>
       </c>
       <c r="E7" s="59" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="F7" s="59" t="s">
         <v>195</v>
@@ -14195,39 +14192,39 @@
   </sheetPr>
   <dimension ref="A1:X7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.73046875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.86328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.73046875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.86328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.73046875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.3984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.1328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.86328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.86328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.3984375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="17.3984375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.1328125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="24.86328125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="19.86328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="59" t="s">
         <v>161</v>
       </c>
@@ -14301,7 +14298,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="59" t="s">
         <v>212</v>
       </c>
@@ -14371,7 +14368,7 @@
         <v>1.9623842592592592E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="59" t="s">
         <v>213</v>
       </c>
@@ -14441,7 +14438,7 @@
         <v>1.8121527777777778E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
         <v>214</v>
       </c>
@@ -14511,7 +14508,7 @@
         <v>1.9979166666666665E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
         <v>215</v>
       </c>
@@ -14581,7 +14578,7 @@
         <v>1.7653935185185186E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="59" t="s">
         <v>189</v>
       </c>
@@ -14651,7 +14648,7 @@
         <v>1.8998842592592594E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="59" t="s">
         <v>190</v>
       </c>
@@ -14740,35 +14737,35 @@
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.86328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.73046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.59765625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.265625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.59765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="27" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="22" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.59765625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.265625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="21.59765625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="27" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="59" t="s">
         <v>161</v>
       </c>
@@ -14842,7 +14839,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" s="59" t="s">
         <v>223</v>
       </c>
@@ -14912,7 +14909,7 @@
         <v>1.8332175925925925E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="59" t="s">
         <v>224</v>
       </c>
@@ -14982,9 +14979,9 @@
         <v>1.7003472222222222E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="59" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B4" s="59" t="s">
         <v>182</v>
@@ -15058,9 +15055,9 @@
         <v>3.9324537037037035E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="59" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B5" s="59" t="s">
         <v>182</v>
@@ -15134,9 +15131,9 @@
         <v>4.0693981481481478E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="59" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B6" s="59" t="s">
         <v>182</v>
@@ -15210,9 +15207,9 @@
         <v>4.1888888888888884E-4</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="59" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B7" s="59" t="s">
         <v>164</v>
@@ -15286,9 +15283,9 @@
         <v>4.7436458333333331E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="59" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B8" s="59" t="s">
         <v>164</v>
@@ -15362,9 +15359,9 @@
         <v>4.9196875E-4</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="59" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="B9" s="59" t="s">
         <v>164</v>
@@ -15438,9 +15435,9 @@
         <v>5.1593750000000001E-4</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="59" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B10" s="59" t="s">
         <v>182</v>
@@ -15514,9 +15511,9 @@
         <v>4.4791666666666667E-4</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="59" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B11" s="59" t="s">
         <v>182</v>
@@ -15590,9 +15587,9 @@
         <v>4.619444444444444E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="59" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B12" s="59" t="s">
         <v>182</v>
@@ -15666,9 +15663,9 @@
         <v>4.7138888888888881E-4</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="59" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B13" s="59" t="s">
         <v>164</v>
@@ -15742,9 +15739,9 @@
         <v>5.3782870370370367E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="59" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B14" s="59" t="s">
         <v>164</v>
@@ -15818,9 +15815,9 @@
         <v>5.5107638888888882E-4</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" s="59" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="B15" s="59" t="s">
         <v>164</v>
@@ -15907,24 +15904,24 @@
   <sheetPr codeName="Tabelle11">
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="84.86328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="36.73046875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="84.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>225</v>
       </c>
@@ -15950,9 +15947,9 @@
         <v>230</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="70">
-        <v>46075</v>
+        <v>46124</v>
       </c>
       <c r="C2" s="71">
         <v>0.38541666666666669</v>
@@ -15973,127 +15970,127 @@
         <v>234</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="70">
-        <v>46075</v>
+        <v>46124</v>
       </c>
       <c r="C3" s="71">
-        <v>0.50694444444444442</v>
+        <v>0.5</v>
       </c>
       <c r="D3" s="71">
-        <v>0.66666666666666663</v>
+        <v>0.65625</v>
       </c>
       <c r="E3" s="72" t="s">
         <v>237</v>
       </c>
       <c r="F3" s="72" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="G3" t="s">
         <v>233</v>
       </c>
       <c r="H3" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="70">
-        <v>46124</v>
+        <v>46186</v>
       </c>
       <c r="C4" s="71">
-        <v>0.38541666666666669</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="D4" s="71">
-        <v>0.52083333333333337</v>
+        <v>0.76041666666666663</v>
       </c>
       <c r="E4" s="72" t="s">
+        <v>237</v>
+      </c>
+      <c r="F4" s="72" t="s">
+        <v>239</v>
+      </c>
+      <c r="G4" t="s">
+        <v>240</v>
+      </c>
+      <c r="H4" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="70">
+        <v>46187</v>
+      </c>
+      <c r="C5" s="71">
+        <v>0.53125</v>
+      </c>
+      <c r="D5" s="71">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E5" s="72" t="s">
         <v>232</v>
       </c>
-      <c r="F4" s="72" t="s">
-        <v>236</v>
-      </c>
-      <c r="G4" t="s">
-        <v>233</v>
-      </c>
-      <c r="H4" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A5" s="70">
-        <v>46124</v>
-      </c>
-      <c r="C5" s="71">
-        <v>0.5</v>
-      </c>
-      <c r="D5" s="71">
-        <v>0.65625</v>
-      </c>
-      <c r="E5" s="72" t="s">
-        <v>237</v>
-      </c>
       <c r="F5" s="72" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="G5" t="s">
         <v>233</v>
       </c>
       <c r="H5" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="70">
-        <v>46186</v>
+        <v>46199</v>
+      </c>
+      <c r="B6" s="70">
+        <v>46203</v>
       </c>
       <c r="C6" s="71">
+        <v>0</v>
+      </c>
+      <c r="D6" s="71">
+        <v>0.99930555555555556</v>
+      </c>
+      <c r="E6" s="72" t="s">
+        <v>242</v>
+      </c>
+      <c r="F6" s="72" t="s">
+        <v>243</v>
+      </c>
+      <c r="G6" t="s">
+        <v>244</v>
+      </c>
+      <c r="H6" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="70">
+        <v>46201</v>
+      </c>
+      <c r="C7" s="71">
         <v>0.41666666666666669</v>
       </c>
-      <c r="D6" s="71">
-        <v>0.76041666666666663</v>
-      </c>
-      <c r="E6" s="72" t="s">
-        <v>237</v>
-      </c>
-      <c r="F6" s="72" t="s">
-        <v>239</v>
-      </c>
-      <c r="G6" t="s">
-        <v>240</v>
-      </c>
-      <c r="H6" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A7" s="70">
-        <v>46187</v>
-      </c>
-      <c r="C7" s="71">
-        <v>0.53125</v>
-      </c>
       <c r="D7" s="71">
-        <v>0.66666666666666663</v>
+        <v>0.75</v>
       </c>
       <c r="E7" s="72" t="s">
-        <v>232</v>
+        <v>245</v>
       </c>
       <c r="F7" s="72" t="s">
-        <v>241</v>
+        <v>276</v>
       </c>
       <c r="G7" t="s">
-        <v>233</v>
+        <v>246</v>
       </c>
       <c r="H7" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="70">
-        <v>46199</v>
-      </c>
-      <c r="B8" s="70">
-        <v>46203</v>
+        <v>46228</v>
       </c>
       <c r="C8" s="71">
         <v>0</v>
@@ -16102,66 +16099,20 @@
         <v>0.99930555555555556</v>
       </c>
       <c r="E8" s="72" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="F8" s="72" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="G8" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="H8" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A9" s="70">
-        <v>46202</v>
-      </c>
-      <c r="C9" s="71">
-        <v>0.41666666666666669</v>
-      </c>
-      <c r="D9" s="71">
-        <v>0.75</v>
-      </c>
-      <c r="E9" s="72" t="s">
-        <v>245</v>
-      </c>
-      <c r="F9" s="72" t="s">
-        <v>246</v>
-      </c>
-      <c r="G9" t="s">
-        <v>247</v>
-      </c>
-      <c r="H9" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A10" s="70">
-        <v>46228</v>
-      </c>
-      <c r="C10" s="71">
-        <v>0</v>
-      </c>
-      <c r="D10" s="71">
-        <v>0.99930555555555556</v>
-      </c>
-      <c r="E10" s="72" t="s">
-        <v>249</v>
-      </c>
-      <c r="F10" s="72" t="s">
-        <v>250</v>
-      </c>
-      <c r="G10" t="s">
         <v>251</v>
       </c>
-      <c r="H10" t="s">
-        <v>252</v>
-      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:H10">
+  <conditionalFormatting sqref="A2:H8">
     <cfRule type="expression" dxfId="2" priority="1">
       <formula>$A2&lt;TODAY()</formula>
     </cfRule>
@@ -16182,147 +16133,147 @@
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.265625" customWidth="1"/>
-    <col min="2" max="2" width="32.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="26" width="9.59765625" customWidth="1"/>
-    <col min="28" max="28" width="32.3984375" bestFit="1" customWidth="1"/>
-    <col min="29" max="52" width="4.59765625" customWidth="1"/>
-    <col min="54" max="54" width="32.3984375" bestFit="1" customWidth="1"/>
-    <col min="55" max="78" width="9.59765625" customWidth="1"/>
+    <col min="1" max="1" width="5.28515625" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="26" width="9.5703125" customWidth="1"/>
+    <col min="28" max="28" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="52" width="4.5703125" customWidth="1"/>
+    <col min="54" max="54" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="55" max="78" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="140">
+    <row r="1" spans="1:78" s="74" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="159">
         <v>2025</v>
       </c>
       <c r="B1" s="79" t="str">
         <f ca="1">CONCATENATE("in: ",YEAR(TODAY())-1," für: ", YEAR(TODAY()))</f>
         <v>in: 2025 für: 2026</v>
       </c>
-      <c r="C1" s="141" t="s">
+      <c r="C1" s="140" t="s">
+        <v>254</v>
+      </c>
+      <c r="D1" s="140"/>
+      <c r="E1" s="141"/>
+      <c r="F1" s="144" t="s">
+        <v>255</v>
+      </c>
+      <c r="G1" s="145"/>
+      <c r="H1" s="145"/>
+      <c r="I1" s="145"/>
+      <c r="J1" s="146"/>
+      <c r="K1" s="150" t="s">
+        <v>259</v>
+      </c>
+      <c r="L1" s="151"/>
+      <c r="M1" s="151"/>
+      <c r="N1" s="152"/>
+      <c r="O1" s="142" t="s">
         <v>256</v>
       </c>
-      <c r="D1" s="141"/>
-      <c r="E1" s="142"/>
-      <c r="F1" s="143" t="s">
+      <c r="P1" s="142"/>
+      <c r="Q1" s="143"/>
+      <c r="R1" s="156" t="s">
         <v>257</v>
       </c>
-      <c r="G1" s="144"/>
-      <c r="H1" s="144"/>
-      <c r="I1" s="144"/>
-      <c r="J1" s="145"/>
-      <c r="K1" s="146" t="s">
-        <v>261</v>
-      </c>
-      <c r="L1" s="147"/>
-      <c r="M1" s="147"/>
-      <c r="N1" s="148"/>
-      <c r="O1" s="166" t="s">
-        <v>258</v>
-      </c>
-      <c r="P1" s="166"/>
-      <c r="Q1" s="167"/>
-      <c r="R1" s="168" t="s">
-        <v>259</v>
-      </c>
-      <c r="S1" s="169"/>
-      <c r="T1" s="169"/>
-      <c r="U1" s="169"/>
-      <c r="V1" s="170"/>
-      <c r="W1" s="171" t="s">
-        <v>262</v>
-      </c>
-      <c r="X1" s="172"/>
-      <c r="Y1" s="172"/>
-      <c r="Z1" s="173"/>
+      <c r="S1" s="157"/>
+      <c r="T1" s="157"/>
+      <c r="U1" s="157"/>
+      <c r="V1" s="158"/>
+      <c r="W1" s="153" t="s">
+        <v>260</v>
+      </c>
+      <c r="X1" s="154"/>
+      <c r="Y1" s="154"/>
+      <c r="Z1" s="155"/>
       <c r="AA1"/>
       <c r="AB1" s="79" t="str">
         <f ca="1">CONCATENATE("in: ",YEAR(TODAY())-1," für: ", YEAR(TODAY()))</f>
         <v>in: 2025 für: 2026</v>
       </c>
-      <c r="AC1" s="149" t="s">
+      <c r="AC1" s="160" t="s">
+        <v>261</v>
+      </c>
+      <c r="AD1" s="160"/>
+      <c r="AE1" s="161"/>
+      <c r="AF1" s="162" t="s">
+        <v>262</v>
+      </c>
+      <c r="AG1" s="163"/>
+      <c r="AH1" s="163"/>
+      <c r="AI1" s="163"/>
+      <c r="AJ1" s="164"/>
+      <c r="AK1" s="165" t="s">
         <v>263</v>
       </c>
-      <c r="AD1" s="149"/>
-      <c r="AE1" s="150"/>
-      <c r="AF1" s="151" t="s">
+      <c r="AL1" s="166"/>
+      <c r="AM1" s="166"/>
+      <c r="AN1" s="167"/>
+      <c r="AO1" s="168" t="s">
         <v>264</v>
       </c>
-      <c r="AG1" s="152"/>
-      <c r="AH1" s="152"/>
-      <c r="AI1" s="152"/>
-      <c r="AJ1" s="153"/>
-      <c r="AK1" s="154" t="s">
+      <c r="AP1" s="169"/>
+      <c r="AQ1" s="170"/>
+      <c r="AR1" s="171" t="s">
         <v>265</v>
       </c>
-      <c r="AL1" s="155"/>
-      <c r="AM1" s="155"/>
-      <c r="AN1" s="156"/>
-      <c r="AO1" s="157" t="s">
+      <c r="AS1" s="172"/>
+      <c r="AT1" s="172"/>
+      <c r="AU1" s="172"/>
+      <c r="AV1" s="173"/>
+      <c r="AW1" s="147" t="s">
         <v>266</v>
       </c>
-      <c r="AP1" s="158"/>
-      <c r="AQ1" s="159"/>
-      <c r="AR1" s="160" t="s">
-        <v>267</v>
-      </c>
-      <c r="AS1" s="161"/>
-      <c r="AT1" s="161"/>
-      <c r="AU1" s="161"/>
-      <c r="AV1" s="162"/>
-      <c r="AW1" s="163" t="s">
-        <v>268</v>
-      </c>
-      <c r="AX1" s="164"/>
-      <c r="AY1" s="164"/>
-      <c r="AZ1" s="165"/>
+      <c r="AX1" s="148"/>
+      <c r="AY1" s="148"/>
+      <c r="AZ1" s="149"/>
       <c r="BB1" s="79" t="str">
         <f ca="1">CONCATENATE("in: ",YEAR(TODAY())-1," für: ", YEAR(TODAY()))</f>
         <v>in: 2025 für: 2026</v>
       </c>
-      <c r="BC1" s="141" t="s">
+      <c r="BC1" s="140" t="s">
+        <v>267</v>
+      </c>
+      <c r="BD1" s="140"/>
+      <c r="BE1" s="141"/>
+      <c r="BF1" s="144" t="s">
+        <v>268</v>
+      </c>
+      <c r="BG1" s="145"/>
+      <c r="BH1" s="145"/>
+      <c r="BI1" s="145"/>
+      <c r="BJ1" s="146"/>
+      <c r="BK1" s="150" t="s">
         <v>269</v>
       </c>
-      <c r="BD1" s="141"/>
-      <c r="BE1" s="142"/>
-      <c r="BF1" s="143" t="s">
+      <c r="BL1" s="151"/>
+      <c r="BM1" s="151"/>
+      <c r="BN1" s="152"/>
+      <c r="BO1" s="142" t="s">
+        <v>256</v>
+      </c>
+      <c r="BP1" s="142"/>
+      <c r="BQ1" s="143"/>
+      <c r="BR1" s="156" t="s">
+        <v>257</v>
+      </c>
+      <c r="BS1" s="157"/>
+      <c r="BT1" s="157"/>
+      <c r="BU1" s="157"/>
+      <c r="BV1" s="158"/>
+      <c r="BW1" s="153" t="s">
         <v>270</v>
       </c>
-      <c r="BG1" s="144"/>
-      <c r="BH1" s="144"/>
-      <c r="BI1" s="144"/>
-      <c r="BJ1" s="145"/>
-      <c r="BK1" s="146" t="s">
-        <v>271</v>
-      </c>
-      <c r="BL1" s="147"/>
-      <c r="BM1" s="147"/>
-      <c r="BN1" s="148"/>
-      <c r="BO1" s="166" t="s">
+      <c r="BX1" s="154"/>
+      <c r="BY1" s="154"/>
+      <c r="BZ1" s="155"/>
+    </row>
+    <row r="2" spans="1:78" s="128" customFormat="1" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="159"/>
+      <c r="B2" s="80" t="s">
         <v>258</v>
-      </c>
-      <c r="BP1" s="166"/>
-      <c r="BQ1" s="167"/>
-      <c r="BR1" s="168" t="s">
-        <v>259</v>
-      </c>
-      <c r="BS1" s="169"/>
-      <c r="BT1" s="169"/>
-      <c r="BU1" s="169"/>
-      <c r="BV1" s="170"/>
-      <c r="BW1" s="171" t="s">
-        <v>272</v>
-      </c>
-      <c r="BX1" s="172"/>
-      <c r="BY1" s="172"/>
-      <c r="BZ1" s="173"/>
-    </row>
-    <row r="2" spans="1:78" s="128" customFormat="1" ht="21.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="140"/>
-      <c r="B2" s="80" t="s">
-        <v>260</v>
       </c>
       <c r="C2" s="75" t="str">
         <f ca="1">CONCATENATE("≤",YEAR(TODAY())-15-1)</f>
@@ -16422,7 +16373,7 @@
       </c>
       <c r="AA2"/>
       <c r="AB2" s="80" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="AC2" s="114" t="str">
         <f ca="1">CONCATENATE("≤",YEAR(TODAY())-15)</f>
@@ -16521,7 +16472,7 @@
         <v>2002-1986</v>
       </c>
       <c r="BB2" s="80" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="BC2" s="92" t="str">
         <f ca="1">CONCATENATE("≤",YEAR(TODAY())-15-1)</f>
@@ -16620,8 +16571,8 @@
         <v>2001-1985</v>
       </c>
     </row>
-    <row r="3" spans="1:78" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="140"/>
+    <row r="3" spans="1:78" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="159"/>
       <c r="B3" s="81" t="s">
         <v>0</v>
       </c>
@@ -16873,8 +16824,8 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:78" x14ac:dyDescent="0.45">
-      <c r="A4" s="140"/>
+    <row r="4" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="A4" s="159"/>
       <c r="B4" s="81" t="s">
         <v>219</v>
       </c>
@@ -17125,8 +17076,8 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:78" x14ac:dyDescent="0.45">
-      <c r="A5" s="140"/>
+    <row r="5" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="A5" s="159"/>
       <c r="B5" s="81" t="s">
         <v>220</v>
       </c>
@@ -17377,8 +17328,8 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:78" x14ac:dyDescent="0.45">
-      <c r="A6" s="140"/>
+    <row r="6" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="A6" s="159"/>
       <c r="B6" s="81" t="s">
         <v>221</v>
       </c>
@@ -17629,8 +17580,8 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:78" x14ac:dyDescent="0.45">
-      <c r="A7" s="140"/>
+    <row r="7" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="A7" s="159"/>
       <c r="B7" s="81" t="s">
         <v>222</v>
       </c>
@@ -17881,8 +17832,8 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:78" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="140"/>
+    <row r="8" spans="1:78" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="159"/>
       <c r="B8" s="84" t="s">
         <v>4</v>
       </c>
@@ -18133,136 +18084,136 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:78" ht="14.65" thickTop="1" x14ac:dyDescent="0.45"/>
-    <row r="10" spans="1:78" ht="18" x14ac:dyDescent="0.45">
-      <c r="A10" s="140">
+    <row r="9" spans="1:78" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:78" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="159">
         <v>2026</v>
       </c>
       <c r="B10" s="79" t="str">
         <f ca="1">CONCATENATE("in: ",YEAR(TODAY())," für: ", YEAR(TODAY())+1)</f>
         <v>in: 2026 für: 2027</v>
       </c>
-      <c r="C10" s="141" t="s">
+      <c r="C10" s="140" t="s">
+        <v>254</v>
+      </c>
+      <c r="D10" s="140"/>
+      <c r="E10" s="141"/>
+      <c r="F10" s="144" t="s">
+        <v>255</v>
+      </c>
+      <c r="G10" s="145"/>
+      <c r="H10" s="145"/>
+      <c r="I10" s="145"/>
+      <c r="J10" s="146"/>
+      <c r="K10" s="150" t="s">
+        <v>259</v>
+      </c>
+      <c r="L10" s="151"/>
+      <c r="M10" s="151"/>
+      <c r="N10" s="152"/>
+      <c r="O10" s="142" t="s">
         <v>256</v>
       </c>
-      <c r="D10" s="141"/>
-      <c r="E10" s="142"/>
-      <c r="F10" s="143" t="s">
+      <c r="P10" s="142"/>
+      <c r="Q10" s="143"/>
+      <c r="R10" s="156" t="s">
         <v>257</v>
       </c>
-      <c r="G10" s="144"/>
-      <c r="H10" s="144"/>
-      <c r="I10" s="144"/>
-      <c r="J10" s="145"/>
-      <c r="K10" s="146" t="s">
-        <v>261</v>
-      </c>
-      <c r="L10" s="147"/>
-      <c r="M10" s="147"/>
-      <c r="N10" s="148"/>
-      <c r="O10" s="166" t="s">
-        <v>258</v>
-      </c>
-      <c r="P10" s="166"/>
-      <c r="Q10" s="167"/>
-      <c r="R10" s="168" t="s">
-        <v>259</v>
-      </c>
-      <c r="S10" s="169"/>
-      <c r="T10" s="169"/>
-      <c r="U10" s="169"/>
-      <c r="V10" s="170"/>
-      <c r="W10" s="171" t="s">
-        <v>262</v>
-      </c>
-      <c r="X10" s="172"/>
-      <c r="Y10" s="172"/>
-      <c r="Z10" s="173"/>
+      <c r="S10" s="157"/>
+      <c r="T10" s="157"/>
+      <c r="U10" s="157"/>
+      <c r="V10" s="158"/>
+      <c r="W10" s="153" t="s">
+        <v>260</v>
+      </c>
+      <c r="X10" s="154"/>
+      <c r="Y10" s="154"/>
+      <c r="Z10" s="155"/>
       <c r="AB10" s="79" t="str">
         <f ca="1">CONCATENATE("in: ",YEAR(TODAY())," für: ", YEAR(TODAY())+1)</f>
         <v>in: 2026 für: 2027</v>
       </c>
-      <c r="AC10" s="149" t="s">
+      <c r="AC10" s="160" t="s">
+        <v>261</v>
+      </c>
+      <c r="AD10" s="160"/>
+      <c r="AE10" s="161"/>
+      <c r="AF10" s="162" t="s">
+        <v>262</v>
+      </c>
+      <c r="AG10" s="163"/>
+      <c r="AH10" s="163"/>
+      <c r="AI10" s="163"/>
+      <c r="AJ10" s="164"/>
+      <c r="AK10" s="165" t="s">
         <v>263</v>
       </c>
-      <c r="AD10" s="149"/>
-      <c r="AE10" s="150"/>
-      <c r="AF10" s="151" t="s">
+      <c r="AL10" s="166"/>
+      <c r="AM10" s="166"/>
+      <c r="AN10" s="167"/>
+      <c r="AO10" s="168" t="s">
         <v>264</v>
       </c>
-      <c r="AG10" s="152"/>
-      <c r="AH10" s="152"/>
-      <c r="AI10" s="152"/>
-      <c r="AJ10" s="153"/>
-      <c r="AK10" s="154" t="s">
+      <c r="AP10" s="169"/>
+      <c r="AQ10" s="170"/>
+      <c r="AR10" s="171" t="s">
         <v>265</v>
       </c>
-      <c r="AL10" s="155"/>
-      <c r="AM10" s="155"/>
-      <c r="AN10" s="156"/>
-      <c r="AO10" s="157" t="s">
+      <c r="AS10" s="172"/>
+      <c r="AT10" s="172"/>
+      <c r="AU10" s="172"/>
+      <c r="AV10" s="173"/>
+      <c r="AW10" s="147" t="s">
         <v>266</v>
       </c>
-      <c r="AP10" s="158"/>
-      <c r="AQ10" s="159"/>
-      <c r="AR10" s="160" t="s">
-        <v>267</v>
-      </c>
-      <c r="AS10" s="161"/>
-      <c r="AT10" s="161"/>
-      <c r="AU10" s="161"/>
-      <c r="AV10" s="162"/>
-      <c r="AW10" s="163" t="s">
-        <v>268</v>
-      </c>
-      <c r="AX10" s="164"/>
-      <c r="AY10" s="164"/>
-      <c r="AZ10" s="165"/>
+      <c r="AX10" s="148"/>
+      <c r="AY10" s="148"/>
+      <c r="AZ10" s="149"/>
       <c r="BB10" s="79" t="str">
         <f ca="1">CONCATENATE("in: ",YEAR(TODAY())," für: ", YEAR(TODAY())+1)</f>
         <v>in: 2026 für: 2027</v>
       </c>
-      <c r="BC10" s="141" t="s">
+      <c r="BC10" s="140" t="s">
+        <v>267</v>
+      </c>
+      <c r="BD10" s="140"/>
+      <c r="BE10" s="141"/>
+      <c r="BF10" s="144" t="s">
+        <v>268</v>
+      </c>
+      <c r="BG10" s="145"/>
+      <c r="BH10" s="145"/>
+      <c r="BI10" s="145"/>
+      <c r="BJ10" s="146"/>
+      <c r="BK10" s="150" t="s">
         <v>269</v>
       </c>
-      <c r="BD10" s="141"/>
-      <c r="BE10" s="142"/>
-      <c r="BF10" s="143" t="s">
+      <c r="BL10" s="151"/>
+      <c r="BM10" s="151"/>
+      <c r="BN10" s="152"/>
+      <c r="BO10" s="142" t="s">
+        <v>256</v>
+      </c>
+      <c r="BP10" s="142"/>
+      <c r="BQ10" s="143"/>
+      <c r="BR10" s="156" t="s">
+        <v>257</v>
+      </c>
+      <c r="BS10" s="157"/>
+      <c r="BT10" s="157"/>
+      <c r="BU10" s="157"/>
+      <c r="BV10" s="158"/>
+      <c r="BW10" s="153" t="s">
         <v>270</v>
       </c>
-      <c r="BG10" s="144"/>
-      <c r="BH10" s="144"/>
-      <c r="BI10" s="144"/>
-      <c r="BJ10" s="145"/>
-      <c r="BK10" s="146" t="s">
-        <v>271</v>
-      </c>
-      <c r="BL10" s="147"/>
-      <c r="BM10" s="147"/>
-      <c r="BN10" s="148"/>
-      <c r="BO10" s="166" t="s">
+      <c r="BX10" s="154"/>
+      <c r="BY10" s="154"/>
+      <c r="BZ10" s="155"/>
+    </row>
+    <row r="11" spans="1:78" ht="23.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="159"/>
+      <c r="B11" s="80" t="s">
         <v>258</v>
-      </c>
-      <c r="BP10" s="166"/>
-      <c r="BQ10" s="167"/>
-      <c r="BR10" s="168" t="s">
-        <v>259</v>
-      </c>
-      <c r="BS10" s="169"/>
-      <c r="BT10" s="169"/>
-      <c r="BU10" s="169"/>
-      <c r="BV10" s="170"/>
-      <c r="BW10" s="171" t="s">
-        <v>272</v>
-      </c>
-      <c r="BX10" s="172"/>
-      <c r="BY10" s="172"/>
-      <c r="BZ10" s="173"/>
-    </row>
-    <row r="11" spans="1:78" ht="21.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="140"/>
-      <c r="B11" s="80" t="s">
-        <v>260</v>
       </c>
       <c r="C11" s="92" t="str">
         <f ca="1">CONCATENATE("≤",YEAR(TODAY())-15)</f>
@@ -18362,7 +18313,7 @@
       </c>
       <c r="AA11" s="73"/>
       <c r="AB11" s="80" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="AC11" s="114" t="str">
         <f ca="1">CONCATENATE("≤",YEAR(TODAY())-15)</f>
@@ -18461,7 +18412,7 @@
         <v>2002-1986</v>
       </c>
       <c r="BB11" s="80" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="BC11" s="92" t="str">
         <f ca="1">CONCATENATE("≤",YEAR(TODAY())-15-1)</f>
@@ -18560,8 +18511,8 @@
         <v>2001-1985</v>
       </c>
     </row>
-    <row r="12" spans="1:78" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="140"/>
+    <row r="12" spans="1:78" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="159"/>
       <c r="B12" s="81" t="s">
         <v>0</v>
       </c>
@@ -18812,8 +18763,8 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:78" x14ac:dyDescent="0.45">
-      <c r="A13" s="140"/>
+    <row r="13" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="A13" s="159"/>
       <c r="B13" s="81" t="s">
         <v>219</v>
       </c>
@@ -19064,8 +19015,8 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:78" x14ac:dyDescent="0.45">
-      <c r="A14" s="140"/>
+    <row r="14" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="A14" s="159"/>
       <c r="B14" s="81" t="s">
         <v>220</v>
       </c>
@@ -19316,8 +19267,8 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:78" x14ac:dyDescent="0.45">
-      <c r="A15" s="140"/>
+    <row r="15" spans="1:78" x14ac:dyDescent="0.25">
+      <c r="A15" s="159"/>
       <c r="B15" s="81" t="s">
         <v>221</v>
       </c>
@@ -19568,8 +19519,8 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="140"/>
+    <row r="16" spans="1:78" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="159"/>
       <c r="B16" s="81" t="s">
         <v>222</v>
       </c>
@@ -19820,8 +19771,8 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:78" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="140"/>
+    <row r="17" spans="1:78" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="159"/>
       <c r="B17" s="84" t="s">
         <v>4</v>
       </c>
@@ -20072,7 +20023,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:78" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:78" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="C18" s="64"/>
       <c r="O18" s="64"/>
       <c r="T18" s="67"/>
@@ -20081,7 +20032,7 @@
       <c r="X18" s="64"/>
       <c r="AD18" s="64"/>
     </row>
-    <row r="21" spans="1:78" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:78" x14ac:dyDescent="0.25">
       <c r="C21" s="63"/>
       <c r="D21" s="66"/>
       <c r="E21" s="66"/>
@@ -20101,7 +20052,7 @@
       <c r="AF21" s="69"/>
       <c r="AG21" s="69"/>
     </row>
-    <row r="22" spans="1:78" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:78" x14ac:dyDescent="0.25">
       <c r="C22" s="64"/>
       <c r="D22" s="65"/>
       <c r="E22" s="65"/>
@@ -20121,7 +20072,7 @@
       <c r="AF22" s="65"/>
       <c r="AG22" s="65"/>
     </row>
-    <row r="23" spans="1:78" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:78" x14ac:dyDescent="0.25">
       <c r="C23" s="64"/>
       <c r="D23" s="65"/>
       <c r="E23" s="65"/>
@@ -20141,7 +20092,7 @@
       <c r="AF23" s="65"/>
       <c r="AG23" s="65"/>
     </row>
-    <row r="24" spans="1:78" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:78" x14ac:dyDescent="0.25">
       <c r="C24" s="64"/>
       <c r="D24" s="65"/>
       <c r="E24" s="65"/>
@@ -20161,7 +20112,7 @@
       <c r="AF24" s="65"/>
       <c r="AG24" s="65"/>
     </row>
-    <row r="25" spans="1:78" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:78" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C25" s="64"/>
       <c r="D25" s="65"/>
       <c r="E25" s="65"/>
@@ -20181,7 +20132,7 @@
       <c r="AF25" s="65"/>
       <c r="AG25" s="65"/>
     </row>
-    <row r="26" spans="1:78" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:78" x14ac:dyDescent="0.25">
       <c r="C26" s="64"/>
       <c r="D26" s="65"/>
       <c r="E26" s="65"/>
@@ -20201,7 +20152,7 @@
       <c r="AF26" s="65"/>
       <c r="AG26" s="65"/>
     </row>
-    <row r="27" spans="1:78" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:78" x14ac:dyDescent="0.25">
       <c r="C27" s="64"/>
       <c r="D27" s="65"/>
       <c r="E27" s="65"/>
@@ -20221,7 +20172,7 @@
       <c r="AF27" s="65"/>
       <c r="AG27" s="65"/>
     </row>
-    <row r="30" spans="1:78" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:78" x14ac:dyDescent="0.25">
       <c r="C30" s="63"/>
       <c r="D30" s="66"/>
       <c r="E30" s="66"/>
@@ -20230,7 +20181,7 @@
       <c r="H30" s="66"/>
       <c r="P30" s="67"/>
     </row>
-    <row r="31" spans="1:78" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:78" x14ac:dyDescent="0.25">
       <c r="C31" s="64"/>
       <c r="D31" s="65"/>
       <c r="E31" s="65"/>
@@ -20238,7 +20189,7 @@
       <c r="G31" s="65"/>
       <c r="H31" s="65"/>
     </row>
-    <row r="40" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="40" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C40" s="64"/>
       <c r="D40" s="65"/>
       <c r="E40" s="65"/>
@@ -20246,7 +20197,7 @@
       <c r="G40" s="65"/>
       <c r="H40" s="65"/>
     </row>
-    <row r="41" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="41" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C41" s="64"/>
       <c r="D41" s="65"/>
       <c r="E41" s="65"/>
@@ -20254,7 +20205,7 @@
       <c r="G41" s="65"/>
       <c r="H41" s="65"/>
     </row>
-    <row r="42" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="42" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C42" s="64"/>
       <c r="D42" s="65"/>
       <c r="E42" s="65"/>
@@ -20262,7 +20213,7 @@
       <c r="G42" s="65"/>
       <c r="H42" s="65"/>
     </row>
-    <row r="43" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="43" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C43" s="64"/>
       <c r="D43" s="65"/>
       <c r="E43" s="65"/>
@@ -20270,7 +20221,7 @@
       <c r="G43" s="65"/>
       <c r="H43" s="65"/>
     </row>
-    <row r="44" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="44" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C44" s="64"/>
       <c r="D44" s="65"/>
       <c r="E44" s="65"/>
@@ -20278,7 +20229,7 @@
       <c r="G44" s="65"/>
       <c r="H44" s="65"/>
     </row>
-    <row r="45" spans="3:8" x14ac:dyDescent="0.45">
+    <row r="45" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C45" s="64"/>
       <c r="D45" s="65"/>
       <c r="E45" s="65"/>
@@ -20288,28 +20239,6 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="O10:Q10"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="F10:J10"/>
-    <mergeCell ref="AW10:AZ10"/>
-    <mergeCell ref="K10:N10"/>
-    <mergeCell ref="W10:Z10"/>
-    <mergeCell ref="F1:J1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="R1:V1"/>
-    <mergeCell ref="W1:Z1"/>
-    <mergeCell ref="R10:V10"/>
-    <mergeCell ref="BO10:BQ10"/>
-    <mergeCell ref="BR10:BV10"/>
-    <mergeCell ref="BW10:BZ10"/>
-    <mergeCell ref="BC1:BE1"/>
-    <mergeCell ref="BF1:BJ1"/>
-    <mergeCell ref="BK1:BN1"/>
-    <mergeCell ref="BO1:BQ1"/>
-    <mergeCell ref="BR1:BV1"/>
-    <mergeCell ref="BW1:BZ1"/>
     <mergeCell ref="A1:A8"/>
     <mergeCell ref="A10:A17"/>
     <mergeCell ref="BC10:BE10"/>
@@ -20326,6 +20255,28 @@
     <mergeCell ref="AK10:AN10"/>
     <mergeCell ref="AO10:AQ10"/>
     <mergeCell ref="AR10:AV10"/>
+    <mergeCell ref="BO10:BQ10"/>
+    <mergeCell ref="BR10:BV10"/>
+    <mergeCell ref="BW10:BZ10"/>
+    <mergeCell ref="BC1:BE1"/>
+    <mergeCell ref="BF1:BJ1"/>
+    <mergeCell ref="BK1:BN1"/>
+    <mergeCell ref="BO1:BQ1"/>
+    <mergeCell ref="BR1:BV1"/>
+    <mergeCell ref="BW1:BZ1"/>
+    <mergeCell ref="AW10:AZ10"/>
+    <mergeCell ref="K10:N10"/>
+    <mergeCell ref="W10:Z10"/>
+    <mergeCell ref="F1:J1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="R1:V1"/>
+    <mergeCell ref="W1:Z1"/>
+    <mergeCell ref="R10:V10"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="O10:Q10"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="F10:J10"/>
   </mergeCells>
   <conditionalFormatting sqref="AC3:AZ8">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">

</xml_diff>